<commit_message>
delegates lists and images updated
</commit_message>
<xml_diff>
--- a/static/2025_LC_DELEGATE_PROFILE.xlsx
+++ b/static/2025_LC_DELEGATE_PROFILE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Getting to Know the Delegates" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1190">
   <si>
     <t>Username</t>
   </si>
@@ -3248,27 +3248,15 @@
     <t>/9j/4AAQSkZJRgABAQEAlgCWAAD/2wBDAAQDAwMDAgQDAwMEBAQFBgoGBgUFBgwICQcKDgwPDg4MDQ0PERYTDxAVEQ0NExoTFRcYGRkZDxIbHRsYHRYYGRj/2wBDAQQEBAYFBgsGBgsYEA0QGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBj/wAARCAC+AN0DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD6yooooA8m11saxqTgDcs0hGR33GuC0zxHNcalImGDJuyCeuK7fXLmGTXtVhDZZZpR+OTXlWhZOuXSEc5YcV9JqoxHBaNmhpHj2K68VPppbayuVIPbmu+1C9Sz0iS+ydq4II6ivni4s5rL4jQ6lExEM5Kk/wC0D3r2Sa+F/wDDu43H94i4NKjUcrp7lVIJSVtiwniiKPSZb1jlY+57Vb8NeKLbXdwikDYPXINcKEMvgq5jOPmGOOByK5f4aXV3o+uXdncE4ilyN392m6zUop9ROknFs941PVI9NjQyEZc8E8c1HLr2nWmgyatqN5DbWsQy8sjBVArjfifrmm6V4btdTv7lIolJYKT8zcdFHc18k+MviL4i8Xf6Pc3MiacjnyLRW2oue59TjuemaKuIjRV5FUcJ7SPPJ2R7d45/aXCrNYeB7FZMZT7fODxxjKLxjnu1eF61418Y+I5XbWtev7rPODMwRT7DOP0rm4ZEX94zlwrfNxj6Y9fSryRKYvtDNtUtyqj5cY968WtjKlR76HVFRhpFWICZCp8xWO75st0J/wAingShhgY4AG0jnj25/wD11YIOzZhgCBtBw2B1A/Pn8aJ2URrCNiDdkFl78Dk9R3rmuwvudD4W+JvjjwdMzaXr90sC9LaRvNixnOCp6Z9R619K/DX9ovR/FM8Wj+JYo9J1NsKsob9xM2cYBP3SfT9a+PbgRpJwZI0fp37ZJx1xVWO7T77LlTzlRzn2rroYypSe90Y1KEKm5+n6So0fmIylCMgg8GpY5kLD96p9s18VfDL476volnD4Y8Q3LTaccLDdSHL22eMHuV+vIr0zV/EfjTSrdb6LdcW8/MJQ5DA9CD3r2qeKhOPMjheHkna59Hj2PXtUnO726jmvnvw74w8balPbvLZyRxFwrEDpXpl14ouLCaC0uM7mXIOO9bQamroxnScdzuRn1wB1p4GFOfyrOXUoINFF/cNhdueeM15hq3xgWPUmgs7d5I1ONwBxTlZbkxhKWx7EMbsY60bEZslQSO5GTXE+E/HttrexJWAc/wA66nVdWttKsxcXDhVboT0oSvsS42dmX2jRjh0Vh6EZrV0lI47NxGiqC+cL64Fc3pWrW2rW/mW7q2OwrptM/wCPVun3u30FcWY3VFouj8Rdpy96bTl718+do2iiigD50inubn4meJ45GXy01C5UfQSNxXMaOf8AioroA/Nl+v413UdkIvFviSdh9/Ubk+/MjVwukEf8JRc85+d8V9RJ/ATR+FkVlpY1Oea3IyylmUjBIpYdSey0e8t7gBEPysSeh/yK0vCgI8Stj++wOOnWsf4oafJplnezQLhZV3qQOhBrCXux5jojrLlZetST4Tn5646+lUpNNjt7I66CFVBiZiegHeo/DF2b34ctKwwwUBvyrnPil4sXw/8AB2bTYZil3qUohXHUJ1c/lx+NOMk4qT7DpQc5KPmeL/Ebx5qHjPxN+9kkNhaAxWseQABn731PU/gK46COedsb3CD5mG0/mfzp+n2V1qEyIsRaRmwhPAyfpXo2keCooI1a/uGJYAnb0Ptz9K+dxmMTldnpwouu7RVkjh4Vm28mNlBO7MY49TiprqQzXXkxRvJIQMgkrt4H8q9etdB8OGMb9OjkYHGXyeO4rrtK0Hwl9sW+bSrYTdpdnQ/jn1rlhik+hs8ulbc+d/sRiZTN5roV+7CoByOc4H1/WmPGk0kZ8ppF3CPZtYMen8PvmvpG88GeG3uBdQ21r53A+9k469B3rUXTPD1oqzPZQPKDkuE5JxWkq1hxy5t7ny1PaSxzsoWYLFw8UoyF5yPzrPa3K/MF2xsSCVBwT2HWvqe70bw7eRCb+zIo2bPbA655rhdY+H+mTytJZyLEMElNuRmuf69FO1jWWVTtzJnhaSeUAFT8hyff2r2T4TfEyY6engzV5PNgebfZySHJiPdBn+E9h65rgde8K3+lwyvLGTliAY8sCv8AnFc1btLa38N0jNHtYMG6EEHPb8K9LC4nkfPBnkV6DjpJH6R+DbeD+wFzDHnPXaK5zx4oXxRZBFA+XI547Vc+EutJrvwx03VkbPnxAsF5Abow/MGqnj4Z8UWW4fw85/CvqVLmV0eNZqTI/G2oy/8ACOWOlQNt80YbHpW14N8F6bb6Gk93aJJJIuSxWuT8RYfXNOD/ADKE4z+Fet6UoXR4FXgbRTluE5Wikjy7xV4eTwz4ggv9PHlwTHkA9D61d8e3EmqfDFRGW8xgVBHXOK6H4jRq3hXzWAzG4INcfcTNL4IgBwcSAfNn1ppXTQLXlbMT4HeIrpbRrPUHPmRyGM7j79a+lNMINoxH97+gr5wTRxoU6arartinbJIHevevBV+NQ8LpPno5U857CvPx0XHD2fQcdal0dFTl702nL3rwDpG0UUUAfLr+KLuL4u+JdJeN1jXU7gK2Oo81q29P8Oot09wFX95lg31rY1rw3YP441LUERfNe5kZvrvOavooRVX+Ef0r6rmUox9DGClG6bOd0nQBY6kZm+9uJ3fjVrxboP8Abvh+S22qXA44zW5u79RntTxxhc8Dvnmp5VaxpzO9zz3TPCUmm+GJbSIHLYyOf896+b/jl5r/ABNtNE8xmW0tUyM9Gcknj6Yr7UwD0UAdOe9fGnxYifUf2jNXSJtz744wp+7hYgMVwY9qnQdj0svTqSl6GN4R0W4W8EkuFjDFuhzkfzrtbyJtqiL5io6+1Q2NultarBE3I4JJ6/8A1quW/iPwxYXuy/u/mU4+Rdw4x3/GvipVJVZ6K59LThGhD3nYrWVven/UxbuO/cdK1LNdTgmJUOyn6498A81Un+Inhe1vibKZljCkklCMke3vSnxtpd5taC4jYvwGXB6nrmt1TlFaocasJaKR2NhehrfdMoB/vAdahuy5ZmhyD6A8H3rISczKJLYrID1G7jFSprMNkPNmIXAxj0/OsJSbZ2JJD5pbuCPnO7HQdB61mLdzLu3Bm74NbUfiHQ7uzzJeW6tuwCzAnNE0OjSyN/xNrVZfvHEgyB2rnkpJ3saKcGrXRjmyNyrAw43Z5I9R6d68f1jSBaX00TY4Y/LnP+eK9pkk8nlG8xF43qcgmuP8TaZDLbyXsX3txLHpjNduDqtSsebj8OpR5kezfsnaubr4d6pokjZOn3nykd0cZ/mGrvvH/HiKyOQMCvHv2TZJo/Eniu1TP2d4reTkfxbnH9a9u8ZaXcX2t2ssQwoHXrX3OCk5UY/11Ph68eWtJGH4nt2ik0y+2/KygZ7dv/r16T4duludBhZCOAM+1YeraE+peC44Av8ApEQypx3rhNO8aXvhWVrS7t3YLxtArrk0tzHl5krdDuPiXdRxeF1hYjdK4AHvXLXEDQ+BrZz1aQHB471hy6zqvxB8UQYt5IrWJs8jGa7zxdYix8GWlugJYOBgD3ojJPYLctkT2mlJq3w8e3xl1XKn6f8A6q6L4TtJ/wAIfdRTDDxXjIR9ESq3g7I8PhTn34rp/C+nrp9vfqgG2W6Mox7oo/pXHmT/AHLCi/esb1OXvTacvevnjqG0UUUAeS6krf8ACTahu/5+JME+m81CoBbG4DNWtYI/4SK+zn/j4fj1+Y1UA+bOOvSvpqfwokkGCwH8qeQGU49aYMgDjtUoB+nvVCHDnnr618s+ONI+z/tE+IZyuBtjlQ+u9F/wNet/FTx5deC20eaElrSaZo59n3iRjA+leYeJ/ENn4k8QDWLN13vbIjvjBbaWxn3wccV4Oc4ymqc6L30PocnwrUlVezRwnifUZltDZWbGPeRvlBwQvcVyYs9KilRr6Xd8uNoySRnnAFdvN4ZuNZjkmjJMh7dBXDa14U1PTL5ZLktLGGBaE5AcDtkc187hrJWvY9TEau/LdmxJpHg2701po7v7JKmMRyXEOT/wHcD2rC/smCwCz2srSRK2Q8ZOF9yO1XrfRtGvvFUV3FY3FpYS7PtNgED5I6iNyOAfpxmu31bQIJNSW/07RE0i1nVle03blfP3WAP3ceneuyr7u0jnopzvzwt2E8HJqWoosdqs0oXjEa5NQ+MxPDm0uGa3k79vwr2z4DeHrWPWvskQDuIy2C3Bx9O9cr8ZvC8Ufjado49sobzCjfxDv+dcMmklU8z0afM7032Pnz+yiZkAvyi5z+8O3J7966qDwdALbM2vJ5ko3NGsmGPOeh7U6Lw5pVxp2pjVmu7e6mjYWdxG58uFwcjeBgkEcd+vSsq10yyt/C1/Nrus3a6ikapY2FoZJldgfvuXGFXoODniu5xcoXU9TzNIVLezujYhn1rw5MsUTG6tGJBjJOfr9eK6NmW/tiAoMMqEbTz1HQ1yHhy41d7dIr6JmVjhC/zEfj3FdlCrKu0rg45xXGp8s7Pc7o07wutj0j9luzAvPFF0MjC28J9M5c19IeXG/wB9QxHrXgHwO1bw/wCDfAeqXerXm2e9v3cpGhYpGnyru9ydxx6EcV73Y31pqemwahYzLNbzoHSRT1Br7bAVIeyUE7s+Kx1OaqOUo6N6FrgjAArL1Hw1pOptvuLaNm9SoNanRenI/lTgR1yOa7bnFsUNM0HTdM4tLaNT6gfrVrUNOg1C3WOUcKcjNWQ2O3404H5vw6etO7JIrK1jtIPKjre0z/j1f/f/AKCsjAIGc/StbS/+PVv9/wDoK4cw/hF0fjL1OXvTacvevBOsbRRRQB43reqWieKNQiaQbluZAR7hjUcd7buq4kAGPrXH+Lom/wCE61hY5CzteTHrwP3hqrHfCCFfMlMYA7txX0dO6itCpRR6HHIkgyrcetSsu6PYG5ORnHFZGi3EdzaiRWYgjgf41rjBwO9aGZ4T8b9Mup/D9u8w3LBdKTjngg4/pXk2iOIb5oy67GJH44r6O+KVp9t8J3saoJPLUStxk/KQf5Zr5WEF5pOrXEUjNJG774pB91lI6ivmOIKLdS/dH0uT1rUUuzZ6bYX66ZeLL8roCOSf0ru9NPgzxK5W8tm80joF3A14rFPI8g3v8p9K7TQb77KipHKqscESIefpXztBuD1PanGMz0aPwb4bsZftFnbrCB1xgevX/wCvXG6zGuu6+mkaOjOIgDI6LwuP8niuguL27vdGkitQod87fVhXnz+L7n4fTXNlLDunkwz7QC8hYZHXoO34V2VqnPG0EKFLkerPd/g5Dpmha2DdzLA6g7/MOMVm/F6yttX8TmWzmSRiARInIxj1r550/wCJM66s15Kbq1RmAUSqGHP0J961tR+JUlzcJcw29zcKoyzQxngd++K5akZqmqSj1vc3pKl7R1ebpax1+j6Kj+dp2pQiOTOVyMhh/hV3/hVukXZ85zBH0zztUfUZxWHpHjeLxRNDJp9rdCS2/wBYssW1lHfPtXbXGox/2TIs6BkYcpgHcP6VMZSStM1lCMtYMx7nwzpGhQbI2SRhwMDp9DXE3yRpIxxjnIxxgV0Wr3TSNtLSH1zyK5jVJCFJHCqM896ihJzlqRiEoxKOryX8/g6RIppI1ThVjOM5bkn8c19g+AbMWfwx0G35XFlEx+pXJ/nXyL4Ohm8T3UWkqW23N2kKEnoGfB+uOtfbNtbx21rHawhVjiRUUDsAMD+VfUcPwlzVJv0PmOIqkeWnBbk44bPH0pyFe9NB9uhoC4r6Y+WJQSMdR7U7qBnt0pi5UjJzTh09cUxNEi9M4rW0rP2Rsn+P+grGB4A6EVs6V/x6v6b+PyFceP8A4LKpfEXqcvem05e9eCdQ2iiigD5s8U6DPJ8QNWuF8wRy3sucHnlya5nUPCOoT28awTSYjXGCeG617BqwU+JL87elzJk/8DNVFClj8vH5/wCe9fTU37q9Av2Od8I6bd6fZRC5kO7bg7v5V1YJCkqOx4qIBVXAC8/hUy4K4A7en60XJ2OPuL2NtUlhuFLLkhg3fI/+vXz18Q/CjaBrCi2LSaZMxe3c/wAGeqZ9q+nLzQBPOZ1bLEcj1Fcr8QPBsV/8NdQIiYzWyfaYlH95Rz9eCa5Mww8cTSd91sd2X1vZVUns9z5os7gxwiE87MgH1/Gug0u+8uZZANgB7kniubmidXR4jweD19Kv2km5/m9O/c18Ty2Pq4Ss7M9p8D3Nq0TS3EgZVxtH92uH+NcGhalIl1KySXgQKiQcuRk1yt740m0S1ks7UMs0iN8wHArkdI8WkyeZLPcTX8n33CFivJwB+ddNGEuW5nWxCvyot6D4D8VtPb3FtpdwqtJ0ZlDAAf3Sc9/So9Z8H+M9KjkuLzTboQscOEdX465KqTgfhWtJ4j8SLFHNFpupCE/xCFwDkdRxV2LxH4nbdMdK1I2/GWNu59vStJ6u9gjh5KOlzsPg1FZQ2ck0Mwd3AEiufmAxjGK7HXEtorgpBIwQj7i4PPoD6V4PH4r/ALO1xb3TGazvt2DA0ZUSgnJJHevRLbxEuuqsoR0YAFieP8//AFq8/EU5R16HfhsRF+7LdEt3K/zeXIzIRlsn+Vc/qVw9xbLGxEZbg55xzzWnczlnZNx6569f8Kf4a8N3XivxCLSJPkjUzSE/3QR+pJrTBUXUkklqYY6soRbb0PQPgX4VN1r0etSWxt9N04EWykf66Zhgv74H6kelfRoIBwOtea+BNM1XTI1trnCQp8qooAwK9Jz74I4zX2+Bwqw9JQXzPh8diXiKrm/kOBI6npSh0PyqylvaqOpTPDYOYs78cYrg9L1zVTrV3bXaMqwniTPytmvVpYd1IOaex5FbExp1I02tWeledGON3409Zoyx2uuDXGXF4zN8soDIPnGffrVCG+uy22KUnqB71l7NnRY9GV07OPStnSTmzbp989PoK8mOp6pCoLNtHufevRPBVzLd+Hnmm+8ZT0/3RXDmEbUWXT+I6SnL3ptOXvXgHSNooooA8l1c/wDFSX+Bz9ok4/4Eaqq3GB27GrOsf8jFqPJ/4+ZPw+Y1VU9ehJ7V9HT+FAyUMAxGOfWnqOMDGW7VHzwP1HpSg/uzgfrVCLA+bGepxmporX7e32IR+YZhsKddwIx/KqikkZJ5I4Ga734e6DBqltqc94m6GSE2gPcbh8xB+hFRUnyRuwvY+F/EHh2LTfFeradazrcQW1zJGkkRypAbse/pmsFLZ4bgqUJ7gdfSut16zf4efEnVPB+rMT9juPK3uPvJnKSD/eUg0y606NmM0TKy5x8tfH1qa55NLTsfW06ykk0czPY295Mong3FWBD+3pWs2o6fo0KmSxjYou3zFjAYc561BLsglUMepwR6Vfj0176NQuzBxy3oa523E6ocsvUZo/xr/wCEa3RJPcSQPn9y8YZR9K15/jnba/bx2LNcJCpyERAo9O1c7qXw7aYGQJ94fw8D1qvpvw6ubG6EhChd2QBxtHftVyxFou7ZtBVVKytb0OmjutK1o+etlHlvlMkiAtx74qGJbaF5Y4Ixu4xgY496m+ymxRhtVO+RSRRB9xjXaW4LDr9a4tar3OiXLTXmZ4iMs/zcgc5696+gfgp4dXT/AAlcaxcRYm1Bxs3D/lkvC/TJ3H8q8bWXRtKvbA63I8drLMizFBlljLDewHsK+snsItLjgt7fy/svlKbdovuvGR8pHtivo8mw6U3N7rY+YzrEPlVNdRFjjVi4QKx7jr9Klzg4qFWyuTUikFt3519KfNGHrk9xFEyRIWLMBj2qEaStxpc8iqVaRfxBzXQSQRzYLAcY61IipFHtAGPYUqLnTb10Zyyw/NU9ozx++0bXU1K4dWfy8qSQOoqO2OuWdwr3HzR+d8nHO3HevYmt4WUlo1we59KibSbKRfLaBceldaxHdG3LY8/uNTubm8ZWtdzKwCr0yMV6T8OJWm8KzM0ZjIuWGD/urWc/h+wMiOqYdOQa6fwzYxWGlywwn5TKW/EgVw5nUUqDS8h0l7xtU5e9Npy96+bOsbRRRQB5DrMsQ8TX4Lrn7TIDk9PmNVgydNwz65qne+HPE3iD4gatFoelXV1i7lG9FIRfnPVjwPxNei+GvgPqBjW58Va60Pf7NZfMR7F2GPyH419C6tOlFc0uiM1JvdHFZ+b059etdHpHgvxJrI32umyRwnnzJ/3a/ryfwFe1aN4Q8O6FEo07S4VYf8tpR5jn8TW4Oen6Vw1Md/IizxW6+F2o2GkzXd3exSygARW1upYyOThVycAZOOa7nwfoE/hvwhb6ddTLLdZaSd0+6XY5IHsOAPpXVzRLJJGWGdhLD64I/rVcqS3IrB1pVPiZzypXqe0b2Vkunmz5G/bJ+FEusaFF8SdDtma80+MRagkY5kg/hk/4ATz7H2r498O+OrrTEOn6mWktWGElJz5Z7Z9q/W3UtNgvrGazuoVmgmQxvG4yHUjBBH0r8wP2gfg/dfCr4pXFhBA76Hf5udPmPZSeYyfVTx9MetY1oprnPXwNZy/dvdHA67ruoyX05huEZVb5WQEbueo9sVJpPjm9s0dLkyFlwV9+e/NYCyT20fkt+8h54JPy/Sqs0JYA20x54IA5xXP7OE1sdXtqtOd0z1a1+KjusMbFZFTGQx5547f55rSHxDtbiaOVZWWIx7SDgDdnrj868TfTbuMMUjY5xyvt/KmRWd/5reV5m4ZGMmsJYSElozpp5nVjuj1jxL47tVVYba5bzGHO0A4BP6etP8OeOGhsFW9tJHJBKyAYDc5FeX2ekXFzOJJZGB689RjsfyrsLO2xGF5CIoCr/Ol7GnRjbqbQxFbFT5nojS1fUbrUreeW8kzJKuwYGAgPQAV9jfst+IpfiN+z/J4e1OUNq/h6Y20MjfeMRGUB9R1X8BXxLf3X2ZlnJO2Ng3T0NfXn7JcTw+NNR1iFVittRjWPbGfkkwoYP+f869DLuaUJNbrU8vOGoVI9j1CSOS3upLeZTHIhKsD1BzTkPPoetevah4U0TVrpp7u2YTMP9bGxU/4VzOpfDe4hjZ9KvBMP+eUwwx+hHFetTxkHo9GeRKPY4oH5sHvTsjbtY0t3aXWmTeXfwSW7r2dcVzuoa5DFqIto5VbK5yD0Nd1OPPsYydtzo1PHcU8cnIPNVbSdZ7WN1YcjBxVhSdpOKT0F6D8kYx6VuaN/x5Pz/H/QVg/Unit7Rj/oL8/x/wBBXHj/AOCXT3NGnL3ptOXvXhHQNooooA7zTfl0e1CqqjylPA9qsnLcVBp3/IHtf+uKfyFWScVRIx2A+WnqPl4qJuZKlX7uKYETkiQD1qFhhqtSICucdKrycNmqiyWLtDLzXmXxw+FNn8VfhXeaEVjj1KL/AEjT7hv+WcwHAz6N0P19q9N82OOIvK6ooGSWOAK5PU/iN4ftbr7JZu19MOCYeUU+7f4VcYylokVGfs2profk1qujXenarcaXqVq8F5bSNDPGRgxupIII+orFNlGsjYGD6j/69faP7T/wn1HxJqln8QPBfhu8vLq5zFqlvp8RlOQBsk2rzyMgkDsK+TtS025srt7bU7K4s7hOGiniMbqfQggEV59RSoTcT6ijKniaanHcy4I7hGxHdP8A8C/+vV+3tZGI8+5bjJwDj+VRJZktxNt9mHT8atx27x8GZeRxjNZTqN9TRYdLdFiO3hikymC3QH1HSrifuozg9arwIFxkgt696lC5UsRwp5B71jKd2dtOnyGRqwmlxAmXkcgBe+ScAV9/fs5eGv7F8F6bEy/PHGpz6kAZNfIvww8E3Xi7x1DKIGe1tJAzEDIL87R+HWv0B8B2ljo1nHAHVVgjPmY6j14r6rLKPssHOs1rLRenX8T4bPMT7XGQpRe2rPTlGYwKchOMfxCsWDxXojMUa4aL/rpGy/jnFX7fVdMvHH2W9gkb+6rjNea4vsA/UNOsdVsmtNQtY54m7MOnuPSvIfEnwOaS6e+8O6gG6kW116+gcf1Fe0+hFPFa0MVUoP3GKUIz3PmzT/DfizSLh01XSbiHB++o3Jj6jitn+Hp+te8kAjBANZN94Y0PUG33FhGH/vx/Kf0ru/tTnfvx+4zVHlVkzx3q2TW7on/Hi/8Avn+Qrpbz4dWrlmsb6SL0SQbh+dZMekXeil7S7KFid6shyGHTP6GoxWIhUpWiyowaY+nL3ptOXvXlGo2iiigDvtOP/Entf+uKfyFSyOB3qrYvjSLUD/nkn8hT9odqtIkkU7mzVharhdvap0psEPPPFUriWOCCSWZwqRglmPQAVdrF8RWktxpFwkSGTzEKsgOM0ob2G0eL/EnxNrF7qFnfWly6aLazf6RaKP8AXxHgue+V+8B7GrdtZ2rQr5MaKrcgqODVu80OebTngmt2XI9OKw/Dt1LDqEnh26Xy7i3TdCDxvj6ce69PoRXdBODujhlNU63LN6S29TprBr7T3ITcYh/Cf6Vc1LQvDHjLTWt/EujadqkYGNl7ArleOzHkfgahhu/LUJL+tWE8tvnTHuvY1u2p6NHSqTg7xZ8mfHT9nnTPDugzeNvhzcCTTIPnvdNafzGt1z9+NjyVHcHJHvXzYJZH+8Nq+p7/AI1+inimBNLvhcQqPslyDmPAwD/EPfIPSvlH4p/DJJPHlle+CrISw6vKIBYW658m5J+6FH3VbqOwww7VzZjk7hSWJo6x6+R7GWZ1zSeGxHxLZ90eRQTvgKi546+ua9h+FHwJ8ZfFEreSE6XocYy2oTxnbJ/sxjjefyA7ntX0d8Kf2afCXg7TbfUvF9rBr2uEK7LcKGtrZv7qJ0Yj+82enAFei+MPFEGlaHLBbSLb28MZMkiDARAOQoHT0rzKWDV7zNMXmjUZcrsl1PNdDHwi+BOhrpseoajrWqIxZ0hiAaR84JzwoHQde3evW9J1uXWPCtvdppL6XHcqJPIlYNKFPI3HsSMEj8K+aPAmgXHxJ+LEuqXsJ/s21cTSqRxtB/dxfjjJ9ga+r7XTHkt0AGB6CuylWnVW/urRHxWTYupj6lTFNWpt2j3fdsyfM/e4YbhTLiygl3SRYjkAypXjmukj0BNwLGr0eiW/G5M4rXnUep72jJPDtzNd6DDJcElsdT3rXqraWcdpa+TCNq5yB6VYU9j1rlnq3YSHUUUA1JQcVyHigY1aPn/lkP8A0I119cj4p/5C8f8A1yH8zSAw6cvem05e9ADaKKKAO1s/+QTa/wDXJf5VICVbjNRWmf7Ltcf88V/kKuJHnmtk7IgRWNTqfloEQpwXHGKhjDNIxyMGnDFBApAUJ7KCXOYxzXm/xB8KvCtv4k0oeXeWT7sgcEdCD7EcGvVCBUVxbR3Ns8Mq7kcYINbU6vK9djhzDBRxdCVK9m9n2fR/JnmtnBBrmixajajhxh17ow6qfpVR7G7gf5Ccj+Fu9JZTf8IR4+k028DDTrtvvn7oyflb8Oh9vpXo8umwSLnaGB9K7PaqL12PNyHNp4ylKlW/jU3yzXn39JLVHlOsaZNqujyQywq38QU8EMO9Znwi8B2lhqmpeJ5WeSRT9nhSXnym6uQe55AB7An1r12TRbQo2VI9s1FBpkdjo5trSIKHYyH/AGiTk12/2nKOGlh4PSVj0KmFVXEQrSXwmRq88yQsIwdzcDFeC/FO6vLsx+HLYMzylWn2jJOT8qf1/KvoXxHc2uieE5tVvEwsEeQjdWb+FfxOBXlPwv8ADc/ijxlceJtVTzIbeUyAsOHmPI/Bf8K8epaUOVbv8j5rirMq1erRybCfHV+J9odWdX8NfAa+EfBdtYbALqXE10+OS5HT8On4V6ha2+yNR6U6K3UHpVsKB2qZSSSjHY+twuHhh6UaNNWjFWGhAO1PUCilFZHQLQaKTNAC0mKWikUFcj4p/wCQtH/1yH8zXWOSOBXJeKP+QrF/1yH8zQBiU5e9Npy96QDaKKKAO408f8Su1z/zyX+VXt6IBk1x8HiC9t7dIUigKooUbgc4H405/Ed7IuGht/8Avlv8au6Jsdf5gI4NMaULXIr4hv16LD+R/wAaU+I709Yrf/vk/wCNGganXo+7mnEmuQXxLfL0ht/++W/xpf8AhJ7/AP5423/fLf40rhY6wZNOxXJDxRqA/wCWNt/3y3+NL/wlOof88bb/AL5b/Gi47DvHPhiPX9BZ4owbuDLx/wC16rUPgPXo9X0EWkj/AOk2n7tg33io4BNP/wCEo1D/AJ423/fLf41zUNhFa+LG8QWckltcMxZ4oiBG+eoIIzg9etaRqJx5WfNYzLK9LMqeYYOKfN7tRXtePRrzj+KO91FZmjeOHgkdat26f6DDnrsAP5VzJ8R3rNkw2/8A3y3+NA8SXyw+WsduOMZ2nP8AOk6l0kfRcrvc89+KGsXHiXxda+C9I/eeVIPNI6eYR39lGfxr1PwvoNr4d8N22mWy4Ea5Zu7MepPvXCeHtEs/DmuXOrwGS8vLjJaW7IYgk5JG0Dqa6z/hJr7/AJ423/fLf40uZHzOR5PWpYitmOOt7ao7K2vLBbJP8WdYo706uS/4SjUP+eNt/wB8t/jR/wAJRqH/ADxtv++W/wAam59RY64ClrkP+Ep1D/njbf8AfLf40v8AwlOof88bb/vlv8aVyjrqDXI/8JTqH/PG2/75b/Gj/hKdQ/5423/fLf40gOtBpa5H/hKdQ/5423/fLf40f8JTqH/PG2/75b/GmB1BOZetct4o/wCQtH/1yH8zTR4lvw27yrc/VT/jVC/v5tRuFmnWNWC7cICBjOe596GIq05e9Npy96Qz/9k=</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEASABIAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADNTgAAJKSAAIAAAADNTgAAAAAAAAyMDI1OjAxOjA2IDE3OjE5OjM5ADIwMjU6MDE6MDYgMTc6MTk6MzkAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjUtMDEtMDZUMTc6MTk6MzkuNTgwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwAGBAUGBQQGBgUGBwcGCAoQCgoJCQoUDg8MEBcUGBgXFBYWGh0lHxobIxwWFiAsICMmJykqKRkfLTAtKDAlKCko/9sAQwEHBwcKCAoTCgoTKBoWGigoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgo/8AAEQgA5QDIAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A9/20bamK03FQMi20YqYLShc0hkBFROtWGWoJnWJC8jBVHUmkM85+MS7dDt244nH/AKC1eXabpN5qAUWsDMvdiMD869n8TLa60I4p4Q8Mb7wGPU4x0/GmWlukaBY48AcBQMAVx1ayv7p3UabUdThtO8Ahyj385yDnZF0/M10UXhLS4UGLcMfVyTXTKmPrUhiyvIrmc5M3UEjk5fDOnbcfZYxn0JFYuo+D7OQf6OZIX+u4flXfTRhF6Vlzn5ueKSkyuVHlOqeG7+z3MqGeIfxR84+ornpAwJyjj8K9qkHzVh6zoVnqGTJGElPSROD+PrWkZ9yGjypifRqrXGdn410OsaDcac5LqHh7SL0/H0rCvI9sZrZMlrQZu9j+VIW9j+VP8vgY9Kb5dA0hm76/lRv570vlmk8s0BYXePf8qXePU03yz1H86adwP3TTQrBM2V/GnhuKikB2ZNSqp21RDWpveBH2eKLAnvLj8wRRUPhBvL8Sae3/AE3QfrRWkdjCe59eSEZxUdTSKM8io2FbHKIKXOFpBVPVNQhsYcthpT91B3/+tSbSV2NJt2Q6+u47WLfKfoo6muTv7ya8fdIcKOiDoKgub2S6uC8rZPb0FLEQVGOa4atZy0Wx30qKjq9yS3hL8kEAVeit+P8AHvUtmnYgFuwq9gRrjq7DgCsoxubOVilDAVYEgn3qyy7c/JkVd2jaAOn1psoVo2U84Gc1pyEcxiXseY12ggn2rDmUEbH9eGFdNcSBSCcbQOp6ism7t1+bB756/SspRNIvQxZo2UdMgVVliOST064rScgBk6e9Z1xIdoAPQ85pWApXKIyMrgMpHIIrhvEvh1hDJPp2WXq0XcfSuwvJDyNxxVA3WzocmriSzzMSOEAO7P8Au03zH77v++RXdalo9vfq8sWI7n/x1q4+5ha3laOUKjKcYJrQaaZV80+rf98il80+p/75qTK/3k/76pcj/ZP/AAKgqxGJT7/98ijeT/8As1Ou32/76p21PVf++6LisUZzmM0qt8o+lTXCjyzjH4HNNjUeWucdK0WxlLcs6HL5etWTdMTIf/HhRUdrhLqJgBwwoq4uxlJXZ9mSNk1E1KxG7ikfiug4jD8S6wNKtU2bTczNsjUnr7/QVyMt08gaSV2eQ9yetZPiDURqPi67mDEx26iCIZz9T/OnNIeAelceIlrY7cPGyuX7dt4q9BtSRGbDEcjHasW3m2Fcc9+taUDljk/dHWuY6Ub9lchWXjg85rRWdS3qccdq5y1clgOAQeMVqQ7iwHOMZ4q4smSNCa5EQ42knj5s1D9pDR5DY4xxVWcEZ2Euw9cVW2u65YeWWGAmST/hVtiSG3ModlUuQFPPzYJ/SobyXdGcDAA4JYcmpvJkAOZEQA8EAkn9ao36BVA8xmPQg/5/zis2WjLd2Lknrz0OcVnX0i7sZJbrxWosHzbl4G3k4/z/AJFYOoIDKc9e4BqRmbeXH7z2BzVDd8wzjGamu4S7blJHPQiq0ibVwCM4yatEMd9oCk7azddhS8txMoxNGM5HcelPkfrjiq7T5AFaIzbMq2tJJ0yoz9EBqz/Z8o/gb/v3XovwSeFtZ1CxmjV90YkXdJsxg47+zfpXs/8AZ1t/z7x/+BA/wrT2LeqYvrKWjR8qLYTf3H/790rafN2Rv+/dfVf9nWv/AD7xf+BC/wCFL/Z1qettF/4EL/hR7F9w+tR7HyVdWE3ltlD0/u4qvFauYlYDg19a3Wl2TwuptITkEf69P8K5bwDptnJ4P08yWkLsFZSzSoCSHYdCPamqb2IdeL1sfOiwssq/WivpvUNIsjHn7FbAA88o3H4Ciq5bEe1TOq4B6VDdyeXazSf3ELfkKezVR1nc2kXqr1MDgc/7JroOY8C0iZpbl5GJ3Mdxz610Eb7lwTXL+HiXeZj24roLXqd2etcNb4j0KXwl+NsYGK17FwvysOCOuKx4lMkgUcD61tWkQ3YYcYxXOzYu2oPmcdM8Vsr8qfKM+mKzII5Fy3nK3GcBcVahvEj+WYgD155qoiYskrqxLrlf92hrhW27n3DpyKknlgnXG8Lu6c1RUbfuc98+tO4JFu3xJ8yRqQDtOwLiq98hPUAZGDuPNWYpFQMN2eeajZkccH5uvGM/z60AZzxKYWHDA1zdxFtdmAGcnHb6V1U9zFHbnJXcOpBzmuavriN24I4pSA5+7IDsvAPpWZcA+XkdMYrSvMM7HoOprPuwDEQpHT1pITMSaTLGqzSdOec1aaLbuyDVCcYkGK6ImLOv+Fcxj8e6fhgN7MhJTdnKHjFfSIj9dv8A4D18tfD5yvj7R8bj/pKcK20/nX1QHf8A55zf+BAroWxyz3G+WB6f+A9NbaPT/wAB6k3v/cm/8CBQS/8Adm/8CRQQUp3Tafu/jbVyfgORU8Nxx7k+SaZebfP/AC0bvXZyF9p4n/8AAoVyPgremn38eJ8R39wuBcgfxk/1oGi/dPuGP3R9R5OKKlut2ORL+NwGooGaRNQ3QD28qnByhGD06U/NMcblIPQjFakHzr4YJa6nBPJ5IroV/dsckc+9Y2mWj2XifUbVgR5TOpz7NV64nAk9K4qq947qT90147iG3Xc7DJOKl/4SCGNSm7JHTGM1x97e+ahWNjx6d6wrx50BYFh9KzVO5bnY9MTXoH5Mi59M0PrkYPLqx6DnpXjVxeXScfN65qsmp3Kt95vzp+xF7Q9jl15N331J6cmmyeIWZQqsffnrXkS6hITneQfrV2z1Ji/zkmk6di1M9attZYrlmwB1pDr0ZZm3kcdK4SO9KWpdjgtzXP3mrybmCnAqeRluR6NfeIl6b8IOgzWLfeIkQnkD3z0rz2bU5P75/Os2a6mduCcfWrjS7mTqdjtrzxDu/jP1qmPEDcgfnXJK0zdD+tWI4JeGOc+wzWnIjPmZ1kGqecfnPXoaQkNLntXOBnT2rRsJ8sMmnawrnV/D9BJ8RNJR2RVE6sS4yOBnp+FfUebf+/a/9+mr5t+FFoLv4kaa37w7EaYeWATlVOOv4V9LBbj0vfyWtlsc09yPMH9+2/79NRmHs9t/35apts/pef8AjtLtn9Lz/vpaCSlKYcfetv8Avw9cn4QMaSa7GWt/l1KUjMLHghTx7V2siz4/5fP++1rkfDLSpr3iWIfa8i7VyBIoPzRr1/KgpGjcNHjgw/hCwoqa7aTad32r/gUwooAn3VnaxqQsIoztDPI21QTge5q/XnnxavprEaU8Ofvvkev3aqbaWg6cU5JM57WpLZvFk9xGDDNLHiRf4S2RyD3zisHWpcM0SuN2cFQMnP0FQ6/pRvL+K4FxtMg3OGTlTn2q1b6Oq2Li1HJJy3c89zXLJpu51JNKxjRsYeZVf8VC/wDoRFXIYXvF/dBh6HYjf+1KzruxmSTkFtp6etXYdekswqqqqQPlXuavkvsK/ch1HwxdCMy3E8ypjjEEY/8AatczcaQI24v7b6SAhvyTcP1rc1Xxhd3MfkuOAccGudupg+Hcqc9u9X7N9SW10I20+6DgRp5voYznP4HB/Srul2kklwqNBKJM8jaeKq25+6YsrkckcVvaDFM+oWpdFl5OFkcqoAB5JHIAqakeXqaQ1Ogfw3NLZg/Nj0xXEapot6kxEMEs3p5aFj+levw2dq+lyk6pYxSN1XFy3T/tvjH4CvPdb22csvk/ZjIy7VlgVlzkjOcsTn8awi9dC2n1OLfSL0SETolvjlhLIAy/VfvfpUTWaI3zX0JH/TIFv54qa5JaM7ssc5rOGc9xXSoGDZp2+nGUZguHfHcpt/xqx5MsCfMzfn/9jWPHfzQZCED8Ktw3jSxndNsPYdcmm4Bck81JCVaWNT/tbv8A4mpIY2hfehEqjsjAn8s5/Ss+QOzbmUfX1q7p8e85qWrCO6+H/iSDSNSeVILOW6kj2Qz3IcrCT1+VeST0z2r3L4feJv8AhI9LnkvI9PhubeTy3BZl3DGQcZ+o/Cvl5o/JPmISHzkfWtfwr4j1XS0uRp108JkI34QPnGcdQfU0uawez53ofWe6D+9p3/fbf40hkg9dN/76Y182Dxr4kP8AzEZj/wBsU/woPjLxIf8AmJXH/fpB/Sl7VD+qyPo55LfHP9m/m9cloc8C+MPEqYsNv+juMh8coRx+VeLzeMfEX/QTuv8AvlR/SsiPxNrEWoXE6ahcLPKAJHBwWA6U1UTE8PKO59MXFxCQcLZZ/wBkP/Wivml/FmuN11S7P/bSinzE+yZ9U5ri/iPbxXEWnmYZCOzf+g12Oa5nxrZyX8NrFEQGy5HHsKup8LJo/Gjzq52T3BdeQTnpWn4fOzICgpluo9zWWYHtpmguBiRev41taQqhWB4Gcj8h/wDXriZ27kOt2iRy+YoG1hg4HQ1wOsWyJKzBAevbNeq3TRSQ4bDJ39q4vXrCJC2SwXrkcitITsKUbnnc8MfmcRY/A02O1Dt0/Cti5t0D4QM59MGtLRdEmnnVp4/LiB5BHJrZ1rIzULsl8M+G2vkE037uEHjI7VJBBHqfiizsrAMtsYwGJGDjO4/pXY+YYo1hgBRAMYHFO8H6H5WrT6lcKQ8p+TIxgVy1K0Wro3jT7Hf/ANl2Ft4cWAW8YwP7gx/+uvAfiTapZalDLaqEjY9AOM19C6o6/wBjhU+9x9M+leLePLF7uMgLkocjIqU7SQW91nCSaaLyy+0WoPmIdsgxwW9vaso2J2nJIfPSun0+7ns7WNJATHjlSOhzVm4soL6HzIiNx5wOorr9qlqjHkOFlgkXgqGFVzGQfu4/CuqlsbiMYMYdfyNRppck+FED7jz93pVe0RPIYMUbyYwPat+w09oo8kY4zzWtpehbdrSADHJrTu0j8vC43dBispTvohqByF8Auc8VStXEEkhYEhjkfNtqzqsmbh1B4ziqE8exVEpA9Mik9iqejL4u0/uf+RqeLxP7ifjNWT+6B5Zf++TTsw92X/vg1nY6OZmhJdIR0jH/AAPNUjMPtBIIxjHWo28vsR/3zVYlfO4PBq4ozmy+0g/vL+Boqmdnv+dFWZXPtEmsjWr+C2urFXlQTlyRHn5iu0gnHp0pvizW49A0aa8cBpPuRIf43PQfTufYV454a1Sefxcl9eOZriTcxJ7nGcfTit6ivFnLSdppm94mYjV5HwRuAOD1p2m3QxtkYqpH3sZxVbxRei9v0uIxt3ALioLc4AwR/jXE9juT1OoiJZcqvmL3Kcj9KbNapOuM5HXBHSudEzxzK67ge55FasXiKeMAF5sAf3iai5diT+x4VGWAHvjrR5ax/LHG30ApJPF0jcF2AHfAB/lWDq/ie4ZWX7TKVPYOcUtWNKx0VhG09/tmUrsG5lIwcduK6KFtjjGeua57wLb7NLEj/wCuny7eo9P0rftcjJYnANZS3No7HRanbZ0tWRiRgFs4OBXnPiBEeFgeq8gmvR5r+2g0Z45CHkZThfQ9q811qUPG2e4ya0na6aMoXs0zzO7vP9IZZAAM49gau2Vt5qZKMATwy96sC0t7mK6ilABLZDdxWBbXT2btC52vG23NabozsdIltcRN8jlh6OM0pvb2N9kcCg9MqnWsxdcmXCrcyjjoWNNm1WWcFXnkx7uaEDLN/c36AmQGNT3b5R+tUG1mK1QtLiaYAhFBwqnsSe+PQfnVC+nXoMHv1rAvJtze1WlciWiHTS+ZOO+TUviC6zcLuBV25xWfC2JQfTmq2uXTS3cZbghAP1NaqN9DLm5dSXzj3LUonx3Y/jWb524DineaewqXGxpz3L/nf71RmX581UEjU5XJPNNITkWxNmioFb60VViLnvvxg1jztYhsFb93apuYf7bc/wAsfma43wpcI3iG2SQ4D7lB9yDVPxTqp1HWr67zkTTMy/7ueP0xXO/amSRXRirqcgg9DXRJXVjli7O565r0MSSbIG3LgEnPf0qC3LBV6H0rA8N6lJqVi73HMqyFSR34FdBbfcHUkdTXDNW0Z3RaeqNG0CmQFsZ6c1dfZ0VV57VTjVflGBzzyashxGM5G7uOorBm6KWoWsBXBUGsSy0D7fefI22McnPettl+03GMkFuACcgV0OmQ6fp5Te8aybTnJ7ev/wBerQmzEi1hdGuns7g7dgAHbIxxV638TQlWU4IPRs9K5L4ptDepHJa4ZwMbhxkeleYQa7cWC+WCzJ/dznH0p+y5tQ9ry7ntWqeKYQp+fI+tcdrXikvlYefxrgZtdWf7zMPYism91QudsWdvcnvTjRFKsjsIteMbOdwLntmp7SGTVFe4V13E4xXniz/MGUbT7V23hG/EMLCQsFznitHGy0M1O5qroszNnfGB6scYqpcWN1FnADLjqDXUCaKdCY2R0IzVW4wV25rK7LOJnlblWBB6ZqnMQWxzXR6lEG6qD26YxWFcwBDkH8K1iYyKq8PzWbrzqt8qqc4QZrQkIjUsewzXLyTvNKZJDljW0EYzfQuxNniphn1pdAtZNQ1S1tIigknkEa7+mTwP1r0VPhprPQ/Yx+NElqEZK2p54oPr+tSIuWPTp616J/wrXV+81mPoP/rUD4bap3uLX8v/AK1LlZXOjz9VPt+dFejp8NtRyN15aj/gJ/woosxcyOXvJfm61nSSVJdP81UZXrdmB2fgK6GbyFjz8rgfmD/Su8tX28DGenPpXkfhW7+za1CD92XMZ/Hp+oFeowzDbuzkfzrlrLU6qL0NppCiKdxzioPMctlyCDznNUvtBlAAYgD3pklyyRsSenGccVz2Oi5Yk1RbZmCHBxjI5OazJdXAVmYbmPykn0rn9W1AQSNluTkg1iR6n+++9uJYnk1tGJlKR2F9fvPE4dQQThccVxWo2G5mz1P4/wCetatvOs8f79guQepqwtzbLFgJI5GcsoqkLc82uoxHOy81WxzXa32n6ddO0iSbJCPutxk1z1xZxQyEeYG/3au5LRnRoS/FdFpUvkxkA5HHNZWyNPUHrzUizmMfKRg80mC0OkjvmWQFXI4wMdDWlZ6mZjtbr35rhf7QO7GTj61ft7kny3B78+9S4FKZ1F03pyKx5mQEjqT7VM0o8rI71T3DBOevApJA2Z2qOI7KY9PlI/PiuWVq2/EUu21RD1Zufw/yKwFOa6ILQ557mxo901pfW1yn3oZFkH1BzX11lXUOn3WG4fjXxzatyK+sfC9ybrw3pMxOS9pExPvsGf1psg0mFKEXFL1peBSAZ5Q64oqXNFAHzBcNkmqEjc1PcPyapuatgOSVopFkQ4dSGB9CK9W0u/W6sopU27XUH8e/+Fea6NpcupzMFykEY3SSY+6P8TXU6Rf26SGxtRsjQZQk5z6/jWVRXRvS0Osjn3Nj8cetOuJlWDJPHoKx4rgbgOd1TynzoTkk57Cua2pvc43xDM0lxJ5YO3PA9Kg0rQdSu/30C4HbdxmuxsNKjknPmKOvOea6eGMW8AjRQMDI4rTnsQo31Zwdr4c1A58y4jifONrJ1/EGtyy8C69eTLAPKAf+I7iD+Qrbl1K2iXbdJlSO3alh8Safaq6w3k8SZzsDnGf55/GhSTL5exgax8ONdspfLinsbx8cLCzBjn2KiuYuvBWu2iGWaCJRnn96Mg+h967ObxPa+Y7fbJS5HcZ4rL1DV7O6X5pj64BPNPmQuXzOAvLK8BxIsaY4xuz/ACrNkt7pTwrDvnbxXf8A2+wh/wBVGpbrzVGWWKXLbRyenahSJcThykwfLjPPOBWvpqlmGAcY5zWxLbxkZwPpiqxiWPlUGPWm5XI5SZnwm0Zx9apmXrUNzcbjwMe1V2m2xs79FGTSsMzNedpLgEcogwfY1lqavW0nnSOJeRIearXUDW05jftyD6j1rojtYwl3Jrc4Ir6i+Hk4k8D6Mx7QbPyJH9K+WYTyK99+GOqyHwfZQbkXyi6cjJ++T/WonLlV2CV9D0syj1o80eornGvZBwZSfwAphvG67zWXtkXyHSGYdjRXMi6bPDH86KPbIOQ8DuG5qsTk1NOcmrOgWgv9as7VxlJJVD/7uct+ma6DNK53MdsNF8HxxgATTL5sh92HT8BgVxlpDMJRcrlURs7j/Ku78bsz24AB2seKzjarZaPIskW4FBtYDPPenCPNqa1HytIe0nzAg+/HepoLnoMHP1qhnfp9rOh3Aptb6jiiCUZyrY9a5WjVHSae38QPNbH2hpFxwAOvNYFhNz8oHTt0rXgXcwBBIbnismaIz9RhMgbHAxn1rj9Qs3DEg16pHpqzKNu0HPORzUo8P2zc3KLuzwB/WiM7D5WeHzWso5GT+FQNHMo6EV7u2gacISptlLddxGPT25rJv/D1nuLBFTA496vnRPIzx+GKRjkhgPWryNsGduTXYXmioJCI+AOpxWNfaaAcg/0pcyFZmNJOzMPmzn0qC7fYuMkCp/s21t5H0qlft1zVohmc7kmq2oS/uwg/iPNSu2Mms+8fLJ9a1itSG9BlvxMK2NQtftem+ao/e24zx3Xv+XWsuJMTrXU6R8pAPToatuzEldHGx9a9V+Gd3IugXcaJ5jRz7gO+CB/hXM3Xg2U7pbO7t9rElYXJDgen/wBeus+H2l3mmQ3y3UW0FkwyMHXv3BIrOq04kxTTO6sZxcQoenOCrDpVqeIDaVRRxk9azonAIzkc1fkmBt+Wx8ua5bGoCMD+6PwJ/rRUSygd80UCPCZOSa6T4cQGTxKr4z5UMj/+O4/rXY+Ffg/qGpw/bNauo9Osl5K43SMPr91R7scfWu0GjaBoOjSW+ji2N0SPMdZWd9vudoXrjox9gK7XJEwi7nFeIz5iorZ27h1HvVrxlarY+GftCOMxsMxkfeDArx+dGsW7GPGSeMj2rX8W2sV38PHnhRpGdFZgvO0gjP8AI10UbOEkKt8SZwmgwf8AEpS3c5bbuHtnn+tZ11G0Eh7YPNatk2YUkQYVQBx6UuqQrPGZozkgcj1964upqtilpt/5UgEhJX0zXaWF7H5KEEk5x+fvXm7DBrT0vVWtsIxyOmamUblRdj062uwzDDDaRxz0q0Lwo3H8XAJrz6LWPnIV1/KrLaoWjH74gdSAc4rHkZqpHY3WpqMJ0+b6d6oXWoDLLluB/Ea5OTViCpUnpwRVGfUSVIZydx55xTUWHMbdzegs5/h9+9YWo3O7dk9AO9Zd9qRI+Q8D3rKutQaQnHfkiqUSHIvXd4FXAxjrXO3Mxdyd2aW4nL5z/OqEsmelbRiZNhI+7pVK6PNWelVpua0juZvYu24yY29RXR6epAFYdmn7mEd//wBVdRpqDAB9KGVA6XRI7a6ZIrqPzDjCgLuOfwBP5Cuv0sWNhLvt1iAA2MA23j0w842/igPtXC2W6N9yHoeCD0qy3iHWopTG+ozts4VnO5sduTzWbjcux3E1ti4VdpWObmB9pIbP8PA5/D8BjpAz+XIYJQVcKcBujfQ9DWZpPiuTyvK1IykE5863VA3/AAJSNrfXhveuiuNa0bUIE+06o3njHztAYifY7Y3yPYk1m4CsZpYYOeP6UVtbdI1O02x3sS3ajCSCVEDH337SSfXB+lFTyisOv9Tu9QYNeXEkpH3VJwq/RRwPwFUmIWOTCgZX19xUbNiRew70pzMzDgZH8q6Dcz9QKmIMuSMdq2vh/dJd2t5pk5Uq6l1DZP1GAR2/rVF0V7NgBkjkZ4rL0G6/svXoLnOFSQFvcdx+WRWtGfLJMyrR5kVdR0tdLurmyjJKRnK7u4IrDMmxmRhkV6b8SNNihuIdQt0wrjEgQ5Xaeh9u/FebapAY33Dp1BHcVnWhyTaIpy5o3MXUYSvzxD5Op9qzhLnrWw5yOeQayb23wd0XTuKhMsabkxnqcdaX+0geC/51RL+ozUEoU9OD6UNIE2X5L09RIPbBqtNeswIMnBqg4xUbEDqaLBcsvcL6k/SommyOOKrtIO3NMZi3FUkTcWSTPSmKvGTTlj9aV+FpgRSNUSxmV1RfvMcCpOtaOgQmS++UZ4x+Z/8A11SJZbtYCJI064XiultowijscVUt7fN9LgdG2j8OK1liKj7p/AUmaRWg+3fy1wRkd6pyzrPMp77cGrT/ACI54xjNWvCfhkaxbPNDrGmJcueLeeUo3sASMVOwypBwfarS9fWrmseG9W0T/kI2csSHpKBuQ/RhxWfECVoGXI/aimRggCigD3bxJb6D4YuGiTRTeyg4ElxdNj/vkAVzd74nmvrV7KLTtMs7eQfN9mt9rHHI+bJPaiipitLhBXV2c7u8stjoQOM/X/Csi8UeaW9DmiirRUjurrN94HhkkJEqwOgfqQFzj+VecRgXVph+vY+lFFbYvaD8jlo7yRgyIA2PXNUrpAoyKKK5DcyruIFSw4NZTOelFFUhELMcc1A54NFFUiRqrmplG3pRRQAueDUEh+YL7ZoopoBpFdn8PrKOWVp35Kk4GPaiitaSvIzlsbGnRDcWPJPJ/Gr8y7eBRRWbOhbGXeOfsdx/1zJqDRVAthxRRSDqdhofijWdHj2WN9IsP/PGT94n/fLZA/CtpfHt0/M+ieH53PV5LEE/zoopcqGS/wDCZSEDydD0CCXr5sdiMj8yR+lFFFLlQWR//9k=</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCACcAMgDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD6AxTSKmxTGFSWRMKjIqZhTGFMCAjFPUUEU5KQEiipVFNUVIBQA5RTsYoUU8CgAXpThzTMbeR0rjfFHxL8O+HLiW3ubrz7qNC7xQfNsH+03Qfic0JN7CuludtTga+ZvEXx91CaaUaVClnbEAq4UPID6ZOV/T+VYcPxs8UQKHXVFumYhnjltETbx0Ujr+VaKlIj2kT63pQa8I8C/HNb24hi8SQRwwyjalxChwG/2hk8fSvarPUrK7wbW6gmBGfkkBqXFx3KUlLY0BSimqacKQC0UUUAGKWjNJTAWiiigQUUUUAZdNapKawqSyIimVMajIoAiI5pyigjmnqKAHqKlUUxRxUgFAMcvFJLIkUbSSsEjUbmYnAAp3SvCP2g/GrNJ/wimnl0JAlvZQ+35cZCfiOT+HvTjHmdiW7K5l/E34r3WqfabXwzdm00+3JR5cgS3TeiDsuAST/+qvEpmkN46KT9oI3ARneGUjJB5wODzS6ncuAIYpY1LR/v8J/qhnAUfgB71uaP4fvrixi3QeXYbw4QqFkk643EAHv0966dIIys5s5fG+78mGBJCQMbn3ckcn5cf/WqW6guoisFxGNmcjYDx+Nesab4IhsCztANzqCvH3fYVYu9BidRmMZQYX2rJ4qCdjZYObVzy+PfpCxCUq0co3GM5+XP49TgVWtX1SS6AsfN8z7y4bHHrXo934dEzl5VDrjAGB8tc/qUDadDJHbx4AGAf4h61pCtGexnOhKG53Pwi+L2o6TqsekeLLl57FyEWWT5mhPY5/u+1fUEUiyRq8bBkYAqwOQQa/PSd2djjLBSSH6Mo9/Wvqb9m/xk+saHLomoT+ZeWIBhLH5miP164PH0IpVYdUTCXRntNFJRWBqLRSUUAOFFIKKYgzRRRQMz8U1h6U+mmpKGEUzFSUw0AyNhT1FIactAXJFFSqKYvNSLQIqaxfwaVpV3f3bbbe2iaVz7AZr4f1e+fU9Sv9SuWlkubmVpmeQ4yDkj6D29hX1L+0BqL2Hw3uo4toa8mjtuT2J3HH4LXytelL6aC1tWCedIqBV6Lzj8cCtqeiuRL3nY6TwF4fTVXXU72EbS5cA9JGz1x6DoPfJr2jR9OiZPmQEe9c9oVpHaWMMMShURQqj2ArrNNcKgBNefOo5zuz1oUlThZFvUrVHt0bAG0Y4rnZ4VFdaxBtiNo6d65q+4Y9qia6lwfQy3QH0x9K53XrBHUv5eSBnI7V0uNze1Ur1d6svrxTpycWRWipR1PEvEgW1vgUVQcEHjhvY12PwFvGtvibo7Q/Kk5eMr7FTkZ9jiq3ibRFdm89tvOd+OgrM+F8n2Px9onlsN638ShuxBcDP5ZFesmpRPFkuWR90ClpF4pa5jYSgUtJQAtFJRQAtFIaKYFKmNTgaRqRQymmnmm9aBMYRTlFBFKtAIlUVIKjWpBSA8S/advxBpmhWrKHWSaWYjPQooAP8A4+a8J8JQC68VW6BMC3QuSfpgfzzXrX7Tkit4h0qJg37uzLBs8AtIBn8lP6V5h8P7V73Wb6Z51jMahQO5zk9q0elNipq9RHsFtGY1UGtO2m8vGK88uo9etN0tlKLiFOSA/P5Grmj+JZJkYXSeXKpwQa8+VJpcydz1o1U3ytWPR11DdHh+lZep3un2oL3lwsY7L1J+grl9S1lzAfJJXI61x7CEXIudWunZM5CKeW/P+dXThzfETUny/Cd5JrcUwYWcDsmeCRyfwqmLqV3xJBInvisW88a6VaWqRWCWiLjgCfLfjhf61Fp/iVbzKgFW6g7sg/Qir9k1rYxdVSVuY0PEVp9r0yZQMtt4xXAeEba50zUI9T2hzYt9pjXpl1PGT6DrXpMDefGwPRhXPQpcpq0NhHCht5m8p89cscH9K6Kc2otHLOCckz6y0G7kv9EsLuZAktxbxyuo7FlBI/Wr9RW0K29vFDH9yNAi/QDFSUjMKbmlJwKhdqAJd4pwYGqZOTTskUDsWiaKr+ZRQFiGijNJmkNiUlLmkzTARqF6UvWhaQiVakFRr0qQUCPmD9pKXzfH6Qb/AJfsUKHvty0rH+lePadcXsMt2NMLgsqs5U4JH+TXffHq9aX4pavtj+SMxoD1LFYV/qaxfhnZx3WpXqykE7VU47f5xW8moU7smmnKdkM1W2uraezTTL1ryGeBJGkwjGNz94Nxlce9dJoelyz3Ej/aDPFG4VXII8weozyPoa6eDwLaSziV2coDnaOBXQi1it2igt0CpGOABXJWxEXGyO+hhpRleTK954ei/seJiuGb868917w/JbXVrPFA93BGQ8sbDIJBzgj0/wDrV7PqUUkNhbnkrtzWVZ3NuLry5cLu7N3rnp1XCR1VaKnE8W1uC3v9f/tKzt5Lbc4kNqU3oGGOnTjjpiug8N+GooN91La/M53bnHJzz24H0FevnRbEnzVRGzzwBWVrESINqjAFdE8RKSsjlhhoxdzlguxvl4FP8NaZLqPjGCREZ4beVJHIIG0FhnqeeFP61HcsEkwD3r1T4f8AgvTVh0zXibgXhQuyb8xs2ThsEZBAx0I6U4aoyqvlZ6RSUUZrQ5hrmqztU0h4NVpDQMcCKUGo+1KpoGiRiBRTD0ooGMHFNZqN1MNACE0gY0hpM0CZKDT0OahBp8ZoEWVNPBqJTUd/cfZNPubkjcIYmkx64GaAPij4kXkl/wCPteuXkDhrufyznoocqvP0Ao+GF4kPieSF8KJYgR7lT/8ArrAuZfMuLgjLeZHn3ySD/Ws6G5m0zVYJ4ziWEjr3/wDrHNdE480XEinLlkpH1ZYXK7eDnisq+1yxsb54bmQLcHqCO3t7VxmgeJn1KK3e3O1G+8xP3fUV1lxpVjq3ly30CyOowGyQR+VeTKPLpM9uM+bWBf1HxrYCyjWVtyooUKtcvrXi3T72WNLKBxKpG0bSCa6BfBmhxbLgRvJHwSrS5jH1/wD11WuhoNpM0lsLJGU8MMCmlHfcLy2RqvfHTVEckoZccGsLVtcDE/MD+NYmtapaXEggM0cryfdVWyf0rAurWS3i3vKTuPCk5xWkKd9zGdS2xuNei5lG096+l/CcRh8NaYh4P2dCfxGa+YvAuly614gtLKEE+a/zEfwqOSfyr6viVY41jQYVQFA9AK6ErHBUbbJM0hNJmmsaogjkaq7NmpJTVegCQNQpyajoBoAn7c0VHuwKKQ7iZprGlpjUDDrSUUlAmKDUsRy1Q1LD96gRYWuc+JdwLXwBr7tIY82ciBh1yw2gfiSB+NdGK4b44XX2b4Z6uQV3SCOMZGerr/TNOO4M+PblXF07R8EpnHTvgVk6mWadfM5bavOeOgrQdkmM0jsQSmBj+9kEn+YrN1EbZE4/hU4B45FdRiavhLXW0m6MUvNrKcMM9PevVYWvbsRPbaj/AKIV/wBXIMgfl1/GvCm+8f0Fdz4F1zYw067k25/1T56e1YVqd/eR14atyuzPTxpGuxR7rS4spopMK2ZCoP1B/wDr1Q1rRvs0af2hqDSTsceXBgLn0yeT+QqG5t9a6W7iSFuRgZFQroOpzSebfTFQRySeQPQVzRklrc9Kc1bRMl0uzsLRna2jUyfxyZz+APpWVrU4klJz8o6Vb1K4t7CEwxuAFHIHeuJ1XW41YhPnfso6D61rTi5O5w1ZKKsTeI7zZp6JDM8U/mBlKNg4wc9PrX0P+zX4ybWvDUujahcyTajp53K0rlmeFjxyeTtPH0Ir5NnneeQyStlj+ldD4E8T3nhPxDbarYn95EcMhPyyIeqn2NdnsrxsedKp73MfepcVGzV4Za/tAWLgfa9IkiH/AEzuN/8ANRWxZ/G7w5cnEkN/D7siEfo2f0rB0proae1i+p6m7E0wmuJs/id4Wu+E1LYfSSF1x+JGK27PxNot6QLbVbKVj/Cs6k/lnNS4tbormT2Zt5pM4qFZlYZVgR6g0/cCKkoeSaKaDkUUASZpjGl+lNY0igopBQTQAuali+8KgFSxH5hQItV4p+1FqSR+F9O03zCjzzmY46bUXHP4uK9pzXy5+03qLXXjBbJpE2Wlsiog67nO5ifw2/lVU17wpbHjsilbUyHG3IAXv/Fn+X61S1HCzKAckIgI99ozV26WRYbeNiMsofHpnNVdWieLUGhcpvBAJX6CukysV1XMnQ5wDjFEjbZMZ79R2qaPmRnc/LnGT3FOaHzJsk5C8DjH1qoq7Jk0tzrfDvji9sLTyLtjKqcBieas6l4/luIysatnHUdq4eZNrY696jdgZBhdvGPrWTw8Oa7RqsVU5bJl6+1O6u2O9yqnsDVGinIuea2iraIwlJvViopNWIULfT+dOiiz978qsDCjitkjCUh8bADDjIoaEj5oCWHpnkU0ZPt9aUAAgg4+lMi5JDJIvIY1p29xcheHbH1rOViWyASfWrtrdtG2WVSo7ZxTQmzbsdV1K0wbeaWI+sbFT+YroLDx54ktMBdSujj/AJ6OX/8AQs1n6Hd2V4NhwJQPuHvWk1nbyybMAUmovdApS6M37P4t69CB5wguP+ukYGf++cUVnQeGxMu5QNuM0VHJT7F+0qdz6WPWmMaeTUZNeaemJmgtSGkzQApNOjb5h9ajNCnmkKxezxXw78S9VXWvHmtXiSFopLmRUb1UHav6CvszxXqX9keGNV1DIBtraSVd3TcFOP1xXwnMvmXwj35yQWcjueT/ADral3ImIVP20I/BB2c9qguiH1K4kQ/KrMwLdSM4H41aSRrjWFMHzEyYTd254zWexD+ax6s3B7e9bdSehYtOFXgAjLgkZzgZFSwe9NVsIVOGLKoB/u+o/SnSN5UXH3jwB71tTWlznqvVIZEvmM7t64FMkg9KsxJsjA/OnjitOXuZc1noURFz05qzHFgZPWpMAcjj1ozzxQkkDk2LQOtGKB2pkDwCfanqopg61J1oELyenFNMZboxp+MUq8GgYkJmtZFkjZgVOQQa7fR9SNzbxysfm6Nj1rkoWB4YZFammSrBNJGudvDUWJe56v4dv1aMAnPGcUVzvhu62yDJ7UVm1qaxlofTNMan1G1eaemNzRRRQAlDHpS01qkDzz9orVhYfDiW3/jvpo4Rz2Hzn/0HH418lGV2knmcfNjP4n/9de+/tVXMvmaBbbj5Aill29i2VGfy/ma+flP7g+pPJ/P/AArppL3TKT1H2JCM8hYqFVunXO04/X+dNEWfJijO4sAT2AJpyYW1uOAc8c9uRUhw0wBHCrx+CnH8q0F0GwfPIzEYGelPYBrhR/d5NFqP3YNLByHbuWOa6YrRI45PVsmpOtL0pBVGYuKOlLRQDE7078qbmhe9AEi808H1pgooAeXAoBJ/+vTYwD8x61KKAHqTWjZyZXn7wrNzVuy5NMTOn0eco3XA70VW0vmPn60UrAf/2Q==</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCADCAMgDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD6poorO17VYdJsWnl5Y8In9400m3ZCbSV2cT4suN+rMeoD4H4Vx2oS+ZdSNnOW61na5rN7d3TvJKVyc7U4AqO1mLw/N1FegrHIk1qy3IcR59aqSvU8jbohiq5QY+Yn6CnqwuN38rVpWyq4qqUHBAq5GQqA1cY6akOXYYFYjn1pfLLIR3XmneYu5gWH50z7VGjcsKd4oPeYgBdSDVeRD15yODSXGoW8Eh3SKB7mqlzrmnx/MbmEA9fnFS5opRkTsgf5WznsarvH1BBBHvWZc+KdLi63KZHpk1XbxjpUq5SbLD0Rv8KylJIfJI1SCOOaa0foa52XxxpQyd0nv+7aoovHmktIFEhBPdkIH51PNEfLI6RgREQ3FJGflFU112CVQ2wMvUHGf60q6xan7w46dDUOUe4KMkdZo1y9rdwTRMQ8bBgR7V71EwlhR1OVdQw+hr5qtNZtNw5wPrXrfhXx7pUlna2dw8ySogTeUypxwOhJpVGpJWM+Vp6ndlaYRT4pEmjWSJw6MMhlOQaGFZJkuJHimkU89aQ1Zk0RMtFPIzRTuSadeffERmbUI1JO1Y8gfWvQGYKpLEADkk15P8R/E2mfbv8AR51nZU2tsPAOT3/wqaLSldnp1k3GyOD1RMSnAyaLTckf7zCjuWOKx9U8SksfKjA98c/nWDcarPMzmWbYijJOcYrdTV/dM+R21O3uNRtYV+eUYH4CsC/8a6XbAhZVkI7Jlv8A61eaa7rjXbGK3YiAHBc9Wrn5roKDt5Pqa6FGyvIORHpd58QwQfs1u5Hq7Bf5ZrPXx1fToQpjT6DJrzwyblyxJNS2sm05DfnSbSY1E7Z/E+oySKTcOB3xgVXn1G7kZg9xK3PdzWGkoKjaTU7zZCMO/Bpuw7F67lM1usm4krwarwTF42jYnjpTbdt25D0YU0J5bZ7g8VnKaWhoole6iYrnJ+Xp71mlnt5OGODz1rYuH3crWbcLnIx9K5nUbepXLYgmnfO9W+oNV3bK5ZAR1OOtOPy8HpTkXKkj8RSUuVCsT6dqlzYsPsU52HnypOQa2F8VSsNjQLHJnucrXMXEBC5HKnnjtUUM5VgswLJ+opO0tSbWO9tdfkH+vhWRP70PDD8D1/OtyG+JijuLCZgWPDLxz6Ef0NedW/nKFe3+YI2SP71db4V3ahqcl1EjpZwoI2Utnc5OSR9P89azY2j6k+DPiCfWtDnju8edbuAcDsc/4GvQWrzn4H6W9p4eur51K/bJvkB7quefzJ/KvRzTv1OWa10IyKQ08im4qkzFoZiin4op3J5Tzb42+I7qwa20y1ZlWWLzZNpxuySAD7cGvE7uQrCbi5mGMFiSeFFez/HLTy32LVI/niAEMhBztwSR/wChN+VeFeJ7K8mjH2SNbiEHc8OdrHHQg9D9Kx5rOx6djmdW112yYf3cf8JYZZvc+lYN9qk9wgWdzt/uDjPuap6rLcLct5kbxcnAcc5qmoJXJ5zXZRkoiauSyTFjyeOwqJ24pCDSxxmRuw+tVKr1FYkjUlQe1P3beByfarccAKCnx2yKc8GsXVvuUo2K8HmZ56ela1uoMZDdetQxqoNSM4XOOcjih1pFKKRLG4ByP4TUkrZJIqunyL296k3joTUSm2UIE3ZH41BLFkVMZVHOcEU2a5hAyzKAfeoBtFCaHPPfoagGYWz27j0q1JeQcgtnscDrUTNuGQjnHBOw09bGd0LIg8vegzGeWX09xWbdQAfMmCvbFXILkRPgHKfyqWaBJFLQspU9QD0ppWDcyxcSfZfJXhc8+pr6T+GHhS41nR9J0y2t44LaGIPdXCxgHLfMcn+JucAe1fNsYMVyDt3AHlfWv0P8B3OnXvhHTLnR4Ugs5oFdY152kjkE9yDkHvkUpR0uK+tjTsrSGxs4bW2QJDCgRFHYCpSMVIRikxUpmbgRUYqTFATPSncz5CIiirAjAHzc0Ucw/Ys+TFwvQt9NxwalhZEV1kDNCcZweQB2Pt71W3UyTDoyt0YEHBrrq0VUREKjizyvxU8F7rVxNDkRljtUdAKzLSL7TcLCHEa9C5GQK0vElsbGYxxhThipbHU9qsabbxW1rGJY1aZuSWHSsl7qsdFy94bfRRbkX9gk0gbAdWY5HPJycdcdMVVmgtJtRhBs1jtFA3sDt34HpnjNTNwoCgADoAKpzp5kilmPHT0pObEo9TO1yz/s66wrLsYblCk/KPQ+9UElkJARmJJwBmt3XvMuIYpLgrtQgEj06Z/lWNIgRWIC7BKVDZ5A+lCloNXHvNc2zASgjPTI60i3rhgSoP40zVVVDC8TuyMDgsm3+XBqK3glnt5poxuWHBf1APehWaux3aLx1FmUjYPzqFr6Vu4GKqcgZwat6bEZ7qOCIfvnYAN/d9aLJD1ZF55eYB2YhjggGukj062aEACOMgZHzksfz4rkl4mGDjDda7Oxd/siDKlgvLKcge/uaUhJXOevopGuiql354+XJ/Qc1ueHtasrZ40u3lt54zxMoOQR0PfPfgisPVLid7giaRyVGMk9feqBhYxecfultvuTUzpqrHlkxNK522mw219Z3L3cKzo8hYPgrjJ9VHFctfRxwXzpaOzw5+QnqPY44zXWWCmG3kMkflqh2cqQBtH94H1NZGq6YIpEniKqrEF1DZAOeceo/WtHNaWJjGxQ0+XyLtJmjWQqeQRnI7gjvnpX2P8As7PBc+DRPaySFVlaN1Zv4+Dkj1wRk9+vufjm8unluW8lFAlwVCjG0g9f58V9s/AfwxceGfAkK36GO9vXN1JGf+WeQAq/XABPucUpydrDUU2mei4pNtLRWBsNK0AYp1FADW5op2KKBNHx8GpCazbG+juZmRHclVyQyEf0q6X4P0r073PPaszktXtUllknlIOJ22r6n/OKyLhiJM+3Fa91JvSdQfmWQuPpnn+lZ0iB156HmuOo25NM7YwShGS6kS3G7HYYpkr80rx4Ax2qKZXHNZXGiZws1s0TdMVn6bpwS5Bnw4z8o681IrEDIyKuaZBLK5ccRr3ou7aDtqUPGPzXVtEmMRR4IAxjnNYtrPJEsiIzKsg2uAeCK1dRgL3c7uxMa989ay4U3SYUU18I3rIsBMxmtvQ7dbK1lv5G/gKoB3JqgkREfSlEsslulp/CjFh7A9f8+9K72GtHcyZl2Sdc9z7VbtrqWF8xsQD1FSagYoiBEME9arR/OSeBzmtb3V2Z9bIsalIJjGy/eIwamW4kNvY2RRHjV/O2qME885/I1c0mOExbpFVnToPX0qxpOn+TI9xLtWRjgIewqLjLEdzF9iEZiljkYMCTyGJOe3AGOKSxMl3G2nyKGaMAocZOO35dKtzQZB3kIB+NVm4kCwjLHjdinFW1kJvoia1I8P69p19HFFNNbt5ipKu5Qyt3HfBr7P8Ahb4sPjPwjBqkkIhnDtDKq/dLLjkexBFfGt9Coa3U87EOPfmvrz4IaQ2j/DfS45VKy3Aa5YEf3zlf/HdtTUnzOyNo0uWnzvqzvKKKKgkKKKKACiiigD4P8J6kNSuLqUReXsVV65znP+Fage9HG+3PzYI+bGM/zxXL/DzizvmB6so/Q/411W9iH8xkbnIwQcV6FPWKbOGekmkc67IXcjqSaURCSBWHBx0qvHIgX7p/GrsTr5KkDjH9azrrS5rR35TLuD5bYcEVFLMjBcNk1duRvJ71mTQYziuRs6OUsWkBnkXdxDn5m/WtTVB5FvshwIwMda5tfPhb9zK65/unFOZ7t1w0zEe9b060YRtYynTlJ3uJJcRhGiOHOMEetJY2mF3GnWlid2SD15Nai28mOAQB04rGzZskVuF4qtNFhg6davSQPnp+dM8rB+ZhjuOtHJIcmjFvx8gJHPaqsZO4YB/CuhmhhZfu7/rVTyDk7VVR6AVqnGK95mbTexPo0Acu88qRRqv8RwSauG+WMFY/nPTd61leQR3PNWIIsd/zpVKylsrChTtuy0tzLJID1Pqea0rEM7gyHJqhCMHhc4rQtj8w28HOKx5tTXlsWLyZbe5WaSMSxwqHZCThwD0455r6r+EfxN03xzYeTFD9jvoFAaAD5SAOq+g9jXytqMMMlpdeZLsmwPLXOC3ynj361V8N38mkxQy27Mt6GLr5bkBOmM4qpLlV+5M6jlaK6H3wrBlypBHqKWvmr4U/F7+ykuLXxI1xPDI/7p1O4q3HygHHFfROl6nZ6raJc6fcRTxMAd0bhsexx0NSJSuXCQBknAHeqrajZKyq11ACzbF+ccn0+tO1FkSxnMs3kJsIMmQNvHXnj86+RfETS2esSyvqwJEvmBrV9wwee4HIPtSclFXYNu9kfYVFeY/C/wCJWlax4fjj1bUoYtSiZkfzjs8zuGHtg/pRTWuw7rqfLVr9ksI/LstkaHkhTnJ/GpPtZKnMgG7twcVnwIhXJA9ql2JxwK6YylY5pJXJhHb44CfjSOqiL5MY5xio41ynzKB7U9lAhOOuc1NRvl1Lp25igxzlepHWo2iJ69atBOS3rTZMBvesEdW5TK4Y8fpQ0nlpzj8qfK+FJrMnczXCRKcbjgmnztbMGkjWsZ2kOegFXbh2WPr29ahiSOFAEHbFNmkzVc7tqwUSqxJOadGuSM/Wmbvmp8bYrO5TRDc5RuOhqC3lDEhuoq/IA35VmXC+Vdbh909RTZC0ZdC5qRYh2/Go4WBHFWBzzSLaCMdQueDVuBfmAz3qOMZqzZRk3Cr6nqTQSzP1TdN4gjheVwhjz8pxjrU+i3BNrcQSokgEpBLD5sDpzXS6jolnBa6lcGaOW7gliAcNGcBo1JAIfOMk9B9fbkLBhHJcknrKaU29jNW3NaPSLTcrKHXncMOeDXpXw78ZX/hDw9eQWT26WxmDtJc732k9h2Ga85hnHlrz2rRha2l06RLq6eGOSWOM7Y1brnkZ6EY9s55NSuZMGk9D1HXvG/iTxLZz6dBLZOt0pZIrcbnK9QFwTnpnmvHvEGjajpQb+1LtdxbiIMWJx6jGOK9Fj8M3Avo7i21y406XaYgbWxih2Lj1R+4JGep71WX4caW90JdS1q5uhnc25AMnucgk+9a2T1aJi0tzhdDsbm+jH2SeBXJzs3ANx35PA+tFdVffD/RVvGNjcahFCBjaI1YH3yzZoppIUnroeeWsoKDmrIfPNYVtb6ptxDE0np8hP8q1NP8AD3iu/cra2E7EYyfIIC59SeB+NbqcYx94ycW9UXRIKSRybiONckOjZx2xg81vWPgC/Eaf27rFrZkctHar50p9ic7B9QT9K7HSdIgttNuNP0q2aT7SpV7i6O+VuMcYAA79BXBXzKhH3Iu78hwVnc8vUfIaqSE/rV6aNoLiWKQFWUkEHsaz5T1rS52lS7fC1SswTL5voeKsXI3HinwqEUKOooRLH3F5tXo30pkd3vHzAr9aJAD2/CoWQADjinYOYm8zrUMl0ekYyf0pNnNJt9BRYGx8N0+PmTn2NOYeYCW6mmKtSqfWixN+4lu235fSrytjp35qnt5yKtRHIwaC7luE1veFrD+0dZt4AxUMclgM4AGa5+M4613nw7j8prm885YCqbAxGevU/wAvzrKtOUKcpRV2kZzlZXOpm+H+8zOt/O0c+DINqEMRwOGX+lZQ+GdnDI7TS3BDnPMKLz+WK6pNe+QCOYzKowXPGfpRbavbXG4mK4iIOC9tKDn6rwa8mlm1VfxIp/gc7fY5+38B6TEuJFll/wB5gP5YqdPB2iRNujtMH/ro/wDjXS6xqVotjb3Yu0aN22MNoRgx9R35yOvGKwL3VXjjDwPa3ETHC7GyentyDXq08bGcOex6+GyipiaaqU5LX1LUOn29suIlCgDAyxbH5miSMY4f8hQkwaNXU4DAGmGXPXNdlzyXGzsyCS3J+6x+uKKc0mc9aKdwNK98RatISjLJDGxIREXBP1NOt9Cv5LdRdTFFl+c5YHr0GBx0H61JoMsOt3zXk0eIrcYWOMERq393nqcdTXYR3ER5GwZ98/8A1q8DGTXN7O+257ea4yCpLDUoKPV2MGz0PSrZkEscs7ZzwDz9TWmt3Bp8ckkSRRJEpZmUA4HscdfSnXZDYcEIDwGJ6D6Z6muD+J2tw6XpS2Vu4Msq+awPp0UHHqef+AiuKMeeShE8nA0PrFaMHt19DzHxfcJd69eXcYA86VmbAxhj1rm5utTRStIrBiW3cjJzk1HMCcGvoIaKx6OMpKnVdlZPYpkfNUSt1P4U+fI9aqi4WNvnOB9K1RwvctAbuaRucVWbUrVPuvuqM6hG2NuPxNAEwP739KXvUAuY8FgRUJvwGPzLTEX1BJ5FDkqpyeKzxqQ3cKWPtTmu5bj5VQKB1zQBehf5uSPw71dj7VmW5IIz1rThxigaLMfNdtozrb6bCY2BJG4n3rgrqcW1sz55AwB79q6HwpcGbRAN3zRMV/A13YOCbbZy4p6JHQSTxsA8YbGeVz901ds9VW3jIEZZ275Ofx9R9a53zWgl3EEr0I9RVsSsUwhJQ85HcV8/m+B+rT54/C/w8jGnK5s6rrL3OhzQ3G0CNvNRSMrwen0wWrnIt8N6t1bSFY5Thoyfut7dsZGPpU1wN9vMoPDxsOfpXJreu1uE3kFRxx0x/hU5fFTpSifR5PiXTTi+57H8PLi1Jv7fVIzPGAs8W1iGVTkNj6HHHTmuyvPDNpcRLPpN/mNhkJOMf+PDv9QK8T8N679jvra9PMbApKo7huD+GcH8K6vT/GVxZzOm+Py92Nhdf8a93CxVamm91ocGbUnQxLcdnqvmbmpWN1p7bbm2kXPRjyG+hHBord0jxHBeQDdIAr8NFKMq1FaPDyvoecqvcW2hTStPt7WWYFgvzueSx7n/AA9sVlX+rhpNsRCqowo6ACsm91h5GJYKfUnmsm6vXkPJGPYYr4Zz1u9yp1HUk5y6mrca3MANvykHknqa8u8Z6nLf65dGVyyKwVQTxwB2rrzMWYZ9a841SbOqXY5/1rDj612Zerzb8j1Mp/iNvsCOEOc596vXUBjiikx8kqBh7HuKxnfMhx2FdNtL6Dag/e8vIr38JQ9q5LyO/OK6jTgvM524qk1tuPPOavMwkUsvPOCPQ0wAjHGfWizWjPIeuplTWiRv8yDaf0qKTT1I3RNxW4yq4+YA1SltgMlHK+1MVjKNljqwpfsWDyRVpoWPO7NKtvu+89AiNI1BCxDLetXoYBGgHelhVY1+UfjT8ncMdKADbjFWoSdvvUQ7VV1K8+zx7Iz+9bp/sj1oW4XItWufPuBEnKRnn3NdN4Jmws0J6MOK4yBeK6fwu3lXX1FelhtDlrao7JLVpo2KqTjrxVaGUwExNnaTx7VcjvJLVsocxP8AMV96p3bxzN5ijBPUV0YihHEU3TnszljpqW1YNg4+tcIx8u4dR/CSv5V2VrKGXYx+YdPcVxl8duqXI9JWHX3NfLYShPDVp0p9D2svkruxesD5lnLGw43EY9iKi2rkfKPypdNbDSj6H+dB4mx74r1sA7VJxO3OI81KlP1Retpprc7raeWIj+63H5UVHFypzRXrHzp3rvluWI/WkIzyMD61Cju4IzgKM8USLt2oSSx5LelflbcmdCikO2YdeOuT0rzHVONTu89RM/8A6Ea9OjV0Cb+5IHPtXmGtDGqXn/XeT/0I17GVL3pX7HoZd8TKqNmYj1GK7iSPy9Ntl9I1/UVw1mhkvo1Hc/nXoOsvHbQkyOFRFAyfYYr63L42vIjNajk4w7HD3pNpcuwB2E8j/P8AnmpFZXUMhyrc1UvNTgubnYFKxHguf0NVFlewucP80LdcfzFRiYqT54HJSbS5ZGqTio2OakyrJuUggjIIqFziuM3IWUg0cUr03qcUCJFP1p6jJoiXPSieRbeMsevYetMRHd3It48Dlz0HpWQQWk3OcseSamQNcSmRjnvTzCxfgVvThpdkSlrYIRkit/S/3cwPvWZaW7b+VPFegfD7wp/wkl1NCJmt3VCYzs3BjkcdRzjP5VdXFU8HSdas7RRnyOb5Yiw/vrfH8S8iqxGDXU694S1DwxcqlwUmiIyJIs8D/aB5H8vesO7typ3KODXZhcbQxcPaUJKSOedKVN2kjNZirBhng1zOqBv7SmLAjexce4NdTItZ2qWgnhyB+8Xlff2oxNBVFzpao3wdZUqmuzMzT2/0hh6p/UU+Q/6QR71BYti6/wCAc+9SD5rxx7152E0rteR9BmKTwkX2Zfj4Wio5GxgDtRXrnzB2EbMrEH/9dWJ3Z8OuQMYNQxkDPt+AqWSSPbgHII5xX5cbdmPUjcu1tw9/oa8413/kK3f/AF1PevQR8m1lPBP9K8/1wf8AE2uh/t//AF69bKvja8j0cA/efoHhmDztYi9Byaf4/vzNqEkEbfuonIOO5qx4ZIt1u7s8eXH8p9+3865ucm5Esjcs2TX07qezopLqVKl7evJ9l+JRVQw4q3CyzxiCThh90/0qtCMVO8OfmWtYLSzPPlrqLDPJaNsYEp6VZ+1wv/Fg/wC1xTVxeRhDgTqOD/eqm0YYYODWU6Wt0VGfRmiGBHDA/jQWVR8zAe5rDmjaJvbsaburnatozS9zXa9ROI/m9+1U2d7iYAkkmqu7NadhBtIJ+8a0pw52TJ2Rchg2qNop6Jhvm/KrcYxH9BT4IAFaWXhBz7mu+yirsxScnZEmn2rzMEjBLucAAcmvqz4DeFp9D0e6kv0RLiZ0wjDLBdgYfQ/OeK+Z/AN2X8caE8i7YY72KTy1OM7WB5Prx/OvtTw/Mo+1D7v71V5BycRIP6GvnMzxdOdaFCbtHf1OxUJU1d7m1NbxTptniSRe4Zcg15h45+FVvqCyXXh8R285yTbNxGx/2T/Cfbp9K9SVw3Q0O21T3x2rsi4Q/eQ081/Wpm1fRnxv4h0G+0S5MGqWc1q+ePMXAb6N0P4VhTKAcEV9aeILmK/voLSWNTJF5jFWj3ZUxPggH+VfIHjm7e28a65HaYjt0vZljjUAKqhyAAPSnluerFylBrRdV1+RLwLl8LM+6tjFeiVRhGBB9jVe15vJCfX+lTwag1xujkRckdRVaE7ZZzXZHkeK5oPdHoVXUWBUKi1TLBO5qKiRqK9I8U7NziPii05kGaKK/MXuU+hauBjZjjn+hrz/AMRHGsXOP88LRRXrZd/FfoejgPifoS2v/Iv3/wDvVh2v3D9TRRX0GJ+CB2YX+NMq/wAVW4/9WKKK7InjshTi4Ujg7h0p7ACVsAdaKKb3IK9+B5Z4rNoorkrfEbQ2Jbf/AFy/Wt22+8KKK2w2zIqGtGB5Z47U6Yk2dxyeN2PbiiijHfwfmjsyn/ePkyTwUSPE+nYJ++K+zPCrM0N2WJJ+2TDk9geKKK+A4h/3in6fqddb4jrFJ2jk0+YkR8E0UV9LS/hP0PP6nEa+7DUJGDMGFrKQc8j5TXx34wOfFOrk8n7ZLz/wM0UV4nDnx1PV/md9Pcoad/rX+n9ad/z8fWiivrsN/Hfob5h/ua9R0PaiiivXPmz/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAC5AMgDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD6fC07FIKWvPEKBS4oFKKoYUtGKKdhhS0UjEKpLHAppDFxVa+vIbOEvM6rwcAnGa4fx18RLHRQ9naShr5SOSuVXnoeRXhHjP4hX+szJ50oTyiQAp+VvWqW+gj3m++JWmwsTC0cgHG3fgn19qfoXxDstWZxGNm0cZYc/rXyjDqMo2kSfe/vNjA6VctNZliDBZSJBgnae49+/wDKm4sR9bW3jXSpVIlmVHB243A5PtXRW9zDPErwyI6EZBVs5r49fX4nto44nZJ2Yeb8xKnjk5/Oug0nxbqGm7HW6VY0jwoz0z3GevPr9KNeoz6o60V5P4c+KkVxdxx6jGI7d0GJQ38WOeK9RsruG8t457dw8UgDKQc5qbAT0YoxRilYY000ipMUhFJxER4pKkxSYqeUQgFAApaKoQ7FFJmiqGMFKKMUorNIQuKWiiqRQtFApa0QCV5D8ZfiCdHjfS9MmAuWwJWQ/Mg9vevQfG2qnRvDt1dqV3IuVDHGa+P9Tkutf1iQwCW5unfexxnmlpsNK5BqmsNKwN0xlckk5OP88cVgS3MtzdMAjOJGyQmeOa9J0j4ayyt5usZwcYjB5GK7DTfCOn2CgRW6g5zkjmsZ4qMdI6m0MPKWr0PEW0y7dt628rJj5SQR/k06HTLxExtdH64Knn0r6Kh0yIKAIlGPap00WOXbmFWCgEHHQ1j9cl2NPq0e587TaJeQSLIsL4lXGOlPhkmtk8q5huCm3GTkbTnIPHb29+9fRbaMuPnt8geoqhqXhm3nQmS3VieCw4pxxc+qB4eL2Z4GdWfesaO/lRglcjGPf9BXo3gXxxdaDcQsLmVrWUqHjYYVRyCff8s1b1v4bxXW6S0zFJgDPUEVxep+F9U0JJJpImliUYBA3Y55P6muiNaE/IxnRlE+s/CviG18QWImtZFd14dQc7TjNblfJXw68Zy6Rr0LKzRQkmNkPRVJ4z9Oa+r7G4ju7SGeGRZI5FDKynINarszImxRS0U7ANxTcU+kxUNANxRinUmKkQw0U4iigBKdiiiiwBRS0UWGFKeASaKxvF2rRaNodzczFh8pVAvUtjir2VwPEPjp4omuZv7KjZzBv3cd+cVufD/wna6NoVvPNEGvpU3yO3UZ7V5eb251/wATwpLsuEd0bcRjaQc/4/WvebmXZZoB1CjH1rlrSsrHRSiZ8wDyHj5R6CkRUD5Kk4GelVhK5Y7eOe/SnRvKTxj1PFci3Oq1kam1PlAQc4Iz3rXtYsLufByMj61z9s7hgXGWB9a001DYv7zGQOVx0rWNrmUhi30d3cSKoYeWSrAjGDmmyFRtJwce3Wo7i9V48xJlucAg8fnVVbqSVcbCvtntTdiVcmkdQWxg47CoZUiuVZHVWU9QaimLk8quO3NRhsdgD9azfkaHlfxQ8JrpLLq+moFhJxMoHT0Nel/ArxjFcaUmlajcqLrf+4Q9duOn6U/VoU1DSp7ScblkTb/9evFtNNxofiQRG4+zhHBSUDJXB6/5z1rsozurdjmqws7n2TRWL4Q1BdS0C1nWZZm27XcZ5I+vNbVdN7mIlFFFIBKKWkqWgEzRRRSELS0UVaQwopaKdgCvL/jlJLJo9taxlQkkhyxbGCB1PtjNeoV5N8doXksrYwTokoyApOCckcilPYDzX4X6RJLcNfzplFcqjY49/wCVeqzOPLCselZ3hDTms/C1nniWSNWbjuRV2fZESZ3C85wT0rzqru2ztp7IpO5EmBgAUu8s6gFBk8YP9ar3l/axqAZUPOM5qhNqcRG8TRnHAAaubmOm1zpo95lHlgZCnqOPbHr0qyLWOVl3EEqAMnvXHW+rBZcCQr9e369Kv2urCVmBYsvUcVaqIh0XudF5CBimzaqimgxrCypw2Ouen1rlb3XZIxgb2bruz8u3H8+n5VWl8QxwFTPMFjYYC5yAeaHUQKk2dTKSA20bjjOBzVRonX7qgA+prkJvHml2zNm4D7RjCDqaqyfEOyeQbVlG3uTxTXM9kD5V1O0MhHBHavPvHUYstWtL0IgXPzMVDAc9cHjtXQWPiq11G6jilTyVflXJ4p/i7T1u9CvEfJMcZdSvUgc1tTbjJXMaiumdb8D9WW8sLyEyh5d4cbWJAGPfpXqQrw39nS4BF5bxmQRqu4buhyT0r3Ou+JxCUUUUwCiiigBMUUtFJpALRRRVAFFFFMArzv4zJCNEhmn4RHwW25AB7/h6V6JXL/Eayiv/AAvdwzpuTHQnAz061M9gOe88QaLayRrwsCMF+q8V414n1PUL2+ked5CCSFij6CvUdYm8jw/pyuGG6BAcHoNoFYNza21pZQ+UPMuLk4jQfecgZOB+Z9hXny0Z2wV0eSS2+pysxPmMvbgn9KxZLi+ikw0+yVCSVY45r1C81XSdMfytW1e0tG34aNf3rj1yAQM/nXE+Jr3StVmc6ZrFtc/3FeHYSPwNVGbavYfs1zWItH1+/tztlcuoAPJzz9a7jTb2WSx8xMlnbBPtXmWn20rO6SqVKjIxyK9T8Gae1zaxxyzFU7KoyRXNWSTOuGkRk95MbUtGpdepJHb6Vwup3E0+FV28tTwCeleu674fjsrdhbXL/MvR+mfwrx/WNLuVuXEalsHkL/OlBWkO/NEzobNrqbyrWJ5nJyewz7muptvCV6UHm7YxjJ2kk4/KsOwvLPS0MmpXUrIBnyYW25Pplef1rrofGvhLUGW2tbHWYrsAKpiMhJb04Y5/Guq8rXicskr2ZVOkT6coYMSM5AAyK73wzP8AbtMaCR9/BXOf4SMdK5K61CIyBILz7bau2w712zQtgkBhgcceldD4LRort1xgMjHp0xUK7eo5JcrsdJ8AbB41ubl42EcijYSScDuOfpXtFef/AAbsXtvC8Ty53SfMDjHHavQK9GK0POExRS0lNgFFFFTsAUUUUgClooqwCiiimAlZ+vWR1DSbi2UqpkXALLuA/DvWhR2pbgeRaxaGLQdPt3IdoEEW4DrgY7/SuY1LwzNq1vIxvZrVlhaNJI2wQDzj9Ocdq6vQrttf8P8AmzfNMt7cRSHpgrIw/lipbm3CRGJR1/WvOm2pXO6nrHlZ5Jqtqr6Rptkmh6WL6wbK3AQlJ+MEydWyev3jyPpjkdI8Jw2s0ytdWVxNPH5ccMUbyCIZ56jkjjmvX9Q8O2t1IWZSx9AK0NE8LJagllSFW5ODliPc0vrDUeUv2S5uZHmuj+GbzTle1WczQyD95GyDEZHo2Sf/ANVegeDbKO0j3SAu7n8h2rXubMSEi0Krbjh9vU1qaRpOxNxiwTjrzXJVlKUtjpglGOrK+uww3Fiw25AHNeatpM89rcxI0g3fupDGdrlPTOK9nuNOZ4SpTqMZx1rkLm0ksbotGoDnqOxFCclK7QtHGx43ceFLfT9Nu7W6+0iCcgLKIt5BHIyQevtitDwlGuh6r9vstRhup1U4eS3CsxIwWclzk4z6e9ewx2lnrMIGwJcKuNyj73HIPrWY3hW2gmJaLnoCuMdfeuuNSVmu5ztJu76HD6Zo0d/rNxqF27T3Mp3F2A5P4dsYrs9Ot1ivFG3G5WDf98mtODT4LVSVVcr9Ki+We/hWP5Gc7M4x14pJ3YpP3Wel+D7BdO8O2UK5/wBWDz781tU2NBHGqL0UACnV6iVtDzwooooASiiioYBRRRSAWiiirAKKKKoBKKWipA8k8GWMmnHxBanp/bNw6r6KQuMfkTUmpTSxzJwWLPtP+yMV0N/ZfYfEt/IpIW7RZlGOAQNp/XB/GuS1W53XYPPcL6V51VW0O2k+ZmpatHDHvm2scZY1Ue/l1e8OnWb+UgXe74+6OnHuaw729aO3OG4PvxxVVLq50zRJLqHd5sjZ46n8657NnWopbncWdtbabDkyCRgcAelX4NV2DGB+NfLGr+NPEI1RyuvTwfPxH5A2qB+FdJ4W+LjNi11hkL87Z1TaG+o7U3SqJc0QfLflZ9C3XiB5YWyoDAcBaxrSaPUVaK5O1+SGz0ryfXPitYWFqWtyJ534VFOQPrXDnxx4gu5hP/bkVlCx4jWEYX88n86qMKk1eQcsI6RPd9TsZtDvVvbWYNBu/ep6Z7j+tdHbahDeQo3AOOfevO/h1rF34iVYb+eO5iUENKgwrkD0rYaOSwvCiuwiDcds0LmW4pRjexr6l8mWG0R9eBjHr+tUtPQnVrQA5DSqAfxpk0zTwjeR97sa1PCtqLnVLUcDbJuyT2BBx+hq6a5pGNX3Ynq9FFBr1DzgopKKSYC0UUUwEopaKmwBRRRVAFFFFACGjNBoqW7AYviaKZoopoSuyIN5gPXB6EV5RrzMJsoDj8q9qvovPs54v76Ff0rxfVYg0v7wZ+baQetctdXdzooSszBsD9tkBbd5OfmOOta+qXcIsCJlQQBQetUJ3is4yE2rzyCuNvTNZGmxR65czm4maK3hPzuDy/b865nE6uZnKXyafqM25LESFiVQsclsY5x2Jz+lUrnwNYTLvEk8DgbQqxFgWJ6A+nI/WvV7S3sbVPLtoIlUHh5BvY/0ArTtb6zT5JUgkQ8sNoU5+oFWpyWwOm2eI2/w9iEjNLMbjyycoi43e2eec/54rXTw9Y29qcWUJbKlflJ29ufrxXrcV5Yxq4tYILfd6jeT+J/wrNuhZS+Ys1vC4fhjGShP5Gq9o2tReyZneDLyxs4QLONIpDwY17Y68mt/UJI5F8z5SSACfUf/AK65LWdHjjDXekzYkABMTHbjGPT6U7S9ZL27iYlmYZ+UZPU8n0H+FQ9dg1juaa3LfL7/AC56/T/PtXoHw1tEmlnmkBPkkMpPqc/0zXmMZZvUknjb0/8Ar17J8NbYw6CZmGDO+R7gDH+NbUI+8ZV5XidbRRRXccYlFLRU2AKKKKACiiigAooopgFFFFIAptONNNJsArzTxfp32TVHIT93L+8Q/wAxXpVY3iy2in0h2k4eMgo3oen5VlVjzLQunLlkeBeKRMt1Md27JJVc9KwdI8I6neh5E1ea08xgfKRAVP5966nxIF/tEKwwx4AbjBot7nbEpBYbRwV71xuTijtjZsRPAzsIxN4g1GNAPnI2D/2Xit+1+FtlHEssniHU2VsE7JFJP4ba5q88Umyl8u+V2Q8Bl5zVWb4o6LaMsUpuA6kqoWInn8KqN5dLmntHFWTsdsvgLSDG/wDxUGqqE6kyoAP/ABysC78IwRyn7Jr+oyx8/K2zHtztyawZvi5pW3ZGl3KEOMiEDGeO59qgj8bNqLRrZW7orkKGkPTPtTaaWqDn5nuWLzweZ5X87W9QCsPuoyqf0FVrPSp9NYRSTNMg+6zY3cV0Mcv2a3LzPucDJYmsu/1CHhi6ntgYyM8c1MZNkzsdFoNi97PDEnzyOwXr3r3fT7VLKyhtovuRIFHv715d8IVikvtxUllhLKWxwSQP5Zr1muyhGy5jjrSu7BRRRWxiFFFFIAooopgFFFFIAopM0UXAWkoqC6u4LRN9xIqL7nrQBOaQ1zk3iQTsUsI8j/npJ0/AVl3upSz7hPOSqnnBwKrkbEdTdapaWwO+QMR2XmsG81T+14ry3EeyCMBSe5JBrlzqsTXTgsixoAY0zlmY+3etTS8fYLuVVZTLLuIbrnaP8KvkSQ1ueTeOxOoDwFjNG2xlzwx6f5+veuJs9cubK5aKaRy2/aN3OeSCAO3I5+lexeIbdkvIruFN8kUiOEI4YqQRmuI8ZeBnury3bSBiYsXVg27cCpIUDuflb6nJrjnSUdGbObTuiSYadqFmZJWLMuQQOtcPrPhpftA1C3kDIApRWHzZPQ/1roFtrnS1hgZyTPG08m9sDhsDPtn6kkmsObUIvOiikkwmCST94A+v4H9K5oxnB6GznGa1KB8MLBHH/pe5lGOB8p3cV1FlplnpzLFGWLGRcEtnJ4yPxOcVgXupxLE8YcFpPmGG6Dqf5VpW0F3fXUKpGzSJtYkA9M45/nz6VpaUtyXJR2LGvaleQjaMrGA3zfw5GRjP5j6j8azbfTbubUYmDSNarhnPXZ8uSAe3JArvfCPhL7cvmaqy+QrBvn5LjcSTg/7+N34+9TeVHJ9j0+GJFdQWkUMWwRx+QwcdOvStIpRVorUyTdSWp23w5MlvBLcRALKV+QEcEeld/puvxXCAXC+W59OQa43QF+zrEkeAq8U6adEZREVUqSSGODx7V3QglHlM5yu7npEM0cy5idXHsakrhLW6BVZY2Kt3ZT0/EVpw67PCVEmJlPQHhvzpOBNzqKKoWeqW13gK2yQ/wPwavVm0MWiiigAoooosAxmCLliFHqTiqFzq9tCDtYyH/Z6fnXH6hrk1wT5aSynOOfkA/A8/pVB5rqVSs0iRI3URsN35/wD1hTVNdQOmvvEMmMIyxL+v51yt9q0TzljOJWzhgCWP6U1oID/yz37Rgbn3H9aQxuEJMON3oD/SrVkBLHdSPHst1EYP/LR+/wBB/jUC+Q24tunTPO5txz9Og/KlwccKkfuTtNMMG5N2VDZzkPyf5UxFiEwpEWijGGBwRz+gFaGmHFsynGM7jjjGaxxEFiHQHv7/AEx396sWJMcjKSNrjHpnH9aY0R6sokDDHFYZ1u/0pZnSO2YOuAZcgjaAAFx04GOBXQ3WCDmuU8QRF0PXptpOKe5SMDVdU0rX9P1drJkhu4SrxwO4WViB8xAPQblDjHoTweD5hrLzXck3lxvHudnO7jJPQd+Ppg/lz03iTRPP/fWuYbtPuOpyT9fUe1cq2tT2f7rVYduODIF3If6iuOrCpT1gro6KUKU9JOzMe30/y3Km8COzbQ5DEqufYHB96908IXvh/TdHfz7z7VcunlXErDaArtyRnknBA4GOgzjNeN3ev2UKbo3gYnkbRkmm6Va6prt0HdpLe2IYAHjKkEHP1BPH51FN1aztayNKtCjTV7npmreOr3WJ49O8NFRbYZJrhBlVySDg8FiQB6DgdckHq/C9glpbh2O+ZsFnIwWwP8K57wzokVlAscEe0AY4/nXd2EYRQrjnHy+xrvhTjDY5HK+hsWb7F3f3uDTZwrKSyq3BJyePxqGH5Fbr0PbP5VNGFZFJXC8ADOK0RmxkLxRniParcBlOD+hqSKVypO4yIPwZf6GmPGBIPlG30wTUcMu2ZldgAeAhHT3pMSLwuI8Y835umG4I98Hmtey1m4gVf3hdOwbmsTaswMcoBHuc5/WmLHFENqNJGOx3gAfQdKVhnoFjq0U6gSfu39+hrRBBGQcivMINReN2AeOWP8iD9R/hWxY635bARy+Wf7jng/0/KocBncUVQ0/Uorr5Gwkv90nr9KKm1gPMxOTM+9FYj32gUkTmSQkbz6eWeB+dVpP9d/20pbr/AFh/3TWlhD2uAd37w5HYvkj8gafJIpKqZCOO0lRaD/x7itGH734UhmZNOVGPMm9/nU4qCOSU8iSUjpgqP6GrF91lrDufun/PagDXS53ffQAjqw3D+lRi5/fJJ5hYocgFlP8AWsWz/wBYn0/pWvcf6ofj/OmI3ZHEmCvRulZV5CkjYYEKBVqx/wCPC3+lMn++v4f1oLOY1XTo1heaRlRByXI6D/PftXkniNm1XU1s9FtxcANjdxh29fYD1/yfWPih/wAiXff7if8AoYrybwT01P8A68pP5rVx7iv0M+00WCxkkll+zXcigyOIiFSIZwFBx1JHp2Jr0nwiNL1G3VbKQeYqZeAnDr7+49+lcbo/S7/3h/IUvw//AOR/tP8ArlJ/6CKUWB7RaWwiUAgdPzrRhUZz0449qrQ/6qL/AK5/4VbH3oPp/hTaJJJCwkUKwVs5IJxn/JpyNM4G4vjpwM/rmo5vvH6f1NZ8/wB6T8aSYGj5kiH5JTjOMEg1Axd2ywjJIxl42zxWafuL/ntVzSf4/p/Q1TAttMR1Ur64wg/WqzSlx8qRHnGSrP8Ar0qG3/4+DWhb9BQAkcojCgeXnGQR8oP/ANerRJKEERnI5DHO786oxf8AHsfr/U1bm+5F9KlgaFiSqh4pjGcZAPQH6dvwoqCT/Vt/uj+dFNK4H//Z</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDIyOjEwOjAxIDE2OjMzOjAxADIwMjI6MTA6MDEgMTY6MzM6MDEAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjItMTAtMDFUMTY6MzM6MDE8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCACqAMgDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD0JRikkz5kWPU/yqWCJ5pAkSl3PRQMk1HKrLcorAgjOQe1cp0Eik7uKmU0lrOba4SVVVipzhhkGiSUyzPIQq7jnAGAKQiUU9ajTkVItMQrc0qjNKKs28nkSLIgUkdiMiqvcCuBU9sUWZDKu5AeR6im/eYn1pcqilnICgZJPagBbho1Z3HyR9eT0FZdprVhdXbW8Uw8wdNwwG+lc14g1ptRmNvaEi2Xq3Td7/SuVuLyFZyFkD7eDg9K6Y0tNTNz10PYghZgFBJ9BTCuODXJ+E/FZ3JFdSlsfcl/iH19a68Msih1YMG5BBzms5RcdxppjIzscMRnBzg96W5l86Zn2hcnOFGAKUipo7dXgkYvhxjauOtICi1PitpJkkZBlUG5jmpfKA60okSMH37CncVikYifapIC0Em9G2nHWkllJPyjFV3JPU0h2GzlfmCnOTVUipmqJhSuVYiaqdrGYtQmQD5HG8fXvVqR0QgMwBPTmkkysiSDtwfpUsY6F/LvB6Giorj/AFmRRRcTRo200kEqyROUdehHUVHKzPdq7kkkEknvUiwyGIyhG8sHBbHGahJ/0hR/s1kWOaZVbBPTqTT0dW+6QarXlkl1GySZ2sOcHFLp9jHZxKkZYqvTJzRqBszRwRwQNDMXdh+8UjG001eagWrqWxFmLnzExu27M/N9cUxDVFSAU1RUqincLD7eNPMHnEiM9SBzXD+MNdR2e0gkxbKcO46uR2HtWl4y11dPt/scThZ5B8zZ5Rf8TXAXOlvcPGbidg7jIhReVHYZPf8ACumlC+plOVtDOvtVkmYW1spG8hQq8lj2+prO1KD7ETGw3SqfmdScZ7j8Kl1L7NbXR/s4uRGQBKWySw/iHpz0rEnndywd2bPXJzWt+5BoWd+8bBkYjn1rtvDniy4tMciWH+OJj+oPavLyxU5U4q7Y3xRwe47etCd9GHmj6R0rUrLVLUTWbhv7yH7yH3FWmkKj5R+deJafd3dl5eoaZIwA4OOcf7Lf5/WvUPDGvw69YlwBHcx8SxZ6e49jWU4cupcZXNWQk9TmoGFXJIsWom3py23bnn61SYk1ncuwxhgZPSoGIq1NNJJCkbHKR52jHSqzCpuFiW4Ns6wiBHVgv7wsep9q43xXqd3ZTLFa4AYZ3Y5rsgLcWobc/wBo3fdxxiua8UXkVhsma2Ezk4UntSuM5jSYdQudRhnm811DZJPSu7VN/wAp7riuJtdW1K+voQq7IdwyqLxiu6i++PpRcRSxlcHqvBoqaQbbgjs3NFIZeSeVbdoQ5EJO4r2zUKI0t0ixoXJXI2jJrTudN8q4EEcyTlgMFO+e1WRpl5oEiz7xHJj5ejA+orGUmti1YxWypwRg1f02SyWG4F5HI8hXERU9D71XnEkshd8s7nPTqTQ9tLDJsmjdG64YYNXcQLzUyiprBIVlzcqzR4PCnBzT1VRQBNBaSNatcLt8tW2kZ5rn/F2tPpNmi2+PtM2dpP8ACB3/AFroI3C9BXn3jt2u9cSBMZVVjA7ZPP8AWtKMeaWpM3ZGBYI91cPeXJaZg2Bv+be/9QP8Kg8Qan9lWS0tmzO3E8gPT1Qf1P4eub+rXQ0uxRLc4lIKRHHKju/1Jzj8fQVxT/M1dr0VjBau4yZv3Z5NZMjfMa05WzG/oBUFjpz3TebISlsDgvjlj6L7/wAqVr6Ib0I7KxkvA7/chT70h6A+g9TUGpKttJ5aAqw5I9Pr71tanqKaav2e3VRcKMBAOIP8X/l9enMuxkJLElicknvTaSVkSrvU6Hw3rD28nll8RucMDyPxFdr4YmNnrcN1bttUtsmjzwUPcf4H0HrXlEMsttKJIWw38/rXW6drscpjcHZPn5kC4APqPY+lC1VmD0d0fQkMHnShN6p7scCqsnBIFMsbpbywt7hDlZY1cfiKsX0cUTKIphKCoJIGMH0rifY3Io7l4YZY027ZBhsiqE06JgbgWPapmOeBTbqy+yTYmjCyEZ654pMY+3+zmGUzs4kx+7CjqfeszVbe3uFUzpvUcgVp6fNbxXG65g85MEBQe9U71lK5C456elK4GfEqqMRRhB7CtCH7y59KpEMenFTwHaVzSuMW66bh/Cc0U5WRpGVuvaii4Hovh/RrRbOK4kGZ/vZLfd/CrepWp1W3EYlUAP1x71W0E/ZWkhumXzM4AJ6VasZIJL64bAXHQ561zTqKTikOzV2Ratp1tb6KyxoivEAUkx827P8AM1x17dS3E2+5JaXGMkYrsFn+0a6sRkUwwguuTncen6Zql4t02WVvtsSrsVcPjr9a6FJT1RK93RnKhyakQ1HD5fnIJSVQkbiOwqe6EKXDLauXi7MaRZLGpKlgCVHU46V5/dFZNRvb6Y4jRmAI6gd/0wPxrvUneKCQBsIRkivMfEU/lQJbITn78n19P8+1dOH6syq9Eczql011cySuANx4A6KOwrJlJ7CrdxIF6sopdNgt7pme6ukiiQ/dyNzn0HoPU1vcgXSdLa+DzTgrbpwAM5lb+6v9TVTW9XSzYw2RQzKNoaP7kPsvqff+Z5q/4g1gRxtaae2Pl2M8Ywqr/dT+p78/U8ZNGfRs/SnzJaIXK3qyAvk5Jye9SIwHWo9h/uv+Cml5z91h/wABNLmQ+VluMKy+ppzwFP3kfG3k1HaupcfMM11vh3Thf3XlMAFaNkyemWG3+ufwp7ol6Hp3w3u2ufCNqXOTGzR5+hz/AFrqd8LWjIsLtcZyGHYU2w0Oz0bR7Kys5SyRRgOSMZbufxOakhv49Pdnicbiu05Ga4nK7ujdLQzjuJ+UGrVza5t4pTPvkb7yn+GqM+pcnyUqqpvrwsI/4Rk89Km47GlbSpZzrKHUspyM9KgvruO4kZzyzHJwKwJsnO52JroNKRJLJGC89M0BYqEyt/q48e5qDyJJSwkkwR2Wth0NVXjKzAjv1oEZbQtC4dWOR6mitOaLIopDNuHUGN28wYfNnOaSxndLol5W8pjl+c4GecVB4e08a/HcRRXKw+VyW27iTWBYrepezQRyCXa5QnPGB3FeZKk7ps6lNapHUzahawXzPYys8akYJ9e4rq9K1+2vYfLuBtccMrLxXnyiWzmRWjAKsGLYyBzXZW2pWF3pDwytGkzgjgc57Gt6blCTexnNKSRn+I7W3WWS5geNFLACIfzrM0+6+zXCS7Fk2/wtVC8bZdOgcvtON2c1ca5S4ht4YoFSReCw/iNdHMRYTVbkm1up1izkE7F4HJx+XNec3losszyT5lkc5Ofuj6CvQ9ZhktLaWOQjJXsa4K+l2xnH3m4FPndrIqMVuzn9Rs7NMkqoPsKyma1QcRurZ+9jita8ljSPM7hD2BPJrn7q+iMmFP4EU02aaExlYg7TxVaQktT7eYSZVRTLhjHwRUvQ1WwfKF+bH1qPzIC2DIoNV5ZQeDyKg8mOQ8/zoiKTNZYo9uQFcd1IBBrYspP7JDzxoTayKCccmFueR/s5PPpXJIDBIPKZiBzjNd1oTwX6RRygMkg8uRPUHg10U5uLujlqRUtz1YpJcLHiUEOobg8YqG4to1HAJf69alSPyQsMKcKAox2FSy2dwuH2kiuRyfQdiheAPao8NuY1j4d/U1TsZFF0FkmeKNgQxU1ejElw0luC/POwdzWQRLDcfdIdG6EdCK0TuKxFfqsc8iR7igOAWGCRXT+G2M2lr5jxYU4VR1rE16NZJklE6SFl529qf4fvI7WTyyqlnP3qoGtDopocHiqc8Xy/StaQAjNVJFFUiLFJlyuaKeB1WigRX+zzabZLcx7fKnHG0881k2M8kUjnBBZs5p7O0c6Wsdw08aj5FznB9BViW8jnKQvbi3eLhiRjP+etc7RsW5Lx1DRGQM0gxzyaSOCNbIyPchZwcCPPWsi+QWVxvkk8wkbl7Yqj9uaWTc7fhTdnuCudFpt29jMZXg8wOCBuGM/SrVraNNbvOGVSD92spdWaSGOPaDs6cVPFcTSd9opXHYTXrny4vJdi0zru654BA/rXA3zyCXfGNzA8A9K7TW0X7OshOXAK5Pp/kVxskoDHjJNNMuK0OX1aO6VWaSZRK4zleufc/wBBiufmid2O5iWzwc5wK7a+tzPyBgeuKypYoLXkje3vWinoHs7lbRLR0dWfO4jB96NcUxucetb2lBbgBkAx3PpWZrkW6VgOTjNYuV5WN4wtE42SSXzCBySeOcChlePZtySc7jtztPtzVzYplKkVMsBHv71spGUoXKtvNLb3KEfv4+MnBAz3HPNb/h+9aDUoWBIXdnFUIY1XlutXbREa4Qpwc1SZnJWR9GQXltBapPFiQOAwYc5qaDUEuOS+D/driNPnmtLe2iWPcioBnPSrkbssxb5snuOlc2z0JNbUiy3izWzhXHUiudubiSWZySS2ck1pNKUiZmOS3Q1m6dPtuZIpTxICM471aY0jPmnA+81PtZB5isrDg5rP1aJ4rhwM4zxms+KR0f7x9KpSBxPYbOQTWkbdeKHFc94AuZZtOeK4zuQ8E966d1rQyM6QYcH1oqedMr70UwODivYLa5R4Wy4PBpuqalLLOzDBLd8dKqyxiGzRXg2u3Iamy2zKIljbzHk6KBzXOaksNrPeWk07TqFj/hPep9IW1RXN4jnI+Q81XnhVZIrYI0UxIDbqvx7zLFayjfDEQXaNecUmBbgt3W0W4O0IT0zzViK4VMBv5VJbWq3Vw39nt+4iw21ycE1etkgvJGa6ATC4UCpbKKfiCWOTR4ljjAKMcuOpyK4DcqsWk/CvRtYtQ2i3Gw4KrkYrybVZThiMgVcfeQ1oSalqII2pxj9K5ucSXl1HBG20yNjce3vTpJM8CiBM8qcOO/pVNWNE7nW2j2em2wgjfdhcZzzWBqFyDOXHPpms4/a7aRndxNEegIwRVfUNQmFvmKJQx6MRmsuR3udCnGxDqcYgkS4iYMjEBlzytWYyGjz7VmwSz3S7blUAznIABq4v7tdvUVpr1MXboPLDpnntVnSmY3cY/wBoVSbJ6Vv+C7Q3mvWceM7pBn6Dk/pVoxm9D2+GyiNpHG3ysFAJHriqd7C1qQv8Pr61pRfvWZTkEVJIizwtHKMsvQms2lujG5zt1dbEA2ZUdDWRc3DLJvClSeQa2JISdysMoDis++j+VQ2MqePehGiaGW+nPfxtLO+D2zWBrdu2mo0rjKrzxXU3U4ayUK4Vu2OKy7lUltWScGXdx60JvrsF+iOh8AX6XulpMqlO3IrrWdfWuS8EzQafatDMmBj5Qa3BJvXcOldOj1RzSlZlxhuFFNgbclFKxSZxT2gutQRIH3xRjd83T/69Mt4Iv7Td5G8gx/dK9yK0h5KONvB7kVWvprZVO0gmuW50WKMV5El5PLfxi4LDCkgcYqvY37WjP5AGH65GaRZIZC28H2xUlrDlCFXO6lcLE1tcTAM8e5V6Eir8EkmzdnJ9Kiit22eWhwvfNT26Kqks2COgqGUXdNN1qEptFiLGQFcD0xXmXiOwnsb24tbiNkeNmBBHcV7p4OvtMs7WWSVlW85yWHUe1cP8UpzrEcF8kQVoRsk2jqOxrSnJJ27kO9zxe6fyY2I69qk0qONoG8ycpI3Zxj8ql1KHMw/utyKvrbRm2TcoPGCDWsjSCu7mTf2cqpIySpJ1KhTk1mC2u3tUMi7WXgAnrW3d6dbg5ty8LD+6/H5VSaxlyT9rnY+2P8KlM15CkIp405UZ/pTopDIMchh2NLNbXYHNxME78gfyqC0jMM7biSD61SIloaEK7uOK9P8Ag1pdrLrMl1ellgiTYrD+8c/0z+deXRt82OOte1fDdPK0o2zRhGj2yMx/iL5z+QAq0jnm7nqDeHrZYnktrjdMo3DJGCPT/wCvXN6kkkarOnTuKjhe5EMcjB4zIPu55+hxVy4IlsdoB6VkibWM62jjuopBwJG61zt5p9zb3WJ/mjP3a2ULWqvIPvAdKh1e7W60tJwwDL1Gaq+mhPUzEsI7p1jkO1Rz1q/LawRWrPEgJQcZ71j/ANpQRQiYAvIe2arXPi2NEKCE+hFbRpS5b2IlJXsaUU6z2xmC7XHatTQLz7ZanPBU4NcDBrN3+8W3t2cMcjiuh8GvexyS+fbyKr8jihIUkdtbHD4oqCFLl2BSIj60U7MFsatr8PYY0kWa/md2GAwAG33x3rnfGnhqPQPJuEYy2bEIS5+YN/hxVS+8f6hPcI4aJAq/dUHGfXrXP+JPEWo66yG8mzGnCoOFHvj1rj07HQua+rJ7SeyMuOAPetiK5s0XKgYHeuKsrKS6uooI2+eRgoJOK9D/AOETs7XSYxcXbrcBhvVQTuGOetLkb2K5l1K8bC8z9kj3HufT6mp4tK3Y86UA/wB2Mbv1/wD11esikNqYYI1ig6Ko7+5Pc1p6ZAOXIGB61SppbicuxUt9JtreLz5wVjUZy7ZJ+gGKguXt5/Nt/KRYGTDrtzuznAJ+nP4j0qHxDqZuLsW8R+SL5jzwTWMJnZp3UnYHb8l+XP8A47WsYrcltnnPiHSmsNQe1fJjOXhYjG5c8Gsl5zGvlMOfWuz8cRP9oh3k5iRY1PoVAz/OvOtemkik82NTg9AvatLKRSbjqS3UrIeQfaoFutnsfeqB1Jp+ZcqxGc9jVG6vAmdzFjnGBWbp62NlV0ubE12HHBzWfJP83HU1Rt53YtuUqvYnvT/MAOerdgKqMLESm5GpZHMyD7zMRgete26LfLYwuZycs2AFBY4BPYV414ftv3y3d0wjiV1VSTjcxOABXpenKbeGRnx5hhYsQOB8ucD2H/161Ub6swk+h0pnl+zlVYnau0Y6gjitvQr03di2/IDHj2GMj+dc1vwkhGR8z9f981p+EGzpqDOSAoP/AHyKmS0JRoXOjXTBprZ1nOMbM7T+vFc7f6BqSWUs0y+TEOdpYV28UpjbIq4zR3tu0NzGskTDBVhkGoSSYO58/wB/ZajIW8uUBB2DYrlria9sbpvMyUJ6mvXPHPw+uvLkuvDM7jjLWrPz/wABP9D+dePa0t5ERbXRYOv3lYYIPvXoRqJrQwcWtzsvBvjddOuFhvYo5ICfv46V73pbQXllFcW4UI4yMCvk6SERafHgck5r6M+FF4b3wlbjdygwaicUtUOL7nYbVXqaKV0QLknmisedF2PAJjsXfIcAVe0LTdQ1pgLC0lkizzKRtQf8CPFd9ofgm0jiWXWNty+c+V/APr/e/l9a63ekUSxQhY4kGAqjAFcnJ3OhSt0OP07wfFp+yfUJhLICCscedoPuepq7dTyTzYKMV7YFXNWn3xKM96zbUbpMjoOatKxJbUFpUjQfd4/Grus3g03T9oOJGGBRYxrbQtdXHQDIz3rjtc1Br68Jz8oOBSsA2OYrG0zY+aReT9c/0plvMzWNtEMkuI0fHGdxAP8AM1DffJpfYEh2BPXhDUsSFFg284ljHHsy1aGVdQtX1S1vY5Hwz3G+Bz0VgMbT7H+efavNtYtLixmaO7iaNs4ww4b6Hofwr12ziW4tZEVRJtdw6YyfvE9O/wDnpVOeJ+Ejl3Jn7ko3j+YP5k1CdmarVHh148arhiQPSsyV03cLmvoCbQba7Qx3dtZMJI25W3AOcepJxiuS1bwv4fitY5jpp3BQXEUrjJJwON2KtO5L0Z5QC0jhVzknAArpNE0BgjXOoIY4F6L/ABMfTH9P5V1em6ehJ/s62t7C3X/WShd7lR1+c8fz781PqVxbWUK3V6xjtwwWFSjEuT3+pH6fU50jG+5nOVloVdMsWlmiuLqN7dULRxwbgU6jH1boT6dumB0yIRA3q0DD/wAdrG07SprvUI7nVBAphnzbrCxACnoCD1PH4V0jJiFRkfeCfngVbMkTKu8y9v3knX/fNbfgtP8AiWyHHPnyAfgayIRuMvIH7yX/ANDNb/gxcaU+cf8AHxL0/wB41L2KNkjipoDxxTGGDToutZDJ8O/yqDk+tc74t8BaZ4m+aVWgvQuBdRDk/wC8Oh/n711IIjjzyXPWqlxeyou1CVxTTa2E1c8X1z4SeI4Iv9Dktr1F6KjbG/JuP1rovhM+o6W02kalaTWsqfMBKpXIrtmv593EjfnVqzu5ZD+9bcPQjNXKo2rMSgkT3clzFAXjAkFFQeJDqMmjOuirEZ152Mcbh7HpmipSQ9S1veWQADCiq99MFBweBVocQnFYV+Tu61BZDPJ5kJz2NaulWsP2UTScJngdzisdfuN9K2emlw44+Wk9gMTxRqhf9zGcKOMDtXNQKXkH1qbUiTctmlsP9aKfQCXWIv3MUSq3zROv/fRC/wBasAASW644MhJOfRSf6U3Uf+PyH6R/+jUqNCWmgDEkfN1/3HprYBPD0DXNxOWdlj8xsn05rprq2t4IWcAO+MKzdeazfBKg28+QPvt296uawcW6Y45/rUSKjuYS3kc97ItsQzQ5WQqeAdpGPr8w/Sud1SCW+ljt7Q/MShJ7ABwSf0rQ0mNItV1pYkVF+0scKMDkQ0yx+Wz1KReHWLhh1HDd6uI5PS5R1CVI4DBbJ50cSnbEGAa4dew/2R/ngcw2tjsEmpak9yokt1b7Mx3rEQOij19/WoJ0UeKbIhQClp8pA+7x2q1qEsg8SaVEHcRM0gKZ+UgZxxWy0Odu7HabDNqmoQX7NG+nqFkghePayOONx9+v+emvcR74duMDzlH5kVfRQLO0IAB3ycgenSoGHzN/12X/ANDFK40MtT8r7Ry0khByR1c10fgxf+JbMOeLiTn68/1rn7P7n/A5P/QzXS+C/wDkG3H/AF8v/SjoBrSLUlqoVt7YIHT60klPA/cr9P8AGsyhWy7Ekiqs0G/pU57U4dKQGPJAQ3NT242dKuSjioRQBPHKRRUVFID/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEBLAEsAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADODIAAJKSAAIAAAADODIAAAAAAAAyMDIwOjA3OjIzIDA4OjQ2OjU4ADIwMjA6MDc6MjMgMDg6NDY6NTgAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjAtMDctMjNUMDg6NDY6NTguODIwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwAGBAUGBQQGBgUGBwcGCAoQCgoJCQoUDg8MEBcUGBgXFBYWGh0lHxobIxwWFiAsICMmJykqKRkfLTAtKDAlKCko/9sAQwEHBwcKCAoTCgoTKBoWGigoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgo/8AAEQgAmADIAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A2rpUttTgulZUM/7mRS2N46qcdyD+hrR68d6zGt3C3tuxBRm86EtzjPJH4Nkj6ipdLlM8XmupEpA388ZwOnsev418dKCcObsfUKWti7ig0tJXKaDabTjSUhjaaR1p1NNAxv0pKDRUjE6fnTTTu1NagY1jxUK8mllOOB6VVmukgUlzTi7MLaG/ahVt18sgyn05I/CsDxB4e3J50cjo7HLDrmtbwPP9tu7xivCqoGe3WtjW0AtQO+7+lfSuEa2X+0a2Wh5XPKnieS+55PPpjxnJZiao3EBXua7q4hDA1jXlmDnivm7tM9dWZx0sZxgHAqnLE/Xd+ldFdWZGcCqElvjqK3hVIcDjfEss1rBGsb7S5wSODXPRpjk8n3rp/HEWyG1P+0RXOxrnH+Ne7hZJ0kzzK6fPYAKeqntUiR89KlWOtHIzsRqvtRVhU4oqOYfKfS9yMT25HXJQ/QjP8wK5XQZbyxi0yeb95YXEOJZB/wAs2JJUn2wQM9PyFdBrsjRrAUYqyvvDcHGAR39iah8N+XN4dsoXRSv2dFKnkEFRXkRbVK9tP+HO1r3jXxSYqG1/chbdiTtHyMTkso/qO/8A9ep65JKzNUxpppp5ppFSUMxTWp5FNNIZGRRinUUgEpjU9ulU9Rv7XTrV7i9mSGJf4mPX6eppqLk7IG0tWE3Oa5i9tLhZmdiW3HOc9Ky9T+IiB2SwsGmjzgSO+3P4AH+dZq/EK4Zhv02Nlx0VyP6GutZXiWrqJisdRi7XPVfh1A0Ut0W/iVf610Ouf8eY/wB7+lee+BPH+jm6eO/MljJIAAZBlD/wIdPxArvdWnjn02OaGRZI2YFWQghhjsRXv06UqWWuE90n+Z5spqpi1KOxzcg+XBqjOoPatCQcVUkH86+WZ7KMuaEGs+e1B6CtuRfUVWkjpJFXPNviHAEsbbnnzen4Vy1tHhOldv8AE6IjT7Rh083H6VyFqvyivcwrtQR51dXqjlip/l+tSqvbFP2VTkLlIAnrRVnbxRS5gse6eL43bSZDDy44A6ZzwKi8Iox0qym2lY2t0A3EZPAqx4x3r4bvnizujQSHHXCkM36A0zwe+dDht2OXsybVj67DhT+K7T+Neem1R+Zvf37GtPEJUwSVIOVYdVPrTIZSW8uXAlAzx0Yeo/zxU5qKaESrg5BByGHUH1Fc6a2Zp6D6SoYZ8yGGXiZRn2Yeo/w7VMamUbMaY00w0/rSGpKI6KU1HK4jjZm+6oJNFrjM3X9XTSrYN5bT3Eh2xQp1c/0Hqa4yPw3q/iC4+16u6qxPyIzYVB6KO1dZasLi7aZgvmNxn0HYfSugtIhHzwa+hwGGVNX6nFXfNvscengS0+USSZVeQFXFXv8AhFNORMeQvpn1rrlQE5P6VRvJVRz6e1enUgkrtnPTd3ZI42+8KWo/ewr0GNmaytOurrQJCkbu1mW3SW5OVz/eX0b+fftXdXDLtYD3rltYgDMSMZPU1yVJK3K9ma+zu+ZbnSQ3EdxbpLCwaN1DKR6VE4yf0rE8GzFY7qybnyiHQ/7LdvzB/Ot5xzXzden7Obid9OXNG5Xdc1A61ZZeaY461mizgvicmdGtz28/+hrirUfIOK7r4n8aTaKOMzf0NcVZj5Rx9a9bDu1FHFUV6hOq04L+NSKKXbS5h2IivFFS7aKLhY+gZkSeF42w0cgKMPUHg1y/hpv7P1AWjtkSr5JJ/wCe0I2n8WjCMP8AdNdPPaQTMXeNd5GC4+Vsf7w5rlNS0p7DU2kM0rWd2ybZX+Y21wp/dtnrtP3fyBPNclKzTjfcqemp2FJVXTbv7Xa7mXy5lJSWM/wOOo+np7EVarCSadmaJmXr0UjWEk9uStzbgyxsBk8dRjvkZGPXFXoJRPDHKmdrqGGfenk1R0uUMbm3HBt5SmP9kgMv6N+lVvC3YWzLp9qQ06mGsi0RtWbrspi02QjgsQv05rTasjxMpbR7jHVcH9R/TNXStzq4PYytGnyB9a6i3uCcelecWviDT9PZcl5yWwQnQf4/hXWWGs2txGGjYDIzgnpXuQnKmrsyajPRHT7iy/ex7k4rKv5rGF/317CHPRQ4J/Suc8TaoWh8sFwrccHFc9YX+mWEby3Jd3Of3knmOMgFjgKrHoCcnHQ10LERqe7a7MZUpU9djsZruNnzC6uvqprOu33Lz3rEtb5bi4WW1hfaeAwjYBs/UD+VaN47quWUrx0PX8aw+K9zXZEXhq5RNeMXUyRMo+oIP8ga69q4HTV8udZoWiW8lYoksrD92CD90HjJ/wAa63Svtaxul7JvdRwxHNeXiocz5kbwi0rl1h9ajYcVKeeajbp+FcZRw/xQH/Eptf8Art/7Ka4u0H7sV23xPUnTLTHQTcn8K4+yX5BXp0naijlmvfJlXinbfpUyx0/y6zcjSxWK0VY2UUcwrHvVQXtrDeWstvcpvhlUqy5xkH3HT61PRXKtNhnGMNR0jVJbjzGubcBVuEIG8oOFkGBk8cHvkenI6uKRZUV42DBhkEHrUWpRj7JIVjV8DJUjOR3/ABxWJpBtL26nS3kmV7ZzGYw5XA6g49CCMfT8K6nCNaHMt0ZJuMrHQZO4jHasq3cQ+JbmIf8ALxbJNn0KkqR+orVRdq4zk96xtaV4NY0m8RMpvaCVgOgccZ9Bkfngd6wpr3nHujST0TNomkxxSiisLFoYRVHWIPtOl3cQ6vEwH1wa0DUUo+XgUR0aY2eM2c/mKtpBaLI6FVGflUDgfe2noD09uvar+kaVdfbIZXaNCx5WKTePYfdA645BPeuoj0bTEsxczJ8yrnBPH5dKk0u/soo5Li4ljhZHGyNhg7fXJ6mvabi1YiMWne50F1oUM1uizwiTco3Z9axToFnaXASK7igJOQrld+fUHjmtfVvGWlW1nG2XkOOEj5LGsPTbt9fupJ7uFba1ZSqRE8nkc10rk+wrmb5vtHQ6PodtbQu8hMsmOHlw34cdq5bxPIqOwGABngdKdfahdaHu8qX7RaDnbuyyD+tYusXP2ucHnawyMd+9Y1J7RSsWo7tss6BDDevarLEJPLdmJPYEY49+n5V1sJJA3dQoHTB49f1/KvOtN1G4sLyF7aQKhlRJSVz8h4JHvXpUUQhj2jJPUlupPqa5MTNQjZbsqLvoMbnp9aYw45qVqYwrzTQ4v4lrnSbU9hPj/wAdNcfYrlBXbfEgA6NB6+eP5GuPsF+Qdq7oP90Yte+XESpNlSRrkCpdtYORpYqFOaKtFKKOYLHsyHcoYEEEZBHelrH8Lys2lrbTNmezdrWTjHKHAP4rtP41sHpSkuV2Mk7oa1cfoii08Z6haKMLJCHOO+0jbn6KwH4V2BNcxeW4Pji0cF1Y2cnKnGeQOfUdOD7VpRatKL6omfRo6OobuAXFrJETjeODjOD2P4GpBIhk8sMC+NxGeRTj0rFaO5oV7Cc3FqrONsg+V19GHBH51Oaov/ol8JOkNwQr+z9j+I4/AetW5GVFLMwVVGSScACnOPVdQi+gppjVlQ+ILa41aKxtkklL7t0oGFXAz9fQfjWs1ZtNblnmPiWW5tbyTTzuEYcMCP4kJ4/w/OsO9ax1S6traWfNzIQkcMXMjn09hXpnijSP7SthJAFF3DkoT/EO6n2NeeqtuL5Z57RFvYHB3EYkjYHjnrXrYVwqR13RlUnJaHoPg/4YXHlxTNaW8Ic7lNy5cjK5B2jitLxF4avrayf/AInMUcpRXjSCJU6g9RyeorHt/H4jiH225kwAAVaRiOmPu/SkOrG/VXhTZBj5cLtGPYV6MvYRhZXZhFVnPW1jmpNJl0+OWa+vXvruQ9D91B/dH9TWddSeXGWLZONg7ZxW7rUhRMnqen41zF1ICvJ+UdOa57c2rNHLl0REvFu3qa9ajkE0KyL/ABqHH0PNea6Ho95rVwlvZoM53M7HCqPUn+nftXrOg+FrfRNAJ33DGdsASZ8xpTxyvIVe6gewJ550WWTxkW1pY5auOhh2lIzn600j6065QwztFJwynBAPSmZ5/Gvn5QcW0z0YyUldHJfEZSdJtyO04H6GuTsF+UZrr/iEudHiPPE47+xrlbAfKK3i/wB2T9o0IxkVMFyKSNc9RU2KysaEW2iptvNFFgO5vj/Y+uLftxZXu2G5PaOQcRufQH7p/wCA10Fcz47jlm0+3j81orJpgLp0AJEf07jOM46DntT9DubnTJl0nViWI4tLo4xOg6KfRwO3et3T5qanfU5VK0muhYvJ2XxVp8CSPtNvM0iDoeU2k/kf1rL8TXb2viCw8vCs8Eqbu4UlCT9eMfjWxqTBdb0r1fzVH/fOf6Vx/wASmmbWdEhtiVmlLxhiuQM7T+OADVUUnNLy/wAwm7J+p12ioTG0zD75+U9yPWtM1maf55jjUyBioAOFAA/KtSsaqalqarYpaq8MenztdZ8oLlsdfw9/T3ri/wDhIpNWso7XBikXmR85V8d8/wCeldlrFkNR06e1ZtvmDAPoQcj9QK46fSJ9EhM7CGSGQGOUAltu4YyAR9Pb+dKmuf3O5V1Fcxd8BW5lW71AgeXIxigJHJQHlvxP/oNdaazfD2mw6VpcVtADj7zEnqx61ok1nUacnYFfqMYZ4Nc94m8PpqS/aLbbHfRj5W6CQf3T/Q10TUxvypQnKD5og0mrM8rt49Pun8m5fy3ifEkbHBUj1rp7zXNJ0yz+eSNVQdM8mvN/ieLeTxVi2DwF/laQE/vGycn2GTj3xXORaTK06vLLJIMcFmzivoYQSipTdr9DhdeTbjBXsdRqPiw3s00jgiPdiJB1NbPgbw1qHil5NRug1vo1q376425C+wH8Tew/H3h+Hvw+k8RXj3N9KLTRoBvaaTINwR/Ah/TNe4Wr21tY29/a2gtLO0HlJpKDHnAfxEfmfxPXnf6eHwftGpNaHn18W4Jq+pJpuladpljAJ4gmlyOH08gfvGlxw8h7k/l9BgVqvLcR33+lRJP4jlTYLYH93JF6+xAz+vvih9vdLsPGn2yS+A2wdVsvc+n+fqZXSXS7OaFpJru4jIZ9TRgGXJ+4vp05PQAZ7CvWaULRp/15Hkczqe9V6f1cZPoVpMlwTLPc3EJxLLCoPzk5w46gjPpz19hkXnhq+tZiiCOVggcqsi5Of7ozkjP4+1dTZLN5nkWINyJUyyyXCfOrdXdcEYHAA7857Zmfy9O277OYWdxIsSRn5s9BvG3JUDHAGB+lefictw1e7as+510MfiKVl07HivxBhddIjDqykyqQCMZBB5rk9PXCCvozWtLsNRxp+qLFdW8+Wt5Zcopb2PLlv9pevfPSvM9d+H91ppeTTVlmgU4aKRcSJ7f7Q9MYJBHHWvDxWU1KMb0veX4nsYfMYVHapozlIl4qUDNCrirFvC0rYXk968eMHJ8q3PTckldjRGcUVYvEmhjHkxGU9wp6UV0fU638pl7en3O71DS7TUJraW8iErW7F4w3IBPtUl9Zw3tsYLlAyHn3B7EHsatUhrm5np5BZHIXs1zY6xokGoZkVbsrFddN6tFIu1v9rJX61U+KVpLJplrdWmUuY5tiOoGQWRlXr/tFR+NdB4ugjm0V3mBKQSJOcHBwjAnB+maqahbTX+mX2kTyYuhHugmzjcRyj/UMBn6fjXVTkm4z7b/18zKSavHuXvD93FqGjWd3CFCzwq+Bxgkc/wCFaVcl4FvI/s/2RY1hRw08Ue3GzJ/eR/VHyPoRXWH3rmqx5ZtGsHdJjW6Vma9Hv0e8x1WJnXjPzKMj9QK0mPFV7zm2lH+yf5VlF2kmW1oyPTWJ0+2Zs7miUnPXoOtTnrmobPH2SDb93y1x9MCpic0TXvMcdhM801uVIPQ8dcVJDE0sgRSoJOBuYAfrV2KzeNpHjiivRnyofLmADP3PuF/Ku/A5bXxUk4Ky7vY5MVjaWHi+d69keNeOPDc19pMc8ZMl5YqsU24kuCBwfcEAEH2xWL8O7QeIbw2zyFYFiMkwHXggYHpksP516P450x7iaA6bHIGx5M6LcZ81cFwHIPRgjE55PB9KraR4dPhnUde1Sa1e2Zo44v3MeYAWwSBg+oXP4/Wvr6uDVapFJXPBpYt0YOUnY7TTbj7bawadO0c0tgdunW0Y27iP72ewGMHnjk983v8AS7jUDPYBZ/EaLtuwf9XAnfHv+v16Hn7BfIvrKyt9Rhiklh8ySeSLY0Lu6gfN16grz/eB7Cu4ksTb6daSRSxWuVzMwI8y7O7aF+rZH54OAMV1qXKvZ7eZyyjd+138v19TMTy9Ot5k8PPC8F1n7ZLO+CZMdB3/AAHb/vqtiRLe3s7TT7dtPaKONZb0ScEgex7k+vtTtPUJdM/nWEEdn+8YRLkOxJ43H0PHqduf4qZ9jkuI/N1PS4HmvJPOlaN8DyU5A/E7QPYilbltFCuptybNGK0eaBYriztZHuB511JA+zanZfU8cfnWYl7uDXkMeoW08waO2gC5WJF6kKe/b8aXUFjMKW0kNxp+qai2d8TFyqDt+Xp6mp5DCLmCOW4v43tCqKDwHc/dU49OST/vfSqTV7NaIzs0rp6sbeCIxra/a3gnRVluRP0UEYCArjBJOffntVpxKqQT3Ihjm2+RdKlvIW2kZGSD+P41BJM5vpprhRqGlwLueRE+d5h6AdAOR7Y+ubFlcLLgRG5njluAtxHK2xYzj7v0X07+9KzaugclB8r1OT8W+E47pp5IVWG+jcBmwVEufukggYJ6ZGfU9yPNwr2WoNDPGySqCrKeCDXs0Vso1ZbSW1sZ4o52j8uNsMEdTjd656n3rB8T6At3F9oCSC7jd4g02CWZeq7gOcgbgT33ZJyMeVisujOar0tGvxPUw2OdNexqbPY4SEPJNvP3NuAKKm6KF5B5BGMEUVUE7GsndnbUhp1Ia+MPcILuFbm2lgk+5IhRvoRisC18650G1mU51CxBjYdSzIdrqfrtzj6V0hrgdV1ufQPE1/AnltFeKlxGmM7XAwxxxwcLnn6VtSTd7dNSJ269ShdXSWOs/azKIrS5kNwjKN3lTAYYcdQ6jkdyK72wuXubUTSR+UW58snJX6+/tXlepqdV1BGYusCr5iGJtu1yeOuegHFei+GdOe7s0vrpZWdk2+WBtLsBgtzwBwD39K7HRWJaUNzPm9lrI1evNV71ttpOT2Rj+lSwj9yhB3AjIbGM+9VtUONNusdfKfH5GvMcHGfKzoveNxNKYNplmw7wIf8Ax0VaRS7bVBZuwHWqGhEnRbA/9O8f/oIre0e1WZ5JpRAYowCxlcjvwAO/OD+GO9deEw31nEKn0bMK9b2FFz7F+3iks1+yLMtveyJukSaPckUfc5Hc/wAsfU0ZRbu10LbT/NSCCWOJYv3aKw2rwfXczg+vFW9M1OOT5o7mRbMyEtcSAuWYBHGB9C+M8AgcdRUa6hp0lqJGvCf3UcrAo52lySgGT+JPUn0r72nGFLlhFWt0PkZzqVeabe/UytYtlklvI5rVGgBlPkQkggBIxuJHGdqSKP8A61bFrotxcaTavY37pbzXH2idLgAqATkJz0GCBwOoxnNPUwXIuFttWUyGZbVXcNncRlmIY8gKSAOQOfWtG6vbiaOZYbnT5o7h/s9upfhVHDvxxx+lJvTmix3t7jT1OVuhc3IvbuSXTQLi6SJ5BlmaBcYYYHJJwPTIrpY7sCOBrufSpJomaNNq7cBASWyerAH0xkfXMGmW7LYQxadPpxE84WJUfJMSnJP1zkn65ptvbSXa2aTaZE8jFiWjYD/WOSTj/cUn/gQqo01ZXYp1nd6fgWnguRZ6bpzWFtcwXJ82Y27YKr1GO54/UdakM1ne6hK00F5HYQnYSwwkYTp+BJJ/4DSRyWg1HVNRja4sXt0+zR7gShOew6nn/wBCqWBZY7C1t7fUf9IviDIJhjCAfMQO3H8zS95XkDVOSUBlrfwM0+o3GoTyQYDQjyyNozhQeMnJ5I/3T3qFLyW3a4mtrtL82MJWSNwNzSueff8A2fw71csZLiQR+TdWs0e97p4uOEHCYx2wB1rm7Hbf3llFcbdOvmma5mZB8kgBxz2wcE/40aqyfzHGMZNtdDU2/YrayGn+eQsyPdwH5RvfklifQD9RVjV5ok0/VF1C484x3CyJBb8YJAAHbpg1Bqz3VzaanaXsy2qlFuC6cM+ACT+QA+lWZIZ21LUoLS3jt1+zq/mydSVHf/JqrPmTZN1yPq9ShrFpC99dSLpEqo0KXIk3HcSpA4HrjPerF35EceoiG9urbZsukWZC6j1OPwP51JfXULzaPLdak8iyRvAyw/dY7cduOuak0m6802DtqMDR3FqbcpKNpJXqfWoUVZxNHUlaM7HkfxXivdItYNa0tjNYXB/fSIM7XY7lYg8jcCM+jD3Aor0DWbH+0vDYt72K3kikSS2uZIG6BW3rx3IAOPc57UV59bB1ak+als/M7qWLp048tTQioPtRRXxR9ENbp1rnNe0e51Kz2maJZFk3BSuVYAYAz1B5PPPXpRRVKTV0h2OR8MzpHrWnRKFf7T50b28uB5UsY+ZCcHp1/EHivS73XbeORYVX96MHygMscDnAHWiivWpTdKoox6o4pL2kbyFsVMujTXU4ILzExluCck8dAenqO341VlQSIyN0YbTRRXJmSSqq3ZG+HbcXfuZnhOVrjQrEFcOqeSV91JTH/jtddb3ccVovlwxGOEiV0lX97NjAG30BYtjPbmiivZyKnHnq1Oq0PJzaTcacOjHWdheWeoapIZLOMfZWMcTMdqL1BGPqwP8Auiq4Oorp1zmbTgwt7ZwMtjgc9qKK+iXxJnjczUGh8ZvotW1EjTbOcxrJcI6KDyY0A6/VqfIssOoXUY0Tiz0/YNrgDcwzkAdD2oorN9F5myd5X8hXgto7WzD6ZcW5S3VVkVj8jy8HrgcDJ/CpreWysrea5S7urdlXbDu5Cu4G0YAz8qBOPrRRWjSaZmt16mgsNxDb2Wmy6jaMkY+03E7jJXHP0Hpk+gqRnv7s3N2LSzu5Lhfs9qY2AYx92J7Z60UVi9ErGuju2Y+uzw2ulahDJYy20k8qWEEq85GAPp0z69KNIguRZX3lCK7jVfslrK7fMuxSWB9TkHvRRV+0fM7+Rmqa5E1oRSO17IL+KUXOqTWzwOc/u4doJOfxB/IcVfWW3j1TTri/v2uXu7fa0cZ+UkDJ9s5wO1FFNtzkr9iowVNNRCDzk0xhZaasTWF2rK83XbuwTzz3PrU4t544syWFpN9mviNyYGEY5zk/WiinJ2mzON3SsZ99DBbXlzHNZT2nlX8U4kjfcDv6/h/jRRRUQirHS2f/2Q==</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAC+AOEDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDh9PvHWF1vDExBLbQ29cgEZJznvx25xVq1FsAPtNwqshHyR5wcsBgnkeowR+JrmN8k2nF4XLK7FRvXgHHTj0Az3/Cm2t0sDSJdud2NqlSoK8cg54/qDk147g3qZneGbTVsozpDrDONuHPzmQjtnJCnkE4HGelO06+MFv8AaIpXtsZAjePIzxyoXA4x6DAPHpXDwskMXkczSpufdG+7cmSQTz05P0qTTo7mWa1W2Zg4ckOTuAPp/L17VDpW3Y7nQw6TZJZzyzRB8na+5CVc4JG053A47Z9PrWVcTx2WrtZWriRFA2NL/Ce+cHgD8OOvIrevLu3VUmF20jMTH50bgkr9OcfX0471y2pTQ3UbhYN10rFjKoyxJ6gjOSOvI/ICtaV5asTLEYvYZfNYQSFMSPF94sucZGOcelXJidRt9rQeVEke9pFjJCDPUEflz71U05CI1lSNlA43shIHYjOOCenNXQ2opvtjHE0E2GaSKQqoXuMdiB6en1rS9gOdvYIt2ydt/wAp3KrOpXHccH09xz+Uujve6PM8miX6xzOCNzovQHt154znGMV0On6RHb3E7y7fssZIBfJJX1xtPOD9M+tXtJgtY4lguot9mHkcbnxMrE4yBjg/d6A9etbQr8j0Y3tZljR9XuL9m+2/b8iUFpjISowSwYnaBtB6Dp/T0u3jlEEZlO5sAkjof1NZfhTw7p67Lh0xdAHy545MMqrgFHIPJ789c+1db9jSMDcxJA7cV9Pg5vk5pPc8yvFN2SM9MlcHNSLGp5JY+1Vtb1K10uJvNI3YGAe9eZ6j47u5GKxMExxgHAVu+cdeeP8AOa0qYiMBU6MpHr1u0ZAHmKB04NWVmgiBwNx9a+f28X3ENzG884kRxtZc5GOp+nfn39q2NN8XmFNwnlMKclcA8erf59fSudV4zeps6UorQ9kbU1UfKFBzWddao7McBjUOnbLuFZI2EinoRWrHaArzHxXWo046nM3N6GBJdTMMc59abE9wFICgk9yMmuhks4hjOFPvTUsGzkEAfStPaQS2M+SV9zBjgmdssD+IrUSy/wBFeSd32IpYqvBOO3NbFvYNkEndXG/E7UrrS0htYIGZ7pgqjfjp1AGcnPTp+PSuXFYz2cHJG1LD8zszkPEHiaYzTW1qzRW7najbv3jEEZAweM56/SuNija73JI0zIrfxsAWXtnJyPWm6lO+XMzrHOoKOrA+YCucgjseSO3eoLi7VI1haQbuGI28n2J/Pivkq9apXleTbPUpxjDRIfLF5FzMzo5CgqQM+g+U857/AJVlw3q/aGDlxEwKbRxuGOTj+tRHUgdwl371XaCPbp9fT/8AVUdzPPNbrLNG5jVdobGQT7cZ/H6UlDuXcuRLHKqgjcYz87Y3EZ9MevHp/WrjyRtAyQ4gLkgJI24jgcnPT681SsJYVghO+HLD52Eny/TGMn0yfU03UJnjus2hg8xRhWCKC2ensT/nFS43lYm5a86b/npb/wDf4UVj+Te+k3/gOP8AGir5EFzoJPssFr5gvIndcLlY9wC89xyAMehrN1iziuFjuIGNw3zLIsTNlMd8kbcc8AEnmsC6jjitUUGYOrbvmHc+/wCHUe1Ogv7lTiMykkMDlt2SRyf5flRGDWqCx0Vn4eEdrLJcPLDcMTmMqQ4QA5PUZB5/757VHbwm1BM0qZcEI8O3GCvOccEVeTV4zpqm6ha8LZfOQgD8gg/L2ycDgjjGKk0m0F/AZNOjiWNsLJHIm7YeAWXIII6A/Uc1k5P7QjPhZYblPOO5FYKW2kkEYGPcVtPpNq1nk27pc78YA4Kk/wAOM54ye3Tt0rB1aRbe6t4rYTQNglhIw2Y6fLxx06fSrlneqlurS4BYFkZVJC57Y6fyxTae6A6K1VtLs4njkL24lDIko5HfLDPB4+uKQ3aX9rIkdx5YaQsq7NqN6HJPB69vXmqtrJHfRRedEREwYbnZtvTIPBzx9D/SqQht7C/ld4Y/JADM7Ejacn5QOQegwTULz3GdNLJDawgLKnmAbmZMliMc45OOnrWAmpT3Th4bcMuyR9xcFzhRknHVuMD61kXGom4laGJttsSThskse2T2HocUaI0izvtCtbxLkxS/OdpBOMccYz6VUIWV2xHpHhHVLpLVL60tzfWqutu6sACCcfePfJOR616mbopp7XN1H5YCF+Rg4+h6cYrgfhdpSyaNfTvFPDaPH5YCOW83BJyh79vpiuo8XXz3GkjT4lUzXMO1/N/5Zgj7xA7+nSvdwtT2VLmbMHSdWajFHlPjrxbDchVg2zyY2yZzjPfAB7ZP415ljUp8m1hmdSeGVCK9o03wXZ2zeZP/AKTL2Z1zW6NJiwPkHHQAdK4quNTeh7VHLJJe8fOcml6uWO+2mXBz71bs01Kzhnint5/LdNoLxkhfevoQ6VGp3MimoZLGNc4A69DWccW77Gsst03MT4K+JDLLJp1w2TsLKTznH+TXrVvciSTbuHC7gMZznp/L9a8xm0W1M/2iBTbXoGBPDwfx9azx4v1bw1dpFqSi4g/gcj73rg/05xXo0cUpJI8nE4KVN3PRdU1iQeIbOxtWjdXUmVQRnGcH3GPbOeemK6Jb63s4Y/tW1NxCA5zk15HaeNdOu5p9Uktg9wMLbDBZkzkHHBGPmPT8s16DLeBrC4uZRGiLCDGJXG1eB15wT1H+cVrCtzN6nK4WtoYnj3WTbz2awfaLqzkl3uoT5ByAPmxwNxGPU59K8q8UeIf+EnvnlErIqsMlsjKgYUNg9q1tX1q4s5IWuGtjBICfLEYbyc+n3vXrnOe3euC/jd4IoYpM8MflOOMD3PSvMxNRydrmsEkWNqOxacyPcAlmx0I9x+v4VVvVh2SBTM0shOdz7dw9Md6aLjcAs8glKkbVVunrnj3P61ait4NTuom8u5dFUlzGRhB1BPHA/GuRe7qyjNt5mijTzkMW+QcPzuHIH0GDj8aSwme4vM/aEXfwFJ+UD054HHv6CuguPDqXEnmxzoyoNwVyFJPrwPT6dMGmWukzfahHEInSMMp3qvyLz0OOf1xVe0i1dAUbzT2hux9nMayR8ErwHPtnvU1kLu7mkhjjMiopZsRFmUc+gBAGT37d61rqzFzvnnuolLlsqVZRnHYDkn8Mc81y+uamtldiKyuGWONCCqs2Vf1POMsD24pUmqlkwZa8i8/572//AH9NFZGLT+/ff9+//r0Vv7MLMvQXEFzfzwLBJdQNmTCw/vEUAEtwD0A56dzWc1ussTTWkO6AHBXfvZT247fl2FZVrdXSSN9mupoZHzEQrEblPUEjt7Vsw2d1a2kLTzeVYzQs3mqhXzDuPAYjk9M9O460Kn2LsSRGVY1VJ5Wi2kKIhn8GHGB/9f3pqX7qpfeVUsV8sMT156d+QPxAq1pFnHLLLEnmptkwJk+8BkjOVOD6dSOeM1TvQ1lE9nFg5wzsrAgjdwRx8p/E1k1d2YmjZf7PqmhQxrOElgBZmk5YNzkKc8+49/asWz1BlSVZQ2zOTt9fcHv1qG0n8tnaUAbVPXn8Paqsih5d6ROIm5CvyR6fUdaIw6MSOqhuoJbWTz5NsuOCFJG33x6cc1Vku4zO+xUfzpAN4OwEY569Mk//AKqyoboRxpHGg4/iB2kfXnn/AOtWxbSLdskhyjgjB24Oc9P5n+tRy23AtR2drFp6310sqOH/AHilcY54wOMg+1VdPuUe5CbfKhk+8E4OD355Ix2PX8a1rXT5FikLiGcN+73O2DjpkYPYc8ficVj3ljcwW7+ZsbyyRuVScfQ9T09wKcLbgdd4Z1fWo7o2GjaneiGFvLGWAURbs9CTj8K9NiEk0hlmO6V+T+XFcN8NNMMGjtdzA+dO3VuoUH/9f6V6LaIrbifSorVm/cvoj3MvwyjH2j3Y+OLHWrSwDjAJ79KfCVbpzVtSNw4A4rC56ZSlh9jWfcRAVsXDZHyt+VZly+Gy3r6U0xdDOkQhuvFZ2pabBqlrLbXSgqw4PcH1HvWjJJkk02MZUkjmtoVGmc1SClueNanYT6LffZ3+eKVsZPQnsf8APeuq0PxBFLaXVndzCBJIdrM6edtweNqdiT09P1Gv4q0yG/h2SqD746Z9P5/hXF6nN/ZXlwKzCSM/vA7AiRhnHH58n1rrU/to8HE0vZzsM8RTXzymG8vYzHEQwLuD94cdDxx2OMVy1wkkUiC53IHfEcygtkfmOOtWluUuWlN4kzs5JLjox/AdOOf/ANVXdMUSpLLDLKIyMbXXjj6+lZSnrzHOY9vp960ysqbwedyONuMcdT6Vu6f5tlA0ETCMM24/vFIAwO4/p71Nl1JiW4iIzlwwCEHHrjI9OKytUijtNs0U9uW3YYY83OQeTknHbr19qhvn0Fc0XEuWO8KWclVEpd+vHPrn+XamTai9lMojwsob5i5y2Mdjn/PFVFvvKCmxhiaVwCFABJBHUg/09Kwmafzv38oQ78qjjJ5/QUo07hc6SPxBfSQzMZZpMDPGSR6cDr/PipJPAt5eQ2+s63e6faae5QTLBIHlAP8AdjUcnHYc8H0rO8NefPdP5Np5rAEEoPlz79R/npXVSfZbYeXc3EkZKFVbhctjs3scDp27VcJRpO1hXKv9jD/oFQf9+xRV/wA7RP8Anncf+BMH+FFHO/IrmR5C25LgF/oQO1aEaG7ZIbYO0uOULZ3H2/w/+tVa8EiLtZVToN2cj8+v/wCuoFcyj5MF84xycV0mjN7RdTa1MsIXz4pEx5ZmKDPqMEc4yPxx3qLUr2S5vpGRpTGcbDIoLKB2yOwJP+RVWC3YOplYxDdtBC8HpnAz/hS6lFKjxedG8bQjYf3e05z696nlV7k3GmNzGSAWLAqwI6e9NjeUcFmyoIAYZFSnUQZAxVpDj5mY56fyp8TqGyhLKGBZOM//AKqnW2oEUm4BSyOqdc4yMe1aOlXj203lpGG8wYywOSDj8P0qaNFuVGci3X5QQS3cADH6Zp6xo94jSSrtJ2llwMD6fX/PSs201ZgbrJcacsRWeMqqlinLBc+q9Pyqq0kriKVpGkhYANghh78HP61FcLe20cbPvljYqQWXovbg84Ipr6TN5KS4C2f3g7uMKMkc47dOainZbiPbdEhSLT4VjUKioAB6DFaloGLFVyeMVj2V1HHpFvNKdqtGrevUVUXxnaWcbefgL2x1xXMqcpSbPpo1oU4pM7i1t8Lktk+lTKv7wKQMkZrjdM8c2F4SsDAHHG44rc0vVo7u4nkVhtjQKDnOT3qnDl3NI1oz2NQplTj0zgVnXkJb7vWsjUfE6WViZQVyvykE1xdx8S43uBGg5HcciqjSctjOpiYx0Z2Ukcqy/vMbR0xQZcHGelczH4lup5ElaFzH/FkcYrW+1RXS+ZbnHqD1FN0nHUzVZSE1CTcoI65Feb+PtJnfxLL5UjJbyKJGZzkKSOQAOeo/WvQNSBjhUnOfSuN8ZzW8+pQs8ZysKq7hsKGyep6da6Ifw2eXjt0c9BYTQbkkLCBQcSggkA8dCOpzUd5IY7LOnyTO6squCcEf7Xbvx+NUNUv4kKRwGQkEEK2BlvbAx/8Arq1pNtM0sckskdvvOFXCs2eh4yORx2qLfaZ55nKb67urdGkKwzOMOzgBc929PXmtIQwvcyWMUYit3GS6SJNlwrjh/wC6ScYHXr6VYurbV0OLS68mDyGjw5CiRehGDnrwcZ9SKo6rYy6fuvGupJ5fPXy2WIiM5DHG7AyRtAxxnPFdMeVr3AIrjQ7yCIvDKBctkbFPGz06Dn/CsSSC5Vl+0pN91kVj3PXHPbnnHrWiupatLMXa5ciQklCAW7Z4PIPp3rRvNTnGhyWd6JJd2XxJJs2cHgrt5OSDkn+EdqmCd/eBEOg63Jp1kEhlESIfnQKMtx1JP+R7Vprr0N1Msd3El2rLtG87DyMZBGfyHua4uzcBJACVGMZ9jwRn0OauadfLFI8TMhiUEk+WCOeo6d6zlSi3fqBuf2NZ/wDPjd/9/wBP/iaKqf2rY+sP/fkf/E0VXNIRDIoutNmZSCV7nsABye35e9Q6PZwozzNJuAy2AD/LHv3qOOV4tOuI7ZlKSYIVwCWXnt+FT2d3/Z7/AD71l2GMBMqeMHv649Kck7NI1lsWrqJdUYSOkkccXRh0HA68e3H/ANaq9w9soja6MkssRzsL4RsdiOfX2rQtLvzpgJDHBFI7b3A5dl7EY9DS6npdl9me4hKxvGM4BJ8wHOTycA4/lWSlZqLIXZnMXM0Ml0726BYm/gHQZHOKcZEKfJkHOPvdqqKq4+XOT2x0ppRo8E9M9K6uUo6vR7mU2rxQQ7lkbLZGdx/px/M10PhTSoo5Ve5jcqp3BXTcAAD2744+X3FchoV0I3SN44zE339+W98kA9q6h9UuZbC4aJ0BZsusS4Ug9wfTGR6ceg546sZLRdQH3lu8eoTS2d2kiouREzhSWCjcoXOc9O1WfBN/Dc6vF5qRXquS5tmjHO2N3OTznGBXOOYry4COfLkl4UDLbm7k55B4Bz9af4Oni0nxrZGOZJIzMqJJgnKuMc49Ax/LtTjD3fM1pWU4t7XO08ZeNBFO0elRRw2kJIBdOeOwXpx071wl9401S5X5beCT08yBM/litTWbZIL+9hlX95FcSKAexDGuZuIUZyfNweuMc1004RS2O6rzNmro/i3V7NyVtNMfdwVlsIMj3BCgivXfAuu3d9ppZBE+VLFEgjDqenzEJjOfQcjHQ8Dw+3tN3I3ED+I1778KNE/s/wALtKVInmBLgjpzWWKso3RrhKbcrHA+NPFF9YaiI7aO1mlcFsS26FYxnHK45bI6HIxjIOcDhbnXNW8x547lI5ycnylSEE/7qAD86674k6c8WsSTIjDdgMe2M9fzP8q4e5tdvWMnPdTjNaUUuRMyqxfO0WIfFviFTue7lfHYyE/1xXb+A/F0t7qUVveKN0h2hwuDn0IHFecQx5fAV8+h5ro/DpMOr2G5Qw89Mgj/AGhVzjFx0RMOZPc9f8RbrgLbRNsOR5si87Pb61RutQZrEaRp9uj2cytHNI4JLMR1/DHX2qa6ke4ikhs8eY6HZkAfN26YFWfONn4cS8mRV8qCRyAuMNtx/M1xt2SO2mleTZ4cPLh01bk7jdbyAzSjr6bOvvuz7YquuplZRK8KmUbSuAAOmDkc5refSYJ9jEBGLbiVJJYYPbgDnHvTJWsrUYmgtZegdshgg7cZDdB/Ot3UT0sfPFD+3blY1XYGUkDJc59xkGtC3juJLR3jsyADu+Ynf35B+8Bye/PftSQvZTKY7GFF3MQrSJhQcjHLZPv+netKIrHYs8EsbqWO5bUlx16IPxx+IrJy5fhVhNnMsb+NkxZzqxUH7rfOp/U8VIdYudRsp7cxl8qQ7L2GP8f/AK1dFaRwSR/af7LnWVuDuQ72xgZ2jgDp7Zp8lnCJJLm2sBFuG50YkNyO2QAOh70c66rULnn8W7yXUKd/TjrxntUa25beQshA5J9PWugtdLkv9VZ9Osr4I65QMhYn14HTnpWpY6XsnuYpkZBDO1tN5YzyvVefx/rWzmolbHF7YPQ/9/B/hRXff8IVZ+k3/fB/xope2h3J5jk/Dc8Y80+UW2xnEhOcNkf0zVS6vnhkEgIeZtytu6YPA4qbQ2AnmhZVfAGApzkDOQOR61QtdNvbzVVtrG3kmuHY7Y0XJ/LtWtldtm72I1lZCTuZmJ68nmr9nLcSxmM+Yc/OVyTkDvVq10zULbVGtpo0t7yI7mSYhSuMDjPU+1b/AIhtrqA6e8lsgNxG0qyq4O9OuMA4HB6fSplNXSRKOTQDd0HzcZ6YprAvn26ZFOjkXsD1wFH402O5QtiVGj3f7X69KtXGJa3U1pcCWFyjKD847duP1q1aX1yJZXjn2szM6hflUMe+OADgmmHTxMqeTcoUwSQwIYfgeDntzUUtrM8L+XZvGykbWbO5h6Y6fTA/Oiye4WJpnjCFriN1bqrRyAY9xxW54RsIbnxVpCW8gcNPErqQM8sDk8n6fhXL2Md9ETJBG4XaNxKZBwQcc++KvaJrkuia9pepeUWmtpRI4J4kXOcUNXVkVBrmVz2X4geFprjVLnUbAF2Mh86IcHPZh+H+ea4qS08uURT27rMDjYyHdn6V7TLqCXEqaha/NBcKsq8c4ZQRkevNTvq0cCfLAjTHhcIMk1wwryguVo972UZvmTPN/D/g26upUkvI2tYcbgGHzY9cdvx/+tXr+kW622n7IvljVQoHoBWJBcSQQzPfkC4ufugnt2H+fWtu3uohp7IeHxxionJzd2dNKEYbHIeI9MivFk835pCTjvXn+reEL2yUywQtPb9fk5K/1/z+NemT31vamRrl14bkscCq+lXrXF9cTWkgeFSMhTkH6VcZSpq6Mp04yeu54z9k8ycRJAzTdAoU7q6LR/D0lndLc3vyyLkLF3U+ren06/Tv6xfSWc0WGhjJI5yornTbRSTMFAVQM8VbxHMtjCVDle5V0iNvOZ1wdgxgnB5rW8TBz4NvJSg2xwrGoyAXYuM0zT4VtgodT+9JY47AdP5n8q5fx/4vtbzST4b0+RTcy486T+FMc4zwMnHrTlF2Rh7WMYT5n0OJaa3aZVWdoGJ2FBNzg9h6HmobvQkuuYsxkA5dmOCQcdec8/SptNeS18URrqlsssURVWieHZnHHbOM9T+f17rxGr3EMKaJoHlCST/XKqhTt4I25AIJwATjPHtWUpuEkkeJY8ti0O6iYSJtfO7C7gRjnjPfv0rW0nVLLTtPdIrSJJmOXcy7vm6jjoPSqepLrzLNZ3EUjsxZRCI8PtBx7+n9feqen6DqS3kSXVu1sGzs83GHxgELxgnke3XNbtcy95jsbH/CUqJEjdVjkwVEjvlQee/YDjAx/hUH9ul4SWj+07lwUjDIF98knGc+nbtXRWvgCXX7W2mtJbNVWMrIZNylWPIXGTwOn3R+NcVrulan4P1j7JdpCrSJ5ilGJSReRkH8OhrOHspPljuJR7HTaDf3ccn2uSytXhwdoDvjkAjgEE9DxkdfSuWmnumuhZTCQj7RJcsEP3i6rzxk4GM/SrFjJfWmiQ3kp3W0s5igIAJGM5/w/Hin3lpJNqjQQIk15JGyssK53P5jKNp6k4wc98c960iuVu5ST2J991/zyP8A3wf8KKd/whmp/wDQMuv++l/+LopXh/MKxXksbyZlZ4QSgIBCgHnr0qfRpdT0LVRqGnRKtzgqWf5gVI5BBNd4mmqqEvMxJBO04PHtUjaXB5RI592FcTxTtZ7C5naxyF3q2sX2pPqM1laC9ZdrSqnUYxyM4PHt/Kq13Nqt35K3MS+XCuI0XC7c43Y+uAfTr613S2kKoMbNxGMdSKdHbIQNwLnAGAvGPeksVbZC5mtjy200SZVwYC47En3J9cVI+iXk8zNChSRuf3ShfbHHavV4rDMe6KEcDuhHTipIrF+og5564HTNN5g0w5pHn2nR3tnaWdsdPtZ0t5C4MycvkNkMQc/xD/vke9T6xLeXNs8Fho8eneaArvDMxV8f3kbgnjr1z3rv1091IVAmP4snIpzWEokI/coCO56Vn9d1vYd5HB2cepSFherqM0Y2jaLlUVyoxz8p6Dp/Ok1i2vb1YVg0vZtLB0uXFwrehGQCDwc8+legDT8xgCSM7TzuBOfenG2XaQJlxnghO9CxrTuh80i34SaSTw7aLcxLFLGpjZVJI4PH4YwMe1atqtuIZ7ieZYSq7Qx/h4zms3Rc2krIZgY5eo2Yw3ODk/WrU8fk2V3DcJnfu/d/eyOQP0P866aTVZ8/3nq4fEN0+VbouDUNB17TUi86FoydjbSGIIyAc9s9cjt3rnda1n+wbdI/+PoD5QVfJ4wOf8fakv8ARrOGGF7dFUIoQbPlPHbilis4J7XyzeX8Hog2uv4ZGRW6nGW6OuFKa+GWpykds+v6mLrUS6QHlI+yjHH4nH+eK9CmuND0q2hitp1tTxywJB6cMa5q80yygyI57yc9t5Cj9BmqcGh2l9MDLACB3OWJ/E1blG2xnKjKL+LU6zVUAaJ0I3M21tvIPP8A+qolCorMfQ5PpSL+40+3Rf8AVxsFAbqAMD+lVrm6T7O21DtYqm7HXIzmslTUnpsU6rS97ctG8d4pnYBQidF7HJOPwrz6PRFttWlu4HhQyEsT5QbO488NkevGMVp+Mdbm0m3tLKwkVbqb53KjlYxjqPc/oDW1oMianpMNy0atJ91wOgbvx+v40Yv2kIqS2PJrNuVkT6XqFhZ22x5GZgclmi54GB0HHTA+lXo/Edg0rRicLtwORjOar/YwQuEPXONtP+xLJ8xizzjpz/OvJbi9zCz6lHWHsn0e6XTJ/sk03Ek8Q/eEZ5+Y85/Hv71ys3hma2nkum15rmYvuzdRl8AgDJH8JBJJx0wMV2kulxNlVAwR8wK4zxz3qEaaMDcnIPv/AI1pCu6asgs10IPBN1plhp6P9sL3kigSu8hG4hRwAfTPv37cVzXxme21iPS/sP7+7idv9WMgow5GfXIrrn0pPLyscefoajj0pGbMaKGGSSC3f60o1uWp7Rbhr0R5gtpJJolnZRxskcTmSWM/KcseHOfUAD8K0LKIXGrRyXuYBDG6Rzoud7STsc4xjADt7celd9No+TnbnkE7H6+1R/2TNlflkGOOCDkflW31tvoPmfY57+x9I/6GGX/v7JRW/wD2KP7v/ji/4UVH1l9ybsmNtCNwkbdv7kkmpUtLSJDtj345wKRiRHhfvHJ7KPpUbODGGkcLns3PeuJ37jsTO0ciZSIDnqevrSwuRwqqcNjCtuxVOQrJ9xy59QO3H6VKkpjQEJkkYwrkZ/z/AFo9QUSyJyOcFQAOdvFKt5G+OCcHpjHNQpIHKNHHwRnG3cfzNIk8qMcb8HjngUcqK5EWfmONisSTx8h4/SjF1t+VehxzVEXjbSGZsrxnBOaja5LRnJHu3+f61SSK5Il4SSrkSYJ+oBFM82MKAFUHr8hrOZ9hDF84xkbR69c1Ks3XoR0wPx9atRHyItvKrMEwGOM89q0bS7juIWKSLJPChjkTdls4+XI9Otef+I/EP2dWgsGZpznJUDCj/H+Vc14d1e40jWFu55SVk+SWPOQVJ5z7jr+FephMPKmueTtfodOGw1Sq701oe42tjJPGyuobBCk4wMkc/p/Oo7lJtwUrA0XUZjwR1HJ6d/5VseHb+C901QhbDD5gDz9P0qverEOJGKxo28Dr8vTn3OCa6PZ8msWdMaiqe7NGJLbSyyYigiijJG3EfzYx2/WnxxJayDcpG4E5x0xjn8M1vIwWS1fYfuMGY4KjCAjp3yR/3zWL4tuoLWHLbWm4MWzsx9vTlf0pqnKTu2EqkYq0UYGpTG4uI41cqQuXYNwWx29uO/vVXWdTt9JsVllfzLhhiGFP4j/T/wCt9az7rW4LFR5GLm7kXiPGAgHc+grir66kmuWnuZDJO3cnhR6CtqcOaVuhhUnyq73Ekd5rmW5uX33Epyx7D0A9hW34Z1ptJuCeWt3OJFH8x71ze8yMFFXokGAOcd67ZUo1IcklocV+p63DdR3UazW7JIjj5GqWN2Q4aFD346/yrkfBizbTDAjyK25yqgtgAdcfhXTLPCPlIU5Ockf/AF6+VxWH9hUcVsdFahKhy832kn95b+1KcjykyOmP/rimCdSeWXI46/8A1qrvKAQBtI9xTsLtz5DEfe3L61zWMiQzMzKAEz7Hn+VNEzgkqshGM4JyahklKupaN8jHX+ft1oeTeVIQg90A/wAKaix6E7XqovKMTj06VH9uzIVKN+APNQrBJcxlmik69d364NQfYZSAz7V9gTzW0cPNq6QMs/bP9iT/AL5Wis/+zJv7o/76NFP6vU/lETsYiyiYZIGVCr05pkk6qrFpGXuFL5x/hT47W4CsX/djb8zFuBgZ6dc80W9oVkV5VC4PGFPbr1/LihYSq+ghkU0WA6FGzgkgHpnrRBNNJG7t8wzxtToMVMtvHHCVmBUfeKkfMTk8cdAKks4FEga1DOMYfL5wPXn8K1WAn1DQro8zuPLLg5/u9/xolLoxE7yKQemMdfbrWhnyXkjlhD5UYyOCSOTkd/p+dMYQpJlViJbn5sdgeMflWqwD7j0KAhnO5UXcxG7YpGT/AJ/pVJjcoxVoUAyPlzg5/Dv2rWedThWLEbsZPHPOMDuOf8mu98H+BftEa3utgLGwykQyrP7t3x+RPtW9PLuZ2TE2kedxWt5PcpBb2jMxbiJELMfXj+tdRpvw11u5iLyizsFb/no25hk56AEfnXsOnafZ6dGyafaxxA/eYLjd9e5/GrMgcoxVgJMHaWGQD9K7oZbSjrLUpVlHZfefGHj7TrnRdfubEuuY3KMyjGff8iKztI8N3+ptDII2jtpGI85hwQOu31xwPqa9V+NvhR7G1tdZtpZrt4Zf9OuZ23NMzHhtvRVB+UAe1T6Fqlv4ghju4wI5EhjheAcLEUGMKPQ9fx9qzxFN0o8x9BHNFWShBW/rojPYT6NMzWTERDG5M9qdN4tmhZDcRKQQd27ODn9D+Nas8ate7JejrjIrntV0ySEukbKYz2YdK5KddrRnJOgpO4/UPiARCViSHd1wcuS2Tk/rXE3ur3+oyNlnjDHO48ufYDtWymhSTN25/u8VBPaCC5NrCF3jiQjkn2/DvWyquWiNMNg3UlZaLq+yMC4lWzt2AGCx+Yk5Zz7msbzHlfPUk1oaxY3UcwM6koxwrgHafbPrSWtsEUV6dKCjGyPIxFTnm30FtYtnJ61egQyMAO5qIIfwrqvA+gy67rENpECA3zSN/cTPJqpy5VpubYLDKvU9/SK1b7L+ti5p/wDa3h/+ztes4nigDlYmP3ZSOqsPQj+vpXsdnYaH4/0X+0NM22l+P9Yi9Y39HXuPRu/6V0lx4dsLzw+dJuIR9jEYRQOCmOhB7EVxHgv4aX+jeJG1BdYeGCJsR/Zxhp19HBGMe3OcduDUOimuSaumdGOxFDHRdePuzjpbuulvNdfvOY1C2k0nVTpuoC3t7vG5fMlVRIvYqTgHP59qjV3PzK559BXpvi34d6TrUctwfMi1GTn7SXLlj/tAnBH5e1eQNZahoOqNpOohox0jcnCj0Ib+4fXt3xg15GJy3kV6ZzRw8alL2lKV2t1s15+a/qxqtLkfOw6dSM0wmPOUJDD2rbh8G+If7H+3rbxugG4Rebudl9Rjg/nXOW4MgPmZYjjCj7vX0rzp0KlL4lY5k77FxpZDGykK4Y5yDt5xSE+YpLKFbGOOuKqmRQfvsxx0NJHP8wHGByM4zThWnDZgmT8+n6D/ABopu7/pkfy/+vRW312ZV49ivJIm4KpJdVzjoo29Tg8j6UkrxmMeaBO2OVGNw6ZGeoPB9etIuUZcyBdwZTxtABOc/wCfQfiSKscZVlADDDY6AfTrj/CvWIHyTKrosFuUfIbEgAAx1J+Ufh/kUxJSjkebDs3fMFRj9OeP5dqZ5qxqgUhm27fLXhSOuPX8hUzDarZ3JLszuUcg+vT09aLdQuS7vlJiIChtwZduCOwBPpg5P9aNgjU7ZBvJYZB3NjoPYcg/5xVWQEM6MxLMMk4PGMc9PTvSSPuXYxfcRgYBz29xnr2z3pgdn8M/D0ep33267xJa2z/ICOJGxkZ9hnOPpXsBA6msLwdpv9l6TbWzAB44/wB5tUAFySW6Vuk9WPQV3QjyxsZt3Y7dt61Qu7gt+7j6scUXM2Caithum3HsK1SEY/iDTINV024025H7i5XyW46ZBGfw4P4V82+EWuPD3jG50i8+VxI1vIO25TgEfWvp6blpSP4HVhXzh8ZJkt/itc3NuoXZJEGI7sI0JP5MB+Fc+JhzQaN8PJxmmjvtStx9mSYffQ5qK4WF4fMmwF25JNLcX8baWrvz5gAVVGSxPQAetdF4f8Li0s01XxRjAG63sS3A/wBqT1Pt2rxqOGlVfkexXxMaMfM5K80PWZdHW70yKKFZm2r5zBH2YOZBnoP1PbpUHh/wosMfmXh3yN99ufm/Ou8uJZtZujtBEeeTjGfT6D2rWtdJjh2vJ8xA/AV61PDQh8KPPlj6sqfsnsYDeG7S/wBKNpPbgRMegHT/AOvWJc/Ba3ktd9rqEkE2chXQMoHp2r1SztwCHYY/uj096sPLvO0cKP1roUUcTbPni9+Fmv2TEpFFeRg8eS/J+oOK9c+HfhJPDWmbrjD6hPgyleceij6V1SEE4Rck1NDmRykA3P0aTsPYUKmubmOj65P2H1eKsm7vu/Ukjiyw38nPCDoPrVtikCgvy56KKqyXKWrGKDDz4+Zuy0iozSKgOZG5Zj2qzkCWYbsy/UJ1/OqGotbztG9zbxSyKMRgxhmAPpkcfhVyYoT5cAygPJ/vt/hUQCR5I+aQ9WPaj1Gm1sYt1fXEK7Y7fYmPugVwniHTLWWCeW1tmtbtQZMoxw+OehOPyr0mfO/J5rPv7VZSrhBvXkUqtGNWPLJEp2Z4qsjgBMRhDyflqWZpLdG5iKgZ5PvUWr2l1Y6jLaTQ7QrbkOeCOSD/AC/X0qsY2kO18AnkqOT+Hbv0r5KpTcJOLOrpdE321PUf98H/AAoqL+z/APf/AO+U/wAaKy5SeVlnzE2yRP57sNu5w+CemByceo56Z9uURTc4aVhHkLtzjIycke5/HjOKaUZ33XTSK4j+RmjywORjAxxwP5VLe/L58UyxZbGB90p16A/UfkMe30AhJFSy3dWYtycg4OcgDPQ8f55pEiDQJuMgR/mcMAMA8H69MUySRIn3R7N7bTsyCW3ce56c5z3PtSRS7Y5E2yxuCEwWAyeRgDHByfXnHvRcLFlzJtkyp/dhR5agE/z9sf8A1q2fA9jDqHiawTIZBJ5hQqcfICfoOR096xJHKY2qIhzgZDEt+Huf/wBVdd8J8y61dXByVS3O07cAEsB9M9aumk5ITbseuW+ViAH3pDmlnkH3F6LUQmHzMO3yrVfJyf1r0LGRHMTmprLnNNbDrTojszimBBGgP2hpCFQkjJPAxXy94lin8U6hd31jC81xfapi1RR8zL83H4KIyT2r3P4k6jdweGW0zS0eTVNVlNnAkY+bDcu30C5Ge2QapeEdGj8OadBY6dGl3rKqwluFGUhLHkKfXAUE/wCyPwxqe80jqoSVOnOXV2S++7/L8RdH0K08NQwXusuLnUY4wIoFPyx8dvf3P4YHNXYIL/XpftmpOUt85jiHTFaEOgDcJb+QzSt8zZ6VtxxqFBYbUH3VohBJWWxhKbk+Z7kNlZx28YwoUDoKtRRb23N90UgJkbnpVmPj8KsQS/LGfU1TUkn9BU13IAOtVDL5MRkP3sYQf1qgLanfJ9nQ4AGZXH/oIq01ztXyLYBFA+Zh2/8Ar1ksWtookB+dxuY+5oaT5fJj6scE0IVi/YRB2MuPlY8f7o6fnzUsshBZEJDycsf7q08yLb2rEDhQEUepqi0vlxljy7HP40CJZZQgCLwcYpiEmqm4lsnqaswnPSmA6RM1AyVeRd/C/Mfapfsu1SZMKKadhM4jxXoUWrWRBAWdPmikx0Pv7eorxnMsF3NBPAfNRtu0sMqQcfU9R0r6IvnY5S1Qf7xGa898eaeH0+aS5SGRgMiTyhuU/wBfSuPGYWNZc3UunLl0Z51su/7p/OipPKT/AJ73v5//AF6K8f6ozo5od2aUJ3ulw6h2QFsqdyt6Z46ckf40y7s2ZgZJTmQFVfeGYKMKx65HOKkthPPHd3CCA7ELsZASdoP3R+XrVRI5IowkhRVcbsRjBGecA479813EXGPiISOrZduMiTPzDjBxkZHIx71IltJDb7pXjZWbEhhkVgMdc4ORz69RmnOrNsUSMEbEnXqGY4zjHp0zipbqIfYRN5km1T5W3j5sKGyfzP8AXNOwmyFmdmZJHT5zlMjcvXt/gOtd98MwsWl312igGSRYN2APuAH+o/KuDmPl2q7USNn5JQZKjpgZ/D8q9D+H0vm+BhNyfNuCQT144yfyraj8RMtjplvXYgIOKuW07tw3FUbdRtXHpk1cjGK7VczLO7FG6oicClgUzzLGpxnvQBSm0/7bqBeDIkCGJ5x1jQnLInoWwMn0AHbnZtbOC0tzHbIEhjHzsOpPoKtNGlsEtoBtwdu71Pc0/UsW8MVug+UDJ9zWe7AzHJkcyScDsKYzGQ+1Nkcu3oKaDk1YFqPHSlmmCR5JqHcUWqTMZpdp6UIZIpMzbm+4v60wf6TdKvYGnTHYm0elS6WmG3d6GwGag2bvjsMVHp433Jc9F4FN1Btu9u4p9h8kK46k80wLNxIXMIPTc7fy/wDr1SabzGJ7dqsT8QBv98fyrHLlUTH8RpAakZz16Vp2cBkxn5U71lWC7wpPrxWytz5KbYx8w4ye30oEaOUgTbGuW/nVG4zI2ZZB/ug01Umm+9IAD+NOjslP33ZvbOBTQFOby+cH9Kw9YtEu7aWGRQ6OpBFdDcQwL8uw5rMngj527hVLsJnln/CFP/z9j/viivS/sqe35UVHsYdg5mf/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAC+AQIDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD10UtApa5xi04U0UoNMQ8UGm5pc0AOoptOzQA4UUmaWkA4UUlLQAtFJSigAoziiqVxqunW7Mtxf2kTr1DzKpH5mgC7mkqnDqunTttgv7ORj2SdWP6GrmKAEpKdiigBlGKdikxQAmKaafTSKBjKQ06mmgBtNJpxphNACZprNQxphNACMaiY05jTKBiZopMUUgNKiilpkhSikooAWlFJSimAtLSU6gBadTadSAKWigUAGKxPEHiSz0dShzPdY4hjIyP949h+vtWb4x8SmyJsrBwLjpJIOSnsPf8Al9ennbuzsSxJJ5JJyTQ3Y0hDm3L+seINX1iRhNN5Fv2ghYquPcjlvx4rJj0eGTLKfnXnbyfpVuKFnP8AjUjW+1uRS52bKnEy9Q0sWwjOdrDAYAdR9asaH4h1TQpVFvOz264LQvlkPsAen4Yp81tuY5/I1DNE5++c4555xRzvqDpo9c8M+JrLX4f3JMV0Bl4H6j3B7ityvArctbXCTQM8cyHKuhwR9K9Z8H+JRrEP2e72pfouTjpKv94eh9R/kO6exhOHKdJQaDRQQNpDTjTTQMYaaaU01qAEpjU6mt0pARN1php7Uw0AMNNNPIphFAxKKSigDSoooqiRaWm0tAC0ooFLigYop1IBS0CFpaSlpAFZPijVP7K0t5IyPPf5Ix79z+Fa4rg/H0nm6gkWfljj6e57/ligaV2cTIzyTMzksxOSSck0+JMtT5F5qzaRgckc9elB0ov2MKhVLD8PWrE8aMoKgA9j60y3jLAYA45waVwysc59SfSgCrPbqAMMD7VnzxgkitWZXeMsAeBg96y5iSDxj8KWhRQlQKTipbO8msrmG4tn2yxNuU+vt/SiQZXmoCMDmmJ6o9r0fUI9U02G7iwN4+Zc/dbuKuVwnwxvS7Xdo2TkecvtggH+Y/Ku6NBytWYGkpaQ0AMNNNONNIpAMNNNPNNPvQBGwqM1I1RtQAhqM080w0AJRRRTGaFLS4oxTJEpRRjmloGKKcKaKdQIUUtJS0AKKWiloAQV554yOdaufYLyf90V6IvWvPvHUZi1aZyCA6ow9xjH8waEhx3OYUqvLsAM8Zqe3v0Q8Rbu/IrntRvBEpaUnYvOOpP0qvb6xeW9ml6bNlsmfYHKggnk92GehzgEdqOVs6OZI6ifxBAqbAvzZxkHpU9pqkc3JYHHb1rz+91WS5g+1S26FGcqrqCmSBnAIZgTgjgkHnvVrw2bm9k22zc+9RKLSKjJNndXOpRLE25duBz6Gs+O7hmXLfKM45rl/EX2qzyszgBuuBWJaXGJB9ouCsfozEbvoACT+VEYtjlJI9DlEBTcsiD6ms254ORyKxBqkAh2iNGHTKZ3fkQCfw5qW3ui0alXDwsMqc1Si0S5pnoPwwOdakAOP3DHH/Alr0xuteefCmHfNeXGOFQJn6nP9K9DPWg55biUlLRQSRmkpzdaaaBjTTGp5pjUgI2php7VG1ADWP50w9KcaYaEAlFGaKYGnS02nCmAtFFFAhacKaKcKAFooooAdRmkBooAjumZbWZo2CuEYqxGQDjg14no+oXWq6QlxfO7zt98sxOT3P417e8aSxvHKu5HBVlPcHqK8cs7Q2j3cLS70SQogwBtUcAYoLgVnsEn+Z13EdAaz7/7a1q9iLJ5rRm3hQMbW9VPY/hz3roLeZY5QD0q+5887I1UjHJalfub20OSsbO7bSv7PubOO3sFYswOHd27knHX+XHpWh4ftYba/UxoY41AUKvXA759a0blxzDEN7AcueFWreh6TLIzSuFAAyMnrWc5dEXTjbVnL+IIBc3ce9PN25ZlY9R6Vl3ljb2+lyxw2kkhmIczR/6xCM4GPTkjArqNWtJre8GEOQccc1HbqsqlCNki9jRCWlgqRuzmbLUoIdCk0qC3VfPIM0jgEn0wuOP1NNs9P8mNtpPl53KD2rr0hB4cLnrkjrVPU1TBVMA+1WpdiHDQv+DfFf8AYV5p+mSW/mx6jdLCGX7ysxCg/Qd69fIrwjSLGa78b+HDbJuNvceZJ6BMMSf0r3c1RhNWG0lLSGkQMammnN1ppoAa1MNOamZpDGNUbVI5qI0ANNNNONNNMBvFFFFAGkKdTRTqYBS0UUCFWnUynA0ALS0lFAC0uaSlxQAory3XIvJ1zUYxjJlZ/wDvolv616hmub8Y6VA9pLqEMQF0CokcZyyjjke2RzTQ07HnDOQc1Yju3KBEOCwxuzVK6YIzgelQ2k4Qkt0/nSaOiL0GeKNH1K7sxHp8pKOvz4bDA+tYlvf674esxZ37zyxLwrLkj6E110GrGWNgikj2q1G0c6gN5LnOWUuCfxpdLMd9bpnA6pda3rMKw2cssKj5mPO5vQA9AK3vDqaiIR/aGTIoA3MRk+9X7jyoZiUCOBnmM5/PHSnDUYiwTpnuaTtayQ1vdk09yApBPOOxrKkmLt+OKivJ8ykKeKS1XzJR3xzTiiZSO1+G8JbxQ8vBVLNgT771/oTXpxrnPBegR6VbG7MkrXF3GjOjH5Y+Og/PmujoOeTuxKaaVqbQIaaYTT2pjUAMao2NSNUTUhjGNMzTmptACU1qdTDTATNFJ+VFAGpS5plLTAdmjNNpaBDqWm04UAKDS02lBp2AdS0lFFgA02WJZ4XikG6N1KsPUGnU4e9NEnjPimxk0++licH5SQD/AHh2P5fzrmNRmMdmEQ4dxgetbWra4+q+J/EFvOxK20kaoD2Ur2+n9feue1JGM0bgKcHkdc+la+zsWp3Rc0vTpJpFju9UMK4Hy+TkE9z94Vvt4JkaMS2viKMBuCGgwAfwauZabzoxkH2x2qP7Vq0a4t5C6dgyhiKxafQ3jJLdGxc+G7u0yZ9at3GenlEEf+PVzt7FcqRIbkOiMMt5e0kd+5qYzXc7ZvXYj0GAPyqLULjy4eDt7ACnFMUmt0W/M3YPUmup8Facl9qltHOyqjtyCcFgOSB9cEVxWmyItsHlYEnv61BH4gnt/HGmSRyFIbcgADtu6n64x+Vaxp30MpT0PqZjTaht5hPbxyr0dQ30qTNYNWJFNNJozTaQCGmtTjTGoAY3NMNSGo2NAyNqjNSNUdACZphpxppoATNFJRQBpClptLTEOpabRQA+lpoNLTAcDS02lpgKKdVe4uooPvn5v7o5NZ0+qSNkRKEHr1NbQoznsiJTSNeSSOIZkcKPc9aqy6jCUdIyzMRgHHArFBMpyzEsfU9aW0RlaXceM11RwiWrZi6r6HhPiSf+zPilrEfIjuAMf98qc/oafDdA3scUxxDIwXd/dJPWtn436G8Oo2GvWy/Ky+RNj+Fhyp/EZH4CuQicXdsCPSsqmjN6esTSP2mxeVSm5IT6YI5/z+VX4bu9ulVlOIghLMDnbjA/r/OqOlaybG1mtrqITKzB1dhuIPOc57EE9MVQvdQzMi2gEcOedo2EdOnP1H41k4pl3kjXv7qRLVZMb9zMoORk4xzjOec1gzTrcLuuGIwCAg4JPrU63ULQoPJAZVKjnGT6/wBf8iqjJ5kpfHUkgenNJJLYfvPcespPJOAOgHas1o/tOpW0sEgaVp1jdMcqSeD9KtX0gggZj2FHwws31Tx1YxYyu4ySfQc/zxWtO97k1NEfSC3l5ZrGkLgxqPuMoI/xrQt9Z3gedCV9Spz+lUrlQ8rAdM4qIqvQHBrodCElqjm52jooLqGf/VSAn06H8qkzXMhCDkZyOc1bhvpo+G+cf7XX8656mEa+Bmkavc280hNUodQikwGOw+/T86tZzzXJKEo6SRomnsBphFONMJqShjVGakaoyaAGtTDTiaYaACikooA0hS0wU6qEOoFNpaLAOpajZ1jUs5wo6k1k3mpM52QZUHv3P+Fa06Uqj0JlJR3NS4u4YOHbLf3Ryazp9Rkk4T92v61RjiLZLE59qkWHnK9D/nFd1PDwjvqYSqNguXOR8xPepfL+X5vyFRYdMdxTmkO2ulLsZCyQBFym7PU4Y06DAh+XJyc5PWmb2bauAee3GKsBflwOlMClqmmwazplzp92MwzrtP8Asnsw9wRXzzfadd+G9ZnsLxSDG3Bxwy9mHtXvninWo/D2i3F6wDSgbIUP8Uh+7+XX6A151p9pL4409ra5kkbVYiZobhlLZU43I2MnHQjA4rnq0+aLkbUp8rOPuIvNjDrjBqgVKnkVv3mi6jorGO+h/dE4WaM7o29s9j7HB9qyrlG6qK4WraHarNXRXHPWpA20UxVY9Qa1PD+gXHiG6kgglSCKNcyzupIT0AA6k9h7Gmo30QNpK7OR1e4Mh2A8d69U+AHh9onu9buV2mRDFbA9WAPzEe2cVJH4J0HQ4WnuopdUuFGQblvLiHvsX+pNcjrOu6nJrdpexyeS1kf9Dit02Rwj0VR2Pf1HBrtpUGzjqVLn0ABkmkkRiV2Hvg1meENfg8Q6fHMAIroL+9gP3kPfHqPetxkx05rbVaMxIFhVfugA98DFI0fYDBI4qwoB/D1ocDJwBU3GU2hY8jpSRTy2xJRvlHbORVhiAvsajK7gCRSaUlZjTtsXrXUI5vlfCP7ng1ZasGeAqpZP/wBdO0++aLEchJTpz1WuKrhusDaNTozZY1G1LuzTDXEahTDSmm0AGaKSigZo0uaSlqhC0UmapatMY7XYp+aTj8O9XCPM7CbsrmfqN01zKETIQdPf3pkUYXtz60RRgBjzk/0qWMhga9WEVFWRzN3dx2PTj0okVvLynBHJFL+P508c9KokbA4kX5uGHUf1qTy17ioXQggp1BqRHxjPT+VADJGht2LvIiDpl2xVS717TbaJibuGRh0SNg7H8BVm8srS9KG5jWTaMDNSW9hZQD9zbQj/AIAM1XN3FY8o8TQa74ovEuPs0hs4cmKBB931Y+pqXw1ZXtncebF5sEicHBww/wA+9eupMgXG3A9AKjkgtZuWTa/ZlqvaK1mhWfQ4pbu6a4l8/wAuUSjDqyArIPcVzOo+GY9xeyzg8+U/GPYHv+OPxr0ybSlV96qJEJywBwR7imyaRC5DB9oPXcMc1EqdOorMuFScNjwfVIDDuVVIYEgg9q9K8EpHpHg+zBgLXlwWmZO7Ek7SfbaFrSuvD1jLqK3EyCUxnH+yx7Z9cVoQ25mvs44AFYUqPs5Nt3NatXnirHPXWl32pyF7qRIoz0Ucmn2fhWzh6RB2P8RHJrtks0AGeTTxCFOBx+Fb876GFl1OHuNBWFg8AaMg8Moq1p9xqEcm1ryR1AwBIc/zrsGjRh8yjp6VA9pbkn5Bz7UuZ9RlCzvX8zbcPz64ArRJJxwB70xbGDfuKAsKlKquNvApAQn5m60ZzIq/hT+Bk/jio4fnkyv86GNDpiAuB0JxVOeHHI6jj8O1WrgYeNc9T6U3bukYHPPAqRkmmy+ZbbT96M7D9O1WjWXpzbL+WM9GGR9R/k1p15tePLNnRF3QhpppxpprEoSikoosBpUUlFMYtY+qSbrvb2QAfjWxXOyP5lxI3945rqw0byuZVHoWduxc+oyKhhbbdbezDrmrQJWMA9/UZFV5OJFb0Negc5ORzT0XinnBxxSLwccUANdcjjtSRAHhgfQVL1qMDDj9aBEnlijZjvTg2RS+1IBpT/6/tTdnpU3HT8qM+nWgCPyjjjIqvdIzKELZycAmrhOD7VHw1wM4PBNNAPjSNbAWxiyMcsDjvn/P0qKK3WGQ4GDVoHAGBjNN+83TtxUxio3sNtvcax55IFNzx6UrHLcDj+dDdB/KmIa2f0pMgLkc+9O2c5PT9aZ0zjn3oGITjtn1pOSM/KO9LknryBSscKccfhQBDcNtjx68YpLcenpUUh8yRM9KsxLtUcfQ0hkF02JosehpsZaSQbeMck0l1/x+Rg+hqSVxDbs/TihDKEb4v0kz0kxn26VtVhQx5tS7Hk89a2o33xI/95Q351xYuNmmbU2ONNpaSuM0ExRSUUAX80tMBp2aZQ26bZbysOoU4+tYEa/MPfitjUmxZvjuQP1rLUfKCK7sMvduY1Ny2R8q5+lV7jhatH5tuPTmq0wyvzdDXajnZajbcimndahtMmEVNSEKeDTGOGGB3p/8qY5+6ffigCQn/wCtSg8g/pSEZU/lSrwP60gFI7/pSO23GCc0pIw2B060jjHJxmgBd5HXp0qurH7YNvQ5qQygjaR19qqW7kXQz2BNMDR3nPP4c0yV9rLnrg/0pkkmPpVS6kZpogDgYb+lAy0JNx+UcU8SZXAGO+aijGFBPWp1XHWkAfw8HmoeS2V6VIQevY0AYORQMbjHaiVsKacc9eOKjm4XHegCFRvf6frVhFwP6elQKR3+tTxnLHGcj1pAULgf6cfZcVV1B28vngO21f8AGrcn/Hw7VnaiWe9t4VOAvNVEGWjgwqo5wPyq/YNm1QHquQf8/Sq3li3gz1PrUmmnMTD3zXLileJpS3LlJRRXnG4lFLRQB//Z</t>
   </si>
   <si>
@@ -3410,15 +3398,9 @@
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCAC+AM0DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwCrCMbhUMgJfirUYX5jmowUwzV+cn7Incp3QPlHPpWBfMRIRXQXJzC1c9qGfMzSbLiVnl5wBUMrHmkuNy/P2pjOWXis73LKjzMLjk1csmZiM96z5vlmwavWL4pRYjZtxV63QjHFU7H5sGr8ZxIBW8RM534jD93Hx6VkafGTbgit/wCIETTxxKq5bIAxXP6PZ6nq2rJouj2z3DAZldBkD1/AV6+Fp+0po+fzLGRw1V9X2Ib2dC32YIsjsOV602W3vmjVIwQuQAsYPT04r1zwZ8IPLZbjVpUDnkhRnHtXUXXhjSbHCJaq20fKcc12KpGmrRR87U9riJ81Rng+maDqsgExeaNSD1z/ACqv/aWvaLdFhcXULoSEaNyjY/A177b2NkTtKcAYxmoNW8PeHrzT5ILi3C+YAAc/d981UcTrqiZYPT3Wcj8P/wBoPxdoaxQan5esWqjaBL8sqgf7Y6/iDXt3gv4q+G/Hehv9kka1vI1zLZzkBx7qf4h9K+b/ABz8OpbSOW80e7jaNTnaxwcVxFhd3Wm3kcyTNDcQMCrocMCKqVOnVV1uYKVSlK0j7w+G8iyBsHua6e4OK8c/ZH8c2/ifRZrK7dV1Oz++vTzU/vgfXg/h617FcDPNeRWi4TcWepSkpRueEftYN/xKG+leCaLKY7qFx1Vq93/ayONLYe1fP+iMG1CFSeC1d1H+Giluz0qy1+/DwKq5QdTU+vWt3rV1A0KE7TljTLW3jS1jIwTivQvhnZxSQbnQNx6VMopM51U1Zn6JaS29vDG6nI68V6V4XX/iXDiq11p9ssHmbBn6Vf0HAtSAOM1zSWppCVz50y+Ce1V3kIG3NW7g4XArNumIO6vKufbE0mBEcniud1J8zsFPStS4m3Q4zWFcAiZjUyki0V7xjt60kf3KcwJHIpVwI+BWV9Sihd/8fS7q0LIKeajnhiZN5+9U+nLleRWkFqT1NSwyE4q5G+ZgKp27BF4FPt5dt4rN0zWqBjfF0RmWKGP/AFh5P0/zmvSPhhp+n+GvD4igiUXFwA9zLj5nPpn0FcNdRxXevW5RGHcEng4ArrIhcXEKpEORxnNe1S9ylGKPisVL22KqTfe33HZSa1Ay4WQ59DWRqF+0jFscdMisb7FfR/M7jDHqO9J5VwQQDz71V7mSikF1fSQyEqeaz77XJ3wm0N75p2pW0vILcnqazVsHVvMMuT2UinoO7JL28aS0KN93HIryjxBBjUGJwArnGBz+Nejaj5qMRj64rjtctGbUXnaMuM9AcY966KWhx1veL/7P+uXHhz4raZfQMdjTiCZTwpRztb8s5/Cvudn3Rgj0r8/NJDW+rwPn545VPB96+9tNnMumQyZB3Rg8H2rkxy96LNsHpFo8Q/a0f/iVsM9q+etFP/EwiJPevdv2uLlPsLpvGcV8+2MxSeNge9a0P4aOq+565pSXU8cKqpKetexfDuz8jT1J9Olec/CuaK70yMMAzAeles+GUAt8Y7VEr3sczilqXruVDGVNW/D8Ya1JHrWdeAZrY8NRH7EcetYS1ZUXZHzPdMTyKo3SMyZPFaDH5eRVS8bsK8U+6iZyx7VOazbiMGRj71qTNt4rNlOJCTUloqzLgYxSKMrippDu7UQ/ewRWMjWKuRrFleRU1qPLp77QMUuMqMVtSloRUjqTRsKIxmYGlhHHNOjH7zjtXQtzI3rO3QXltMp3MVwcdOnetSbxAbK1+zQWxY92HDH8ai+GHhfxT4nvGupYrPTdKtJGigkecvJcZwS3lgccYxk967HVPhxEQ0EGs3gdeZpbeBAUB6ffDDH4V7UIuyufDYitCNWdn1ZxFrrV/cNslt5419zkVoi9ZYlbeD8vrXS/8Kse0097i31nVZCsJk/frGQ3thVXFeWa5d7W1SztppZZdNAEreUETkZ4+Ykn245FU6b6EU66kSeJPFflySxWxjaVTzzwK5v/AIS/URLhrm3Rm4z6D2r0b4Z+B/Cmq2kV3JZXN9NcRrIftMpXORnhVIHFdD8Vfhxpmj+GdDk8P6VpNq95qUUN4y2UbK6vnIJcdsfma0jFHPLEtyPItO17N2EumLrIcE/4UeIo0W3kZZPlX5iQeoq/remSaDpNrdrY2Enk6jcRFhYoqTKrAKSoHHRvSqmkv511cpLYQOCw8sPuIUEk4IJx02449a0tYObmRzuiSfa9WitQyY8wKHUckk8Y9TX2R4a1Gf7DHDniOMKPwFfJOtS6neeKIYWuGWC14S3i+WLscle9esfsveK9QvdZ1bQNUfc1vGJockkrg7WGT25FcWNTcbrodWGVr3OW/auvrhtUjjZjsLc15HDLhk+ten/tWXP/ABNkTb95jz6V5fp9pdXKgwwO49QK6cP/AAo3Dms2e4/BGXNuoz3r3Lw6P9Hz7V4f8DLUx2aiUbW7ivdNDVorHey/LipqazZHQbfNtbNaei6nFDabTXL6pq1q07IsnzA021vkaPhq5XLUcotHi7bvlJqvdoRyKvFAxwaZcQkrgV4Z94jCuA24mqjxlmORWvNDlytVZIirNgVNzQyrwMsfy0y1DnrzV6aHzOtNhj8uNuKzvdmkSsxXBqSMZQEVC8ckm5lXirFgHEe0itoWRnK7ZLb5zg1IoKtRAozmnMa2iybHtXwU1F20+9tdm4+aHtQW/g8tABjtyDXWSWlwbiO4dZFkDYBjyMjHc14podxcxCF7Z5I2hRSHjYqSCAeo9810sfiLxJNAd2uahDCq8iOcp+o5/WvWhWSSTPicRgnKrKUX1PVNS1K30HSZ7zW51VJE8tA/LnjO1QeSTXgkGjFtH1TV7u3WOfUblnWNQAEQkkKcdSAwGfb0rTe+sZk+3a3qO4rJtjFxJNNJ9cAEmptWnR/Dq3treWl3ZzfckhkBUD+n41UqzstNCaOFjC93dmD8LfFkXhq6XRfEHmS6ajk2s+cNbk/wscjI9OR0r074heJvDuq6BZw6Xr+nytbyiaIfaFJDBTjIJyOTXhd14w8KXs0un/JcOMq8+0eWvHTcSNx/3c1a8F26jSdkgEkZJaIOOVHpzWqqtLVGU8LTcrpnoWo674estJktL+WO4kYg+TGm/c2OTk/KOfU15us27UbiYps86QsoHYdhS60YYeETGDyPT6Uy2ZZfLPQ4raE7q5nKmomF48Jtbq01SKRldJACueG616P+yrB9t8ZaxqZXGyxjjJ92Of8A2UV5/wCLbP7ZdW4dGkVEbYv8IfI5b8M17Z+zX4fOh+GJp5Wzcag/mPgYwoHFc2KdoNmtNvRHnv7RFlHP4kh85CyhucCm2qW+i6PB9r0yaFZR8jPEQD+NeseIfD9rqGptczIGMfzDIz0rl/iZr2lXOlS6YLbZKGDMWxgY9KunU0hEqnRnO8krol+Cdodb8XWenWpWM3Uu0E9Bxn+Qr6fvvBdvp+l+W0/mR7cMwG1s47V8dfCHWrnTfEMGoWD7ZbWYPGT7V9BeIfidq+vaXHC0S2qoNzeUxyzY65q60opvucdWFVzXK9DyD4sXNr4U+Jj2RuzJHNEJVBPKZJGD+VR/8JdZooCSryOxrzX4zy3E/wAQmu7yZ281uXdsk/jVSMpsG2bjHrU+yi0md1Ofu2Z3lwpD4HapYyhXa3WnXSgnIqMjjNfNn26KU8Q+0Nis+6wHYVspHu3GsbUFYXRFSWipJwuajnKi1J71LeLiPFV1w0W08+tZy0NYlSG5KLgVatn/AIvWmbIlHIp8ZQtha0jqQ1YkVgZvSiRvmxTV4lzSyetbRM7ne/Du5gltYoXG5oshkPUrnqPzro9aFku2EEKknrXA+CbgWmqwSMcKTtYn34ro/HAu41hvbbn7PJ+8U91PB/nXp4ZqcfNHy+bU5UKya2lqZHirSbOe4CHbNHjgEZ59Kx5vDdv5bwB7uKOQEyQRuwR/qOldDY6lerOPsFjZgEHzHcs0gPYjJ5HsMfjTtYvNYuLVkmWyAz1G/n8c1va3U4otT6HAzaDaW828QhdhwpKjirq3QhTZEdu0Hil17+0YPmiuIm9vJOMfia5f+0bwSOt3DDkH/WQEgD6g9fwrVRcle5jKSg7Gpq16JVBbuOuOtLo85a4VPyFZU0v+jx5POMn86u+GGj/tIM54QZrVKyMee7O88O+HdOuI01K8aV3X5fJyAmAcgnv39a9M8D3ke1kU9BgCvENf8Ytomo2tkAskE0Qd+eV5Iz/n0r0X4S67p+oSExTKSw6ZrlxFKfLzPYqM4uVr6neKVdpif7pr5u+N+tNp3iKdEy3PNfRcsir52P7hr5w+Jelzar4wuIvKbZnliOBVUYRbXMdUas4U5KDG/BvWheagkQbDMe9e5ajew6Rpay3ThVZeMmvEfh/4Xlt/FFvDpyFrh3AVM9fWus/aUXWbHR7OwuY2jeZ1VCrZDA8dRXRVpqVWKWzOJVGoNy3Mv4q28eraS+o28fmY5G0Zq78Nvh62oeHlutQfy5HwQpPQV1fwv0Lb4Vhiv13AqMZ+lct8TPGVxousJY6eWWONSMKK2VP7KM3VtqzakjO3JPWmTR/LVzZvjpZIv3fSvkT9FRnhflwKy9UQCTIFa7qyyYrM1JTuNT1NUZF0AY+arxqqirdwuVIqowOwjFTLU1SKN85GQnrTrHk4Y81DfF415pbMOWDGtUtDGW5oEYkpTTc/NnNSZBbFaIgtWrsqjBrtPDesR6pprWsx/fRLtb/aHY1w0zx29tvllWNcdWOKtfCwprOoa09nLJ5mk6cbvgcP+9RceuMMTXdgaNTmlK2h4+f18P8AVoQclzX+Z0M26yvklA+XODU2q6vA0IIaPOOTt5qGxurTWLfyzKhY9GVutJeaVBbR/vXyK9BxXU+Zp1NDmtena5XAcYxgkDGa5HWwsasldh4lsWhYiNgR2rjtbj8vJncLkdM1rBdEZ1Z3M5Zj5O526cCorG6nFx8pI3N+lU9T1K3t49gIZuwFd7+y/wCC7rxv4yF9dW7f2Lpbq9y7D5Z36rCPXJ5Pt9a1aUY8zOXnu7Ixv2hPC2oaIfDcwkY3WraUJ/LYgYYOcqP+Ash/OuL8H+JvEnhjUPOCSW5XtKp2N7Zr2/8A4KFkW+seGdhw8ImQ49wjfzFeNabqBvLMJvHm45VhkP8AUGuvD2qUVzHNUk1UdmfSPwG8Wz+OLa3t5IVW6cYlAOQvv9Kk/aM03TPBmnJeh1Mk7YAbgsa8V+EvxG1D4f682o6Xp1rLI0ZSW2l3BHXrlQCMEf5zVf4zeONU+KOrJfXt6loIV2w2yITGnrznOfwrl+pyVW62O9Y5Kjy9SHTviHe6J4ih1iy2NPA+QH+6w6FT7EE1u33xRvvif460mwurKO2htX3eWhLc+pJ/CvMG8PX8cWY5YbnjohOfyOK6D4I6HqenfEK3u9RtjBA3SRmGPx9PxrqdKO9tTjVRtrU+rNakg0rwmrqyrsh4r5xn8d6WNc1Br+Lexmwh254Fes/tCarHZeBS8V0vzRYXa2cnHavlP5pSZG6scnNKnTstTWtL3tD6zs5AwxmrJAZeKzrdWStC3OI+etfDs/SyldKRLgiszUBkkYrWuctPms++TMhoLizCuFwxFVLpcLkGtO5tpZHOxCaqXEKQr+9bcfQV2YfLsRX1jHTucuKzfCYVWqT17LVmNdQtN1bpSQgxLhjge9S311HHny1H4Vg6jdyu2d9ezSyKyXtJ/cfOYjipXfsqf3v9P+CbN1qNtCuQS7eg4rLvdck3EJ+79hWJeXMm7bnJqEg42t1PX/CvTo5fh6W0bvz1PAxWc4yv8U7LstCfUNQnuMszMV7ZJr0z9hSKfUvilrlsyq0F1ok0Qz/E4eNwB+AP515TeBhbsR6V9LfsI+HItKvNH1W5XZLeRTOWPo6tj/x0LWmJajTaPMjK8rs+cvHS634D+IuqaJFdTQrb3DGHJyrRk5X9Kkt/H+vTKI5pVk44JJ/xr2X9vbwHulj8Z6aFkjglMVw8fOUJ4Jx6Ej/vqvnC1geRQwYce1csOScbnXzSjpc6m88UatPESXAOONpP9a5y8vdSvHZTKQc8mp7ezvZ2EERLFzjAOc+mK9j+H37NfjW+urZ9eWHRrOTDTNNKrTKmM8Rgn5vZsY70pOFPVheT3Z598F/hhrfxB8Vx6dZbhEpDXl2wylvHnqfUnsvf6Zr7c+H/AIZ0fwrpdr4d0O3EVlpy8t/FLIerse5NXPBPhfw94D8Epp2gQqkAGTIR+8mbuznu3+RxipbeQWmjXF1KQp2l2Y9uM1wVq7qehrGPKmfM/wC2bZPrevh0BcWcMkmBzg4Y/wAlFfPGmOExjt0NfWk2lSa7ealql1H/AKwNFGrDOBjH8sfrXyjPavb3MkEgw0blGHoQcV6WBlenY86DlK83s27FqdzIoY/mOoqCaJnbzoTiRfvAfxD1+tEeU75HoaZezPbW/mRKS5OEx2Pqa7TQns7x1xya2NP1J1bJb8DXNW+4KDIct1Y+pq9bseuaBnW2+pvIvEjKPQmkaa2Y5ltbWQ+rwKx/PFc/DIRg5qf7SfepLUj6HkiKdakjOUpkk3mJSW5NfA2P1aW5DOPnzisTxZqA02xkmyA5Rtmexx1reuD83FcX8SXR5PJPQRHPOK9LKaMauKSkrpankZ3iJ0MFJwdm9B1xrUs0YSEBVZeue1ZOoagD8oIJHXmsTS7krosCx/ekjGWz2xVi3j4LN0FfbH5y33G30w8suzdOtYd1M0jZX8KsaxMN20E/Sq9rEWUu3TtUsLleMoZ9rMN+MgHvT0UkkkHHao7qxmeRZT+6wwKMev5VoRx4LH9aRm2ZmoIzKIzwW4Cj+tfYXhRR4X0HTbiOEFLExRCMHG5Vj2kD8Ca+Xfh9pTa58RNJ04Dcst4hf/cU7m/QGvsHxNpKn4cySFfmhRZh9cnP6GvMzFtx5TOvzfV5uO6/QseLbLQPEPgmSC+3NpeuW48mYp9zcpHzDtw3OOhAr40+Jfw41jwJ4ik0q+jZoutvcD7k6dmB+lfZHgUDUvhnb2jLuTypCpP8LIWxj8gKq6p4b0Txf4Pn0PxDES1rG8lpcKP3kGASdv5Hjoa86jVdGTj0PV0kk2eO/sU+BtLvNSufFursskmlyiKygYfKsxXPmN9ARt9+ewr6WvPLht3unwzRqST7Y6VyHwW8LL4d+G+naaU2SzJ9quyRg+Y/OD7gbV/4DXR60skukyxRn5XZU3fjn+lTWm5zbF1KFjJNc2oikO1JpvMjT0UAgt+Jx/3zXKfGbxP5E8Pg3TPmup4xNfMv/LOMnCR/7zn9AfUVt+JtVtvDGlf21eOPLghClSfvOo4UfUAH6Zri/g3o15q11c+NtdUm61SY3EasOg6L+CrgD8axjdp6GeIcpx9lTfvP8EdPZ6Ktn4chg2/OifOfUnr+tfHPxe0o6T8S9Wtdu1WuWlTjqH+b+tfdEkYeFkx94Yr5Z/bG0E6d470+9ZNv2uz2tx/EjH+jCvRwM7T5S61NRirbI8bZQR0ppX5ateWAKYy+gr1jmK3lxyYDLg+q8U234maMtkKetSYw3TvVbO3UXHqR/KgC+xC4560bqhuDxmmLIcVI9z6Xts+XU8ON2BUURzCOKsWo4r4Ox+q8xFcAhhxXnXxFmD38pCbiCVHoMYr0m+IWFnx91Sa8q8ZYmg86Rn+cEkA4yc19BkFL3pzfofK8T13y06fzMXwqUn02JOdysyY+jGtbWClta7c845rC+HsmWuYCRuSdtvPQHn+tT+LLne3kxnOOtfTHxpkxlri89ea3LeIQ2h3feGMcVR0G0I+ZutaV/hYNvqakDNmBluNzchTwKsSoUt846ikt4yZOlSagdsOKQmehfshaC2q/Eqa98vcLK1bacdHchR+m6vrW+0+G40W4smGI5IjF9BjFeR/8E/dCij8N6prFwgzd3PkoSOoRf8XNe8atpz28bNGN0ZOfpXkYmXNUZ0QinCzPJvgJfltMv/D9ww820uZjCwH31DncPz/nXT6lYxprStFwskoVgOnP+IrzTQbibQ74ayn3F1a6R/fEhBX8QTXrkCrd3lrdwsrIyBvrxkH+VcE9ZSXYwwdaTlOlLeL/AAew7WCY444IhhpMdPSovFDwaZpEPnMI0QNI7HoMDkn8zVqFo5dTCucvkhT9DivN/jRrFx4i8Tp4X01tsFs2y6mHTOQWH4Y/Me1YxmnsdGJrexitNXsu7PP/ABVez+PfH1ppaK32SaTcyf3YE5OfdjgfjXtFnClvaxwxqFWNQqqBwAK4j4I6NFf6hqGv2lvi3eT7HYcf8sIz9/P+0xY/lXqtrYQ2yiSc73HQCtJ+77prhKLpU/ed5PVsh0ex2L9ouBx/CDXgv7dmm/aNG03UlTm1nKE+iuD/AFVa+hi7SAFhgdh6V5b+1RpX9pfC3Vyq5a2iSYf8AYMf0Bq8NLlrRZtU1iz4z24FNZcVY2CmsBX0BxFSRc9az7xNt6T6gVrSKKz9RXFwpx1WgBZBmGqrE5q3wbfHeqsgAbpUsD6htlBjxU1qpBOaihOxcGponHl8V8Oz9U6EPiE7NHuHH/PM15Z4kUy6RIqgFkbIz6GvSfFsoXQZM93Qf+PCvOtURw88LDO4EfSvqclilh2+7Ph+JJt4qK7I5DwDKIvE11bEqTIgI2jgdc/yFaWqIDesOpJrC8OEWvxAhXORIGQH36/0rqYbUy3+5j3zzXsnzpLp8JitcmobwbivfuauXjAsIkGAv61DMpXAPpUgQ2sYBLVDqXJAq6OFwKjtLV9Q1y1sYxlriZIh/wACYD+tS3oI+0f2V9G/sb4L6NE6bXmgNy4I5zI27+WK9Ka5KQ7W+YVm+GrRdP8AD1rZoAqwwJGB9FAqS7kypx0rwZyu2ztWx5LoGlW2t/DvXFCj7RDrd48frkSHj8RkfjWx8Hb5b7QVgMoaWx3RkZ6rkFT+Rx+FVPg/82k+IIP7uu3Y/wDH657Rb/8A4RH4n3trL8lrfJlCTgKCdwP4Hctc9f3Z37nm4lqjiYVuj91/odx4ivodL0ma4gk3alJlLWLcTliQC5X0XOc+uK4DxdpbaB4XSxgcnWNeZbSE/wASmTO9/X5Uyfriul8AWbaiq63fZefUZTOA3/LOIZ8tB6AA5+rGsuwceK/jZdagvzWOgIbK2PZpv+WrD6fd/A1FGCvzHbTXtGqkt+nkdx4NsIdD8N22m2cYjjgjCLx2AAz+lXpGYnk5Jq1NCDHx/DVOQFWAPX/P+FOS1OpMmj+6KwvHGnpqnhnVbFxlbm1ePH1Uj+tbYOFAHYVDOm+N1I+8CP0pJ2ZR+fF1A0Nw8LjDRsVYehFQSL3xXVfGDTjpPxM1qy27VW7Z1Hs3zD+dcvJ0xX0cXeKZw7OxAR8tUNU/1sf0NaDjCk1natndHj3qhjEH7s/Sq7upxViEnHNUZPlkZT2OKTA+qPlaHdTYWUNiqkcuICN1V47oiTrXxHKz9Qc0O8d7v+EbkKdnU/rXA60Hu7BpYDiVRiQeo9a7jxNc+foskA6sf5c/0rz7UGmibzYeq9R6ivqsoi44ZX7s+Ez+SljXbsjkZIks/EumyrIzyfakDELgAE7T/Ouvnuhblwn3s1hahFHd31rcwKAEuEZ17jDCtuO0NzfscfLu5Nepc8Qk02J3Xz3FJfDNxxV65ZIrfyoz09KoTMWuG/SgTEYZ4rpvgNpg1b4yaLbMuVWfzG/4CCR+uK5dTXqf7G9kbj4tSXZGRa2pwfQswx/6CawrStTkVTV5I+u3O2ECqdw2RirFw46f5/zxVGZjuYD04P4f/Xrw2zrPPvgewdvEy9v+Ehuv/Qqu/ELwbp2vTQT3ck0Xk7kLRYBZSOhJB6EZ/Os34GnZqXiqL+54guB+bCl/aWvb2z+Gck9i21mvYUkbnIUh+mPfFVOHPPlsY16cZwcZK6KmteIhoXgeabTZUuLxttlp2zGJZmOxCPp976A1sfCfw/HoOlRWanc0ca+ZIesjnlmP1JJryH4Fm78QeIrNb35rXRi5gXHDTP1bA4+VSQP96voKxVY5JOMZ2/8AoI/xqZR5PcNYX5Fc1EJJA9TVW6i3vuH5f5+tSeYAoP8Anv8A/Wqa0tp7j5o9u3OMs2KzepSM85BOR/nmhunHfP8AWtG40a7K5MtuOP7zf4VWk0y4H3rmH9aixaZ8gfte6Z9j+JwvFXC3tsrE+rKSD+m2vJ3r6J/bm0eS2j0bUWZXG+SLKjpkA/8AstfOkh7V7mFlzUYnNUVpMimPymqN8N23PbNXJTVa4I3DNdAkV068Vn6kvl3jYP3ua1ML1qjqaCS4wP4RzUsaPpKHRfEDqR9kC/VqIPCevySZYxpWrL4h1Fh/rdv0FU21fUHbm5f86+WSR9r7TEPqjJ8R6beaPNHBePGxlG9SvpnHNcV4hQ2l86eh49xXWeMp5ZvLllkZnAIyT2rnPGg32dtd/wATR4Ye4r6jCR5aEV5HxuOnKeIm5PW5yOoyQx3gmiLRybgSF6Mc+ldPfPJDKyIMZPWuM1MktvHau+1Ly3kjG3l8V0HKUXXFmrE8k1XkB81j71a1b91bhB/DzVaU/e+tAmIAAte3fsRwf8T7VbvH/POMH6Bj/WvEGPy173+xWgSyvZB1e8YflGtcmKdqTLpfGfQ80hK/UVXlPLY/z0qaTJX8f8KrzfLlv8968eR1HnXwaOzWPFo/va/Of1rY+NTWifCDXpLpVcLHH5asM5k3jYB7k4H41ifCuTZ4k8VIB/zGpT+eKl+Irrq3jLwv4Xm3C2vb9ry4wfviBcqn4s4P4VpJXmKUVKNnszK/Z58Pz6RpaJeW4S6LO0xPXcc4xxwPm/Qelen3SiO+kTPI2g/98LUHh9I5tckcLj+HGeyk0/WbgLqtyFX+Mf8AoIrnWrbL5bJIfu+Xk1s+Gzvs29pDj8q5+NwV5Fa2ht/xL5sev9KYkal4WEJJIz9aypmderD86yfEV3NBZlkb5iwGa5+S/uNpyQfzp8tylscL+2xEt18OY5uCbW6jf88r/wCzV8myda+m/wBpC7kufAF9C442oR7YkU18yScV6uD0pWMKnxEEh9ao38ixtlmwMVdk5qlcIjXQdlBYLwTXSQiCH7RM2R+7j7Fup+gpuqAosSp75J79KuNycVX1JN2w59aGUj//2Q==</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEASABIAAD/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCAC+AKkDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD79X7tLSL92loAKKKKACiiigApGIHU1yXxV+I3hzwFpZuNYud1w6kw2kRBkk/DsPc/rXyR8aP2hPEXidprSG6Njp75X7JbOQGX0dhy/wCg9qyqVYwNadGdR6H1X46+L/gLwszxXuuR3FynW2sh5z59CR8qn/eIrzXXv2sfC1mxFloF3P6C4uUiJ/Bd9fGer+Ibu63KGZV9Caw5pZXkyXJ9cmuSWLfQ76eAX2mfaTfth6QG2jwiT/3FP/tVXNN/a40OZ/8ASPCtxGuODFfK5z9Cq18QIzY+U4z3zUsMskfWUt79Kz+tzNHl8D9B/Dv7Sfw51KREu5NQ00t1e4tt6A/WMt/KvTvDfiHQvEFiLvRNXs9Qh7vbTB8exx0Psa/Le31GeFsq7fgcVv8AhPxjrGialFqGkahc2d1Gflmt5Sjr7HHUexraGKvuc9TBW2P08or5f+BP7T5meLS/iAFZfurqlvHgg+ssY/8AQl/LvX0xpV/Z6np8N9p9zFc21wgeKaJwyOp6EEdRXXCaktDinTlB2ZYoooqyAooooAKKKKAEX7tLSL92loAKKKKACvM/2hvi1pvw90V4IZIptXmTMUR5EI/vOP5Dv9K0vjx8R9O+HnhGS9mkR9QuFZLK3J++2PvMP7o7/gO9fn/8TfGV/wCJNbuNS1K5eaWeRnZmI+Ynvgcfh2ArCtV5VZbnRQouo9dg+I3jXVvEmsTajqd5LNLMxJ3uST6Z/wAO1cfNO7Nu3delVbi6Lsee9MjkJOF/OvNk2z2KcVFWRZXliz8/WnqN2fQ0yJCfmPNX7K3DdDnHWpUTXmsRRW54O0irH2J+QFOcdMHPr/KtrSNPDsMKeO6r3z9P1rbj0qMQqskY3H0cZHPpkVXs7ke1scM1u6rgiq7eYkm5TjHb1rstR01Id2Vz05xxz7elc/qVoEzt5GcZ/wDr0/Z2DnuirBfyRsCDhgc8cV7V+zJ8dNQ8B6ythfGS50W4f/SbQtzGf+ekWejeo6N9cGvBrtJBkcflUbSvkMjEFfeiNSUHcipRjUVrH6yeGdY03X9DttY0m7jurO8jEkMsZyGB/kexHYir9fB37GPx2bwZrq+HvENwzaHfSYdjlvssh4EoHp0DAdue2D93W8sc0CTROskcihkdTkMDyCCOor1KVRVI3R4talKnKzH0UUVoZBRRRQAi/dpaRfu0tABWb4u1uw8OeG7zW9TmEVrYwmWVj6DsPcnAHua0q+XP+Cj/AI7k03R9M8F2k21rzN3eBTyUB2xg+2dx/AVFSXLFsunHmkkfPXx6+I2o+OfGV5q97KQsrbYoVPyxRj7qD2H6kk968xvLhpWJ/ACpLqcysxz1qrtJboeRXlSnzM9unTUFoRpubnFWLZW6kfeqS3hw2alhwknAyO1TqaaIu2cB25Pcfhmtyxs1LrkbsDnBx+Az9fWs/TZAE27WJbjpjmt7Q/P3gCFVPUDb19/1z/nNNXRWjOg0SxKoq4RUUfNnjt6Yrcht9pCqWDH77AY/UjFQaLBuKiRW6ZyMdR+OP61Nq0wgtmMO4MvYDO4eg71onoQ4amNrELRyNDuDbuRz94e+e/vXJanCw3MBgZwf/wBX+fwrd1DUJJdweKT5Dt3kYBwMcZrE1C5Qvjdz2zSd2GiMC8t1Kt/eHTHes24hKeoz0x3rdlBlY7QDx0qnfW+2M8Zxz/KokhxMeIPFcB1YqQcg19w/8E+vi2viLw03gDWLlm1LSYy+ntI3M1sMZTJ6lCen90jH3a+K2g3Jk4IFa3wu8U33gX4iaT4msWZZtPulkK5++nRlPsykj8adGpyTM8TR9pTfc/Vaiqui39tqmk2upWcgkt7yFJoXHRkZQwP5EVar2DwQooooARfu0tIv3aWgAPSvze/bU8Qv4g+O2t3W/dDBcm1h+bI2xARjHsSCfxr9GtSuFtNNuLpyoWCJpCWOBgAnk/hX5WfEyefUtQl1GeTdLPO8rt/eJYkn8/51z4j4bHThfjuYMbICMng/pTmdR8/btVJX3fxYCjn+tQyXLPcGGMMzdOFyq/lXmxhqezKdkaMdwrttDgYOMf0rp9K0WXykkNm8jnoh5c/8B9K57RvC9zJdRvJdL5isSNqj5+e45wPz712kN5q+n26RyndHGuMeWCvr04wfelUmlomOlTk9ZIv+HbS1juGiu7GRGYhcHgrgZIz+FdDZ6YjKr7eem3BG31Bz/nmsPw/rsVxcMs8kbMTlSCQ4ODn8MZGD610el6pFcwxqoMZLfMpA69OPqBmspVE9jpp05LdG5YW7Q2/C4YD1x+ORVPUbSZmyqsQoJ2scHIGePc1sWsq/ZuT16etUfEF7FDGDuVW28ZHHr0/AVHtTb2a7GNJpzXNwBuCmQB2kUjAGBjB7dev0984994UMlmLmPUYZJm5jgZAT05JJA4PPb0IOOav6hq9lBa+WZDtY4KNnjp8v6dPWs6NpLy4V7dpFVQVBOcEehH0zTVaK0IlQk9WcdrSixuSkiG3O4qpAIXrjBB6c/rVSW4WVdrAhscEjqK7HWPC+nyWry3MbK7gYbewUcH0OO5rhNW025sQ2zM0Ktj5Rgoe5x6delbxqRkck6U4asktyiho2PGP1qrq0I8sOhycdaitrgSqBu5U9R39qbcTYUqT9KhpqRaknA/Qf9gHxZJ4n/Z30+3uXLXGhTvpzEnkooDR/kjqv/Aa9sr48/wCCVurOZPF2hszGPbbXMa5+VTmRGOPU/J/3zX2HXs0ZXgj52vHlqNBRRRWpkIv3aWkX7tLQBj/EI48A64fTTLj/ANFNX5aeOJXi0lQw3O0nHt81faX7fnxe8UfD+10nQPC00VpPqsEstxctEsjeWCF2KGBAzk5OM9MYr4e8YXRuobcsCCy7yD2yM4rlrTTdux2Yem9H3MWJsQ4BwT3/AK1JpxWGRVUrGx5d36D8amsbXzFLKPuiuf1eSSTWYLPzhFHJNtZn4VCT94n2rijaTselJOKuepeF9U0i1kj2LLcyucbuEUH/AHm7e4Br0KQ30tqAunaXjADQvO6k4PY7ME/hXDfG34UaXovgPw3rWi3F3NZSn/iaX8Q+0SKWA+cR7lXHJ4yv1rrP2dNM8B3PiDWLnxFbTWmnXFnELZUtJrWVJ1wuYEWWWQjAJLM2CTjaK0+qpxbciI41ppKOhleIfCkV9A11Z2s1hdpz5e4Mp+h71z/h/Vr6w1IW907Blba2Djv/APr/ADr1TULGa1n8vTnvNQs2YruniiS4TAJyNsm1+AOoU89fXzvxxZIuvCW3TY2cOm4MQQcckf56V586bg9T1ozUldHpWh3fnWIkLc9Rz3rj/HWoTG4dImPtitnwa5bSMYPC85rE1CJJtUzMRtL7WrJRNpS0MTw/pstzcm4v5mROvPYe31rprPWls5AlnY28UKnHnXs2zf8ARQM/nilm00LdJGtwLO0m5FxLDJIsWO2EXLH24+vPG54q8D+Ej8C9Z1zSNSGueIobf9zHMzQmJN2GYQ8E4BY5YNXRRoc8rXsctfEKnDmtczNe13Gns1/p6tbucedaOxCn3DKoxwehJ46Vwms31sJDPZSLLDnGwg7gR2IPIPQ81mfCjRdL1z4geGdDsrgXxmJTVI7B7pTLlifMbzFQRsoJGF3Llc9DU37Qvhq7+HnxJXSre7N5Z3ABguJG/eRDPKSEcH6/jXVPC8qumcUMc5uzVihdW0SyG5txhZuSoHAPPas3VwSodTwTW5pcMk9tmF92cfQHrVDxBarBagAr2JA9f84rFSvoauNtUfRn/BLGV/8AhaHiKMMNjaOGYD185MZ/M/nX3HX5efs5/FPxR8LNR1TWPDlppkq3MEaXLXsbMAikttXDDGSefpX6Q/CbxVD43+Gui+Lbe3a3j1ezS48lm3GMkcrnvg55r08PJW5ep4mKhJS53szoqKKK6TlEX7tLSL92loA+L/8Agqwph1vwnebelrcLkem9P/iq+TNUkLyQKDuxGuCRjtX3H/wU10RdQ8L+EtQdcxwahPbvngfPFvGf+/NfCt0+7UOuVTK8159Ve/I9XDu9OBuaHCHgYEckdabHo0Ml80/lhnDfLntS6HNj5QePauhszE0O7HTA47ivPd0erC0kkWND09IvLWZJNmd3lIzYfHYjpg+9dpocs4VY4EisLcNlUTgjOMgHsDgVymnyzNNiAsxbooH4Cuv8L6HeX1wsk6swU52/wjn3qVLlRtyKXQ0tSufs+n7bQtll+aTJywx2/L9K4trTM29gTuJ6mu28VWot7cpJ8obqc9eO3fH+eK52GMPeqPT+EDvXPUqs6qVGJ1HhTS2XSvMxlNnYdBisDV7Em6ZlwOSeld3oLqmi7CvVc5Fc/qKAXTOcr0x781zwqNM6alNNFLSLcyWLQSp5sJUjaT909eB+H4VXurC4s23QRLqFt1aNiFdPpngn9RW94dWM3LCMjBYblz6elX9V0mSSBpoN2RyeMnrXfCpdannzp2ehwcOpWWm6g2pafLfaNqEylZZIo/Kd+vG7jA6dK5PWtEi1PWGvnlmvJmYb5pn3yHnuTk4rvNe81Jtt0AvOCcZxj1qnJPEkJKrGy92UD+YqZTle9wjTjbaxgWOn29hakRoF3DDKBjmuU8WYTfgD5s9RXVaxMxDFSPw/z9a4rxROWXJ9a1pJ3uc9aSSsVNPdZ9GksMfLMxDkevQCv0+/Zms20/4A+ErQoU2aTEQCMcEZB/EEV+cfwk0X+3LeS3DIskd3EqcctuZF6+n+NfqbpNpDp+l21hbIEhtYVijUfwqoAA/IV6OFi/aSZ5GOkvZQj6lmiiiu88sRfu0tIv3aWgDx/wDbe0Uav8D5pgm6TTb2G6TjpyY2yew2yNzX5p3SOl/IsgZTvOdwwR3/AD5r9dvHVlHqXgvVrGaPzEuLGaMr65Q9Pevyd8Xabc2Oss1ycPMxYKfvY4wSO2R+P6Z5MRHW524WXQZpr7SDnvXR6ODNhAfT/P8An1rkoHAccV2Xg8BpFLZ+nrn0/wA9686qezQdz0HwNosckwdlHBwF6g4IA+v/AOuvRGmTTNH2wxBiqfeJxgj1z7Vzfg1USEYHJOMLj/Oa0PEV7EdNuYWdWZo2TJySCRjJPeuKUrbnpwjdaHIafczeJ9UaSR9zu3yAtwPTHatIeHp4NUWQr+7Xj6+v9K8ssdf1zwvdEW8UhZXIR0TfG305B/StfTfjD4hs76FfEOiMtnJgNPHG4wM9SpHb+lRUoVZO8dUVSxFKKUZ6M930nSYjo2Pm808YxwR71gapolxLdqY9zKp556jP+eKZZeNFazjkguEELhWRuxH+TXn/AIw+KniO81GWw8J2TXgjYpLesh8pW5yFA5bGD+VYwhKcrRWx0TqRpxvJ7nSawk2jXySD+FsHj3/+tXUaNqVxHHGHKsWA2lwfmBxjkHpj8q8f0+fxlrt9HHdzm4STBaQwiKNecZGWyQD+Ne0fYrQaNFDFJva3hVN2PmOBjPoeldaXJo3qcl+fVLQg8UaXb3tqZo1XceF6cfX8cV51rlgbaVWQkK6Bhg9Mj29DXfx3/lJ5cjg7f4jyPz/KuS8WTxGPKEYC7VAP5fhVSXUmL6HC6zMAGHoOTXHa+cyEDv0rpPEE4DHsMYrltSffIgxznpXTRWh5+Id2elfsq6ebrxpp8K/fn1qwi2lh9w3CbyB1yAQfQ59q/TFa+EP+Cf8A4etb74tWM0rJH9hha5aJ4GZ5JADj5uibS4PXJwOMV94V6mHjZXPCxM+aVgoooroOYRfu0tIv3aWgBG5Uj2r80/2u/BA8LfFjWba0lheLzmuPLhUbbWFnPlpwc7grLnIA5A54NfpbXzZ/wUE8Ci/8N23i6ytZZZI3S1v4o0BV48lkd+MgKwwWBBwRWNaN4m1GXLM+Bd21smuu8H3IVhz2GMevpXL3NuYbvYXjfgH5Tj3xz+VaujuYSp34BGcnnFeZVjoe3QnY9a8P6wFhVvvfL0HXp2+uKh8W6vcpa4J8rzMuSyk4GMj6ZA/l6iuc8M3aNHGZnZUYlUIbCqDgZJ/EflU1xdaYNMFzNgoo3KW4GSOBjPQAAcnv2PNYexT1aOv6w0rRZLpd8C24q088kokB+6qrwcAEHrnt2X1rqNBSHU45bPUNMM8EoOH+zt82QT25HPp7fU8npPinTg/lQeUXZeWYjk4x/n6V0mh+K7WJlWaf7xI6ZA/zxTVKT6WB1YdXc01+HvgmO3WOIasFixi3E8wRj3wmeRnjHHWpntE0fQ7OztNIliIclsxMqxLkkbgR83GMD1JrR0/xbv0+UxXasEPGHw2M4yBWXeeLomUqqlpGycqpOfyp+yk+o3OCs7FG4vQ1vIPs7wtb7nG4ZEh/gAyPXk/h7CpNF8RSxXAS6Qx+ZjaNu4dOfTjr+VZ1/wCM40fy5rFpOOU8ts9O3GayLjxHoutXDW6zSWs8a4jMrFCCfTOMjOOKzVKz1RTrWV4yOk8Q6nJFL5iqqsc5B5xz/wDWrmNc1cSKSrbfoeB+HFS6hIJrVIZ7na0SbGdn3ZA6Yx2246/pisG+tn8newIU84HGSew9+1a+zRl7Zu7RjatcGVjgjavX368VB4f06XVdYZMbhFG7FQOWwpOF6ZOAx/CrjadNIyxpG25mCrgcHJxn9etdP8PMWDtP5cUMmyQIbiVkjk2AsGOcZXqeAeSvHNdFOJw4ipofUP7Bvg9bTU9T1+aOYtY20dhazsAFnD4dmI+8GCpEvPYnk54+mq5j4P6HaaB8P9PtbWzltTPGLmeKZSJFlk+dw2eQQTjB5AAHaunr04K0TxZO7uFFFFUSIv3aWkX7tLQAVneLdHtPEHhq+0S+jWS3voGhlDDPDDGR6EdQeoPNaNVNW1PTtLtWudSv7azhQZaS4mWNR9STQ9QPzd/aq+HV54B8fzWUsDrZMxNlIbcjzlyzAI4HzgKVU55BU/VvOoIpBIsaL+8UHCg/6z5eNp75/HPbrX1D+1x8Y/AfxM8UWvgjwxq8d0+iPJcvqUTAQySrtDxRSAZbCN8xHHzdGxx4Z4isA1lfXMjwXcaPL/pUwEYeUMFJ2tz83ybc8gLgHJJrhrUrM9HDYi6sZdpdraWEgUTNE4Vg5XYqtnLc55+7jpjgn2q3axx3omSSOORZht24O3rnIB68fj7nFUfDcd3qNils0SlWcLCXXCA5JboDk8ZOc/49G1pLZwrNMzndho1EGxAp6kAD6YzjOG46Vg2+XY71FOSu9Cjpug6Tb3CPDZwwSqScSIAGJ7g9q9I8CqiNHazWEWwgAOUH0/z/AL1clGkd3CRhc4x04/z/AI1Baza9ps+NNvZYhn7p+ZR+BBrmVRvRnoRioao9yvLDTEtVb+zPm2clTjIyMDgdPvZ+oqj4gGlW9gfIsNkoHy7R7d8e9eXx+LfHi8C+hcY43QDmpX8ReNr3EM93HEp6mOIA/nVc1iue6tqS641yybZJHjDMVRc4ZlPb8D3rHvdLeQszIWjK5CnnHuPXvWnYQypdG5uGaR16yElmPPr/AIVHqk93JuNvCvlq6oucnJOcDCgnnGAMevpSpyk56GNaMeT3jEtzsjkk1ARtFHG3lKW+Yn+9zzk4/HcB7063s3u55WuUaK18lGaWQZ4YEBeD94uQF78elXLXRpLfU55iWvLOOSNITHgq4YCYFcHOdxcAdMlSTjOS0dp7oWLqVR2DwxXJbiXJycLnHyKfnx1UdtxrtlFLc83naWhFpej2nkxXS+bNPNaPK0UeEOVk24B6R985zwDgHt6v+zP4J0rxf40tTYWb3FhHcLealI52xsEcFQw3ckkDA6kSEng88JrOnRrDHeXEaWltEVUXCzKkSAFCkkZySVI4yTjKu3X7/C6X+0T4u8G+Ol1LwRFa2ENmhhubWWDMd8C25t64BHzHg9cAeprqw2HlUeiPNxWISP1N6UV8q/Cn9uX4faxp8MfjLS9Q0G/x+9aGM3Fvn1BX5h9Nte5fD/4w/DPxoqDw74y0q6lccQNcCOb/AL9thv0rqlSnHdHIqkXszuKKRWBUEEEHoRS1mWVdV1HT9K0+S91O+t7O2hXMk1xKI0QepY8CvB/jB+2D8I/BfmW2m6hN4mv0yBDpabos+8zYXH+7mvhH4heNPGXja6+0+LPEWoaswOVW5nJjT/dT7o/AVxuoKEXaqDP0r0o4BJXmzjeIb2R7x8YP24Pix4jaW18J29j4Us24V4l+0XOP+ujjaD9FH1r5w8d+N/F/iu8a58S+JNU1aZjnfeXbyY+gJwv4CnXkAxnFYl5FiSpdGK2RcZdzV+FzyDxxpdukkq+bMwPluQQCpBwfcCvfdPe313T30CG7S1v4yrtuQ7J0iUhOgJOCxPsRnnLZ+f8A4es1v42sbkDmJ2I/75Ne0+ILy38NW0Wp2hZr+P8AeRFMbjnqQf4R79a87FQm5JRR6WF9lySc3r09T0f4cabNd3BiisUtkld2aS6A2pIwXb8oG3djP8QAwDmpPHmmtNeXF8kUTcqhlV38scqS2ZVC4JfAKvg7fywfgj8UdL8VudJ1C1/s28iX5VDbo5MkAkM3U4Hce3PWvWl0mLU4kmuY4Xs1kM724m3sw2vhcEZPDKTgZ4PX+LjnC65Tro1XCfvHm/hy0SZvLV1LMRyHDDnuCOD+H6V00GjWysDKf3bZG5ccHkY9qvXOjwWFhdGKJoUWRXiZbg7/APgRK/u9pQYHIG45ICmspbuKW68u3uYSshj8tQ3yu75ZRzjsD2BzxgdK4JUJRZ60cRCSNq28NaY6D55OmW6Y64p7eHrCNd3mj5V7ntXP6l4uhsriS1Z9sq42liCFJPTBOMjGP88WtP8AEFtMsVrNI5e4VTt42pvAZQeuBtOfxA9aqMeZbClUUXuTX1hBBaNOQWAB4A+Yc4yB35IrK8J+HLjUbk3UbsiynaMIWC/OjbTg9CBjGMHPfqO30mykutLFx9maZYdk8hKFVZljkVkB6ffUe3QZzWt8ONLlsmklhAFnGrl2xgsSxcZDdgSW9Du44Oa6KVLld2clfEKSMG68NDTdHIa3mkktZiLQ+UEGw8R/MM4CFM9M8ZxtIryW8tv7OWHVIrCS5KEXN3cup/dPuwYipGeWLAd/lJPX5fZfif4rstK0Sf7ZfQQLahzMomCbWLli/PQlhjcexODXyj4m8W6x8UvH9xpOnQta6VbyssjwSMPMiDcBuxJxye4A9OdqjjFOT6HHRjUrVFSp7vQ3PjZ45bWvCOrWNnaTRWlvDGYLuZy0lzh1Ric5BVhz26Yx1J8ksIWaMOzljsC5PoBgD8ABXr3xs0aC1+EsZgURvCwQqOyHB/8AZR+tebaXbgQL7ivYyy0oKS6nnZpT9lWlS/l0KdvC1XYWeBgy5OOcg4IqQQqshGKVQfMP92vXaseSelfC39oL4o+BfLj0nxReTWceP9Dvj9ohwOwD8qP90ivT/wDhuH4mf9Abw3/4CTf/AB2vmfYuTnpTdkfoal4elLeKH7Sa2ZpTL8p+nSssQSTSGRl46Ct7ZjpWfcWktvI01n0PLwk/K3uPQ1co3FF2ZkX9uVUnbWA9sZrogDgc11MjC9t3jgysqnEiMMMn1qKLTUt4zxlmHJrD2ZpzGf4NttniyyBAwzkcj/ZNezfBLRIPFOmXF/rRVjCcQxv0KdFbHcDGMV5JYo0WuWTrx/pCqM+5x/WvbPCMMmj+NotPj+WygZY5McgxtjH1I/pXBjLwTUV7z2PRwNNVZfvHaK1ZzvxY8LpHJ5emxTRNC3m200ZKtGwzjGOmP61U+H/xy8S6BN9h8RwfaHhxGssfysiehOc9zz15r3PxtrngeyaTShe293qUI/1FviQx/wC+en8z7V4F8VPDlrrkjarpUsNpcxD7joUEgLd2Hcden/1vDhTqwm4ze+x79ephsTSU6EbOOj7vzPdtN8c6J4x0xbRNQAWRf9Kgb5Q4KhShB4PTHUdM9sVB4t0+S1tbiXSr0wi4jWCNYmJwCQAQdxCABduAVUBnwOTn5Ov7DU9K2tcwS2zZyrgho2I7qw4P4V0nhPxfrtjAsCXsjQ7SvlF/lAI5GPxPoe45pOpy7o5Y05PZntF54TS4t47pMM8FsyXOZC29jllOCCVJ4bH+yfXB6/wf4Rt7a8ivpr6OT+ITZDBQEAV8jjcdpUY4wobggY8LPi/XJvKnmuxJsKF1kRlEyr0VtvBHqOM1OvjjxHIoD6xIoXOFVQA2TnJ7/wBKl16di/YVmfTVjr2i6LZRjUNR22jR7f3jH5Ru/hHYkj8OQK4H4o/tB6bp2nzW/hyLz5GwVlRcR7tvAJ4PHHI9eOK+ffEmpXD3Cz3F5JcbVwqyZIHHAGTWLDFc6i2ZjtQnOO+PeoeIXQawr+0T+PvFniPxrqzNdzvPPIxSMQDaXUkYQgdV4HXpXq/wD0keDLy107VrEQx3Q33EroVcZ/i56j29BWX+z/4PjutSfW2ti8Fq2Fdl+Vm78/p+dfRWoaZputeFJBdLFBcKhaOQqN0WB6+h/wA9qeHr06uIVCXzPQqYGrhMveNtvov8zx/9qC3ItbmwtXVoTaCY4xgfMvH5fzryG2hKYx+VegW97da54J8V/wBoIwuNLjZFV/vBCeB/wELj8q4qFNrcV9Tg6XsnKn2/U+RxlV11Co92rP5f8CxBdxDy94HTrUPlqqNIzKqKMsWPArSxkcgVnXFuxut03zQqcxoPug+p9TXczz9itHuuW+QNHD2c8M3uPQVJ9gtvR/8Av63+NWxsZeOlJ5aetCaE0TtJdSKfIhyP7xOBSR291IMSz7f9lak8OvI1rOjuW8u4dR9OP8at9Go3KKC2EEDs6Iu9hy56n8agvE5rWlAzzVO7T5etOwGDOjC8gdeCtzHgn/eFe2+LppNM+G83iO3lZNQuh9ktAq5O9jy5IIIKpvI6849K8Yuwq/OwyI5FYj1wa+g9Ns11KPw9ojEeUkcl0+4cFiwUY+gz+deNmDkq0OXs/wBD1sC4fV6nOtLr9f1szxO88MapotjFqNtJJK07B2nZiz7zyxLd8nv716F8LdKn8ZXyeHyYY7++Ux75eEKhTufA/iABO3vxXX+PtIsvDmpyrIzPFPEsgjRAytnghgfw5HNcd4rltrHT7TxD4QmvNJ1S1Q3kOWDJG0UgBZW6g5H3SCD344rjo2r1XzLbQ9DEReGwcVF/Fr8j1zUPgxc+C/BMNjNLb69ZysfNW4tRGy7lG3KFmBHy8EH2wO/z/wDFb4fW2iq2radbXFrZiXbcQsCRASeCueqn9DxXofhX49eM/FAZfE8FhcR2xAZbVDCZGwfnPJGeTwABz0rf/tTSvGXgvxDaLbTRiSzmDLKi4VthIYEHnBweg6Vx4/BSoyU13PQy3HfW6cqVWKbS0fU+erWCBoB5d2q88kk/4daS7szHGXiv1+u0sM+2a5TT5ZOqNtwelX1MkqghyCxxgmuGUUgjUbQXBPnYd2mfPVjW74Q0W91W4UTo1vp6HNxckHagAOFBx1Y8D613+heAfD3hrSZNV8RxyapNbgGRVz5SZweE3KX6/wARA9vWrN4wbWNBlutK02zs44lZYC9shaIA7cooG2Mnk/KM89TXThsK6i57aInEVI0ZKnJ+8+nr57HrnwS8deCLbyvCsyx6Ts/dKs6hY5OOgY9zz17mtn47XY0iwiGn8C9kw65+WNBywz6HgfSvlzXtDupdHnubi5Wa6uYWdGdjtQLj9a7b9m3xVqniu4Xwh4nme/fTwsUNwzc+RhiEJ6kjYcE+oz0rppYem1dfFvcnEY+rGrr/AA17rXTzOo8faEmleH0uYgV/4SCymS495PKLJ+ip+XvXkScycHqte9/Fbfe+Eb60L7W0mMzxt7jOcfrXgqL/AKvH90V7GXVvbxc36fceJmuG+qzjR+f37fgSY7Go2AzjFTbcjPpUcgr1DyStJCDyvyn60zy3/v1awKTaKBH/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEASABIAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDIzOjAxOjIwIDE0OjEwOjUwADIwMjM6MDE6MjAgMTQ6MTA6NTAAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjMtMDEtMjBUMTQ6MTA6NTA8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAC+ANUDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDydmxSjnPsaXZn2wB1oZAMlmIBristj31Vq25+n3Aq7oznoaqwuYCUOB65PT3q+o+XikkQEHIBOPStaNZRvCSuma1MO5RjOEtV1IGgjI8ws27Gd4NOtptx2MQx6qw/iFVzdJ9mEYyW246dKsra7ZY3Q7QOq11VIcsHGvfrb5f16HNSqc01LDJPbmt5/wBepYFX9MuRaCeUMRJs2oPUn/CqNLXlJtO6PWnBTXKyW3uJYJhLE5V/X1rc1K5spLOTaIGeRVKhEwwbuSa56tnw/oNxq83yfu4QcNIR+g9TVRm0rGNajBtTk7WMhFJYBQSTwAK6HS/Ceq3+1hB5EZ/imO39Ov6V6N4f8OWWmYMMIMnQyvyx/wAPwrpEtx6UrGU8U9oo85tfhuWX9/qGD6JF/iamk+GeVPkajz6PF/ga9Jgiy3A6VoJEOAadjD6xUT3PILfwVPpfmS31q18FPyCD5hj/AHTgk/nVW48T+RIY4rEoyfLiQ7SPbGOK9xjhDcAAfUVS1rwdY6/FtubbdJt+WVRhl/H+h4rWLlFWiZOVOc+aur/M8MufFF/MCsflwj1Rcn9axuWJJySeTmuq8Z+BtR8MyGVlM9iTgTKv3fZh2+vSuWFYzlJv3j18NCjGN6KVmPUYqaMncO/NRLWzoGi3GqzjYNlup/eSnoPYepqYxcnZGtSpGnBzm7I0/G5zrKf9cU/rWGleh694cj1eTzIZGhuI1CZZcqw7Vzh8H6urELFG4HdZBz+db1qE+dtI4cBj8P7GMJSs13MVDzVlDVuXw5q0Ay9jKR/sYb+VVCjxNtlRkYdQwwa55RlHdHqU6tOp8Ek/Q3vCOlrrGrLbSSFIwpdiOpA7CtnX9TaCN9JsbM2NmjYfg7pSO5PcVyen3c9lcJPayGOVeQwrb1DxPqOp2f2W7eNo8gkhACcVrGcVTcdmctWhVliFN2cV0vs+/ma9j4P1O7t0mDW0SuMgO/JH4A0Vy4mcDAZsfWihTp/y/iOVHFN3VRf+A/8ABPKlOUznPOKay4bA6ZFWvKXbt7UBAO3vVc66HmrCzkkpdv8AhxMUjfdP0p+KhuW2QufalTi5TUV1O6rJQg5PojDXhwT2OcVvRusiBkOQaz7SzEsLM5IJOFNOhjntZOm5CcHB617uOVLFNwjL34/ifO5e6uESqTjeEu3QtTz+V/Du4yeegqZSGGVII9RTPIRm3yKGb35AqSGy82ZVgDK7HAC9zXjtUGlG9n36HtxliItzaTXbZ/kaOiaa+pXyQpkLnLsB90V6/pNnFZ20cUKBUQYAFZHhfR10yyRDh5iMyPjqf8K6GPiue1mc1as6r8i9BgH0rQgj3ITnp2rMjYhat28jDpmqRjc1rG3DSYJINatxpzwAMWQjrkGsbT3fzQea1RuZApf+LJzWiSsZSbuN8t45DuHTrW7otyikByNwHrXP395tJXIx7d6rQTkMJN5yOgqk7MmceeNmeg31jbahbPDcRJJG42sCAcj0r5w+I3w7udE1tDpUTSafcklPSI/3SfT0/KvbbHW5EwcZUgAjOeam8SW9r4j0G4spSU85CoZeqnsauSjURnh6tTDT02Z81ra6RpR/06Q39yP+WMJwin3bv/nipZfFd75Yiskhs4V4VY1BIH41matot5petTaZPEz3MbYAQE7x2I9iK0rfwzOsYk1K5t7GM/8APVwW/L/69c6c3pBW/rue44YeNpVpcze19fuX/AKEuq385zLeXDexkOKYlzOGyJpM/wC+a2V0/wAPR8S6vNIe/lwkD+VTJpGiXOBaa1sfsJo8frxU+zm+v4m6xNGC+Bpf4X/kUbPXNStmBhvZx7F9w/I10dn4sivIxBr9nFcxHjzFXDD3/wD1YrE1Twzf6fF5wVbi3xnzITuGPcVkoaOepTdmP2GGxS54W9VoztNR8MpJaG/0Gb7Va9Wj6un+P8652M4PNWPDutXGjXglgYmMnEkZPDiul8V6Zb3dlHrmlAeRL/rkH8J9fz4NVKEakeeG63REK1TD1FSrO6ez/RnL7qKjzRXOekcFio5X2AcZJ6DNWCtQyRrJJ8wyF/nXVSUb3nsjya0pctobsiWeIqDvUZ7E1VvJFlZIldcE5Y54rQ2gdAKQop6qD+Fa0q9KlU51F/f/AMAyrUK1an7OUl56f8ErrJHGipGQx6BQetEIMjeY/HZV9KlaCNuqL+VOVQowOAOlTOtT5XyX5nu2XCjU5lztcq2SFrqvAlgJ757hxlYRgf7x/wDrVy1en/D608vQPMYfNLIXH8v6VzxV2GNqezp+p0cXAq1Ggquq1Mme9B5q2LkIyOK0IEXgGsuN9vcVcguRtGcNzVIbNe3j8tuv41c3DndjrVG3kBXI69smpWlznk+1arYzaEMKyt8+fwqSOxUdCzD86reaI15yxPb1p8d2A3OB7ZpXQNMu/ZRbSK6thCcHPUfhV6LFsC4YMjenaiz1LzF8ppA3s/UfpVe5+ViFQqOw7VW2xlq3ZnH/ABUaaHSF1GwEaXCERSy7QX8s9Ofqf1rxfM93PyZJpmPuzGvevENsuoaVc2khKpIuCQOnevKdT1WTRpGstKtPsSDgyyJmST3ye1ZzXMryeh6mCqKHuU43k/loZK6LqZXd9gucf9czn8qqSRSQybJkdHHVWGDWk2sa3CRLJc3aA9C4O0/nxW/pGpQ+JVOnavGhuSpMU6jBz/jUqnCb5Yuz8zsniK1Je0mk49bboyfD+v3WkzAKxktifniY8Ee3oa1fFOl272kesaUP9Fm/1ij+A+vtXL31s9lezW8v34mKn3966/wK/wBs0/U9Om5iaPcB6E8H+lVSvP8AdS+XkTilGjbF0vK/mmckhr0jwJa3J0S+h1CJo7Gdcoz8ZyMHA6+lYXgPSIbqea+vVDwWxwqEZDP7/T+tdpNcPM2XP0HYUoNUUpvd9DkzPFqbeHgtrXfZ76GbB4a0WJNsv2q4buxfaPwAorOfxXaJI6eTMQpwCAOaKy9q+y+4x9ljXreX3njkp2rx16Cmqm1cfn70kbmVwWGMDIH171Ia6a0XT/dvfqdlGSqfvFt0LVzpskFms7svJGU7jPIqdNNh/shrp5G34yuCNuc4x65qlLczSxpHJI7In3VJ4FQVjeN9EaKFRpXl1/DsamipZ7ZGujDuBHEp4298eprLm2ec/l/c3Hb9KSkxUuV1YuNPlk5X3EFe0eHoxb6NapjG2Fcj3wK8gsYPtF5DEc4dwpx7mvY2xDZADIAAA9q0p7Nnn5jK7jEmWRd3XJpTdRHjzApFYUszo5SNiGPU+lUTG5YqG+tJnJFnVGMScx3Sg+hqq1zLavh3Dj1FcxcPLANybwo6lRTF1lGiKM+GzzuoNEzvbbVVIxkdPWrUWpjaQBj3zmvP7DUV8wKnzseoFbEuoCJCHwvqB1FFy+U35r5i+1ST9KdHJOeQOK4qTX/KOBIM5wTRb67PLcAI+QehAoJeh6LaXEqkGUNgenNb0F0kkQ2vuHevObO+mH+sc7uoIPBrotPuHl+6MPjPHeqTMX3Ne+G6KT/dNcjaiO6lQXMaSPF8yMwyRXU7mlt33dcVyNkcXi++RTjNxqR8zGvG8blzXHto9IuTebfJ2EYbue2PevOvCkbyeILER5yJNxx6Dr+lPuLTWNXvpF2XM6q5Cl8hFGfU8VqK1t4VtZVSVLjWJV2nZysIq5zdSam1ZI9PDUlhqMqMJc059F0MvxTKsviC9ZDkb8Z+gx/Stz4ctsur+RvuLBlj6c//AK64zcXYkkkk5J9a7Bv+Kf8ACrRP8t/qHVe6p7/h/OsqUvfdR9NTuxcEqEcMt3Zfdu/uNvwDKs2h30Mf+sWbeR6ggf4GtcGvMdD1a40e9FxbEHsyHow9DXpGjatZazZ3F20MtqsAzKxI2+px/wDqp8vtkknqjy8ww06FSVW14v8AMptoOnPK8jwks5yRvIANFRv4r0VGwsd649Qqj+tFZexf8yBLG9FL+vmeNrGqfdUD6VYsrOS8l2RAADlmPRRUZFbqK9npMP2ePdJJh2465rRtyvKWp21Z+yiow0uEWkWaL+8aWVu+DtFTDTtP/wCfUn/to1KxnyNiIRj+JiP6Unmzr96AEf7D5/nisudnA5VJa834jZNI06QfKs0R9VfP86oXOgTIC9q4uEHUAYYfhWpHcxu23JV/7rDBq1CSHBBwaFO+6HGtWpvf7zQ0aHTpreKAW0cc8QBViPm3DnOa6a4IWEK0bOAo6HvXEWIkOsybTzvXr7mu8jXeqk84NarREVvekrnEarevZztuilZm+6CMf/XrnrrV9Xj3MohjH8O1N5/WvVbzR4L8fOMP2NZ03hsIObGOX/aDn+VEZJbohxdtzy1L/Xrxys80jRbuNkW1ce/FQj7bJcbJI2IzgH1r2C00pEAC2Sr/ANs8AfnT5dOtoJBMY0Mq9DjgfSrcl2FGDWlzL8DWBs4wbqMCU88jkV2urQRXdkQ8KOAvdQa560YtOSPxrsdLQSW+H/iUqc9qhK7OlqyufPniK2urDUJFjiYqTlcelZ8mr6jpwDRbWbAO0rzXttxpkVxMY7hAXjYhWxnFUtQ8N2Uo2TwoCemFGD+FXFrqYTUujOA0zxZeGJnvLJSikZaM4I/A122g+JY5o1kicbCMHK4IPofSoo/B9sj/ALltoz93aMVs6X4AZrnz0bMQHOBjcfwqXq/dJWitI6SzkhurcPDJuDD5h6GsoaNDa2wnnu1W6z8sOOCPr61pxRfYIhF821Txn+VclLNLN4hHmtiPDlR7ggUK3MmxuHNF+hxviLWNSGpXVqbyQRJIVCphePw61iQRS3Eqxwo0kjHhVGSa6vXINCtdWuH1CS7muGbe0SDAGffj+dUpPEy20Ri0WyislPBkI3Of8/jSqRXM3OX6nsYaq/ZRVCn0Wr0X+b+4uWWnWvh+Nb3Wisl3jMNopyc+rf5x9awdT1CfUrx7i5bLt0A6KPQVTmmknlaSZ2kkY5LMck1NY2k97cLBaxtJK3QD+Z9BUSlze7FaHXToqm3Vqu8u/RLy7IfZ28t5cxwW6F5ZDhVFdX4juYtI0mHQrNwz/funX+JvT/PoKRpLfwlaNHCyT6zKuGfqIh/n865F5GkkZ5GLOxySepNW/wB1Hl6v8DGF8XUVR/BHbzff0XQlzRTQaKxPQMY1u6dqNu9mkNzIInjG1WIJDD8KxbqM288kTdUbFVya1vbQ8idKNaKudZ9qsAOb2P8ABSaVbizkbEd5ET/tZX+dchnFKDU+72MfqMf5n+B19zahlAlUEHkEf0NRQO9vMscx3RtwrnqPY1j6Tqb2jiOTL2zHDIe3uK6KeFWyuQ0bjIPqDScVa6OScJUpck9ja06xzMk+ARwx/AcVuJNsBB6Z4rB0e4eOy2Svll+VeOuD1/LFanJANaL4TOXxGlDPkgg1t2MxZcNXOW5AHXmtaznC5NSapXRo3H3ct0x+Fcnr96lsvPVuFHet6+vFWPk4GOea4uS+V7+SZ1BK8IT296Y4o1dJ/wBWrvwzDoa7HSr6KBIjJlyTgoeK82sdRaXc0ciOucZUg1oxajKh46exqk7Mp2krM6i8iW31ryg4eN18xWHAPtzWvFGjLiRFdfQjNcUmqwyDM5UyRH5WzyueorqNOvQ6ruYdPWlfUlx0LkwgtBlY1BP+z0pseqOPlDkL0xmpTLFcIUK8dOaw9QtzbMShJQmn6Gdl1NG+k86M+vWuamjCIJnHzhmA9snNalvMWUA9+KreKnhhkht4AcqoZ2z95qmTsrg3aLR5v48Xbr7H+9Gp/p/SsS1tbi5bbbQySt6IpNdv4o1mPT7+NTp1rcO0QYSSrkjrxWHP4u1KRdsJht16YiTp+eaqrGHO22eng6uIdCChBbbt/oiey8LSpH5+r3EdlbjkgsCx/oP1+lT3XiC1063a08Ow+WDw9yw+Zvpn+v5Vy9zdT3Um+5mklb1ds1EDUe1UdIK35nSsLKo+bES5vLZf8H5krSNI5Z2LMxySTkmlBqMU4VkdxLmim5ophcj8SLi/D/8APRFb8en9KyTW54iieSS2KIzfu+wz3rK+xXR6W05/7ZmtpJtnjYapFUo3ZWzSirI068PS1m/74NQzwS277Z43jbGcMMVDi1ubxqQk7JjAa6zRZvO0tM8tExT8OorkhXReGW/0e6X3U/zoXVHLjVenfszprbmMHP3Tj8//ANVban90D37Vzds3Ircjb93z6U4vQ85FqKQfWrAuVQHnFYckhVzyapXNzLIyxRZLscCg3jsalzcy6jcfZrduD95uyisDxW0lnNFDbjciqQQe+a6G0aHTrYRqcueXb1NVNSEVyjMQOnrzVJClPscXpNz/AGfIzxQkbzl0DcH3rdTW2eJmiiYE9yelZ1xCsDnPGe1TaeokwuAV9qtrqZqepo+G7V7ySWKVdqlSQQckNnrnvXTaLdyQO9tccvGccmnaPBHa2+Qoz79qj1mEMovISBNH94A/eH/1qlo1jUvodDDcOWBU1YnPnQjcea5rTtRDxqwI6VuW9yHUipTFMgmkNtC0keS6/MoAzzWXq07zXAaVt0m0ZJ9etal3ex2BSaQggttAPckdK5qaUySFvU5rOs+hjLYwfHgP2yzc/wAUAH6//XrmBXomuWFnfQWcl/dCCOEHOSAWHHArJbXNHuP9BmsAtgvyxyr95ffHWt6lJOV27XPQwOMaoxhCDlbf+upy8EMs8gjgjeRz0VFyTSPG8UhSRWV14KsMEV1Dalp+g2zJor/aLqUczuPuD0pV1fTdat/L1xBBdKMLdRqT+YH8un0qPZx25tfw+87Fi6rfP7N8n4+tu34nLUoNJIAsjKrB1BwGHf3pBWJ33JM0Vr6b4b1G/txPFGiRt90yNjd9KK1VGbV0jmljcPF8spq5Hdz3LX1ra29y0KNEWYqM+v68Vmatc3dtLGqX1yyugfDEqR9RVrUvsgvUMl9JBPEgXCRk479fxqlLFp87l5dTlZz1LQkk1vK9rfqeLQSVm1pb+X/gE9pFNPYGaW9u9zBmXax2rt/vGq80jz6CrXDF3SbajMcnGORTlWzjiaNdVm8luWRYiM1T1C7SYRw26FLaIYUHqT3J96iTsjanFyn877WsVK3/AA1xHd/RR+prnxXR+HVxY3Dn+JwPyH/16zXU0xj/AHT+RqrJ5YB9wP1rdhkzGBXMTtkxJ/ekX/H+ldDan92KmOx56WiJ/L8w4AyT0qa7s47eASIMOqnk0kTBWGatzuJkWPPLcYqikcBNdaje3rRWkDbVPzO4IBrct7G+EK7mtl45Bcn+ldfFFGsQUoo9cCqN3YIwJXCn61VwscvLazTNiVrXjp8x/wAKtWGnXER/cpaufQTH/CpJtJEz79rOPVas2ekBJAyySL9eP5076Dsht8+owW7EWcpIGRsZT/Wqeha/9rJjcFGVtrI/BBrrLa0xjzHL1j61oVtBcf2hagpMCN4B4YUriSInt2tpd0YPlOeOPumtS0mxjn8qk+Wa1XPQiq23yjnjikNsqeLJv3Nguf8Al4BqBelV/E0u9rX0EyCp1PSsJ6sip8MTJ8bn91p3+4x/lXKg10/jY/Lp4/6Zn+dcuK1q/F935HsZd/u8fn+Y7NOWm1e0fTZ9UvFgtx7s56KPU1MYtuyO2U404uUnZIbY2dxfXCwWsZkkbsO3ufSu60nw5Y6WFlv9t1d9Qn8C/h3+p/KrVnb2+kW/2exA3f8ALSXuxpGf5hnJJPWtHKNLRav8DwMTjqmIfLD3Y/iy1cXUkrA7igxgBTjFFZ11qFrasFuJlRiMgHrRWLnOTu2c0aEmvdjp6Hl+pTefqFxJ2Zzj6VWpKWtnq7ntxXKkkNpaCKQVNhjhXWadH5Gl26nq+ZD+PT9K5zTbU3l5HEOhOWPoO9dTMwOccIowPYCm9Inn4yd2oL1IAd99GOyKWP1PA/rW/ZHcuKzvDmmS34lumBWDOWf2HQD+f40lpqCz61cpFxFEFVB6daIwdrnG5rm5V0N9R0qxbcybm+g4qHcjKCOM0Rtg8GmWmbUbhgAeKf5cffD4ORu6VmLcYHSk+1lOeooNDY+0omOgA9qUtHOMOFI/z0rLWZJVBI7U9bgLhUwKoRoiLyvukle2e1QzqJoXjcDDDFItwWyOoph3sw20gbKFqXSIxP8AeQ4z60TttUsaum0Z3LJ364rN1bCKqqcjJ5+lKSaVzNyuc/rL7/s+f+e61oIeRWXqB3XNnH6y7vyFaSnmsGgqP3ImV44wGsB/0zNcwDXQ+N2/062T+7CP51zlb1V77PXy/TDxJUUuwVQSzHAA7mvSdLtE0XS0gTH2mUbpW9//AK1ch4NtRcayjuMpCpkP16D+f6V1s8vmzM3qePpTv7OHMt2cOZVnOaorZav9BwJqlquofY41SJfMuZDiNB/OrBfaCScAcmsrRVa7uZtRlz8xKRA9lFcqRz0oqznLZFmy05RGX1AJPcyHLMwzj2FFX2NFMTrTk73PJ8UVcstOubwEwR5UfxE4FaFl4W1e+nEVnaGZ/wDYYYH1PautQk9kelLEU4uzkjCNLGjO4VAWYnAA6mvUNJ+D2oTqH1LUILXPVI1MhH8h/Ou10L4Y6HpXzzyXF1N3Zm2j8Mcj86qNGT3OWrmVKC93Vnken2f2C32Hm5k+/jsP7tW20jUrx0ggsbplk+84ibGPrjFe4WmladZMfsdpFEP9leT9T1NX4yu5UVAMnGat0LvVnlPGS5ua2pxf9mf2b4WitAoV1iLzEDoSMn/CvF9Oka11yZWziRFfn3Jr6L8VQ50+RVUDcNor548Qxm08UMpGMRKv5E1U42VhYeTctTrbebdHjNODlXyKybCYlQRV/wAwMK5zutY0BMCvNMZgejVUSSnZoKRdizt4P61Iqk96opntVqEZPcfjTEzUtU/vGrhkCjC9+tUImEa/1qC4vVT7vLdqZm22aU1z5cflo3zN19hXRHQ11H4fXLLFi5t2a5jbHJGMMPyH6CvOpb/yiZHOcctXu/gqxkTwrAl6uJZov3i+m7nH64rSEea6ZhXlypWPnONJLjVA6I7RRxkBgpILE+takcbb1BUjJx0rp/F/gbxTYagzaIUn0zGUZQNyD0ZcZP4fpXnN1rmr2V1JBPKnmRnBGwf4VEqMYu7udMYTxCXI1ttf/gEXjDc+tSYVsKqjOOOlYddCniq/H3hA31T/AOvUg8V3B/1lpaP/AMBP+NElCTbv+B6VKWIpQUORO3n/AMAseBhiPUH7hFAP51sA1jQ+LjGpX+z4Ap6hG25/SpU8V2px5umlf92X/wCsKVSEZJJS2OGrRxE6kqjhv5ot6q5TTblh/cI/OrGnRiKxt4wPuoKgjvtL1qF7SN5LaWUbVDjqaurE0AEUhyygAkd6xnScVfoYyk4x9nJWZp2caiHc4B3HjIop8K+baxYOMAiivVpQSgrI8uc/ed2dDp3gnQ7RYxJHJOqDCq78D8BgV1dnFZ20IitoUhjHRUUAfpVdh0AqZlwo4zUJA23uWsJt5IH41FJsIwnU/pUPUVKi4GaZJEVC8Cq0zFZ0CeozVs8yVn6q5t4Gl9Dk0gNDVoBPaouFyWGPWvCPizpD2t9aaiqEK2YpDjjPUf1r39dl1aYB6jORXK+NtEGs+G7yAgNcFC68fxryPzx/OpkrmlKfLJM8N0uf5Rzwetaqtj6VzNixgco+fbitZLgqvPIrkaPYNPd6VIslZq3II4NPFxigEjYjkzirSygCsNLn6/lU32kKPeiwpI07i7YrtXgVQkmweDk1We5LZC8+pqorTXV1FZ2KNNdTMEVVHJJq0iHZI6rwJop8TeK4LcgtZ25Es5xwcdF/E19HMFhhCrwOgrm/h34Wg8L6GsKANcy/PNL3Zsfy9K6OdhnnkAZNdMI2Vjzas+d3JI2DKNpzXN+JvAvh/wARln1CwQXB/wCXiH93J+JHX8c10VqCIUDDnGKmyKGr7hCbhrF2Pn7xT8FtRtGebw/crew9RDKQkg/Hof0+lee3nhfWbKYx3OnzRyDqrYzX2HVLVdOt9UtXtbtN0bqRkcMp9QexrP2MWd0MzrQVnZnx8+k6gn3rK4/BCa1vDt7Dpa3EWp2rqsmCGaLP4HNepeJPhx4ist0vh3UxexDnyJ1VZPoDjB/SsC8TUbK3jN/ZSW02MSRyoRg+3qKahGHvLobVsbKpDlkk0+zaZ5ow+1ak/wDZ8TgPJmNF6jniu+v5kFykTMPP8sMy+3rSC/dc7I41J7haytRt3uZFuI323SfdY9D7H2rmnKPK4rW5NSq8RKPMrJfM2La8aBSAAQTnmisSHU4cFboi3mXhkc4/L1FFZxrVIqyZhLDXd3E90UZepjTI/vU6RsCvSPPEHzN7Cpv4ajRcACpH+7QIhT75rO8RKX051HetGOq+pLvtHB9KbAqaFqSx6PHPJklV2kdyRxVBfFUE2rfYr62MAcZilV85PpVPR4zPb3cAOPKfeM9MHt/Oud8WR7DbSLw6uQD6Vk2yoxTdjA8aeD59OvJ7yACbTZZCyyx/8syecEdq5Z1eMbZAc9j2Ne0eHb9pbNWYZz8sikcNXL+PNAh02eO4t9otbrJWIjlD3/Cs5wsro76GIcnyS3PN95Q8ZHrS+e/t+dT3Vt5fIbIz3qmy/MKg7Lk6XTDr/OpBKzNnOBVbGB0FdP4I8LTeKLmdUuI7eK3AaRmUscH0Hfp6imkZzmoq7MN5iRsUEk8AAZJr2/4P+AX0xDq+sxbb2UYjib/lkh9fc9/yqvovhfRtBljure1Nzex8pPctu2n1Cjgfqa6DRdduIdWWNyXSZtrA+p71rFJM4Ktfn0Wx6AxCqT0AFZ0zkwlh/E4/IGk1CUoDgnniluV2Rhf7orU5b3ZpJ90UN0pI/wDVr9KH+7QU9hynK+lQzSMjqAo57063OVNMulzs9jR1BvQmVs024ghuYjHcRRyxnqrqGB/A1VllMU3qOtW25XIOKGhp6HI6v8P9FvizwRyWch/54n5T/wABPH5YrjtY+G2pWyl9Omju0HOw/I/+B/OvXA2/5TwfUVBIx3N2ZOcis5UYS3Q1Vktj5tvrDZcNFfW22aM4Kypgr+dFfRt5Y2t46tdWltOQvBliDEfnRWP1V9GbLFtKx//Z</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCAC+AMsDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD7tkP7s1DIdtsx9qfIcrnNV9QbFn9akDPVsNmprdz0HrVerNmBnPekgEZ3W6UnqGFbGc81n3EayKMcMOnvVyFiYlJ9OaYD880A8UlFABmkY0hPNeb/ABN+KdnpFvJa6C8NzcLkPdv80MRHZQP9Y3HYgD1JGKL2BJt2O717WNM0XT2vtX1C3srdesk8gRfoM9T7CvKfF37RPg/TrpotHguNVaMHMn+piP0LAsf++a+dvip4l1bxDqTXF5qM1xJnHmTSZbHoF6KM9lAFcb9kkk+bzGz2NZ+0RtHDze59Kx/tMzEFU8OWaIxP371ifrnb/Suh8LftCWF7t+3+HZY1/ie0u1lI/wCAMFP618mw2EgOfMNXrGK4hcNHOVxS9oy/quh93eF/GfhrxMqrpWpxvPjJtpAY5h/wBsE/UZFdJb8R4NfG3w8lF4irdSxuyEENkq6keh7V7t4H8ReJdNjjSSVtWsMYMc7/AL9B6rIfvfRvzFVGoupnKjKJ6nToz2rP0PV7HVoWks5ctHgSxNxJET2Ze39e1X0+9WpkSelMmOFpc/NimTcsKAHdEojpW4Wmx/eoAP4/xqeM1CDhqljoAfRRRQBkseKq6q2NiZq0MbgKztRffeMB0XipAiq1Zg7cjpVWrVqcW7H0FJASr83zZ+lW4CRHVSyYNAR3Bq1D92mBLTWbHeivMP2pvGc3hjwMmmabOYtS1xmgikU4aKIAeZID2IBVQexbPagNehznxk+Ja6ldXmk6VdFNGsnMN1cRNhr6YfejVh/yzXoxH3jkdAd3gXjTxQ07sAwVRwijgKB2FR+JNVWHTYrKA7YoUCIoPpXnOuXzyTH5j7VzyldndSpqK8zVn1ASSbmkzSrqa+XgNXMLOx71LG7H+KpudNjq7bU1Kc46VPHqUYrmrcnaOamDMOhoHZnd+GtXWC5V1cg56g17b8OfFJkt1R5BkYr5dt55Ubcpx+NegfD3X5LdSrt8xwBQRKN0fUEjT3luNW0Kb7PrFquY2HS4UdY3HcH3/TrXbfD/AMTQeJtF+1pF9nuoW8u7tmPMMg6j3B7GvGvBWutBPH8/31Bx3rprXVU0Dx5bavAQlnqmIb1R90E/x/gcH861hOxxVKfU9cjOWzSHmWhM8ULzKTW5zjpD2pI+tJIcmhaAF/i/GpY+tQjrU0f3qAJKKKKAMc8c+lZWS0jOe5rRumxayH0FZsf3RUMY6rcYxYsaqYywFW5Di1x70IQyxfExX+8K0YPu/jWSjbZkb3rWh+7TQx9fK/7T2qyax8Y7izDFotKgjtkHbJG9j+bYP+7X1OT2r4/8YFrn4meKJZiWf+1LqME9gJGA/QAVnUehpSV5nkHiq5kW6kz2GFrk7hmZ+e1dl4tsx9sl3/IoJJJ6CuTke2ZiI24z1PesG7HfFFeJctVmFcAlulLDApk4YfnVvyV8skYrPm1Oiwlvt4+b9KtR7D1ai1SJYwvV2znFNAAJ570+YOU0dPgjkYLkcjit/SLFkmSRP4Tz7VytvK0cisGHtXY+DtSspbhba6uBH5nAJNNSuTKJ3+galIZrbJZWyOD7da7++f7ZpsSsCw8vK+1cNpulHdBPE26M8qw6EGu+tICdLG8fdA9qaMJWPZPh3qbat4PsLxyWcx+XISfvMhKk/iVz+NbUfQmuJ+Asrt4SuImPywXbBec4BVT/ADJP412q8LXZF3ijzZKzaENKOlFJVCHR8tipo/vVDF9+p160APooooA53UGItCP7xFVYcLgHvU2pcRoPeoBywqBk0aru69KfISYx9ahb72KmkH7sUgsV5sgcVr2bb4VYdwKymGa0NJP+jY9DTQyz/GK+TviJai0+LHiiDH3tQeT6bzv/AK19PeMte0/wx4cutd1RnW1s03P5a7mbkAADuSSBXyz438b6B468balrOh2d7a/6PF9rS7VQxcBl3DaTxtVfxBqKmxpRvznkfxg86RpIYOEUZb615JeWdzI24XjReq5/rXo/xO1y7uLe5sNKgDXV1OELnsK8813w9aW2ik3N5L/bttcMt7Z3RKqACQPKIOGH459qxXqdT22K0Mt/Zz83u5PQNW1putbofKaTPvWFFpGmx+G0nke4h1KS5O1IkZ0EfoSTjOc9D9aWys03r5sjKTwV71M4pmlKXkdYL/LLIsg+Xtmo9R1KRYd6tj3qCxsoGtyI4mO3vWXqkIWUoGbpkLnqfSs4xVzom2kMbUdSeTC3Bxuz97FaehyXn2qKU3o3A9A2aztP06wl02+F2Lhr3YDbDafLzkEg7Tk8ZGeBWx4F8P6DNpd+mox6gNakQJpdtYhs+b2LsxK7c4zz0zitrqxxu/NsfSnwQlvl0uFLg+ZaTglWJ4VuuR6V6oEC6PMw7J2HtXgnwh1bxL4c0+88M+IoEkktSHtpk6ejDd3HTFe86bcKfCH2yTdsMSufWl1Klex6J8FbQ2/gyWYqF+13buuD2AVc/wDjprr/AGrgvhP8QPC+uLF4d0x7iK6tI/mS4QLvPViMH1z6V3vQV1wtyo8+d+Z3EY9qKO9HaqJHW/MlWF/rVe2+8anX71AD6KKKAOXvDvZSfSmQDMn0p9yczGmodvTuMVBSEz82ak37uOwqMj5aWMYWkA4+tW9FbKSD3zVNvu1Y0k4mYeooA439q7RbnX/2e/FOnWYcz/YTOgQncfKYSEDHchCPxr47+Bsv2jT7lZJHkuH00NKzDrh3VcnucV+gk6K8ZVwGVhggjgivivVPCaeA/jf4n0C3j22K2jTWh7CNpRIqfgJQPwNY1VqmdWHkrSieVeJ4Wtr1jj5w2TXL68zXt808uS7dTk13fiyH7ZduIl3MTgfyrmJdOEE4Ep+bPOawcjtjFMxFsZ7mDy1UKi98YqGLSlS6ByzHPNdDdzQQReWg3uw4A7fWtDS9PMNqZbsJHM+DHH7dcmolN2No04os+H7KOPTwXhwGHAxVLXtDtZ906oQPTHSuktb6VYUJ+ygKpOGYDOO2PWugWxh13wzFBYSw2+oyFsJIcK47c1kp2ZvKCaPKodJKkmE57da1/Btq9lq6XBTHlnIxUNrdG3vpLS+haGeNyjr1G4HBrsfBdlp+pKLXdtl52v37mtuZ7HP7NLVHZeGLlNVuGDrksOvfNek+LtTi0L4HXt85OIvJjO0ZPzSovHvg15x4c02bw9cs9yM/3fc11XxP+1aj8DZLSzgeeS8v4IgicnAYtn/x2nHZmc0m0jI/ZfttW1v9pSC/gupY7K2sDe3cSH92AybUXH1ZT68GvsBjXnP7OPw/g8EeEfPmQNqmqRxPdSd1RECxxj2AGT7sa9FbpXZRi4w1POxVSM6nu7IX+Gk/hpaaa2OYlt+9TLUVvjb+NSg9qAH0UUUAcoSXmb603P8AOn/djbHU8VEfvBfQVmUS0LTsZjBpq8NigBW+7UuncTConztqSzP7wH3oA0x8y14T+1boKQ+JLHxHFatuu9Pls7iYfdHlsHQH3O9/++a92XAHWuU+OmnpqXwr1aPy1d4YxNGSM7SrDJHp8u4fjUzV4lQlaSZ8LaDL5njIQS9AzHBrlfGt8TrNx5fADnH510moq2n+NEmYcFsP+PBrnPFli0via6kx+6i5J9a5ZI9OErMy7MPtMrnLtzz2qlq15qs+tfbWvplZPuqp+U/UdDV+OQSS7EPPoKZNB8x34qeU0cr7Fi18SKIQ1xazGVesaKSGPseg/GqMN9rOo+JItZeedJIziOJJiI4x6BRx2p3kndhRx9RitnR4YV+VWQtnpmiMYRvYHOpK1+g7UftF27Tz5MsjFmfuSeTVzwdqstpqkW5ipVxzV/UbZYNLEjrhs8ZqDS9NFzHHqEQ+TzRHIB/C3UfnRyle0PdfG0wm8PaPer9+ZxuHrwP8a9K+D+htrWl6bbywebax3ZmuTnACiNgM/UsBXkF5crdaXpdgDn7OobOf89q+l/gLYtaeCFkZcec4x9AP8Sa0pQ5mcleo4xujtuvSkfgge9KKBy/0ruPNA01j81OamdaAJ4fu1IvNRx+lSR80ASUUUUAco33eaZCclmPc0+4BPyqOTxSYA+UdqzKHjJGO1J0aiOhz8woAJD8mPepLX7wqF8mpLc4agDUHSotQs49Q0u6sJT+7uoHib6MCD/OpV+6PpUkfDUAfn78ctJn0TX3SePZLBMySj0ZWwf1Fcj4ilDeG7y7/AIpGj+b2719U/tvfDx73SX8VadCWBwt6qr91uiv9DgA+4HrXytJE0vhOa1cEMpII9P8APFc8o2Z3Up80Tzl77UIbotbW+/J+8T0rQj+3yoHeIliOctVvTY0idt4HFF5NGkmVYj8aNDaK1Kywa0WHl2BZSM7vMAFami2WpvcBZYY1H/XSqUepEfL+8wP9qt7w/cwb1dgx9QTUto00exm6trPiJIzY3ViBZRyfLKWyfwrt/hSzXeh3cbA4kmi2n/aBJ/lmqmrGG9sdjIuAMDArb8E240/RHniGFUFUHq56n8gKL6GbTT1Z1ng3zNQ8WpZoCwysaDHsc/zNfafhWw/szw5Z2O3a0UQ3D/aPJ/U18qfs+6dFaeJLG8uvmubqUGJT1Vd3LH+Q/Gvr1gc1vRW5yYqWyEHFNT7tObIWgcCtzkGsOM00dadJ92kWgB6mpovu1AvpViOgB9FFFAHKzHaxPftUcf3c1LdgfnzUS8RisyiROtJN0zSQ9ae33eaAI2PSpITk1Xb71TQmgDVjP7tfpUy/eFQwnMKn2qRW70AZ/juzW/8ABuq2bbcXFjNH83TlCBX576kbV9RurUHY24hl9/avrj4qfFbTL7xtpPgXQbgXD3eoiG8uI+UygLGNT3wVG4/h618U/E0XFh4ou5U3RyJcPuA6qQeamtFxtc1wslLmsc/qEbRXjqOzGqFxFI7Zp8mrieQtKMSd/Q+9QzX+77oxWDO2LsTW1pIeeDWxo9rOGDD7oPOK5+C+cN1NdBourRpH5ZNKxfMjoIFZ2WMdSa7p7nS9G8MWxuGUkjKxg8sa84XWYIl80Dcy84HeqcWoXeq6st1eOSo4jjzwoo2Qt2e//AHUJrzxjDdz4DNIhVB0Rc8AV9HfD/4hpd+Pta8Ca9LHHrGk3BETEbftUJAZHx0ztZeRxnPSvlr9nK5N78TNH0W1O6Wa4SWcgfdjUgtn68D8a9M/bYsZfDfxS8KePNMIhnuY3sbiToGZDvjLf8BaVfofaurBx5pWfU4cc+W3L0PplucCjFeY/Dn4n21xZ2aa23lxXEYMV2einusnpjpn8/WvTo2SWESRurKwyrKcgj1BroqU5QdmcsJqSuhj80gpzjikYVmULH96p0qBe1TR0ASUUUUAcncNvLN+ApmeKWT7qrRJ93pWZQsJy1SP901DD96ppOENAFbPNSx9ap6le2enWb3d/dQ21vGMvJK4VR+Jrxn4m/tG6JpRez8Lw/bpun2mYFY8/wCyuMn8cfQ1pTpTqP3UZzqQh8TPf7q/stO0s3eoXcNrbxjLyzOFVfqTXzj+0n+0FBPDL4U8CXZ/fApd6mp2/LzlY+446t+XrXkHjn4m6j4ltGfW9QuJZpyQOQViQHnYuQFycjIHQe9YHhPTtLu9UFxNKfLUF5GNuxwo+nqePwNehRwcYe9PVnHUxDnpHY6b4RXUMPx/8F27yr8lyV2nszRtn8eVH51X/bc8Ky+FfiO2rQo39m625kXA+WOU8sPx5P4GufutWt9K+I2la4k0gbTb2Gc7oQoAVwxXgfUfhX1h+0R4NsviF8LLi0cAv5QlglAyUOMhh9Dg479K58fC8kdWBqcqPz41G1D/AL2Ln2qCLDRbWGGq3cRXel6rc6TqEfl3VpK0Mq/7QOOPUeh9KZcxHbvUfiOa8jms7M9rlUldGZJbakJDsJYH0rX0u3mSNWnY59DUMMzR8EEirUdxv5x06U+ZiUEa0kqfZVT5QMU2G7W2j3Z596zxIW5/Wqtw0txcR20CmSaVwiKOSWJwAPxpbuxb91XPqz/gnD4el1DxRqPi+5QlVYWlsT6AbnP5lP8Avk17F+3lpov/AIPwSquZbTUYnT8cof8A0KtP9knwbH4Q+Hlnp4QB7eBVkbH3pG+Zz/30TUf7Z7sPg/eBM7lKuuOuQwIr0MOrSieTiJc1zyz4a2Grah4L8g2jO6puVRsBZh1GfMPUY/EE1teE/F3jPwhdLbNPs0/dkRzvHtx6jLZH6e9eL/DHXr2KNZEfyZMjlgWBI6ctk+o+hNdN4qW4uYftayrsuPniKxBSr91yPXH5g+te9Knd2lszw4ya+HdH0vofxV0aby11I7RIPlngVmQ84OfTB68nrXa6XqWn6nbibTryG4T1jcHH1Havhi11hYYHguLppDncgzk5xjGe2RkfiD2rU8N+NdT0PU1FpqNxEf4XjkIz/wDrH8xXNPL4tXizqhiql0nE+3sHNPjPNeE/Df45S3Gy31hUuVGAZhhX/HHB/KvXvD/inRNVZUtr1FmYAiOQ7Sfp2P4V59TD1Kb1R2Qqxkb1FIppaxNDkG/1uPSibhqxfFXirRPD6+Zqd2FkYEpBGN0jD1x2HucD3rx74nfHfVDHJbeF9NFqQNouJsSSfgp+UH65qqdCpU2RE60Ib7nsviTxLoXhu2+1a3qdvZx4JUSN8z4/uqOW/AV5R46/aHsIrSceHbBiicfa7zgE/wCygP15J7dK+ftUm8ReINYa+1a7muJpSPnuJxliTwM5OBz6VkeOoZwq2MTRCKP5CUufvNgFz9z/AHQPoRXo08FTj8TuzjqYqb+FWJfiX8TvEPizUGOpalcTKpJCbsIvsqjgdulcfJeHa87A5UZBz3PA/KopLCaM5kjZdxOS0pI/RR71HNb2ozE100zE5KxqNoxkZz2x9eldWi0RlZ2uQJJLcXO+TG0AZYH7qj0+g4HviuhW4XT9L8twFecebKpGdqDov5kD8TWbpNlAreZ5w2R4eTgvgAZGWUdM59entVbXb37Tv2k4dupPRV4AOfz/ABouCS7DGmF1NvkCt1dti4ZgDlsEd8Z/Kvvn4B6v/bnwn0W4lbe32NYpCe5UbT/Kvz+ExjhhnRdwTAYnv/nkfhX2H+w/qv2n4Ymw37jY3TxjnscMD+TCuHGK8Uzpw/uto8u/bq+FkthdHx5otuSsZCaika9U6LLx/d+6fbb6Gvn7TbpZrfaT1FfpR46TR5NLaHWHg+z3KGNklwQ4IwRjuMGvgT9oD4bzfDTxwiWcpudD1XdNplxg8KDzGT3ZcgfQg149amnqj2MLVa91nLx+TgrIlK00KLhRVKaVg2etNMgPWuU7tC004EbGvUP2L/A0njH4rrq1zCW0/Qds7kj5XmJ/dr+YLf8AAR615RcAm1yor7Y/Zb8Nr4a+AuhtaHybnV4zqF1MOGYv90Z7YQKK3oq7OfESsrH0v4RtltdDijUc4yfrXl/7Yk/lfDW4c5+VlPHswP8ASt74P+I7uXVbnQ9RnaUhPNtnc5JA+8M9+1cb+3FcJF8M2jclVmnjjYjsCwz+lehR1mjyqmkXc+StAvp7S+PlMAUVQ+P4mPJz784/AV3ekXM2rW8lvKT5ch2s+QDHKPf3Az9Qa830Wdbiczv/AMtpS7duOp/nVy6vJI3jjWUq0jKdwPQkjB/+vXvdNjybN7M2taYWV8qvcQtMzFJUiO4Fuuc/dwRz1p8lrf3AFw1pJGipkMHDN7HH0A/L3rC/4S+xmsUgjkkbHmmWSVd25m3qASckkbh7cVY0fUJbXdtBTduI2HC5xxleh+92ApRqc17MJUXBrmVrmvoV5cJL5sFwMfeARH/LhfqK9R8E6/f3Vj5WHlkjJKKIHHHccr24I/3gK8jt/EU6iJ2ni+YZysZOPX7xHfPatTQvFV1Z6lG39pT+WGz8qKnHQ46/wnP4U5XaBpJ3Ppnwb8R9b06OOO4DXVuAMrMj5A9mI47da7WP4naO8YZ7S4Vj1AZDj8civle78U3dhdMFuLkI43IfPH3Tkjjb67h+AqMePr5eGuLvI/6bp/8AEVzSwkZa2NqdeSVrnm2teO7/AO0XlsNQnY+Z5plklZmfIxyc88jr/tVyl7r1y7bxKMtzk5P86wtaeVdVQ4wS5jYehPPP4gUzfJJhNrEs2AOua126EJJq51eg6lKu64bym8mIykmJTzyB1HXrWPq99M14++JWKjaSE2/N1bp/tEir+nlI7Hf8pEjmU7hjKJwAfqQPzrnL6Y7juOWY5J4PJ/8A1ii4KKbtcfcXwEbkRL0wPmbH160yaWSaFQ7EhDgqBwO3T8P1qPT0Sa7QO22NTuO5eMAZP8qkaKS3uvJlZWaRAxYdMsM/zxWbZp31NnwtMS/ksSQdy9MDnkfU/eqjrkTR3TK5JGAcDsRwfx4B/GnaT54ukkjUnIzuzgArz1+nH41tarpDXOJYFa5P+sDDKxAdDz36rwPzqmRfsc5YiSe1kixtUHlj0Gf/AK4/Wvpv/gn/AHiiHVrASFgpjk+6QCeQSM9eAor55jgtLOb9+ftM5U4jTG1M45I6DnByfSvTv2Q/FVxYfEy+gUQt59g7JEpP3gy4Bb2yenbpXPiNabN6PxrzPojxwz6h43m3PuhtY1jVe27kn+YrD+Jngmz8ffD688LOii6x9p0qU/8ALK5UHA9gwyp+tbmlW8k6GWeQSTOxaVsY3MTkn2rQiia1lWZOqnIrx7HprQ+A72wlgmeGWNlkiYpIjDBUg4II9ahaFQvC819DftM/CjURrV9448PQ/adPv3NxeW0afvLZz99sD7yk5Y45GemOa8Oa07nFcM4uLsz1KU4zjdFCKLMKgivv3wbbvZfC/wAL2bj5o9Jg38Y52D+tfG3wg8IP4u+IFhog3eTI/mXLL/BCvLH2yOB7kV93ahZQw+HdJaEqVW38nCn7u3HH6/pXRho7s5MZJaI5nUJLqyWO9sJvJu4ZAYZPQ57+oI61yf7V3ikeIvhvbwyxpZ3y3AWVHQPG2VYZXPUc9OorudUtTJBEgPV8n6AV4Z+2A/2bw/ptqWH76/BYEA8BGz/MV6GHi/aRPNrP92zzm10WRYYw1tuygUPb9Rk85Q9fwPFYmvWtzLcXEtp++RAdskfVey5HUckCtPRdSa0R5IZmhWKPgcvGS2APlPK9TnBzx0rc8OzWGpXEU2oWwiJlBN1Ecrhfm5ZeRyF4PrXs3ep5btpY8gkWXRbwWVy+99oIaLJ8vJIwxI4Pyjp6/l1/gu7e6tWFzvaPDMMg7sHGcg/St7xVoEd5dfaoPIvY5JXlViVWRlX5V+YcEkqetU9Dt1sZAssckZkdUCSx/ngjgj3rno0I05uae531sdUrUY05rSJUuEZI3iI5hc8Dp/nr+VLDd7V3snEbBu/I6Efkf0qe8tLlbp0WCVwVwxUE52naentz+NVI7O4WQK6eWrgoTJ8vP44rrOFONrWOtuJjc6DayMwZoGMLkEduh/T/AMerM+0Rr8pB49Km8PkTaTJC9zErSQBwFbeA6HH8OfRfzNV5oSZC0Mv7tsMp8pjkEZ9PeiLE2uxxerWNtPpl1NbXIl8oqyxSHd3yQP4hgbjn0FR6ToU89wojtoWZVyFjmIbccKMFvcg/gaks3a4sb6WZY5PLtZWJZcNyMA7hzkAH86j8EagC0dw/2k/PlQLjABVRjt7/AKVl1BbG14h06e3he2WzmVUCwqPtKNgKASeB3yv5VxupWB83aYrxSemYcg/jmtvUtdkuph/pFwofMrB0WTqSepx2x+VUre9uppJFSZZCF2/vIsdfoaWpUerK+g6MZbhVaYKJHWPa0b7gCc/3fQH86sanbPN4gk8oJMSxxncFUDjPIHOQQPpXX+DW1KJWnMdk/lRu6g7hx05/I/nWB40kuVtCZYosBtvyyntye3ILMT1pD2Y2EWkBHmk3U8f7xIUUbVI6/KOB+Naeqa08+khHnEUds20QW5yxiYfxN04Ujp/d5rioLiaRjGu1IwNwReF/T8K0tDdWj+zldyuWhOe45I/mf0pPVDe+hUvA/ltCAsUcbEFV7+hJ7/U10/7Pt8bP4vaS/CrOZIm9fmQ8f99AVzW0lvLduZA0TEf3lzg/pU3w/u2tvHOjXyj/AFV/A5HcjeMj9D+dRUjzRaNYe61c+59Fc7Qc/eHNayFWXDVjaTxx6VsxruTdnmvIcbM77lnS4WzJGspCnkKRkGvAP2m/hG2nibxd4ZtMW/L6haRLxH3MqAfw/wB4duvTOPf9PYiZT6Gta8hR4WVwGVhyCKmUFJWZcKjhK6PBv2I/Cfl+H77xTPF8+oS/Z7diOkSH5iPq/H/ABXud042+Sn3EOSfVu9VvDmjWHhzw3baFpEX2e1to9qAHnGcnn1JJ/OrDKAoUcCqpxUUkKpNzk2VbriZV9Fr5y/bSuP8Aia6Habh8zyuQfYJ/ia+i7o/6aw/ugCvmL9sku/i7TG3YWO3kOPqyj+Qrqw+tVHPW/hs81tHc2pKP80rH5T+Hf8T+VdF4fley02a5ikeCRIjyued3P5YVPzrmbYGNV9VX5SPxP866iZhbaKu9FdWdm2+ynGPyUV6zvZHmS5XJmTqGpPb3bFB5ZiVIN8Hyn5Rk5XGCMk9h9a3/AAvqIvoxHdamsW0743XEb7xyAc8c4XpXD3zkyDuc/NkdSTn+tbPhW9uLdT5LquJA6sUVipBxwSOOAKEuZ2KleKO38Vx6JPdJOZ7i6SVVfcWdiQw2sQR9E/OsS8XT4oG2aLdMFGQXhPGPc/jUuvX95LokSG7mIhdo+XPKkblGPbav5VyLTSPclHdmVjzk889aOXQIu7Oz8FeII7W68qK0gt0jl+UNOo4cbSSBz12UmpeLDYahNaP9jYxyEA+TIflzkD8iK4HT3e31NkDdVZeD0I5B/MCu6jjtruNLiaMl5EBOQD29agD/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEASABIAAD/2wBDAAMCAgMCAgMDAgMDAwMDBAcFBAQEBAkGBwUHCgkLCwoJCgoMDREODAwQDAoKDhQPEBESExMTCw4UFhQSFhESExL/2wBDAQMDAwQEBAgFBQgSDAoMEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhL/wAARCAC+AMMDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD9QKKKKDUKKKKACiiigAooooAKw/GPjjQPh9oc2seNtXsNF02AfPcXkwRScZ2qOrN6KMk9hXkn7Un7Wvhr9mvw/i68vVfFV9EW07R0kwcdpZiOUjz+LHgdyPyF+NXx48X/ABy8TPq3j/Upb+UFvs1spK29opP3Io+ijp7nGSSeaVwbP0H+KH/BVbwloNzNafDPw7e+ITGxVb++m+ywHH8SoAXZT77D7V4LrX/BUv4q6hMX0q18LaZD2ji093I+pkds18XLH5ikSBVYfdUcnjrjtiolhaDG4zrk/eIJOPekTdn2toP/AAVI+K9jMjalaeGNYhH31k09oyfxjcY/Wvevhb/wVW8I+IWht/iV4evtBkbiS90+X7VCrerRkK6j6bzX5cQwxRtvcsBvChY8jd9cfXFNN20kgjZlDDJ+7gsO2TTC7P6DPAPxO8K/FLRxqnw/13Ttcs+N7WsuWiJ7SIcMh9mANdPX8/XgP4meIfhvrlvrfgfWb7SNQtj8k1tLtbA6ow6Mp7ggg+lfpV+y7/wUZ0f4gfYvDvxsNpoGvykR2+sR/JZXjdAJM/6lz6/cJ/u8CmO59t0UisHUMpDKwyCOhFLQMKKKKACiiigAooooAKKKKACiiigAooooAKKKKACvKf2kv2gNF/Z4+HN1r2tSRvqVyrw6PYnlrq425GR/cXgsfTjqRXperatZ6Fpd3qWsXMNnYWEDz3NxM21Io0BZmYnoAATX5TfE7xJqf7aXxe1DxFdNcWPgLw27WmjRyKRuTP3tp/jfG4+nyjoKipLlRUYuTsj5d8WeKvEPxU8V6jr3iS5vtZ1XU7gyzzMNxZiRgAdAoGAAOAMDpS23wt166kiK2kxjnfB3elfVq+B9F8Nxm30WzijYgb5No3Nj1NT2uhjjaMgf1ry6uPkpWhE9Ojl0ZRvOR86r8AfEEihrWG3kLAbR5g+Uehzxn8a6G5/Zp1uPT0byglw6kSI0oIXk9CO2B79RX1B4d8OrHIhmCkIc88Vv6tbC8t9sBfCr93OR+H+e9XTxFRxvIirhqalaJ8FXnwW8Q6eLhI7WYmN/aQMPUEZrNf4c67NZRrHpc5nEmNxgbJx7Y46V9m6hpPl7gRk56is1dNZXzwP6Vl9eqXtY2/s+na/MfF994TvrGRPtFnOkrEeYvlnjjrtI7HP5VTmtJrCQiSKVEOeSmMHsQSOK+3p/DsEyZlhR3H8RAz71x/iD4T6TrkbpJCIC/B2rkc+3T/8AVW0ca+qMJYBdJG3+x/8At9al8KZLLwn8U57nWPB/EdvdMxkudMHTK55eId06gfd6bT+pmh67p3ibR7PVfD17bajpt/Cs1rdW8geOVD0Kkda/C7xb8DdS8OzTz2P7+0jbK7TjaM/pxXu/7Gn7U2qfs/a9BoHjGe4ufAmpzf6RE2XOmOxx58Y6hc43KOo5xnr3QrQlscM6UofEfrRRUNlewalZwXenzR3FrdRrLDNGwZZEYZVlI6ggg5qatSAooooAKKKKACiiigAooooAKKKKACiimySLDG8khwqKWY+gFAHxf+3N8WJvEl0vwo8MzNHBIqTeIp42xkHDR2/0xh29coP7wrybw/YWnhPwnb6fpaLHbwL+LueSx9zVPX7ibXPEusa3qCn7Vqd3LcSM3UGRtxHHpwPoBVe4vGaBY0PCjAryK9Zyk+x6dCiuVFeW4M90zSetbGmSRBvmwe5rBt7dmbPJJraggaNQyhc+4rkuekkrHUWt8kZwHwwxj2qSbUgy5jYEdDjoa5f94zcgEH1Hap/L2x85/LgCrVTQydJXJ7yZZkIA3Nn+EiqmYYJAJGyRzx0p0kG+MAov4HkVF9nVVKsoYk5y3UcdvSoUtbs05dLIfNMrZ2jIznOarMAzfWnlRt2qoT2FMjyrDJBrRu5ko2K95ZrMpikUMjjG0968o8VeA4o5JljVFBl3hthJ5H/6v1r2ZcKSepxx71zeoR+dO4kyewYDt/nFXTfK7mVSPMrH1r+wP4+n174WXPhfVHZ7nwjOsduzHlrSXc0Y/wCAssi/QLX07XxX+xbGNH+Il9HCuyLUdLdGUcBmV1ZTj6B/zr7Ur1qMuaNzyKkeWVgooorUgKKKKACiiigAooooAKKKKACqWuZOi6ht+99lkx9dpq7UdxGJreWM9JEK/mKGM/MzWIzDIYs8dG4qvHaFkU9M1oeK2is7q6mumIigZshepIPQV4N46+JHiVbx5dFHkWY4jVF3Mvb5q8Fq7Pbg+WKsrnuNvGsTfMRmrf8AaUEGQ2OR+VfHM3xS8W296H+33e5eGWTnP/1vwro/D/xc1Oe4jGpO7BeCrchvxqKkHCN07m9Kpzys4tH1N/akKx8FB3yelC61AqgZ2564zk/j3FeQaf4zN9gMVJxn5m4rRbxIFZjG4JXqSc1wfWW0ej9VSPTG1OFnZowNxGOtOjmjuMbmFeH+IPiJLp0JeIE88rH0Jrh9T+N2usrR6cDEQeTjqPcmtqLdU58QvZdD60j09JVypAqC809rcA9c9CK+RNO+LfjOaQCO6vJMNwkfOfavTfCPi3xlJPFc6tPCYG6Wt0MbvowHB9jXd7PlW6PO9o5P4WeuTXHl5BFZvliab8eKq2fieHVWaK5tpbSYcHdyvPow4q/aRFbgBcY6A1nfWxry+7c97/ZPtGX4hxkAkR20pPt8pH9RX2RXzN+yPopbUtZ1N1IEMCQrx0Zzk/8AoH619M17GFX7s8Wu/wB4woooroMQooooAKKKKACiiigAooooAKKKKAPy0+Ilyt54omsGfav2yRSPfeRzXIeINW0fwzqRso0+2Xca5kjSPzCue7dlHuxFb3xU0u4j+Imt+SGVrbUpwox/EJW/wryi4+Hs8OpnU/EkkGtW95cTST2Mlw0O1mK4fcOCQBtAPGK+elCN3dnvUpSVuVF3xTqmka1pLlrTS2uG48qO7tjKPThZT/OvHby3EN04sS0JU5MLjp6Y9vcVoeLvh3FqHiC5l0K6sNL0zcWjhvcqyH+78isCPqewrT0X4W6hqFul14burTUIbIKbiNrggOcfMULADt0B7VpKlTcVyvUKdarGb51obXw/hlvpESaNg5xtYfdx+PU16dqHga4s7RJVjk/eKW4XAFV/Dul2Wkap5elqzIJAE3DLAYBOfzxXsOoTxtZRpOCdtv0I65ry+SLk0z2faSUU1qfJHjC3vrOVlYN5e7gtz+tZOh6XFc6hGt1HLcu3PkwgksPw7e/Qete4fETwzb3mjTXVojSzxg7UHcnkAV5dovw0uLe5B8b6tZWlvOA7WUNyyMxI43OFIOM9AcdeldFKnyxu9jlrVeaVluelaLqlj4fjt1t9HgifPKpd2ob6czZrqLrxZ4e1uaKyvI/sV4/3IrmPy/MP+wT8r/8AASRXzZb/AAvnXxEhmls73ThL8ogY/MobJBUgHcRjkZr07Xvh2NV8i38HwXOlaSsQFwt9deeJ34wyxf8ALMjHVWH0HfrnTp7KRwwrVb+9HY6rVFj8P3cSpkxvwo7Dmum8P6sbpoVY5IYCuI03wjqbWEFtrF39pFqoWOR8sxHue9dFodq8GoQRJwd47YrKMGpXZpOacbH6Lfs36ANH+HMN1gB9Wnef/gI+RR/46T+NeqV8Ofsx/FDWrr9oqDwfJrGo3ll/ZNzNJYvcM0FrDEFVMIeATIeMe/rX3HXuYealT06HhV4OEteoUUUVuYhRRRQAUUUUAFFFFABRRRQAUUUUAfnh8Z9Iit/ih4qWIDnU7g59Nzlj/OvI9W+FNt4hkZmluoJD/HBMyn8s4r2T4vXSyfELxHNlT9o1a4I+gkIFc9aTBVU5GB19q+brN87sfSYZL2SueTW37PeiQ3QfU5NR1AqR8k8pK/oRXazeH7TSNKNtY2sFpaqgUKqjJx9P8+9dPceJLKymSOGE3c7rwqpnLZPf6VmXEmo6+Sl9YpaIzYjUPuIHueBWM6jjHVnVCnzPY57wV4fSS+Lsm8lx15713PiWFVjuGeMpsIjU4A6Vv+AfBKtcBQhKwr5jnHXHpUmueFZb+O7WIqVhY456+wrm5KnLzJHR7SnzcrZ5ZY6O18wiUBlZt2M45xVjxT4Ot9ZsxZ6xZRTRr92QfeU56gg5U1P9ik0e6DbpItrndit2z8RaZNc/Y7m4Pmjkb+PMHqPUVrSq80bXs0Z1aXLK9ro8U/4UPNDMW0zWbmKINnyyqsVHoCQDXWeHfh1NpfyzXFzcsDjc7dfoBgfpXpJtrXzt0ZXa6sVKsODjgUWrP5gMahx9a3ipdDCTXU5C+sXsSVXI29RT/DOm/aNSjkcfcbca3dbhaSQ+YoBYkce1S6HZ/ZY55ZBjCmuiF72Zx12lG6Or/YZ8Jfbf2lPHHi6EPJaf8I3DFG7fwvPOMr/5LN+Br75r5m/YR0aO3+Hur6qkAhe/vI4D6nyk3fzlavpmvWwkXGirnlYyfNWdtgooorpOUKKKKACiiigAooooAKKKKACiiigD8wPjHrkkHjfVlYlQLyUsffzG/wDrVwVz46EcJCyZYDHUmul/aNb7H428SQoRvt9VuYz7ASsK+d9Y1Z4jsDN34r5itCTnofT4SpFU1c9Q8L+O/K14Ha0pLjzGyTgHtmvSm+NGjNdrZssKXJP8XysPwNeSfDFrRkCzJgEZZjwGPqTio/HtrpEdwV1IwuEBaB943r1Jwc5xxWSoSeh0vEQ3PfD8Vkt41SCUwsi4+Q7SQfU+lWdK+KkUUEiTyqyyZLbsZH418lSeOIo1SCG5lkjiGEklGCR2BPf6+1Y+q+Obu8kFpZSumeHfByv0rFUsXGpa5u6uDlTvY+ttS+M3hOOQHUILaSRmwf3uM9qyLjX9E8QeeumsixSR+ZDtO4wuDwQe3HX6V85aB8N4PETwtrlyTuAfn/WFeuR09R+de36R4WsdD0xbPSViggjGWaTLNIcd2NbOhO/M3d+hjGvDlslb5iab4xuIbjypH80j5SeePQ/nXQ23jVIId6n515Ybu/1rxvxRfP4f1JmU7lLZ4OOvp602z8RiaPdDJuLejd/cetTBziVP2cj2seKBqUiszgE4O010d5eLbeF76ZeCsBK7ep4wMe9eG6PrDCZWZgAWB256V2eseJB/wiT27EbrqVEC9wM5yPyrtot3PLxduh+hn7Lfh/8A4R34E+FIpI/Lmu7T7XLzncZCWB/75216tWX4V0ldB8L6RpkeNmnWEFuuBjhEC/0rUr34LlikeFJ3k2FFFFUSFFFFABRRRQAUUUUAFFFFABRRRQB+R/7ZF5N4V/aK8ZaVfDba3V4t1Cw5wJ0STJ/FjXhOrWqSTQy7lYFQwVSCW9MV9cf8FWfh7PD4u8OeLYXVbXU9O+wSqM5EkLO+fQja478Y96+EdH8TfZLZredixiA+YemK82th/e5onfh8TaPLI6zwz8Q/sviIW+oTnT9N3bZHxn7oA25HHUfrXsjWfhXU7OG8v4pL+IKSrSXW3cT6YGcc15Z8GbexvL++nvLWKeFVO+KWMFTGSB39s19I6L8N/A2pWdrC+nWjIy5jm3lc9hkggev+I5rixL5Z2joelg4qcLz2Z5F4i8F+DvEcaC2S+0e4j5VoplnR/YgkH8jXMRfD3QLK7Xyde1F2VgxA08YB7YxJX1LP+y94PudPMljc3Vg74Ytb6hvVM9eJMj04HrWZN+yDpcNvNdaf4s1XZwYtqxDaP9rj68CsYyrx6ne8Nhpa3X4nkml+GdMXypI9X2+UoKm4tpI2c4ycnkYyB9ORTtW1+/8AC+kTfaJRfwquRNDKHaLDHHA4xj1HcmvQL34A2+n745/FupBCMbTJGzN+GzH/AOuuN134F6DbTBr7V9VuoiP+PVpwpk/3igHHtjmqdSX2tjmlQgtInkl546tfEjpb3G53Zm2TAYI544A7jHftU2nWklnI4jyy7v4T0HWud8UeFYfB/ie5h06Nls7d1dMc7QcfL9cgirOseOoodPWO1g2XOzcSoGAOeQMe/wCldc6KlFcvU86Fdwk1LodxFrkel26zTSbSD8oY9ePX0zXSfCW8j+JHxQ8O6Vcq3/E01W1to4wOArSgEnsCASc+gr5yj1qa6kj86UAPw3zEjP68cV9g/wDBOrQZPG3x/wBHkktI1t/CtpcalcsFwS+3y48n/flBA/2fataWG5XqY1cUprQ/WmiiivTPPCiiigAooooAKKKKACiiigAooooAKKKKAPlb/gpJ4Bk8Yfs23uo2ce+58K30OofKoJ8k5jkx7YkDH2WvxousxzSCMuNwBZRhQPx71/Rd4l0Ow8T+HdT0jXokn03U7SS2u434DROpVgT24J5r+fX4qeGX8F+M9f8AD0Vxb3C6RqU1sJoJBIkio7KCrjhgRjnpUtaiZZ+GnjiXw3rTRBkFvd7Y5Fbpj/H/AD7163N4k1TS1a48PSrLbH5nt5QdoPt3FfNcSGK5DLncgBZVYE44wMevNe5fC3XrTVNJkh1Y4lgTOQxKuOSSeOOP615GZYaT/eQPbyrFxX7upsX1/aYvNHbyrq0vI9mFIWQMh+nA4qz/AMNXXmpOtvaxagFbqAVGa0rj4X6H4oVJ7V1bzF3leNyjOPbNJZ/Au0sf3kk6IfvbT02/X/PWvK/dpaxafqeynWctJpr0ILP4o6/q0m61QW2/jzpX3v8Ah2H5VqXPiv8A4RvT5b/VHe4k6lnO5i31q9D4P0vR4N5eO4iLbQM4yeflz0z/AFrzX4oeKLZtNkttJgk3x/K0rnqpGeccD+XFXh6E6klpoZYnE06UXrdnEeLvE517Urm4nd9rtvRskkjPbkcc1y13dLNPG8gaRHATJfnA6f8A6qqySfu22oQrtzkduMEn8D+lJbZaHo25k2/5NfTQgoxsj5Kc3KV2WVbYfLtw2SSM7eh/pX6Y/wDBO7XNA+B2nvp3xOR9F8Q+PreDUNL1C6wIpbIFkjjJ/gYuHbnggryMCvnv/gnz+ytL8dvGa+IPGVmzeDvDdwJJvMQhb6ccrAD0IHBYehA717l/wUo8nw/8SfAR05FtkTSZolWMYCKsq7QB6Dca6sHRjUrqnLZmVWcoxuj9IlYOoZCGVhkEcgilr4K/ZP8A2yrPwvoZ8N/Fe6uTp9qoOm6gsbTNAveJwMsV7ggEjkdMY+0PCHxL8K+PrdZfBviDStWBGdlvcqZF/wB5PvL+IFa4jCVaMmmtO4U6sZLzOlooorlNAooooAKKKKACiiq2papZ6NYy3mr3VvZWkC7pZ7iURog9Sx4FAFmkZgilnIVVGSTwBXyv8YP2+vC3gzzrL4e2p8TaimV+1SExWkZ+v3pPwAB/vV8b/En9q34gfEp5U1rXZ4LOTOLGyPkQgem1ev1Yk+9ejQyytU1ei8znniYR21P0S+Jn7VXw++GKyRX+rJqeoJn/AEPTyJWz6M2do/P8K+XfHX/BQPxVqxkXwZYWHh6x523Eqi4nI9QWG3/x2vjtryS7YvKzMT6nOar3Ekl7PGZD8gXB59OK9qhlVCnrLV+ZyyxFSXker+JPjf4z+I0/leIPEer3lvK3MUtywjx3PljCj8q+f/ipZxXeuNeafGGtn/dnavUjufrzzXZi6aK2l8nCl12g+g71d+D/AIQXx78YPCOgTiNo9U1eCGTzV3JtLjOV6EYzxWmPwkJYdxStbUmlUcZ3Z83ahuhnAZEWcsQqr1UdOfzrS0fUpdBuD5k5Teu37pPDAZx7nP4CvoT9qr9kvWPgj4knlUfatIuZALe8VQM8sACB0PGcAYGR6181XEfD4UMU+Qbjk4+v4k18beMkenrF6HqOj/EqddPitzN5rx5ZpGALR5x0J6dB3q2PjBLfLsmuPM8tlCjOPlz/AD5J/D8a8d3PuCKQFZcsdxBXOe/f6fSm29uCI5JYwcnAwOSef8K45YGnJ6nZDH1Y7M9W174m3epab5QlmjRFDJh+G2nAYDrnJIrgrrxBdagk7zFwNwKFs5Xg5P05/WsdpG8tlyT5mTgt0Bx0/LGKeu6PzYwWYSqVb2H07f8A1veumnSjBWRz1K0qjuxY8pIz7yPNGSSeDnGM/pXtH7Lv7N+sftE+NW0qxZ7XSbBRLqF4FyEQkfKvbewzjqPWrfwF/ZG8c/GK6068s9NmsfDcly3m6jNtwVHJCLncxO0gcbcjr1r9evgf8EvDXwR8IQaP4M0+O3VgrXNwVBluXAxvdu546du1XJ6GR1Xwt8B6X8LfA2keF/DKFLDR7VYI2ZVDSYHLtgAbj1Nfmv8A8FKvGy6z8eLDSbd9y6FpSLKVPSSRixB/4DsP41+pE0nk27MOirmvxH/aR8RN4y/aD8c6nu8xDrEsEbZ42xYiGPwSvQymnzV79jLEP3StoOoM1qCG5AArbh1u50+RLvTJ5IJ42B+RtpBHcHtXHaOGgw0QyrD5k/wrct2+Ujlh6d8V9nTjpqeZJnvvw6/bJ+I/g5UWPXpNUtocbrPVh9qXH+zI3zgewYV9MeAf+Cgui6qsUXjrQ57CRsBrnTpRMmfUxthgPxavzhkRmuliib5YjukI4yewP86ulmjUFSVPtWFbLMPWV3Gz8tBxxFSOzP2f8D/FLwt8SLUzeDdZtNQKjMkIbZLH/vRthh9cYrqq/FHwz461bwzfw3ek3lxa3MDbo5oZSjofUEcivsP4L/t/TWywab8VIWv4Rhf7RgULMg9XXgP+h+teDi8lqU9aTuvxOyljE9J6H3XRXEaX8bvAWsafBe2fi7QRDcLuQTXqROPqjEMD7EUV5DpVP5WdfPHueK/Gf9ujw34JabTvh/HH4h1NQQbpmItYm9sfNJ+GB718O/Fb9oDxb8TrxpvFWr3V0oYmK2VtkMX+7Gvyj0zjPqa84mupGzJId0jcnPaqJy7ZY5NfXYfAUaC91a9zzKlWU9wmuXm3NISfrUMbbm4oun8uP39Kn0mzSaMTXDcbiAoPJx1JrqSM7lq2U8bQSfQUeVtjIdhuPzDHof8A9VSSXAWMLbqE4PSod3y89cYrVCGTSHywmcAV6h+x7Ym//ae8AoBu2amZf++Inf8A9lryqZsc4r2z9hmEzftP+FnGAtrHdytnsPs8i/zYVz412w8/RlU/iR+lXxY+GukfEjQbvTPEETvBewmNmjYg4OCfY9BXw78Uv+CdfhPTdNu9Wj8Rf2RDCsklxJcsiQou4kDcfugA4zzwO5r7+8YeJtM8I+CbjXfElyltZWFuJJZG6njgAdyTwBX5C/tL/tE+Jfjf4yv7fUpJNP8ADemXBXTdKjY7dvaWX+85Bz6DoO5P57GDlV5IvU9xNcl2eJeLfCfhfw3d3VvbaxPrRik2rcWNuRG42jcQz4JG7IBwcgZ4rkNPvNHimxq51JYE4AtY0LP+LNhePrW7qK7t27kVzFxp5klPlr1NdzwyS3MVPW9j6T+EvwS+H3x0skh8I65qVpqEEYafTbxk85H4G7HQr6FcjnscCvsv4M/sF+BfC6zX3iDTW1hrhQogvwkidME425H4H8q/M3wKup+EtYtNd0O8uNN1GwkElvcQNtZGH6EdiDwRwa/Wn9jz9rDS/wBojw9JpGtfZ9P8caHGBfWinat5GOBPCP7p7j+E+xBPJLC1KL5pNtM2dWM1ZKzPb/CvhWy8O6db2Ol26W9rbIqRxr6AYGfU+9dZGQq4xUMUO1elTKmKGzM5/wCI3iOLwn4F1zWLltsWm6fNcMfZELf0r8Mlmk1PUri8ujvmupmlkb+8zEk/qa/TT/go18ZI/Bfwth8G6XMBq/i1wswVuYbNTlyfTcQE9xu9K/NXS7c8ZFfTZFSvGU/kcOKlsjY06Er2rbW18xVK4Eo6Hpn61SsYduK1YztIx2r6uENDz2xttp/kxkyENI/zOR0JP+cVBcxhTWhHn5QMFe47/hVW+jKx71+ZCeG/oa0smrGdzOxR5hTlSfwpyqWpWiNYuBSZZj1i4jQKsrYH+0aKpGFuxwPpRUezKuNmJZqRFzzTrj71OjX903TI5rJlmZeZdselamm4h09SwGcMenOCcf0rNmG6YjitLaUsIhngp0H1NStwAtu54pjNgdKWo5DWiFchmkxnJwK9/wD2A9Ne/wDj+blDgabpFxKfcsVRR+bD8q+eZmHzDHI719Q/8E34RN8YNdduq6fFGPoZdx/9BrgzOVsNI1oL30fT/wC1w194wuNB8F6GsskCEXF4EzjjhAfXufwr4O/aw+Es3wx8c6aGj2R6zpUc+cf8tFJRh+QQ/jX6/f2Dp7Xz3jWkBupPvSlfmP418K/8FPdJi+1eALxVUOTewtgckYhI/r+dfE4ShbEc73Z68637tRSPzzm0xps8GktdEWLMkwHFdXDZock9q6n4OfDP/hbvj6DRHuVs7SONri5bncY1xkL/ALRyOv8A9avacY048zOa93Y5DSfBuqeJbOSe0jFtp0PEl1JwgwMkDuT7CvbP2fvg7P4I1/TPF1jdXUOsREyW8ysUMee2B1BXgg5619H33wX0ZJtL8N6dBFbWFvglVz8wHr688kmux17wDbeHltorEosaKBgV89jKtapd3sjuw6pxa7nvPwu+IMPj7RVa4RbfVbZQLq39T/fX2NdTrep22g6XdajqUgitLKJpZn9FAz+NeO/DPRzLIlxZSm3vIUJjkHTI7MO4PQ10Xxavj4i+H9zbMDCJWjWbaeCd4Bx7dadJtx13IqqKlofmV+1x4iv/ABz40j8R62zrLrFxJ9jtyf8AUWsWFjUf99ficnvXkumwlccV7D+1ptX4nWemwoEt9K0uJVX1LlmJ/IgfhXl1jEFAPBr7vJaHJhY+ep5GLqc1RmhAu1flODihZZIc/avXKtjqPSpU4pXxJGVYZUjoa9qUW1oclye3mEg4Jx296r6xfGOGKGMKTcPzz0UDJP54FNtI/L3eXx9arM32rVpd3W3jVB6ZPzE/y/Kiz6gx0LdOatLHuqFVG7oMCrsa1dibkPk+1FT9e1FHKFz/2Q==</t>
   </si>
   <si>
@@ -3464,9 +3446,6 @@
     <t>/9j/4AAQSkZJRgABAQEASABIAAD/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCAC+AIADASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD6WIwKYSD2qS3nguV3RNnnkEcinmH2oOVor0hHFTyRCm7KBEDA4pAPWpmX0puwk0DI4xmhkRuqqfqK4r4ifFrwR4Pka1vdUS6vVODa2jK7Kf8AaOQq47gnPtXiHxC/aB8W61bzx+G4v7GtfLYiWGBp5zhEJy7BVXBkAO0Z+6QTmjmLjTkz0/4xfFG28H+MYdGWxsPJSJJLua4VSxLnhEXep+6Dk89RxXDf8NBW1wwZfCmmzJtJfy7ggrgMSDgEj7p6j0zivIb641C71BbzUbu/klmlZ5Jry6SNnH2jqdoLEgQjOCcEBh2rjbiczJuDPIywlsh1uMHYxzuGGHMnbPOcZIopxcm3c6HCKSVj6x0T4s+CNUjkttQ0ufS7obgGRvPjDDPUr8y9D1UY71uaXfWmoW3m2F5Dcx92icMPxx0r43a6ma5fy2Zyu8hVJkIIM5zsbDLj2PHfLcVp6R4n1XTr7z7S6ljkjZgWiZiw/wBYckHDjoPXHfmt4x5elzGVNPZn13HEh4kjVue4zXJaxDE13MGhjI3njbXG/Dz4wXH2gW2uql1b5OLiP76429emT83QgHjHzGu2vJobvNzbSrJHKSysK0VSElbqc06co6sytN0Oxv8AW4bY28cZlbG8J04roJPAyRSFY7uMYP8Acqr4XGPFNn/vn+Rrtr75ZSfWvOxcUpHRQm7HeaBNFdWa3EMqssmSDnrz1rSwT3FeAw3N5EuIry4jHokrD+tXYda1qLlNWvOP+mpP866/YyMPaI9wMbZqOSM14/D4p8Rp01Wb/gQU/wAxUfir4g+ItJ8MT3a36tO3yQBolJ3HqfwGTWdSLpx5pbGtO1WSjHc9A+InjPQPBWjteazdqsmzdFbRkGWX6L6Z7nAr5p+I/wAYPFHixp1juZNK0pgyx29vMYRINjYLS43yHI6KAOAO+axNUurvWZptV1O7uLu7aUl5HO5xngHJ+VAM4BPPPTisSyT7TJIkERkPl9YU80jnbkyScAYcdO2PSuL2rn6HoRw8YWvuZ93g3h+x5ZS2ALS0OPvXP8cnt09twPKiqti0srSxTuuChx516SfuQ/wp9D/48v8ACK2dQSyV5RMYZjuJKTXLTEAee5+ROO3P1Df3qq25S1KpH5sYwFJEEcKgZhXJdskcjk+wP96toyugtZl7UhFaWP2m2TakdtlmjiECjAuWH7x+Qc4xj/dPQGvPLlWldGcZj2hQ0kQkUf6hMh0wfQdPQDua9BvHV9OuVhU7mttjuEE7KWCKdzyfKo/fkMB6A9Oa4S6bddNcFdjtIHBljMTnMjsDvTj7sYGe/wA2MAZrfDbMzrblUh5rPhty7cjkTIvyyHOR8y4L/QdeTUu8tnzCHVXIBY7lXJkxhx86kb8gHp1OTgUyGGM7GJ2hduZGwBwIl4kj6ck9RgYwMmpIdv2uKR2xkqQ7Nt43R9JV4z8x+907810mRct5ZF/fqxG7dtYsNx+VDgSDh+AeG5/EmvX/AITeL/MtP7L1ABljdtkoXDjOMA+uMdPyyBXkFqiHy4FLAuigjZhsbGXlOjdByvPOOpNdN4JYx3UeCDu24IbcCMdM+nHTqMcdK56kb2a3Ra1TT2PoPw5Fs8UWp9GJ/Suw1JflDelcV4a1KCPTtN1K5+UxRlJX6lv7pPvg4/CugPirQ5YyDeKuf7wIrGveVnY5qa5bowlAp6img07NekcTHpzWB4+mkmtfLJXybWRiN2Of3akgfiR+XsK6CEEsBXFfFC4ZGW2iJX/WSSupxySBgfQBR9SfbHl5pJ8kIrueplUU5Tk+iOV1BVh0/wCxpHukZMOdoIQ/Q/KvcbmyfvHtWBbyGa7DjEnzRsP3ZuJB88TnA4QH5X4PAO4dDWpqWCpzEJH2h0Ux7toBySIx9OrHpnjmsqRmkheEgO7DYiNKWOQJlAKRcDkx9/7rdCa5aNuU9Cp8RTvmkMaxGR4XMSoVM6Qf8skXhUyx/wBaxGeSNynvTENvHN9phhDNlpFaK3L/APPRwA0h/uqpHqDjqObV1crbzSG18sNkuoQrGx5BHChmBJWEcn5WPoaovarJcKHtZJIgQu77KcspcJ96VhtyIZO3DZ7GuyKujBlu8mD+d5nlyMsi4AzdP8ucFVX5BxBkE9VyO1cBHLshaOGSNS0RGIJWj5MP9x+uS/1I9Aa7O4uw2kFJWX5kDbJL1U3N5Er/AHE6fPJ07MPTdXJC2klVwPMm5YcOlyuP3K9chj/M4AHCmumjGyZhOWo8t5M7TA7cyEhmHkufmfByvyscoB9eB60z542ZTlZAu0cCJnwDj/YbBjA+vTnJpVhaKNo94jypHl72TBHnDlH49RkH2Henx27iUgp/rCw6Bcn95/AfkPUdD3wO5rRiJYfLFxsGFCMGI2EY+Y4yg5XiTqnHHA711fhB9s0Zb5iAMkkHpxnI6+xrlo4WSd1PAj3DOT8p2qen3kPy9eRx2Wuv8IRyC6kwTkKXIPfIHPpk+o4NYyYbI9b0mZm8JtG2PkkC/pn+tU+PSl00suipEvR23E+vAp2wnqMU4/CcNR++zqt4z3pVkXdzXva+DPDcnTToD9M07/hBPDrf8wyMfQmu1U2+qPO+tf3WeF2siht3XaM15/8AECURS+ZJjdhEwW24JPr253c/l3r6Y+JPhjQtE8C6nqEFlHHLFDtjbJ4ZmCj9WFfMfjBYr3WAZLobY2UDIyflG447jJI6AkjAGBXiZpFqtCPkfR5PNToTlbqc/r3mvMLVl6jasS5GdwBBEY+Yk5HLEDlfes/7O32FjGcR/MQBGPLDbT/CCqABlU4LElZD/drQumt2vJpLxlhhLeXI87AKDgjJBOM8NnJY8thcgCuY8QeOdAtrxMCS7lRkZfNO0ZBhYgFgT96M/dQYJJGQSKxp2S1OupuSKw88pbOWjVyxVHeQFFZmwViCqf3duuecMoB6jipPavaQGSW2CyJC33rWPqLbAPzuS2WmPbLADHzL8uFeeJfEV9CI7CwYx+WE3rZuyt+7KE5kOBnLNwBgsSMVRkv/AB3NIzurqrFtyww28Y+YrngYHOxf++RXZCtTWlzH2c30Ou1WciwvIFmbaPOUL9otuQEihXhR83GR1+Zc9NvOLqFj501wBC0jebNgm3ikzmaJQQyEE5x1AyeMALk1iX0vxAuHMrXOoNuJLbrpCGy4c5Ge7AMfUgGobjU/F8bZu7U3J5z5tpHJnLiQ8gZ5YZPPPPY4rojXhbQxlRqdUa9wBEyoJVjDOMq0jxKP3sy9JAVwBnp05AyQxpLUhYVVlMaOoUnAQHKRjHBKH/We2M46njDh8TXNmgF1p20BgcI0kRGC57nHV/TsMd83NO1vSroq4ka1cKAPMXbkARADenH8DdV7+pJq/aRfUnlktzprm1SSNpwfmG8sQQuOw5P3emO6npnArc8Dsjakqy/KrLyMYwSORjsfbv1rHsW8iFSzKyBZCHTGCPMI3d1IOMZX5TjkBQTW1pcYttShkXHllSDj+HHb+R9uorNgz1LTYyNMVMgiOVgPyFOb7uK7P4X+C7bxH4XkupdRFqIpdig/xDaDn9a1bz4Y6XH18TQrjruqI1qaVmziqU5uWiOZ1T4X6lpmbiwvLyKSM5ULO2CR2xXqvgPwzdavoLG/e6tZHhCyBLh1ZWI6gg10euQ276gkCyRsCw43DmuotLRbe6QxrhHTa2PUV8Zw1D2s6ut4ppHo5jUtCF1qz5r8faXqnhp7qxvdX1a+QzqkUU95JIj4O8HDEj+H0rxfxdrfk6gbe1iS6vEOEjjUOc4I656Dc3JOM9dxFfRn7aRukk0PTtIAj1LUTM32lh+7to49gMjep+cADuT6Zr53+wW+mzyRW+6Rix82eQ5kmb+8x712TTwkpU27u7t6dD1sJFV6MZJWRy99o+q6ncrLq1/9n2qF8q1O4hRjA3t06fwgU620PSLBZGtLRPMbkyt80jH1LHk1uXW7zA54A657Vi6vPvjZbc/MerY4ArL21Wo7XO6NGlBXSGRLIsrKGVeMjJqBoWkmxGd2Tgj3qo0phtwGZi6nIbt9MVQGqXIuhNC21gxzgdOa6adBp3bE6y7HQSWzpHmSNsnpg1R1DJjBwSR3Iwas6frTjTt1wivJSXWsQG1KLAgYgc4rt91LRmbuzCvo/Mhw0fynqCK5rUNCt3ctFG8JPeI4/TpXW3l+kkH+rC7T3HWsubU1hfZNHnPRlBq6cpLY5qsYS3M7wzqN94elEOoIJ9Lc4kkGSI8kfMV/hPA+YenORxXqGipFJHb3UEgktnDEMCCPUdOMHBPH4dxXJ6atpf2gdI1WQ5Gwjhx6EVueAok0CRvsnmz6NKxe6syNzWvHzSReoGclfbI5FddPEX0Z59ah1iem6tZ3tzpFubeS5jhiVkKRTsi5DHqAfTFcnqFhcBiHgmkOf45Gb+dex+E9EN34FhuLWaKaF5ZDG5JG9c8MPyrD1zw/c+Yy+XbL7mU/41+L5lnFs0r03LRSfU+0wOFg8JTduiPpJdD0keIoGj02dWWQEl24FdN4s1nSvDnh+41rW72OzsbNA0sz5OMnAAA5JJIAA5JNQW8bNrHmFjtXgDPFeOf8FK4biT9l6+kgdlFvqNtJJtJGVyy8492X9K/ROEcL7CliOVJa9kunkfm2MxX1ivSptmd8WPFHgf4m61p11oWr3d3Da20i3DW+ImtiMkB4pVVjlip6jhT17efat8MdVu083TtVtZ1kOI8o2XOQMZTcqnkdTXlfwB1S+g0aWS6LiWWzO2U/eddwHJ78Ec+9N8cCfcbqFnikJys0TFXX6EciuipJ1MRJ1FufT0abo0Ixg9h/iKG5stYuLXUbyz8m1cRuY7tCrN1IznqMYPpWPq+oWsduzxz2RRccLdooX6liOa53xFZ32pWNnD58pEO7zZZMksSxPBzknBrFvPC0Msci/aDcFl+UTEr5ZyDkYz7/AJ9a6oYaldO5nPEVktjZvtRvhg2ljb3Ybtb3iSMPwBrLuLm5RvNltJ7dieRJGV/nVew0Z7C4lkuNNtb0PFsX5ypU+o4q9oN5qVhNKtlfXdrG/wAphMxOR6NwAy+xFdsqcbGUK02zX0tZrixWQghcdqo6teR23DGuws9aSysZG1PT7O8W9IlWJYfKaBMY4ZCvU7iAQeMVieJNU8IXtu2o2nheGMSHayS3MzGOXc5Krh8bdoXGcnnrXPCmm2rnTOs1FOxjWM32xg5dY1A4yas6rFCtjuWRWOOorFt7+KUSS/Y9Ot1ijZ1ieGSQlhnCfM23Jx60R6pe6tc7k0HSVijTL+VC0LjA77Xx1reNOxy1KyJNLvHtpv3ZOzPzCvRPBt6n2qGdCBgq2feuB0e60aWdo5LJod4xujmPXuCGzz+NelfDvwZYvFY6j/wlUUFhdrJxcRDcjrzsJ3AcjofUj1o5UzN1Fa59M/CLwS138MbSWF2EJlmMSCUhVUyMwXHoMkfQCtC4+HN3KxVZUTPcDP8AOvWPhTotlp/wu0Wxt/Lki+yK+9f4y/zFvqd1aNxpMJb5cr9K+drcFZfUryrzjdyd3q92JcR4qEFTi7JaDbNVW4XPVjk15D/wUamMX7K2txgZFxcW6NnsPM3f+y1670uEYdq8d/4KNTKn7Mt5GyFjPqFsiAdzlm/9lNelw/K1PEx7P9D4/DS5sXRPlT4Lwz3t7fw+ZuhsrRIQAflUllxj8EP5V0HijTDcSJAmAI1O4/0ql8D4/sHh3VLuQH/Sb8unrtCAj9Xata3l+1X0mSeOTmvOxM2pNrY/TqMYs4TVtKngXMEzKqnnisS6tnDf3iPSu51qyUrMRKQxJ289K5hbO5gmJuNSRIj1MkCscd8YIrpwdWckRiKMUYn2a8ZjwoHtWloNlbf2nbtqe37OrbpAQfmVRllAHJYgYA9SKpf2nd3+qx2OlpG0bybPPaMrnHJwAfSt2TR7xLyPzZ41VVIPzfdGP0rqrVpQsnuc9LDqV2jDkaeS9uru9iWJ7htwiRtyxAAAKPoBWCLCaS31CFFbbDcx3AB7q4dSR+S/nXZatpTvuME8YVVzl3wD7CuWulnEiumVdSPow9D60qDmm5PqViKcXFRXQt6Tb2yxbTEFyOWxVTVrO33nekbf7QULn8q0bO9snVrVpfs9zs3GNwcEeoNMsdHivJnH9qWcYPQPMA30FdkZtqzPNlQZkRWFqbVnSH515CrxmtbRPtt54osrIbhb6egSNRnazg/M+PXPGfRRVmN9L0mdI3RJZ1YfNHJu/M9K7/wLp9jqviJbuGERrIhcKp4Q+g9quMruxjKnyRcmepfsMeLfF2s/tJeI9CXUbybw/pdk4kilmZoo2VkjUKDwp3BvwzX2BJ1r80Pgn8ctc+D2oa6ug6Zp95da5fNPdy3UTu21ZJNiDawx95j+Ir6//ZT/AGhrP4tXFxomp6X/AGVrltD53lKxMdxHnBZM8ggkZBz161105JKx5eJovmvbQ9dTmZRXj3/BQCPUH+C1vJaQebBBqsLXXGfLXY6qx9txA+pFexL/AMfC/UVNrFlaajYzWF/bQ3VrcxmOaGZAySKeoIPUV5HD9H2kMSu7Pm6WI+r4ilUtex8A+EpTD4PHmhVPmOxArOivyshkU9SSQPSvVf2pvB/h7wF4gg0vw3aNZ2V3ZC5MRlZwJDJIDgsSQMKvGa8L1KYwwhR1IrlrYdxm6cuh+m4XERrU1UjsybVtc3M5DYHt/KuU1bUZ9UvPsUUpAb/WN/dX0/Go9YuSIZGDfKqkmm+FrY2ljHczn/Sb394Qf4F7D64/nXXRoqER1azk7GxFpky2sRsgiPbg7FY4zxXP3uo+ILO8Y30beXn7ipuUj/eBrr7eby4VZVZn747fjVLV5pJV3CKNnzyvmAH/AArOMnOp70blT92C5ZWMmTXLFrVZPP2DGSH7VlyeKbaO6+WDzo2/iD4I98Vf1S0jnjzJYKHxjcWTp7c1lxwR27j5B17jpXVGlFIwdWTZozH7S8ep2xw0HKgdSvetm8uIr2yVyoMyjO/HOMetY8MhbG0D6U9ZyiBFJ29uelFrF3Ra0Mx3N00FxErKR1xyD616H8E7oW+q3ETMcRxnbn6V5VHeG31FZF7EE13Xws1CO1mkvJ9xQyJGdoyfmYL/AJ9hVx92LZx4hOTt3Ldn4bg0rRZb6WHfNOxYjb0/GvVf2IZ4Ln40afKbZ1kNhcbcr90AAZz6c4/GuAm1kyTGDzE8mPJYnmvbf2CLS61HxPrWvPHH9ktLcW0DhMfM7BiAfYIPzFceCr1KlRKXc6s2o06eGbXY+k4+blPqKuT/AOsUVSjyLhfrVyT/AFyn3ro4Z+Gv/i/Q/Kqz+E+Yv+CgFts1jw/eEcTWssQ+qOD/AO1K+WvEUj+YwB46cV9p/t46Gb/4V2OsRAeZpOoruJ7Rygo3/jwjr418QWpaDzF9MH61WYR5cS/M/Qsjq82Bj5aHOrCksckchwrDkHvVbVJruW5YWcQkkjHyLnGfap5t8chwPrUmnoMlzwzdaIuyO6SbZT0++8S3KnGmSFl42NKoC/maiN5rkd1tvNMmiXuR835Yro1vjAu2QA8cMOtI2pZ/5bDI6hiP60oy12KcP7xzl9qTPMziGQAcEFDVOS/t5eNyg91J5/Kuk1LVIJV2tbwyE+oBrmtagiuQc28aBhzha6FZmEk1sybS72MyFVkVhjHBqZZNkrgHg1kaXYW9kS8EZXcPmySc1bkkO7r2pOIRm7C30wEwOOc16H8Pba6tfAr648H+iyX4sxKR/EULYH6fnXm1rBPfX0dvCpZ3YKqgZJPtX3d4N+B8Fp8DdL8L62ZGfaLy7iBC7LhsE4PqBhf+A1yYypyU7dzagr1FK2x8i+LpHimQ2E7q8nDjGcnsBX3x+yXoul+EfgtpemJKPtky/aL1nwC0zjJHHpwPwryfwn8D9A0Xx6dVuI5dRhjQG0gnxhJM/eb1x2r1vT7ay0yzlChVeVt7BO7VWB93XocmaP2r5Uz0OP8A16n3ry/9p3466J8KY4dL+yz6hr2pW0kllbxbdkWOFeUk5Cls4wCTtNegQ6/pZkGPtH/frP8AWvn34i/ArxJ49+NGseMdS1HTzYTzRtYLJv3xRRoqhCNvHRj9Sa87KsZ9WjWT3buj5rC5FXq1oKtFqPU8Z8PfG/4i+N/CF94I8X3Vvf20wN2Lx4QtxmORDs+XC7cn0zisHUI1ktmA+63b0Nei+OvCWieE7y/toZobjUFUxOYV2xwjcCwB/iJIX0ry6a62yMjdOhraWK+sT5j7SlgoYSn7OJi6nZbmYL1INZ1mpVtp7HvW1cT4myef61VuoQZPOhHX7y10RloT1ITC8i4A7elUr7Tl25ki3e9alvO0IyRxnmrDajbv1Xc30qoPUqSujl1sFDfKjAewqG4hA4btXSXt/CE+VBux0rmb6ZmnY9K6LmDSKswxnaenSpLe1efAXvWjoulz6jyFxGDyxr0f4P8AgGPxD4wstHR8LITJO6j/AFUSDLN/Qe5FU5JK7MutkdN+xz8M/tHiKPxfq1uGtdNfzLVZF4nmB4I9VUjJ98D1r6ysY7/WW+2ahOy2qnKxg4DfWvNfgzqeo6b42XwXJZ2slrYxMAxXBaHOUK478816VqutyySGCwtRlTtjTHA9zXiSxLrzZ3KkoRTJPJWa6+RVVCwCZGOB7UupeRHG0SKCccmsa00zWbfWLm8vdTXc6hlg3cL9Kk+1RSxrezNgRthl/wBoV6dGM4Qszza1nO6N9Ps9tgx/M4PPFJbaldPcPEx4MTADtnFV3B65wPanaSAl9Ezc5PPtxXzLXM0e5sj5T+N0jW/xG1i3YnLPJJ/388t/6mvLdQdgzMOuelet/tbQf2f8XpmC7VurOKTj6FP/AGSvHr58nIP4V6VGHLImpLmRm3VyY2waLfUF3YLfQ028jWXPHNZV3bSR8o34GvRikzjkmjfaaBxhyFz3HSq81sr/ADRzJ+eKw47m4i4cZHoak+3RH7yMPwrVRRDkzU/s9m5Mi/XNFvpEDT7ppMrnJC1mpfp0SPJ9SakW7uH4+6PQVorIiV2jp45Ixtt4gqRL2XvX0R+xd4fF1p+va0HjjkkCWNs7524+/IM9v+WdfLlncEMEVvmPb0r7L/ZdWGy+CemtFkSTTTNL/tNuxn8lA/CprJSjYzjeMrmzD4L8S6d8TbTxFFaAw2z+RcMHH72Jx1X2BANd/HbxWOnztujlkuSVQRfMfzqhHqDyw+RI25GH4qexFQ2csjwtc2UxhuYZNk8RHyN6MB7/AONeb9SSk5Q6nWsS+W0kZd5oOpOFne5dWY5Ktzx6Cm69cPZaLcX6RrHHDCTN5i/K+B2966r+0orm3U3kAEi9FzhXPpntWX4g0681fSrqOe3YDyWAjI2qox0Hqa9CjzWtLc82vZS0Lsfzc7eMfpToSVmztwyEH6+1JYsWt0YAcoDyfarEZywHdh/X/wCvXzSPdPDP2zvAuparFB4w0iJrhbCBo7yFBlvJ3FxIB32ktkdcHPY18vzHPQ59/Wv0Vtwst09tL8yyL/8AWzXzT+0/8GdP0j7d4m8PTRWcUOZLqyIIjyT96LA+XOfu9PTHSvVoSU15mMny6M+eLhSG3c/hVefDJyM+uKtsNy8cVXeIbuf4veupAZlyUHB6e9MjSF/4x1qxfQFiVD/mKzzbOJPlcDNaR2MJLUvLDEo4xSSY25HSooonHJfOKWRu/NWhNWJrHCXCsT3r7R/ZvYSfBfStp43yn/yI1fEryFWAWvsj9kid5/gHpckn3hNcAH2858U9zGeh6jCgAGDz61HayeRq1wsgPlzRqzAccA4JHv8ANSRsVwQabcAnUIWz99GQ/ln+gpqJi5MvMGt5Ggm+aGQZVwOCOzCnW96klo2maj5ktqx4KSFXjP8AeUjp/KptDuDLarZyKrGMExse2O1Qa1AgMdzGAqzjO30NNWbsKS0P/9k=</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAICAgICAQICAgIDAgIDAwYEAwMDAwcFBQQGCAcJCAgHCAgJCg0LCQoMCggICw8LDA0ODg8OCQsQERAOEQ0ODg7/2wBDAQIDAwMDAwcEBAcOCQgJDg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg4ODg7/wAARCAC+AN0DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD728YRg+JG9pD/ACFfPfxrt/M+EF77Qk/zr6K8Yf8AI3yx46SH+Qrwn4yKv/Cl9SLDJEBx+tebLY5f+Xh+f/heNo9Rt2jh2tnh/SvtT4K6lqEHxOtGN1bwqsZG6RAR2r5L8MWvmG1fzAE7jvX158G9N0qT4lWwurKe7GwnYiZ9K58bKP1WT8jSin7dep9x2N1dXhaX+0LNmPdY1q+8d7IAovbQqf8ApkM1d0LRfDc0Lf8AEiukwMbTbmtlvC3hiQSbNKv144KxNXxtPB88ebufTOpJaHC3VnfNqSD7VaEd/wB2KhurDUvKKi4sW9vKGa3rjw3oiagFGn6gcdcxNmsnUtC0eKLzWs9Rj9/LfFctfBRt6BGUr3MfTrHU7fU9ySWLDd/FEK9Gt59UEa7m04+yx1wFpb+HY1ZmS7HuVauhgj8INbf8fEit2wzZqYc0Ov4k3OqbUNW+VVXTSufl+Su2sW1CTQlcrZbyO0fFeOfYtBd8w3VyVHozcVoW91pMMXk/2pdKo7GRv8K9ahXlHz+Zm9To7y61n7ZhYLBlB7pVeO41iadUENkuf9g/4VktHoUgB+3yc/8ATRua0LGz0ENv+3S57HzGrmlCV7t/iVqbE0es+SPls8Y5/d1D9m1Zoxt+yZx/zyqvOmiuMLqUv/fw1JbxaOpydQkY/wC+f8K7aMJcuj/EwnK+hYt7XV2m2n7KPU+VWlHDrETZX7KxH/TOq4XR1UMl84PqHNaEMekyKubuRv8AgZr2KcJrr+JhyxbLCHWGjwVtgB6LUMDax58i4t/bCVoeXpKx/wCukyPUtUdnDpmZP3rN83vXpwjK61/Exm0yxDFrRAAkgXP+xWxZx6pH/rbiAewjpkEOm7flLN+JrRSGx2fKG/M13xi7bmPUjmXUpBhLqJPpF/8AXpY7W68v575dx9IwKkaGy2/MGx+NJHHY5+WNvxBqrEmXNb6wZm26lGqZ4PlDNc7rVtr3kReXrCL83/PMf413eyzx/q/0rK1JdNXy99uWOe0ZNOwHnMNl4ge9j83xCypvGdqKBXo32adUXGtSjjnlf8KrwQ6YbiMrandnp5Vbyra7eLfH/bOmJKx8N+M4tvjSaT1c/wAhXhHxiVv+FN6gFH/LBuv0Ne/+NC3/AAmEyH7ofivCfjAqn4N3+f8Aniw/nXmy2MP+Xh8R+DYd5s/3ZaTPyk9DX3V8A7bWH+M1qloLaNvIbcZRkdRXxR4NyqWqs48sDnHWvt/4Ax6O3xmtvttxOq/Z22bSRk5H9K48VrRaZvRSVdH6IaPb+IoYdrtYtk/3SK6Bf7cUHdHZtx/CSK4uFfD0Z3RaldQ8/wB9sGt+3n0UrtXU7hjjvK1VQlFRUb2/7ePRmm3e34DXfxB/bLL9js2XH9+oNSj8QSWLLHY2bMV5DOcfyqrnRW8RMo1i5Vtv3fNOKdqkmipZ/Nrk8PHGJzXLWa5JPm/8mX+RtC6klb8GZS2WrQ6Y27SbGR9vZ8f0rzy8XWodVZl0O2Uf7Dgj+VddNNpbWp2+JJ8bevm//WrhNa1DR9L0y41C68Tzrbxjn5slj2UDuT6V8rVquUlCC09U/wBDqkrK5q2+qalbws1xo8SKBlm3gAAetcpL44iu7qRdP0u3umB5nJxEPof4vw4968M1r4jrqutmC81CaLR0+b7MJMFgP+ehHUn06D9a5+88eQyaBNDocGWc7Q56AfSvYo0owjeo/kZxp1aukUafxN+K2radbtb6TrH2aYD5haQJGo+hOWP518qah8Z/iIt27R+NNXhIP3Uvnx/PFWvEbald6lPNJIZGcHcF7D0+leW3ulytvKwvuj+ZjjoPWuapVTl7qPpqGBhGHvanuXg/9qr4ieG9UjXV7yPxNp2Rvi1CEFsd8SDDA/Umvvz4afGnwz8StLUaPaQw6qE3S2Msi7x6lT/EPpz7Cvxzms/3O5VJb24rc8G+J9S8J+MLXUNPupLOaKQMroxUqc9eK3o1YyOPF4Cy5on7krdXfmD/AIk6r/wICte1vrpB/wAgtef9sV86/B/4tW/xE0mOzvtU+w6+kecZG25Cjkr6MOpX05HGQPfoY5CP+Qpu/KvdptWPlpKalY3vtlwf+YavT+8Kmsbq5xJ/xL1Dbu7CslI5FX/kJ7vfirVnGwibOpZ+b1r0YO7t/kcjvc6m3ubg/wDLmo/4GK0I5JmX/j3Vfo1c9CuP+Ylz68VpRgr/AMvxP0xXWtiTQZrj+GFfxNG647xr+BqFfmH/AB+MfxqZVUf8vJP40wJP3v8AzzX/AL6qndfamZfLjj/E1Z2p/wA/B/76FZ195OBuvCmBn71AC263i3C7o4seoNaY87vsX8688j1zTofEawSaxjk/KZBXQ/23peP+QoP++6m6QHx741/5Hi4XvuFeH/Fxf+LO3+MH9w3X6GvcvGgH/Ce3Xrv614j8Wsf8Kdv88D7Of5GvPlsY29+58Y+C41+0WvybnwMAjivvb9niDUm+Msf2O1gZxasT5vYZFfCngnd5lqGwseB8w6195fs7JY/8LoTztQli/wBFbbsYjJyK562sLehdNWrI+8ZIteWD5bGzZj1+atCxj1VYC01jaqx7K1Nlh06S0K/2pcL6ESHP8qmtUtIrP/kLSsP7zPz+taRgozvd/ej0XJtf8BmLPc6pFrkn/Elgb5fvCQZrD1bVL6SDafDqt9GU1duktZvEUmNflUBRxvHvVW5s7HZj/hIpFbqB5gNfO4uU5JpPT1iehTUVb/gmFbLeyLuk8Mx7ccjKj+lfE/7QnjKS48byaPYwJp9vp37po0I/1pGXY+4BCj0w3rX30yWtroU039vOyxxl2YMCeBk1+R3jzWJdV8T3V5cNumuZnnlJ4JZ2LH9Sa46dJQfN5eT/ACOyklUnY5eG8mkZ/MmPPOTzXXaVqASw8qNhg9+nJrgIGX7OxPVunFbVm7QLARtVQfXOanmaZ9HCmnE7Ga1eRRMVRgRyrHn9axLy1t/KmIVV+XbgKF/DHf8A/VXRQ3fmW0ax4DFeBtyfyqlqSsunXDZUrt3YPU89OnFaS5bbWLpt3PINYto4opNq7euDt69gc157NGyXO7Jznmu41y4f7ZJHgKueGU4xXnl1NIbpvmz74qoxSkZ1JNxseqeC/Eep+H9ZstT026aO4trhJY+/I5/HPpX7B+DfEmneLPh3o3iK10w+Xe24dgq5CP0ZfwYEfhX4d6LfyQz+Xur9Vv2VdYutS/ZzmsxdoPsOpOqhhnCuqsP13V69N6o+OxcVF8zPqeJoDHxprDj+6KtWbRfZyBp7Dk/w1Qikuwrf6Sh/CrlnNd+R/wAfSZz6da9ODs/+AebuaytDlf8AiXsPfZWhHJBjixdf+A1QVrptv+kp+VX4jchv+PhPwFelHYwe5dVo8c2jfQrVlSoGVtCv4VXXzieZ0/AVYDXGP9aPxWtCSQOuebUr/wABFZOpyIqt/oTSYXsorW/ff890/KsHVTdbZNlyi/L6UAeTaXJFffF2SNtDZdg++yrivZI9Nt9n/IPj/FRXj3hePU3+K95JJqUTxgcKqCvcFabbzMPyqI66mVPY+KPGn/I9XA7hufyrxL4sr/xZ7UOM4gb+Ve2eNMf8J/eevH8q8V+LXPwi1Dt+4b+VcEvhNT438FLH9stcKd2B8vav0B/Z1lng+MG6PTVuGNoc5IGPmHPNfAngtsXdspdVGOuea++P2d1tm+LrC41JoB9jOzD43HcK4azkoaPsVTSdVH6CW891Iq79MEf/AANaS8eVbchdLEw9MrSW6W6w/u9QkYepfNFw0LQt/wATJk+jivSbfstX+Rtb3/8AhzkPmbU5P+JGvA9RVaZ0yQ2g/j8pokaQa3ceVrnygd8Gsuaa6S4P/E8X8VFfn+MxDjJpf+2n0FKnzWf+Zz/jzULex+Dnii4XSDFImlT7X2DCsYyFP0yRX5G+K75f7emAGFU7cZ61+rXxMW8k+APixv7SWbGmyMVCjkAZr8gvF0vl61Ipy2Tnk1OEqTrQk338l+R3UVGMx9pqkMcarNMIUU8MzccfzrsbW70NbGGa61+0hY87TKMYz9eK+crqaTVtQaA3g060tyf3u8DcehOT09e9UW+Hnh+48NSai/j+4vLphkhYJZYgfZ1GP16V6PsoNe9Jr5Hoe3qr4Ip/Ox9oafrXhd/JFvq8E8jMFOx1ySfTnn8q0rnR7i6HkwTfuWbbJI/IUcnI5Az19etfB+k6lcaJrtkiahHqlnHMDBcwt97Gcj8e+fSvpJvHl5beCLWb7buYAyPnoCQf5AmuCunTkuVtnrYZqcXzJIk8X2Ol2r+W1ykcwTDIDxmvFNQk0cCR11a38wE/K0gHf3rjPFXjK+1jX2t9PbztQbcpkkbhV9SeMfWskfDmFtLXVNa8YWbSSKWWG3YsBn1bG0/ma7qVOKSlOTR5terNy5acE/O53VpdRlvMSRJF/vI2RX6XfsbXsMvgvxZZ3O59r28kYB6Z8wH+lfkbptr/AGLqURsb5dQsZ22yPvz9OR71+nX7Ed/cya34lt41Hz6eHbce6SKP/Z69CyVrHyuKbknzKx+iSfYVibEUmMe9FvcWS26/u5eD6GmtJfLbsNsfTrTreS8+zr8qBs16EJa/8A8H4TYiurHA+ST8jWlFc6fsA2Sfkay42uh/ChPoK0I3vCM7E/OvSpyt/wAMU09zUguLDI+WT8QavfabHsrn/gJqhC15/dj6cc1ZVrzdzHGffNdabZLVi0JrRhxHJ+Rrk9auNNVbjzFl4XkAGuq8y7/ux8VwutXmoCa6VYYmI9TTlLlRJwHgWXSJvijqf2aG4aQddytXvqi32D93J+Irw34czarJ8Q9UeS1gVMcFWr3RprxW/wBVGc/7RrKm9DOmvcufF/jJv+LkXy+gFeO/Fb/kkuof9e7fyNeyeMlx8R7xvXGa8d+Kn/JKr7/rg38jXJL4TQ+CfC9xt8QR7Xbcp+76191fAfVpF+LVqDp/2jMJwDj1HPNfCPhvzo/FC8Ltz1719sfA+Ga4+MFgq3Pl5iblfqK+fzKUo4ObjvY3oJe3iz9NLPVf+JWu3S9nHTIrKkuWkuG3aaf0qnbhre0VXviSB/FmrEZ3NuN8K+YeY1q1OMZdPQ9104RehnRyR/2hcf8AEqO41mam9raaZc3lxppjghjaSV8fdVRkn8q1w7rqNxtvFOD9ao6vbtqfh2+0+a5Uw3MDwvx2ZSD/ADrxq81za/kjtpO2h+QzfED4xapYeP8AxJe+IJ20q9SUfZYwdlpDNlUjCHgqFK84yCcg15PqFxcalp1vOzE3Eka9e5IzXq/iy4uLf4fap4Xjm/s+6S6e2uJlbLfuVRAuPZPXgmvFI75Y7exIbI8teAe/pX0+DlJxnFrZ/oe7iqNKnOnKntJfqcFq/hnXry+hmRoo7GBtxWYbkY5+9t/ix6HjPWup1bTdNXxLaw2fjieTwg89tcXsl+0x1CIKpEkMaxkRhS3Py4yMDIxz734b0Gx8R+Hl83b5wPy/Ln9O/wCFdWvwV0ua/ZG0ay8zgmXyi3PrgnGa1+syU7FfU4Thd977nxI3h3S9S+IOp6nod9e/2M07yRLcW2CwAG1dwbD5JPPUAdWPNfSB0CFv2R7zUpdPVZt+1GVclsDk89K9b8ReBfD/AId8OW8AgSa4fCo57ZwSQPYdB7mtDVLOGz+Ccek8J5kYYxY429h78V5uKxkW1GPQ9jCYJxTk+p+ffhzR9LZI7rVLv7LA1yWuW+ymby8MNo28AkqScsSAR0Pb3n48Xnw/1v4X+FbH4Y+KJrO7VVXWptTubtbhsfxIUPk4HdVQZwuMc1oeDvDOl3HiW90a6iWOOQlTnnr0Pvg1X1/4L28d/MscMMkak/8ALVkzz6A4/SvU+uxVmjyXl7lHllrr0Z8rx6VfWPiy+WzuW1TSZpD9mncBZHAbKs4GAHx1xXsVv4+8d+CfCy3HgXVrrR9TnibzTZztEXAaM7WI525AJHGcY9a1NQ8P2fh+0aE7ExwFX/6/Ncss8a31mz/6tIZtwxkdUH9a9CNb2sOZI+fq4VUqqpzP3J+GPiCTxR+zL4D8R6tOTq+peH7S5v2UYHnvCpkwO3z7uK9At/s/2eMec3PfNcX8P9Lk0H9n7wbo5hDSWmi20cmf74iXd+ua9K0m1kuvLHlovFaRnqkfNumnJofF5AH+ucg+9Xo3t9nM7e1bv9mtDjMSP6c1VuITEc/Z0HtmvSjJpFciRXieHOftEir6g1a8y33f8fUn4saordNHJj7Mp56ZFEl4zH/j1H5iumM0S0rGgZrYL/x9SEfWvJfEV9Zi9vFOpSxkN0D9OK9EEkihi1uOPcV4R4i1Jm1nUFXTxJ857itefmOGs1FGv8L5rP8A4SjVGXUpZTuwMvn+le7NNaFv+Px/xNfPXwkmlkv9Xk/ssRgP1yK9xW6kA5sPyIrBVUpNf5mlKF6aPmHxk3/FybxfpXkHxUX/AItPqB/6YN/I17L4zUD4nXY9xXjfxUH/ABau9A7wN/KtZfCZn5/+H0t/+Eq+ZpFJ7DpX3R+zxItr8ZbeWOEzj7KwwfqvNfE2hx3B1uNvkEeev419o/AZd3xWtw10UH2c4K9+RXyudVJUsvqSi9UjuwsebExXmfoXJdLcpza9O1UVkVZMNbnHpVKHCoMXre9DK/mf8fh+mK/O8NWda0patn0tSCitCZXhM9wfszZB96qtNGBxC/XkUW/mb5v9MBz0qnK8yyY+0ofwrbEOPNsOnFWufmF8dNAutD+OPjDyvMVri7e9i5CKFkyytz1ADMpPqp9K+SNNuhdWsEfnLIytyRxxnjP6V+23jb4d+D/iJb2sPizS4tUEB+R0leGTb3QuhDFD3UnFfjf8TNJm8G/tTfELSorNbSKLV5ZYo4yCixPI0ilQBwNjJx259K+ry6uq1NwtZpL59DSpW/eQ120PV/h/rS2V/HD5ihV+XbnrXt/iL4waf4f0C3isoxJqD/u40ChmZjwAM4z1xXxRYeIksi0qyDdjJyat6XrNjdeMV8ReILoLFAdtlG7EAvjl/wABwPqfQU1RqOTPpvb0Ywjd6ntGpfETS9P1y4/4WFrNvpWoLhvsTTACJWAYAZ4JIPJ/wrrNQ+MPw/vvg3CzWgvNQxttr5bseWyDoCvc4/kK+f8AxJ4m8A69q8Z8SaHBqV9FGsUVwE3SMuM7Nw5x14zxivL9a0f4cXmuXFk0mp6Db28gjbT4JsKqkctt5PtwRQsvlK8tV8r6BLM4wdrJ27NrU9Et/ih4Vm8QR6lpuoQNrKyACGJwVfn7uM9egr3ufxnBqfhOOaRfLkZcnjGOP8a+Oo/CvgDw/wCIo5tOt4bNo9rR+ZJlgfzODnNbmoeKXt7fbFcmaNwMjPK8cfpg1c8JpaN/mZ08Za7qW9EdB4u1BLy5YQnDckk9W/zmuV8K6PfeLPjn4e8K2TNJNdXEULbE3H95KnX24B/CuNuPERkuWkZjtHJ3da/QL9gvwboura340+JF9YC71WwuI7HS5nJ/c74sykDpnBUA9gxx1r06adKhqfK4+snWUkfp7HCv9npBDIVCKFUDsBwK7DT7b7NaR/vm3Y65rkra/wDs8TMbXdz2NXv+Egkwv+ilePWueM/e1PFi4rVna+dmMn7U270qBPIkkbzbrt3auNGtS+Z/x7nnpzVmOWS4G4W5b8K9FVG0v+CHMn0L94VS8KxXXyn3rLvLr7LbM7XmDjjmiR2jlG+1PtXK+ILrdbbVtz+VRVr+ypuRg48zKd74mvN0irqJUYOOBXxxq/jbXY/G2oBNYDRm4bggev1r32+upIY7nMR+4en0r4p1W+hk8U37fZ3LGdtxx71jldeVepNyd7HJi4qMUfbHwZ16S40u+f8AtRTI74YYFfQcE8xi51IfkK+J/gzfW9voE0n2d/nuOuK+qrXULV7RW+yyNx/dqvrF8ROPY3pq1JanmXjD5viXd568c/hXj/xT/wCSXXn/AFxb/wBBNeweLlx8Tbz6CvJfiiu74Y3Yx/ywb+Rr6KfwnIfAOkzKdahR1cc9uh5r7U+Cj+T8TrPy7bdmA9R7ivkvTLGea/smhmiXplSfmr7E+DNs0fxNs/Ok24hPT8K+Jz1yWX1fRno4SMlio+p9zWKu1srNZqf1qRzl/lsevvVeK6hhs1VblhU0cisNwuD+NfBYOL9nFH1tRJ6FCOFjeXH+ht165qncQKJdzWjqMdq6CGTHnN9qG4HpivK/iN8WvAvwz0GS+8aeLLTS/kLQ2gbzLmb/AHIlyx+uMepFd1WE6k1GCbk+iVyYqEI3k7I6YeQsys0LrX5hftyeB5tG+K+j/EbTbELo+sRLZ3865Gy5jB27gOcOnHodhz74fxS/b68W6pd3Om/CvRYtBsslU1PUolnun91j5jT6Hf8AWvinxF488feM9Rm1Hx14v1TxFcMCIoLq7Zooc45VM7V5wQFAr7PK8mx1GarVGoq23U8Ovi6Dfuq/mXtOMl3frau/X+L+92/X+laF94X1i61WG4jhjuobbaY4p5WSEHcTg7QTg5HP0rjdL1c2uryQSNsZ3xvPP4/4etexaP4ljt45JcxzSlAh+flgTxnj6+mM17XK4TO9TjUgtTrvBdv4z1K4j8v4eWF5LE3meXFLbqx7ZXJyenWuo8UWHjORXjuvhLdDUHlDpP8A2ZDcZ9dzhTnOB1PYV5/beJNe0LUftmk5mhVvMWNmI24PG0ggjtyMiui1L9q3xdHorRXeh3iTeVtMn2xH3e+doI6d65+VvRWPXhOlHWo2v69DxrxvZ+K4GmOpeBTDcdvnhRhn/dII7151ptrqnmpJebbaORtv2ZHMgiAxj5u/T6V2V/4s8Q+MNcmvtQiNpZSZZt8292HXGcAfgBXPa14gtYbb/R+i/KVCgYx17/Suqmmo2seRXnB1ea+nQwtQuEi1jy2x5a/NsVsbvb6V+sn7I3xa+Cvg39l3Q/DGoePdL0PxRf3E15exajutUZ3faqiWQCNiEWMcNX42XH9oarY6xf2EMkyWVrJczFF4jUYGSemMsv48VnaTqkzaJ9nuP30JO7aex9R6fhXasHGvC0nY8GvWvPQ/qggvLa90iK6s7+K6tZQGjmgkDo49QwODV5VZtu6T8TX82fw/+LXjv4canHeeB/GGoaH826S1WQtbyH/bibKP+Ir9C/h1/wAFDJgtjYfEzwVFOnCz6roc+xsf3jA/BPrhx7DtXmVsuxFPWn7y/EwVRPc/UpY3aVQsw/Out0+FYoctON3UjNfM/g39pT4H+LI4W07xpZ2U0oyItSDWpX2LOAoPtmvoazvrfUdPjudPMF9ayLlJoJQ6MPZhwa8mdadCXvpr1ujspOLY3VpGErGO4VuK8q1jVLppSvmK2DivS7+H5PmtyAfSvOdS0XzrlmjjbmvLx+K/c819Oo7PnPPtSurj+yrqVkX7h5/Cvii+uriHXb4/u23znqOetfeWqeG7hPDt9JtbAgbo3tX536kyf27cbmOTKf51pw1iqeI9ryu9rfqcWOi1y3R9T/CWOZ/BsMjFcPMeAPevrLTLO4/smPbMoGPSvl/4Qx2qfCywZmKyMxOT3r6b02e1XS41JfOPeuWGKcsfVW1mzpUeWmjznxcP+Ln3v+6K8q+J67vhfdenkP8AyNeq+Kzn4oXn0FeZfEtN3w0uhj/lg3/oJr9Mn8J5h8AeHvs8njS2U+ZvV+3TrX3v8K7aOPxZBdYWOOO3LSPIwAUepNfAXha3uV8arN9oTy9/TPPU1z/xQ+Ketapr+oeGbO8kt9BtX8t4Y22/aGUkEuR94ZGQOnTvzXlV8E8whKina61OqnV9lUUrH6xeKP2hfg94PsJn1Txlp+oXMWVFnpUgu5mPp8hKj/gRAr5y1T9vvw3Z6lIuh+Arm+t1PyyXmoLEzf8AAVRgP++jX5aSXjyE5c1V3PjJbjvmtcNkODowtJOXrp+RvPG1pPTQ+wPiD+2j8VvFU97b6LdQeDdLmyBFpaYl2+8zZfPupWvjvWNa1DWtVmu9UvJr66lbdJLNKXdj6knk1DctlOKzFUtchcE5PAr3qOEpUFalBI451KlR3k7mraLHHBmOPbgfeI5rDuGb7bsIPXrXTIphtdvTj5s+tYLxhtR+XDda7pQSiZHbeJ/hrqml/s8fDP4jQeZPoviS3uYvtG3Ihure6lhaFvqiRuueuWA+6a57RdQmtdQazk+R5AFtyzlcsWAB/P17Z9q/Vr9lHwf4b+Ln/BKofD/xTB5+mJq17DHKmPNs5xM0yTIT0Yed+IJB4Jr4u+OX7OfjH4V+JY4NUtTdaQZz9g1+1jPk3ScYVsfcfjJU88HGRzXg1YJSd9j06VRuOm6OZ0vV7jT1mbULQzxwW2UhmRjtYjjjBwMcjPp9ap3fii1utXbTF0WFbhmKyyeUG+UbhtJ6HBOT0z715vqV9fQ2yw2bTw3MeS0iyFd4Hqc8dscduc1y2gaw2m+LbW5GLlYbt7jdI5Ayw+Y5xyucdeuMVzxw8dzpniqqXKek65p11Z3dtC+NPQo6RD5fmT5grMOoPIPXPXuMV896gtxqHiK5gibcqyEBk4VsNyR04P0/KvV9U8Uah4k063Sa3jk1UPhfKG04IwECqAOSTkDAB7V99/s0fspbdSsfHnxG0pI5wyz6foksf8XUSzg988hD+PpWytBHLOUpM8Zs/gjcfDH/AIJI/Ezxf4iszB4q8T6dBFbwyriS1tPPjcBh2aQgOQegVBwQRX572cJS2X6V+8f7ZSR/8MVeLLNjtxAjY9fnUAfrX4beRtO3GTmu+gmonBN3kOt8pKNx+Unmukt93NYUcfPK8Vt2PzptY/Mp5+ldaTZBuW9xJGcq5Tiu+8K/Ejxt4L1Nbzwr4p1Pw/NnJawvXiDf7yg4P0IrztV2oOvSpw25V3ZrOUYyXLJXBNo+8/CP7fPxg0e3t7XxJDpXjK1ThpLm3+z3BH+/FhfxKGvo3wn+3f4B1zU7e08VaFqXhWSZwpuY2W7to8/xMQFcD6Ka/IDOCG/OpI5m8wBWx+PFfO47Isvx0HGpFrzTt+G34HRCvUg9z+kC9vLfUPhxe6hYXsN5ZzWbSQzwSB0kUjgqw4Ir8x75S2pSsbTdlyTwfWsb9i74sahDrnjT4XahdtPo97pE2o6XG7Ei3njA8xVHYOjFj2zH7mulu/Ma5k23ydf89q+JyDKamTYvE4eTuvdae100/wDhjbGVVXhCXqfYnwr0uY/CPSrg7Y8LkLjpXvmmtL9hwRHx6rXkvw2tlj+Cuj7izFogzH1r0COWGNdqyFfXk1+R4jNsTSx9b2b05n27nuUsMqkEcf4qH/Fzbz6CvOfiQp/4VteY/wCfd/5GvRvFX/JTrwewrz/4jf8AJM77/r2f+Rr+o5/CfKn58+H1jj1tppLdtq5ZpD0AGea+ZNYuvtHjPUpsf66WR8d+Xz/Wvf8AVriXSfA15dtebfOVokjxyd2c/pmvm2Zw2vb/AO8j/wA1rpy+nKKlOXV/kLqRL1b+tI33aVl2n60wnt6ivaGQycoDU1rCS7TnHHC8frVZmVbiNJX2qTgZ7+1aqbAqhj9KAHbGaHn+VZPlH7U2PvZ4GcVrPMqLtjG4npmoUX5s4+Y9TQB+nH/BPvVLi1+G3jTQZJM2p1hbiIdldo1DfTIVfyr9JtQ0TS/EXhW60fWtPg1PTbqPbPbXMQkjkHoVNfmT/wAE9VTUNb+IWkyAFontZ0x/tCVT/wCgrX6jatqmj+EdMFzreoxWkLHEUbHMkp/uqvUmvNlFKbvsNXvofm18af2Hba8kvNW+GU/2WZgzNo15ISh9opDyPo+f94V+cqfAP4wXXxjk8I2/gvWP7SLtGQbZo4VXOOZTiMLnHO7HSvun9qv9qD4uReOdS8D6Pp1x8NvCbKfsup20pN3q0R48xZ1x5Y5+5GQ6nhm7D4FuNY8c3WgR2DeMNem0shmW2bWZzHyck7d+Ov8AnNcn1JzV4OyPXp1Jte8rs/Tz4E/siaP8Nxaa/wCKPK8SeMwoZG2ZtrA46Rg/eYf3zj2A7/a1rpq2OnNNLhQoyOK/I/8AZd+LPx4b402vg3S/GseseGrKzN5f23ieOS+2Qh1TZC+4ShyXG1fMCAA5HGD+psfxE0fUNO8jXLebw7Nu275xuhf33DoP94D61k6apS5W9Tkq858iftjb7j9jjxhfTZVZLm0gtx05NzGT/wCOhq/G25s2jIYD5T39K/Zb9urVNNj/AGNPDtnpV3bXsWo+JYd0lvIsilI4ZXPIPXdsr8jGhDKUONpHevTowvTucRyscbZz2zVqNvs9ysn8J+V/8as3Fq0L7gCV7NiqMkkccDtMyxxqPmZjwKtrlA6BW+XNPH8vasnSLr7VpokVWWPOI2cY3Dsa1T09eelaTWlwJPvDPT6U5SFVmPYZNRocZBptwyx6XcN/djP8qFZq4HoXwJ8WR+Df2q/COsTfNbzLLZygtgYuYHgBP0MgP4V9n+dZtqJX7HJktjFfmVNcSWd9avb5WZGUxsD90jGK/RDwF4guvFnhDStajvIBJIAlxHnBSReGH58j2IrwcVSjGTrJatWfyvb82S9bI/VHwDHGnwb0O3WBV/0Rev0rVn02bz/lVQK5nwvmPwJo6LM24W65weOldpGxeIeYzk/jX8U4rmeLqafafTzPuYNciPNfFP8AyU67+grz/wCIy7vhpf8Ar9lf/wBBNegeKP8Akp119BXnfxSuo7H4OaxeTf6mCwlkc57BSf6V/bUldHxB+WfxA1ZZobDS4lWNbeItJgfedjn+WPzrxNtv9qRno3ltgfiK6vV71rzU5ppMFpCT+tchJzrCn/pm2QD7ivepw9nBRJTvqT7hnn8qRl+bPWmnp0GTTdyqe3XmtCineWcd1ZyRyZG7oV4IPqD61U0uS+V5LG9VpJIxmKfGFdff0PtW42ATjDZHekjU4yw+YnP0oAkjj2pksWPqTUwXgf0FKvXPHHc09VJP93J60AfcX7DCa1P8ePF2m6LrUuiSXGjxtJPbwo7/ACyYwN4IH3jzjNfqVovwtsJNSe+1nULrxHqRbMkmoOXc/iT29q/NH/gn2rN+1r4kVVzjw55hHridB/Wv2gOmpNJHdQsI3HUeorz6kE5u5XM0j57+KHwD8I/FT4et4Z12xghJDGznhQefaSbTiRG7H1B4I4INfif4q+G+vfCv4u+JvAfiaH/TNPRntZtp2XURHySL7EDj0PHBBr+iqNmtdfVmxJE6kNj+E+tfkL+3X4w8Ma9+1xoOi6GDJrmiabNbapeRpvi3SFWWE4IOUG4nB6uR1Brooe7OyOmjKV7HI/8ABPnRIdW8W/FjVriMzXcU1lbJIQCVjPnNj8So/L6V+rMXg3R5oN1xYpIvcuOtfmB/wT31CPw/8Svixod9LFJc3EdneQRqjDeqNKrnr2Mif99cV+sdj9r1aRf+WMPoBXHOKdV8xFVvnPzQ/wCCgXh3Q9F+EHw/bS7CKxmn1ifcYhjcFhGT+ZH51+UzffwfXtX6o/8ABSTU4V8TfC3w7DJ/x6Wl9cyDP/PRoVVj/wB+2H4GvyrZl8xifxrvppKFjnbbB1VkKt8ykVzMmhx3GqNc3spuLMHMNvj5F929Tn14ro5JAqNxuyOgNMztgXb0q2k9wGpsWLEeFUcAUM2MLkVTubhILiFP+WkhOcdAB3/lTlkYk+56U3YCffhs/wBKrahIw0O62/8API/yqXd+PfOaqai6/wBjzYI5Q1hFNRYGDqEwTV177B0r6L/Z48RW8PxFbQ9QZmtb9g1sob/lspH81z+Qr5ovFMviCTo3zcDFdLouqXWg+IdJ1LT5TDfW12k0DjsynI/UVw1aftKco90C3P6SNA3J4c02NYR8sK4z9K7SK7KwKrW4Yj1rxj4c+MLfxl8E/CfizS2/0fUtOjm8sHPlvjDp9VYMv1FegrqFwR8zBT6Gv4dxSnTxdSLXvKTTVuqZ91TS5VY5bxT/AMlNuvXAr5s/aq17+xf2WLiGNik2pXUdmCDg7SS7fomPxr6S8UAj4m3fvivgX9tLxNHLe+FfB8ed8Fq1/cNng+YTGg+oEb/99Cv7eoxUqiPg3sfB9xJn+IMR371jK4Oqf9sz79xVKe8ZZMnsdr+1Jb3Ak1H6oc/mK9oo1G5qpI25dvXjpUrScdOlVZPutjrQBetH8zTYieCBtOfaryrz+HesPSZP39xbsehEi8fnW4KAJFH7zHtUvf71RL97FTZ+YdeRyKAPvP8A4J73ccX7burW7Njz/CkwHOM4uIDX7dQ8SjtkV/On+zD4qu/C37Zfh++s2Iae0nhYDjcuAxH/AI5X74+D/Glj4i0iKQOIrpQN8bGuKo17SwHG/Grxwvwr+BPivxhIvnXUFt5enRHpJPIdkYI7gE7j7Ka/n1m1TUNZ+L2oanezvfyXe6WWeQlmldm3MzH1JP6++a/XT9vzWpF+H/gTw+kgW3vbi6vHHvDGqDPB/wCfg9v8D+SVvZrDevJ53zE4Ix1559P/AK+fc47qELRUj0KKtD1PQ/gj8SI/hX+21oet3mF8Pao403WC/SOCV1/ef8AZUfjqAR0OB/QVbvb6f4f8yNPmIwg/vE9P1r+ZvxFafaG8wEMTyTjj16n6/wCecf0DfAnXbrxx+zf8P9fvZmuJG0C0aeRurz+SokJ+j7vxrDERSnzdzOvG1mfk3+3/AK/9v/bebSRJvbRdBtbSUZ6PJvuWPXqROv5CvgoN82a+gf2nvETeJf25Pipqhbcv/CRXNtGc5zHA/kIf++Y1r523fu+natIqyOMtbvUZz196asfzsyscNzjNRL0FV7y6Wx0qe6c8IhbGcfhVAYc0rXHiW4YHdFD+6THr1b9ePwrWj+4vesXS4mXT4/O+aZ/nc46sTlq6SONViyaSAFXC5PrWZqMmdOmHC/IePwq7czLGhx+ANc7f3W60mUt1U8k1M37oENxIsesTN33dajFyFvFccsiYQerscD+p+lYeoXhXX5oww+U8k1HYTNO0l4v3N3lWw7yMerfQD+tcb3A/Zj9gPx9a6t8DvEXw/upmk1LRrz7dZI5yWtZgFYL/ALsikn3lFfdcylpyfIcfQV+If7G/jP8A4Q/9ujwzHLeJa6fq4bRrtnPDGYZjXPr5ywiv3tjt4RCvmOqt7mv5g4vyv6tnsqkIrlqJS267P8Vf5n1+Ak6uHt1Wh574p/5KRc9e1flh+2Jcr/w1Y0PmD5dFtUOD905dsH3+YfnX6q+KY/8Ai4EzZ+8RX48/tPXX279sfxn5mfkmhjQnnbsgjX8uD+df01hleZ8cz5X1CTIkuF42fLOuOn+1WXZ33l63DH/eYrn69P1FWtUaS3aa6jb95AD5inpIo7frXD6hcNaz2t1BlY3bei55QjnH0r027Io9YWXI5qUFXH3qwI7pmVW6bgKtx3LZxzzTAmVvI8R28jH5GOxz9f8A6+K6Pdxtx+Qrmbv57Rn+6w5BHYit2OTzLSGXlRIgbH1FAF4deDUpbcBnt2qGNcDdgfh160/H7rd2z0xQB638BZo4/wBtP4cpJytzqRsyCMg+dE8X83/rX7baBZ3Gi3tvNHkKPkkH94djX4W/CG9Nj+2T8I5tu7HjDT42HrvuEQ/o1f0MWdjHc2rNgcrnmvNrpuasB+f/AO29rjah8TPA2nqxH2fQ5pCO4MswXj1P7ofjjvjH59yMwHyskmDyAoB7/h/THtmvtD9tJvL/AGo9Es2UMqeErdwRx966uh/7L/k8j4nnkVb7y9oZvMGCQB3H+f8A62QfaoXVGNz0qS91EepRNJbjYq7xz3/Hr3/+vn+LP6+fsk+OE0n9gTSNQv2X+ztJ0zUJLkkjMQtppm59ti/yr8g/MWV1j2lWzwQfy/p/nmvujwj4gbw7/wAELviHqFvD/pyXd1pQlU4Jiup44Xz9BM/+TWWJjdJruTWX7tH5feJdUuNU8SahqV4/mXV3cPPM2MbndizH8Sa5xTzw3v71JqE26dh6/wD1qqwtlsH7wqDzy9ubzFXpXN64xuNRtNPRsqzeZN7BTx+bY/I10X8DN6VzWnj7Tq17dNyxmMS57BCRj88n8algbNtCBGD1+tX5GWODd93jpUatti4Ue9Y+qXjQwMvJ+nFUBn6hfr5m0NXNahd/6Jt3bWc7fz4rMmvmk1P7uMH1rA169aN41GRgFuPYVxzk2wFWebVvEUlvBndcSnc4/hXP+FdzlbJIIbZfMuSnl2MAH3R/FKfTP+Fc5ocH9l6HZyRqsuo6g2xHf7iZHfv0/rXYTRtoscMNs32jWr+TZ9rm+6p9eOw7AVNmgLei3Emm+PdFht7pkm0+YXt5cp/yzcfc/EEg/gK/pos7v+2NJtdQsboNZ3EKywOqZDqwDBh7EHNfzIaTZxw6jJYxuzLE3m3cz/fuJPU+gHpX9CHwU8QXWsfsj/DfUFJh3+HrWMqeeY4xGT+JXP41+V8aUU6NGrbZtffb/I+gyuo4uUfQ/9k=</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAkACQAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDIyOjEwOjEyIDE1OjIxOjQzADIwMjI6MTA6MTIgMTU6MjE6NDMAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjItMTAtMTJUMTU6MjE6NDM8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCAC+ANEDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD688BL/wAUPo3H/MOt/wD0WtbCrlc1meAVI8DaMcddNt//AEWta6j2xQA0AbcEU5Vx0PWnKOwpyoR1FADdvrQq54AqZUA607A7CgCNUNOVBnmnc0u0ntQA3A9KUcU7aa8X/an+Oll8N7P+xdHMV14guEzz8yWSnozjux7KfqewKbS3Gk29D1LxV4l0Dw1Z/atd1a00+Mg4M8oBb6L1P4CvKPEf7UXw4012S0TVtSYdPJtwqt7jcwP6V8T+MfG+seItYl1LWL+e7uJMlmmkLcn+Q9ugrAl1KeRiIwRg9m7ew7dKzlVVvdNvYu2p9oXP7XGlnP2PwfdS47PfBTj14Q4qpH+2DZiRPO8ESLHuwxXUcn8P3Yr5As3nlUjc3TLFsnv0yOKmkE58uSJ1UAnDdunr2rD6xJlxpqx94eDf2nPhprTpHfTX+iyN3vIN0YP+8hOPxAr1jw/rOk67p6X2jana39tIMia3lWRfzFflrHeTIQpOWxyAc8+1b/g3xV4l8MakuqaBrF1p824bxBMV3n0I6N+IrSNe+5Dos/TmkIBr5z/Z1/aWt9cmi0H4gtBZ3jEJBqUYCxSE8ASjoh/2h8vrivo5Qrxq6NlWGQQetbqSaujFxa3GbBTWjJPBqbaRSYIpiINvHSm7farGPWggHtQBWIyfSk21M0eOlRlcGgCJk+bimsOD7VNz3pjL3xQB+PtFLj3ooA/W/wAAj/ihdF/7Btv/AOi1rZWMlc5rL+H6D/hBNEz/ANA23/8ARa1s460AJtHpSkdqULk+nrT1AFADACadtApaXFACYA7UozSqppSNvJ7DJoA88/aQ+J2n/DDwDNqcjxyancgxabbMeZJP7xH91c5J/DvX5269qWreJdYuNUv5pLm5u5WknuJWP7xjjP4f4V2/7S3ji5+JfxyvpluGNhazm0sEBO1YEJAYD1Y5Y/Wtux0TSE02K2NqrAKASf4q4cTX5ZWO7D0eZXPGb7SsNHKS21mw2BgA1aGipaSKXbKsBgISd3/1+le02XhLQZ2LPbD5gPlD9B7V0lv4Q0OXTzbNbJ5bEYx1/CuSWKV7WOyODm1ueB2dtc2tntmizFI3BU85PT6US2Juw0UO9WjX5lzlW/LvXven/DPRPs7oyyDd90+g9K2tD8E6LpUZEFnG5/vOMn86TrK2iFHDu9mfMOpaLcWd6InidcgEr0Iz7elaFno11cqsNvbu7hshNvIxX0pe+HNKnxJcadDIyd2QU210/T7FibezhQZ/hXis/rUo9DX6mm/i0Pma6gutOvmhvIHhdv4XHX6j8a+sP2F/i1ealOPAPiG9MxSHOkzSn51Cj5oST1GOV+hHpXGfEjw3Ya/o8hEEa3SLlH6fhmvHPD93qPhDxzYanZyCO40y6WaJlHDFWBwfr0/Ou7DYpTOLFYV0z9M2HbNNqr4b1G21vw/Y6xZtugv7dJ4z/ssoI/nV3aa9A84j2j0pNp7VJSYoAiwe9BAPWpSKZt7CgCFo/SoyDjAqxj1prKtAH45ZopcCigD9ePh+CfAui/8AYNt+f+2a1squKyfh/wD8iHog/wCobb/+ilrZxzxQA2nAH0pVUHrT+g4oAaqUuAO1LR+FABXJ/HbxGnhL4PeJPELOFaz02UxH/poy7U/8eK11oFeC/wDBRrVW079nKezRtv8AaepW8BOM5CkyEf8AkOjpcqKu0j4q8CwJc6it382VBO7tn616BHqG3Cq31GelcH4KkWK32Kyqe4B6/X866G3VzJnP3u+a8HEVHzO572HppxSsdXoeoq0mFf5sDPvXeeHZjcQqGYDnr/nvXlul2b+YHjHcZ967zwq84xGXwoGc+tcEanvHoxpJQ8z0extgYVXtjin/AGaV/wB2B35waqaFdGS1VTJuZeOnpWhb+YZgy9TyQTXbTtJnHNNN3M/WIJIbdsttwOlcvJe7ZmV2OD0rrfEkU08Ox8AE4auF1azliOW6FuG6VjXunodOHUWtS8l3G8LJvU9ua8a8Y2W26ulj+Z43Yjbxjng5+lejudsgyxArgvHdu3266lL4SQfL70YSs1KzM8ZRTjdH1v8AsK+JV8Q/AOyt2mDzaPcy2kq5yVG4so/JgPwr2TvmvlH/AIJlystx4wtFYiJfssmzPG796Mj8APyr6vxX0kNYo+XmrSY09elIVFPI9KTHeqJI2B70EfNxUnXg00r6UARsMimsvFSMPakYUAfjZRS4ooA/Xz4fjPgXRP8AsG2//opa2lXHXrWT8PwP+EF0T/sGW/8A6LWtegAox6UqjvS0AAHqKKKXFACV80f8FTHdPgNo+04Da/ED9PJm9K+meK+Ef28PjTY+P9F/4QeLRp7KPS9cdnvGmDEmISREFMcHLHueKyqySWptQhKU1ZHivgqGdbdZAOGAAHtXbaL9lWQGZt7HG7BztriBaa9ZeHYbtLCWazEW77XCu5EX7u5sfd545rR8NxXF9EhN2Isn5gSD+deJOHN7zZ70W4yslqj1vRbaxdl2MuOnJrufD+lW5Y7GBBXP0rxWPRNcghFxYXjXKKPl8pxux7qTVzSPiFqGisIL8yRSA8iVCCa5nRjD3k7nVGs5e61qfQui6ZGbpQNoYdMGrl9ttpv4cZ5avENN+I13qOxobhg6nA2Ej+VWNb8cXsNqTLJJvYHnJzVfWoJWtqDws5vmctD1y+a3ktt0ki4PvXJa9cWM0flRyK0i5wDzmvJrjxhfX6tbpczGPdyS23t6npWx4ZhibT5bi61Z/LxnbGxfH1Jz61ekzOMXB2Rfu72FpNuFVj2Nc74ojElm2V3cmjW7u0ZcwT+YqclivSsXVdadNGuQ+T5Sk5I+UD1JrOMHzLQupUXK1I+h/wDgmbp8UfhnxVqHmK00t7BERnJCqjEfq5/Kvp7Ffn/8B9Z8ReFfhbLrOl6zc2v9vOGjtIn2tIVyoYkc8AnvX3xoNtLZ6HZ2k1zJcyW9vHG88py8pVQCzHuTjP419DQqqasuh85iaEqbTfUsUfWnEZpuK3OUTBpPpTqKAGY4waQrTsUUAfjTRTaKAP2B+H//ACIeif8AYNt//Ra1s1j/AA/A/wCED0T/ALBtv/6LWtigApQPWlxRQAUU4DDc0fSgBMfKf0r8zP2vNCbQ/wBp7xTYsrfZbrURexxbflPmoJM+nBciv00r4n/4KdeHRD8RfDniKK3CrfWbW8koX7zxuTyf91x+Vc2KjemdeCk1VS7nzbYxatc3ltaR3E6WE77GjDnaATnBHSp4obp9ejtYUkht9wV3DE4GcZ962dPljigt5GwPLnRzgj+8K7/w/wCHopJmkYYAPHrXm+15Keh6cqTqVTN8C+AkvPF5im1+dtKDeYJoAfMYY/1eMdc10eu+CY7GO5GqXErRqpNu8m1y/PAZSDg11nhuCHSY1nUHfn5RjmjxVHdXlq17eFSuMBTUqvpsaPCKmt9D578b6/f+DNdsH0O3t90rcj7P1wfQVuaTrer/ABG8QSwam6WKxKGfyIAGI6YH4mtTwPZW+vfF6aZ4FktNNTylyON5IJ7duBXbeJtFtNG+LGm6nDAsdtexGwm2rxuOGQn8RisquJpqbpqOprQw83TVTmduxi3Xw8ghdPs891PbEjdIWy3PXj6Vd0Hwc1hqcjTaxfRaSshkV4WbzmGOEIHA57+1el6TphW33xE53dBxWnDAssJjlhVtwwSVGTWlCs1DVasyxNCN9zwTxFcaxbeYU1O8KEny8yndjPGRXDahDrPiC+jjeeQWsQkiu2Jxv+bpXvfxA8OWvnea22JEBY+mPX9K4DR7Jbbw19pKhWupHn5/2mJH6VUsUuWy3JWF5mpdEdF8DtMt9V8WeHdHu4T9hkvI7YAHomeVHpnGPxr7wwBxXyR+yxpMuva9pNrbw7U0u/F/czoPurHkqpJ/vMQv5+lfXGCMZ9OtduXR/dN92cWayUqsUuiQ3Bop1BrvPMG4FNpxGKKAG03FPIpKAPxlooooA/YP4ff8iHon/YNt/wD0WtbNY/w/48B6J/2Dbf8A9FrWxQAU4cUZ+XFGCRkUAFKoJpVGOadQAigCvl7/AIKfFR4J8MHAyL+fBPb92P8ACvqI8da+Zv8AgpHeeGr74UQWf9pwSa1p+opJHaRMHkVCrBt6jlRjHJ7gDvWGI1pNG+GaVWJ8Z6fcADYRuXGPSvU9H8X3b29v/wASy2keONY9ylkaXAwCeozx1ryOzbCK3TBzXpnw/vIU8skRgsRjIB79a8Kba06M9+mk5JnaWHia/KrO/hi6l2EHKSjH05Fc34x8dar4jnuLGz0+PTRb5UtLLu2NjrgDk16DNr8Fr4fGFXzmX5QfT1IryH4haJZ3slzrRv2tpZOZVV8K5x/M1UZxWi3NKkHKLbeh0X7PNraW94sMkxP70+ZI5wWbPJb16133xssLW5uJdPt71VaRVaGSMgmNxyGH0Ir5v+HGsa1o3iDy7SKfUbe5PyjOXjb+orv5tUj1XUmbW7q6s7iFfkiSTZtb0Y4Nc9TC1XN2Wr1ubUsTR9krvZWsejzeKNa0K0tFudPkuCyr5jwMCHf1CnkZxWvonjq/1W3b7B4Q1CR1XndhSK5T4f6bFLPFrT6k08af6uJpN4B+prsdPuzb3rXFu+3dw61tTlbSS1OepRj0ZgeJJdd1mOSHU7SLTbdhtdQS0jr3GT0zyOlcjrkw2NDGgCRDAHYe1dd4w1nzWl/eDJ7A5xXnerTlvMyc55x61lKXPUuzqUVTo6dT3T9gtL268a39zFkW1nZOtww6FpHXYv8A445/CvqvFfP/APwT5014fh3rGqsgH23URGr9yI0H9Xb86+gK+iwsVGjFI+VxUnKtJiFcmmEYqSgjIxW5zkdJinsMU2gBtIRTiKSgD8Y6KKKAP2F+H/8AyImif9g23/8ARa1s1j/D/wD5EPRP+wbb/wDopa2PpQAKM1IBikUYqlrOrWGlQ+ZeTqm77qdWc+gHU0PQC9WP4q8TaT4ftfM1CYiRh+7gQbpJD7L/AFOB71yXijxhqd1+7sD/AGfC3G/hpCPx4X+fvXEagE86SVWeeWQ5aWQlmY+5PNQ5MlysS/EL4ha9q9vJbW0r6XZsCGSB8TOPRpRyv/AMH/aNeBfExrV/DeoabFGkMU6HISP77ZzknqTnua9Y1i3kkhfPoeK8F+N9zdWzMsLkKWxjnI5rllTcpalxqWseWxwmIeXkhgMc1u+FpzDcKm7Bxg59O9QahaqJWiLfvkQFhn1FQ6ZJ5V4rk8KfmJ/SuKpSsmetTrXSZ2viTWl0/S5L68m5RflQ98dK8ruLjXfF16UglYQNgZL4Vf8ACvS/Eum2HiTTE8+LcsY+YIcGqPhLwtpMc32VdSuoCDnyxtyfpkUU0orzKnNzfkXfhH4Qu7S+tJptRtDeQuCI3yCwz2PQnFafjTwRqdx4gv7yC7tY1uJy/kFyWUEd8cdq6vw74Ktp4YXTUpRhhlnAyO5PSt9vCjwafNdyag/KggkDHP8AOtF7a97lqNLltY898N3cnhtZbe8jdNp2RBfuNnHII445rrtM1SG7sX8mf51z0OM4rntZ0OTdsk1PCyDBQoDn8PWqVrbf2QAd7FVPLE4zWdRJvzNKbcPQn8QXTSXDHAU8jGe1YF0S6MTwPrUurX5ubp3XIBPAz0ro/hB4afxJ4riklQmxsystx8v3sHIXPua5VScppI6aldQpO59Wfsg28Oj/AAa03SJ3WO+ZpLmWEn5hvYsPr8uK9WrxWzb7rx5jZMbSnBH0rrtG8Y31rbrHeW4u1HG8NtfHv2NfQU/dikfLylzSbO8orndO8a6HctslmktXP8MyYH5jIret54biMSQSpIh6MjAj9KpST2ESEZ601l7inUHpiqAjoIpWGKSgD8YM0UlFAH7E/D//AJETRP8AsG2//opa0727tLKEzXU6QoP4nOP/ANdefaZ40hsfBmj2Onoss66bbiSdj+7hPlLwMfeb26Due1c9q2qXOoStJNNJM7Hl3P8AIdhU82omzttb8b+Zui0kKo6GWVeT9F/x/KuZkkkupmuriRppWGC8hy2PQeg9hWJDuDfN8oqzHI38Mhx6VJNx+vIz2/A+6c1SsyHhAY9c4rQRxLGU5Zveq6WoivWyPlUZoEY2uQAQvngY7V4J+0lpax6Gt5bxbpXlHPpzX0H4ixJtQHCs2Wrz/wCO2kJd+EN6xj5XVvpTsJaSufMHiCea315LpmOZoFOegbipoGju4y8WBkfOnUg10HxM8MtHoEN6iFns22yHH3VPP868/We6sLlZ4HJwMlTzkehrhq6Teh6OGlzU1bodjo99LDHsZm57Cl1q2vbu1a4sNxkj5wvH+etZWk6jaamrLGRHcLjfFnr9K6XwzfizkCMzBc/Lx39655d0dtOS+FmDo3jD4l2cYjtLC9YRngGInp6E+tajfEr4nahLHpr2E6STHBT7OQR9eMV6DofjCCHiWNWVTycVtL4zsZI93kQxkfxY5xVRqprY09lLucfpul65Z2i3mss7XDKGYuc8nsM1S1i5Z4f3h3NngZxWv4s8RjULgJHjaowo9fwrmrt0H7yQ7eOBWC1ZrNtQSfQZZozsF6DufSvoX9nW0gTwHI8aBWa5YNgYJIC4zXhug20kqebOmyPqBjB+tfQXwVsZLX4ahmR/9KkeUJjkA8D+QNbYW7qnFjrxoJvqdXp0oW4kidxlDitVCVww6Vy98ZbDVg8yqA+OgwOmP6V0VrJutwV/KvUPIvcn8mJ2EoUBvUUtnqF1pGoLPZyeWSPmVRlX9iO9LbkhmzgccAVSuObjOAcelLYVz1fwzq0OsaYt1Eu1vuyRnqjDrWjXlOiape6XIZrOTG7AdSAVPPeuv0fxhbSFY9Qj8hj0kXlD9e4q+ZD5jp8Z60xhii3ljnjWSGRZEYZDKcg05hmqKPxcooooA/RvwXEW8J6WS3/LjD2/2BWxGnlqWOK5nwVevaeHdKiuRhHs4QrHp9wV1WzzI/kxjHFZmYzAfazU8jHTtUkCjy8Ecio5MB8UB6joXCtx1qfIdc469qoSFkkBBOKtW7txnnj1oAyNeXY2WHqMVjfFK3Enw/mbGSqA/lW54uBKxY/iYVF4stjd+DZbcjO6Kh3YlueZa9oMNzZqJ4laO8hCsOxOOn5V4F8QvB914fv2SWJntZSfJmX7pH90+hr6vsbZL3wfAZFYNHGOf7pXvWB4h8N2+q6dJaXtutxEw+ZT39CKzrUVUj5joVnSn5Hx1cWM8N0s0AZCrbgQe9b+i+IZDtS8gUSA8Sev1969K8V/CXULZZJtKbz0XpBIcOB6A/xVxGteGLuwZje2M1uyHlmjIU/Q15/vrc9qNSlUV4slj1TzN22AnPVkerEF8GGNkyDryBgD86w7Cw8242xs2M8cdK6XR9AR2VpZ1UDqXahuFtS483RiQXbSY+zxNI56Fq2/D/h6efbdXrcDkL2I/pW34X0KNVT7FayXBXvHFuz+X9a7bQPAmtanMjXsf9n2o+8G/wBYR6Bf8a5nKc2owR0fuYR5qkvkY/gTw1J4i11baJStlAQbmTsF9B7mve7OCOC3jtYwqRxqAqAdFHas/wAL6Va6Np62djFtUYJHdj6n3rZVAF3bQGPU16uGoeyjruzxsXiXXnfZLYz/ABRZG60p2U4eMZB/z9KXwfOZ9NQlvmUYNabp5luUxncOlc/4QJg1G4tOcI/Ge3NdBybaHSbQVY46CuevpJIrvBd1z2B4ro4z8xHtWH4liKr5gA4GaNxFqzdmh+8cetWWdfL2v0xww61kaDdGSMp1+tai8rkAdOlAF7S9TvdMcSWdzjd1Q8q31FdboXjK3nxFqUf2eTpvHKH+oriLURjl12nsfWi9uo4128HjoDRqB+Xm/wB1/Oios+360VRd0fpF4dso7vwHpsTr1sIsH0PlipvCl40tj5Up/fWzmGTjuKseBwW8G6WD1FjD1/65rVPT4hb+MtSgAIS4hjnA/wBrJB/kKkg6BcMmRVSQFrgAA9etT25IXFRkn7QcLx60A9R8kO5duKakbiTFTk5jPWmwMWk5NA7GX4o4+zKfXpVq4jEmlhO20VV8UfNqFtGOK0WTbYABegFAjm/C8OLe4s3AIjckD2P/AOuotMRWafTJB+9hk+Q9CV7EGtSCPyPEHIwJo6zfF8LabqNrq8YO1HEc+O6noT9DQTyq5JeaURIGWPzOckjg1j+IrK2KQW/lZNzcLCQ6c4zk/oDXbWbRzwBx0YbgfWsvXGiXUdPG0c3WSMDn5W/KiyJlFblOHTNPEKIdPhEcYAUFPSj+xdJWSOY2VtuMnzkxjp+VdQ6QNGC0YLVFcRwYU+XjB52ms/Zp7o6OZpWRWt4LeP5I4hgHjy0wKsxxO/OPLUdeOalhDBf8KmXpkir5V2ItqMhRYVIjXGep71MrDaCVHWo2b58Y7U7cBDzTGSMQB1rl0c23jWSPPyzKCDXTqVK1y/i0fZtfsrpR1OxjQLQ6pAd4PtVXW4w9qwwDxUsZLQK2eo9aW6P7n5lzx1oEzlNKmNtq3lv0J4zXTc7cjvXNeJrWSPF3EceWcmtvQLtLzT45UOcigFqWrqUJHluw9KzbE/bLxpP4F4Ge9SeKJTHDgfxHAqzodsI7NFA+bq1AdT8wdtFGTRVFn6XeCzjwnpEnb7DCGH/AFp18ir40tHA/1ls6Hn0ZaTwPiTwdpkZH/LhDx/wBafqB/wCJ9pbMef3iH8h/hUkGnHHnIGBUPlk3HB4FWWG08d6jDLHukc4AoAkKKE2k/e96r26tHcEEdajtY57qT7Q7bEz8i96s7AtwozQUY+o5m8SRxddq1s3Qxb7QO1ZWmoJPEl1O/SLgVqyPuwp4yOKCdbmXqC4khm/ut6dafrdlFqOlzW8gyskZH0PapL5C1uuBk7s1Pa/Nb/MMUB1Oa8C3bPYNaTf6+zby3B9qs+II/N1jS5Yh9yZiwP8Aunp71Q1JP7I8cpKAFhvgM/7wrbuFAurWRf8AnoMcexFBMldFtZlPDNjbT7iSPyRt5ye1TyRb1+4ucjkimXUKZTYu35uSD0oLew1H3cKO9LOxC8daesYHIFQzFt4z0oEWLdMR/X1ptwSqBeKdGf3fJpt4Pu80FElv8yc1h+PoHfTRKg5iYMDW5bj931FV9fi87SZkx/CcUCItDlabSYm9U7GrUwDW55PHSsXwTKWsgp/hyCPxrfVcblP8XSgRmSQiaAox3A5BFYngp5LDxBd6RIcKp3xe6mugtQyXLKR1NYPi6M2PibTtUVSFZvJkI9D0o1DRGr4mTzZ7dR/E4rWgwI+Bgjiq6RJcNHJgErzzVhPkVi3TOfwoCJ+W3HpRSZFFUUfpd4TGPB+kyxHkWEOR/wAAWoPEUxXXNIkHAkldcZ77DVrwYQPCOljHWwh/9FrUHiaBDarIfvWswkQ/of0NSTaxvwYKhsdKqXzebOtuvAY5b6VLay/6LnHao9PG+6kc9QcUATSMVuI4g2BjAFIrASOW6r0qLWDsuoX9Tg1JMMQyN32nFAFDQwWjmlY8yy4FaM2Fu0jzyq1V0eMLbwDszE1Izf8AE06UDI73O0AdjU1qR5PJpLpM7jmlskBXFD2FYxfiJbeZoq3Kj95bOHU/5/Glt7gXOgw3KsMqyHr7gVsapCJ9NmiboyGuT8Kys/hloAeUlC57cOBT6g9DsVMir96m3EruydwDzj0qYjNuG6HFVZsmLnGc9aQE6t8oqKQgyDPrT41AUvk4PQVBNQBZjztP1pLzlQMduadbfd5pLxeetBQWmMc1LcDfAyt3BqK14bFTsoKc0EnO+CxturyI/ehlOB+tbdvNunYZ2unbPasnT4xaeLrhE+7cRhj9RxV3VHNve29wv/LR/LYUATvHtvQfWqXj+0M3huQqfnRldfqCK03AKbj1U1DryB9Hnz0ZKAexFocm61Rick9fan6hcBIVi43TSBc+3eq/h9tsOAOmBVa8cvrkYHCwxF8f7TNigEfmdiijPvRVln//2Q==</t>
   </si>
   <si>
@@ -3515,9 +3494,6 @@
     <t>/9j/4AAQSkZJRgABAQEBLAEsAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMzAAAJKSAAIAAAADMzAAAAAAAAAyMDI0OjA0OjIxIDE0OjE5OjM3ADIwMjQ6MDQ6MjEgMTQ6MTk6MzcAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjQtMDQtMjFUMTQ6MTk6MzcuMzAwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwAGBAUGBQQGBgUGBwcGCAoQCgoJCQoUDg8MEBcUGBgXFBYWGh0lHxobIxwWFiAsICMmJykqKRkfLTAtKDAlKCko/9sAQwEHBwcKCAoTCgoTKBoWGigoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgo/8AAEQgAvgDWAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A9/8AhT/yS7wb/wBgaz/9EJXVVyvwp/5Jd4O/7A1n/wCiErqqACiiigAooooAKKKKACiiub8ZeMtI8J2hfUrhRcMhaG3Xl5SOwHYe5pN23C1zpCcDJrivF3xN8L+FmMeoagstwM/ubf8AeMCOxxwPxNeR634i8X+PN4Df2RorDAjRivmD/aPBb8MCuYl8AWiHfPO0z/kPes3U7G0aTe51mtftHkSY0bRIzGDjdcynJH0AGPzrGk/aL11lwmn6dG2c7trnjPT734Vz8vgjTxgAsPU4HNVX8C6ezE7mPt7UvaFexZ6z4S/aE0y9wniGya0bOBLbN5i++QeR+texeHtf0zxFYi80a8iuoM7SyHlT6EHkGvkmXwHZSQ4gYxt/eHUVf0vwx4g0CVb3w7qbpcLyQjbN317H6GqUyJUmj67orx/wD8Xo7uQab4yiGnaiCEWbaRHIenP90+/TntXr6kMoKkEHkEVadzNprcWiiimIKKKKACiiigAooooA8A/bV/5JZpX/AGGYv/RE9FH7av8AySzSv+wzF/6InooA9V+FP/JLvB3/AGBrP/0QldVXK/Cn/kl3g7/sDWf/AKISuqoAKKKKACiiigAoorh/ix4xbwnoK/Y136nelobX0VscsfpkUm7ajSu7Gb8TviOvh67j0fRVS51uTBZSpdYVPqB/Eew/E9s+X6fpG7UH1bxBK1/qUp3nzTuCk+vb8OgqnotsbWSXUL+VrjUbg7pJnO5iT7mrF1f4B5rmnO5106djYu9RLZLNWZNdlz/9esSS8LNwamhctzWTmdMaRceTNRmbmmSZxVchqSlcpwL0VxitG1vthBB5rBwQOtMa5MZ61aZnKB1eo2Wn67a+TfRAMPuSLwyn2NP8E+LdY8CajFpuuzG+8OSNtjuCSXgHqPbplfyrnbHUvmHNbDzR3lq0Myh0YYINaqXY5pQPoyCaO4hSWB1kidQyupyGB7g0+vBvhX4um8O+IYvDepyvJpl22LOVzkQyH+DPof5/jXvNbp3RzSVnYKKKKYgooooAKKKKAPAP21f+SWaV/wBhmL/0RPRR+2r/AMks0r/sMxf+iJ6KAPVfhT/yS7wd/wBgaz/9EJXVVyvwo/5Jf4P/AOwNZ/8AohK6qgAooooAKKKKACvmn4h6uuv+Pry4DM1tYH7NCCcr8v3mH1NfQ+vaimk6Ne30oJW3iaTaDgsQOB+J4r5RikZ1Mjgb5GLsR3JOayqvSxvRjd3Ls1zx1rOuLgsetLM/vVQ/Ma45M9CnEmhJLZrWtRwKy7ZcOK2LdeKyudCRKVzTfLqcJRtq0yWiq68Gs27WteVflrLvBzWkTKSM9ZTG4rYsL3pk1gzjFLaylWrVHPJG/rkBvbI+WMzJ88ZHUMORX0X8OdbbxB4O02+mdWuTH5c+3tIvDfyz+NfOVnOSBt6+hr1j4D3cif21pp5gjkSePPUFsgj6fKtawepy1V1PWqKKK1MQooooAKKKKAPAP21f+SWaV/2GYv8A0RPRR+2r/wAks0r/ALDMX/oieigD1X4Uf8ku8Hf9gaz/APRCV1Vcr8KP+SXeD/8AsDWf/ohK6qgAooooAKKKKAPPPjvqD2HgGZY+tzPHCeccZyf/AEGvAYsiIdPwr179pKWRdF0hBJtia4ZiuMgsF4z+v515JEjLp8TFSSRgACuWs9Tsw60IJASajyAwFLPIQoSMbpifuDrUf2S/jjMj2rhBzvYjA+tc0k3ojvp2SuzXs4Q/JIx6k1rQxIqj5gfbNcO63R+aOcM3QqhBH6U2O9ubdQHLBu5Pep5HHctT5tj0JocdDSeVXPaZrDTRAMckVZn1LyoyWOMVSs9Qd1oaskfbNZt5bYyetYV1rrs+FYj8aqx6ndSvn59vqc4rRNGUkXbmLbmqYjKnParnmrIo3kq3X2NMiIZtpxVpmMldFqzfBXNeh/By5ZPiG8IYhJLJ8qOjEFSD9ev5153aoC+B19K7D4Wzr/ws7S4mJ3BZBx/1zato7nLU2PpGiiitjmCiiigAooooA8A/bV/5JZpX/YZi/wDRE9FH7av/ACSzSv8AsMxf+iJ6KAPVfhR/yS7wf/2BrP8A9EJXVVyvwo/5Jd4P/wCwNZ/+iErqqACiiigArP17V7TQ9Lmv799kEQycDJJ7Ae9aFeX/ALSFtLc/CnUWgYr5EkcrYOMruwR+tTJ2TaKguaSTMHx14n8IeNbHSje6mbWG3usvDMu1pAQeN2eBxyRz9OteKfEzU4D4vnXTAi2KQJGkcJwjKm4nGOxx1rL0X95HAshL85GT74rY1OETOdwBJBHT14rjdTn3PRjS9m7I4iXVpW+VVSIf7CBcD2xV2zl1LVIJXtxLILWIuytKVAUfTkmr0mkxspygyOlJaw3NjIDbKwx02nFCmg9jYyYbm5v7iGKN7SadyirGC7NliRj94pHGOee4x3xegE4uZbaZPLkQ7XCkoQfoDt/QirdpG9rcie1tPJmGfmTIIz6HPFNeOQ3m5iXuZOCSxYn65rZtOJlGDUifSzrEFz/ok9pIjdBcKcj67QBU+pT688ixStpkat3QPxzjvWnodmomDZJcZB44xwB/In8RTtcjRJ1kYcRkHgZ7isYtc1jpkny3uckzzj5leWQHvwuMfTH86ZJdyRIJXF26srOPKDuCo6nJIGB+QqwIPOjNvIDuTkgYw3pVvV511TS7Wzu8xC2yEdEwQDjIPOCOB6dK3SSOVybMuXVpY3xbzXNtPGfmSVGRgfQ5JGfatC18capEoW5h0y8Tp+/sowf++kCt+tVWEEGmT2kZExmYF5JEySB0HOayI9LkLZDkCq0Rm1K+52lv4mEsAvFsoYpRIqmNHbaQWA4zkjr6mvUvhjodzb/F2B5wfJjt5biJxwGBBX9N3TtXiNnpdw8dskEgBzvbcOCQ3H8q9o8K/FNNDmnGsaWGurUeVG8MnDggEsSRx0HHNDlHRoTjLY+kKK53wJ4rs/GOhLqdgrIu8xuhOdrDB6jrwRXRVqjBq2jCiiigQUUUUAeAftq/8ks0r/sMxf8Aoieij9tX/klmlf8AYZi/9ET0UAeq/Cj/AJJd4P8A+wNZ/wDohK6quV+FH/JLfB3/AGBrP/0QldVQAUUUUAFY/jDR11/wxqeltgfaoGjUnoG7fritiii1xp2d0fC1nbXFnfQ2sqMrwOY5MjoQxHP5VuXI5rqvi9ZLonj7VVO2OO+RbqNjwBn73/jwNcpdHCkjp2rzmuVtHrqXMoyGwxhxzg/WrcUCocgCqNpKBWlHICKyudFuxHMvH3QTWcbbEhIAUt3A5rUkYBcmmwR+aAw4FU5OxKirlnSYAijA7VW1yMljitvTYx5ZPpVXWIcSbSMMRnFFN9QqLoclDD84JGe3uK1obGKVf3kYbiqvleXcbW6GtW2GFroTdjmsrlKTRLVuVUqfp/8AXqrc6dDDHg7mJ54wP8a33YBayr1wSaLsGkM0yMF/ugYHHtWN4pA86/k4IyQ36Ct/SvvZI4waqeF/Dl34p8T2ulhWH2qUSTH+5GDuYmm9dDONk3Jn0H+zfocuifDCzNxkSXsr3W0/wqcAD8lz+Neo1BY2sVlZwWtuoSGFFjRR2UDAqeupKyscEnzNsKKKKZIUUUUAeAftq/8AJLNK/wCwzF/6Inoo/bV/5JZpX/YZi/8ARE9FAHqvwn/5Jb4O/wCwNZ/+iErqq5X4Uf8AJLfB3/YGs/8A0QldVQAUUUUAFFFFAHk/x78PLe6TBq8SfvrUGF2xn5GII/UfrXhd8M2cT8H5cEj1HFfZE8MdxC8U6LJE42sjDII9CK8D+Mnguz0C0jutJRo7aZ2zFnIRvYnsfSuerT15kddCrooM8aWbDVpWs+etYbHDVPbTYxzXG46noqWhvTneu0d6xtb1TUbRBDZLGpI4ZwcfpVh9Qhg5mkCjpya5vVNXN3cIIkITPy853cj+lUoOTtYUqihG99Tc0rWNQis0e6UsSOWjORUWqa7rUM0c1vAJEY4ImfB/Ws/SLyWzvBGdzBU5BGMcZ6fWs3UbueS/ErMVGN3LcfSto0kmYTxEuU6611M6lErPGEk/iC9q27d8wgtwcVyeg6lBKBH918DArfFx+744xVcttBKfNqT3FxhTzWRPNuai5uM1SVi0gHvRYTkbls7QWbSonmMSFAzj6/pmvevgP4ca00aXX76Lbe6l/qlIwY4B938+v0xXA/DnwbN4gu7IywE6dE2+eQ8A/wCyPUn9K+kY0WNFSNQqKMAAYAFawjrdnLVnpyodRRRWpzhRRRQAUUUUAeAftq/8ks0r/sMxf+iJ6KP21f8Aklmlf9hmL/0RPRQB6r8J/wDklvg7/sDWf/ohK6quW+FH/JLfB3/YGs//AEQldTQAUUUUAFFFFABXIfFbTv7R8FXwVd0kAEy/h1/Qmuvpk8STwyRSqGjkUqwPcHrSaurDi7O58MX8ZSZs+tVfM2KSeg5rtPiX4ek0HxBdWrj5FclD6qeQfyrh2964JKzserCV43Ri3Er3l2A7FIcbsnGQK1NPvrSxkDRRhT/eAyw/GmDTIp8s27k8471s6bY2MLKP3XX+PAq3JLREKD3Y5NfDbxIgmXHBmXP6moJtVtruLbcrGoHRVQLj6Y5rrYrbT3X5Etm9dpFZ2taRZNDuSDB6cc1pDyJmtDhr2BFkM1ieFx8hOSfUitLRdUe6jKynLhc/Wq15pMsbBrZgnPKk9afZW5gl3MrK4HI+tab7nOrp6F+V+etWdIga4u4wMkk4x61R616f8FfDjav4mtZHTNvbHzpCRxx0H4nFSldlydlc+jPB+ljR/Den2QADRxDf7seT+tbNFFbnGFFFFABRRRQAUUUUAeAftq/8ks0r/sMxf+iJ6KP21f8Aklmlf9hmL/0RPRQB6t8KP+SW+Dv+wNZ/+iErqa5b4Uf8kt8Hf9gaz/8ARCV1NABRRRQAUUUUAFFFUdb1ax0TTJ9Q1S5jtrSFdzyOcD6D1PtQB4N+0LAT4ki4/wBZbqwPqRnj9K8QkUhiPevpr4l6SPG/ge217TImWcxiaMH7xTkj8ea+bJlPmHeu11OGB9a460WpO56FCScNBIVJHFOuLAuucYPrml0+UCUEsB6ZroYo45gOeg5ArHqdSs0ckulZbd8/TscVLHY3KcLM+zHQkmut+zxjAwBSPAgHpW8W7GEopM52NGiOXJLVBM2560NSZEBPas9BuzVoykPtIvNmUDrmvo/9ndY/7N1UxgfK8a7vXg1872sTvMsFuC00h2gD37V9L/DG0Twbb6dpd+yrc6sGdcnHzqM7fxGfyq4J3Maj0PUKKKK1OcKKKKACiiigAooooA8A/bV/5JZpX/YZi/8ARE9FH7av/JLNK/7DMX/oieigD1b4Uf8AJLfB3/YGs/8A0QldTXLfCj/klvg7/sDWf/ohK6mgAoozXHeM/iV4W8IRsNW1OI3I6WsB8yU/8BHT8cU0m9gOxqrqOoWem2rXGo3UFrbry0k0gRR+Jr5b8bftKatdGSDwpp8dhEcgXFx+9l+oX7o/WvD/ABF4l1nxJdm513Urq+kzx5r5C/QdAPpWiovqTzH1r41/aE8MaN5lvoQk1m8HAMXywqfdz1/AGvm/x18Q9d8dakJdXuMWyEmK1iyIo/w7n3PNcVGpx15+lTW/+sGcV0RpKJPM2fe/wmnjvfhroLgAo1qqkfpXlnxl+GjwTS6xosRMbfNLEo6e9dp+zjd/avhZpyk5MLvF9MGvTpI1ljKSKGVhgg964q0FJtM3pVHDVH54apdSWF5g7lKkHn2q1aeJJo5uX4K/N7V9G/GH4Mw6rHNqGhpsm+80S9/pXzBq/h690y6aK4jcMhIIIINc/KtmdPtJbx2Ok/4SoKQXUfMMjBxg0+TxCfKAb72Q3/Aa4mG1nd0Qo4DHBOCcVNLbTzzkxRSBcAZYYPA/zxVqCIdWT6Gxd6uJ5SVIKbvl+laFgzNHwH8124HoOwFY+maQ8lwm9WJ7KOf/ANdfR/wf+FrSvFq2uRYjHzRxMOvuabV9ESpPdl74JfDkwrHrWsxfORmGNh096wf2pNclste8Pw2ErQ3NoDcK6HBU9q+kY41ijVIwFVRgAdq+M/2i9U/tD4mXyqQyWyLCPqBzW1JamMpN6np3w/8A2hdNnhhs/GKm1uAAv22Nd0be7Acr+GR9K9y0fV9O1m0W60m9t7y3bpJBIHH6V+cU3BNJpesanot0J9Iv7qymHR4JSh/StpUk9UZqXc/Syivi/wAFftF+LNGKRa2IdatBwfNHlzAezgfzBr3vwZ8dvBniTZFNenSbxuPJvsIpPs/3fzIrJ05Iq6PVaKZDLHNGskLrJGwyrKcgj2NPqBhRRRQB4B+2r/ySzSv+wzF/6Inoo/bV/wCSWaV/2GYv/RE9FAGz4T+Lfgzwz8M/Ctvf6xHLdw6RaRvb2ymV1YQqCpxwCCMckVyPiX9pc/MnhrRB6LNfP+uxf/iq+ZbT/j2h/wBxf5VLnmuyFCNrszcmd14p+K/jTxGHS81uaG3f/lhaDyUx6fLyfxJrgmJYksxZjySTyafnPApnStFFLYnUjI/Ck2eh60/HenKPmqrCHEYFOh+/kimN2xT4+GoYz6r/AGTdV83Q9W0tjzBMJkHsw5r32vkH9mjVhpvxBjt2YiO+iaEg92HIr6+rjrq0jSOwHkVwfj/4c6Z4ohaREWC9A4kUdfrXeGvnr46/GhtLvJvDfhKcC/T5bu9XnyT/AHF9W9T2rmna2pvRjOU0oHA6l4B1Sz1WWwihimkjP/LJh0+napLH4aa7fXAhjtUVurfNkgepFc/4R+Keq6TcPHqw/tGwlOZFY7ZAT3DDv9a9W8EzaBd6s3iLwNPnUwv+k2k7sJCvcYJ/lxWEbX0O+rTnHRnW/Dz4Q2eiul5q5W5uhyEx8q160iKihUACgYAFZfhvXLbXbHz7YlZEOyaFvvRP3BrWrpSS2PNnzXtIr6jcrZ2FxcyHCQxs5P0Ga/P3xZqDarruoXzkk3E7v+Ga+1PjNqTaX8NtanRtrtF5Sn/eOP618M3nygY57VvSXUiWxnzdapTDPTNXJKrEda6LaGZEq/WnhcdaVV460YosB03hLx54m8JSK2g6xdW0ecmAtviP1Q5Fe7eDP2m/uQeMNJ9jdWB/Uxsf5H8K+ZNvFOA6cE0nBS3Hdo/Q7wl488M+LYg2g6vbXMhGTCW2Sr9UOD+ldNX5mxSSQTLJDI8cqHIZCQVPsRXqngj47eL/AA0Y4ru6GsWS8eVecsB7P97881jKg+g1Luev/tq/8kt0r/sMxf8AoieivN/j/wDFvRviH8M9PsrSC4tNUh1OOeS3lGV2CKVSVYdeWHXB5orFxa0Zdzxi1/49of8AcX+VSn16VDa/8esP+4P5VJj3r0VsjF7i5xilPPNN5pVGQfagAP3en40KML0pjNyM+uKeOOnpTAT61JH94ZqJugqeFflByeTigDq/AuonSvFej3wJ/c3KM2PTODX3xE4kjV16MARX51WrlJAyn5lOR+Fff3g28OoeFNIu2GGmtY3I99ormxC0TNIj/FlpqN/4c1C10S7Wy1GaIpDcMu4Rse9fGnir4N61p4DQyE6vtLzWsr8zsOrxP/Fnrg819w1geNfD9v4g0OeCUmOeNTJBOvDROOhBrinG50UanJI/PlxLbs0N5FLFcxnbJHIpVlPuDT7TV73StQgvtLne3uoGDI6nB/H1HtX0JN4Vs/iZ4VE86raeILVnhN6q8SlDjDeoP5ivnPUrZ7LUbi1mKs9u7RsV6Eg44rn5bM9yEvaJwluj3PwZ8XPs/ijR9YwYYrx1stVth90sfuyr9D/UV9bKwZQwwQRkGvm39mn4Y6Td6H/wkuuQQX087/6NG4ysQHcg8E19JKoVQqgAAYAHat6aaWp42KceflXQ8g/advvs3w/jtwebm5RceoHNfINz6V9H/tX6i5u9G04DEao0xPqc4r5vuCQTXbSWhySZQeoeMc9akk5Y/Woj1rZECDANGOeBSN04pyg9jTAVR7frT0OM7eM8U3+VKPSgQYwOlAH5U5BxjmlAzwKdhFDVRi3U/wC0P5GinasMWy/7/wDQ0Vz1PiNI7H//2Q==</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDE5OjExOjA4IDE0OjM3OjIyADIwMTk6MTE6MDggMTQ6Mzc6MjIAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMTktMTEtMDhUMTQ6Mzc6MjI8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAC+ANIDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD2ecw21vutZTchht+dQGB9TxWdC+flcfTAqJiERSTjj1oiV5s5banoOpr1YRUVY8xmhaSbJOG7VpLeylCskkhH8OD0rIsoVjyEXHueTV4piuaqveOinsaUd35xjady23/Zq3bMJPMuIyEKnOxR1FYsVWg2xeM5PoayaNUzP8RXC3GpMQTgKBk9elULQ/Ow68daNV4vGOQfaoY5GjViuATgZPaoZrEt3EojTngVm6rqMUNqQr5YjnaM1DqzSSWUwKkvjC7f4jntWVLavDZzzkNAJF/e7sEDHp+dSl3LI4vEsRmMEbh5C22NR0Y+30ptzrE6QXNy0scfksQIgeG9K4LV/EXha3toYA8kk9q+fMhjHB5zz3+leceIPFRvLsvZ+aADjdI5yfTjoKduw7rqfQlv4h8y4WO52W2RlN5++fTNXG8baJbyiCW9gEuPm+fhfxr5c1bxFfTpEl5dSvt5Vc96n0jxPqGlwtHDFE0Mmd6yRq2QfXPNLlYnJH19a3kNxEktu6vG65VlOQahuJBLsxkYPI9K+bfCHjW50NBJYySTIo3y2ZbKY77fQ49K918NeIbTxJpsV9ZMdrcOrdUb0NJprcE10NsZAGDU4OF4qBT8vFOZ9q80tgI5Dhjn1poB9DTgQ3NSt0pAY+o5E45421TP3Tmrupn/AEhfpVKYZTIqWUdB4ZBGixe8rH9ayNKbE2tP/wBNm/QVu+HB/wASS292Y/qawdMANpqzjq00lc3VC6Fa6YNBZjvj+leU/EfB8TWKjsK9ZuF2raKP7teT+PSD4sgTqQuf0rttdI4+pysmd7cd6Kkf77cd6Kuw7n0Xl7kpHAXmkI4VavaVbugYkkA9VY55rHeeS3KbAo4yWFammzz28ayXBVoTzmM5212e1UWcN+p00enlFXE0ZlYj5Aen41Zkt0QbHZS6jJIO7PtWFBrtuGZi5LDrkUkniCOOFXkt2yxwCDmsKjblc64TVjo4miaPYIokbH3+c0lxCY0XjnrnHWs60vop4xJH25PtTri9O0uqhsj5feoVy7mHfln1CUcDGO9JbxgeZk5bHOegqrqmqQWt03n7md+QiLk8Yz+HNcx4u8SLp/h69uYZkj8wBIlBBYk1ElqdEFpqaWseIvsFrJcSQgWwJ5eQIW+g9K8b8b/Ea+1lGtbcfZrQrgqGyXHua5bxBrt3fviaRig4VN2QtYPm+YXLdMflTUSnJDZpDhhnGeetZs7gR4BO9uc09nDOVZtq5PNNWHzo1MZ3dsCq2I1ZE7y3zrnHyDAPrV+GSRfO80jiPAAqzY+H7x1SRV2Fmwo71rTeE9UjHmhdxYYxip9pHqy1Qm+hg2l2kPzISj7uo9MV3/w58dReGkljvInlt7hwzFDypAx0rzq802S3lMdwjRN/tDg0sMUhVEBGAabSkRblZ9Z+GPFOneIY92mXCHaPmjPBH4V0a4A+bmvkHw1rV3oHiGC8t85jb5lzwy9xX1B4c8QWviDTFurN8dAynqp9DWTXLuWnc3A67jz3qZyMDpVSJAVJPXPerGN0YweRUoGZeo58/j0qpNxGfWrOpOFlyT244qnMQIckhiaTGjq/Dw26HZ59Cf51gaVj+y74jvLIf1rodHG3RbMHuhrntHIGjTt6sx/8erGKvIUnoQ3LhpIl/urXj/jcl/Gy/wCyn9K9aun/ANOIH92vH/Fzk+NnPon9K6zjT1MFy29ue9FK/Lsc96KZVz6SjnW6BRmiQAdMCqE9pFE2yJi3GSN3FYrSmK0a6kmGMYwRzTodSt/JcxTtuH3t0fJpTxFlY8p1r7nQW0FlcKkLNGsw5ySTu/Wr2nWVte3QX5d8R+ZTyCPWuVs7iUm3LKEEx5bAy3pikju7yK8uLdJDG7n5ScDb+NY/W03sXCvHqj0LUdL821MFmEiGckovzH61jX1xPDNb2Mbnc2FVieQefX6UmiXrBSsl0Z5hxx1NYXiSWTdNNK/ykgH5v19citKWIU2dUailscd468S3Wma1fRkRG4MSx7yTjk5wPfp+VeN6tqc90cM+7Dk7R0FdP4xmWe8vJGfkPtjDyAttHrzz1rgLqZo5AF4yPStr3O5XsX9rsfmxyMc1lXUpQleCKljuXVMZO6q+0sXA5JGfpRcCO3jDyncPmxgZr034b+FPttsLiRAMt2FcnoGkPqNyItnPGcV9GeC9NSw0+GBY8BQM8Vx4mqk+VHpYLD6c8kVbHw3DBtKxLwOuOavy6YNnMYIHtXU+WiAcfpTXC7eADXK4nf7V9jyfxZ4ctr22YtGDjrxzXmGqeHmso2MLHbnIyOntX0VqUKsTleD2rjdc0eIxyFkzxWlKu4aGNfDqorrc8PtlV5JUmyHWus8A+LT4V1JxODLYzfLKo6j3Fc54vthZ3TywDbsP4kVh3V0JZBjHIBOK701ONzx3FwlY+ufD+sWuqWMVzZSebbyZKsa6CM/L8tfN3wv8Xx6Av2K5LvaM28Y6oe+PavfLLUIZbeKeF98cqBgRWT03KtdXJbwDz2BAP1rPuogVyoAANXrk7pmIOQelVZ/9SalvQDqrQbdGtvaIn9K57Rxs0EEfxZ/nXQ52aLF7QH+VYdioXw9bYH3sfjk1EHaRM/hMy6AF423n5c15F4iUSeMLg+iGvZrpAL1sjb8orxnVm3+Kr/PQKRmulPU40c66fO3Peikc/O31oqhntEVoZvMzcpLHF1zhdzemK0NP0k3LCa5tEdW4wG5I9qTTb+OzhjFtYoCyfvHxuJPc81t2l7p1lp0TQBxLyTAwLOc989q8ypUknoeRFRZi6r4S869SXT5TGqjd5SvuYH29Kpx6fNA+J8bydpDH5vxzXVQ6rcLLbD7EYftBIjwwBPvWXfXNmZrmO6M4uE+64IYk/wCFRGo3uimkMuLR7SO2a3+V5QQSXBP6Vzni6GdNPlO5vlHI579663TojcWMUlw+wZyNq/N+Ncj8U9aubLRXijdcb9q4A6e9bUZJysjroatJHgmrzGTUGwAP4SRxWYTliG5A4+lTXdy0jy79uWJbmqAYgZUgeuDXpI9J7EZfbPtII7Vf0uPzLhSOhOOmaqbF75LMOtdR4L09ppN0QyQ3ORkGom+WN2aUYc8kjqvBNq0eoBku0ty5+VWjDE+nWvadLku7Eo90sVxGf+WkQxj6ivH38JandXv2m2kCR9kBwQfr6V2Giw63p1w4JkktiSoEmOFx1JHfNccowlHmvqepGU4NU7aHrYlt5rcPwARWRfXThdloiEnPzMeBWbDfOmlgOQXY8VyPiK51e7meO1ElusS/IdhYSn2xWVFqpKxpVi6SvY6C4GoSSHZeWm7uhjrPuzO8TLcxhJV+9g5BHqK5fTrPxEdYRo0zbrIcvICpK+uB3rublGMGJMFgPSprR5HoXRqc6Pnv4kN5d06J3bn3zXLQWqKpLn95zkV1PxSHlas6r7GuWkbEZkWVcEAsvfNd9D4EeTiv4jJonERjYD5T0J7mvVPAfjtLK1SzutzBAQpxu4rxmBzO8cRYgE8e1b+ko1vqUZhmUFSCGzjJrSSuYRlY+ndD1ODUbdpbd96Z4PrV65x5GR0ryLw1fahpP2KF3iMcw4C8nLdRXqNlcrc6euM7hgEHgisJqyNWjsr47NEPtbn+VYyAjQbEDvsrU1xtmgze1uf5Vm4xo+nj/d/lWC+Izn8JY1GKK4jD58oquCT3rwPUwo1zUyD04Jr17UrqVZJ41kOz0/CvG7rnUtXY9N2K647nHEwmJLH60UpNFalWPdFsPKuGhkMrx7dzMnGPYVlWt/NDLK6I+1mIjDnnFdW11cWdpLbWx85GP+t2cn2rmNR0b7KPtCRXDOw3DaeN30rlqUmtWjxWrLQv2XnXih7qX5ugJbO2rV0we6jhUncg6qo/Wqmh26XEci3VtJCEGXBYAE1ZsdFljgvLlFMikYQM3I/GsvYJ6ouNKTVyXWNRis7PYswbaNzygdD6AV4t431iXUPMWVJBhiFDDGcd69N8V20MunxRpvjkjXc5deMjv714l4ma7tn8u5QmGIkht3XJyDjtmtKNJRlc9PDQUTlNQKlsdx3qKPA+QE7HwTxyDU8zK+8xrw46HtUYUKgLE7hwAO9dh1BxuKkjHbsa9T+FmmfabNJE+40jZJ9jXlDMGmYupC7cA17J8Dp9/h9hx+6mZfz5/rXJjZNU9Dvy6KdXU9ksdIjW0V2ISMDr3qlfLC8gitgiZ4G9utXzPvt0RyfLAyR61hX/AJM8u5sde3avM1dopHuxWvMzSuLCWGGICRJDwTzxVm1MEzGBwY5AoOcgjn3rKmitpYMTBpOmBJyBip9O8pcqD97gYPSr5XTewpWmja/s8wZZjn8a5/WpiiyYwOK3JL8i1aOQksnFcZrlyTBM46Y61nVd2rE04aO54X8QJPtWrSbiM4xzXJlWaQI0Y29NwFdD4xYy3TSAIR5gXOfm6Z/KudkZyqhWI+bJGeK9jDfAjwMVb2jaGPGizxSIW2HrnsatPJs2Fc461UuSI2Kht6r0ap7QPPxI/wAijINbHKdx4HvjHrlgzRS3LuGV0znaccEZ/wA8V7XZSblSQIUGcNzxXz34P1caNrkF7hXEbbSpGQVPWvoDQ28+1U7CqyuJUBP8LGsKq0Nou533iGQHw7cMP+eFVpQRp1gvsP5UeJx5WiXK9tgxS3h229mB2H9K5ofETU+E5nUH/wBIuCf71eUXhBn1Mju/9a9T1JuLgjruNeXEobe9c4LFyDxXYjigYORRUgj4oqjU+gZDbPOqRXDpGfvKr9aZcIRErwbyVbPLblFVdc8KvZW324XKswGdvrWfo+pYiZL64CW+c4H3vpXPXvGXvao8ionF2aNK3ttUMM11GkcqM2XVxz9a6PQD5tmYZroCUtnAUDFSeEtUtGs2nEAK5JXe2dwrKvb17XU5Ly0P7iRtzQKBxWkZW2R1U/dSJdegitpSuowvcRyKUDbcrz/Kvmrx0Ik1e4g3PIC2BuYkqo6DPQ19Y6jcR3+j77QRvvX5t/RfXPpXy18WFjt/Ex23CTiSNSWTGBxjjHatUle6OyFr6HBNKFDK/B4wD1qMkKThDk9qZeFTOQvUYHJqtIf3hyT8vcVRqMkclSMEDOcV698Cmkgt78u2IWdPlPZjn/CvIGIRwwbcOhFdv4Y8djw74bu9Ng06KWaZ1dbgtgrg8ZH4msK8FODR0Yep7OakfS/mLLbKFOCBggdaqWWniHCvEjxk5JI5rnPCPiCHWNLt76BlwQBIufut3FdxZkSAEEGvMTcGfQQkmrrYo3tniMrBAvPUlif61n2OnvDcl3dgT23HFdROFC5yKwNTu/LbanLE4FOpNtlqV1Yu3jJ5LICC79TXGeNLqO10+SOP7xG0fWti4ult4d8jjdjPJ6V5j421oYd/vf3R6mslFzmrEzapxbZzfibQPJ8Hw6yWdZZbtoyM8bQo/rXHSKXiQtg84Hriup8VeLv7S8JaXpEIwtvlpBt+8x6nP4Vx6kttKSADHzA8V7cNFY+anLmk2LdJkYiUFFGT7VBYy7J9rEhG+8Fq5JCpXc2Dgc471T8tFYsM/Q9qozLpZBMDFnap/E17R8K9dnmnFlqDKyEKY3z0C9j+FeKW6qUGF+fsQ39K9J+FCyxa1AWUFWyd24ZGKyrL3TSB9EeLGVtGkZDuDbAPzpdQ4S0X/ZNU9e3DSBnIEk0eFPOMmtDUQPMt/ZD/AErkp/GFT4TidRlxDcZH8TV5arg2l2w7ykV6Zqj5t5yfVv615dbAtYzYHLSk11xepxxRW+ain4PpRVjPoC61lp7ryJVEkYGWO3pXOS2trrFxNaWytGMFiSNpFVl1/SLIp5GqST7m+d/LIwK2G8ZeESpj8wMyDJZlOXP5VyVVOSPMcpS+I5PSLi903UZLFbjaM4zjOa7LSdPsJEaW8u53mL8qrYB9qydV8SeFZ4xcW9wkN7kbcJwPrxWJfeI7K/kaJdVtVjJBztKkGnThNrUuLaWp1vi+/aw0a6W2jSJI0JZXOQwPH54NfON5pU0rXMwjztJwwGMj2Fe52dxp72MlvPqVpNHIMHeSTz9a82+Jlk6XccmnSM9nFFn9wfuN/hXRTi1ud1CpfQ8nWLdIxc4HX3qzMiiM7VYr0znrVlViKzrcxkuSGDhuB61SdxGerMp+6M1rY6LlGRdvycg05FSNz5n7xccYPepHAklG4kLjBwM4qdP3dqoJUrKSSuMYx3pW7lXOl+GetXGka8IVcmGcENH2JHINe/abr0Ii/dOFH9xzgj6GvlzTZTY6jazp95HB5PXn/Cvf9JutOvbZBcIyS4GK8zGR5Zcx7WXScouJ1VxrrtGQm0Z/vPxWLPq8FozSSyme4bjjoKfDpdlM4AikYHpyRXQab4dsI8SfZI8ju/Nc6sek7rZHEbNU1qT91GwjPUngfia5jx9psWi6TJLcyCS6cbV54H0r2DWdUtbGB44AJZEH3Y8cfXsK+f8AxXd3Ov6pNNdSgxK3yIpyo9/eu3CYadefubI8/HYiFCn727OKjfzeCMEcmo3UGQGMMB35rZm05llby8D1GKpG1ZJCPLkPGQVFepKjKJ8+qkZELTEcIpAHXvVZpWdsnOavR2V0VbyY8lhn0NH9m3inL20hyMnA5GKycWt0UmiKxk2zqMfeIGK+gfhvph8mzzD5SGQNISvL8jAFeNaXoFzfKz28YMkXzNFuxJj1ANe9fC5roW9tDdQSxBZBsEww5H0rCtflNaZ6B4tAW3tlHe4QYH1qbVDiaP2jP86g8WcvYr63S1JrH+u+kRrkp/GFT4Tz/V/l02dh6Oa820f57aPccbpW5r0nWuNFnY/882rzKxby9NgYHDbyf1rsica2JJIiJGHPBoqQ5Ykk9eaKuwz3j/hBdEmkcw2tvtC4D7duPwFeea38PyL1msoHwGwVOQGHr7V6PfyX0bwCGXzlnIBK8bRV2S+ksXjtJpFZGHPOc15tHnhfmdzz3Zs4G38AwpHDLLo4MLEBmeU5+tV77wTob6nNBbQFGAG1d5HNeoLq9s8KpJ0Tsw/Ks7WIlWWItsLsN429RXZQvJe8y2oxjY88tfArJJIChIXhcNWjZeEokgcXKM0uflBORiuz0sho5Mg4JrjPH/it9HlWz07Yb6X7vOSnODiuxRsrFU4tWaL+pfDfw1I4up9PRdqjcA5VeO+Ogr5w+I1hp9p4ou00jyvsSsBGIiWA45GT+Nd9req6k8Mf2m/up5JASUMpI/Lp2rhdSs7uQtLco2MbiH7elEaE72Z388bHKyHMG11xzn60ix+fKNifKcqoJ4FXbiydpVdefmwBjrWrrGjNo2nWolXFxcguc9VFKpB03aRcPfjzI5u4QAkD+HgfhX0B4DMcuj2kjoC+wZyK8d0Lw3d6nGk2V+zSOyh8ZPGM4/MV7X4asUsbFIip+XoBXmY6UWrI9nK4Si3J7HZ2ITgtxipbqRJQY1Zj7A1mW8VxdfJAMDuxOAv1qn4n1SLw9pxaOTzbt+EI4APr7/WsMJQnWmoLqd+KrxpQc30OZ+ImrLZW39mWOElm5lK9QPT6muBtrZTbTzEjEQ+VSQct2yM5xjNM1AzXUzEAySSnLHGS1Ot4Zp/MtpVEMiDOCOGr6yMKdCHsE7dz46tXqYiftWr9iBLS5ugZERirHllWpv7OKsE2Sh+wIyTWhbxzwXRh8x44VYqzJkAkfSuksIormRIrJ5VBOGZM5X3Zz0A5Nc0nK9ou5cErO6OP/syYNlA7sDj5T0+tbOh2djFcoda83bKCG2H7n1x1rsPDunWd1dws0beXEGbzDJ9/HO5s9Ae1Tx+E7e9M99cymGEFnEanbgZHHP1q6VaEYyVUyqU5XTgcl4ns7Kwjtv7NZS7L80kZ+96HNdH4L8Yy2ktuNWdp4YiNznlo1zjPuORWHHp0eoeIINItyxt0/ebv4+UDMM/UfrXQ+ItAt9P0C0nGneTLM/k+X5mWJPAJasasaSp8r3ZtBzk+Y9N16aO6uNJeF1eKS4DBl5BGKk1nIml9of8AGvP/AANqjpqFl4fu5fMks38yJs87SOR+B6exrvtZbMt17RD+teSo8lRo3qP3TgfET7dAmxwPLNeYIcaXb/U/zr0bxM2dAnHpFXnAGNNtgPQn9a6FqzmgTCXgUVFt+tFajse/waLdRebcGV0XdmKLOciozot9qdzFJNMsaIc7RXSl5bOETTkYPC5qFbpEkZlQsuMsewNckJK+qPPlBSW5Yu9IDQJ++UHHIUcmscW8dqshmV2kcEKW5NXG1K3giSQXeGkbBHXFZmoa1Ct4sUUwkRjguRkCt432CSS0M7Xtcj8PeHJLqUZlY+XEM4+Y9K8qtdGvdX1W9vr+QjYuTIDkBR0A/U113xGmTUYrO0gAmMUwkkUnAyeFH9aiWSdtHuNH0lJLq/jTDrAm4Lng5J9uPxrvjFytynTC0VdiWvgMS3Om3lxJvsXDiUL1UbCQSe3b86xfiMySaVbkIqSXkm5EB5WGMbVz9TuNdZo+o6hbaEZ71ZI7i3iksZ43Xbkbf3bH36ivPtWkm1vV7W2Od0mI1H9yNRzW1K9OUpy2iW4+0ShDqHgPw4t9ci/uUPkx/wCqUjr712HiTwfZa68UlwXQxggFPT39q6PTbKO1s44Y1CoowABW54csYL7UhDcSKkYG457+1eBUxEq1RzfU+kp0IYeioWOI0vwsdL0eaOND9gBDB2HIfoCp9f0rTgtoI+Y0JHbzGz/IAV1nia8inmW0s9v2WA4+XozVx+tavZ6PCxmbfPj5Yh1Jrm9lUr1OWmrnVCpClT56rsS6jqEWnWT3F3IFjXoq8bj6AV5Lqt3d6/q24hnkY4RAOFHYVb1XULvXLgl/mYDKRL0Uewq5oUSWbK/+jpeqdpS6Xjdnsa+mweHhl0G5a1GfOY7Fyx0uWOkF+Iuq6Tb6PpVjPMjtNIxBQgqSMZP9KxQ8Qniy7LlwTITkhT1+prYvJJNS1Az6w88yoSP3SjZFz69+lZaz/Y7jcixzJ/ddeG9OK6cNSVZN7s86vUdJpbIbqF7BeT28MaSJawDb1+dyfvE59a6TT7+KSAWFnZN9lRWkkBl2vKB2yB+neubmv4rmWRobVYZZmzK2c49AoxxWnoNm+o6ktskQkZiADt5X1NbLD01SvLoS60nNKJs2Oq2gaVxMtpJcAEtJwsIGRjj2wPrWzfXFzdabE1ra+euGZWQ7ScBfvDqOTwOe9Vbq0sx4stNChVUtvIy8rKC4lbLKc49Cox713dvY/wBm2m26lt7OH5Q7S4IJ9V7j1x2zXmYiUdOVHZSvq2eT+ErB9R1+5uGkks5IiGVlOCpJwFye3bmuz1hLyW2hg1hmuPKZmgnVNjI54G8Dg+ma5vUNasF8RXDQp/xLp0MErrwzjs/1Bq1d+MJjfJYJdJe2jxqiyOuCJOMNn6hc/jWtfD1JtNKysZ0pxgmpM5SKVNF1U3tvHdQXNsTtaU5GRx9cev1r2ea/XUNMe8TAWaFWAB6cdK8r8TQtfTKWmUrxhyfmG4D5H+nOD9e9dL4Aumh0u90q/BS5tjuwejIe49s/zrzalO+pvJ6WRF4wQx+GJZAeXj6V5whxp1sD1xXo/wAQpx/YMkaY2qvGK898vNnbD/ZFRDczhsQ7j70Um7HGBx70Vdyz6D1KeSe0AOSq8jJrMee7ey2x7gnc+tbs2neZcNArE/Sr+n6RmI20zqoPc9hXJJtv3EeYoOWxw9vYedFmSfac9KsDTxbyR7V80lufaulvPDsFrM5EoYY4xTILFUB+YiupQk9UyfYS6njuvWF//wAJdHbKTM1y5kiEb5HB4BHY10PhvSdT8K6vPcaq6pZXMLRzyxn/AFZPOT34PerOn6pZWvi3Kwk30ZkjVRGPlJP3zj29yfpVvxd4kFu32C3j+1XEwxJuJBUf3QOg/Ku2M6ijyJbnfGELJt7Gb4u1O4fT4bea6S7iVR++TP7wdifU/wBa5Tw7FJPr1tJCu8qr7uedo5Jrcut2pQJpNnCHvCd2yME7fYsa6/wJ8Ov7PuI7zV5d80fKRITheMHPr1rtiqf1WVOe7KjKUa8Zx2QtuxaMc1Zjj/i/LtXTXvhqCYqbArb4+9uyQw9qzrzSHsbC4uJrqILEhc4U9hXzn1WblZH0H12m43bPMvFXie7TUJNO0tQpU7NyjLsfauPvYbnzG+3F0lboWO4ls4xV6LzjfS38wnjLbm81ByCfSm3M9rdKkkt3MWVi23Z8x+p6V9FSpumlCivmfO1q7qtyqP5Emi2VtCzo90FuVUuGA6N6Z9am8Qy72S3uUZUIADKuS0pGMmqKmzAUr9pU/wB0KK1btrvXoYwY1tjbjepduZcdOPWniqCjaT/Eyo1uZtIqaRomNON7bztaXZJVVztDsOlVddkS5SGUrsnVAkoA/iHB/lXXS3tjf6XLpki/YL0plEkGAzjnAPYmqegadaXHh+WYoramrtvQvyCCex/P8ayw054duckXXhGuuRMi+H/gg6mpub1W2Fdwx/DXRard23g7ULi30yyha+kiAEu7cqg5B49TVzw3dT6va/ZNMliiWPd5spOTGCcAf7x4HHQVwviGSWHXLiF5IppIsL5sakBuM9DznnH1FVRg6tVxqP5CqSVKCcUddcaNJcr/AGhaFZdURQ1yhHyHcB8p/D06VahksLi38jV4LmGYfNiTM8bewI5HJHBArI0O8OoWTNcXGLxLmOQEj5mGQuOOvFaFxBd6TbXL39tI8V1cMpmzt8ndwrfp/KuWvRlCfLc2p1E43GwaXavDcNbLYXqKCFt7eECT/wAeOa4TxPpZtybqG0uLQ5GUeLaoPXKnJ5612EdjczxrJq260u7c+WZl+Tkchsj19T1NL5Mtxb3aXcTHUwAzKx2rdR9CcdMjPP51VPEOEtWDpc0dDjzr0VxCs0wVbsYW4TblZ0P8Qx3BJ4PXJ9adYahHa64gQnE0Tw/ezweVxz9OKxRab9fhhtFdlMoIU9VHUj8P6e9FzphsWhvY1/dh1ZhnkAkj+Yz+NTiY01blCDm1ZnU+L3P9izZOcgda5V3Kx24/2RXVeOkMejtkjDEGuTmUk2/oABn8K4IbsaI2XLHjvRUjKcnrRVDPqOCBUYvGxJzgNTbizmVvMjn3buo9KvaHeWbSAXB2r9K0tWmtXVY7RQCf4sVG25hGHu3OUTe15sZSxA6Glvw9qplkAwo4Hr6CtO+hWGLz43Hn1xHjHXJbe3SHlpJOQVPQ9q1im1oKMFzXZzerwRQ30klo2zUI2VnmRsF3yxcE/wB3lRUGjeGdS1XWJHgZkidcyXbjnnrt9/8AEVo+DdEl1m8SSVGSGMbmLDO7J5/DjpXsVjaRW0KxxKFVR2FdkKjprU3cFLYxvDfhmx0K1CWkY3/xSHlmPfJrcZM+x9RxUzLxxRtNZynKWrLSS2KvkuFKrIQp7ba4/wCI98mleH9rzKWmfZhxxjvx3rt34NeQfEq9lutZREmEUVv+6jLAMrN3/wA+1VBXlYJaK7PL9Rcagxd7qXCfdUKBz9PSqdvbTZBY71B9K6+SG6ijaaV7IRtyTNEN59sd6bFqflWj28eGL8EGNVA+gHT8a7KFWpGd0rnLWpRlHVlHw/ax3V35bqzybCYxnALe9bunLNDepeSqDn5HVlzjJ4I9BzjNTaboUDW8d2fLednBAi/h/Xrito200NrsmsWuIHVtzK+woOx644pV8QsRW02ChQ9lDU4v4gaYlxfJOZxExZV2EdM+/wCH5VU8O2NxpEOqXOobnuBZO0ILZZicL+YDEVFr+pre6q5mVxEWRE3DrtwCSP6CoPB0Ekvii3S9Dizume3Zskr8wJA598GokqkFyyZUXFu8UGi67/Yccdxp5kEiMTIGb/WKDn5v6e9Qf8JFaxNcXE0csk88vmiOMgnO4EDkHGMDn69ax/GlrP4c1SSzMhnsXJa2kc4DDuK7H4b6Tay2kM+oWiPNeSbDgZATCtkegxk/jTnXpxSkt+oo05tuPQwrrXL+8lOYo4IpH3tFCAMntkj+mK9C0TSLu88P20GpSx2izMJA7ys8kg7AqTjuPzqW38N6LY+JtMt5EuHWQMXXGQWz8o9uK6G9t2sbqKXUIYz5cu1lbIVVbAGO3GBz6daqvWhNLkFSpyi25MfJCktlcaQbhWuDGtuwlG1+BgMAexxnPvWFYatDcQRWGrSJZ6zp7IsbTDAkC5GMn1Xjn61veN9Dl8VTaf8AYVWF4oy0kjcEAkADjvxXI+KvBsem6Eb661SWSeNNqljkM3ZRnmuWjClJWb1ZtUnOLuloirqUWn6TqlxbySrDdTxo6TFflOMj7w//AFcVzt04vTfhgEjVmj249uo9eAT+NZ+mkXmradFqEubdXCDechUznb9Cc/nW/wCJNIWLVGlht42gYMZfLlOQxPXA7dPzp4jDqk7MKVV1FcpeKbg3HhuDfncrBGz61hy3MixrbcbSQ3T2q14qLRB7TcTGWWSPI529s/57VQm/4+Ez1C156VmXJEwJxRTd1FVYk+i3j2Ebjj2zVn+0QkYU5OO4qCZVZctkmqfygnit+REKFiPUbm5uJsRMQvTmuE1B5bvxVDDI07H7gKjOznBI/PrXdocyZHrXN+E5JJvGMccuwqwaU4HYNnFbQSTsNR6nqmgaemn2MUKZJVRuYnJJx61qp93mq9v/ABfSrK8AfSoerNthyinEY60xGpXbipEV5T1NeB3QufEGsX1s1y6wM7vjGQBniverjiBj7E14d4XVoU1C/BBKME249T1rsoS9nCU0tTGquZqJy+qtqNg72MtxLtQ7QM9R/hVCOBxGJkVwgJwxyBmvWE8M21/d/wBpagfMhwFEIHYL39+KPG9hFH4QSSGGKMgqSq9FGSAB+VdlLMIKUaaWrOOphZWcr7HDeG9fubN/s6QJOZGGM9a7+6tZDZBLpN7yL8wbOCcf54ryeyeaC+hktpDHKDlW9DXqt7pOtrowu7u8tppUUSL8zjHvn1/CsswoRjNSprc1wtRtWmcV4ljh0+/srO8SJbSWPG1k4WQHgn88Z96y9Gulja704GRp2/fWa7dzGQDGA2cHvz7VT8SX0+tXfmXRwyjYBuJx+Jqx4s0NNM0zR9T0+aSKYqhTB+7lc/zzWNbDSShd6sunWV2O+LBttQ8P6VcmEbzCAqjnYycMG9u/4VH4Clu7xLIW8exRAg+dtqA4x+WFBx3qlNcyeI9Au9MEUcUyq900uTgMoJO0ds+nSs/wdeibT4bWZcwRosgx97OQDzn+6x/SuX2DXus6Pa3sz15rW61fXrWKG5VYrLCLMoyXYjJHQ8AYH4V0WpXdvO0keoy2qSbfL80gqXHP3gen51z3gLU/7UkeGGIWu2QA7DwDgnj6g11N/Z2AiuIksopEicRHzf4nxnJA7VzqfvWl0Kskro5y41mGOfTbSSeMTJE6zMGDAtkYOc8g8885yR3pfGmiza9pESWk5iiizKyyrgM2M5z36Vj3nh+xhu7f7ZGZHvpyqtEdgiHGCFHHcV1Vva/uWTduEBaBweCCqnBVhjI46EV1VrUbTp7mcPfvGR4PdWk0N59lljZJSdoUjBOen4U7w63leJbWKfhGmEMoY9j8rfl/Sut8Z3tpc65As9ufLiwZXTAkIHGFNct4mQQS2M9uzFWXKlgA27IJJx15au113Wpq63RhGkqctCHxQGi1GdZQA/7vGOQBzxVeYf6SDVrxVFmSK6BP7xlUqfZVP/sxqq7Zmx3xXjdTre5LkUU0LxRTJsf/2Q==</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEBLAEsAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMTcAAJKSAAIAAAADMTcAAAAAAAAyMDIzOjAxOjMxIDEzOjI4OjQzADIwMjM6MDE6MzEgMTM6Mjg6NDMAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjMtMDEtMzFUMTM6Mjg6NDMuMTcwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwAGBAUGBQQGBgUGBwcGCAoQCgoJCQoUDg8MEBcUGBgXFBYWGh0lHxobIxwWFiAsICMmJykqKRkfLTAtKDAlKCko/9sAQwEHBwcKCAoTCgoTKBoWGigoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgo/8AAEQgAvgDYAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A+nKKKKg2CiiikAUUUUAFFFLSAKXFFQahe22nWcl1fTpBbxjLSOcAUAWMVmazr2l6LGW1K8ihOMhCcuR7KOTXlniL4l32rTyW3hzNpZKcNduPnb6Z4X+f0rg9RusyM4eS4nY/NNIxJJ/Gs5VVE2p0JSPUdV+MFlbyEWWmTzoOPMlkEefoOSapWPxk898S6Ngf7M//ANjXj88Ulw+ZGbB7U+G3eMEp19TWDrs6Y4VdUfR+i+PtG1IhZJHs5COk4AH/AH0OPzxXVoyyIGRgykZBByDXynp1xcQyFcBh0YN0Nd14c8TahpAV7IvJbDl7Z+QPp6fUVUK/czqYVrWJ7nSVieFfE9h4jtd9q3l3Cj95A/3l/wAR71uV0pp6o5GmnZjaKWkoAKKKKACkpaKACiiigAooooASiiiqAKKKKQBRRRQAtKKSnCgCvqN7b6dYz3l5IsVvCpd2PYV8+eMfEl34uvt87Nb6XEcxQ5zgep9WP6V2Hxq1otJDpUL4iiAlnA/iY/dB+g5/EeleRNdbzsUkr1Nc9WdtEdWHpX95lm4vVA8m3GyFeAB396hDFsZ4/GoooSwB/Sr0cIVMHmuSTuejGNhsS1Kow5BPvUiItSBQW4FZNGqGKPTrVu3neEg5PFOhtWdulWmsjjOOBSV0N2Y1Lma0uE1HS5GguYzubYenv7j1Fe1+B/FEXiXTS5AjvIcCaMdPZh7GvDcG2bOOO49a1/BepjRPEkFyGxbu2yQf7DHn8uD+FddGo09Tz8RRTV0e/wBIaXrRXaecNooooAKKKM0AFFFFABRRRQAlFJS1QBRRRSAKKKUUAKKGYKpZjgAZJoFVdYcx6PfOM5WCQ8f7ppAfNfjS/l1PVJ7jJIllZznsM8D8BisSwtWllw3HHFdDFZrcXDu+fTg0klktvKp7ZzXDN3Z69KNlYLG3QLg/eHBFLdxRD7mfSi6IZQyA574qACVjjBAzWbaNUmSQAE8DFTrFtbtinQ2/zAnPPfNWWi/dgAis2y0ia1OFycZ/pWgpV0xxWXCkm3gdDgHuatwOSFByMDGSKQMq6jbZVgBg44rLhUxTAEn2FdNIoYY4Ixg1lX9sBLGVYAqRkCqi7ESV0e5+Eb06h4bsJ2OX8vY2T3Xg/wAq165H4Xyl/DjqSTsnYDP0B/rXXGvTg7xTPFmrSaEpKU0lUSFJilooAKKKKACiiigBKKKKoAooooAKUUlLSAWq2rJ5ulXkf96B1/NTVqua8R+MtE0eWSzvbvbclcbVjZwCRwCQCBSbS3HFNvQ8Ttn2TMO2TS3DPcsyxkYBx71BISheTrj0qoNWjsjlvmY8bV6/j2H41573sexFWVyO5vorJ/3jOcdwtVf+EntvO2/MynjOKz9c1u13ozeVhjtBMhIB9MgYzWWtzZSSBWAhZh8rg7lb6EVMoaaoaqa2TO9sdRiuYyUbAOABVtrpEG5yBxk5rl/D1tLLA7q25UJ5HfFT6jFcNb7jkD6Vg1Z2OmLurmvb+I7GGTbKQOeTmtSDxDp902yBJDxyyLwK8okSF9vmu8jMflSPGTWtpN3b2kwhfylOeVa4UNWns7K6MXUu7M9KWUFMow2npVC5Yl/xrLTVIJXWBEeG5HzeW+PmHqCOD+Bq9BKZ43DcMDjFRfWxa1R6/wDC9caBM2B805I/75Wuwrjvhrdwr4fEUksaS+cwCswBPA7V2NerS+BHh1vjY00lKaSrMwooooAKKKKACiiigBKKKKoAooopAFLSUooAWvk7xjf3z/Fu/thO6xm9ZdmeCuc9K+sRXz58XfDTab8S9M1mNSba+fBOOj4x/PH51jWWh04VrmaZCgCQyblznjFVDplldqGuYwwzllYZB+takaApg9KhmVkY7EOMelcDk0z1oxTRxfi3Sbe5FvFBuMFuCI485CjOcA4z+dZg0oXMyssPlnAUoMbTj1GOvvXcXFuZ2JlOB6DvRYG3WVhEocIcEgZGfQ0e2exP1eO5d0CzW10wRxxhRt29Op9a2otMV9LKsoL/AEqrEzSBcnavYVqwu8ce1OR1xXPOTbudMYJKx41r2jG21WUiN44Wbdti7+o/z60yz0e2vNa+2SsIycAR7QFwMAAjPTA6V6Tr0tsqtJdRAR9GcjIH1qrDokTBZ7bbJH1wyhh+dbqu7HPLDxvqQW/hLTZFV4GkQ53D95kBvUDt+FbI05IbVhnLjqfWnWrxxsFWIJ7AYq2+PLOOlZOTb1NVFJaHCeNNSudKFrPaRxlmDKzsM4APb8698+FOsSa54E028nJMu0o2Tk8E4/TFeF+PohJoZxy2/CjuSa9x+EmjzaJ4B0y1uciZk81ge27kD8sV24Z3kefjElT+Z2FNpaSu08wKKKKACiiigAooooASikpaoBKWkpaAClFJRSAcK5zx/psWoeHZGlwGtXWdCfVTXRUy6t47q2lgmGY5FKMPY1MldWKhLlkmeARy+XIR74q+yqYi8h6Djms++ia1vJIn+/G5Q/UHFZt/f7YWGcEA15klqe5F3VzG8Wa4tmHgtseY52gitLTLvTNE8OxTalKysBuIxyzHk5rC0vRm1TU/td4CII2yAf4j2rqryxtJkEc0Ec0Y6B1zimoq1g5pbopaT4xsdUjcWjjEZwQwwfyNXtQ8ZWemRrLcyqiZwe+foK5668O25vCbaLyCemzipF8IWt3JumDNgc5JNZyjDmKUqnL5nUf2/oniDQLn7IytvjZWHrxXH+CfEcul3D6desWRTgbjniuo0fw1p2lxubdAHbqTXKeJ9NS11BbpFyj8N7GklHVIblLRs9PjNvcoksWCOuKhvHVEIGAe+K5DQ9RaOJVDZUj8q25LjzlBJrNp3sVfS5q+GtCTXPEOnLcDfb27tM6HkHGMZ/l+Ne3dq87+FdiXa4v2PypmJR6k4JP+fWvRK9XDRtG542LnzTt2EpM0pppFbnKLRSUUALRSUUALRSUUAJS0goNUAUUUUgFopKKQDqcKaKUUwPIviZpRs9YkuUX9zc/vAQP4u4/r+NedzorSfMR19a+j/EWkRa3pctrL8rkZjf8Aut2NfO2q2zW93LBJgSRuUbByMg1xVqfLK56eFq80eV7oztR1iDTrXMj7U8zBx1AA/wA/nVqPxRYy2qPawyyKw++4IX+XNZjafFeXrLOBtDiRf61rx2MNpcedGgC9WQ9DUR5djaXMnfoY8nir9783ksvQ7cirVl4vEbYiWD1/eE5qC+u7NLh9tom09iAw/Wixl0T7TmXT4WwePkGDScI32BTlb4jb/wCEw094mFyGgbH3kO9T/UVz0uvWuotKsLebFlcHGO+K35xaXsw8m1jjix/q0UAH61gazYQxatEYlwJnUvt6cc1k1FMtObV+hesrY27SoDwh+U57VtafukkQcknj61myTfMcDluK9G+F/hmS7uV1K9Qi3iOUBH32/wABU04OcrIdWpGnG7PRvCOm/wBlaDbwOMSsPMk/3j/hwPwrXpaSvWiuVWR4cm5O7EpKM0UxBRRRQAUUUUAFFFFACUUUVQBRRS0gEFLRRSAWlFJSkgDJ4ApgVtQn8qEohPmMpIA64HU/qK+VbK4nm1nxBbzM7/Z7ncgfqA2Sf5V9F/2khvr+4lJJ2LHEo64y3T9DXgV1sj+IfiRdjRmYxSbX69DzU148sbM0w0r1VYLVxJNxw2eueRWnLG7pgANnisi6R7a4MsQyR95agm1kxxghgfXNcDj2PWU+kilrGjHeSSykn+FyMVDpmgP5uWdnHu5qrfajNNINrg+1Tx3rW2N0uTjtxTlz2sSnBu52Nnb+TDt4QdOB1rI1LHmoSAMHqOtQR68JI8scAd89agWRr2YMMhc1hGm73kazqpK0dTsvhtoseveI4Y7zJtly7KP4sDp9OlfQ8MUcEKxQoqRoMKqjAArx34QQPFqF3MBnyYcH2yR/hXscbrJGrocqwyDXfh4pRujysVJudmBpKWkrc5xKKDRQAUUUUAFFFFABRRRQAlFLRVAFFLUN3dRWkJlncKooAmqK6uIbWEy3EixoO7HFc+/iB7gMLVUDE7UQHcT7kjgCsq3zJcyz3V0JbpFLEZ3CMdMAd+a0jSurszlOzsjdvNeVY/8ARwE3cK8wxn6L1/PFZFvqb2y3F1qF7LMSmUhIwBxnoOK4E6hd67ps2pWzyfaLVsqOMbcDPGK6vwzepqXh17gEM2HTOOcAcA8D2q50/ZyUWZqq5alrw/cO2uy/aF2pKHSJSORjkZ+oB/KvIfjTF/wj/wARLHVTkW19B5UhA4BU9f5V6n9pEGqLOTlFl3D8XH9Caxvjt4a/tzwi8qAfabVvMjYnr2IAqsVBNk0KjjJSOFyl3bK6t+8xwezCsPUNNSdsZ8uTuD3rH8E6uZLNrOYnzoeFDdSPSti4vCW2SYYdg3UV4zThKx9BGUakUzEvdCeI5jkI+lZ6adO0g+dmHqTXQ3F5bhXBeRTjo3IqrbyW8gG2QlickAAU+eRLpQJdP0fdsBYufQc11Fvbx2MYJ2mTHHotZtldiMbRtRf1NV9f1E21m8rfKAOM9TWEnKbsbxUYK56h8EbsX2teIEXBWCOFM47neTz+Vel6Zq0Nra28F2WTI+V8ZX6E9q8v/ZntfI8K3+oXGRNfXDSjI6qowP616XpqCSxhd16diOBnrXqUo8sLM8CtVcqjkdErK65Ugj2orn1g2yb7SV4G6gA5X8qfDq81vciDUURVIyJl4UD3quVvYUasXubtJUUVwkmBypPTPf6VNUmolFLSUAFJS0lAC5opKKQC02SWOIAyuqA9Nxxmsz+2Iri4MFkfMYHDP/COD+fSsGSeW78RG2kPyBUbhuep/wAK2jBt2ZEppK50F1quMraoWOcb3BCj+p/CuV1i6zqFuLqYSKxw5cEAZ9K1LphNM2zlVJBrndXhDTjZlWz2pXtsYSqXZz/ieG6g8QSRWl1M9gApaJWITnA+h+9XTeDYY2lv2DKxKHIBIwMjHP51kXafbJpzIzvJiNTzjoue30FdN4OtFs7B92S7KoIJzyST/LFdc3y0WTFpzRx/wuEa3F9ZSxu6vHnbuyuRXQaLpraeLu2h3eU90zAIQQAwUYyfoawPCVuLfxQxIxuZ1OOM9etdpcKzaoscacMob0A2sB/7MKivq7+gqT963qcttbDecGEipxubJJAKjAHckV1TSpr+kh1wBMmGB/gPTH51yet2k0LTMHVSrSKCBnHORz07jvW38Pn8yXUrbaRGsvnLnuD/AExj16101knC5MU07Hzb8RdFm8L+K/tEEbpbz/Nuwcb8/MP6/jU9nfxX0au+Ccc5r6S8ceGdO1izmju4lPnp5bYHPsw9xxXy5rOg6j4U8QSadcDzMfNHIvAkQ9CP89a8etDmVz1MNWadjYmt7OfgnHrhqls9L05DyJG+j4rGkuAMfabWZD67DUkN9HuxDDMx9ApNcji7aHoqUb6nVBrOzh3RxqrAdScmuG1m5n1/WrbT7blppViUA8ZJxVrVJrhoiChiTHc811fwL8LS6l4hbVpYGFrbgrDIehkPB+uAT+JrXD0le7OfFVny2R7s9vH4e8Faba2ChUULCCP4UIyx+uM/jW/aoBpp+UHay8fgD/WqOsBJjBZsoKhC5UcYzwP5GrlnDPaWbozCWEu2GJwQBx/Su+Vo0/meRZykZy3TrLeRwK5ZI8oWO4ZGeo/+vVax1iy1OzkjvNqGMCSQFsZO0NwfoRWjZ+W00zkRZ24OWJ/WuTsbe3luJDHKgE0YCnnrtC9enatKUYyuYvbQmN8P7WVbfUpIgjbUVuVUD9MdK7iy1VZI1Mu3GBmRDlf/AK1edyIkNjFczKd8NzEpePp5bnGPwJFdYSltrUaDf5ckYGAmAPrWcrON/U2TcHY6cXEJcJ5qbzyFLcn8Klrlb6ynZB5FwqxqcNHJEWB56j0/CnRauuk3UVnchxHICUcEsuACT15HSs+XsaqomdPSGmwypNGskbBlYZBFONSahRRRSA878N65b3k22zV3dGbIRevHH9ahtdQ3eJbuSOGVpI1WMqVxg4zz+dM8CRwWHiq7tEVFHlhlIUDKjIB/Ig1q30qRa9OgyA80ZJ2nH3F713ys6vNFacpx8tqdm+pSi1dbfUAk8UiF2wVp17dQy3/zBkBIIJHBrS1KCNpkkKoxVsgkA1sRxRXcS71VsDoRmuRSuthKCuec2t9ax6tf7pVJUr8qnJ6Af1rf8M6vFNPOpSQFRGQCByNv19qxbDTbVfFWqSeSnLhRxxnPp0/hrtdEhjF3I+xc7UGcD3rrrTj7G1v60Kp0/fVzgNG1GBdc82VWi+YMMjOQQa6+C4judctXUMF3NFyB3Ab+aiqtvZxzea8kavsjBG4ZwRRq80zSaYdOSMDzVdzgDGGX/wCvRNc03G3T9DKNoNSNXXLWNZ5TtyWKuCeT0wf5CsDw3frbeIVjh/evJbYKryF24XJPb7tXPEaOlus2pTvkxt+6Q/ewymvFtU1a98RWskWlh7GDEkYRDguu4HDEeu7n6UJp01d3Zq37zsb3xP8AidEv2jT9GuhJdH5JbqM5SP1VD3Pv2+vSO2sLjxf4EsLzUZop7xJXW3nGdzKONj8deM5+me5rm5/BM+q6PdSpb+U9sr++SozxVn4cQajZm2igupYo1mJntyoYCRcbSO4yCenXGDkVyt+0i0axfsWpEfkSWm6C4V1dDgh15FRtIiKdpx9BXoniTw/c67cfaLZ4UuQCChBXcBjbn9efTHFcfp/hS7uJPN1oy2tqrlTGgzK5H6Ae5/LvXnSw04ysetDG05Q5rnN2mg3/AIlvTbabHuxy8jnCIPc17V8LtY0S2vj4U0uXzbqxtw0kqYMbNn5wD3OTk/X2rxnxlrt8kM2keH4JNN0qEHeeDJKenLD/ABz79qpfC7UJfCPjOyvLwFIiTFMM9Fbjn6HBr0KdKMI2vqeZiKzqPTY+kppv+KhuMsVHmKg9AAB/XdXQG52aZAX6uAQR3yc/41ymk/6bG1xuG5yzLu9STgfUEj8K19dMtq1jbwBiwJOz+8FXH/swrorJNRj/AFocsG1zM1bMAK7diCa8+8PS4tZmUlWtrplOD1UN/wDWrsI9QlgtW+0Wzodh7Y7V5p4a1Zhf6rA1rKYmujlhzgHzPb6UUE9TKzsdbqlp9o+H2pjBM6oyhs87lbj+QrUt/K1Sw03UIvmWSFSQSSORWda6jC3h3UY5NyJ5ituYcHfj+uazfAmswQ6W9luMht5XRQvOBnionTai35lSd2vQ7TTwHgClRlRtPFcT8RLkweJNESJmRY2BYKcZBDDmuxsbzDl5IHSI8ljXm/jzVrWfxJMhZi8UDOuFPZXooxfNcWtj0zRCV27GOGj3Dnjqe3T0rYtbpLnIUjepIIz6HHFcb4d1CQaCZ5EMMoUxRBurZxg/1q/4dilbT5WjbbIkmYyf1oqU/ek2bU6vKkjq6KiglEqZxhhww9DRXOdSd9jwvTNXi07xlpdzO8nlSI0D54+YEY+g6e9dnrDMdcgnSGMrI6NkLk+nXrniuU8caCh+3lGVWT9/Hx0JHr+P6Ct3wne/2n4f02e+3NKkirkce/8ASvUlKPNdI4tXB/eauozoJGw7RnPIIP8AMH+lXdJuoyQGm3AgjG1j/M4qLXbL52YbT35yDS6TZ5jRsJnr1NcUbE3d7HKQTRxapfvmUBro8cDoHz047iuk0G5Rt7h2XpkFevy57EDv6VjvYl7+/wAFFCzFgAueoPrXR6Fp+2CQnyzyozgj+Ba6q7jyF0m+ZGNoE0Mkl3GwkwyDHyJ7+1XtPsI4v3crO8WcruBJH/j1N8P2GGlP7s/ux/DitlYGXGPLH4E0qzXO7GF3ZGFqOn2227kfznaQElm2sf1FeceELKxSyVhjJaTOYv8Ac969nNkZYpA7Icqf4K8j8NQeU7QFRgPIRhj/ALFPDcvMW2+U72CCK30rUGikGzfLkHK4+X3zXnTRTWOpG6s1LyLKqsikfOGPHI9/bvXppRP7F1FGBALTd89jXjemTyP470qIMdj3McbDpkBhj+QrOKXv+qNKjbUUezLp91HcSNboI+APM2HOfXkZH4VJb6JHtUSo0hzlmYNlv0/SrCrI5+90/wBo1NG0ikfO3X1NY8tzPqeaeNdAszeG1SJVBtk6MM/6wfjXAeJNCvHL3E2SqouDs255YZzj2r0LXNXuW8V3cRkYpDEFAJz1I/q1dJpkcV9p8xnhRiUwSPlJAJ7j61rUo8tLmW5rCpeSicB8HvGcP7vSNXmVJFZVimc/Kyhh8rfQDr/k+xXDu2twrKRsEfy9x1POe3QdfSvIPDvg+yudWbbmNt7jO5j0b616TomnSWEcayTeaIxtTk5xzxyenPaqqQtJX7GXOrOx1vmR/Km5eeOtebeXHp/ivUhvQAyJJ971Zf8A4o128LlZVOB1Hc/41xXiGcp4luQFHzwbj8zfwjI7/wCyKihR1ZaqWOukjhu/Dt2rbZIwgYjP91ia57wzp9vp2qXf2eMIsrhv0962tJJuvD9+FyrsjLncT/CfWsS1WVbkvK3yBVJwc5z7YH65onH449mir3jGR3jIhtPmCuvcHmvNPEun26+LjII4wGtXBOB6PXZi8AuIYAXCumenv7ED9K4fxj/o/iKPzGZy1vLgD/dY98+vYVnRh79gU+ps39mmpQ20cEjK0AyrIcguen5D+dbumfatKtkhuh5sSjmReuaxvDM+/UptwykcYkKnk+3PetnXtaaxS3jgQGa4J2lhwAMf4itaylzezRCaa5maA1SGHUI4CRmVQ6kd19aK56NxH4itZph5glwY+OU3KCf50Vy1FyvY3pycVY//2Q==</t>
   </si>
   <si>
@@ -3527,15 +3503,9 @@
     <t>/9j/4AAQSkZJRgABAQEASABIAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDIwOjAxOjI3IDEwOjUyOjM2ADIwMjA6MDE6MjcgMTA6NTI6MzYAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjAtMDEtMjdUMTA6NTI6MzY8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAQDAwQDAwQEBAQFBQQFBwsHBwYGBw4KCggLEA4RERAOEA8SFBoWEhMYEw8QFh8XGBsbHR0dERYgIh8cIhocHRz/2wBDAQUFBQcGBw0HBw0cEhASHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBz/wAARCAC+AI8DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD7OVqlDVEqnFQatqtj4f02bUNRuYre0hXLySHA+nufakc5eJOPmziuK8YfFbwz4Fc/2pfKJQuRBH80rfRR/M4FfNfxX/ah1DU5LjS/Cg+yWmdhvW5dh32+n6/hXzpcXd5fztNcXM0mSWeSUkknvj/E0Gqh3Ps+5/a88Px3IWDRdQmj/vZVR+tdBqX7RekN4dn1TT7O7EkKkmGaMZB9cqSCPxFfD2jzWpuFMizuCRlmcj+vH4V7HoU9rdWs8NvJN5nl/dd0KMfb5s9uhAqXdGihEo65+1h42urmWSxu47UZO1VhXCj8Qc1gx/tNfEYTrI3iKYYOSvlKQfwrzXxHYfYdYu40jMcRclF5yAc8fnkVjmPa3IYe/StEroT0PrTwP+1trZuEg1cQXsePmZ02EfimcfiK+mvCHxS0TxZbRur/AGWZlB8uUgj6hhwR71+YulWkd5MsbBGYHI3cH8CCCP0r3jwHrN7orr/pErtD85Zm/fQE92xzIvP3xyO4PIEtWFypn3qZIiCd64HU5oaNc5xz0rxz4f8AjzTtYuf7F1eZIri6XMcisoSfPOM+v6HtXrEthIJWnW4kPO4JuOPp1+tG5nKNtCSVI50ZMhgeSPbP/wBakFrCkZjEabCckY4NRwac8TTtu2tJwNpOF+g6VA+lSgARXTQ4RVAQHGVbI79OxHcZFFiSxLBFujdgAYj8vQdQRj9aqzaVZ3LNIYV3SLhmQ7Sw98dazrnStee5B/tGGW2IOUdNhB37lI2jjAwOp6VfjtbszEpKqQp8i8kkYyOhGORt/L3oAl0+2W1tfLVdiLI+1fRdxwB7Y6e1ZmpE/bFwM8r36fK1a1l9oKzLdMjSK5wUGBtwCOPx71i3hze49AP6/wCNZzGjcvL6y0exuL29YJbwIXdj2Ar4J+OXxwuPiJqTWlkzRaHCxEcY4MnuR/n+Veq/tYfF+G0tpfBOkz/6QxVr50P3B1EefU9xXx3v3MAOp/StLGsFZXJYgHfc2Bwfw9qZc7pG2de9TxjaFPZcH/P86jBDt5h6Dp71aQNmhYSwWSB7iSTPaNBgmuu8L6la3N2lvbx308jfwwKRj2J3VxukaLca5dBSMIf0FfS3ww8FW2jxK4h/eYzkjmuXE140l5nThsPKo7vY4vX/AIO6n4gtPtEcKxSFy4LnLEY715zqXwu17SwVAR1HYH/EV91aXHC6+Wye3Iqzqvw/s9ZtpGSMbsZ4rhpY2ods8JT6n51NBqGgXCNd2JKjqHXhh9eorcsvE1xNEGhdvtUR3RsepXHK/wCfrxX0b4w+Gm2B4bi2IXnBK5r5x8T+GrjwtqO7YdmcqexFd9HExqaPRnHWwsqa5lqjqdG8USMqtGxjAxJEufukf3T1GDg/y64r7D+CHxUTxpaLpupXRGsWqACTI/fp2P8Aveo/Eda+Aors2sxUMUiciRPTa3+Gf1rvPB/iq58OXtrf2shSe3YOGzgHBB/oOK1kranPpJWP0raMIuBn8TmoSKwPAnjG18b+HbTU7d1JkXDheit3H51tXcDyvGFleMcg7OD0qjnas9RS6jIyMjGR6ZobgEnoKp3Olm4e3/eMoiYscD73zA4PtU8tkssvmGSQHAG0EbeD9Pc/nSESFeG9a5m5/wCQhKPQY/WumjiZS7M+7d04xgVzMnOo3HsxH8qifQo/LLVNQm1DUJri6mkmuJnMkkrklmY8kk0yJwufX/P+fwqnIC9xsTLc9f8APSpUOXC++a1SNWzQaYiLb6n/AD+n86uWNg946Rxg4PpWZu3Pjr2r3T4WeB1ubZLy4XAbkAiscRVVKF2b4ai6s7IveAvBvlRxyyJgcdRXtGllbUKgAAHHAqvbacIEVYo8ACr0FrIDyuK8GrVdR3Z79OkoRsjqbKRJEUFsH0B5rtdGuwkZU9hxnvXm1mGiIrq9MuuFBPsBUU5NMVSCasdDrOmW+qW5SWMZIr5x+LPw7S5sZgI+MEo2Ohr6FW8K9TWB4rto9R0+RGjAyK39rZ8yMlT05XsfnFqMTWiNFIG8y1kZGHbafb6j9a2NKuEaPdM7CBhy68+W3QE+x5/P2rofiv4cbS9cnkjUCO5Q5GOM/wCcGvPtIumiBjzg8j/636V71OaqU1JHhVIezqOLPrr9lbxu0Oo3nh6eQCOYedChPGQcNj07V9ewsWX5vwNfl14U8TXPhbX9O1OzkZZ7OQOuDjcv8S/QqSPpX6SeDPEVt4n0Kw1W0k3xXSBseh7j680l2IqR6nSFaaVqZcGkK0zAhYfKTXJQIZdYkfPAduPXiuxfhSfSuQ0xllv2ZeQ0j4/DI/pWct0Pofk+g8tVB7dKsQj581Tlcs65yF9elSRS7lYg8YroNLm34dsDqes20P8ACz5P0r7E8PQw6TpEO5cKqjgDJr5Z+F9r9p8QRnH3RX1raTpBbIrdhXi5jO81E97LKaVJy7lKW91q9YyWirawD7vmjLt747VW/tfxJZyfPBFcR47DB/Srt7rkCfKzBQPTk1UXW7SQfMzqPUjP8q5FF9jslbuaemeMZjL5d3YPEfqK7TTNchuU3wg4U45GCDXBB43VZVKTRnow5rb0i4jxiJdq5yR71M7LZCSudqdUB5LdOxqK61e1Fu3nSqgx3NYksoVMmuU1plvnKeYwxx8pqYq7sKWiPK/jgdK1Czke3uo/tELZVcEE+oH+e1fO0i/Z5RIPuydfrX1F4k8OWJ0+48yIu209XJNfPGuaZHHd3FvETtH7yMf0r3MFJKPIeNjoNvnKdtdY2Zx8p6+1fWP7MvxHn0+GbRZyr2isHjBbBDdCOfYdOOn5/HcTFcjv6V6J4F8UXPh27W+sptkhj8uRSAcjI5wfoK6pqzuccHzKx+ndhqNvfruibLgYYHgrV0ivnH4Y/GeLW2t7W+Edtfx/6tlPyzDPb+RHv619F20y3FtFMnKyKGH0IpXujKcbMSUZRh68Vx+gLtvFXr80p/8AHj/jXX3DbY2PpzXKaB814/sHP/j9Zy3RHQ/IWS5aUqg+7mrkBwij+8azYly4NakK4IPoMV1MtHrHwZhD6w7N1AH86+mmgDwjPpXzL8IJwmqtjqwGa+pLRPOt1PtXz2PdqrPpsB/BVjx7xHp91NrlxBeatJZWckRMBRMhnHRSc4HPesHwNoh1jXEt7rWmsrRFdp5pJBGY8A4PIxgttGM5PbjmvdNQ8PWupLtuI9wHQ9xWRH4A01JQwWSTB+6xyK1pYyKhZmFfBzlPmTMXTvtWmzPGt7HqFm+dlzChAbHr26dwTXfaGjGNNw+Zu1LZ+Ho4kVdgVF+6oHArp9H02GKRWYgtXDWqqTujso03GNmUtV0+4hshMUIjbjNfP3jjxFqsclzFay/ZooGw244aT5gDt7nrn6CvuSHR7TVdFaJkDbl5yOhrw3xv8LLa5kd4mQvzwQD+FdNK1GSlLVM45yddOEdGj5kaHVb3RtUvf7TtY47GJXO9gDKWJwq4z82B04PIrzy6nZ9SiaYtkqpOeuMV9CX/AMM4UZlmt1YgEdTj8q8f+IXh1tK1G1n27QQYn9M9VP5Z/KvSo16c5WicFahUjC8ji7y38i8+XlZDkfWnQyyWd2yHIIOCOx5qSf8AeSKeDjrS/unkJkUjbkhjz+ddjehxRVmeqeGk8iAXCOUuUtft1rMBwChG4cdwc/hX3z8OdTk1HwnpzzcymCOTI6YdQ4/IMBX59qt43hrSbW1jkMjRXN3iM8JB5aocdyDhifoK+7/hGP8AiltPVWLLHawxg4xlVUAH8v5VmkOex3dwf3Mn+6a5jw7g3Mh9Vb/0Kumu+LeY/wCyT+lc54bGWZsfwA/rUS+JGHQ/H6BeSB161oQ52Lup8UPlS56D6VLf3EflKFTkfxdK6b3NVod38MLjyNZTnqQK+stCuPMhUcYIr41+H1z/AMTDjqDX1B4b1UrFDluB1rwcxh79z6PLXelY9KVFPXFWraKINlsfjWJbagkuPmzV7z1EZ5rzkd0l0Gahqvmarb2FuB82Sx9q6AW/2WDzlYMAcEA8iuBvLe4h1KO7hUuNu088is26l8WpctLb6pG1uTn7O1uBx6bs5pqHM9WJ6JWPefDfiPyYmjaQKD2Pel8TaZDqemTS2cwGoJl4h2OO349K8j0bW9SMGya1eGXHJbGPwpI5dTN4ZptQmKjoo+VfyrRN25WYSpLn546GvE8Gq2kczKAWXn6184/HILHqVvaJjkeZ/Mf1r3CG7+wRTQtwo5Br5++IMh1vxWFDb22EAZ54OQPx5rrwMf3qObHO1FnmllC105VRkjI/Gr17pptotzI2XwM4+7xzVjwzJHaas9tcLnDbGB6kccj1PHSvT/smmXtm1teqDFIMJOpyCPr/APqr2pux4cVcf8H7CPWNe06OfcLT7ELZySDlCWZk59Sdv4V9afC55tCuLvw9KMLpwWOA/wB+BsmM/UfMn/AR61816DNF4d8QaZNbwEWM2wXSKRtzypIyfQ/ga+j/AIemTWtWvvEUyOLedVtbbbE53RRMxL9P4nb8lB70lJMmastT1K8b/RJz/wBM2/lWD4eGIyR/cT+VaOoahFDp0zuJVAQ5JjI7e9c74P8AEem6oJobS4EskcaMQg3cY4PGeKzbXMjG2h+UbHc1Urr5jtGTzVx2VUzWa9yWnDbeF7V1ouTOj8ET/ZtT2scEkV9NeHGWW3jPqK+U7af7HfwTqflOOfUetfRXgbWVmt4xuryswpv4j2srqq3KenWaspyrVrw3Kw4M8mB71hWN4GfFWdX0qPV7RoJMmM4PBxXkWV7M9mTfQ6uKeOZNwwV9TUDX1oJNpniz6bga84XwzDa/I15dpFj5d0hdM+nPSt3SdHuonxGwuOMqirhv65rWNGPcGm1c7+AW0qbjdQrGByeSfyxWH4j8TaLpkTQK0omX5gWXhuPao9P06+vpBCbGWOUnBke5CxqPU/Jnp7isHVvA66XrqzT3i3bSKSxXJXA44zzitHRilds5rspeLtZW10tLj7nmR7jnsMV8s23iFrvVbi6mZm86RmU9wOw/LivTfjp4tW2hXSrd/wB5Kuwgfwr3/wAPxNeEW0jK64PSvUwFC1PmfU8bMK96iguh3uvwJdj+0Lf5LgfO+wkFjn7w9+5/PrSad401S2jEXmK8ZGGUqMN/vcc1jabdsiYJYrzkZqMQ77gKuArH8q62ujOK/U6mPxRPcP8ALIYwT8yAnbn1xXt/gLWdX8R6RGlrqF1E0OI/LjuGRRjgAAH0r5tVfJunXncDt/8Ar17R8G9QS31WaFmzDIoJU9+3Hv0pU7KaFWTlSZ6lNo3iMzQiS+vnOeAbpyAfcZqxa+GvEluWaLUrqFmJyVuZAT+Rru7Bh5a45U5xmrjDP4168aMGtjwJ1pp2ufmdIzSxE9B6VB5ZfLHqSBzV9YjISikc8Z/rUktt5UR6cAH9a8257lipb/NE0MgO3O5T/dNeh+B9bewnjikYjpXBx4IC917966TSrSVwkiqdo71z10pKzOrDOUJXR9E2GqA+XKrfKetdzY3KzopBHIrwPQdYe2RYpmO3GOa9E0LXTA6qzZjPQ14deg1sfRUaymj0KTTzcKdvf16VHb2l9pj7ocbR0Gen0q9pmpQyIpDA5rft3jb5sKfrXPGUkbyk0YkeoarIflIQ9yxJJrnfF+qjQNJu9Svp/wDVplnbjA9AK9An8l1y5C4r5b/ad8XRtHp/h+3mzI7m5uFU9FHCA/U5P/ARXTh4yrVFBnHiq3sqTkeEeI9dm8SazdahPkea3yqTnavYVBbriVT71QXpWlAOVP0r6SySsj5a7k7s14W2suOeeatmX7PMjADcPm5rOjmEKlsU1blpmLE8/wAqixpfoaActMZG5JOTXoHw2kkGvW7R/dXlh2IrzhX2n36CvSfhmQuoSA5+aMqMcckf41C+JGj+Bn1xoLm406KQ53D5Rnrx/wDrx+FajtgVS0uDyfP42rv4HYcDI/PNWp/u17lPY+YqfEz839NXbG0jE7n7Z6VPcncyxr97PPtj/wCvWXBd+XEoHXtSm4ZyX6MRz9a8ex9G30NOC2UqXHrg/nXdeGSssSpgDbwc1wen3KqkaN3611GiTGyvEVsiN/8AVs3AYe/vXNiFodeFaUjvG0uOX7nBqxZre2DfdLJ6UWjs43Aj/GuosYTNEpIwCK8yVTuexGGt0O0rxC9sR8zJjqrA4rqo/HIihO1XZgOStYYs4k681ka/ex2dlLtGMA1koxkzWU5RRieNvj7caZ51pYWW+5Ax5kr/ACqfoOv5ivnPVdVvdd1Ke/vp2nup23O7dT/gPatfxLunu5ZW+87ZrCEeK9zDUYU4+6j5zFVp1ZWk9BvQVoxHCLVMIKsxnIxW7OZF/IZDnlTVeNvLb6nFTwddrD5T0PvTbqAoQy81JS1NK1TzOSegzXX/AA+8TadpXiPT/wC0GP2XzCC4HAyCP5muW0tGZkG084HArutJ/Z48S63LDd2t7YQ6fcfOxkkLFFI7KBgn8RUU4ylLQ2npTcnsfZenTKbGKRuGkHmH6tyf5026uNqfjWVpNi2j6RZaeJXlFrEkW9jy20AZP5VYgezupniv7i5gjXo0CBzn3BIr2HNQjeR82oOpO0T817aVVbLGryvE38QB9hxVWSFVmYqpEZ5XI5xRFG7Ejy+O5FeYfQSjyuxoQNgjkDnrXXaRrGneWtvfnap4ElchHZzQvueNlToc9M+lMaGSRgg3HHPTvWc4KasXCbg7o950MlrdWt5PtVr1Dxncyj6fxD9fY12mjsskO6ORZY8/eU8fT618yaXcar4fuY7yzklicHnGQDz0Ir6P0Yx63Y22pW8htruaNSzx8huOjDo348j1FeJi6Dp630PbweI9rpY3ZTsU1xPiktNC0Y7100189v8AJfIsfYTrzE31P8J9jx7msfXUVLaSQ44GBz3rmpNqSOurZxZ4T4jhRT6ODyv+fauVY10mpX7PeSzhUYZIAcf09eawbu3MSxSdFlzgZ57f419JSTUdT5yvG/vIhB7VdtV3fWqaLkVbt22staM5kjTVcKOOlPjCSFVfpnGaWMq0Y/Som+8QMhu4NQy0jUiC2ys67938O1wAa+mP2edUvtT8O6kl00jQ20qLAzkk4x8yg+g+X86+YbJTMFjdcktgBs4P1r6r+DtwtnoSosflqkxXy8Y42qT/AOhVrhY3qI9TA4FY5yoN7xf39D05zXzn8V/E2raT4jufsN9NbYK4MTFeMV9FXHybh1Hr6ivmH40rjWTJ/fAr0KvwnyNOEqdVxlujx3xloR0TWb21iDNbQtmMseUjb5lXnnPOKh0uOOIDAG8nrx1zXU+NJIfECvf28b5WJN7YxlwOf8+1cDYXjQAHjnqK8uT7H0uMjCNaXs9ru3pfQ7IXkKhjLbq4DblB9cUW09unmP5KrJJjLe3t6VhvNJLIIznyl+YkDqB3qhLqM7SHHHYegqUjlPQrSa0u4Gt5oMRqvUDpXU6H480aO3ht4/NsZrcBQJATHJgDkkdOnU4ry/QRJcB28wpMDgH+HH0704xNbpMu1kLAqdpznt19P6VjVowqq0jvw9WNNK2/X9D6EsPENhrMSpDcwtK3ymPeDuPcD1/+vXHeLbpbOyuoLVw0ewokO4ZDlT8qj6Z47HpXjll551C3jWR1bfgc9M9T+VdlFpOreJtHu7a1kkvZ7W5WS3JJaaQbD8mfUKM/hx1rl+pRpNSvodcq86tB1EvI4NJYp2LurtnqoYDnHX/IqzqEkdzZrEu4mNU8st1BwAw/z6U++tDFIHZGSaRiJEKbSsn8QIPQ9DjHf2qIofK3bOAcZx1PQ/zFemmrHnOcleL67mSwe3leN1w6EhgfWkEmDXRao63VtDdJGEeYlXO3kEZ7+nP+cVzs6FSwwM55xTIxFBUpWi7r/M0oJ5Gx5YDD0rUsi08ir9nkOSBjAxWBZMFBBr0PwtdoojjCoPfPJ47ms5Mzgrs39I0ZmtkknVY3TIyyKw9uc46A/lXrXgyQ6dZQpu5YmQAY5z/9YCvMr67EDfZrYs6zpjJXBB9/XBJFd5pFyiRRoG4UAflXRgoc02+x91wzgo1K8qqXwq3zf/DHsyXAutPEgPzRjB+n+f5182/GwYuInxwWxXuPhzVVz5Uh3RsNrfQ15B8e9Naxlt+S0UjB43x95T/XtXfWVos+c4qyeWFxn1mC92W/r/wTx7TZ5JrGTzJVUMwUoB94Adf0H51yesWp0vUHhMgdfvKwAwQen+faup0mNrsrDkBmydxHt/8AWrJ8VBpoI5GI3IQn4V5ETz62upHpV0v2S+YO4JjVGOeduckD/vkfnTbEWbbnnhkMefXk1k2UrRgoCSHGK6CC0jlsnm5XYueOppMxR0lnD4YuIx9nlvorjGTH2z9c81T1KRIE8oYfech+CSOnWuXkuI7SWI/vWyMj5gD1x17Vo3M4JtS25pmXIyeAOo+vT/8AX2VtRpjEnls1adIQ2GCgsD8vPT8Rxj3r274ceHLzVfD0M1nO0K3m5if3jKzcKoIjBPynHJ4Azx6eKNBLJZuocBYwdw6bhleD68kHn3r0HwA9tqfhG/s7hrgz2LSCAfKYwpjeXGCDjmOTP1XggEHHFJuCVzrjWlGKp393cseKvD+nQ6bc3Wo64h1JpAq27W0iluhViX2sCAxyNp9DivNdkm+W1YBTliIx/ex6/UCptY1+bX9WF028xRALDHK5baoOcH6kk/jVq6dbtY9SWMLNAFlbn74D4x+Bxj2+nOtKEoRtJ3M5tTi5p7GBFLGsgLR748HKEkDpj/69TNbWbxfL5okznBwR26Y/P9PerMWiyS3t5FE6BbaRlO7POCf8K6+Tw5BcaFFdoE324/fNjaXJz0x6FeP5CtdzfD0J1aU5JLRX1OPi0JzGk8MiPC5Yc8FCCPvDtnI9ua3dLsonhQNJJjgkIwBP6VqaCq2Mtv5rM0LncyLz1GM/WoNLXbqcMaEiAN5gU8naDnH1wKlkypU3CE6e7dmvu19DbaxOkTJGsryMjEOWIO0g9sfQV1GlX+FUGsd7Pfp6AMFkBLZxkHnJ/wA+9Q2M7Ltrrwk+W6Pt+EcRH2M4pfa/C2h6hpOpbJFbkgVpePfCk3xD8MQQWMif2laSCSJZGCq6nAYE9ux/D3rh7C6b5QP4uK9B8OX7oNuT8vH6V6Lipxsz6TNMBTxuHdOfU//Z</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAC+AOcDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDz+iiivTPCHU7FNXpT6AG4p1FFABRRRQAUjUtI1ACUUUUAFFNZ1jUvIwVV5JJwBWFeeOvCdixjm1iJmHaJWk/VQRUynGHxOxcKcp/Crm/SVzdv8RvBtzIIxrCxMf8AntE6D8yMD866KGaG4jWa3lSWNxlXRgQw9QR1ojOM/hdxzpyh8SsOakWlakWqMx1JS0lAA1JStQBigApaKKAClakp1ADaKU0lABRRRQA1hSU+mkUAKOlPFMHFOWgBaKKKACiiigAooooATisvW9dt9HjAx5tw4zHEDjj1J7CrOr6lHpOnzX0q7hGvyr3Zuy/ia88ilutQmkvr19005y3oPQD2FedmGN+qRtH4merlWXfXql5fCg1Oa+1x92pXLSJn5YlO2NfoO/481mvo8AxtUgjvXU2Gi3N38yRkitKXwrcJFloj+XWvmZ1atV80mfa0sLRox5Yo8yvtHR1Pc1Q03WvEHhG587SrphEWzJA/zRSfVex9xg13+oaR9nJ3LwD3rlNasF2HA7VrQrzpSumc+KwlOrFpo9K8I+MtN8XWhkt/3N1EB59szZZPcf3l9D/KuhHFfNNrqd94a1aHVtPfZNbtnHZx3U+xHFfQ+g61Z+INJttXsWJiuE3YPVT0Kn3BBH4V9RhcR7ePmfFY3CPDT02NCiiiuo4gooooAKKKKAFpabk06gApCKWkJoASiiigBxptOpDQAlKtJRQA6iiigAooooAKKKKAOH8eXhudQtNIX7kX7+T3Y5C/kM/nSaHY/a7hIwvtiqGqSfbPEN9KxDYm8sewX5f6V2Xg23jbVIoVUOB/PrXxuMq+3xMm9k7H6FldBYfCRXVq/wB56b4L8H2rW6NNGMEFun9fXpV/xLoFtY25dEVivPHfpXS6TptxZWMeEYhV649OaxvEiyTWzLyvzHd36f8A1jWjcVE2ipOZ4/4jsI41LYAODkeleZ67Ht3HGAK9r8TaDcAfdwNu7/6/pXlviTRLiNW/d5FcjdpG8o3ieTaxDlmNdv8AAvXXjudQ8MzN8hH2uAHseFcfj8p/A1yWtL5cjwkciofAV82k+PNKn3bVkm8hvo428/mPyr18DUcZo+czOjz05H0pRSBs0tfRHyYUUUUAFFFFABS0maKAHfWm0E0UAFFFFAh1BoooGNooNFACrS00U6gBaSiigAqrqGoQ6bbi4mBIZ1jUdMsxwOe1WqXdtjkkEfmeWhkKE43BfmI/IHjv0rnxdSVKhOpDdJ2OrAUoV8VTpVPhbSf3nj26+stauZLob4ZbxvkVvnjjMnXpydv6+tO0vx039tTaXJu06IXDwxtHl5HAYqNozkk+pPGeK0fEVi2n+KZ7dk2x7gyr3UcfLz6dPwqKPwubXxHb6wYbeOJHMsM1wPkJ4PBH8Wc18vhMRGpFzktXqfbYnCyozULuy012E1zxze2OqCz0fxFr8GFBy5ZCc99uenHWtjSvihrljpM2o6lrs13bw8M7qXZie2AM5zjp+VWLzw5pepXU95ca9pWnJdL/AKWsDCNp+c/MWfHXnJB55qpH4JvtYuhdWluY9Lsm/wBHj2bfPfPMhAA44GMjnr3rSvUp25pbdiKFKpOShRfvd10/rzMzxD8avEev3UGj6TJ9nzCrCVhyQf8Ae6Yxzn+lZGvX3iDT7RJtU8Qo7TLuUNGMsPUAgEj3AxWdqehyaf4xt7e6lEXmsyr5hKq/OQpYY28k4Oe9df4p0VtYWzSPwnZ20lomI5o7neZOcl2Z87iTzk81UalFU04rcxnGtzShUd2n1PL4b6PWJZba8dVKQvKt1HgDCjPzL0x+VYGl3qtq2nzQsVAuIt0kmFVDuAySTwAepPA5ro9X8K2XhmO42yxme8XyzDG5ZY0yGJPucAf99VxbSr53lh/LEsm1SB0HJz+ldMJQXvLocU4Tbcb7n19Y3dpfWqXNjdRXEL/dkjYMpxx1FWRXnvwNhMXgOJmYsZbuZjkk85C9/pXode7Sn7SCl3Pmq9P2VSUOzCiiitDIKKKKACiiigAooooEFFFFACr0paYpp9AxGpKdTaACnDpTaVaAFooooARutKjsjBlJBFNPWkpNcysxxk4yUlujzz4hanNdeKUvJZBLLJGvmMO7DIJ6nGSM47Zru/AvxItNB0p4JbeK4cptRXXd8x6YA6n6+1cP440uGHU7WSMt/pG8kE8DkHj25J/E1QtLW4h8yS1IFwgOzPTdXxNXDOjV9l2P0jDYv6xR9v8AzHqml+F7PWFvfFnimG3OozDfb7ow32UKdyqMdCcDJH0qhJ8WPE+i29xM2g6ZDYQobcS2UhmaTIPLIyggn2yfyrE8Cz/EjxpqknhfSvC+ratLbgSNDbrGimMsFD5zkjOPpnnFe43/AOzn4w1/wu1qvwPuLUWDCRnfWo/PkkJZOPmx1U8E9KrkjK8Zbo0WIcLOL9T4x8YeONavdauLNvDN0pkG0tcR+URnn7rDNbHw4ttNstNNlrmk20yykndJGGKHPYntXpHjb9nH4vaVqEh1n4XytNa5iRlvlfbshMpG4P2jUk89sdTXgun+Idck8SR+G7GwnQmQK8cqN+7B5+9jA/Gmoc0eSlpbfUwlV5Z+0q+9fY2/iQNPsN1vZWsUKfwhFx/KvNV+by5l/wCWcm445OCCK7j4jI02tQ6ep3MiEn6DJGfwxVb4V+F5fEXieIBofs9i0dzcLKCRIivjYB6nPf0NdmDpNw5OrPOzCso1PadEe8fD3SG0PwbpenypslEAllXuHclyD9N2Pwro6YtOr6WC5YqK6HxtSTnJyfUXrTqatLVkBzRzRRuoAM0tNpaAFooooAKKKKAGipBUVSLQAtI1LSNQAlFFFADhRTRTqAEakpxptJgcr8QLOWTTYdShUsbKTc+P7hxk/mBWDpt5HLNDcKwKtgNmvRZI45o2hlUOjgqysMgg9Qa831jwzqHhlri+soXn0hJY0eRefszSbzGj+m7y5Np77D3FeBmeElz/AFin8z6rJMfFU/qtT5f5HpNvdanoslt4i8M3dxaXVuBlraRkfb3AZSDXr+i/Gy4j8KPcXXjO+u53uPOls21K7gnR/mb78Trhck/Lkcn0xXhnw98TWdwyWd9Iu1htO412nizwT4Y1bTTK7wuwB2hkViPTB7V5N1zOTPp4X5VGyZd+L37QdreafcX63t1bTzQNHn+17yYLujZGwrSbMsr4JIJ+UHNfKfhzxJJqXiU3kcAht037B3kduNzE8k+5/oK3PFfhHRdPZw0iFlY4GM/lXnerazb6Wj2ensPNk+VmX+Ed/wAa3w8YN3jqzhxcpQ0soryNLWr63mvtV16Rgwcm2tz/AHgOGYfU/wAq7P8AZ+05lsNT1mRflnkS3jP+7lm/9CX8q8q0nR9d8bata+H9Ftmklk+VV/hiQdXc9gOpP9av+GfiPrXwz8S6joTSm/0q1vpbeSA/LwjlN8f91jtzjoe/qPYwNG0+Y+fzGp7SnyR3PqNTThXL6D8QPCPiCGKbTdetGaVc+TJKqSqfQoTnNdGJM9DnNeofPtW3J6KjVqduqkyWh1FN3UbqYh1KtJSrQA6iikzQAUU2igBactJRQA+g0CigBtJS01qAFp9RU8NigB1QXV1bWUL3V5cRwQxjLSSMFVR7k1wXjL4x6LoLPp+iqup3w+UlW/cxn3YfePsPzFeO654j8R+MLsPrGoSSruysK/LFGPZRx+PWuyhgalfV6ImU1E9i1z4xaHbpLDoEb6hOvyrIQVhDfU8t+H519BfsB+FtJ+L2h/Fnw34wc3L6zDpgeQqC0WDdeXIgPA2sAcdO3Q18NNEsSLDGu1VHpX2t/wAEy9cXTfilrujudv8AaGh+d14JhnjAH5TN+tdeKwVOlhJ8q/q5VCo1Vizj/it8Bdd+EPieTSddt59PDMzWd/EpNpdoOjI3Y9MqeR36ivPtb1jVrKEwzaoJUxjcH6/kSK/ZzxB4X8N+M9Fl0TxNo9rqVhcD5obiMOM9iM9COxHIr4H/AGjP2Jo9L1Sa6+GdlDrEEqtMdJWVWvoFzyUQndKgyORlh3z96vh62GUfe5br8T6/C42Uvd5uV/h/wD4c1y5g1MN9s1qG2x/tjJH86g8H/CS+8cXoh8NwyXEG7El9IpWBPX5j94+wr6w+Gv7Ifw38PvZ+Jv2h/ENl4Ztp5P8ARNIuNyNcEHA86TG1FyOVzu5GSvQ/UOl+A/hbeaLHcfDm+0LUdLhxEsmkzxTQx4HC5jJA47VrSoNRulZHNi8U1Lfmf4HyZ4N+Ffhv4W+GLqeFQ8whMl3eSL8z7QT+AHOBXwHqjTX2p3V/JnddTyTH/gTFv61+o37VGnjwz8FfEVxHEYSyJbxsOCWlcRjHrwxP4GvzbutBkljE1uuHQfd9a9vLsFKcJTPGniOWXvHOwWvAZgWA5x612vh7W/EWixxtpGuXkEZG5UWYlP8Avk5U/lXPYis4d91lDnbtxyT6Adz7CtfQ4LoWp+0wmJdxMSufnCnnkDpzn8693C0Ic3LJXOWvUbV0en6J8ZtWtdkevWMV3GOGkh+ST64+6T7DFd5pvxI8G6kitHrkEDH+C5/dEH0+bAP4E14IyjgbQTzUbIOdvGfatK2WUpu8dDljVktz6hguILqMTW0ySxt0ZGDA/iKlWvmHTtY1nQ5hcaXqE1s5PPltgN9R0P4132gfGy9t1EXiXTftCj/l4twFbHup4P4EV59XLalP4NTRVEz2NaWsbw74r0LxRbfatHvllxw0bfLIh91PP49K2a4GnF2ZYUUUUgCiiigB9FFFACrS00U6gBrUwkDLHgCnyMqgsxAAGST2r5r8dfEbXvE2rXmn29/JHpBJ8qBBtDKDgFiOTnrgnFbUKEq7shXsev8AiT4reE/D2+Bbv7fdL/yxtiGAP+033R+p9q8l8VfFPxL4q32cbiwsX4MMDcuP9pup+nA9q42OAnGea0Y4Fj7dK9nD4CENXqzOUyGG3EYDEZJFKz3SyA2b4fpgjIb61JLuALbRwOK0bGFVXdj5j3Nego9DJvqKvnNbiWZVWQjovQfSvpL9ga/e1/aC0C3EgSO5tL+OU5wNi20knJ+sYP4V89zW8cdnHM0waSRm/dhfuqMDcTnucjH+z9M9p8B76TS/il4Vut7qi6oiyBWK70YEFTg8qQcEdCCQayxa/wBnml2ZdJ/vI+p+k/j64+O3x01C90D4Z+IJ/CHgy0hkjj1ZS8MmrXG35WWVcSCANxmMjOMkuDtr4C1Hwf4u8G+PtX8HfELT2ttbsXVrhmIbzUaRCJA68OrDncVYcjjOAP2MRlmgeGEhD5YZMcYGO1fEn7fltoP/AAkXgW4t7VV8SRW93NNP5atutFKbI5MEP80m7YR0IYZG6vj8L/EUdz31OysfCGsSalrXie28K+H5JA4HlybWPUpGuMZ78glvfCqRX3/+yR+yX4V8IabbfEa6u9cGuXVvJsf7eUVYvugMqBd6nHCvuAFfIXwD0SG8+M17purYN7JeQyQFkKbU3Krjn+JQyA9/ev1hsbW18OeBd1uojis7JiMdOASKirKUqjTHUlZKKPiX9vzVrr/hWGiaf50BtL/xJciHYm15IrSNozv5wf3jk8ADheK+DI12rlRjmvr/APb41Vo7f4ZeE3bEtpoM+sSr/t3k3JP4wGvkNe2V46nB596+oyuHLho+d/zPExDvUZnSabb/AG7+0PJV5sbVL54Ht6H3qwk0TSCNsRuezd+Ox71auYY41E1vdK6nja3yuD/u9/wrNtI/terSSf8ALO0QJ/20bk/kuP8Avo13X5Ph6mXxFz7PuB59Ogpnl7eGT9KuLGPalaJifuj8B/hWy1MzMmj4HH0qu0YYlZPuKNzfStG6VU+8eo6YrKvJPLsGnbgzMdv+6OB+uTWM3YuKuYNx4ivtI1221bTp2intJhJGVOOn8Jx2I4I7ivsLS9Qh1TTrTU7fPlXkKTx/7rKGH6GviHUZN1x5cjDB9O1fXfwpvDffDvQZiwJSzWE4/wCmZKf+y18xXlz1Gz0KsFGETrqKTdS1ic4UUm6igCSmmnGmtQAq05aYKcKAM7xNcNZ+HdTukQs0VnM4Ud8ITXyw0ZFxH8vDxsPx4P8AjX0t8Rr7+z/BeqTBgGkh8lffeQp/Qmvne6jX7LHcHrFIvHrn5f617OWR/dyl5mU3qQW8Yz0B+laMMG7Gc4qCzWJuMYrVhjXjBFe1BaGD7GbdKoG0Ljt0qzYx7rdG5+7zUV5/rCueat6eubcANjaSKFuA9lbHB6Vt+Abo2PizRbgceVqlrn6GRQf0NZfk7VLbetTaXMtrew3XTyLiKUn02uDUVo81OS7plwdmj9yTqVvp3h9NeumK29rZmaZgMkIiliffgV+XHxW+ImqfFDxpqfjTXJPmvPMSGFgCtvb8iGNQ4IwVwuQeH3P3Br9AfivrDW/7MOvanCrObnw9FGNr7CRPHHGee33zX5snDbjDJuy87boxtyCvLgI3AYffXb8qD34+UwEFrN/1/X9X2Pbb0/r+v66bkXg9odJ+J2hauHEExuWto1TYeBHkR5ByQpAO/oxNfpsden1r4EWeoZ/f6nYwxjHd5ABj8zX5l6eG/wCFgeEoX84Zv0P8e1V+zswB3D7pxlB6Yr9KvBVg8/wx+HmisDm6mtZCP9mNfM/ktcuL/jfJFS2Pz3/bx1hdR/aF1XSYW3Q+HtP0/So8dAFt1lYD6PMw+oNfO22vRf2gteHib43eOtbDb47jxDfCFuuYlmZI/wDxxVrz912+/FfXYWHJSjHskeNUd5MpzBEUySYCoCzE9gKj0WFo9MS4kUrJdMbhweo3HIH4DA/CmauvnQxaevW+mWA/7nV//HQ1bNyirCNo+709q0Wsm+39f16kv4fUrwncdo6545qdo1Uc5P41n2M26fy85rVkCorNngLWkHdXIa1OY1y4ZG8mP77/ACr9cgD+dU/EjRwRR2qsMQoE+uBVe0vv7U8UKoIMVpumf/gPT9SKq6lcfbbt3bpuOK4KlXmjJrrodcadpK5ztxEslwJG6Yr6c+ACOvw7t2aYyCS6nZVP/LMbsbfzBP8AwKvmjUZFiQxoMu5x74r2z9m/xE6tqXg+4b/V4voPb7quP1Q/nXh1VZnVV1pnudL2pKUCsTkEopaKAJmprU5qaelADaVaSlFAHm/xuvvL0fT9NDY+03DSMPUIuP5uPyrypYmmspIF/jQr9D2ru/jZcmTXbCyz8sdr5n4s5H/stcTZn0znFfR5dC1FeZhUepX0tfNCv3dN2Kv2u1piORjP4VQsZBbas1n0WXMkeff7w/P+dXbXCXEuWxtBrui9LGbKlwfMuieTWjZqYwyDPzAN0qrp9u15I1w4wm7860WRY5Y+eD8v+fyFUu4Dsbhzjiotp8udV/uGrMfXtxTY42LN6FT/ACoY0fqb8R9UW+/YZTVJFSQXHh7RNwdiASZrZeSCD1PrXwpNGrSGSZpCPNkJaVSSPlG5zuQ/MOsgz8wIAr7C8Tait5/wTr8N3G9W+06dpFu5YZXMdzHnIAPAaPnjtXxyu6GYqnyOkrt820NujXPJ+XLpyf8AbLY7V8rhI25vJs9xfCvl/X9f8Ag00xx+P/CC7VBW6kfapTKfuGLY29Q2c9PlwFr9TtJ+z+GfDnh+/vFHleHPDs+oSA9jHCAf03V+YHhaza++KXgWCZ1MK3rR7SzEBXRs7PmIHOSw7MSK/Rj46asdF+A3jrWlbYYvB0tlGw/ha5DRgj3+Za5MSvaYrl72X9f19+437sE/6/r+tNj8hNSmkvLyW6upGeaZzJI5/iYnJP4k1XKY+UE1NMv7zrTWHcnAAyfb1r7NI8NmTbr9q8SnumnW4Ht5khz+ir/49WneTKq/N696zfDeH0+bVnzu1Cd5x/udE/8AHQKTVrhudpIxWMJWhzd9f8vwNJL3rdiDatreCT1YfStDxFefZdEurhWwfLOPesk3kbQgSc47VW8T6tHL4da2VvmKkHLDsP1qJVFCnJlKF5IwPB6tDol5qPPnXUnkq3fA5J/X9KteWsadASTVXQ7uK38M2aMwGCzfiTmmteTXh8m2iLemB1rgpOMaMV5fmdMryqSfmQ3EdutzHKyhsNz710Xwr1ltJ+KumyN8iXchtHX18xdq/wDj238qqQaH9ii/tDVmC7eVQnvWBp19cW/iG111kKCK8jmj5/uuCP5VzYqm4R16mlNqd0ux9tUoNMWnV55yimikooAnamtSmkPSgBtJupaZQB4b8VpvtnjSfawZLaGOE4PQ43H/ANCrnYWS3j3MePc1b8e718batcQ7nh+0bWHXBCgNj8c1VtsTQhWUYavq8IuWjFLsjlnqyhdNbyX1rNHIuY5Vxg+vB/nWrNC22RY/+W3GfQd6w9U0fawuLefYVYNg98VpXc05h8uNvlb73vWyerF0RatJY2cQW/8AqYgPm9TVtuY2fPCkMR9Of8/WqumxeTanuTxV5V3RnPBIqkwFLHccd6dBnzO3cfWo15WNuvHNSp975alsEj7ktvES3X/BOPw2PMUG01Q2zscHZ5epOAcHrwV49xXz1bzLIojhDhRKEAiYnjBwoKscsD/qzjk7ieldl8O/FK3/AOxb4h8MtKTNpfipDCFPzDzJoHG3kc5DkVwduwa3+fDLuPHOzlSBjepwGJwjZ+Xk181T0qVI+bPbp604yNTwiVj+JXhO6kCDybpTuZThmCchMoCpH8eTy2SM19yftpammkfsr6xbrIFfVzo9mPXAlSQj8RE1fDHh10j8WaLMFXK3QViu3krAflYK3AXoGx83Jr6y/wCCg2seR8B/CmmocNf6pYykeqR2lxn/AMeZKxUebHx+X9f1+GyKztSfz/r+vx3f50SDc5zn86yfFNw1pod00ZIlmUQR/wC852j+da8an2OT2Nc/4kkW41rSNKGCoka6lHsgwM/ia+mqtqm/PT7zyoK8kXo0W1s4bWMBUhjVFJ4HAGKyb66t1yrybiR0RavXgZge4HTmsWcRYJxux129B+PQVnUlZWLhHUy7q5mSM+Quwd2bk/rXPag0hjkkkZmYjGWOTW1qM8fTcpPovJ/Pp/Ouf1B3aMjbgdTnqa8rEy6HdSRp+DNJ/tmFVnkbyYf4F6n/AArvlTTdKhK2tugZeBs5Ofc1z/gG1jk0GJWZo0JJbbxuOe/rWz4ivrXSdPZIQpnYfKveu/CRVLDqb7bnHXk6lVx8zi/EGoajr2prpdrn3A6KKqa7p1to/kafDlpyPMlcnnNb3huOKzk2QqLvUrr55mB+WNfTNY/i6Py9YZpGy23pXDXp3pOtLWTf3I6KU7TVOOy/E+vfBuqSaz4V0fVpm3SXVlDLIf8AbKDd+ua2a4H4IaguofDXSecvbebbuPQrI2P/AB0rXfLXlmElaTQUUUUCJqKKKAGUwmnmoLiTyoXkxnYpb8hQB8z6hctZ65e2dxL5oF1Knnf3yHPNXI8bTwMYrHhh/tSaZZ2J3sXJPXJOastDe6fBuku0liXgbo8t/MV9fSfuI5JL3ijrXmMp8uQg+grQt/39rbvtLFkXP5VzOoeLpvtH2PT7ZPOPHmSrhR+Ayf1rpdCS4azhF9MJZgDvZRgE5NZwqxnUcYlypyjBSZsxqvyIq4AWrPT+dVuY1LZyenSqcd4/nbWzz/n+tbmbNHOVKqcbW/n/AJNSx8L6+4qFJNzAdN6n9Mf41MjfKPQmlrcpHc/CvWHXwP4i8LliY7/XoWaMHBYpCGABwQp5PJrfs7MwKY4ZEYMJmXbtGQwwWADLwRwV/hXJ71554AuDFa6pCzN+81pFCrnDf6MzEEgggfJ27gV6bNJcLcqHO/zJom3M+eZQcMQwIJPG8fxYA6V86tKk/wDEz2qSvCPoiS1eSHxFoy4m+a828F8KptmKht2cpx+75zjJ719Bf8FAtS874bfCiFm/4/ILi4x/uRQj/wBq183W80MniHw4fL+b7f8AKNqjbiJ1fkAFtx5APCjgV7P+3VfPN4T+EFqwO2HRLqQc/wB824/9kFTRh/woQ9P8yMTL902fJCfd3HHrXFW90b3xhqd2rfJaRLbJgficV2U8nk2ssmM7VJrzjwvcM1nd3zcvdztI3517WIkueEPV/wBfecFJe7KRsX9582Mbmxj5uf8A61Y9zJPcMTI5PbrU1xdYySCSaqXN0yw+YoxmuepLmNYxsV5oI1G52GKxNWmj8lljX8TWlKxbO7k1j6oSYz9K4MQ7R0OqkveR3/gbyV8O2szQgYGAeTk+tZmvWK3V9i4mbc3JFdB4WZbXwvaSKo+SBWA9zUMOn/vl1O8YSzTt+7H8K+ma9SNPnowh5I4HPlqSkT6Tplno9rshjCtt3ysev0Ned69d/wBoavK0YyqnA/rXoPiK5ksdOZVYs8q7nb1rzmOb5jiMbnJ5rlzFpKNGOiN8Im26kj6H/ZpujJ4R1GyY8wagWA9A0af1U16+K8O/Zldvs/iODsk1s35iT/CvcK8Viq/GxxopKKDM/9k=</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCAC+AL4DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD9RaKKK1ICiiigAooqK7vILC3e4uZo7eCMZaSRgqr9SaAJabJIkMZeR1RByWY4Arg9c+KcEcht9Lj89+R58gIT8B1P6Vw+sa3e6tJ5l3cvKByAxwq/QdBWUqijsXy6XPUtS+IWjaduCztduP4bcZH5nisu5+I8jLm3s1XjIMr5/QYrx/WNastA0+4v9SvYdPsYVLyXNw4RFA5JJPtXzH8Yv28IbWN9O+HNsty+3a2t38Z8se8URwT35fj2NZe1ZSg3sfcXiD4qDw3prX+sapp+i2SjJuLuRIox+Ln+VeQ6v+3p8MtHkkil8ew3UsZwRp9lNOG/3SseCPoa/LDxp4y134iat/afibV7rWr1jxJdSFlX2VfuqPYAVleSN64wBjtWUqrudUcOfrLo37efwy1q5W3h8dx2srHCnUbGW3T8WZMD8TXpz/GC7ksba/0y80/VrCblLiJlljfjs0ZxX4tWO1WGR3rvPh744134dap9t8O6hJpkj/66FcGCYc8PGflP5Z9CKzlUnb3XqaRw6vqfr9pvxl8zAvNNx6tBJ/Qj+tdXpfj7RdWIVLtYJD/yzuPkP59PyNfEXwY/aK0n4kLFpeoJHoviLHFsz/ubk92hY9/9g8+hNe0q204OQw7HisY4qpH4tSZ0I9ND6VBDAEHI9aK8F0XxVqegsPslyyx/88X+ZPyP9K9G8O/E6y1LbDfqLG4PG/OYz+Pb8fzrup4mE9HozklSlHzO0ooVgyhlOVPII6GiusxCiiigAooooAKKKKACiisnxB4gj0W3wPnuXHyJ6e59qBkuta9baLDulbdKR8kS9W/wHvXinxa8QXmteG70ySFUBjKQp91f3i/mfety+vJby4eady8j9WNcl4+J/wCEV1AgH5VVvycVjKVykiG1lDTKRxtJrj/jF8aNA+DXh46prUzPPICLTT4SDPct6KOy56seBV/xh4v0/wCH/hnUvEequV07T4mnlC/ebAGEHuSQPxFfmf42+IGq/F7xhe+J9ckLTTMVt7ZjlLWH+GNOwAGOncmudrU3hG5u/Ej4oeLvjdqn9o65N9m0qNt1ppcDbbeAeuP4m/2m5rh5rNDIwduOnXitW41Dy7MQg5PcVjSy7pAD3rKpL7KO+nBLUd9lgVcIv3TVm3s1dhgVBDGZGXGRg1u20IjVSTz6VnCEup0kSaSm7O1SfpWhbW/l8AVOh6e1W4ZFZucV1OCI52T2McashdOhyCCQQQeCCOh9xXu/w1/aL1nwhLBZeJZZNe8PZCLetlr2zHqx/wCWyD3wwHr0Ph8TBmGOa0VkcL36VzzpJkXufoZp+oQapZ295Z3EdzazoJIpoWDLIpGQQe4q2Gr5S/Zr+JUvh3W4vCV7Ju0nUGLWBfk29yeTGPRH5wOzAdNxr6sXg49q4nHldjO1mdN4Z8cXvhxhExNzZd4WPT/dPb+Vet6Nrdpr1mtxaS+YvRlPDKfQjtXgNaGi67c6BercWr7T0ZD91x6EV10sQ4aS2MKlNS1W577RWV4d8RW3iSxFxAdrrxJEx+ZG/wAPetWvWTUldHntWdmFFFFMQUUU2WVYY2kdgqKCzMTgACgDnfGHj7SfBs2m2l7dxpqeqPJFp9ox+ed0jaR8D0VVJJ6dB1Irirq6lvpDPK5kd+Sxr52+I1t4u8cftW+B/GdxompWnhjSorqxRpQhSESQyqrHax5dimfqB2FfQagmNQSeBWMpc1rGtrEE33hXMePlLeEdVwMsISfyINdPN1Fcv8QFP/CIavg4It2NSwPjv/goB40ls9D8OeFoZCiX0st5cKOrLGQEBGem4t+VfI2lSbbYKTnFe0/t06gLz44NbKzbLHTLeEqR/ExZyR+DCvC7GTCjac+uTXPU0R3U4qxs/exk9aVYBuqK3uFPBGM1dVQeh4rnUl1O6MdCW1UL0FaMeStQWtqcAgir8VuVUA9a6OZWNVEWNm9OKnTPUUqxdBmpoYxtYk4xUe0XcrkutSSGQq4wP1rWhm81QO/espbu0hb97Oin3YVfs9TsJpMQ3EbSdCFNaqomjCULGtHvjjSeB2huYXWaGVeqOpDKfwIBr7y8GeIl8WeFdH1kLs+32kdwV/usy/MP++g1fBCXSqMHgH3r7H/Z3u/tXwi0HDEiLzoeTk/LM/8ATFcda26MWj03d69aQ4prAjvS8euTXOQaWg69c+HdQS7gOccPGTw6+hr3LSdVt9a0+G7tm3RyDPup7g+4r57rrPh34oOiaoLedsWd0QGyeEboG/of/rV14eryS5Xsznq0+ZXR7JRRRXrnnhXGfEbXRa20enRuBJN80nzchOw/Ej9K7GSRIY2kkYIigszHoAOpr5R1zxBY+NPFeqX0XiG7tp7mZoIraHVJIlyoGFWPdtLbQCcD1JrnrVfZq5pGPMzrtWYNDDnp58R/KRTXSAlo1z1718meN/E3i7wb8bvhfoqeJL660HXLqaO7tLtYpQ3l7ioDFN684PBHavrKNt0aHOSeayptzXNYtrlIJjiua8dfP4S1of8ATnL/AOgmulmGa5zxoufCmtDPP2GfP/ftq1aJufm9+3FCYfjtqDDpNYWko9yU25/8drw3S/4l719M/wDBQTRhZ+PvDOqKTm+02SFuDjMMhxz9JRXzJop3XXlgdRnNc1Xsd1JppI1EwrLzVtrpU2rmoLk+Sh7Yrm9T1g2soAOD1yx4A9a4Xd6I9SNkrm9e6hqFqg+ys23+7mqEfjbULeQJOMH61hSeMYIG2H7RO/8AeXCr+pFM1WaS3YNPDcWzModVuV4YH0YcVryO25mqiud9pvi95ofnOD6VLqXiaRYDt+XjqK5DwrMs1wFl5GeK6jxRpsNvpRljHz4yK5eR3tc7lNcl0jj5r17y6LGVsdwTxXa+HdQttPVC/wAm0cvsOB+NeZWcd1K80iyQxGONnVrhiAzAZ2Djr9eK2/Bera3ql5P/AMTGCxhhjMhN1CAh9B1B5z2z+NdnJpucLnroj23Sb5bw7Nw2AZXDA5FfZP7Kd2bj4WCJuPs+o3UQ57blb/2avgzwJ9riuR9otWtBKS4iIJVc/wBwn+HvX3h+y3avZ/D+8ycxyalLKg9Mxx5/UVzybtZmVTY9o9qdz16VGG/M0/8AGoMEOPNJ91qM9OMUrZY0xns3w91861oaxytuurXEb56kfwt+X6g11FeLfD3WjpPiSBWbENz+5f6k/Kfzx+Zr2mvZw8+eGvQ82pHlkcn8UdUj03wfeRPI8b3oNohjdkf5lO7DKQVO0MQQRjFfIvxH15vh34H1jxCLwX9vpNlM62eroJ2eQrshZZid4YSMo5LbhkZHWvfv2htWW1ufD8LSMwQzTfZ4k3ySPtCrtXqeC4/Hmvjn4zWuoePpfCGhagbm0XxJ4oisDo4YBUsLQvJPK5ViJGc7COcAY75rlre9UsOne2hydv4kl8RfET9ny5uZJDcfbt09s9rJELeSSFmeNWkdmdQ3Qnpx6198Q/8AHutfI/xwWKP42fBS9WHy5JNfEch9Rtbbx0GOR+XtX1rC3+ip9MV1U7ckbBJDZD8tc/4yA/4RTXM/8+Fx/wCimrfl9awvFmT4X1pfWwuP/RTVdyLHyl+3R4NPiD4Qad4ihj3yaBdCWc9MW8wVGb6BxF+dfCXhtXbUmBG3ap/Cvr39sP49ahpOoWnw90qaSOK409H1NYY1Zp1lVSIiT0G0ZOOua+WLHbDcMcbWxgqe3tXDUkuax6VGlJR5mT39uWTg5Jrn7jw79okeR1Zj22tyK6uSRGK7ulWobdJFG0Zrkk7M9OMbxPMdY02a+uvPu45ZZcBRIwOSB0yam+y6jrEmHVsdAzdcV6Yuhx3Ry65571FqVxZaHH5UYUSNVqorE+xbdzlNO0ZtNkViOK7iG0m1TTDELfzMrjOa5PUPEWm2flyXl4kZJ4QHk10ml+NrM20Dw7WhPRlbjFZdeaR0x25TCvPhzJt8yNzEx4OGwaq6b4FvbOfe7MwzklhW3dfFDRtevLiy3SR3Manyp4+U3AdDWn4P8brIVtrzG7OM44ro5+rMvZqWx1Og24a3hRgN0YAXivpX9nH4jQafqyeDbsBX1Bpbiyk3dXRAXTH+6uc9iCO9eHWlvbzW4miIBxkYqLRtabRfip8OdRUn/R9ehRwvUpKpjP6NWcmpaIxnDSzP0FXaVHNSdPpUWGjyvTHGKlU/KMmsTh2FXrTifmpm70pGY9e9MY9WKuGViGU5GOxr6B0PUBquj2d2OssSsf8AexyPzzXz5u9a9g+Fl99q8NtCT/x7zMoHscN/Mmu7Cu0mu5y14+7c4D4xaQdQ8dWt7DPHFNb2ggKvEGJQsWIB6jkj8uc18nW9rc3X7Vr2Mpee08G6M9wkjyFwLjUpAd/JJAWORxtP9zjHGPofxJ8TbPxB8e/GfggDy9b0dbWSGJTk3Fu9tDIzgf3kaTBHoyn1x4P8D7W58Wan8RfijZ2E13LrniC4sYVjZiJdNtfLhUoPukqQzjuRGyg/PWVb3ZSmyKRU/aGvAPH3wWuVZc/8JVCnHv8A/WNfW1v/AMeqH2B/Svzn+IXjy/8AGnxm03UILiVvDOl+PdJ0rTGU7oS8ZZbh1I4JZic4/wBn0r9F7Pmzj/3QefpXdRTVOKZnK9xJO1Y3ib95oOrr62Vx/wCinrak6CsjXBnSNRHc2sw/8htWjJR+Zn7T2mzWfx81O6uEx5tjYz27EY3Rm1QZHrgqw+orx5bppLi7kbG/zMAD0xX6BfH74I/8La+G+janpcQfxVpVjGbULjN3CUUvAT65yy575Hevgi40VrL7QZWeNhIyyRSoVZGHBUg8gg8c9xXBOm1LmPcp1FOjbsC3Hyhgc4FadhfeWFzj6VzsMhjQjr6U6W+8leDz0rjqHRQlfRnWT68sMDFSBgVyNwsmtXRaRiY+gPpVY6gZsKWzk49Ko6h4gFrcraxEK3c+lRRi3LU2rSUUUtY8Nwtcb5WEoXorDP8AWqNvGNOlZIPkiY5Kj7ua2I9ZtFx57iU+rHIq5Hr9mi5Ux7fUgV6FujONytqiPRorOaQGS3WMqM8LjPvWjcILe4EsDjA5OKdD4ss15baxIxzhh+tYU3iK3m1JRAuIpiVeMfwnJ5HtUzipaIKdSUXqet+GfFMgjWNnJGOOa9s+BPg+Lx18TtGuLhA1po8n9qP3BdAVjH/fbKfwr5bsbh7SYDPU19kfsVyG41bxDId2Es41z2yX6f8Ajua4IxlFnRiJrl5l1PrEHn8KdmmKDxnrTsGtDy9x26ndajNLuOQKBjs4r0r4PXA/4mkOeP3bgf8AfQ/wrzTIrvvg++3Vr8djAP0Yf410UHaojKrrBnxL/wAFG/hCbf41eFvHHh2dLDWNa1K10S7Z5Csb3DRAQSsQflGxSjdiqr6NV3xL8GdD+A37Mtzcat4dsbzW9L0byWuVZzPNqEwVFwQ2CRNJjgcgZ5rsf+Cp2kSRfDu11myuY0lsb+xvJ7Yp874M8EcinPUNOoPHIK+1UfiJ4yt/jl8UPh74U8NXaXum2t2PGWoySI4QxQuFtUdSBnMsjDb/AHgM/dJrpqU3N8su5yxk4pM+f/E3wr/4VL4R+G2nSaXDFdQ+LdOS91CPO57mOdUkib1AYFwR/fNfovY5WxiB6hF/lXyF+07HFZ/Cn4ezoTOv/CV2d95zfefzrsSlmOOSRJye+a+vLPP2OPP3toz+VdFNe7f1J5r6jpOgrM1JPMsbpD0aF159wa0ZGyMVRvRut5gehQj9D/8AWrQRw3hlnPhHRGX5X+wW5z6Hylrxb9qz9mvTPG3h3V/GOlXq6Fq9laSXV7Etvviv9ihtxwRtkwpBbB3cZ55PtHhBi3gzQjnk6dbdP+uKVr+JNFHiPwjqukyMAL+xmtctxgvGVBP0Jz+Fc09y6cnF3R+QtxF5LMCOozWLeTsuQTkVva1FNYl4J12XUDNDKrdVdSVcfUMCPwrkrqYtIQ1cdReR69OXLsTW0p8zNY8+hSapeTSid4n9auxXCq3Xj3q3pcg848FiTShprY1qPmsS6Do9ppbJNJsmkHB89BIn/fJrs49S0uS2tYpVtv3AwGhtI4mPuSB8341zM+ntc5IyP901mt4dvJnAQydfWq5/IrlTO+/4p3Vo9lxCZmZsneQAe2cDHauT1jwPZ2N59o01PLhVt2C2R7AZq9onh2a0wZEZj15NbOqSi2th5qkAjpT57szlSsrtlCOE7YyeWAr7i/Yj0CSx8Ga9q0qbRfXUUMTH+JY0JOPxkH5Gvi7RdPudUvLO1s7d7i6uZFhghUfM7sQFH4kj8jX6efDfwfF4B8DaL4ejC7rC3CSOvR5SS0jfixb8MVg/MirL3Ujph79KcAT0pQoPWnBcVBzAuehoJxS0xhlhQGo/PFehfB+PdqWoydliVfzP/wBavPeteofB23K2epXH950jH4An+orooK9RGdVpQPmD/grD4S1PUPg1oev6esjW9jffZL9oyRshlKOrNgjKiWCJecjLg44yPLv2bdeOq6XrXxRuWmj8Sa8ItG0/SxIGikt7aALEjAgEM8kMjB9y9Ced2D+g/wAWfAenfEr4e6z4e1Sxh1G2uYty2867laRCHjyP95Vr4/0HwRoXhvEmmaemmt5SwMlq7xqyKTtVlBwwGTjcDjJr0asXLSJwKaSszhv2urwQfBTw1azWlzb3FhqmlyNNsEkEgSWNG2yrxnIztIU4PHFfX0X3SAc4JFfFv7YtxMvwRuXa5mkSK/spFiZsopWXOQPU5PNfaa/L5g9HI/U1VOLjTSY001oMkztzVOfMnyevH61bmbj1ql5m2Rf94fzqhHn/AIBYv4F8M5PP9m2uT/2yTNc1+0r8fdO/Z8+HZ1eVI7zW7wm30rTnbHny45kbHPlpwSfoOtZ+ufFXRPgz8CdJ8S69NmG10u3iitlIEl5P5YAiT1J7nsMmvyy+MHxk8Q/G3xxc+JfEc4N1IPKt7aIkQ2kIOVijHYAnk9Sck1mqblK7Li0lqe+fHr4f3tr4X8IfEE3B1C28XafFeXl0sQRI79kDyrhRhQ2cj/dcV863W5ZDk98V+mX7Idlonxq/Y90Lw/rsC39lGk+k3MO7DI0UzMjKw5VwrIwI/Wvk39on9kvxP8Gru41GOKTWPCZcmHVoV3NGpPCzqPuHtu+6cZyM4rWrR7HVQrJqz3Pn8Kz/AMPGKba3XlXS5bFWVcW5CSDg02606O4jDwEI/oelcfIlodcpu52Ol6pA0IUkbgOckVqrqECDeCM15PD9qsHG9m68sfSrkGtM2QZM47Vzypy6HRCvHqesW3iK2XarEA/pWX4k1OG6C7MADrxXmDa3LJOAisPbrXRaDp13qlwl1d/JDGQVjbOW59PSnGEl8RlOrze6j7m/Y2+DccOnRePtUCSXT74tMtyAfKAyrTH/AGidwHpye9fVynaDXl37MuqWOr/AnwxNYH5LXz7Cdev7+OQlvzDKfxr1Bfm4rGaaepzuXM7dh6kY5607OelMGF+lKG61kMk3Y6UbjnnimbvSl3fKDVEkgYV7f8NdPNj4TtmIw9wzTH8TgfoBXilhZyaheW9tCMyTOsa/UnFfR1nbJZ2sFvGMRwosa/QDArtwkfecjlrPSxLXwP8AtTfE2L4FfFWbTbvw3e3GmalGL+0vLaZAjKxO9cEDBVwRjPQqe9ffFeO/tPfBaz+MPgPBs47jWNKLXNkSuWII/eRj/eAHHqq121U3G8d0cseW/vbH5r/Hn46aJ8T/AIQ69p1lZ39lcwGC6IuVQLtEqr1DHnLjt61+jlvIJbYyDoxyCffn+tflt+0AnhXwn4L1XTbe+so9du1jiSziffKAJUdtwXO3ATuRXd+Pf+CoV+ukxWHgXwlFbXPlKsup6/J5pDYAOyGMgYzk/Mx+lRSVScLs1lypWifoFq2q2ui6bNqGpXVvp2nQDdLd3koihjA7s7EAfnXyt8TP+CjHw28E3Uln4ft73xxdxtgz2RW2s857TSAlhnHKpg561+dvxL+Nvjj4wah9r8YeJL3WdpJjtpH220XOcJCuEX8Bn3rgpLgc5PJrojT7md7Honxq+O2ufGbUNLbUdlnp2k232TT9PhYskCcZYkgbnbAy2B6V5h5hBGc012O7OOaRSD0rS3Ylu59/f8EufiILe48YeDbmbCSmHUrVD68xSAfh5dfohJD5kDqfmjcFXUgEMD1BHf6GvxL/AGYfiDJ8Ofjd4Y1ITeTbTT/Y7jnAKS/KM+wbafwFftP4d1RNW0+GZT95QfxrbdXI2Z8rftAfsGeH/HXn6v4GNv4T10gs1gQf7PuWPoBzCxPdRt9QOtfnn408Ha58P/EF1oev6fcaTqlo2JbW4GD1+8D0ZTjIYcGv3GuLbzV/xrzD4xfAvwt8atB/svxLYmVog32TUYCFu7NjzmN8HIJ6qflPpXNUhfY7aVbl0kfjmtyzY3c/XmgyKW5jUn6V678fP2a/FHwB1aOPU4xqOgXTlbLXLVf3MvcJIP8AlnJjHyng9QW615NtAP3c+lefKM4PU9KMYzV0T6cu+QfJzngiuws2W3haRjhVUsa5zSV3SgcL7muk0bQ73xx4l0fwnpSNLf6zdJaL5eSVVj878dlXLfhWUZOpNRRTiqacj6t+GNx4i+Df7CelfEHTohLqEXicavLaXBIiuLC4Zrdo39AS8ZDdjg9ufpT4X/EzRPi34Os/Enh6fzrSdB50DMDNZy/xQygfdYfkRgjrXT/EL4VWup/sw+J/BNlCkUP/AAjUtvbR7eEeKAvEAPZo0/IV+NvgL4h+IPAeqLqfh3WrzRNQZQTLZSmPeOu1wOHXnowIr0a+HUo6bnkQqWk7n7KrJxnPPelZvTmvh34X/wDBQq6tWisfiFogvowAv9r6GoSb6vA2EY+6Ff8Adr6z+HvxV8JfFSz+0+FNftNXwu6S1jfZdRf78LYdfyx71406Uobo7OeL0R2Ib3pu47R6VEsx/pU9nby3txFbwqZJZGCIg6kk4AqFqWd/8IdFa+1aXUZF/c2o2oexdv8AAZ/MV7BWT4V0FPDeiW9kuC6jdIw/ic9T/nsBWtXtUYezhY8ypLmlcKKKK2Mz8eP+Cmv7JL/CHx1L8SfDNkR4Q8R3Ba+jhT5bC+YktnHRJeWHYNuHHyivhfzOpr+lLxz4J0X4j+EdV8NeIrCPU9F1OBre6tZRw6H36gg4II5BAI5FfhL+2H+yX4h/ZY+ID2M6y6j4T1B2k0fWdvEqZz5UmOBKoxkdxhhweLTewzwKSTOcGqpbd+dPwNrHNV5FdW3KAfatHogY5s+tAO3NMjl3HBUg1NsHHFJLW4h8bMrBlYqy8qR1B9a/Zr9kv4pWPxS+GOlalb3CyXywpFfxfxRzgYfPsWViD0IPrkD8ZFPzDivs7/gn34r1K11DxFpmkzg6vYRrrFvZyEiO6twRHdRNj/tkwPVSpYdwdYdhH6miPevSmvahuwql4O8SWfi/Q4dRsSwRvlkhk+/C44KMOxBH49a2/KPpxVcpJzmueE9O8SaPd6Tq1jb6npd4hjuLO7QPFIp65B+ucjkHkYPNfnB+1b+xbcfB+SfxR4WSfUPA0jZlRiZJ9JYtjbISSWi5+WTt0bsx/UQRflT5LOK4hkilSOeGVDHLFMoaORWGCrA8EEZBB7E1nOmqisdFOtOk/d1PwbkWOxUESbz7Yr7u/wCCcfwIkjtZviVrEA+06irQaUsg5jtgcPIPQu2QP9lfeug1z9jv4CeLPFmt6xFPqmgaJblvMgi1GO203f8ANueNnUuEBwAqvjg44r6p+DHiHwP4l8LxReAdY03V9J0lEsPL019wgEY2KpHXGF4bGG5IJrloUI0m5bnbiqkrW5Wjv4o0jVQ6h06MpHDL3B/CvwZ+Pnw1vfgv8YvEnhi7jaOG1une0kYYEtuzExsPUYyPqDX71bQy/hXwH/wUv+Co8T+DG8b2Nuran4VmUXZVfmk0+4K4b6RzZPsJG9K71Zo8vY/Nw3HnJkHj0zVjT9WudNvIbq1nmtbuE7ormBzHJGf9lxyD9KzF+TgdaQtjPZu9c3Kuptdn094B/bq+JHheOK31W4s/F1qoCgapDsuABgYE0e1icd2DV+oH7IOqXPxS8A2Pj/VPDV14aa83Cys7qdZvMj6faEIVTtbkLuUHAJ6EGvzi/YE/Ynvv2hvEkXirxVayW/w402f94Gyh1WVTnyEPXywcb2H+6OSSv7PWdnBp9pDa20KW9tCixxQxqFVFAwFAHQAAACuR0KalzJajdSTViaiiitjIKKKKACuP+LHwn8M/GvwNqHhLxbpsep6PerhkY7XicfdkjbqjqeQw/UZFdhRQB+CP7Xn7FPi79lfxFJNMkmteB7qYrp+vRJwM8iKcD/Vy/o2MqeoHzf8AeIH41/Tb4i8N6V4u0O90bW9OttV0m9jMNzZXkQkilQ9mUjBr8sv2tv8AglBqegy3nij4MeZqumDMsvhWeTNzAvU/Z3Y/vR6Ix39gXJrTm0sB+cGOwHNKvzdas6ppN9oepXGn6nZ3Gn39tIY57W6iaOWJgcFWVgCCPQ1W21a2GSKmORXqn7NPxQb4PfGvwp4oZsWdvdiG8HTdbTDypgT6bHJ+qivKgx4FWYcFhu+70P0q1oxs/cqbR7zwRrkms6Cvn2svM9kD8txH6fUdm7cda9Q0PWrPxFpcd9ZsWifhlYYaNh1Vh2Irwn9j/wCIg+LX7PvhXUJ5fP1C3tv7Pu2Y/N58B8o592VUf/gdekmG48O30l/psYJcjz7XOFlxxn/e966Wr6nPG7djuxEGYL3bgD1r4v8A2vv2osT3fw68HXDDcDDrGrRZAbnDW0DY56Ydx7qO9fRXxF8Q3Wv6DNpmjTT2P2qMrPdL8kqIeqKexPQkdjx1r4Z+Ifw31j4SxzX+m20Gt+DpCBdabfxmZbNyQoKn7yo27gj7pJ7VxVr8rWx9TkEKaxkZ1YqVnomeS6HdSaXqdtd2kjWlzCQ0U8B2Mh47ivQtc8fato66f4+8HNH4c8fadceTeTWSLFbanC6M5kkjC7ScptYYwS4IwTWPp/hvSvG29vDbtp+squ5tFvJQyyAdTDJ39weeO1dV8DLWG8+JWnaLq9qdl0J7SSC4XDJJ5LNHkHkHeqD8a8mjGtTaV7xkfseZzwWPwlSXJy1aavZqz/ya7H3J+zn+0NZfHPwtA95ZjQvF0MKvfaOzAgjp5sR/iQ+nVehrpvHfhmy8SX1xpGpR+bpWuaXLpt5Gw+9GxYH8cSn8q8XsvgjPaw6P4n8Lz/Ydbto0mTyxgN8vI/HGCOhBHpXuGnaleeLrfSJ5LCS11KMuk9uASFb5eVPdTXvRjyvU/nms4t3gfhJ8RvAt/wDDLx5r/hXU1K32j30tjLkfe2NhX+jLhh7MK+pf2Kf+CfmtftAahZeLPGEM+ifDqNt65zHcarj+CLusfXMn4Lk5K/oN4i/YN+H/AMQvjoPif4ttm1W5NpBG+hSKPsktxFkCabvJ8gjXZwvyc7s4H0pb28VpbxwQRpDDGoRI41CqqgYAAHQAVzTlroUnoUvDfhvS/CGhWOi6LYQaZpNjCsFtZ2yBI4kUYCgCtGiisiQooooAKKKKACiiigAooooA8e+PX7Jfwy/aOsyPGPh6OXU1TZDrNkfIvoR2AkA+YDsrhl9q/OP43f8ABIfx/wCE55734cata+NdLyWWxu2W0v0Hp8x8qTA77lJ7LX6+0VSk0M/mu8dfDDxb8L9TOneLfDeqeHL3nbFqVo8O/HdSwww91JFc7CQrL/kV/TLrGg6b4i0+Wx1XT7XU7GUYktryFZY3+qsCDXgvjj/gnz8AvH8kkt38PLHTLp+k+iySWG0+oSJlQn6qarnHc+Ev+CWvxNFprHi3wXcT4E0cesWkJ/vqRFPj3KtCT/u+1fo5NbpKvnKMhuvHevHPhz/wTR+Hvwh+JWj+NPCfiTxNZ3enyOxsrueCeCWN0ZHjP7pW2lWI+8e1fStr4HS3j8sXbMmMfNH/APXrqjVjazMZQfNdHnF5oyTbgFGcelcjr3he2a3kguYUns7lTDcQyDKyIwwQfwJr3f8A4QeLdzct+Cf/AF6juPhzpl5HtuHmkHoGC/0qnVplxlUhJST1PyG+NHw1uPhD8QDp9jPL9mZRe6fNG5EsabiMZHOVYEA9x+NenfBe08XfGVVurLwldaj4g0F45rXXbApAGkVtyxybsLzt5BOOcjaev6N3XwO8BX+sQ6tf+FNM1LUYohDHcX8AuGRAzMAN+QOWY8DvXa21rDZwpDbxJBCgwscahVUegA6V5lOMqdRyT919D7zG8SxxWDhR9n+9ivjvb5edzz7wZ8ObvTrGyGoTLCI4I0a3j+ZtwUAgt0656ZrvrSxgsVxDGqep7n8anoraU5S3PhLK9woooqACiiigAooooA//2Q==</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEA8ADwAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMDAAAJKSAAIAAAADMDAAAAAAAAAyMDE2OjAzOjAxIDIyOjEwOjM4ADIwMTY6MDM6MDEgMjI6MTA6MzgAAAD/4QGcaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMTYtMDMtMDFUMjI6MTA6Mzg8L3htcDpDcmVhdGVEYXRlPjwvcmRmOkRlc2NyaXB0aW9uPjwvcmRmOlJERj48L3g6eG1wbWV0YT4NCjw/eHBhY2tldCBlbmQ9J3cnPz7/2wBDAAYEBAUEBAYFBQUGBgYHCQ4JCQgICRINDQoOFRIWFhUSFBQXGiEcFxgfGRQUHScdHyIjJSUlFhwpLCgkKyEkJST/2wBDAQYGBgkICREJCREkGBQYJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCQkJCT/wAARCAC+ANADASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD53KA1GR2NWNoqN1NAEJX0pNvOKk2n0o2nOKAEAxT1XuacFHpT1XFACKtSovehV7mpVX1oARV9akVc0lEjNGMnaoAzjqaTdhpXJFXsKd8qclgPrWaqy6i0myVo441LH3qWG0byf3gLccAmp5yuRl+OSOT7rq30NTKtcpMxjlJjyhB/hNXbTXpocLMvmr69DVktWOgCe1PCGorK/t75cxOMjqp4Iq2FFAiMRj0zTtntUoQ07YKAIdlLtqbaPSl2e1AEGyjaKsbKNlAEGwelGz2qxs96TZQBX2UbKs7KTZQBzCrjrTJk281YC4qOUbqAK9KFNOCgU8J60AMwPSnqvc04L6CnqtACqv5072Ayx6CnD5RzUa3i2ytOSSxOEHrSbsVFXLQhFrHumOWPYdhVWRLnUF8uKL92e7DGa2dE0C51JxcXe4bzlVrutK8KxRjJhBPuK4auJUdEehRwcp6s87s9KktLJoVtm8yTl5O2OwqMWc9uuSruR2Br1i68Poq52KBWHfaKoUkL0rnWKle52SwcbHnF1bWt2Dvj8uT1PBrFubJoCSp3oPzFd5qWmrgqVrkNRsZbNspkp6V20q6kedXw7jqZiFlYPExDDoQa6bQtcF2RbXBAl/hb+/8A/Xrmt67s4xnqKaxKvvQkEcgiuk42rHom2nbfaqGgaoNUtfmI86Phx6+9a3l+9MRCFNLtFShBS7B6UAQ7RTtntUgQelOC0AQ+WfSl2H0qbbRtFAEG0+lJt9qs7RSbKAOR2mmMtTUhUGgCvtGenNPVfWn7aULigBAuaeqegp6p608LQBWuUby9qnBY4z6UeGNOOs6wX2Zt7cgKOxPb/GnagfKtXkB+6pP49v1rsvh9oy2mmW7sMGQeY+fU/wD1sVy4mpyxZ24SlzzR2mhaSibdwGemcV1kGnIMYrO0e3abHlo2PU10KQGJR8wP9K8Zu57yVtCheacnlnC9q5rULZQp+X26V29wyy2rN6ZrnL9bfcQ7dsmmgued6najJxXMahZ7iQV4NdbrmraZFI6+fuPTC84rnmvbK5yqTY9NwxXRCMlrY5KkoN2TOJ1PTPIJeMfL6elZfbFdlqVt1B5B/WuVvIPImI6A9K9ChVurM8uvTtqiXRtQOm6hHL0jbhx7GvRoyHUMvIIyD615aw+XNd34PvzeacIWPzwnb9R2rd9zlZtbTRtNS7DS7BSuSRbKUR1MIx6U7ZRcCDy/ajZ7VPtNG33qkwINvtRt9qn2mjaaoDiyoo2j0qUr6ijAoAgKnPFKE9akK+lAX1oAFXvTwpNAXNPA9KAM7W2xZOg7kL+oNeoaUZ1t4LHTYFkuBGu6Rvux5H868tvP9JkSEfxXCp+or1i31S18Pwea7YCnLerGvOxOrSSuetglbmbdkaSXninw8250Dg9wFIP8q0NP8WzXrkXUDQSDnJGAa5u6+K1jcxMpukVVAyEg8zAJxydw/lUmn3dlrtvLNp06ySRDedg2EfVT2+lZVKcuXWJ0U6tPm0lc7RtVP2Vl9VJrz3xHqsl5I0KTspOBx3rt9ynw+J3jCvt5Fed6VcA660ki8JnZxkA+uP8ACuWjq7o6q7SjZlnS/BUbKLrUXSKIDKrKw3P+HpUOsabpr5RYoWUdDHgfyq1qOvTypc/2fDDarCMvd3cRe5uc/wDPMHAUD0yOlecvrGpvKGl/euTyoT5h68ivQVCb95s8x4mnH3VE0bmxe3JELl4s42Mc4+hrA1y32x7+6101nLPdN88e1cdWzk1R8Q2e2NlIPTOfWknaSCcVKDaOPHr6itzwZd/Z9V8lj8sw2/iOlYmP3an61Jbzta3cU6HlGDCu/oeaz1sLntSiP2os5VuraOZPuuoNT7aggh2Gl8v3qYJS+X7UAQeX6GlCc+tTbPalCUARbPajy/aptvpRtqrgcRsNNK+oqcLmkZcVYFYqaUL608jHFOVfWgBoGTTmwiE9MCnhSajvPltZCOwqZMa3MvRv9M1ywi/vXSt+oNep634Oj8QwxwiaVDg5KH+deQ6Ldi11exnPASdCT7Zwa+lfDcBYggde9eXjKjpyUke1gacakJRZxFv8LGnsYbWe+fyYUCBViCbgCSM4PJBJ5OTzW1p3ge20OMSIS0pAQMxJKj0Hp+FdxqRt9JtjcTuM44BrGTVNPvLdJ7nUYLdicpG7YLc1zTxVRxOunhKUZXKeqSPBpLRKmFA49q88swjXwbowbBI4716rreu6S2lLbBQZGTOcd68xXxHoeiR3EU6tNdSsSFRdxX6+lYUVLodFfl05tDuk0mK4sg0SK2Rz3zWVeeHYeRKjIO4i+UVheE/GEyag8aljaZGN38P0r0G/vIbizEgCgnkEd60nKcepnTjCeyPLtS06KzmJhBGPU5Nc7r0vmW7Z6gV2Wv7Dnnkda4XWH3QPXRQbla5x4lKN0jjoxmEj0Y00j5RUlvjyT9TTAOMehr2EeKei+Br77TphgY5aE4H0rqAuegrzfwPfG21ZYifllGw/XtXpqLxUMhjFj9acEFSBKULjoKBEfle1Ls9hUm00bTQBEY80ojxU23NG0DtQBwiLTpI8rTk60r/drUCninKvc04r6ilUZNJgKEzzVfUF/wBDkA9DV0LVa4XzI5U/2TUMqJxG/bg+hr6W8HeIFuNIs7ncP3kSsfY45/WvmmZTHM6HsTXp3wz1gzaPJZFv3lq5AGf4W5H65rz8wp80E+x6uWVeWo4vqd34o16TVtSh02Bt7ucsT0Re5NXb3w/p1/bwLPDG3kjCsRyPxrm7KyayvrrUp2yGKf8AfPPH5modN17V/GWtmx0WB3SL5yM7dyg4JLemfSuONKUrKLt5nqc8E3znTX/gW3urJHgkuIlRT8yngDvXDXfhPTdKlZY2DHOSWbJr1PVNF8Yx6Lcf8ScJbmMlwl0HIGOcDH6VxV98MvEtrHPc3lrawGNGclpN2cD8v1rs9jGK/iHPKSlrZGFBDDb8oRVxdUubOP5HLwnqufu/Ss7WfCsml+bv1aAumBtiXPJUn16ds1V8NwzyzM0sryIQQNw6Ad6iVFNXvchVXHZFrV55GGWJ5Gea5XUz/osjH+6TXYeKpURbeJQN3lrn8q4rxFKIbBlH3m+WroR2MMTLdnORjbbsfb+tM6SEVIpzasPYU0clW9cCvTR5LJ9PuDZ30E442OG/I17RasJYUcHIYZH0rxDHUGvVfAmqDUdGSNmzLbny3Ht2P5fyqZLqJnRAelLsOKkxRg1JJHsNOVPWpFX1FOVM9KAI9vtTtlP2GnLH+NAHna9KUjNHSlrUCMjFAX0qSgDNQ2AY4qArmd0PcVaxULrtmDfSpKjucfrtiYbp5AOCaseE/EJ0LUi0jH7NMwEoAHvg+vGa3NUs0lhctjnqa5GWxbc2OnPNNwU42ZrGbg1JHvlpJFfWixZBVxjjuKt3unvor293Y5YIBlVO1h64I/Ud68m8B+MW0uZNM1GTEWcQyt/B7H2/l/L3Cz2alarjDZHPvXlTjKg7PY9zD1o1ffW51mg+NbbUtNXz70NMCM2/l4PuSMisLx5410yxtgiyL5xwCiqvb6c1i6l4NjulMkZeFvVSR/KuWuPAn73JkkkI/vE1uq1F68ups5OLuoo5/VL1tan3gMsQ7Hv/AIVoWPl2tsVUYZ+CfQVdbQVs4zuAVRWJqF35ZKxnpT5+fY46sp35pso6pd/ar55CcgHArjfEFybi42A/LH+prfuLkfMEOT3Nc9cWsk021ELu5wqjqSa6KcVE8+tJyRRi5ib2pF+6U/Kuq1/wTc+HdLsriYEtKD5voCe1cvIu3DDqOtdNjk6XEk+8T+Na3hfXn0HU1n5ML/LKo7j1+orMb94gZeo61H0xQJnvdncxXtuk8EivG4yrKeDVjy/evG/DPi678Py7MmS1Y/NHnp7j3r1TR9fstYtxJbSq3qvdT7jtWbVgNFFxmpFWhcdqlVaQhgT2pQlSKuTzT9oHagDy+nKO9Jt5p4HYVowExTkXmnbSetOVewqLgJtHpW5pngTV9ctEu7eJVikcohfI3EDkj2rrfhf8Ox4gkGrajHmxjbEcZ/5bMPX2Fe3f2XDFaosUShYmBVQOBj/62a1p077kuVtjxrwz8Fo5WR9YX7Up/wCWZyFH+NRa78FtPv7y5t9NjW0igTaAgwA3Xp3r2CXUoNMRowPOuAxxGD0Hv6Vx0Hn6zrM81xcvFkkmNCVQHoP0rKvjKNC8d2dWHwdWt72yPENV+B9/BbfbI7nzdsgjVFXrzz9K9A8L+F7nwx4Quby4vmaa0IKQH5i6dwB1z0xXpd34b+y2b20d5LkMgXcx++wLFuueADgeoXtnOFL4fuIZNsTx7c8naMn8a4MZj6aXI4b/AIHbgsHNy51O1vxOcXXtTvIdy6ZOid3dcAfh1qO9uDJBiO5KykZ+6MZro7iKe2VofMDsRyKwpLYTKYmXaw+6a8hVD3OQ8w8Ra3qFrMYrpNqngOp4auUu9SkuCccD+dereI9BW4geKVNyn8/rXk+sWUmjzGOYHZ/C396vXw9SLVlueRioSTu3oQxdCWPFeofDP4cS3Zj8QX6BIsZto2HJ/wBr/Csn4b/DW58STRalqsbQaYpDLGww0/8A9j/OvoC3jSOIRxoEjUbVA7CvToUX8UjyK9ZfDE4PxB4ZTXLaS0lX5cELx0968J8QeEbnRNSe1uQ0YBwHK5Uivq+OwDTZx/8AXrO8T+DbDWoFjuId8knCY4bPr9BXTUgntuYQm1ufKJ8M3qkNbhJwRn92wbIqGfR7yHPm2sg+qEGvadS+C+owyFbGXcPrtzVeD4HeI7iZfNU9iTvFYOD7Gqku54ubJ1UMYmUe5qS0muLCZZraZ4ZAeGFfSWkfs3RlRJqNyXY8ldxAA/DFbDfs9eHgm1rYPx18xgfzpezkHPE8a8L+OkumS11LEcx4WUcK/wBfSu7hw65BGKk1v9nG08szaXeSWjc43v5i/lgH9a5lbXxD4BkW31xBcadnat3F8wj9M98fWs5Qa3C6ex02z3pdopkNxFcIHSRSG5B6ZqYKKkR5ZT1XA96cF9BRVsArV8N6JL4g1m102E7WnfBb+6vUn8qy9teifBXS3uvE0l4OEtISfqW4A/nSirsTPcND0yDS7OKztkCRQoEUAelYnjvxJJpk9hotpIY59QyXkB2lIx3B7En07A+1Raj4gutQma30xzBbg7TMv33Pt6D3qlb+HYmm+1SSTG5wQJmbLc/Xr+NcOIzalFunBXPZwGWNNVa+3YyoNJ1YzeUlzBbiRNxBO5l/xqkfD8+l3ReTVrqZ2OCFCgf1rT1Pwnrl1MJbTWAuOArxY/UGsK+8K+OElWUTWtwEPHzkf0rxY+8ew3bqdXLp96ZlmTUJNzFGKkLtOFZf/Zif/rcVKsc9rEEaQM3dj3Ncm3iXxBo4/wCJlphIA5eP5hWvZ+JrfUoFJyp4NZVHJ6yCnBRVok13mSTK4LDrWe8QdsOuD61pW+15Syj736VJNZ7vm71nezNbmFdWfmRkOoKjofSuI8RaEsM8c728UyRuJAki5UkHODXp5teuRkd6yNasEmhZCvX9K6qNZxd0Y1aammmXtB1GDUrGK4tgFjYY2/3COoP0rehdDhV+Yj0rynRr9/DeqGGditlOwD+iN2b/AB/+tXpEutWmkxRKf3s83EMEfLyn29vfoK+vwtdVoKS3PkMXh3RqOL2NmW4h0+3NxcfREXq7dgKsaRbzFWvb3BuJuijpEvZR/U9z+FZGmxTXd0J70q9wByq8pCP7q+/qa6WH5mCr0WuiWhzIt21nGzBmXPetKKFQc7RUFtV2McDNZM0FOxELNgADJJ7VTaaNYDcy/JF1UdzUeoTi4vo9PDYjVfPuG9EB4H4n9AaWJTqMy3Uq4gT/AFEfr/tUWsrsVyv9le7HnXI2qeVi9PrXO+JtHgv7WSGWJHjYFSrDIIrsZn3OY1IJH3j6Vk3MAuSVztQZLMf4R61Iz5umSXwVrw0yVi2nXJP2Ytz5Z7pn+VdIjBlBHeovi1po1TR766tVI+yt58DDqNvOfxGaxvBmuLrejxS5+dfldfQiueaszVO6ucoq5oZaSNqlxlTUsCJele0+B7GPRPBUBi/4+9WJZ3HUJ6fl/M14uuS2BXqngm7uP7Ns0u1ZBb7ogGOcDcT+HX9K5cVW9nTdt2dmCoe0qptaI9BsLeG0hG8fMavrdRbunFYV1qNvKnmBwAOAc9KgtdWSVijONy8H+lfM8zWyPpnG+51a3MWOgpJJUCZzXOPq8VvgSOAD3ol1ZI1Yl+McY71tGo7bGXstdCxqN5bojhwsmezV5R4h+3aVNJe6Wn7vduktyMhh3x6H3rb1zXGZpJI1YL6Yqp4dvB4kzDAplmLeV5ajJ3emK0jF/E0W2l7tzS8C+I7TWLTzoZS2DtYPw6H0I7V1zzLnANeaeI/BsngFbjXLK7DT5AnhQ5jcn+AAdWx39x2wWuaN40W/tYpo/mzwyk8ofQioq0He62Ip1lI9ItrfzMlx1rP1ew2ZPan6LrCXkIYMOOK1LmH7RBkjmudNxdmaX1ueb6vpsV1C4ZeeeapeDLtLO+ntpIy16wCxzuSSIx/CM9Me1dFq1v8AZpCD/FXH33mWd+l3B/rIXDD/AAr2cuxDpyT6HDmFBVYW6nrukqIYcjr1J9TW7Z8Ln1rmdHvY7qzgmjOUlUOPxrobebOK+okz5Rb6m3bngVdRgOT0FZ1vJwKffXCQ2blzhW+U/Q9aztcsy7fM8s0kpx9qfz5j/dhHEafiOce5raV5Nqqi4mkHyr2iX3rL0uN55GlkXo+5h/efsv0UcfXNbkcflKWYjc3LMadR6kxRB9nCIIUye7MerGsDxBeoUewhdUTrcSk4AHpmte7vpGUx2Ue9uhkbhR/jXL6hpIbL3UvmHk7eig+wqV5jOR8SXVtexmztIswDJkkYYD8dMeleCeAdROk+IrvTSf3TSOoGehU4r2/xRdra203lLsijQsSerYFfMmg3jx6zBcM3zNJlj6881hVNqR20fQVKG4xUKfdqRTmoYGj4ftTe67p9spAMtzGoyM9WFeyeHvDeo6lpt3rNlZI2kzXs4hhiy0iRhsBsd+c9P0rxjRbu4sdUtri1YLMjjYSoYAnjofrX0Z8NPiTotnodpoOpOunzWq+Wkz/6ubnruxhSc9/WuCvRhUqJTdlY78LVqU6blTV9TiNZjFlZP5bblORivJNU8Q6lpd8ZYr1jCP4SfmA+vevsfWtO0fXrVhc2tnfRn+Iqrfkeorx/xh4L8K6fI08Gh2UcoyQzBm57cMSKyp4DkerujqlmHPHazOQ8G6X4o8daHJqVosZtC7RqZpNjOR1KjnI5656g1r6pHrug2UJ1PTpomTCs6lXQj1ypOPxxXo3hUw2ei6fHbOj28turo6HIORn+tSa9IGiNdzymlJK10zkjmtWDeiaPLIbyz1a1MibScfMO4rM8NwtpniG5uNIIjvL1BGoeTajEZyBx94jA7ZAI710upeHhcI93pUUcV4oJaNQFE49P970Neaax4gjhiyPMWYH5QpwysO49CDXDLBzw9Tllqj0Fi4YildaM6a41KbVIw+oSt9oidl+zt0ibJByPX+Ved6lq8uh6wtzp82x5SVljIypr0HWh/b3h7T/E8CKtzJGEvNvG5vukkezD8j7V5r4h0dLZHm3lnxuBJ71boKnPllqnt6GcazqU04K1t/U7vwD4/luNWXTUtvLZk3MXfO3nkr69elewQ6qxhx1z+lfK/hnVXg8QadeQjneEkzwNrcH+de9L49sIII1htZZ2zHuZjsQBlzy3UYOB0x+meTFYFycXTXqbUMZFKXtX6HT/ANgS+K7yOFHNvEWw8xHQAZIX1OPyrY1KwsF1AwS2NtcBh5RuJohLI5AxjkfL9BjFc1H40ntvEWlRQWsr2MGQ2CZCI5QcuCD0BOenG0iu581TM0pwRKDkZyM4x/8AXzXZh8OqUeXqcOIxLrSv0OYGjx6HcEQfJbS/MkeTtVu4GfXn8Qa07O5yQKh8Wa1Z6LobXF3NHFOs6hd+SSFJyoHv0/4EM1S0+5DMpB46162Fd4uPY8zEK0rnY202cVm67qg+2Wloh3HzM7fU4OP1xTVvlt7d5mOAozWF4Z83XNffUm+aG3DKmehdsc/gM/mK6oLdswb6HfWKpZ20ceNzAdO5Pc1ZaNpvmnPy9kFRW6rH8zHLepqV5eO9YtlkNwwVcKAAPSuc1eQlWPsa2rqTg1z2oRTXeYoVLFuKkDyv4i3XkaDqcoOAlu/5lTivm/TG231v7OP519CfGy4t9N8MXNjFKJJmKiRlOcEkcflmvnnTF3X8I/21H61lUNqSPQkOOKkXrUIqUVDEaehx+ZqUX+yS35CuuPB+YAg8c965jw2ubxmPZcfnXRs2VAHHPWvJxsvfse9lsbUr9xt15ccfmI80LgY3RSshA/A1yOt3TsJF+0XUm/73mzu+fzNdZeJutiTXHapEFzWVCTvudGIgrXse4/DHUPP8BaOWf541eP8ABZGA/TFberXW5SM1538MdXjj8Lw2ssTlkunWN1bGMkHkenNdRqF4zMeK+pp/AmfKzXvtDLa58q4/GuO+KHh8Wavr9pbrJBKR9pVV/wBW/wDf+h7+/wBa6DzT5gatqBlu7RoJkEkbqUZWGQQeoqa9JVocrKoVXSndHkfw48RLNd3WgXYDWt6C8QbjD4+ZfxA/Me9Y/jDw7eWV7Jalt0C/Mjnqy9vx7fhXQeIfAs2jeM9Gm0q5RYZ7lXCy5zHtIJHA5GK7PxRoK61YtGjKkwU7Hbpz2NcUsPN0v7y2O9VoQqJ392W54BbQNa27IAVG4lZO3AywB9R/UV6N4d0m81vS7a9treZojG/zkrkg8EckZw2f5/TU+HvgxHtdROrJa3dvLMFihK7ghUEE8jjOccdhXaW9vFYSNa20SQwRqAscagKox0AFc+M5sPS9ot2zqoKnWqui+nU5Vr7WYLC00q408yWcKt5ytcH96/VeABgA59evBFWW+JWtWttFDDocKeWoRi1y7Bvpxkfma3plV2OR71kX9lGoY4FeZHGSludssBTjscJruua34kuPP1VlVYj+7iTO1ff3Nen+ENU+2aLazFssF2N9V4rz/VoRtOK0Ph/qLxSXNiclB+8X27H+levgKt5W7nk4+gox06HdeJtSvbi3h0rTI2lu7k8heiL3Zj2Fdd4O0ptF0yGzeVWYZZ3A5Zj1Pt6d647w4/2q5mvOjysVPqFUkAfzP413+mPwqqMe/evUnLSx5KXU34dqrx196ZLM4HyIG9s1GIA653Nu9QaheR45NhOWA6+o96yLKV/NqDAiNIIx6kbq4zWrjUtjo+oybD1WIBAfyrsr64H2d5dvRcjNcJrEpZDx2pXA8Z+MF15Wl21sDjzZix9wAf8AGvO/CdmbrWbRMcGUMfpnP9K6v4wTtNq9nbfwpEW/Fmx/7LVTwDYgam8pxmMMB+Hy1zz3N4aRP//Z</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEASABIAAD/4QCCRXhpZgAATU0AKgAAAAgAAYdpAAQAAAABAAAAGgAAAAAABJADAAIAAAAUAAAAUJAEAAIAAAAUAAAAZJKRAAIAAAADMzAAAJKSAAIAAAADMzAAAAAAAAAyMDIwOjAyOjE5IDEyOjE4OjM5ADIwMjA6MDI6MTkgMTI6MTg6MzkAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjAtMDItMTlUMTI6MTg6MzkuMzAwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwAGBAUGBQQGBgUGBwcGCAoQCgoJCQoUDg8MEBcUGBgXFBYWGh0lHxobIxwWFiAsICMmJykqKRkfLTAtKDAlKCko/9sAQwEHBwcKCAoTCgoTKBoWGigoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgo/8AAEQgAvgCiAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A+qaKKKACiiigAooooAKM4rk/HPj3Q/Blvv1a5/fspaO3iG53x+g69Tivmz4gfGrXvETzW+mTHTdOORsgJEjD/afr+WKBpM+jfFfxK8L+GWeK/wBRSS6Trb248yQfXHA/EiuBu/2hdJXebPR72YA4Uu6pn09cV8vtK0jFvMLueWye+f1qxbPOQwjwSx3Yxuzjn68f1pFcqPpqy/aB0ySZEutFvYk/5aOjq+0euOM16D4e+IvhfX3WOw1WETN0jmzGx9hu6n6V8TbpS2zYTIcEAHnHX/69OjumXH3lI46daLhyo/QTrRXx/wCD/ix4l8OeXGLo39muP3Fz83H+y3Ufyr6F+H/xM0bxiFghY2mpbdxtpWGW9Sh/iH6+1FyWju6KKKYgooooAKKKKACiiigAooooAKKKKACvN/jF8S7XwNpvkQAT6xcRkwRZGIx0DsPTP54rs/FOsweHvD9/qt3zFaRGQrnG4joufUnA/GvhPxhr974n1+81TUZC09xITgHIReyj2A4FK5UUVNW1e71rVJ73UZpJ7md98jMck/4f0qushjiPQl/fGP8AP+FaeiaRLeQu33VyCOOauS+HJv4cs3bHaolUS3N40pS1RzmWdkwoGB69eea0PNnYswOGJZnZeCSetb9v4VkEWSpLDoKsw+HpIlBKHK9GAyQazdeJpHDzOYgEzsXEmCpO/nBOaXa+QFVgzcYC5Jrq4vDjPkZYKBg5HJOeSPpV7/hE5FUFGJbHB3ZxSdZIaw7Zw8YbeAFOD29fX3FWoJ5rWWO4tXZJIyGUoSGBHOQfUe1dk3haRVUsAH2/NwMGoj4QnfzFjIB6gN0JpqtFkyw84nuPwO+JB8SW50fWJd2qwLmORus6D1/2h+v5167Xw7bjUfC2uW93AWguLeTdE4Pp+PSvsrwhrcHiPw5YarbFStxGGYA/dboy/gcitou5zTjZmxRRRVEBRRRQAUUUUAFFFFABRRRQB4f+1Nr/ANj8L2mjQufNvJRLIoHWNOf/AELH5V836TpUt5KGCM6Zyd38XNelftG3h1f4mfYkPFrBHCMZOWPzYH4msvS4RDYxjyvLIXB54z6gf561lOVjopQ5mT2tsIbRUUDIHpipE4bhT0pyPgbc05FLN/niuV6noR0LVu4HBq7E43DAwDVVY3C5C4/WpbUMZBkfSsJR1OmEtC/GcsNsefoBWtDAGiAC4PQj3qNY8xrt4OMHA5NbdlHti4xnGKdlLQhtx1MeWLap6cds1ArbZhnFbuo2uF3H19q5+TKykehp8vKxOXMtSj4n0aDUrYkLiUD5SOxrqP2cNXkgudU8PTPuSMfaIu2CCFYD9PyrKicSAqRnjoaztLuhoXxH0S/iURxyTLFKS2AVf5T9cZzXVSlrY4sRT0uj6booFFdR54UUUUAFFFFABRRRQAUGiigD4v8AiBKb34ta3IoBKXbAMRjG3AFbvk7bREJJYDqe9UPEMKD4teIFMhy17KDxgHknFa94QAfb0rmqHdRWlzJRT5mDnrV+BcHJGKozTbGCgfOfSkS7IHJK8ZwRk+1ZNHSmjTklIHGfwp9vKRIM/wAqS1RLhPlIbHBGehq62nkBWz15rPrY16XRo287LCrde3NaUdwzIuBnj1rOktfLtIMcszc1omJYoYUzuLDAHY0R0YS1Qk10zL8ucjmsm4xuyCfQ1vNZxxW7NNMI/qK5e8uIEfCSqc856U9ydFuWoGG7g5Oar+K7XfY29yqgyRSqwYdsHP8ATpSJkMueGrQ1ZRceGbsfeZYy4+o5qoqzMqjTVj6KiO6NSCDkA5HenVS0Of7To1jP/wA9II3/ADUGrtd55QUUUUAFFFFABRRRQAVkeJvEWneG9P8AtmqytHDnaNqliT9BWvXifx3u2l17SrEgmKGB52GepY7eaicuVXNaNP2kuU4Dxnc6TqXxMk1LQLuO7s9QhS5Ypxsfaysp7g/KCQehqtfPjJz+tUtK0iCx1Se4gAHmgkr+BqfUA7xnb2rByvqdkIcnumI13idh5azbiBkgnA/zmmaib+4RhZ2zRhTk4H3jz79OfXtVs3Vrp7Rsw3O4ztGMnHX6fWobnxXGr+ZmJIlKhnVHlC5zjJGB2PfsaXM+iHyJ/EzAtdfvdNkSO4VwQTu3LgA9iPwrvNF8WRXvkwjaWb+EE5HtzVW78nVrNjFLpl+6jLRbWgnQ9OM/Toa5uy0eeLVR5lvLDhvlZhtNZylfdGsIOPwvQ9X+1iQICRtQAA+9UNa8Qx26h1I3ID378Yqva6beebb26lWVxnlutUfE+hvHG7QwKXUE7fWsL2Z0WutDB1Xxff6nJ5cAkIJAAUBs1raLo+rmJ7me2jbfkBJn6g56gfUcDHf6VjWcht4XMO5Jo1LOkMXmSBR1JPRR9at6L4m1G8ma1shfzSb3j8pHgaQFRlj5fXbgdenHFdKcraLQ5ZRhf3nqdEXurWFknt0UnK5iLcAjnqT3H0rYh3T6fPEg+aSNlAx0JBx1rmNO1sy6n9luWWQnIPyFHjb+66HofccfSuo09DGqduanm7j5Ox6f8J/Fia7o8Fk1sbeW0t0Rcvu8xVAUt+f8676vE/hqDZeM7GKFSsT28kLD0wNw/UV7ZXXSnzq5wYimqcrIKKKK0MAooooAKKKKACvFvjdaCPxHp9/NkW/2R0f32tuxXtNee/G7TPt/g1pQpJt5AWI7I3yn+Y/KoqK8TWjLlmjwjQbw6jHd3TIqpvKoB2z1H8qmk5Ug1U8JWc2nWd9ZXP31kEyuOhVuPzGKvtHkcd65Oh6W8jIl0OyvGJmjLsRwc9K0dfs9N1eztINaty0lsu1JIG8piPQrtIx9P06VetbXDA9qsX0m9AkYV+OCWOKhy6lqC2sQ3VzpN7pVnp6aZFbWlou2MqA74H+2RxknnArno4WW6j8oSMoJ8sSMWIH1P8q3LfT3ch5SDznaBwPenTQrBPhCC5HY5rPm0NuRJmto8u26gLvhl4OPSrGqLJJcOA/yknBWqlhbE7eMtitVbdkwWBA68isXLU35Dk4YpNCvP3MCm3lUoVK7lZepUqfqenrV7wnDpOjXE0+k6SYryUFfMZS+wE9FBbj866+0gtdRhe1fy2ZeqnqPSsuSzuLKYxqVaP1Ycj/H61spXRzOOpSTTojMZ5Ywbh2LtIR8xJ6mrm0IygVbjhUJncGyMcfyqrJ/rO2BTQnrqdZ8ObVm8UPMxVlVHYDupIH/AMUa9XFcD8MrBla7vmzhgsa/UAZ/kK76u+irRPJxEuaYUUUVqYBRRRQAUUUUAFRXMEdzbyQzoHikUqysMgg1LRQB87eIdGk0fxBfWjoyxYJiJ/iTPBz9KwQAsmCO/evoXx7ZR3Xhm9YxI0sSb0Yrkrg84P0zXz9OMSHgVyVI8ux6NGpz7kyuuMLjJHU1Lbwg9QMY5xxWcCRMCM1qGZRbLtIG4ck81hLVHZDcy/E+qCxsiLc/vZDsU0lnNZWkayXt3EhOBl2x/Oq99bR3xMkoyvRfWuY1PQTfTI0rGVYz8qSDIqYRKnO2x6pHd2imN4XBGB8w6Vf1jX7CDTPPvJIreKMcuzBRz/kV5VpeiapawM8dz+4UhRERwv0reufDtvqmmql7LLJyMnP3an2b5vIftly7amlf3qxGHVdJk3hBiTbzlT0NdXYanDq9mHxtlxyKx9AsbPT9OFlEn7srhi3Jaoox/Zt55aMVyMpg43CjlcR8yka1yvloccn0qpncw9adPc+auRjHtVjSIPtOp2kIH35FX9aqPvOxnP3U2eu+D9OfTNFjil/1kh8xh6ZA4/StukUYAA7UtemlZWPDk+Z3YUUUUxBRRRQAUUUUAFFFFAEN9ALqzngbpKjIfxGK+adUgaCaaNxh43KkfQ19OGvEfijpJ0/XpJkXEF4DIp7bv4h+fP41lVV0dGHlZ2PP2fIDDqOtQXNzI6pCuct+g71BNI0chGcc4qG7k2FZjn7uM1yKOp6Llpoa24LGN20KBznim7Mk8E5GciuSu9VuZrj/AEeB3jTk84J+nrWlpGo6hesBFCQvdcAED8eaqxCep11m2yCTOQxPTHUf5FWNP8ySzLbGUK2ORWPb3F8Ahktp2Rhj5V3gfXGcfjWvdLqk9tG6wmCEjCeY+z9Bk/mKi7ubcitcdc3JtvmdioI78VDezLd2nmQNmWP5hz1rA1W31eS3mtjPCUZSVOC2D29PzrL8NXV2pktr9dk0Z2k54P496drozvZnX2N1v2kkjIzg9q7r4a2xvfESSYykCl2/kP1rz2CPYuVA6cY//VXtXwl01rXQnvJRh7pvl/3BwP1zRRheZOJqWpndCiiivQPJCiiigAooooAKKKKACiszXNc0/Q7RrnU7lIIlGeTkn6DrXinir49RSNLbeGbdtwyPPmHX3A/xrWnRnUdoomUlFXZ7pqGoWmnwma+uYbeIfxSOFH614r8UvFltrGpQ2Vk6yQQIZUcfxn5c/hyB+deL6v4m1HWdRQ6rqE1xJI4UpvJAyfyFJ4p1D+zPE2iS7sQlGgbn+Fjgf0roq4P2dJybuyaVa9RI2rqQGb/ZPeoZZFmjEQPc1X1CQxucfdPNVoJlchh09+1eM11PZTtoa0FskcSYwGB7d6tW1zBBOGY+U/XcOn41Fa4nUYzn61JdaZJdJtXO4j0qG2i42OosdZt438zzrfzMYJfGfQ0+XXLQ27KbuDnG7ZyxAriI/B97Ly0ipnsWz9O1a2m+CmiIaebft5wGyKm5pd7GmlwJ/wB4vAPTPU1i6rahL1bhSAccjpmtye3W0G0HAUdKw9SkAUl/ujJO70pJMltF+1l/dIHOcnP4V9EeFta0q60myjsZkjUQrsidgGC4wOO/Svl+6lmj8O6he/db7O6wL3yRgH8zxW/pmhXer+HfD/m3cMYtn2yeRMC6LjleOh4H616WCoxmpXep52Mm7rsfUQOelFea6HrNxp8SRIzNAo2gE5IA+vX/ADzXW2PiGGYfvBx3ZO31HUfrVypuJzI3aKht7mG4XdBIjj2NTVABRRRQBT1LU7TTYDLezpCn+0eT9BXmviP4mxTpPbeHZ4jdKDtVxy+P7p6fzrzDx3rj6jdbo7+SWIj5wzZ9+vce3avLrrUHZzJA7KytwVbBGPcV69HAwUVKTuzlnXadkb3ifxDqGsTSvqdxI0u4goxOQa4fUCzSAQExg9+hJ9q3AZZ7SWa4kd5pMbnc5JH1NZTR+feYQDCYxiu2cU0omEZu7ZaslNpMJZAHKjdgg8gDJP8AKpfiawnsbF49zNtOSO3ORUGsXCRW9wCfmW3KqQe5YZ/Sr0UP2/wzPnLTRiNvXooFZ1Yc6cEVTdmpMPC2tLrWmJFcc3ES7Wx1J7H8anuY5bGTLfdJ4OK89hnn0HWhLFwpO7B6Mpr0y3u4dY08NEVORyvpXy9aHs5WPfoT9pHzLularGwHQEfeFdNYavAyjBGfSvN5rZo5fk4btjrTlluo+UbJ+lYtXRsm0eqSayixfKyg+tRp4jMajo+OOa8zS6vnZQxz6k1dtLO+uW2iQnPUIOlZ8luprz36HXXmqC5cktyegA5ptlY/aJFmvOccpFnjPv60zSdMW3XlvNkBxvPIH0rYYx28PXn1NDl0QKF9Wcn8StRNtpENvCdskk8agj1DA/pitv4PzkaJOk3KeaVIY9Bwc5+tee+NJZdU8UWtjAC32cGRvY+/410/gvT57Pw7qFwkpMiM/GMZ4Gea9zLINQba3PHzCac7J7HtSiS3jXym82HHKn7wqxaT5YSRvtZecg4IrzKHWbu3fT3s7hlhmBDIeVPHH0/CtDXfEl6tk1vbQxpfSjEc6tgL6nb/AJ/oep4Wafu6nKq8be9oda2uz6xrElhpVw9k1sV8++iHyk/3PY+49+K6uTxx/Yk8VnqaPcOVz5gI5HrkcGvK7DW9N0PQIrW2nV7xuC2CN7kZZsHt6fhWbb6tcR3IQSiWEnJSQBlJPXg/zFbUcHGrq1p2JqV+XY+gF8caKVB89xkZwYzxRXlUNg8sSSLpVxh1DDFyoHPsRn8+aKj6jQ7v8Cfa1Dlb/wADWT2/7y9vmDYIBdeOPpXnGs+ENSsNRK6aTcQMcAMQrD2Oev4V73IFlsoiPvDA/Suc1K223YYD06VzQnJa3OiUIvoeep4E1ue1zPcwwDHyruJ/kKoaH4G1eW+njluoI4lbDvuJJHsMDP517MFLQAH05rK05dl7dDIwT+VbOrLmWpMYRtY8x8YeB7ey066e3upndI1LFwMH51HQVo+G9Dj0G7tZbi6S5t7l1idJU2pkqSM8nI4rrPFsIl0vUh6wDn/ga1gaxbSXPg+dEO6aAJLGQeu3p/hQpuMmwcU1Y4nx9Heavbi6uUjaeIkfJGFIAPI47VyeiX0tlLmMnaeq5r3Lw/baLc6PNearMTDcqDFGoO7O3Bxjknp7eteP+ItFGnalIbQs9qzbo2I5KnkZ98Ef0rjx0YP3oHRhZSTtI6uyuob+HnKsOueas+UBgEKyjsf6Hr2rmPD93skCSAHtzXZ23lDDZYZ7E5/wrxJPlPYilJXKaLz8kJB7EPitzS1kK7CNqDrt4/M0+FLbbu3qPwx/WtSzET9CWHX2rLmNlAsQMRGEjTcfX+gH/wCuqOuXKWFrJNMwMirnb2X6+prSaR3+S3XaPWsG4sf7Y1ZbV23QW+JpwOjDsufc/pmrpxcpWRNRqMbmL4U0e78yS8vYlRrpt7FuWZeoB/ugcH1ye2K6TQrmK38Myu/3Hm27VHrj/Cr2qfu8pt+co0sgB/z6Vt/D+2i/sVA8aMu0khhkH5v/AK1fWUV7Ggmj5iq/a1WecRarbxafFuZibO4AJwfu5x/hW5rd3bNFBLHOgZeRng8f/rrtdS8N6RFe3aDTrYpdoJSDGCNw6/SrepeDtE1DToWez8ttoOYnK9vTpSp41qWqFPDJrRnnazW11a/JJE5PUZB6+1ZkF5b2l2AXSJ0OV29Bj2HFehQeAdGuLHYqzwyD+NJMk/UHP9KzbHwNpFjruJ/OvA8ZIWRsAcj+7iun66n0MfqzXU5eXxpqolfbq84XccAH/wCtRXpn/CI6J/0DIPyorD6wv5Tb2L7mLY+J9LMNqWv7dPMjBZJJArK2BkEHkGppbi1vHD2lxDMvcxuGx9cVhStpF/p9lqM2mxGUBfMzGpJOB+f41cn0bT9RRZNM87TZ0wrSW4CFgexA4I4rJU7R1NObXQ6hEKovAOazLQILq5yAMt2P1qrH4VinVBfalqV2n/POSbCn8B/jUNv4H0FWl/0BfvdRK+f/AEKk0uZDi3qN164svsuoRNdQeb9mOY/MXdwy9s5rL0+WH7I0E0kYLJswW4Iral8PaCllqtmunID9id84z0KnrnNctL4O0TyEcWKjv/rH/wAarl1YX0RgxwwyaT4i0USn7RBE7WckbfwPhiOPXaB9Kq+HdMn1PwJbTXWwm3uXtNwzlQoUjdx/tj8BVzxNoy6RreiXOjSmyedTC+3584OM4PtW3BaXXh+08+SeORLq8S2u4kjwkob/AFbgcbWB3A47Yrn0vrs9C7tarocta+HS8uQCrA9K6q00R5rcKw+YDg11Wk6dC8xB3HcocFjk888nv1qz5X2K4K9VJ7V4GIg6c3BnvUJqpBSRwMuhyQyjeSvPTHWui02zKIBknFat+iSncR39KgkYRQ8dawN9iLVLuOxsnYEA4496wdD1nTdMtB9unEl7fOZnEY3GNeiqcd++Kj1pvtTRpIW2M5UjPXCs3PsduPxrmfFHl6V4fgaBCLzUAwjkU/6qMcnnqSc4/E17GXYXmTqS2PJzDEcvuRPR5PDX9ufa5Ydfi85ht8uLbIYx0xw3Hf8AWus8KaOdH0VLNp/PdA6tJ0yQQD+oNeL/AAp8Dxiz/wCEhuZ8hQxiiQkHK/3j/QV6j4T8WW0mg2z3K3LzkuJG2r8z5JJ6+td9TmWjZ58bbnSashP2KQ9c+WfoQf8ACtCP/kFpng7P61hanrVq9vbyhJgiygYwM55962dKmS88OwXMYIjdMgHgjmsUnzIvoMsQVVsnNZdwP+J9bDjHln8ea17VD5ch4xzxisPUruOx1ZJ5w5REPCAZ/pXUkZHQjOPvUVkrr9u6hlSYBhkcD/GijlYuZH//2Q==</t>
   </si>
   <si>
@@ -3578,32 +3548,65 @@
     <t>Disorganization.</t>
   </si>
   <si>
-    <t>8UpNAChvmpaQLzTwOetACAdOaft5zmkC/NnNKzYoAGNIBuPWkVdx60/btPWgA20gXpS07FAABigtQaRD8wpDFT7wqXvSUo60BYWjHvRS0ikIq89afjaetJtpaQwpwGKOlHU4oAMZpfLo2/NnNLuoGIseCOafSUUDCiiloASndKReTS7aAD7xxQBijGDS1QBRRRQAUUm6ncetMYlLtpQvvRz60BoAXml49aQU5fvCgQlC9QKk2ijaKBiKvPWl2ilB5pdtIQ3aKG6GnbaNtAEfNKenSpNoo2igCJe1Pp20U2gBc+1JS8etHHrQAL1pcCkFOoDUTB9aOaWigYUUUL8xFAgHNLtp5QU0rtGc0D0EIpSMik3UZpMQnl0eXTqAvvSIaY3y6MYqTb70nSmhWYyk3VI3ORTPLoCzG7aWlCe9DLjNCEJnik20bfelpiEZevNN20/tSbfeqRaY0rgZzSU8jrzTdtMsY1JT2XrzTdvvQQ/Ibj3padtppU0BYMZBoZdoPNL0o+8KTJG0EZFBXb3pRzSEMZdueaaKlZcg81GUwM5pAHagigNR2oATtikZcDrTiKbTAaKCvFOK/LnNItAmJSGlK8UUCsN20lONJtoAXNH3hTacKYxNtJTjSbaYBSg0gNBHegBfej7wpM8UA0AIV255pNtOb7pplMZnU0mlY02kIKQfMaSlU/MKYDtu3nNFFJQAtJ1OKOvFKFwc0gDbt5zSk0maKQgoUd+1Ip+YU4mkMPvHFLt2nOaarfMKkB+agYlKBigClzQAUq/epFXJ607GKAHFqaaWgdcUACt81OoCjNL34oAXvSqu5utCrk9adjB60gF27T1pMUtIF5pFoXvSgUAd6XqcUh+oUu3nOaAmDnNOoAKVRlhzQo3HrTwu1sg0DAx+ppqrgjmnM2aUDFACY96AKWk3UDHCikoByaAClAyaXbRjac0wF8vnNFIWpMmgY6k3U2nAYpgH40mDT160u0UBqMC804ClC07bQIQUu2jbUioc0DI9tCryKl8v/aoEY7mgQ3HvRtqTAoo0AYq9zUuKRRmnbT60gADNO2+9N289adSEG33o2+9FFACMnvTfLp9FMYzyqTyvepKKegr+ZH5RpPLNS0UaDuR7aNtSUbRQFxm0Uqrg5zTtnoabigB1IRkUmaN1Megnl0eXTt1LQAzy6cUwM5paUnIqRDKXdRto20WATHvSkUbaVlwDzSAZQRkUvHrS7feghkez3pWXg80/bSMvXmmiSLbS0pGBmimIa33TTafilNMtOwxhuB5pNvGc05l9KRl+U00WMopaSmAUhHcUtLjIpEMb94YpNu3vS7aD060iRAaGXcDzRjA60A0CIymBnNIDUrLuB5pnl0gE7UEd6UrtzzTccUAJSbflzmne4pKYDc8UUrLweaSgAoZeOtKRSZoJY3bxSU40m3igBaDTacppoYm3igGlo28daYCbaAM0KaX3FACMvHWk8v3p38NJmmBk00mhjSUgFFG35s5pqn5hTt1AxTSd+tG6hT8wpgO27TnNKxoPNJUiCmk04H5hTQKBC4xR1OKOpxTlTBHNIYKmCOaeBigDFBNAwJoVcnrQq+9P20AGMUtFJ1OKADrxTlXB60Ku09ad3oAKF60u33o2be9Ax4XvmjNG7tS7eakLAvWiigDJpFIX7xpwTBzmjbtOc0E0DF3UtIq5I5qTy6AGr96n55poXpzTvu0DACl3c03NOAxQMTHvQBS0UALtzRt2nrSd6KYx26kpKKYBTttAGKWmFhAvNO2+9JSqpY0AFKMscU7yx60oUKeKQaiCM5zmnqvNJup1ABtApwzTaXdSE7DqKBzx3ppba209u9IV0Oo57VFJcxRglnUAdeapya5aw5/erx6GgV0aX3RuanBsjIHFc1deLII1ODkD3rOl8ZS4GxevYt0/SnZi5kdtvz0HNMkuEjb5mAHrXAzeLLtlO07T2Oc1nz65eTsC8p564p8rIckel/b4CwAkFO+2Qf8APVa8rbUrhXHzMfXnGKimv7jaWEjZ+tVyi5j1r7TH1Ljb3Oaal5FKSEdWx7815VHqt2kefObp0p1pq1xHukVmRx3zkUcocx6v5g/ClVskDP615sviy9iX/np04zV628aSxzASRfJ3INLlYXR322jbXJf8JpbY6sHPRT/jVm38VWzTESSbFHQ5zU2Li0dJx60baoQapDNtaORXU++KuLcIzbc84zntSKuh+33pKX7wByMH0NLt96Y7obgUMvcUuKSmPQZRTsUbaBibqXdRto20wFopD7UbqAFpxGRTaXdSYWE8ujbtHWl3UE5FKwhu6k3UoXNL5dIzkNZdwPNN21Iybc802miRu3ikp7LkdabtpgNAxS4zS7eM5pKZasNZeDTSu2pKRhuBqiyKlp3l7e9Jt460ANooopENCEcHmk24HWnUhHXmkSJQBmlApSuBnNAhrLkHmmMu3PNSZ4pjfdNIBnaj3FFHagBKTb8uc073FJTAbniilZeDzTaBMKG+7S0hGRQIbRRspdvHWmMUGim06mAbeM5oU0tJtwM5oATFBoz8tNLUAZFJ944pepxShMHOaYDdmDnNGeaVmpAvvQULSquDnNG3nOaXvSAWkY0NSr8ufWkSxNu2jrxR1OOlKEwetAwCYOc09etJS/dpAKxoAxSDrTuvFAAp+an01V285oJoAX7xxShdpzmmg4NPHzUAOAzSqvvR90UKfmFADtvNJT6TbUstAF5paSlAzSH6ABk07btPWgLg9adtoASlVckc0KuSOakC4Oc0BYAuDnNBNDNRQUFFFL92gBQMUUn3jilC4Oc0ALtzTdvNO3UlUAUUbqCPegYZpelIF5p22gBN1KBQq+tOHPHSgBVX1p2MGkC4Oc06gBR1pdtAGKWgVxAKWkyO5qKadY+GIX6mgWhN16c0jzJCwBOTWJqHiK3tVKxt5jY7HGK5m88SzyRvh9oP407ESaOtvNftbZsPIMj0NYd14yyx8lc54ALVyreZK26Qb2cZBBqMuiqI8kPn+7VKPcycuxr33iCa4yNyj/ZxWdIzbV3MN7DcVx0qvMg2hwcvnaFp0mJGG5mEhXaQBVWQXHqxVdxAO0+tOuJVZgxHlnH3RyKh2KpZQWP1GBTwrSEb5Bs9Nvt65piEEi5xup247hhd1QOy9FHJPWnW5ByWOB3I60CFaVgxUkknr8uAaPMA7bqWNljk+QmUHqrHFNmk3HHl7W+uaAATZ428UrSqpwv4+1RqQrAnOARnAqXfA7s4UjcPukUAKNsgI3Hmho1VRwxK/wAWajDA5IXYR705pyykBefrQANKCduPzNK33TuOaiXMjbgMjufSpWG5TSKTFgup7c5jlYc8CtaPxXewjAbIPGawt3lv0zSpjawYnp1HBFFgud7o3jZXUQ3S7PRu1dNb6hFcKGSVCD2zzXjSswxliQPXvWhY6lNaEMh56gVLj2Gpdz17cOOQc+lLtriNJ8cLJtjuE2HoWrrLLVLa6UlJVPpzzU7GsWi3toIp3p+lFIsZRS7aNtAXEpNtOb1pKYxNtLRRQAUpFJRmgBVo3UAZoIpMhrsKfmFN8ul/GlpEDWXbnmk208jIpMYHWmIYy+9N21JTWXjrTAZSdKdtoZeDzQWmJTWX3pcYpeoqiyPbxTakZfem7aAG0UUn3aRDD3FLnIxRTT6ikSOZcDrTSNwPNKGDDFKyYHWgRCUwM5pKkYbh1pvl0gG9qPcU5l255pvagBKGXA60u2lI680wI6Q09k4PNM7UEsAaKPcUUAJt460lONJt4qkMWjqMUgNHSgBSu3vTCtSMflNRk0AY6/eFPzTdu3nNG6mAUKfmFHfFKF245pFIdRSCjPNMQUvXij2pduGzmgQBcNnNLRTvu1DGH3abRS/doAAOetPC4Oc01fvCnE0ABNAoAzSheRQAm33qRflpAtOA3MOaAD7xp6rtwc0m3ac5pd3NA0rjqbnmlakHUUmX0HCnKvIoVeRTgMVIABinAZOKQcnFKF2tnNAxwTDZzSM1I0lANOwxaWm7qdRYBelA+Y03vinhcHOaAF2c0lKWpu6gYuaCPemr1p69aYDQKcvWl20gHc0wFAxS0L81P8ukA0DJpwTBzmjbtOc0u6gNRaNwHNNpJJEgUtKQiAdSaVw0RKfbmoLi8gt4t0kgUd/UVz+qeKo4kxbtmRuB7VyV1fz3jlnlNNK5lKSOuvPGVvblljXeR05x+mK5jUNfm1GbduZR25rPjTJBc/e746U4kR4AIIz9O9aKJk2KpZWYyMeOdp7/AI1EzFmztyjHlc9KseWblS5aMDOB83X9KZHA0kjspUxrweearYRNGEgtSqqW3HIk3dPbFVJNsOSQWJOevvSzTeWjLj5RjCg+9G6IspQb3x1oEPCrMpYMEGc/So0Z58haJlXBKja3saPLMGCCWB6gCgdmLvjjDqdzOe+eBzTS4ZCBTtu5goXAPJ468UxRvUFRjJwfagLMU7JFATkDo3vSKrRjIYBc8tjp+FK0WAdgx3C0kkMixgg4DdVFAWFOwGQrIu5RkYHWmx9BKx/CnxRh8B5Gj45yMjpUGwquOozQFgDck5pc5PUintFuUuq8KOaqsGLjFAidpOnYChWXjIyKasZf5e9Nk4U0AWo5hHC6KOG6/nTPPPpVcbgpPX2pwORmgBxOTS7vlxTM0uTvK9xQA6STcBSiQiPjg+tMZfWjdxigB27cCxzke9SW9/LDNvjZl29g1QKdsbcZpkY3ccjPeiw7nb6H4+MQWK7DFema7O11a3u4RJG2RXjMkJRtqucVZs724085imcDurHiocexake0qwZQQeDSbq4/w140im/0e6IibpuJyOlddEyzxCRGDoe6nNTZmsWh9N8v3pVUNxuP5VJ5Z9aRWhFgiipWTioyKYBtoIpKduoGNpc0baNtAhKXdS7eDTaCXqOoIyKT3FLuoJ5WN27RnNGaU4PFJsoEIRTakZfemkUCGbeM5pKdSbR170FobSMvHWloqihm2hk4PNO20EdeaBkRpKe64HWmBfeglgB3p2cjFJt4oI71LIFZMDrTaXd8ppKBDW+6ajqYjcDzUZTAzmkAe9B6UgNLjigBtDLgdacRTfamSxnWinsuB1puMigBKKNvvTsUxjdvGc0imlo24XOaYCleOtM2g96fn5aZQBjMaPu0HtSfeNMoVfvU7+KkC89aX7tIAY0vSkHWl+8cUxMFPzCnMaTbtPWikAqnmnU1adUsBfu0gGTR9407btPWgA27aKKQmgBQfmFPXtTFB3U8daAHUq/eoFGMN1oGlceOtNC80tGaC0KBz1pwTBzmmr94VJmgoM08fM2KYq5PWpNoU5BpMQuwKc5pjNmlZqQDFCAAMUtGaX7v1pjF6UfeOKT7xp23ac5oGATBzmlLUmaKQBS7aUDFFAbgF5pwHekHWnbKYCdTil8ulCYPWnikAgXb3pd1IRRwOSaNQukAGWAzimSSCPOR0Geao6hrVrYxku/zdl6Vx+reLZr5mjh+ROhwcmnykuSR02p+KYLKMiNw03bnpXH6lr93f5eV9qH+EZrOZjNwPmbqcmjD7AAfmXPTk1aiYylroLuM2GRhjHT8KdHGyqpcbd3pzSR7ViU5kJzyuOtSxyEMCQTjoM9OKojcBLFMyLgrtODuGAaZG22RpEIzG3RhlTTZFPbO5v4WGQKChhlz9/K4K9vrQFmStKkrSB4dm47lKjhe9QoytOTsZB0z0FP2GRuc7R6HFKyAYxnjtnrSCzEaNSrEwtt/v54HNIVSP/VjLGpfMLRlWLIncZ6+lCxpsR1O4n2xigaTI+OpHNMTKoc87j16Yqc7Rk5ORx0pHAUKpzgjrjNIqw2SNSjfOfl5APSkZWaEMygDtzU6qv2cYDFuzEYqOaaSWNELt/u44/OhAMkU4BHPH51EqiQqjEj2qbzNgGeCKaqo8qnPIOaAsMkQxllY/KB81M3fKAOcVYkhVo8Hlt+4nPXjpUfljj0oQDNxXK5wG7Ypu3acgZqadlkKgLtPTNKibfmPPtTJsQ7WbkfKaGT5TkZPrUrDcMAUkkJUD3oFZkUZA7ZpgXbk9c1I8ewZ60xk2YyeT0xQFmH4U1hliQcZo59aWmITaM570HFL0pobc/SgBFy2acrbacVxSUAOZtxyaDhqbQTjmgBy5VieuemRWxo/ia40dx87tD/Em7g1jrkqDjrSqwzk80h3senaX44sLlUSRzHITgbhXSLIGwQQVYZVgc5rwwhM7iCMcjnP0rs/CPjKSJUtbvaydA5OCKlopSPQmG4YqPaaQXSuoZCHB9GzUxXnBHPWoNYyIvLo8upNtNoNNGN27R1pM08jIpvl0wCm7adt2jrSUAJiinU0jFAhaWkWk+7QTJX2FIyKaV2g807IoIyKCBm33pGX3p23aM5ooEMC0MmAeacRTc5WmjSOw2grxQRgZoDUyhpXrzTdvy5zTz0pGXg80CvYjBoxkUuwAU3NSTuBXrzSKKdkUnSgkVlwOtNI3A807d8pplAhhTAzmkBqRhlTUZGKQC44oIpM8Uq0CY0n5TTKkZfem7eM5pisHvSUUUAKRSe1LmkIpoYu3C9aZtp+flNR0wMfbuxQF2nrSK3zClzimUO6U2nfeo+7QAmORzTtu05zSL96lNIQUvSkooAVaUDcRSCnL96pYDtu09aKKKAClVcMDmhV+bOadQAvelAxTV607rxQAKfmFKvWlVMEc0neg0iHenKuT1pBTl60FDgu09acKavWn0AC/ep4601V+Yc06gBtKD81IWpRxQAg9acBk0AZpduD1oANu09aWiikMKcBigDFGaYBSrzSKu4jmpFXaetAAq7SOadSU9FyaQCbfelPrT9lBjJ6HnrzxQIRgFXlqwdc8RQabCyhg0p6DOKi8QeKI7EtDCd8pGAc9PWuDurrzpj5mW3HJzVowlLXQdf6lLfSF3bKg1XG3cAp5we1PVNsbbRkU9fm2kgKfTrVEEaRszKuNhb8an2JHGeSXoRjy7Lg/wAJz0pHXMikFmyuTximG49ZOI2jUq31znik3fMHkUsuDnaeelOjX9z82UYdAR1p8TsMAFSR/e6UikmVULFQQxwTznvU0arks4LZ4608r8oU4JznK0JGSppMpDBH5cjE8bqdINrDa2T9Kn2rGwMh3ADrjpR5B2lmVVOflG7rQBEzH7p/LFSj5GX5tqY+9jpxRGpWZ5HTCqPu5z14FMcHCIcHkng5zSAYVMjE8FeuTSxx7pQrnJxnrgip4YzyFOV7gineWZLwSBQi42//AF80DKkzCEhTnbn1pu0mRiDtXHFW7iBPNLcOnb3ptva5T5myM+lAyuyHaDjOTj6UqRIXbcSgUE7sZ7dKsT/LKwUgACq7NIZFY4w3XigQxVaRQR9wjJPpTlj2tndj8KeP9YQOmcgfh0qVVHVgCPTPWgRTkYl2Ax9cU+NTwDwDUrKNzELgHtSXDcqVG3FMCGRiMgfnTWct34p/3uMU0pgZzSARsrgj0qFF4b1Pc81KWJI44FIMKCcZoAi8s0gQ1KPmDHp7UgY56UyGMjXc3PAFMKndwMj1qbIHUZpC27joKYrEdKw296Vo+Dg03uKYgXmikX744p2z5C27kdqAHbh5IGOnOaZz6cetKrjoRkU5W3HA+UUANXDcN92nKi8gN/SnCMA8mnbF7CgDV0TxNcaRMqlmeDPzLur0nStettUQFJctjkdxXj5HlsH6+xqxa6lLYziSElD3wahotM9pVtwpdtYHh3xAmpWqbmG9Rgr1JroQCQT2AzUmqaGkU2n03b70GlxCMim7KfSUAJtoZeDzS0UAR7aMU/bx1pKBDR9adSAYpaCWIRkU3btGc0+kIyKCBtMp+2ho+vNBadiM/MKTbtGc0/bSEZ4oHdDVNGMil8vauc0lBEmmNK9eajZMA81M33TTMZoGtiJfrT8ZFGwYpM0DeohHXmkxx1p1IR15oIEpW+ZaTHHWgGgQxk296bUjD5TUdIBc/LTaXHFB9aYDWTg802n0MuB1oJY2iiimMP4TTKf1Bpu33pjMULyOacV96Re1OoGA4pPvGl+8cUu3ac5piAJz1opd1JSAMZNFApfvGgYq804L0pFXB606pYBSKfmFH3jinKu3vQIdRSY5pc4oGKBz1pwTBzmmK3zCpN1A7MXNNHWjvShfegpC05V+brQq/MOad92goPu0qn5hSfeNO27e9ADs00mikoAVetOpAMUtACr1p1N2806kMKcF5pNvNLTDYKFXnrS0oXkUgFVcGnClVcnrT/L96XqA1V3HFSbdp60ix/N1p22gWnUVT1yawvE2vJYWjxod0r8DDYI5qbXtaj0y1YD5pm6Ln39a85muJb6Zi77mzleeBQot6mU5dhsjeZIHf5mznJPWoplRm6Yz3FC8khuccEZxQm+PgYKk9DW5iIsTGNipyo/PrT/JES5LKWXp83J/CpfKTfuLbQvJUdzUvlxi43hFdQuTnjHHTNAFcZk2qzYPOOM1O26RkJK4UYBBxTVjMjBhtJY8YPSpvs6w/vCdxHB44GfapZpFCMm+NWG5j+gqNELMMDd6irMMLR/ITz146D6ipBbFSCoA4yc9+KRdiK3+QNGQuT7cipRsVCCcE+opB8qh8YfP1p8i7gQ4yMUBYq7mVXzjPbvU/wBlDEAE7jg9feo1KrGTtIftmpyoTa4ygZQSvXv60DsMbau4EkZO0jqKjjtQk3yZ45yT1qfCtx1yc03iHaCcgZz78VIrMkY+WF2qPm68+1QLNypIyrcU+NSScD7p+8T155oaJWaQqVZRwqg9PegpEa4ZCAhwDkEt0qW3bdGRjmkClh02gdutEJCttBIPbigTKs29rgjGM05vmCDjcn3lxUkisJOGyw6U1IwzDcdrN95uuaaJKzMDITViKMMQCSufXtT0hjIJ6sP1oZCV3kYC9vXtTAS42hlVeajulCtwcjHWnqwZwdvNRyY2gMcEUAQk0jYIo3Attpjg524/GmKw/jBA600IDnJ5HakWMqwIP6VIiBQTnJoAhKkgMOB0Io57cGpeAtNfgUAMCA9etJsGCfSnbvmAHOaQtjIPU0gGqOetHQ9KUqeg70L0PtTRDWpGxAbOKQAn8adJ0JpnVTgn8qYrMGXv0pPukGlC5I5pxjzjmmIFlJbGKl3VDt2/Nmjd5nHSgCXh+CQB6mo5EK8nHtg5zUi4VcHn605pPlIIye3HSgCTSdVm0q4SSMnAOSK9T8P+IY9WhBZsSYxt615L/wAswwOCat6Xq0ulTpIjHCnJ96hlqVj2jnbkdO9GaydJ16DVoVkTCyYxsznNa3DKD37j0qDaMlYRqbT6aaZQpHem0tGKB7iUm3inkU00BsIDRt96NvGaQUENdgK8UlOLcU3dQKw73FNNKKDigXKxpXrzTdtP60m3igQ0jrzTSvy5zT6Qjg80CIz3ppFSMnB5pmKAG0jJweacRSdRimjRbDKG6UrL15pO3WkJ+Q32pdvFIaOoxQSI3KkU3y6kK+9JQIYV255pMU5vummqaQARTT9007HGKRl96YmMXrTy2V6U3b8uc0LQKwmaKCvFFND2MQfeFONNVe5pfvNVDBfvCnUm3aetLSAKKTHzUtAwpV60gGacF+YUDHLS9Tik+7Qv3hSYhwXBzmjPzUueaAvNIQdxR944pQNzDmgJg5zQaRFVdvOaWkzzS0FCilU/MKTGTT1XaRzQA4Uv3jSUq/eFADguDnNIW+alLc4pAvNABTgMUAUtABS7ec5o2/NnNLQMKdj5qTb83WnKuW60gBV3N1pxXHelC4PWnGP3ouA1V709VyetKqds04Jg5zQABcHOadRSry2KQnYOgqpqWoLYwsznbip3mXk5245zXn/ivWftV40KP8q9ffvTSM2UNW1g6ldSMxOBnFVbezhmjDi7iZmPMJYq/r+NV33bkwFYMcFSODUs0JXvx2CgDHatImch0jIzjDZC8HFOIVlY7sFfb3o+y72RIUA3ckZ/Gnx2584hlKY7VRNmIIcyAseGqfy2hViACGOQfQelOii3DDgsD6DpUy2hZc5xjop71DkaxiIMHbtUKR1qXcqoTt59KSOIHKg5PpjFPm3RxFVAweM9TUmiRHIpjhCEFWYA5BznkcUxuHG8lFHv146VYt22zAyH7owM85/wpdoaI4wkm8sVb5sj0pDKigMvAyp68+9SpG26QL8zAfLS+W0TbyoYHooGB+dTRo7PuQYNAEMitHGheNQ3TGevvTzbloQSSVC9ccCnTSNIoV/vDoT/AIVGZnfCIrbehXOBQAxcIVZhikmUNJlX4+lWfsroqBhuBP5fh3pzW6Q72CsW3YDHp1oHZkG3ZbgnAbB6n2psi+SEA2ncgJx9anlhhRygUmQjJXPSmSbHxtQCQdB60XCxXYtG5Ab5vShUlRtznrUot90hZzz6UybCuBv3D1oJIWkO7OOaeuHAzwTSeWCchw3sKesJfGD0qkSxCu1iB2p0iswyG47r605cDcTxTJGD7cNjdTGhjQvtzwvv1qvdKXxx071cSFmXk8Z65p0iqqlcZOOtAjNWMO64GCKlmhMON2M9qbPCysNvPtUQWRnG8En1JoJFZ8EcdfemEFj1p8isvJHApv3WHemIaylWA9acfX0oaTc3TFGN33TketAESkgls8g04r8wOPxo2nkZ609iGTbjHvSAONu7PSo93DBhtqQKAME5FNKZBB5549qYDGU7cjkUxt45IGB2qYruYru+UUnljpj8aAIuo9DTUYnNOaPDZ3UzaYzj1oRD3HO3ymo1bac0+T7pqLdVEkjSbuAKSOQrIARxSK205xmnBv48UAPZcqADyKZgjknn0pfOI6ChpMqfl59c0AX9L1ZtPuopEJQKeTn2r1bSNUXUYRIsq7cfMPSvGNquMHp6VveFdabS7pEfmE8FScDoahotM9cK/LkEEeuabt96js7pLu3R4yCvtVioNoyIyKbUm2m7aCgBo20uz3pdtAxjLkHmm7ae3SgigQxk4PNM21JSbflzmmMSgrxRSg0AJjrSGnYo9xQZyGbeKSnGkxgUE2GkcHmmsnB5p2RQRx1oAixxSEVIyYB5pnagQxvu1GDUzL71H5fvSNEG3ikIpRxRjIpksQn5aSlK9eaTbgdaCQZdy9ajKYGc1IDQy5B5pAR54o/hpWXbnmm4oASgrtGc04ik+8MUwGk0lOZMA80m33oAxGoXrQBk0u3mrAUdaKKKQBSgbjSUq/eoKF24NKOtC9aX7tAwbtS7dp603PzCnjrSYmKBijPNBNCrk9aRI5fvClzzRtwetNHWg0jsOC80tJSgZNBQq/eFPzzTQu09aeq5PWgAAyaXocUEbe9IOtADgMUq9aSlC5wc0AOpdvzZzRt+bOaUmgYZpdvzdaPu/WhetIByrk9adt5pF61Iq80AIvWpaaqjPWnBec5pCDbznNOpV60YpAJTN23JAyfSnNUF1N5EZagiRheKNSNjavGOJJOBzyOa8/Gd288sxOSa0/El899qT5b5V4HPNZspX5FU5x3/AArRIzJVbzG2hchf4ulTEKFZnB29+aS3RVhCq3zdTx1pzgmMjccH+7waoYQ2yTMAkqseoRiVz+NWooyCxdVLDgbe1RW67cYGf96tCzhPccH0FZydjSMbj7eEeXgg/hxUixurdiexPUVZjhK87flqXycqTjtWakdKgUFt2SQl8ewFTfZw3zAbcfjUkajCsw5B4q9GQ67VXJNJy7D5DK8pYgFCd87jTZVZZj91weM4xmtFrfzGyeB+dNnH7pVWIbgR8x780+buHIVJASuzIZB1HemiFo4WBUru6Nn3q0qgMSVxjGRjrzTmzM8mRjjhce9HMg5SkbVfKI2l5D0OcfWiHeoMe3itOGFZOew9KiaMrIQG6e3NHMHKN+ziZGVScgdRVbyzHHtlDADAz689cVeuB5IypIDdfaq1vGxYlvmbPGTxS5hNWK8ro1wGKndjlgMk1Xu1RpFZSVI9ua05oRJIWJO7cVG3jt60q6duTLt15+Yc9afMiHFsjg00NZLK3Vh37VlldrOCAG7E8itq4hnkixGwVVHC+tZkWnyTMTIxLZ6AVaaFysgso0y7Oq7geO1WpJI4Y/lXnHGDTpNPVYywJUqOe9Zs6y7huBUE44pkWHQfNIwckhu5GBUsgi2BNvI75pIYwobL8AZ60vyMmflyTxzQFgwOAMrSSc7mBxUnllsZ4pFgIjZh8ygc0w2Kq7nZXPQdjUcmZCcqAM9M05Q7AZbAz93HWho1ZgdxGKCGMZVjiJwar5LYbbgfWrckZkdcDgcYPeoHPIjC4HdqokjMfy5Jx+FAxG20Hj+dOk+UY605IRMrNnYey4zQBC3HQUmeop3O3JHehcs2Mc0wsIq+9OKgd81Jt4IAyewqHcOQOTQICh2gDkinYAXk8+lMV9tO+9SAiZcc5prfNzUj5OQOtAjKnJHFAFZzxjFRlasSL1FRbTTRDI6lVfl60zYWNSZ2KaYrMTy/enCPB60q/P3xSK+4kEUwsxjRkc5/Cl8zcMLkAdTT5D8pxUTf7PFIDtvBPiVLZmtriTAz8u416JFJ5i7h0rwUTMjBs4YHO6vV/CeuJfabGoO90GGbPJ/CoZUTpqa1EbB0BHU9R6VJszUM2WxFTgaUx0hXaM5pFCbaTbxTgaMU0Awim1IV4pu33pgM2/LnNJUpTrzTNlAxFoxTtuB1pKZnITb700jcDzTvu0uBQNOxHjAprdKkZfemsuAeaBSXYZ94YprLtXOad9KG+ZTQTYjFIy+9LQelAhm3jOabT6Rk4PNADT0pvtTscUhFABt460meKX7wxRtxQAxvummKalK7l61GUwM5pAGOMUEd6M8UtADW+6aZUhHvTCtMlmMEwetFLu5pKooMZNFAoNA0AGTTwu09aav3qcOtBQoGKQ88Upo2kHrQMFXB60/pTaVjUksP4qevWmqvvS4w3WgSVx69ab92lppNBaHL8zU/bt5zTVGGFOoKFHWnr1pqr70pHNAC/wAVKF5oVe+acOKAALyOadt5zmkU/MKdQMKX7v1po+9TqQBShaUDFKv3hQAqrgjmpfu03p9aUDJpCFX7wqVetMCYOc07NIBfu0lFFAAMDmsbxFdbLOTkqcdQea15Pu9cD1rifF2peYXt4wcgfez15ppa3JkcnITJL17n5iM09YdgUFfnPVc9Kiib5Su3LA5zV5G2QiZhuduPpWqMbBFH0JGwfnSq2+TbyPen7slQrAs3arCxluTwU7etJsfUWOEKnWte1UBQMVRt4d5AzitSOP5RWM5I7acblhRlduflNO2fLtxSwoSwNWFjz0rDmR2qBSkjPljAxt9s5q1ar8oGN2fbFSxxlJSSvygdfWp4AysQB9KlzNY0yq1um7jOTSNblW+bj361djQq5ZkDY96srCrLvIyR0rN1AdMxo4QxcgZPYYqVbGQsXJHPQY6Vo/Z1jRiQMGlGwRkbefrRz3KjS7lIQfZ1JGPU8VWFqkkvmd2/StC5TfwpyT26VW3GPahHPrVxl3IlBJlC4hOCfvbei+tNhjPAcZBGfTB9K0FtyzBicjOelMa1djtReS2R/hV8yMZQ7FWGMx7huDbmyM1IwLfKc4b0FWRpkmASfwq5DaOiggKx9KXMhqkzLksRtBXcR/dxipoYURWRU7dTWkkZb5MLvY8Ln86Se1YM+EwCOxznmjnQ3TsjmXV/MdGXKsfWqt1bmRRubAXtjNblxYrkkkqR2qjJYIX++QO/FaxkmjjlTaZjNEDuAbr2IqSOE+WAUVCvSrb2KIxCvubsMYpqwytgkZHStU0Z2Yy8by1Xy/Tk0xQVjJIyCOcVdk08rtJXAbke9SfZjswpA+tHMg5TGnh+VT0UGoHjIbAyQa25rFWHzMc+wqJofL5VeaOZCcSjhV27lJXHI6VWkwAwyMH2q+0EoY7xkN7VA9sO6kVSZm4soNHlsg5PpTcuZB8u0DrzmrvljPuKj2+Z3xVE2IZI1kY9gaI7dY2BzUvl+9Eke6Mc4oCzISpMhIbaR7ZqB4gr7e571c9KayDzA3pQOzKnln0pFXnnir3HpTfJGCPWgCrtI+b0pdxPFTGD5Tg1Ey7QTnkdqCSvKp5NM3ZXGPxqw3zZGKj8sEH1HtQBC2FUmjd8pOKJFOCKRfl4oEIrFnBpzLllI4xSt8tGaAEf7pqM9KkZdy4pvl4700Q9xnI5rR0PVJdMvImhYoM8988elZ+Mg0kcnlyKc9D1psEj3PSrkXVpHIRhiB0q9XF+Ade+2Ry28jDdHgKc9a7baaxlub3E6ikIyKdtpMUihnl0u3inkU0jIoAbTSMU/bSsnB5oAYDTKcRigU0A3tRt4p23FNNMl6jaKdt4602mQDdKjb7pqTHFMI4PNBpEYtBXrzTtu3vSUEyuRsnB5puKl29eaayYB5oJIyKQ/dNO7UjL70CI6MZFO28U2gdhPehvumlpNvXmgBqtSsuQeaQrgZzShsrQIYV255opW+6aatIAbpTd1P7Uxl5piZiiiiiqGFAGTQq7m608LtxzQWhAuD1p3SgcUnLcUDDPzCnjrTVTDdaeOKRDEoXrSUKMsOaQDx94UL1o24I5pfu0GiDHNAFIOtPoGC8sKkAxTFX5s5qT2oATd81LjdRtwRzTtvPWkAq+lL944oWPLDmneXtPWgBNu05zRTiM0i9aBigYpaKXbzimA9V3d6cF2kc01flzTh1qRDlXLdaeEwc5pq/eFPzzSACaAvNAXmngYoATbRtpaY1AEM0rKrYXj1zXm2rTG61GcBunfFd14ivHs7F5EfB28CvOpslv9YHMi7jgY79K0iZS3GwQllcjgjjNWRhYVQruK984zUVuwjXp+tWFkLORsOMZzmmCQyO3zIDjvV7y9s2B97H3aZG33So6mrkcYkkGRktWcmaRjrqWLSPdtXGDWnFFtUCobWMqwHb1q+iDbXNJpnpUqelxIo+lWUXb0psfpUi/eFZM7FEdtPk7See7U5I/kp6gfMPSrVupVsgc+4rNm0YlW3hHOQc1PtKrxUxV+SSKesJK5zUXNeQr/Z2cjLZB5xipmtUZQAoyB+dWFXAyDyKcyKo57iobaLUNDP8A7PXbls89hRLYJwFTn+9WiudoTOVHfHNMbK/Lt5PQ+lNSZMqaZQWywQCOPWpfs6jvz9KsuhH401oyuCBmndk+xRGY0wDjOKNvl4Kr+PWplj3YUH5j0Uinxx7fkYZJo5mP2ZVa3EmWKgH1xzR/q0C4z6n1rQaEiPjH4VF9lOM4q4y7kSgZlxZhxkjk1nzWarnIro2h6ZXFV5rNWBOP0rRTMJ00zmHsU3bgOalFiscZGPxrf+wpwcc1HcWq7eKtVDn9ijGmhLRRqTkr3x1qsLbceeBWtcQkKcDpVVYyDgnrV8yM5UylJEVXAPH0qLyx0xmtHy/m9qhZdrfdqroy5Ci8JkYZPI4BAqGS0DZAJz71pNH3qJl3HBFPmaJcDDFqcPuIG2oPJaPPG4VutZqTgZwarS2bAHB/DFWpLqYODMgoQc7aZIx2hcVqG1bvyPpUc1rkgCr5kRysyiD6U7ZhsVcaAKelM2bWOR1/Si6EQbaYxIbGKt+XTGh+Yc5pgVwtQyQl5OvFXjD8ppvk/Ljp71SJaM9ozH71CqncT0FaUkI2lep9aYYQzDtTFqZ0w7etQ9Gq7dQ8Eg1TZSrUEsU800jFOxShN3GaBDA1D/dNK0ZX0xSMuVPNAEK8UpAznr7UrR7VJBqPJBBNMRqeH9QfTb5JFOAW55x1r2ixuDNCjZBBXOQa8D75xkZzjOK9Z8A6kNQtTEScxr65qGB11I1OVKCtQax2Gg0hGKGXaKA1BQlHbFFBoAGTg81GRinlvlNNbpQAA02lI70mOKaAKTbxnNO20lMlq4ymleKkK4XOabTBaIYRkYpNvFOYccU1j8tNFbiUjfdNA5ob7tIiREaKcy8Hmm0ECFevNNZODzT26UnUYoNFsR4opxTbnmkpifkNb7ppgNSNyKYVwM5pEg3Ipm3Azmnfw0lIQZprdacy7VPNMoAxaMZPWilX7wqxoXbt5zTv4qQ0UFIU80u3bzmmKSzVJ/FUiYL1oaj3oHWgkAucc0u3B60o+8KF60GkdgHWg0uOaVVyetBQKvvTlX5hzRt5py9aQhQvvTlXBzmkX7wp9AxAPmpwpB1p4GaTAF+9Tqbt5pd1IAoAxS0VQwpV+8KQLuI5p6pgjmgBd3NSKuT1pqrinr1qRC7dp60q9aB1pQKAHL1pSabRQAUUUhPy5xmqQXscZ44u8QtCQSOMkH3HauRsVVgNpLFe5OMV0PjGTzNQCKRkdj0NZFtAsbH5Rkc8HrVIxlq9CTyx5ZAzvOMDHH51pW9vtty5A3EYC5/XNVl+ZQpYDdx06VPb7mRRktIGxtzjHHXNJmsRBbmORY/vZOc9K07e3YOMjAXvUKwru3Hh+3Oa0LeHPzEkZrGUjohG7LscWyPpmpVB29KcmBFjHPrUm3aorlPTjsMVSDmpVQsRineXsz3xUyDYm7pilc2RJHC5dyDjpzVvcxZcnAHtUMcyl8A7t3bFXYYGlxxxWUjeOwwLu4zn2xUqxk/LjGe9TwW5VQ5THsatNChXiRUHdjnAqTWNrFEW7Ae3rihlAkKkEgD6ZrT8pVz5c8c4HJ2g5pDamRS5liXdxtY8ioaZojMbCg7VzQFLc4rQ+w5IKuJAODngVI0KQFVYjPfg4H40AZ/klufTtSLiR8beBxmrTwySAsinYDy/QDmpPs584KsY245JbGaYiAWqs+7bkL39aa2WUrtwKvtthQKSM+nWmpCCc5GPSmFijHGcgBSauLD2IxU3lDscH1pWXb3zQKxVkjGCKgkhG01acZOM1C7YOMZqkQ4lZ4c81E0WDnrVtm4xtpkyjyiehGKpMhwKUlusintWZc2u0nmtdlzUEiDnNXcxlAyGGFxj8aY6hlIxg+tXp0HQCoGh+UnHP1q4yRz8lir5YznNMaFeuatGHGKYUwcdarmQuUq+X8/Wo5FGcYzVtl2jNVZIy3Q4NVzIiUURsuzqvHrULxBlbAyanbOME1Gc5wKpO5zuBRlhPcbRVaaINitKYbuM1SePa1WjDltuU3Q8inLBuA5qcjnJFJn2xWiZEo6kIjCqe+KTA9Kl29vWjb70yLFYp3xUDL89aDpuQ81XZNpzQIzbhduTVGVhnArVu1A68is+aNeSBg0zORXpN3Y8D1p6jByaa+CcY4qiRdybcL96mt0o2qvOKG6UARNIemKY1SOfkI71F1FMBpzjjrXX/DzVDZajt2Fgw2n5vbr0rkl+8K2fC9xHa6pGzHq2MY554pPYh7nuCncob1GaWmw4eFfTGOe9H3ayWm50rYR1zTdtPbtSVQxNvGc02n0m3jOaAGFevNG3ilbpSZpBuJTfu04jAzRSEFMp33aTbTQCH7pplSMvvTdvFMiQzFMK9eakppXimUhm3Heinbcg80m3A5NApLsNI6801k4PNOJpPvDFBBH2pCKey7VzmkoENb7pplP29eaayYHWmi0NoxkYzS0hpCYxl255pCKe33TTO1BIN900ypMZWmGM54NIDDpV+8KQDJp23b3qyxc80n3jiikX71IocFwetPXrSA80tIiQNSjikXrR160CFU/NSijbtxzRjmgtAOtPXrSKvPWnBMEUihy9acq5PWkAxTl+8KQhyrt70d6VjSL1pDFAxTl+9SUu35s5oAGoXrQ1IOoqkA+hfmYCkY0qrtYUDHbdp61IvWm4p44pCFpdvOc01T8wqRetIAXrTqb7mjvQA6iik3U7ALUc7bYT607dVfUmK2chX7wGRTQnsec6zMt1qc27AIYqM9Kity6qOVIHfv0qvcKzXLs6/wAZO48itC3Qy7Y9qpkeme1XsZRWpLYxrgGQ5weK0YbNWZpM9Tk8VXS1KTRqrBvlz6dulaFszEGM/L7AZrOTR1wj3BIMOFHer8O5V4WoRGdysDyM8Yq5bqcEk1zSOuMdSdMsoyRz7VNGpkYDoBTUXdg5wKmjwoKnv3rA7YxdiQfMScYPTFWvJZIxhQQepPGKhj2NMrZzgHgDrxUzMWUqzBR1A7evWg0WxPbQL52zOWPcLWvCm3dGvLLgseRiqWnRyRDzMsFbABA5x/StIRkyECSQoCAF3AZyfXFQ9TSJJt87IRgp9GOKesUjMoUEknHykf4U9rdomKSowmX7vzZXp645p9rbyXACNIoVlyUIIHtzSsapiC3lRmRpNrFtvkjBPA65xU0MLNHgJAqr/wAtJVPH4j1qza6SzfKYpW4BkWJwM89ielaO2G22PHa/ZolO0/aWDA8cEgHI5oszRNFS1sFkt8SW0k5bpJCCqj8SKr/YDC0gYyJjkrJgE+w4rVkhhZUKqrODkiMsF/AbsGm/ZZLhmkhgnkAIBEjhgOfSi3cfMjNuNssSE2ikNwHD8j6jFVls0RkYsVaRtpXbkDj1zWpLawI0hBWFmPKnIJxzgHoOlQ3FvB5jNBMI9y+Zsckj3GaTi+g+ZFOSIK5VMEr0O3BNQNFIx+62e3Iq4q+ZkuzIG6EL179c1G4CsHYsNv8ACGznt+FTZjuVNu3rnI68UjIzcqAV7nPIq81uzrmP7p6gnJqP7GfsZuE28NgxlsfjQBmyIaiC5YA/nV2Ur0yNx7VCY+4oM2QFQDUM8Z2kg/hVkqNrEtgj+HFR8GmIzmzuximMDmrkyhckVUkXLEZxVIykQXEIQgg7vbFVW64xU8ylc85qufvVZjLcZJJxjFR8fe9KfKh2kjk+lNZcJjqMVa2MnYikbcCAOveqx4qYk5OOlQt96ghkMmNp4qIr3zUsnQ01lyDzWi2MJbkLL3zUMo4qzt461Cw5q0YSuVzH8tRtH1OasygFajaM465q0zNor7aNtSbfejy6siQzbUEi7varFRyJ71SJM26UsMCs2YkYralXqSKybpS0nHFMiRXblDQFxgdSaV0K8Uc8etNGQ2RT0x1qL1yce1SyM24YOaj4KnuaYDWTcvWoGXacVZ2sqk9qiZc5OaAIlbnPpWhoMqW+sW8jLkGQZ54HNZ7JtzzT7ZsTxnGcMKZPU+gLO4N1GzlAoU4XBznjrU7dKzNAkLWMIJ521qVDN4jdtG33paQGpLAikp9NIpiGsvB5phFSUjJweaNwI+vFLt+XOaCKM5pAJSUpGBmikIKay+9OpG6U0Qxm35c5ptP9qQpgZzTGnbQjK8UjfdNPbpTG+6aZQxaT7tP27e9NyKCGhH+ZTUdS4yDzTWTGeaCbWGN0prfdNPxkU0r15oEMoK8UpXAzmk7GgY3HFNZdvenmkb7poATtTW604dKa3WgRhL94U6mL1p1UaCNQv3qPvHFOEfvUjFFONJt20q9aCGG3JHNG3nNOH3hQvWgqOwUL1o704DFIoVT8wp/8VMX71PXrSExwGTT1Xac5pq/eFOZu1IA6tSgYpF6072oGCn5hT6aEwc5pd1ACNR92kB+ag1SHsOXrTl+8Kaq571KqYI5pMQ5etL944oA560oXBzmkABMHOaetN3U6mAE0DrSUoGTTHsL944pfLpQmDnNOpgNCYORzWZ4iYJpshyCSPu/jWsF7e1c94tZbfS2ZvlcjA5z3pdSZbHAW8AmvCMj1yeK2LdfJkjYMrMCQM9BxWPa5+0xAAYHBJPWtqHelvLtQOEOemDyauRMC0qNMu/fg7sttT7voM5q5bM0bHA3IOrdDTNPjZo12HbJ/FuOAasx4G75mkLcNhcAfjnmuZnXFE8LeZyBz6VPD90joajhAUcDB9asIu1fWsZndBE6x5UjNS8IoB5pkbZQnuKevzMD/AJ9KyOpE9uhAVlGG6VcsbeNndnP7tOW3DnPbj61FGuIiqjleR71raVG7ESfu1duN0nCqMcnHc4/WkWWobdtkbOyhZDjCngc9cVcdREhWPa2Hx5jHgKOScfQVFFCiJho38vcTvUAlh2IGeOa0YdNhmhaR0kePGXRsL7jnPc0FhY2r3ziIN5u/LpHGckrg5Oe1a9npsCzPGLhU+TAK5yD78cVXmvDst0EKWzKgG+H5SVJxt/XrWlp832dJ2a5kiAAEcMMYYy89Sc8UFEkcMKLGxDeeycTKwyDkAc1bgtJ5mEcytIz/ACBm2gYHOelUJpILgIhAtXSPLPMpYk5z06CrKyRXjA7Gl3RYTymIycckcelIq4Xvh5HiUhInCMfkB5PvnNVhbx215EtxbPHalc7osknjjv60s8cSpHiB1UjayyS7fxzipoSvl7RJGseAoHmgsv685oAztqPutgsgj3bxk8t+OOKSNUjkSWQNJEOFDIMEY5BH05q5cEi1kiWOTAIJdwFJ5GAKjhhEkao7bNxwylvu80FIzrhY4HaSI4tn5RZDkjv+FNmWAiRoiCWTdtJ46881YmjjVbjzNrLuKA4zjjgis8R3MaxxqiNuBAAHUY9e1SylJDREqHO9vLZc7lOAD6U57dYbfcgVgw6bsnr1qNfL2SAAgKMFGOADml8xxabH2ZbldpyR3pWY1JFWbd5L4RWHcgYI5qvJmFd2M1amzGyhDmNgDux1PpVeebPzHoB0p2ZLauVbiUMh2r83FR7CpJJ6UNMtwvLYGfu02XasgIzyMYosZtkcjDnmqc3Gam2+WHyd2ahf5qpIzZXLblK45PeoGQg5qy3ynpUMjbgRjmmZSIuNwyMioXO0EetTlTjJqF13AnNUjJkLMFjYetV29ank6EVVPXFMhkbc0jUretM6mtEZS3CoZGByMc1I2dtRH5mqzFiYznmkZPlPNP24pjrhT3pmbIWXBHNR7ucVK6+ZgA4pm3Hy1cTOWoxh3zTPvU9u60witERsV7gDb0rOmj3NmtOQ1SlXOcUyTPnXbzjJFRsw9OTVqSMsrEHkdqjeEcGgze5WVTgmm7dvzfeHpUzDapX171GvfIqiRjEspGcL34qtv3ZFWWPOMcVBIA0gwu3FAEbfdNMXcrAr1HIp7fNxTTHgHFAj2PwJcy3OlrJIPQDnOK6lfmFcV8NZFk0sRhvmXkiu1Re2alm0dhdvvTdtSbaZSK2CkbpS0CkgGkUntTyvFNIoAayYB5phHepGPymmN0phsJ94UpTAzmilPIxSAZRjIpdvFJSM2hpFH3hilJpOlUgtcayYzzTNvvUrfdOKjplJaDGXtTCmBnNOb71DfdNAxq0jNSjikK9aCJDKKcyYB5ptBAm3IPNNZdueadSN9000WhhXim7etOzxSUhMQphetNIzUp+4ahPWgkwtvNL1OKTNKPlINUWKFwc5p69aF5oqWSwNKFpF60K3zCgNx6rgjmjFLSfxUi0AFOFAGTTtu09aQxAvI5qRVyetNXrT1+8KQC7dpzmk/ipzH5sU0CgY4daVT81Npy/eFADmppNOamg/NTGhcbaVetJTlXJ60xCr1qUU1Y+RzTicUmMcv3hTmNRq3zCn00IF606mr1pxplBmnL94VGOtSL94UCJF60v3aSigYd65fx5GG0lWJOVYLj8RXUVynjhitnGoG4M2fTHNHUiWxyFpDumAPG3ll/lzW/Z7fMkJBcbRjHfJrBt2CyZV8u/BOK27UEzFEx8q9SODTkKmXIRJGzL5WCOSpNX1bzs7m8tcfdxVeNSjNI43P0LAH+VS27BlYMhySQMcg+5rlO6KLEakfT1qzHUEJJypNSK3ltnrispbnbHREqZDMKuQxk45qCFTIxIHOCcZ9qvrhYx1yRkjHNZmhLG3l5PXOB+tayQtDsjkZcHkVjwsJGAPetS1kXbkjlf7xzmkap2NOHP2eRVhWRs/65s5A7AenPepYY+0ZbzlXc+WIHTpiobVlkYyXBZYwCyhRwcDPT8K0Y7TdbxXDqytO29Gx0XPXFWkHU0bBJEMLqVlk25YOvCZOMYzz1rWs7OW++03RijWGFlj+8FIOQMgVlaNNHcW7XAlV2STYY2UgMBznP0Ga6RbWyups2kck7q+/EaEA/KcjGelSzbcntbGxe2lzPMpD5fMe4NjtnPFMkZ44/JWRvLwXQRRjdj0z2rZ0nN9ILQyxKOSVIx1B4PpVaOxNvIY7VZS6uY98bBifcelIpK5zixyaoY4zMlvIjgj7Yu0HB54xzxTY9Ne9uplLWsj7yYlKBA/BJ5x6c1qahpt7Yu8klneOV5Zp05A9RxUMUbwWbQXcdxLI37xMkLsX6479KAsZd1ZtazRyyEtNn5UDEge1U7j/TmYAASM24tvIIIHK4x7da1WtxJbkR5ifPV25Tngjjmqd1A6gMCxiVtsu4YwTxuB79elAjNfDkwRsWDDLZ4xzmoYbjyZHwCp7EnOKluoWt5mJkUw42hxxnvULw5VZElWVOdyjgj05osSQSZmd2VvukfMVwOvPFNhdlmYFV8vODx1HXNOLSyR7SBnOB29qIVF06w9Cvyk56+9OwX7CzW+VkZZVEKnKBjgn2rKuH2ZyuUxgt2rqoYo7vR7mCRU+0Q42rt56jJz9K5G6T94qspAfkAHg0guZ28ZO3161ahYcFj0FR3VmbZ1JI8tujUkkPl7cNuDDnigkjkkEx44z0pk8ZhYDqpGS3TB9Km2qNvGApzn1qtJHPJNtDKUJJyDz06YoEyLO+TH61DJlZdo9etTbGDEY+amtG3Ugce9BDK0jNzzkelQNKOQank9jVaRRnJ61aM2Mk6E1Xb71TtypqJl2gmnYzloRtHuzzURXBxVjcO1RMuTnNWloYS3In5BFR7dvOalZaY3INWZsjz81IzfLSkY701elMxluHG08VBn5xTy2MjFRnrmtESDL82c1C3Wp26VAetUSyCSqkn3qtyLnPNVpF5zTMysQRk449KZztIAyTVj73GKZuCmmQynNHtYFTuHftikdfMXjipJJFUAActTdufmz+FNElUrtbrTJFG0mppFqJvuNntVCKY/1gp/UUxlKyCnp948ZpCPRfhPLHtulZvn7CvRlHIIIIryn4Uup1SZCMjGevtXrCxL1GRUSNY7ARkU3ZUm2kK981Nyxnl0FMDOaeKQjIpgNBppXinbdozmkPSmDGMvvTdvy5zT26U32pbBuMbpSLT2Tg80zbTAGOFNNNPZdynmkIwKBCU1acDRt7ikGw1lyDzTNuB1qRulNYfKaYXREyZ5zQy+9OPSk3VSAZt4zmmnpUmMikZfl60iJEbfdNMqTb15ppTAzmggaV4pNvGM07+GkoAiZdtBHenOO9N7UAL1XFRtH8x5qT+GkoA5xetPpv3acPvChlMevHFDUlKvWgkNuSOaUL8w5pR94UL1pGkdhcUtFKBk0hsVfvU4daTbtPWlXrSEL0oU/NS43HFBXaetAxR1paavWlagYfxU9fvU1VyRzTtuD1oAWmr1p1G3b3pgKvWnr94UxetSLzzmgB9IBuakzSr94UDHBcHOadRQvWqAd0ptK1KBigAVckc1IFwc5pq/eFPzzQMTPNOpAMUtAgLbQTjNcx42jDaXuLYIxjAyeorp65bxpkWfJOP/AK9HUUtjjLWVDMuUZDnHI610emwSRl2PIxkMDnNc3ZMJblY3bOem44Heuk0siHKqrFv4lzkfnRMVPc17ffHtYFSfQrxSblRmycFjk+n5U7cHAGdh/Ok2rnaSGPXNc3meiiSIFck96sRqGIycCq0bFsE9M4FWV+UgHnNZSOlF2Few4PbJx9auI27Mh4I+RMDI681StwSRlucHGR7VoQr5qxgLjjhc8cck/pUGiFaJZFyWw27HAq/a7PMREjy5JUFmx2yTVOM4dnK7echeuKsQyJLGjM5Vmf7u3JHb1ppBdG3ZuykxyhWGSqhW6DB5q8yrNpwt5LlzKw8uMQtkxr35+nFYxUeZjJULwG7k+vtWzYxiW3aUK3mFcDEewRkHIbOeatFcyO3XT7OOza2jgkt7eVEdI5MMQ4XGc4GQTVmzt2m+We5NjMT8wjQkBQOuRzWDp+ozakYUmvPPuVAUkLtx6cZrbhtduoRA3jbXISV0OGHt1/GjlRal2Nfy7C3Vo47qe4kkhDiONCA/I5YkcetWLGJtPEQWBo2Ub2Dtkcjjj607w94f07w/pdw97K8+oyBjDdSSkhkDAgYzgVcW4ku7iOWOS3+ZQGYjO3HOevNPlRakxLid5oAHvLu5uJgRJalsKvHAzWVqOj+W0cNwJbWbyiSzSB1I7L045rYktWmvCY7uKQsCCwXAbjpjPFRrbzeaGuBDvhbKRMd27nkE9uKiUewOfQ5DcbSPzJGhkK8EtyTk4xj8etUJoUNgSsUnEmfKZsjGexxXUeIoYvIDy2cUaTS7lMfJA7jp+Oa56TVIWjeFZ98Ub5iCoQ2e4qeVjUtNTFaG1jkOd5tgfnDpwD2H51jyDy7iZYVCo3RTxXVW9k90sUElzFH9od33NwBtUkAj8K528gLXhUMrHJAKnA4FAGesvzbZCRyDx9c4q1ar/pEzKVVCdxBbBFJ5eFCbQ2TnrjBHatXR5YbW7ZJ4IytxEy5bnZ8pAPvQMpw6jF5NwwTeJv3ZKt2ByTWJ4ka3EkTwFjCqjPyfdP1zVqGH/RUjUMCCxBVeDzWXeySrFLblmEbYJ3L154qRMqGZbjA+8o+72xTVkKsN33cGltCWyoTjI6DJpzrkEjGFbB5walgh6MY4oyVGR2POeMU6WdUijxEu5f4gce1NaTrkZyOPaq55Ur600Jkc7K+RtwW7iqszGPjJNTTfLz6VVnbzBmmZyK7yfMOKik5BqSeLpg9ag27eM1SMWMdsKTUTvlTxUkpqFulaRM5O7EXrTWbbTl60yTjNWjJ7jW5qCRvlK1LnPFRSLjnNUZSI+velWk6CkV9rAEZqkYyGNyCemKQc0si4y2fwpPukVYDT1xUTrhqfJx81Rl91BnIhkqo9W5O9VZeMmqRBFj5s0zBOSOop2cc0buw496YFOYSccDC96RZP3ZyOKndsqQTkmmooxyKaIkVvmYFgvAqCUMzg4wB15zWgyjy2HY1Rk2gnAORTJK7KM0xlKjrg0SNtkA9aQtnHFBJ1Hw4vFt/EO1Rnd8u3Psea9oX5cj3xXh3gNNniJDsJbO7j6GvcBksThsHnJFZyNI7D6a1OoZfeoLGUUu2jbVJgNIyKaV255qTb701vumn6DRGV4ppFPU0jDANMBjfdNMp3UUbdq5zQDG0EZFGaWgBu3C9aFp2Mg0hXAzmp6mbGleKbt680/wDhpKaERsmAeaYRUxXcDzTCvB5plx2I+xpD900/bwaaRnPNMl6kZ6UN9008rt700/NQSRCgrxSsu2j+GgQ3GQRmmsu3vTqRvumgBNvy009acv3aa3WgDnfvNT1X5hzTF+8KlHWgpiUq8tSUq/eFAtx6p8w5pQvNFLUlIKVfvUgGTTtu3HNIfmKPvUvSgDFLjccUAIp+anD71IV2nrQvWgYu2lo70oGTQMF+9TqTbg9aWgBV60fxUlKKADbTkak6mlVfmHNMY8DJxTwmDnNNX7wqRetNAFLigDvS45oAQCnAZNJTl+9QCF27T1pR1pKKYbj160u2hfWloGNYVzPjZgNKBIySV4/EV07fz4rkfHTFdPQLk/N9O9HUiRx9uy/aI22ZxnjPXiul01ZI13HgHqR/hXL2rOskbgYOTg9a6zTY5GjVt3ueKmoFPcvXEZbp8wx16UyDCt90g9BzU+35WbOW4xSNhsYXBFc99D0iaGHbjnvVjad2BUEch29KnhVppMKOSOPyrE6Yly3jbb1Vepyx46VpWoDLG2xiijJI468fh1rPgjL7UZmGeSV4xgZHNaVvhrgyGPcxTb1xTWpQLwTj5Bu4zzmpkZI2SXII5AVevtUHzK7E85O0ccD1NTBsStCHAKjIbZ1/WrSJZehZWkaSUN5hGAu7gc9c1vWtxIfLQSMXJGVByCO/HfisKOUvChh2tIxwzNwDV5ZpLiFx5OWTqU4I565piOw0mVLe4nvPsrwxdmKZIx3xmujsmFzNbXS2aTxSlm2s+3JAJYnjjgVx1ndNPZoxmaN1UD7pIf2xnitqG+lt1EkUjSBlwYvKON3QjOeOO+KDaOx0sN0UtI2jt4kDMwiaQ7gBnJBHbjvWrCVeRRIIY5Jl2IIXHXv244rk9LacxxyxJCoZyPJZuRxzitR5FhbbBGA64eSF0J2Y7g55oNEbUFqYpSqRSlYmyW3Age9UtesdJuFsb2zW8e6jnJu0D8ScYAA7DNQnXor5f3cDQd5MscPziq0kiJeTMiCLcFQKsmMEkAnOKCJLUbeNcxsrMGtzLISqsciNcZOPXisPUriZo5EstoVTuEpjGW9R144rW1Jtv7wMZbaFjCBI2SWIwT9MGufuhGJjIyyeTgJEsQIAIOSevfpSH0IZY3jWPbsKsMsT97PsO1Z8w3XDxuZGwMhlTGPwq1dTKvnZikhkcjLdQPSq0Nw0SMRMcbSCxXnkYrORSK0kP2coGULEQGB3csO4x2pY/Ms7iTFuShHmAscjaehqCVwWhVnLjbwMc/nU0s07tOuWO2IZA5wvp71DNCszGCJGZzgbhhRjqc1hX0bSyMQ7Y9632x9giAP7wDeCR1HTNYt5uw7sOnpQFkVbWQxyDAwwPWpJcDOU5J3Fs81EkbbUcEhm5x6cVK0m7Cqdxxk5XGKloCKSQFSADmqjSbe1WJN28qcADvUDqFUtuzjtimiSvI3mKRjFVW/iX071YZepzUBGd7ZpkSIZJCuPaoGk3tjGKlkGar+XubriqRhIbIoOeah9qmZOGbd07YqA9a1iYN6i4xzUbLuzzT2bjpUW7nAqzNsa3yVHLytOds1E2StMzlqxq9aazAcilY4FQNzVoykPaTcMYpN2aj3c0h+YYqibhK3UYqGpfVf1qJvloJZHITtOOtVSCzYJq03QmoJMc4qkQQKfmxjiiRdqls09UC5JNIzBlORkUwI1kUdVwfXNRPhwQDintjBBGfT2pCEXv24pohkDqVUndmqMmVbrnNX5MlSKz7hvnFMgikXLB/TtRw3U7fehmyppmP3Z+hoA7D4ZNGuvyrLyWX5Wz04r2MBxhdoK4+9uzn8MV478L4UOtMsq73Zc+uMA17Iv3egAHGMVnLcqOw0jFGadTGG3mpNBaKSlqQEphGRUlN21aAj27ec0jcqakZflNRZpoZG3qKPvLinFeKb70AI0e1c5pmakPzCkaPbnmmA1ac5+Q01aew+U80iGtSOlIo27V60tIl6DajbpUhWkK7gfWqRSIqVhgUpTAzmmsTg1RQxj8tNp+3cOtIycHmgiSI2XcKQrtzzT6RvumkSRleKTbkHmnfw0lAhNu1etMK1I33KZQM51V2nrT+lIFpTQNgo3MBSheRQowwpV60FR2HAYoooqWMcv3hTv4qYvWnr1pCHUin5qXG7il27T1oGA+9QB3pQMUjUDAdacv3qRVyRzTtuD1oAWiiigAoooVdx61SH0FXrTl60gXkc09VyetINhy/eFSL1poTBzmnDrTAUmnUmKKQgpQfmFJQv3utCAkWjb70L1py9aZQ4cUUUn3jTAB1rk/HjebpoUgffrrSmB1rjfGp22a5OTv+7SJlscrYgRtGOmONx59uldTpUbYGWyWOBxiuaj2b4xncSenSur05vLhTK85yGz0pVApbl3y2WYIRxgnd+FNT5yOMA96me4HzN2x3FNi2tEOcEmuR7nqxFHBAxmrUPySKeo9vpVdTtYjGcd6nt/l+bqazepqmX48NGeSqpyRjr7Z7VoptMcjSMd0fHA6ZGP61StV8zfEcYYYzjpV5kCqo/izknHXA4GKuOwA3mKsSggx45Y9fUGpEkmZiUHODn5MjGPXNIGMiFmUJt4IJz9KdCw2kKzCToVzxitUSTW8byLCF+7nk5wDxWjIq3FxYKXa2RpNk0iH5cepqK1jMduIsAjO4KT6HJrSMltJcogYCJhudSDhTjj680AddNpq6XeSw2BMtoqgrM3c9jntzT47dvLhEs0kZZixjDgjp1PFUIZEtwpnuC9oy7SqcnPY/nir+nRNxE2JGOSJC2CBjsKRrE3rFLa1hEEyIQwLiboQccDP1q6t1NMrl4P3jQhSxXAGOQc96y7fHlugw+0KPLYZ3YIyQe1Xbe7ELOI7prWNjkvcAlf93254pGqYlx58n2SSdoliC/wjlvQEVAUEz3DFtrKhIXYT0GcZzWrdSQ6ha2u3VYbedQ0g+XKr7Zqot42oW62kk6uHJDup2lgORgY9qBmfdLa2kyyzRyCQxYJb/VnIOBj1z3rm5JmvI9yZ8qMkCNSQeO4rb1C8jkS43yTJGrbQu3ccKDj68is231RVUCWGYgxgqwGBnOKBNGfeyKskMUMzqsqbnklGQD1xis7dukCh1dmyABkDpUkrF3kluGKoW2xxKckU6K2F5IkKyNFH3Zhx61nIpFEM8LqDtMmMBuw55NWEvHjkuRAULMgRmY9cnn6U2RltZTCU3nJAfqOmc1DK0McflyL5eerbc59KzNEiCSFre1VVDySqcblOQV64xWfcrJcfKARlCTirzTyW6q0cu0Mu1W9fU4qnNiHDxMRI6lSzHI+uKAKtw0WzNsGUrEFO4+4yaS4kEcaMSpcDGBx3p8m2OzjCEOWO18cH1zVcxx/fYEFfegkZIxZi27Of4ahnZWVgq5AxzUkkuVLLH09/wAKjOFMYCkg8n34oJK2Q7bAeveq5UqGyau7RDnKde+elVd6KTu5FUjORAYi/IqpKNrYz81XJphGV2n73aqjYfJIwRTMpMhkJQEdc1XZuasTc1VlG04JxnmricshkjhlKjjNC/L3zUEhC85zSecK0RlcfIx3cCmFyRyB+dNZww5puAOgrRbENjWkHQ9Ki8wc45NPZS3Q4NRupXq2R9KozkITmlVuabRQQKT3qNvmp3QGm0CGN3FV3+9Vllz3qAoWJNUhMhk3YIAzUSqyqSRxVrIX3PrUczblpgQbSckUw48tSR365qTsRUPC4BHT3pohkMjHd0+WqMw35NXpmwrYqixyppkEWM9eaG/dgcjp34oNLJ90cA8Hg0wOy+E5aPxBMYvusnJIyBwa9fDHHPJ9RXmHwdsisl1OecjGAelepFQazkNDaRqesfvSNHhc5rNmi2IwKcRSUq0DEpKUjFFACEZFQsm0ZzzU9MaPcuKYEJ6U2pWi2qeajIq9wG9KG+6aU0h+YUIZGKkz8tNKYGc0KaABvumkWn7dynmmbNq5zU9TNit0pop1IRTQhGXIPNRumFPNS/w1G3zJTLjsRUN900u33oK9qpDI6G+6af5dMblSKTIkRrSFeKdt285oPSggNu5ajKnNSL92m00WjnKVetGKAMsOaRI4feFC9aNuCOadikaLQT+KnAZNN7inr96kAu3BHNOAxSDrSmkIVT+8FL1amL1py9aBodRRSgZNAxV+9S0m3aetLQAUUvQUlACihetIvJHNOC8jmmMVetSL94U1VyetSKmCOaYDl60oFKBQaQCfxUtAGKUDJpCExkilCYOc0u3DdaWgpCr1py9aQDFLVIBWoX7wpACWxTsFeaAHMehrivHULiQMoyuc49K7Pdu61h+LIfM02Qhct2/MUImWx51bIWlz0IPBrt9KVvKTkHj0rj7FXBRtuQjcjpmuw07P2fdnaccUqhVFFyT542QkZ9hQuMIgG0imWw3x7z1qx5YXDVxy3PUWwmzrz1qaJcAZNRZPpVqBeh7dP/r1JRfs1z+8JwScAY/Wr6SAOp6lefWoIkRY0cDlTtK+vvVtV2qHAAOcc8j61aGK0fmb3b5lL7iRxnsBjtzVqJH3gRqpdfvqRwR9aktUFsdwbIcgIyEZGTzxVlbeSG4cPDujVgFm25YcjvWiJehPtkkm+TK+UASQmM5OMZz71buGZZmLQtIu1V6ADqO1VrVz58uXmZlYkFVKjGOa0fLW6t0KwROZHUJIzkScEE8VSVgTvsXLDYrFY54o2x9yVTk+uK0bKKNQZXViqd+qjPr+dJbxFnlW4I4+WMHGGq7bDybGSEqfMdxmGQbQMEEHPfpUyNIonSZfLjeWNVcH5WUEE8VppdG8u4WG1EQBxDGwZj+mKp3k92yCTMPyjCshwVHQ8Y544rR0FbX9/vtJ7mR4uJIyBtNSbxTKlxdNsKoRLISQTJCOAT6ZoiaNoxCIzIQCfOLhccdhg4qzFEi6hMtsirK0HzyXAKn8B0qpHFHHxcTqDjDeWu48HkgZqS0mVr63+7IsilUXJAbJ5GKxYfNuoHjjZpEzlhnGADmrFxtkWd4VKKr/ACndh2XOM7ccVXjkbT45RGZVZ8AZIYdQCTSFZmW1vujmk8vy0MnDO2T16020aO48wyzqkXIC5yW4yMCtC+WKaSNmuPMSPgqo24980y3j+zxvM3lXO05jjZcAZ4wfXrUMFuZflm4jKiFjIwwgVhjjvn6CqV5HPhFCsSSM7gCAM5PfmtO4tvMuHQIsZ27iFJGPYVkzQsS4jQ5b+LeeMf8A6qk2Kl43ntKFb5IwAPkxg5x60xEJ8o7g20kbT13dxiprpRaTKeSVj8whuhb+vPNRXU37xJgyh3TfIyr/ABUCKsjqjEFFXL8KPeqzMZLx4sfdODzxjFP2veTIwYKAcknpTY4Q07kkbM54OSDj170E7iquchT9eOKjcvtILD8qmVwq4Hyqxxjrmq80gVmUc+9IRW84zEhhjFQMq8kjAq0wHmYFV5lEZdSc1ZlJFaZQJBgZC9/WqLZ3cVbkyxUA9D+dQXEZhZaZzvcj2soLEZxziq10D5i/LwVz1qw0jGNuaqXMhYg5+6MVpHYwmVJOhOzGPeoc+1SSMfXOaj3L0zzVnIxaM0UzzOQKtEitIF7VHI25TSsN3SmsvXmtCWJRQq09l7ikIjb7pqPNSEZFNKYGc0AHSmsQEIxyaM8UhqhEDIW9qiMe1sk5q7sBWoJo+ppisRHC84qrJGfM4NWfUVXkYhcimTLzKV0wXIz7VUkUqvHINT3BLNllqKZvl67aZmQ8MDzg+lNmYDANSxqrKxzz2qGRBKoJ6HjFAHq3whsXj02WcPlGbBWvQ64j4SbW8OSY7S4ruNtZS3NI7CClk+4aCKRuVxUlEVFO8ugpgZzQAUhFC0rdKAGGkLUrfdNMWgAcnaaiqUjIpnl7R1pxYDCvFJTyvFMqrjQhGRTdu3nNPpG+6aYDaD8y4oFFIhrUULtXrSN0p3UYoZetInVDFpm3g0/3ppqkWiInBxSN605l560lUhiMcA1H3qTbnvTdvHWkQ0Iy5B5pjL8pp5PFNb7tBIz+GjbTsU3dQI5z+KhetHQUL96g0iOXrTqavWnVIwVdzdaft296RfvCnfxUhAvWlxuOKAMUKfmoANuGHNPAxTR1p1BQn8VPX7wpop4XvmgApV60lL0oAGpKKAu5qoYq9acvWk28jmnquT1pAOTrUi9aaqYI5qQDFDEFJ/FSmmr1pAOpy/epAMml2+9AC0o60lL0oKEpSM8A4pKgupxCqjOC3G7OMUXsNK4j3iwkFpAB70Q6lHO+0SoSeg3dawrzdJyeQOfUGsO+jIxKgKMOm04o5kU4NHofGOvX05qnq0Ya1bPPymuG03xpcaZcLFc/vIc4OTyK2te8b2cS+Vb4nLx53bsYz7YqjNvQ5yNh9uWJeA3JXFdhDHmNIxxxya4zRbr7ZfK2Pb9M12tuxUfdySKzka0NVoP2BY9o7VKrbsDFIqnrSBcTYz0rme56CJApY4AzWna2TlFZhgNwfbiqcMJZlrftUCxlyMjH3ahs3ighhXbj/Zxn+tbGn7UkRvmYKp+VcA9Khs4Ul24XGTj9a1bXSTMD8rAMMoSvDc45OeKnmN1TG2NifOLmNUHDNMybiOfTPFaM2kyxkOZJeW3sq917EfjWrpHhjyYTNcbYsgKT5hPGRnj6VryaSohhlCPcRmTZGI/mwoGenGelOMynRucpDHMu9gZWR2IKNjjir+l28M0wj8yMEhiWcbAvB4z29K1rfSRcSFjCIVZyFYHkcc8dqrf2eTIwjVli37OY87ucZzniulTTRz+xlEjjikmZ+YyqrgKHy2exHHNaDoESM/aQsoj+dplLA+3tViHRxYwsNu+eRtiLPyo7k5HTirVrapb283nXOHA2hUHy/WplJXKimhLFbpTaNDHC0igkHqCMYPH0ra0yz2tcWk8MUzXp/dTKfLMPf15zjFVbEra3C5C3MohOxnXGMggjHfg1HI0cd3FFLZss86hYGjJwDnLH/vkGo5kapNktwogmkN3MMW+IjGHGCM8HOOeayNUaN5DHlYY3BIMYyeOcZ49MVcuIYbuF+FkKnoxwVIPJ96pzWpkjEcG35wSuOegyee3ApcyLWhiXl1FJIYY/L894iGVj82AMgAfUVHD52mtbsqojMu8nOT9KvHSYVuo7mNVmdk2l8YIOMY/pVZoUgW5V0YMqg7n5CnPQCpbT2Ap6krszqW/1g8w7effGKhhUXkIClhEpG4rHyOeO9Syea0wbfyUwCqcjt61oaWIrG1JWYfaDwcDcozxkn8akmzuYMWxbqQNGZGdiNxfHGDjjFZ91CYY2V51SNmBAUZPUHrWjLDJa3Fy6jz5gMZXoPU1m7XwGyhTP8QyW7Yx2oLK+oS/bJsMyiOMY3dz7Yqrb+UwmDgsvQHsOa0ZEZriP92qsAcgjOBg1lyR+ZGSucg87eB19KCbO5Xu2hgVo4pAcNgZGM02zDM44VYsHcByTxxz9aWKwVWG75juzkj2q2uIWC7FI9qCuVrUqPGrRqMbmY8e1VZ49sjZXn1/Grk0m5jsTBB9aYzhZPm5LD/69AjPlU+cVHOQKp3KlXJPAb9K0Jo5AzNtID9z271VkjLXCxEjkdTVIymZzA4LKTge</t>
-  </si>
-  <si>
-    <t>1Rzb5iCX6dqsSE5aPPU46VA3ysVqjl1IJfkUiqc2MHng1ambOVqlcN2FaROeZAVyflbB9xUXO6nyM+MZUe9QxsecsrfQ1Zyu5JUTJtbdmpN1IzHHFWiGRlt3rS7TIcDqaNwA5bn0Aojk+cdc1QrChMNgnmlkXCHmlY85I5pGbcpFUhWsRUhGRTiMDNI3y4qQGMm3PNNqQjIpBH70wEXikkXcp4p23nGacybe9MRnTxmMq45znjpVWb5VxnnrwM1pzYCj2rJmxuYn9OKZEihNndhsgn1FROwzirA+eYbtx/Gqk3ysCB3x+nWmjMeuCeB2pm07Qo5OaSN/mxVqzhF1cxJkDLAc/WqA9i+HtibPQoSBjdyR+HWutrO0e3S1sYYl6qo6dDxWjWUjUKY3y4p9I1QMbSN900qjtSsuQeaAIaX+Gl8ulK7c80AMqPFPbim0AKR3ppGRT1pCMUARsvHWoyKlf7tRt0q1sAlNIyKWlIpobGbdtI3SnN90009KAFWlbpSKOaVulJmchrdKbTm6UYpoa2IWprdKkaP3ppj4PNMoZ/DTW+7T9uOKRkLA0DGdjTW+7T9u2kZcg80Gctxn8NMqUL8pGaj20EHPYywoC7e9C/epf4hUlrYUDFHcUUKu5utIYq/ep69aTbtxzTgMUALjPFG3bjmgfeFL/ABUDFAxR6UUBdzdaBigZNP8AakC7TnNFACdxS0ncUtUgQUqnaaTHzU7ZQPqKvPNSL94U1F6LmpAm09aAHL1p1NXrTqQCNSgYpo608DJpCEH3hT6TbhutLQUhRSUvSkoAKxfEe77OMVtoMsBWfrUYe3+lJmkdzmdKvpF3RyHKk4yeoq5qFi7Q4RfcEVSaIeYMHHOeldDp7NcQhTyQMCsOp3ct0ee6lp7ZLldw6Vzl3IqMR/FgL+teg+NWj02Dyx99+emCOa81jxd3wLEAZOSa6Y7HBUSTO58IW67Qe45rsU+6MVz3heFUtiwI9q6SGMFsA1lLc0oqw9WIXk5pV+aVmJwKPLzJ14qW2g8xQpPQ9cdawlodvU09Pg3sBjj1rajhwpAGcdumeazbNvJU4GQcVrwkeWzf3vSsJO7O6lG5saPZnzABEr85wx4NdVpdjGZIx5WfJDfKv6muSs9Shs2QF2KryzD6elaOm+JBcXQSM+WGJKhs4JUE8nt0rO1zvjKMFqelaXp6qBIfmm427WAAVjjJ9Dz0o1C2trSWOOaOchpdoA5A985z7dKreCNal1G+Vrq1Cw7gytCMDPQnPp7V1+uahpkc2UgjNwXCLKeWTnlsZ544xVqLSCVSMtUc5c6aYVtx5OyLzThITkDg4JNRjTn8zzJyYneThWyAcc9K6oCK+aHiF23EZBIRsAnLL26evWtTVNLh0vS4WiuRced85KjIQ9xntT5rE2vscg2jrLCAu1bkvuACk4yMYzTIbOFWImdgCQg3jgsOTkfQV0cMk9xC7Z+WMgpHxnqOSae1qlzIsTou+UksSucNj72KXMuovZ3OZZzqF84mQ20UD+WJFi4K4JznPHpULSGaRIrSfASUkK/JwOTz24Fb1xp7TWl0TK4aQb/MUYVth6Y7dM1zlvcLb3AldGnMww2SADz1xVXTItYrbT9qYWyBkckOxGQMnNRTW8trN5cE0bRqN0i4wR7A5qw+3/SLmJhFAXKrGGB981mfa5Jo5MqoXBCkDLfn3pDt3IpL62azkgSGRpXbKFeAhzwc96pywteRTKFaa4hQeYNwGTkDOO9JGzoElZBAsZOY2bO4kED6cmrFvb/LIsyRo7ISWViCMjB+vFBFijf5tLhowNu2MBXVgS2RyMdqkuFGnCNQqeXLCvydADkZJPf1qlcGC2md4CskYxhzkscDBHWotUuixWMRttaPcCRn8KNgsynq1wtqk4t1bcQFeQNgHnr0qta2/wBqt4io2qp5LcnNabWMclqZriYYWPOwDBJzxxSwwia3t8/KpOcAYxijmRpGDMWZ2bc65wp27iMbqqMVOEUYPU+9dFqVtH9jimO1UkciMDr05JrGW3iXzDnLDkHb1zRzIlxaZVFu0ke4Db70TQxKytArEBMuTzW1HGGgiVFw7hu3TANZLSneY0G0nhsjI496d0aSWhmRqZVDIOTnPtxUfkI8iq7H5hncOx9K1ZoNsDbemVzjg9RVJoR5RCthVkGeOaZyle6RdsYBYMucqTms24UNcZAPTHH51sTsjMCPvfdJ65qswV22kHB67Rg0yZamK0TBX6jnOCKqSRnczelbNzCnmfKGQAfxGs90BUgEEn0rWOxyy0MidTyapTKCcluK1pUzkFaqSW4P8P51ZySRmPGuCVOT6daaseO35CtA2vHRfwFIbc46U7mbTKBTFG2rzWrcComtz0zVJozcWVvLVeQOfWg5x1FTtCRxUTIRTuKxGfumm1I0e5TUYj3KfarT0IYjrxTT82KV+SFpOAcZqiXoFFFFSAjcc0GTcp4ob7ppi80wI5+Yyax7oEFh61tSfKtZV6vyFu4q0RLYz4z1wMmoJGEilSMHdmnqx+bHFQSsM8D8aZihpUhuK1PDdj/aWsQWwJGSGOBnFUIsEZNeh/CfRjLqU9/JGNqDAB/nQHU9Nt7dbeFUXnA25NSqKd/iTSVnLc6BdtIy8ZpwoIyKlgRU6kK4oWkICMU1vumnt0phGRQAxvu0wipCmB1ptADKcelIRilWgBhGRTGX5TzUpFN28YpxAh20e1SmPAzmotvzZzVDBlyDzTNuB1qRulNpghlO6rSsmATmkz3pENBt4prdKf2pntQKzE/hprH5adj5TTduRjNMqJEeuaX1ocYpKpDEb7ppop7jCmo1pMhiZ6im0p7mkoJObX71O/ioC4pQMVBQU5fvCm+lOX71A+o7+KnAZpo605etAw2/NnNA606kAoGLTl+8Kb6U5fvCgB7U2lakDUALjApBSk5o6VQwX5jT1pi9akVcnrQwQ+P71PXrTVXb3py9aQhQKXuKKQfepAKBinL96m0q9aAHUo60lFBSCiilXrQAoXnrUF5D50ezqTgD86sUKy/aYTJ8ib1y3XHIqZbGkNzmr6xazYhkwc4+lTaO7JIjH7obmr/iq9ivNWuBbjKhsAdM+9ZtxOLHQ57gq2PujjB69a5r6noxi7HCfEbXzqmrTE4VY22Jj9TWDo+k3At472SFvs7ttViOC3p+XNTXFr/al15J3ebKcbtucbjjOM++a734iGw09NL0vSmYW8Ko8pzwZNuDx+Oa7I7Hm1U22yTRY/KgjwihSOcVuKRHtIGSaw9Jk3RIuc4FbqqJFXnBHRfWspbm9LYeSSMgc1f0+3JyM89eaoRuF69RV+zlWTHbmueR6EbXNCNdqgE5foFq/HOLdQznvzjms0ybrpgrYjUfXmp+I7hQCnTJaR8AH06Vz8rudkbRRa/tIedIUUgLjnueasJ4kt4WMVwrozDEasMp75NUVug0ipbxRzXO7G3JKn9K3LjUbhY0tbnTLVJCMsoTPHY7q0jFmU6i6Hf+A/GUFlpzwyW8RVgAiq3OQc9a6CUWWvTGaKwa1uFOfMlukRRz1znJz6Yrxq1s2kkU7GjibJYQsCRwe1Um+xWMxkjknkjY8xyyDenvnt9MV0qKaOSVRo94h8cJoN4ySiLK8F4Ruz/jWqPGkGqRg3M7RiPc6wou1enQjvXzd/wlLxlxbM0gXG2ZsDHtjvTZPiFcnAeQGYdSW4PtjFcsqDbujqji1FWZ9Ix+LbdVCxdGTdlTkj2xVJvEUvnbmykvVEDcsO/OOOK8MtfiFNHbtI8qDPG1SARz2Nb+i/EKC6UB7gE/7uT+dZulKJ2QxUJdT0C41iaaMwC6a1iCOCpO4nPI57UzS1FqzNdzAlbcCEtyMk4Jx9DXL/2xa3B3szMPbvVuG+hmt4t7GXcCBu4xwe3eod0aRsy2k1vFCGnVYsOQrKSQPciopNQiknWKPftByHVcg++e1V1u3hLJEiYZcBXXcPrVNo5YYSJpTGz/AHlj6CkpdzXlL8l1FJaLFI4lVZi7v0JHYD8ap3kwF4rRv5ikFtzEgEYwRUEzA26RQO0MKgDIXc2c8nNRXhhchczNlcAMcDjnNWpol076le8ukGZGXy4/+WMSDJPrz24qrHdS3jRhmdeoGcZxjpTlszeMxcAbQcAtxV+3tbWS3RmRIxGcM2cEdhzRzImMSZvJZYlZAWYBVYtk9eSR2rUgVPspwQzKcKpX8M1Hp9vbq8qRLvIGXlYce2KtWcL3LMY42k2jGxFyT71NzVHP6kxmuQmPmUYCheB6mqqxmZsJtCIeZDxmrepSzQ6kVI8uRlIKMMkEggCqyMrW8Nuy4aI5nbPVuwx9afNYlq4up5jCKHX22mqAt2aRlAKh1PJOexNaE6xyLCX2DLFRHnrx1z2qtNG0LMgmDDB+VRkihWIkijdBdqSIAqqihwT3yOaoTbt+51JBOQw4Fa+0WzOZovMkaPKDsMc9KbDp7XEa3Eo2rjOwHgdq0TOZxZhLhW465yOKWRS3mLkjb3Uc9a3Dpqsu9UAUEc5pt1apbsmMFj1OKfMhcjOeubVvs7bSW46t259KoPDt8sBR37e1dM8cXIcZDd+lU5LGJZGC87eQ3r+FHOkZypNnOta7s84/ClWyDfL698VpSQqrEevem8BsA0e0I9iZbWXYcn6VEbM5wV4rWICkjue9Rd+uafPcl0kZrW/I4qnJBiYHt6VtSqF5xVG4XDbq1jLuc06fYzp4eMYqhKPmxj8a1ZpA3OKzpiN+cVsjkktSu/AqP7uamkXjOars3VcVaMmRsMnrioTlZBUz9KZtqyJDhRTVp4GaZAhBfimY2NUv3eajkHU0hkUh+XFZl4wEbVoTfdNZN4w2tzVESM/zAqn5c7vfpVfjPLYzTbq5ESdM/jVATPJOvyYB6c5qkYI2Yo8sqKd27uBXtPw/0uSw0lWZSGk59K8y8JaSLy/ggYjcx4LDjgEn9BXtpnt9NslM8qw28a8uwxSZXmWcnODwO57U5vqv4GvPde+LUEczQaXH5+3gyE/L+IxWLH8RtZlk3F4gM/d2dKho2ueuLjb1GfSlrkvDPjJNSYQXIVJz0I+lddxtDZzQAw0m2loqShSvBphGKdSN0oJI3+6aZUjDcMUzbtXrQAlJ0paKACmkYp1I3SgBp+6ahbpU3tTHjwp5pgMpCMUoobpV7jGn7pplP9qGTGeaEAimhk75pKczfKaTExjdKbTm6VGT8tNAI67hnNNIxUhGRTGXC9aYxrruU1GV+U81IehprZ2mgQ0LwaaV5p46U2giRzlFJ/FThUD6iUq9aAMmnbcEc0AKvWnA/MKQDFAP7wUDHfxClpP4qdQMTbubrUgXac5pq/eFPbpQAxqRetK1AXmmgHL1o+81KF96ULg5zVDDbtYc1IvJzUdTqm1c1ICr1pQKRetOoEFIBR/FS0gFAyaXbz1pF606gAooooKCnYpF604UwFX7wqK8/wBSxzgjp+dSquCOaSZN0bDtjJ+neplsVH4jF1aya1aOR+Iyu926Z9a9g8M/AvTNS8CreeJI7l7i7QSwQRy7PLQ/dYnBySO2Biqnw58Bn4leM/DmmsiCx8uW5nZskFIlLYPsxXHtXc+Mvjd4MsdUudIOs+XJbOVfZbsUXAwEB9BXxucYnExapYZan3+TYWhO88Q7I+ePGXgfRfBfi6BdMWRU8pQUkfd35Oa4D4jXcS+II4rdQsCjP3ud2OTXZeP/ABBHqnjK4uom823x+7KnggqcH2ryfXrt7q4MjE5JwM88V9BlzqSoRdXc+azaNKFZxpbHXeHbosoOe1dXa3Q25PHvXmvh/UPJ2hgSOmR1ruLSYFE4zu6Kxx+td8jy6RrecMHAyfyp1tMzKxPy4qpIwhUEsFyccEGkEhV1CNuU9QuCfyrCSZ2c2p0NjdAPGxRnOedvJo/sue+vn3KIoiSRucDHGRxWXFdCPLyKQmMY3YIpkVzbecjsZSVP3lJJ6Y6VPKzX2itudda2lxHNE0V5GFXAeTA498Z5rtbq30ziOTUldCiky7cZ55Gc15bHqFkk6M0FyEHVuQOnpiuktPFVvbSA29p5qqmAsigg1oZqRo61oE2iqt3p7/aYJvuMXJH4jtXN33ijTJibXVbSP7Zt4uLaMqT2AIz+ua27vxNC1vk3D2yMMNCV3L7YFcLr0tleTLMAGYDjBIzjoauLIn5FW6tY4/M8gyCDs8fJVs8gjNZsdy6sYpNvzdGYZNQ32utlgIPKQDH7s4+boTWfDqELKEmViM5Llufbt61pc5ZGjLNFHcAuUMbA7WiYkjj07Vd0vVHtWKRsAWGVbv8AlWBLDbzRySKy7yOqfL+lNWRj5ZzwBjPf86G1Yi7vdHeaZ46ntZGimnHH8TLgCtyx8fKJI2lY+Ux4ftXlEjYkyMvxyrHOa1rdori1WByVB6AdARXNOKZ1U604vU990vxLZ3kKMjb8jpuxVuGUStOxb5DjOfmOM14Bo2pTaZIVEzAA8LXo3h3xO8mNzYyO/I6VxSptHt0cSpL3md/DMrKQGWNe7NxioL6P7SypFIG3dGHQgdaxINagkfG9ZPUEcVftZ0kxnhSTtjHAH41jsd0ZJoSC1EjMCWaMuETb1Y5/StT7EliGEiBixwqk5HqTiqlnG1reR+VJh2fd93OBj0qxNJ50z7t7nf8A6zGAOOoqkyUjVhcyWOHaKONuECH5vxq7outHQpEnj+UY2BhyTxz9K5tJgluV2gbm5bOScHg+1WiwjSFY28wM++QKuScdhT3GYep30moeIp7pSYyzE7257HjFNt7hVuhIp3ljyGGAW9feo9YvG864YW5hQyfKoOSKyv7QO5FILOpycrgD60pCvY6Kd41injlVN+4EBeSOc9aznvUE8rBOGGFA6j8arLeM0bKqgMxJZupPtUC3DRt7g9xST5SZGpbtEtwAGZmCYO7oKknu0kYIo2nAX73H5VnC8YBQcAk5ZvXjgVWmujHMG3U+ck3op44bcuU3HO3O6sy/vNxLbTgVRl1hI4CpfkHPWsq61pypKsB+tGrE5Rjuak10rHBOBjNUJdS3RnBxngnNYs2sA53Pudv0rOk1ZEUpnLdqtQkznnVj0ZryXx37mbIFC3PO4c+1c9/bAQt93I7lqi/t6MtlmVSD2NbKnLsckq8b7nUzTbVGO9NW6XgGuYk8URfKd44qrL4gDEYcEGqVORjLEx6HXy3StgHAHrmqN1cxiNvmrlZNeO7rkfWo5NV8xTg/rW8ab6nPLEJm1NeAZ7/jVeSTf2xWR/aBPBqSK43MMEk+lbcvY5nO5ofWopMdutRNMzDAGT9aXnYSRVJECNQvWjO44xSN8tUJikjHSmhqaXGKYZcHFBJPvppwQaj8wFSKjaYJ1pkiTPtU8Zrn72TcWJOAK1bq6C5+lc1fz7t6g8npVES2Kc0nnSEdq3vD+lmZlnlGUH3eOvGKztH02S+ukTpz83GQK7C+uodF01nAwsfyoD396RrSpq3NIteG72x0jXJ7q7kXyLOPzCO5LAqF/Miud8SeMb/xlemWVmS1U4jiU4AHqfWuaTztRnaWR/mduT0yueK3LPT/AJg3zY6BewoMNdbElnblY8AYDdcCtK3tH28x5HXGas2tmPL/AKYqvrOqiyXbGcyY4ANBcdC/az/ZLqIqw37hjHB6817JasWhjY91HFeA+Fln1XWLaMMXZmBIx0r3+3Qopj6+X8u714qWPcdRTvL96PL96ljG0rL15pWXuKb/AAmgBpGKjbvUjfdNRmgQ2inBKCmBnNADfWiilIoAYRihuVNK3Smn7poAiIxRTm6Um33qkAwjFDfdNObjjNN+8tND6DOxo6jFP2bc803btxQRIRo8KeaiK/Kamb7ppijJoQREprfdNSbNoPNMb5hTKIyvFDLkHmjPOKGYLxVIBNvymoqm6qajwKT3M5HM/wAVLRiioKHL94U7+Kmr94U4daAHCgLhs5pV9aWgYBeaXpQvWlxlsUDBfvCnNQEwc5pGNAAOtKvWmhuacvWqQDh1FOpo+8Kd6UD6jo1yetTH0qKP71SfxVImAFOFJS9KAGgd6cBk0lKp+agBduDS0Uq9aCgpKKVetACgYpV60UL94UAOokyyhRxuIUn2J5oo55xw2Dg9cccGk9gueg/DDx3B4H0HXr5ibe+WxltLWZmIUNI6gj2wpJ96+YdSF1eXdxFatJqNw5aR5rdGcsxPWuv8dXU8FrHaJNIkE0vmMob2wR+dejfDuSCx0WFUQRgLjKYVifrjNZUsLGUnOR21MbJU1Ti7Hm9p8P8AxPrTJPFo9w5eBceaNmOOeTgVIf2d/FOqKodbCwAPLXF0OPrgE17ZNfnzAxZimOrOxx+Gaz7rxALVCxdQp5JwB+vWvRjQjCJ5dStKerOA0f8AZc1GNlN14o0229diu+P5V22l/s42NmqNd+NvmU53W9l0+hZ8VkXXxKRZGjt5JbgL97yQSFHU5Oa+ivg9+yn4s+MHgLR/F1z4nsfD2m6pCZoIfKaeYqCR03AVUYwZK53qjyWT4IeFGUC58WanJg5JjSNCf6VLH8H/AIfxqFk1TW7lvT7TGAfwC5r6Xh/YLiaFftHxK1Yswzm1tFQfqTVyH/gn74bkG688d+KZcckrJFGP/QKPZxL55dz5f/4VP8NlbLDU5yP4WveT+G2kb4b/AAySPizvi3/X9jH/AI7kV7Z8V/2Sfh18K/AuteJ9a8WeJ/7P06BmIkvEHmzEgRxr8mSSzDNfCVp4ziulMxtJlVjlRNcFm29snAyazaih3cup7vN4B+Ha/dt7xR6fbSazrrwT4MXHkyahFjutxz/KvHpPF9tFIpFruz/01PFNk8bwru/4l7fL38xhn6cVk5QRfLPuenXHgLw1ImF1G+HpmQk/nisa8+HVk0RWHWZ9o5AlQEfnmvPLr4h/Z1H/ABLmiZujGduP0xWS/wATrnepQTJk44Yt/Tmq91kc0o6M7HVPhvefMLfVoXX+6Rgn9a5q88D61ADtaGZR2VuT+FVv+FkXqsVmifI5O4VZh+I3mYUqFJ9Vx+tO0SeZmRcaTqtixMlpLherAcDtSR6hJAoWVHUj1FdEvjhWwCyn2J4pG1ayvMmVUJPoKzlFdB87MWHUvMcMowRkYP0qVdQljwp5H97pirT2dhcHKgjPdTjFMk0iEjKSsD23Hip5ClUZDb6sPOGTk5+9muu0zXhCmwkYx97NcS+jyRtkEOAf4etWI5/IyHVgfccVlOm2dFKrZnpOn6mu8SI2AOTznNdxouthcOwDn+6eBXjGmawkSgBhz6tzXY6TrSAJvkxk1wyp2PZo4hbXPW7e+IWSQKGaQfKVHK+v14qWHUC0bLDFINq4VXHQ9znvXOaRrVsqqWZiFHG3v269q3rUJdAStNwD/qs5zWXs0en7RdGW9OhFuA7KHkYEbWPfHXFSXGoSpJBDFC0ZXJlmK7QOOBmo/O8m6j/dxBCcjaDn86i17UozHI4kZi3LKensCKnlsaKSaMPW2kjkKGRWWRtxKncazJ5oBIyLksB80nr+FUr7UEWQyJk+ozwKxpNaDOU29euDUtEuSOhGoR2vzBgxx0PFZV1rBdywPy988Vg3OqLvI+b8Kyb/AFhl4d1x2VTg1UYORzzrxitzqJvEAIKg8j3qjLrxkcKGIb3NchJqi8srkN7c1GdSdl+60h7YGDXTGgzzp4uK2Z0l/qv2dN0hyPZvfFZ8usN5e5TgH1Nc2zXc0vKO+egYYxQ9veMQXXAHTngV1xoLqefUxcmaF5rjCQhTlm6e1Z11qkqgtyW/KoWt5FBJUZ7NnpVeWKV+rDFdHs0jklWcupC+oTSyHLEBqZGwYnczH8ae0O3I4+tM8jYp+fH4U+WxjzN9R6xx5++c+lNN0VbABwO4NMXy0Ybjk0ySMNnD4B7AUco+Ym+17uoY+5qxDIGXg4NZjQ5BAkP481JGpjx8+6psUpGqrFMNu6dqmjvDuA6e9Zsc275SeKl24I+bBNKxaZrxTH727p2q3HdbsA9KwoZTHwTkVcS54pFpo1/MFQXEw2kiqRvPl6frUT3eQT2+tA+YtedntTWkA5Jqn9sXPrUFxcDkhqBNl1r4cj9c1VuL3qOnvmqEkxGSKpXF1yQrc5HHWq2V2RuWL7UR5ZZSck4G7gfWqdrazXkqsA3zH5dw5NezfC34Ef25pv8AbPiGKRLecYtbcNtJGPve1dL4g+CWnaLYvqGkNOZUH7yGVt+Oe1eNLN8PGr7FPU9+lkmIqU/byWh5dpdgmm2gL/fb7zYxXJ+ItUbVr4qpzDF8qKOh966TxTffZbbyVz5kny+m2uZs7ESSL2GPTPPrXrwfMrnl1/d/don0mxG/cRz2HpXR2tqOFApmnWIWPryO2K0OLdeDlqo5kinqVz9itXAPz447d642ZmmuGZzndwD6VveIpCG59KydNT7RcIMd6CWei/CHRGLT3zoAI/kUn+deqxrhc55PU+tc34F00WuiqRkFjnp1rpgvy4qHuA0dTS0MPmzRSARvumoxUtRsu2gaEZflPNREYqZvu1E3SgQLQRkUlOoAYUwM5pP4ae33TUfY0dACm7evNPIpKAIymBnNJTnPamHpQgGuMnNJT2HQ0yqQ0DdKafumnEZpGXg80+pA0jIo2bec0tDN8hoY0mI3zCmBfehmO2haZRCV2tmh175ob71Bb5TVIQfwmmVIAWB5pu2kRI5Yc0tA4YUoG41AdAXrT160m3b3pR1oGOBwcU7+IVGp+cU/+KgocvWlX71IKVfvCgBzUxqe1M/ipjQoXmnAUL1p1UCEXlqkVdzdaai4Yc1IgO4UmAqrtbOacOtOxSAUhDl60NQvWikAlIv3qU9KRfvCgpEq9aKF60NQAL1oAoXrTqAADJp23bzmkX7wpzUEsF60u2m1Inzc0Acl8QLctZwTD+A8jHuK6PwndhdPiXPGzNVtdsxfafPHjLbcj8DR4UCtp8a8B0GGUnBHPFbUn0MZp7naSXg8oANzivM9e1C41vUprWN2+zQnDbT9729q7r7iMvtwa828O3Ba4uJCud08nU9hkAVrVk4rQKMeeVja0tkt4TE0ShcYKp8ufqe9fR/w2/bW8T+AvBuj+Gxpdrd6dpdt9mi/hO3cTnGK+fbe1WSQPV5dPXcp24HU+9cMajPV9jofXel/t4aNf30Katpcum2pTD3ELsdh9lxzzXsvgb4+eGfH2yLRfEVrOzHBgnlEUh7nAPXAr81b5VVHGxeuVx25/WuZuleGaR7dmtpCOGiYqR75BrZVLnJOGp9F/wDBQr43/wDCb+NLXwDpN4J9A0IefcCN8rNcMuMn1wD0r5NWE3EgHQ9gTgAAdKsPC7SSs7tJLI255GJJbj161ctdPeTB2k89AM1M5Exh7x0Xw38CxeJpnZzHiIksp57V7XofwW0/VtLW8lijYK2zy1Az9c15N8P74eGdcjZ48WsrYkBOMDGK+ufClpZHRw8JU20xzGynODjNeLiqs47H0uDw8JR94+J/jd4PXw5r5ghi/d7QVHSnfA34Gx/GKTxGz6s2lHRrdbjzY1zuywAXOfl64zzXtX7UPw+DWdrrMbkFlKsoXO30Oc14R8OfitrHwkXW4NNhhng1a2EM8cg9CCrZ7/MFNd+Dre0p36njY6h7Gp5HG+O9Fi0HxTd2UF3JdmE7GmlPO7HQDvWD5Ld2LH0qxqF5c6lqNzdz/PPcS+a56DOOgpqKeOMV3nmWK00XzAA7TVuyjlLAq3TvSmISy7dpbFdx4Q8HSXFu0+3IAzg1nKXKaQpuTsct9quLV8Mdyjr2qZNaXID/AC+pzmrfiWxkgumCrgnjbWEsKSBty5I4K0RmmtCqlPldjqrVpZ4g8I81e+3g1Ms2QQwAx1WSsLQb2bT7jy3JWEn1xivR4bKC4t9tzEr7wCjL/PNP2lhRp8y0OT8uPIJRQexWtPSdJtrq3unlmlQxpuyrZH5VDrGjvpzEoN0bc+mKuaBJ++ePJxLFtyOOcVa5ZGcuaDOm8AeE/EHilVXQ761ucHiKaXYxrtLuPxb4FkZdY0cW0bfKJI2Eq9OucDFef/DG+a01QKuAVY8E9SDXpvxE1CW501CZGAAzwxI/Km6KlqXHE1EcrL8VoLdDFM5jZTkkx8mse8+Kti0rt5rFW427a8x8SSFrxm3MSSe9YaMWfO45FZSoxudH16oj0i+8fJNIPJRgmeWJpq6skyh3mYKeTtXmuGjYnaMk5IroUwkIGegojQj1Mp4qpLqaMl/CzfIZGbsxOBUXnQJlvLXPcsc1jTah1VOR0JzVKS8fnLkj0q1CEdjH2lSR0UmqwQqT5acegqu/iRFGFAz6YxXMzXbYOBzVSS6kZucU+a3QlRfVnVt4hkfgED6moJNUmk4Mqhe/Nc15h7mlV93GBilcrlOi8wSDL3Kge3NKkVtIw3Xq/QLn+tYEeQ4wcdelXFkgVAzuxPcZzilzFqKNVrO15P2vjGfu8fzqZtFiK5W43ZXd9z9OtZ9vcQbgqrnPcmug+3RR2oUptyu1WCg5qbs0UYmW3hzdtPnKNy5+7jH61BNoixgYuEOeAcdavz6lA8kfyM21du3PB49e1ZtxNHOwCAIi9F6kUaitEa2juMkSoRUbaXcD7u1/YNzSkFVOH/SqzySq2Fcj6cU9SbRHmxuF6xtkUxxIhG7KkeopP7Suojjc23ud1TJrEm3DKjjvuHP50EOKIPOYH7+fanre44/rUv2mGc/PCoz/ABL2pv2O3mOEbaT03DimLlYC8HrS/aFk+XPWonsGjzja49jUBBQkEbWHSgLtFwMoOc0yRhg4qtuPrT45CrDjNPlYucGz2zk1seDZNP0rxBaXup2LalaRPve1R9hfg7RnBxzg9KoozXQAUAN2q9p22KSMOm4k4POMVE4qUXFnRQklNNn1R4R+Kmm+Nrh7ddOk0u4ChYY94ZNoGcdBg4FddPo8dv4Z1bXL+4WCzt4ZNpZeZDtOBjIxzXzZ4Lglk8RWQiyj7wdyk8DqTj6V63+0B49C/CvTtLgkjMt5KyuqHkIDwx+pFfBvLKdPGrle5+myzKTy9trY+X9SuH1bUJZT/q2csPbOaks02OBjOKbawhFY49Me3FWYWVWzmvvIrlSR+Zyk6knJmjbybVPqasQ4bJbk1mrMPM29AO9XvODAbTjFDFHYxfE67mUjjNVfD1q011EFHO7FXtey8aHvnFbXw60k3GqRsR8iEnp14NNCe565pNsLXT4Ih1VQT2zVylAG3gYAAGKbWbJY00UUq0AJSN9004jFJSAj6qRTWjxnmn7dppG+6abAhIxThSN0paOgCN901GOtSEZFNK7RnNAA3Sm06kIoAYU3c5ppTAzmpPWmt900ANWoyvFPWhl4qgGYprfdNSY4xUbfdNUPqNPSj73Bo/hpV+U0B1I3Xbmkj6inyLuUmmL8tMOpG8eG601qlIzUTL3oEOWkPWlHSkNLqQ1c5ZRinL94U2nL94VIx/cUm3kDNH8VKv3qA6iqm05zTgvzUUq9aChegoX7woahfvCgBzUxetOemr1pj6D1604dRTV604feFUHQevWnr94U1BuYCpAmDnNSxDu4opP4qWkAtJRRQAYzxShMHOaQfeFPoKQq9aD1oFJQAq9acBk0gGKcv3qADb83WnfxUbaF60CF20o+WlAyaNvNIaK9xho3BOBg1gR5jkDo5VxxkdOtdFNEWR8c8HiqUOmL9k84tjknaR/Ws3Jxd0dFOClualheC7tPMJ5HykVw2gw+XJdx91nbn6mtbR70xX9zb7vlBDD6ZrOscw6tqUY+8G8wfQ10SfNA5qcVCpodVaYaIKMBhV2CUzKy9/Wsu1G75Dwduc/0rZtoWUJ5YDBvvCuVM9ndGReA5IxWHfRGNicZrrLqy2/MW5+lY19bhhx27VaOSUdTkprcs+B1Jrf0RArYk4A43VVgtd8xAOTngYrbijFncAuo2kd+h4olqEI+8b+m+A28SW7zQzKpXIb5s444OK2vhz8RrrwRrA0XV2lk09nCAjomD976cUeE7+3s7lJI3CCTCODnHPc12ep+D7LUJFjW0SSaQEuFLH5cHDZ29z2rgqRvoz3abtZxPTfE+h6f4+8MSosq3FnMMRSngE4yMHoTkV8MfEDwJe+F9RmhkiYw7yqyEY3fhX0Fp+veLfhXMkGmBtT0iQ5Om3SF4+h6f3fXNY3jb4gW3ii3NvPoDWcrHMq5yqn2OK5aSlRlpsLERjWVpHzF9nWMZKndnpioWXcwVV5r0zUNFtJNxSJlJOQNtZTaHbKVLBjzyu2vWVc+feEcWc34d0We6vvunk9cZFenwQSaTaxiM7DjHt6VlWl1HYRnyk21FqWsSOuCePrWNSUp6I7KVNU1dmX4ijDbndgXHOcVyqWJmkIjwMn+I8GtTVLxp5Du5FUreZrdtyjcQc+lbwTSOKbUpG5b+E7u80i5lFq0kRcQicEYD+mM5rt/BljHceHbKGRs3DxMGVhkq6t93P05rJ8J/EC2tbEafNodp5bXHmmdSRIGIIznp39K2LW4Sz14tanFuZN4XHAOOeaHc2pJcxJqWk79PuUlBWVVwOOnNcTokhh1CInna209s167rtoBpdxcEZ3jeW6celeNCZIJHkzgK+f1relsc+Mioy0Lula1b+HdcuHuJfKRZGYH69q3fEXxg0vWohZ2vmSuBjdjA9a8X8Vasmp6xIyt8gOdvY13fwl8C3Hie7ieOIlS2Pu8Dit5Tsjhp0/aOxmalZ3V8++OBiDknHWsdYGhkKyKyHPda+rNU+Gceg2rCSFd3ljLKMbe3TvXj3ibw3boxCg9fvHofwrj9srnoywMoxuefwqGkXByOtXby7PlLt4LDHWqyxmGeXIwF96jvGJkjHQDvXZzJo8xx5XYaxKL9etRMSeaXzhIGB4K9Pem5zxWRstiGRs9qryNsy2O9TyDHeq8zBsjpmgbK0kjSSDAxVmFiqgGmYEa9MmtHTbQXUyoRxnkUbII+87F3S9AudTcBAAue/Su70j4aiGPz7mJpYSG3MVxtwCc1oeDLBUdP3e1V5z1r6isfAfgvVvh6sz+IfsurzRtvjkHydOmM15latyux7WHwsZrU+PfCXw21Px540h0DQLQXl5O7bI2bYuxTktnsMZrsPjV8Lbn4ZC0trqC1t5t3lssE/mfNjnnFaPw+8eR/B34qTaxLZSXVskM1sBbvg/MCA4OPXtXO/GTx/8A8J/qsV1FE0FnF8yiQ5ZnPBNdsJcyTPOrR5G4nmMkpWQtyfxqK2idtxJzk06Rh5gA5NaNjGNuDwD3rU5UZ8jGPIJNNEmYw2Oa6aDSUnUMU3Bq2ofB8clqB5fGOuKhySNVBs88EobIPX60NGHyV4Nb+seGV09ZWXgjoce9Yaq3PGMVSkmS047kAYowUirCEkdRTxCJV54P96hYjGwDHimTuWbcNxjj8Kfc2ayL6N2bFPgxgYOavTQgR7t3b0pcyRXLdHOSRGNiDTQMVpanb7JFB6FQ2cVR8ut9zlloyzppKzIc4PP8q0G+eb5eCxwKzrMbefStKzjLTpIeinP+FS5aWLprVSPTfBeoW3h61l1i8zIFTy44xwxboRXJ+MvEVz4nvEuJ1WMKuxYlGABnINU2uHdWBZsE7sA4Ab1xVS4kMYPViRyScmvMWGXtPaPc9mrjJypKkthttEGjyencVFMqQsWz71ZgbNuO1YGsX5jZox1+td55uyFm1AtM23gdODmtCwvTxnnt1rmoGbvzmtzTYyzL82KYjZvIhMsY969L+HOki0sZJyvLnjIxj3rz2xt2mkij5Yk4r2nS7cWtjbxKMBUGeKllFpxuHpUT/LUxprru71LEQ0U5k2jrTaQh9NIpR0obpSAY33aaRkUr/dpB0pgMKYGc0g609vumo6EApGKa33TTz0phGRQA0dKG6Uu3ApKAGjrTHPapCO9NaPPOaAIx1pW6UFMDOaD0oAY1NIyKceopCMVa2Abswuc0hpzfdNMbpTGDfdNR09vu0ymAVGy7geakZaaV4NAr6ibflpNtPx2phB9aATOVpVODSelKvJqCeo/3oX7wpKVfvCgESUq9aaxxT19aCgxk4pwXBzmmr9+n7qAGtzSYxS5+YUVSAVetOXlhSBacq/NnNMZIn3qlqOP71S1Ahv8AFS0gFOXrQAHigDJoPWlX7woANmDnNLStQvWgpB0FC9aGoXrQA6lX7wpAMmnhMHOaBMVqEG5gKRutOUYYUDQ8LtOc0U5ulNqQEbO049CKzb+4eG2WIHnnP5VqLguATgZ61jap+8mmYBiq5GFGSfwrKW51UVoc5DIYb4zMeoINSSMYfEWRwJoVI/A5NVGDOrHG0clSep/CoZrpmawnzzG+1uexGB/OuneNjml7s7s7+wjjZcvyx5A6dulbFiFW3/usD0znFY1h8yoQcMvX8q2OV+fYNpAOc9OelcaPXTXKiC8YyEsawtQkK5AHNbtxCfmx0x1rntSceZtHzdjirMJDtDszcy/dye35VrT6X+7IlBDL0Y1N4ctmi6qVbrkit+8tQyj7pGOvWhmtOPunO6XYzjAaCcwNkCSEEkfh1FdL4e8VXOi3R8q5abyjs2zSkkLjoRnmq2n6hcaPcCSGWRGzk8cflXZ2vjzwutgItd8M6feOzZkuFjKysPw71LjcpScWRQeJI74zz/Zs3eMs3mNsVScbv1rkfEN5ayzxws6ylef3YO48dKv6pfeB9QS8ewudWtZ3AEIeXKQjIyOnIxxXn2pJLFIUttRlkizyzoMn8c1HsxyxBfuJLCPcZVaLAJHOT044rlruaFNpQsR1+btUdx5vmbvPOAeSwzmsW8uJNzK0u8E5BVcY9utP2Zm6+hbuL8KpHUemaxL7UPMk2g47YHNMeOSYtnKx92PFQi2ZZBty3p8uR+daxictSq3oVmcyTFec1NFYzXEwjVepA3DmtK10G4nkQsF/eHpjgfjXeaP4Zg/s+R1MbOPu7sjOO9auyMIxk2YdnoqWlifNj2zKc+vfOa0tHDXE0aB13Fifm47HAqS/k3chFV1UAkLwefXNaPg2xX7ctzIgYId+G6YAyf0FZtXOuCadzoPiHfJp9rY6dDKs222824Zf4SRwv5968B1e/a2spmHVjxz716B4o1w6gdV1Er5aXMvlxKGyAoI6V5B4s1DcqQIOh5bNdFOPKjzsTU55GJYQveX6oBku+Ca+6/2efCS6T4fUyIqvIuQcYNfJHwj8Mvr2vQ8DYrk7mXIJwcV99+DbeTSdLtY4TG8qJg7RjAx6d65q8uiPQwNNX5mZXj5khiCmRZZGGCFJ556dK+fvF1uHuJtq7YyMhfSvf/iHdRqqEZL/AMQIxXiHibDSMccmvNXNfU+hq8rjoeM6pCI5jjq1ZV4x2j1rd8QqUvCOmDWJeJmPI+texTd4nx2IjyzM+SQx3Wc5GOlTliUzVe9jyI3B+9xj0qe3bzISMYrRmaaI3crmqzN3qeTvUDKCCKAYitubGK3tLaKHypN+WY4K46fjWCqlTxWhY27My7TyTwcVMtUEb8x7v4FuoGjBWVQwHOSB2r07Q9WtpJEQsAoOADjP8q+cdE0bUDCZbdZXHUiMZPtxXc6T441HS4Vt7+zSd16cbGH44NePXouWx9HhK3KtTpPjT4QKzC/gj3RsoPyjgc4rxe5ty0OwjBB+6G/nX0Qvxe8M32jwWd5ZXB4xIWGQK8v8WaTo09xLcaTcfu5OTGwwV5+tVQk4LlZGKpKq+aJ5gLX/AEjOAMd81fhQIoB+maurop80ncpGfWrtvpEceHkZSqnJUHNeh7RW0PKjRkma/h+2WRUH8K88jrxW9qerQ6fblR97Fc19sMakQjYOlV7hTN88r7q573Z3Rp2Rk65eS6jIw6Rsee/esaTT/LIIzXQzKrttC7QPxqtJGM8Ct4PQ5asVcx1h29qTBzhlJ9CK1TCMfdo+yljnGK0ujn5bFODb0CNn3GKvR5dQjLxnFKluR1JI96tWsQeeNQOrDn8al6j23MXxHxfrGp4WMZqhDbvcH5Bmp9ckMurTFTna+0D1rXsbNYYQO+Mk4rdaKxz25mVrLTDHy5471eWPYOOlT+WuMd/WmlMDOaTZajYhc7RUFxyC2PwqeRd2ahf0pDLEMe21XIzmuZ1yx23SsOh56V2cKBrVFPpnNY2vQr5HmDt2/GgprQ5uODkGtzTkIVRiqFuofoOlbVkgyuB3oJR1/gfTxe6srNwsPPTOeDXqigAMR0IAA9K4b4b23y3UhHfaDXdYwtQwEoPTNFB+6aQEb/dNR1KRkUwpgZzSARaVulIvWhvummBG1ItLQq0AI33TUdTMuQeajKYGc0AJ/DSU5aQigBrdKbTjQVwuc0ANbpSfw0rdKT+GgBjfdNN/hpzfdNNWjoA1xQelK/Sm/wANXEfQa3SmN0p5o2/LnNMBjfdNR1I3IIppTAzmgQU0j5TS/wANIeRTJkJ/EaRutLimk80CszlaF60HrQvWoGO9KVfvCm9xTl+8KBoe3NPX0pn8VOXrQMP4qdTV606qQCfxU5etM/ip1Ax9PXnmmVIo+WgAQ/MKmqNB8wqSpEFOAxTQ3NOzQA2nL94U2nL94UAOahetL/FSAUFIG60oGKT+KnAZNACr94VJTQmDnNOoEIo3NUgTBzmmKMMKlpMaEakbrSt1pKkAwFUk9PSpLex862ucHYYwXMg5OMc8VEzfu8N+dQ3GqyaXDK0ZDmZdpVhgAHg/oaxludtDY4sxo8jmNsqCWCls5Geuaxb9WVp4wNv8QX6HP9K6JYQzBQVQKCFIXle+PeqGv2bRW8NwBkDhj7GtYy1sY1YNq51fhe8XUdNglHJZQrDPoa6q3tmKHepCK2eDnjsK8y8A6lFZ6hJYTNtjkO6M59e2K9jtrJ5Il8klWY4AZePc1lUTT0O7DNVI2Ri6q5hjbtuHTNcdJILi+C42DPPOc12PiK3MDMg+c45YH+lcZDGJNRwxCgHqTjNON7aiqq0rHe+GrBrjO5pGwPup1NXZbGdfNOJAsf3laQHjtxjmr/hmySG1SUtGm4Djec+h7VuSWNnNCXRBEEbALnBPbOe9BtTVkccLU/K0iP5LfxN09qxtW055m2pMxXsAmD+ea9HXR1mkb9/GhUZ+zytgfXd3/Ks/ULb/AEff9gkEbHCzR5I6/QmmVKPMjydtKl3uqy7fVXbAP44qvJplxuZFZQNuQ/mAjr6V6UtlbrI4ltrhTtJ+eIhunUZXBqtHocd0VCSSeay4SJSpzz3+UYx1p3Of2R5i+jXW1syK5PRV71Evh5lkDSccd+K9J/4ReOGQQ3cEzzSDIVrgKuMgccfN69qlh8FzzWJuFtbKG1iJy010Ax5wMcepFFxezPL4fDSyNncqMc8SNx0rR0/wlLcMZEQtGo3Fgpxjvx3r0KHwtDHM5l8q7JiyqeWQA3cYzzjrmty20V4dPj3vcKSpVVhAWPpj5h3qHKw1ST3OJ0XwhNZw+eIS6yn5NvzEDscdqv31pLbo8blX8tRmJQAByOc13ccTW1nHJOy2zqmwGF9rFe3GDXM6lGLpdqpHICQBNghm57mocnc2jTSRwF1bzXEgAjICvkKvOR6Yrbu7WXR9Bmc/u5JU2IccnJAP6GvQdH8KpZqsxRDIp3AN39RXH/FS4jtpSAwWKFfNdewzwFz9T1ram7nPU9xXPD/G2orata2CPhYUy2P7x715rMJL/UFVQXZmChV5JzxWr4i1g3Vzcznlnfu3TnpXonwN+HDahdf21dw/ulBeMFcljjoBXTKXKrnkwputOyPUPgj4J/sXTYnuoAk8jDjGT9a+o9Mt7VLUKAAdoJkXqe+MV5n4b0kyXSYkETlAwyuQOOleiabNHpaqJJneToDHwxHfA+leZOfM7n1lChyRSscB46t5bjWGbyZvIVciZuFHb8a8p8QRkSuQgIHvXrnjbVmvJp7VmaSKI7kDDB57GvK9UhLO7BGGOxrBvU65RXKeQeLLFvOaRcgDk8dK5rdvt8gZzwR6V614k0lbizYqgBb+GvJWR7DUJIJeAx4/nXo0JJrQ+YxlKzuUJ4/MtSO6mm6f+8UgjGKttGPMK54bPNP02x/fkFuPp1rrkeUtWUbiPBPOfwqDbhgBzXRzaeuMAde+Krf2cd/CVBq4syoowW5HHpXRaKLeFsSx5Tuw6jiqB0+XcMLWlptvIjr8m456GgIqx1mg+IrvRmcQMWg9ehGeK7C18TWF1YvBeW0cj9Vkb7wP5V51atItwSxCL1K1K0pmkORs9Mc5rmlHuehSrOmjem8uR22bVGflUU1/KhjOQpJrJkmkZVKtgr3qOaZ2X72ax9nqdH1g0Y2jR/uKQajklQkkACqEbtjjrQscmTnvV8qE63YmaX5mBb5T1FQzOoXIY8fw1FKknOBu9ulNSFiw3Db+OapRRDqNrQdGx7jrTzj6mpI7ccZqdbYHnFVsc7u9yqF3dFqSNBkAipvK+bFG0qeKBWZEyqDg8e9OtSEaaUjCRRlgfU44FJ95xnp1/rVTWrr7LoTkdZmwOxwDVx3M57HPaehvdSZ2HDZY98e1dLGo6Vl+HIcW7SkYLHj2rUxtYNngdq1ZjAV/3eO9MZ8g8VIx8z2qA9xUljW6E1C3+tWpWPymoGG+VBnHNAuppbtsIJ4ArM15/wDiWOfTbz68itWSPzI0UnA78Vzviq58m28vu3G3PvQW9jNsbj5gMZ59a6XT/mYe1clpUbSuDzjNdv4fsTcXkMZBIZhnimZo9X8F2LWejozAfvDkn0rfbpUdrAlvbJEgwEAGfWpG6VADaKVh3pg+9QApFNIyKc3Sm0gGbdvOaaxp8n3TUbdKYDaWkooQDm6Uxvumnn7tMb7ppAMWlbpSL1pW6UwG0rfcpKD900dAGN0pFpW6Ui0dAEZcg80zbt71K3SmN0oAjfpSL0pX6U1apD6CEYoP3DTm6U0/dNUHQZSN900tI33TTDoM/hpKOxooAD0qJutS43L1qNl5oEctjLU7btxzSL94U/0qCRp4pV+8KPvMBTgmGzmgYv8AFTqb/FS5oGOX7wpaavWnr1qgGDrTqNu2igfUlj5yKfjHFNi6mn4y2KkTBfvCpO4poTBzml/ioAULzTugpF60rUANpy/eFIBk08Jg5zQAfxU6m/xUtA0C96cv3hSKMA0q/eFAmSUUUmaAHL94VJUa/eFSVLKE/ipCMUU5c56VLGQzZ8kkNjpWRqkjTRqmQBWvcAkEVh6lJ5coQjmspRZ1U5JKzM/y9oJB6VdW3+22skTgFWXAB7ccVUzgHPStK1+aEhRk49ajmszoXvaHBT2U0EwSM7bqE5Rj1OOelew/DX4m22vafHYXx8nUrYsNjcF+DgCubv8AwVJrlu0kbLFfxLvjfoH55HtxXHtb2018sOqO2k6vGfkusEKSOnHeulSjUWhyfvMNK/Q9s8QmXyi2wRqVyG25y3p+XOa88t1ZtXXdncvzD0NdBpPi3VtL0tLPV7X+07HqLu3+YDI4JOMis+SOC6vPtNpKJYUxllxnr3Gcip5Wtzb2im7nqWjyRCzi3uwupFwWUDA46gU25nNoQDIs7EMiXMqZ28HkDPXtWTZ6kDbrLvAXCgIvU8gHFNuJomkZLYSvGDuOWGB+NQdsZKxq28kEk1o4dZPLTEquSWOeCR+ecVO14908YEtzbwgM0MSuFAYHgE54Hv2rmpr+a6URbFzk5bcAen9OtO0u+ivNY8pP9LIdSVXo6gYZfbjPPNA+ZHSNeXE3nmbWVJULkTXAOBkcIeQ3p0FO0y2OoySvDcSOy4Ux2aA7RnOd2efTGKvWsli9vbrc6ZJc2rBoLVvs6LCV3bjzwcqRjPeukVtPj08W32O3s1YeWk0EoiAPq4G457fWkzSxzUPw5Z/KvU02Nnwyu15OWYDk7lGML9Oa1dP8K6fY6fA32O21OZgyBUBVlbOd2CSDjrW3CTbzK0M0lskMRQ27v5hk4zuAx074qaSVbxfKWJJtpwTEMs+RnIXsR1+9U3K5bmdb6HAqi5IkaQr5TbEBVT2PXj0qk2jrGPljnIVipLyBV3YxW7JZyQqCNxRRgLcL8wPY4B4qSOy/dtPJDEFZQdpBA3A5LZz+lZtmip6HKropjsS0jJ5pbBU8kf8AAv8A61Z8mj+dOsQdTGBkRqRknPAro7rDRvIIyGJO3zBtDewFYMl8bPzJD5PngBRARhuo5FStXoRK0Vqbdv4fYQmW7UrFAN8sZYAADkc9zntivlv47eMkl1Kezti2JWLYPBK54H5ivVviJ8UrHwJo00txP5uszAiK0VyVX3J7+uK+VbS31T4heICn7yS6uJC8jdQvXp6D2r0KceVXZ4lep7SXJAvfD3wVc+NvEEMSx/6LG26ZnGVz/dr7I0nw3a6FY21vboCEHyKi7QuRyM55rB+E/wAN7Pw1YR26wkHYC7Mer9zXoTqissTJ+8jYBSrdRn0x6Vw1qrcrHtYDCqCvPc1dB02W1XzdyIrDB/icemKt6xG26BA0m5QcNwCeKt6favGk/kxBF25yTkmsWe/jnjke4kkgulbCDG4HHU5+lcTv0Pc5Y7HBaxGwuJneRg7EjBOSO/WuSusqWG8tu9a6/wAROCHlz8zNnA/KuOn4YZP40amM1ZaGJqYZxgHG2vKvGmmStcG4CgsvPH1r1fUcKTnnNcfrFuLpZB26YxnNdlFuJ4mKjzI82+0CVYyBgjrWrYsGkU9M8ViX9m2m3jIxIVjnOKt6feKNoY7TnivTvzI+bfus6r7OCQo5461OtkNuQKk0/ZMisDn1rXitwwzxiseax2RjzIxfsPOdtNNqyqdvWuh+yr6Cmm1GOlTzl8hzy2LPISwJ3dulTxK27aM8diMdq2RZ8jHFTPa+btYgZXpgYzS5g5TKmtytvHIp3lzyvTFVfsjrG38Rat5rEKFCrtA96he3cuAKLhymLGpTk9RTi5xgHmtldPPOR174qF9L3scevTFFw5WZZglbBzxViKzJAOea14dP2qCVORViOwPBAbPoVwKVzSMWZK2ZC9f0qRIDwK2jp7rGpKgA0xbPzMjp74zU3Q+VoxzbEsKY1ua3DZhO+TUUlvz0HQ96OZCaZzkysrYAOTxmsHxg+b63s4zkRoCVHrXatHHG0txJxFCm9uOM44H51wGm79Z8QTXDcRt82ev4V0U9NTjrPWxtWcfk28ceMYHJx1qWT5V9ammjDMCOAB0pknADHnHahO47aESniombBNS7s9OKhbk0xDexqJlPnfSp1U9uaZI3zE9/SgXU0YZBtXcMYHPPtXn2vXjXeqP3ReAM12d5ceTpskuMnHTOK8+hy03XcxbrTQSZ0ehRKu0Eda9O8BaebjUhKVxHEN2eueOled6PASqn0r1r4cf8e04J5Jz/APWoY1sdsq8E575p1IPu0tZiY1vummU56ZTEPqPPIFSUxo/mzmkA2T7hqM/dqST7hqP+GmA2inEU2gB38NNIyKctG2gCLbjnNDdKVzSN0oAbQfumlIpD900AMbpR3oooAG6UxulPbpTG+7QBG/SkpzU2qQ0DdKYfumnt0ph+6aoBtI33TS0MvymmLoRrSMMCnAYprNkUB0AfdprdacPu01utAHKr94U/uKYv3hTz1FQT0EA+YVJTF+9UlAyM/eFKvWjbyKUCqQx+3vTl60djQvWmPqDUL81L/FQBg0g6ksfenr9+mR8809fvVIiRetJ3pV60UAC9aVqRetK1AAv3hUlRr94U+gBF606mr1p1A0FKv3hSU8Jg5zQA6hVyetHpSr94UDQ4Jg5zTqKG6VIDV605qAMU00ARSyfN0P4c1iaq6/aAxVsjuRW3JH0INYepZa42MScVEjSG5WbayA9d3artjH86/N8uelU9oCqAOner1nzg5xiuWR6UPiR0unykI2MblOQW/lird/4Z0/xBbxW2o2ouI24DxMFkT0wcetZtiPlJjfeT1yMCuq0yZJFYSggcD92uSK51KUXoepGnGorSRxT/AAX8SaHNdS+FtZWW3hUObaaTy2IYgbecg9a5q+1fUNHuBD4j8NSwTIcfbbFTGV7ZLYIOenSvpTS7MXqKgYBSURUbnI3DJI6muz0Xw3YXllfm5tkuoScGCWPcCVYY57DOPpXfTr30kcFbAKOsWfJGk+NdNucix1iP5OPJv4juX1G7PP5VtWt9K0TNEsLhupt51cH04JBH4A17h4w/Z78LeM5Lu8XR44PKKozW/wAgVupx6+ma8o8UfsnPDC8/hjVp/MVQfs94wkOc8gMACvFdHNGR5nJVhojntYt5ZoI1lKW8gORJyB19qsaU8tvcQNH5Kyw5KTWzlWPBzkHrXL6v8MPiN4SsYrlLkXMTMUIhlLbSOxytc5NqnjGyz9q0+SUHqWh3D65BFKyYuepHofQ+l+InuljMbNH5Lbo4JIw0a92xzgZPPSty28UWkt4lwyRfalbJZo1WIdslQDmvlKPxzrPOdP3beT5SkAfXmnp8RtXjLY05iFAbcFYZ5xiplTTNfrUkfYi+MLZobm3W90+NJz+/nWAgvjkAZPHI9aR/FulZQ3EsZjZgQtq+wDA6njJr4/X4k65OMJYlSCdo2MQOxyM4NI3jDxaVLRWMyr/sR5P86j2KfU0WMmloj7Lk+IGkaa0skd1vaUACLbv71z+q/Ea14ZZGlIziNiEWvkuTUfG90V2JcKZOx4NVbjwp401OVY3E7ySdFdyAaapRW4/rdWWyPoXxJ8XLZVMVzqcEMY5WJW8yQc9q8n8TfHhYvOg0dWlmYYN3OclfpxxWDa/A3Xp1HnqyyNy235go92zxXRaP8CbeEg3khlKnJRRjn86rmpwMXTr13qjymO31bx1rQJaS5uJMq0jg49yPSvpv4R/C+38L2qkoWumUGWYjk/QUnhvwJb2coS3t1iC9Dt5r1LTbP7GiCL72MHIrmrYhNWieng8DyPmmben2Zt4SYz+8xwpXrSQkrdbpSpbPPyY2+/vUK6hJGu0EFvUDpUlwBDGrScvIMlume4rz+a+57y5Y6I2oZFuopWNy0aDg8Y4xwa5bXJDbzJIZFeFsqMNkn3pJdSnklUCRY0UYOeQaytQ3vGxQKAo4yc49aLoGzB1K4IZ0KBFbp8+feuav5DHk7eB3zWrMqN5r7iXU9z71zuqTMpIzlfSq3Zz1HoZepSFm4NYsi/Mc85rQupCz9KzZ5P3gGK6onkz10ZzviTRRfW7uPvqOOPevPyzW9wYpAQwOB2r19kEisO9ch4k8NrdFpIxskHIwuc12Ql0PHxFF7xKvh7WDGuHxtU4xurv9JvYrqMFSD614zJFJZMy5ZSDWxpHiSS0K4JAB5561pJXWhzxk46M9jVQ2eelPWEMwz0rjNM8ZB8b2GG4PzV0lnrkFwBlhg+9YcrW53QnGRpfZV9aDDhcDrRHeQSLw9TLNEWHKk+lI25UQtGWUEnp2xUfkj05q5sVuhH0pmDnG3igTSRAFx15p0cO5jgc4J/SpYwGkCngHNTKqxsNrgn0PFBJHDbNLt4PIyV9KuR2Yj6k1PGd0yKoWJmXAy2fxzVqHZ5JnDhgpw+RjHYGokbQKPlq0YXjI96i+z7cjp74q958WGcsuB2A5qldatbxAksq496nU003ZWljUsRuP5VRuIkHADMScALyc5wKqap4usoQymUVy+ofERY1ZLFCZiMLKTkD14xzxWsIXOSrOK2LPj7VksbNdHiYG4kOZ9pzxnIH5iszw7YmztFYrgtVPSdHn1C6a8u8uznczN1NdTtCjAXAxgCuhtJWOKMXN3ZVbLN0qOSM7SKtqvzA1DIwbIxWaNGrFLbtIqDflulWnSqxQqashgGPbg0jL1J60uMc0rjCE0yRssRn02WHqcdfxrnoNF8sg+/XFdRD91h14qONPmAPrQHLdj9Lt1hVQeh4zXdfD24H2xoR/Epb+lcciBVGRgA5z+Oa6r4fbW1rCjhIyPrmkW7bHo+3avWkp7fdNRtSMhKaRinUjdKAFHSkbpQvSloAik+6ajWlc0i0dABulNpzdKbQA5aWkWhulDAjcd6SnN9002gAbpTevFObpSL1oAaUwM5ptSN901HQgBulMNSFeKaRQBGy/KDmmVLJ9yoqsaBulN68U6jbjmmIZsxzmkblakblTTG6UupAxkwDzUZXipm+6ajbpVFR2ExhaY3WpP4Kjb71AzlV+8KVvvU1etL3FQT0HA4OalXnmogMnFSDgYoGI1PVd1ManqeMVXQYtKvWkpV60D6i/xUvWk/ipy8sKA6j4+OKev3qRBjNC/eFSIlXrRQvWhetACgYpGp1NagBV+8KfTF+8KeelACL1p1NXrT1XcwFNDBetSU3y8GnUCE7inL94U3uKcv3hSKRJRRRUADU2lakXrTAa3auf1H/j7auiZfeud1D5rgmokbU9yAtnHFX9OILDcPl71RhAMqhhkVdtZFjkyjdDjpXNI9GO5tWceFOz7pIyM4PWunsZfs0DMpLALkgDke1cvp+TIWHO0ZznArdsrkMTlSnmLng5x3rlPUjKyPVvC8CNJIIXB8mJZ5WbgrxnGP0r0rw/MLC1HkspNxGrBm4z84LKR2yMjNeF+GfEkQ1LWbc3Ie5DxRCIKRujxnfnt06V6bY3jiI3A/fBfLRVJwCCyj8OtXE6LqUTr7OWaz0a4EarJbl8SKyZBG4FQeeecc1XvfDIeSZS8kMmNwaFtg5GcAc5HvmrMjJJpExDthpPLaJeMj+L8MZ5rWkMFxBLYSxS7bd/LSdGw5jVchenHPeuuOxxOPL0OC1Twzp62M9lJ5Kq8QdCu4uXyMnO7A4rkrX4YWvmSFY7i7+TzAWbCY6EbcHPHvXs11pMdrYzW5ZRAQux5l3PyQeO9cxqNrrU2jXUUOp7fJ3RpIto0RAxxgk1ErlRjCS1RwH/AAqvQdUF1dwtp+kiENA0dwpQuykcn3OaqW/wUiuphJbtbhYkBYSxFVkycfKe/XNegeDPCulTadfSavIdRuZr4ySxsDIADGQBnKkfNg5rbTSooJFtoekBUxiSQsqhiF657A5xUc0kR7GD3R5hp3wbspr5oZns9mQMLECT+GePWt7/AIUdoGns73Pk3MfQNHLsY8dlwa7bQdHWSaeYyK1wkZaZI4ujbwAgbcOx3ZrQurW1SC7KCOFuHEZGZM5GQDR7SRtCjDsebL8N/D9taqsFqke4/ediWHfqRSXXhbSrS3Cxol05GR+7wQQM9c11d1ayX7JGDtVxkKx4z2GccVGu63tHt2tYVCkozK+SD9cVnObZ0wow7Hl+vItraFYLVYGkGW2Z55HWudtbNlyfLBLV6Lr9tF9u3TIFjjThM53fj29awLtLaGXMeFAXd61zOT2OmMYRehUggW2AfABIFTySv50ZT5U79+1Zt1qQmkAXp6Ui3DldpPFQk7XYVJJaI1ty+YMc5qy8bzIu+UEL0HSs6LDgEtz6VPNGCuGZlWldDpwb1ILh4bR8lfNGeecVQ1a6adAU2jjoPStT7PCVzk7ccgDJNZ9/pcLW7Sq/zdgeD+VHMjaVN2OPvMx5YD73UZrmtWmV2ODk11F/blcgAnaa5vUrFZGLI23HXitoNHn1lZHPzEmTGOOeazrhfnrcuLUhWGefXFZc8LbtuPxrsTPIkU1kIYCmyxlgSWpsuY35FIXDKeeavW5jLU5/WNHik3NtBb6VgNofzEAYz7V3uxZHGRTGs45MkLz6VspM5ZUYtnCHSZohlTyKljlvrUfJu4712LaWp5xg0w2JAICD/exV+0MnQ6o52HxNeWuAwPHc1pW3jwRgCRcn/Z61bbSY5OHTcO/GKrt4as5HBaI4zyFODRzRe5Cp1EXY/H8HGSyVch8dWjYJmOPesibwXYs2F8zOMjJzUP8AwgUDnInZV/u7c/1pXgV7OqdD/wAJrZbgfP8Aypknjaz5xIx+nWsFfAaNkeaceu3B/nViH4fx7wDK3PcCnzQFyVOxfk+I8KYUhmHUHpj0qK5+LV6zFowoBXa2FwD6U2LwHaZYO7sV52+tWYfCFhEw/dMw9zwaXPAr2dVmFP8AEDUp9xHGf7q1nyahrGqNwJcN32mu+t/D1lEQyQqCOmeRV6MC3XaiKB7KAaTqR6IpUJy3Z5zbeEdQvDuuG2g9iea3rPwtaaeULAvIO56dK6V0CAkDr19ajIPcZFHO2X7BRKke1cIBgVI4AUnFSMiH7o6VFJ0ING5OkdER59qpvw1WmbZ1qtJ/e7CgzkVpZNsgGM5pjDdSN94mlFaIwYwx+9DplMe9SU9F5GaYxlu21n46CovLPmZBqeNQ0zNUmFDc8DBoKGru2YZ8juK734baa0aTXjLhW+Vff3rhIbd7y5it0BLSYwB+tez6Pp66bYwwqMbUH59zSJZdNRtw2Kkziom+Zs0iQooopCAUjU7saY3WmwInTqc01akk+6ajWgBaaRinUjdKQCLSt0pFp1MBhGRSbfl604jFIfumjoAxulNpzdKbQgFb7pqOpSMimFMDOaAFpjelOHSmN60ANf7tRVK/3aiqxocRQ3SgmhulHUzluNbpTG6U9ulMbpR1Egxlaibjipc4Wom+amVHYUDK1GyZapcbVqJm5oKOTU8il7imL94U/uKknoOX7wqSo1+8KkoGHcUq9aTuKVetV0GPXrSgYpF60BqB9RVG58U9Vwwpq/fqT+KhgPXvShMHOaROtPpMQq9aF60L1oXrSAdTWp1NagBV+8KkqNfvCpKAEAxTkO1gaSnKuSOaAHbst0paTbhutLQAncU5fvCgjFC/eFBSJKKKKgBGpF60rUi9aYA/SucvvmuHHpXRv0rnNQ+W6kHXmoka09yKOPLA5qzDGqewLZNRW6lmIweB3FWNoHGcgda5pHpxNSz+WQgn5G4Jrp9NdFlgjU5O0jB4zwc81ycO/wC8h44roLdlSNXYbmHYHB9Otc7O6DOw8P2MZ1C4YxhriSJUJDDJ5Bz09K7bQ9YiMZR5FZZF8qNTwQQeTj6CvN9LvEs9UjmSQhQFYLn72Dkiu28PXkGseZE0CpdvLmJumMkZ57cUlozoR6rYKpt2tSW875YvMA6K3GceozXR6cpulmuIizPcIFUwnekRzyXJxjIXGMdWrk/Bd1dalb6tLIiwtY3CQyhmy+9SCABjkEDOa7LwrbztqVxGJo9QgkgiYSSR4AADOSAG6hgFx/tZrri00TMj1pYri9g+0XR8jcqtEikSjA4I55BP5Cn32qW8d1JKtyQYF2mOOQuMEYyex69MVBrE0Talam3imgu5kkaYTrtA4ICr16+tNj8iN5LY2ccT26yA4YHIC8sT369KmRENjk/h3NFqb3MctwrN5TTKwGwckn5j9Bird19o066W9uImkVlxDbWzgsyngM2eMDOaueH4rXwvo0EsVjGst1p8LgPKHB3O2SeBgACq194kh1iFLt0W2byRDNNsHlDDAKFPfnHOKg0SbIF1CVY3tPMEp3iWUFwBnoMgdfSqFzq8sJuAs6wleSI03N9BzUCyXywyrAytGUMhbYI14OBk4ya5bVtYS3uRB9uSeeSPMhiO4D1B6UjSOm51Q8WJFJhZZmVo+cgHB7H8DWfdayiqZwZsMPnQtkO2evTivPm1VY71mg3IMY3HJDHp07UTatcRx+WJC0bcnJrOUQ9pyuxr6rqn2jfvLBySVY9uOlc1NI7fIXzgYPvUMupSzOS75WmR7n5HJNYy3NoXkyxbw7o92cEnFalvZbtp3ZB7YqCCErHGTxjOa1LGRY1yAXI7dKwlUsd0aXNqxY7VRuAbBXnpUkqfbFCqcEHHPenCGWYtIEYKeoxVnaWkjMUYjZf73IrHm7m/JbYr/Z5La3dvKYgHbuHA9M1kTSCNWLLls9zzXVXEksFoRcEbWOdo4FcdqkiySEqfwpppja0MtlWa45HB/GsbWLFY2Zohn1GK6GzAWQM3OM+3aq2rOiI37rdnoc4xzWkZWZx1KacdTiZoMuARwao3UChTxW9OAZCcVQvLfdCzA8+ldcZO55MqZyt7bjBOKzWQK2QK3ryMlSKyZF2vjFdcXoefONmVWbAJpYpArdaWWAlSwPTtis9ldHzmtUc009zTa5CnJPHrU8cySr2OaxhLkbWHH1pPtXktuXKqKHEUKnK7M6KOHzP4eKnSxBwdufbFUNM1aN0APJ9DXQ2tyksfC8noc1hK6O2KU9UUV04tISByRwMVKlmFAyeTx0rQhYxzB8ZHTH4VZjt14JXcxNZ8x0chh/2YWY7QS3UH9anW3IlhYDkDn8q3orQR3cYYYRgQSB04NOm0kx3luyRsF+6S3A+tPmJdMxGhAmZipHHOOvSontswREA4J6kYror/AE4Q3UsQKuu3IZep9gKhFnCtrAdrmTJ4J46VXMg5LGAo+U8dKgOdwyK1podrkbcA1XkthyR1qkZTVipJymcdKiKEqexq0wKKQV4qtJITkBfwzWsdjklsQSKFUj86gf7341M7FlBIxmq7NuNaHI9yCY/MQRwKgkbEbenpVibgk+oqjNnru/CrRL2K7Nz0py/dzTNvzZp6/dxVmDFzjmpW+UA1FjPFSN85C0i1sOij285qNZBM7rnGKmRtvGCcnHAyapabpt5rGsSWtnG0h3bSyjIA7mhAdt8O9PS91SS527o4FwGI68Yr0tuQBWb4f0OLw/psVrHgyAZlYDG41pN0pESGN901HUj/AHajoJCiiikAfwmmU8/dNMpsBHGVNR7cd6lbpTG6UANooopAJjFLRRTARulNP3TTm6U0/dNHQBjdKMUN0ozQgFprfdNOprfdNADf4aa3Snfw01ulHUBMZWomTHepVpGX5TVARkUN0pcZWkbpT6kS3Gt0pjdKe3SmN0pEiN92mL1p7fdplBcRxXIxUTLzUm7DUwrVFHIJywp54pEXDDmnNUk9AX7wqSo1+8KkoGHcUq9aTuKVetV0GOpV60L1oAoH1HL9+pP4qjX74qT+Khh1Hp1p9Mj61IvWkIF60L1pQKRetIB1NanU1qAFX7wqSo1+8KfuoAVetPBwaYvWn07ALuy3SnL1pmMHNPXrSAGpF/1gpWpI/wDWUFImXrSYpV60hNQAD7wpAKUfeFLTAZJ0rnNR+a6kHTkV0cnaue1Jdt5JzUSNIbkcJIzhiCe+atKyn5dvJ6nNVIeMVbiTe/B5Fc7PUp7Fy0nMaGPH3v4q3LGXeuW4wRXNRtiTI5A610Fuy+TC2c7jg+1YyR105dDWswLq8VVxlAzhWbAOFJxmur0a8guGML4j2sgdiSAmSMHNcLbyL9sdFOOMBj06V1FlIWkJWRYpZU+6OQQqk9PwrJ6bnXHY9T0HWZ9Lvr6SPC3LgK95EMoxH3WPPX+Guotbu2jjWOza4t9Q/eSGWToWcgsAc8AAE+9eWabq0EfkMySpbyII3bPIOeTiu00HUFg+2RvZNd2qgRmaQESBSRgKexzjtyKqMrItxudJD4ssLnxWserzz6hdyW26GIdIiOAPfce/GKT7bDrNld+SVSBklt1MoKM7M4LkHJ4UA/WuVlvrWG61e9ks/LvnAitYGPMagYyzY49elQ+INe0+z0lbaO7lnvoFe3W2g5i5Xli/rls9KfMxqGmpptGNJ0u3xAv+pa2DTMXEiYJACdgBk9a5VvEt7qzSSS/YtPtVZYoyqnaEToAmeuRknNULjVLlj5MVx59zG6b43clYxsIPP0NYt8+yN8BJEjZiqK2DnBzimn3Ha2xoa1481XVHW1Ny1vb26FDJGflmGcj5ccdPWuRbUpJJnk3YMhwQoxx7+tT3F01zDGMmPA3FGYZ+jDHFVbJEvJsMh8sHBVepPb9afU56krbmlp6yzRsGhZYl6SO39MVDcXLJjuM4rV1BmsbeFXBUY4G8c8dxWDcKzLuHQHNOW2plS/eMtWq/bLgQLy7EYrrR4fXT4V8113Yz0rmdBhCyebg+Zn5eK2ZZbyeZt4YkdB7V59SXRHu0ael2WdySZRfvDgVqaTpZudwUlD9OtO0Pw9LII5yGO48fJmu7s/D1zBHGzQtiT/Z7VyO53JJIxbHSfJZULGVTnIYYFaDeFZLgHygu4gkYPPrXoOl+Gy1rE32dcH7xkHArS/s2MqBGsPljjeowfehU5NaIftoR0PEb7SpnhkSRTvj4A9ea5TUNM2sV2kN3b0r2zxTDa2tzE0W3Z/Hjk1wvii1tri8kELbAyAg7eCepFWotDk1I8ymtWh5z1PpVe8zLF938a6CWNA5TCuF6kGsidPLdlP3TVdTGSTicpeQsJDiqzx/Ic8+1bF8oWQ8cVnSqCfauuJ5FWNjn7y3DSGsae3LOeK6e8hwGbNZUoAyMV2x2PJqbmR5OOMVWnsw2e34VsFMsMLTGh3MARgGq16E8t4nKXVqUzhqpvIY8grkV0t9ZMjsCMDqDjrWHeW42kZ/HFaxehyVIW1KEd0yyDHyiun0fUv3YJPSuNuWMe7HUVY0vUGjwPU9zVSjzI56VVxlY9Q0+cT7cZb2xW1bfIQAMs3TPFcn4fvl2jLgFRnpmuptrxGZGkbKjrtHOccVwyjZnuwkpIsvhmXJIAZQSBz17VrXSP5hOCUHABOQRWRcSCZgpwpDKOuCMkc4q9LcLBLJGhYr9wktnOO/SoN1oVrzPBCgNkDcD78mqsWyaKKVHZuW4PbtmrFwTNG4VsMRxTLiaNYLOOGBYxBDtkYPkyEnOcY4qkZS3M28Uq3LZqm8uM8Vbupllww4PTbWfIC2R0961izlqDJmLcdjVV1CnOecVachcDrjvVGdtr56gdq3jscMivJksoJ4FQvj1p8sme1VbiYp2zyB+taHLLc</t>
-  </si>
-  <si>
-    <t>jmOFJzVKTJ5qeZvmZewGc+tRVpEhkVOHSmZ5xT6oyYo60obaxNJRQUTRyHryDjjB56V7B4XsYLHS7ZoYUjkliDSOowWrx2FvmAxngivcdNi8jTbVM5KxKPTtmkJlgYAOO/f1oooqSSF2+Yim05upNNpiCiiikAH7pplOPQ02mwBulMbpT26UxulADaKKKQCA80tJjFLTARulNP3TTm6U0/dNHQBjdKMUtJQgFprfdNOprfdNADV6UjDApw6Ujcg0AMWhvumkXsKVvumjqAz+Gms1O/hprDNUZyGt0pjdKe3Sm0CEb7pqKpW+6ajHNNFx2EpaVUz3ppamWcmvWkNFOWPdzmpI6CL94VLTVTa3WnUDAdaF600NzTl61Qx69adTV606gfUcqfNnNO/ipFPNPVdzihgKn3hUi9aQR4opCH0Uitk0tIApGpaTGSKABfvCnL1oCYOc0lUhj1608dRTV9acvWmMdSr1pKVetSyQakj/1lK1JH/rKRSJaKVetGOKgBB94UtIPvClPWmAyTtWDrC7Lh2znpW83IrL1KEeeS3IYdKzkaQ3M+PEfJOVHerC/Lls4J6Y5qqqsuFzkZz0q2hU4CptA65Oc1gelDYkVR5ZA4J61es2IkVfvegzjtVEcEc1KsuMcVnudMXY24ZBFJnYN3JyTxjGa6KG4WZLdo4Gkxj94gwQScAVytrIZYjlsKB0xk1r6XqCx4VWZCcAjOQcEEHHbkVhOLOynJM6mxuHuo3yWjnGXVWPGVPK4+gzmtdbjXLG+t9Re+UwXEXyQxtuI45O3uQOa5mxkJuASqFcY3dGJJ5NbMTJapthZZ5CcHbklB1Iz2z0pR00Oq50T3Akt4bk6hbSpITvM5O5xjqwx69vWuevNQhffi3doULhpYI/KJYkFTnJJGRikW8sDcrLLLeW17HxEsUY8rHfP0HPuarXWsDzX2Sfa5GJP2yYbQBjGNvQelWS5LqRTMyJuLO/muJH+cKq8fdY9T65xWT5ivNciJy8eflkUHK+vHfipJmWVmit7ZYFwCZmUk5zywOcdOMYqJlLbYld0bqNpG0r6k4quVmLqLoV7gl5kVNzRIMGRhhn9ATW1o9m1wruNwkTou3j881BYxhs5UFQQRGDuJ59a73QPD8/8AZ6Pc5t4mfe2xAxYEcDrxzWsF3Oao7nH61ptwkSz3Fo0cf8LnJz/hWT9qXyuOc8V6n4khkutJWKUOIlyqqUz+JNeQXlm2m6k0DnKt8ysBwfalWjdXRrhZckrM9g8E+HbSbQLad9vmM2Tx0rtNJ8GxXJmu5PLEeQAoGT1FeLaP4quNIVYi+YsfdJwK9E0P4lLbyWzgLhCCV3cH9K8ux73tLrQ9TsfDMVvFOTtgVVGxcZPPGa6XwvDBFNscrKrKI/mboeucV5h4s+MEWp3Nu1iFj2Lh17E4rGsviZPBMspI3KQcCmrLUzleS3PpuzSOWI2xij67VBOQanvNHt4rfyvIhDKPkMa9c8V5Nofxah1e18ohYrlj8rbufftXQW/jpbVRBHM003Vg3atvbRijm+qVHqmY/i7Q0EjIqL5iEGT5eF59e9ea+JY4o9Li2BTcGYpjHNeheKPGkTr5Qwrt/Gefzry3xdryS4WJVQx87h3rn9pGTPSjTlCOpxt3A0bTArtIbBGKwtSYeYpztxWxeaobhVDHLM2WPTNYGoRmdshttS3qPlbjoZF3Lucrt61Qn4UnNWbpWiY7uMd6zbm4XBGePWumJ5lYguXBibjNZ3lmQ8VM10u7k8U2O4Rc4OD2rsWx40txFtyvUZqKaJcHt706bUlj7j86zLrVBz83FaIzlLlQalIGiCMckfxdK5vUlCx59at32pK2fnwa5+8vjJhc5rWKOCpUurFC6/iNUVYq2OcVeaMspJqFrfe1dF1Y4zc0PUGCkBsA13mkXBWENu+YV5jpeY2wTjmu70mTcsZLEBeo65rnnFM9LD1dLM6+zmZlZ32uzdXI9+K0UYyg7gMeuKy4GBjjKjEbdRnrV0s25SDhR2NcUvdZ68ZXRIgX5sfKRxzzVG5uuNqBRkbScVJcTHawX72O1ZXzM3zDgdTQtiZMkbLAAkHFQsB0pWkCcnpTDJFIp3n5e4FUjlnqilJugDZGc9KpSNuyentV2cjYxByo6A1nTPty36V1R2OGe5DK+OMVVkb2qaRg3NVZnwpIGa1RzSZHIu5gc4xUTOFyD0qZm4qvJh881pHYxkNAL5YdAakqGMlTgHIqb+HdVEhRSqPlzSN8q0AT2KebcRj+8wX8zXukX3VHQKiqPwGK8T0GEzajaqP4pVH617cMHOPT+tSxBSN900tI33TUiI8ZpCmBnNOWhvummBHRRSNQAfw02nfw02gAbpTG6Gnt0ph+6aAG0UUUgCiiimAU0jCmnUhPymjoBHSUtFABTW+6adTW+6aAEpG6Ufw0E0AM2980N9007+Gmt900dQI2+7SN0pW+7SE8VRDVxrdKY3Sn0jLhaZI1vumo1qQjIpu3bzmkUhcYUGoyM96lb5lqI1RZya9akU4bFRr1p6/eFSShW+9RQ33hRVIoFXc2Kfsxzmmj5TmnhsnGKYAvWnL1pq9acvWkh9R6feqaNfmzmok+9UqttNIRJTKUPk9KB96kAqjBpaVetB60AJQOoopV60AOphp9NbrVIfQevpTl601fWnL1pjHUq9aSlXrUskdTI/8AWU+mqMPSGiVetOPSmr1o3djUDAdRSmkXrTqYDDWdqaksp7GtVfvfhVG/j2wnuQRj86iRcNzHxtkB61IjfKRgbj70xj82epBxj+tRySbeWBwK5up6MSwsh3BSCHP8NTRMM+h9KgjZsqw5HY9xTjJ5OXIyc0jpvdGhbyFTgVq2cgwsqrls4I9KwvOCqrqTnuPStS1mWFC5OIz+PtWcjalLXU3I7iNjGzAxyqcgh+DWnpVxPKkkSyQJLku6qxXKdjnHJrlcySXCgSxc8BjJtOMc9uKv2MstrI8U16iEfdwu7K9gTUqPVnROZ0MkkgtzOqs9oP8AWMZBjPbtnrUa4ZTmJokkXPTeX+i4/HPYVWhkjmUkG3tptrf6VJMUXoQTjBAqSFUEMSG7W4VVzut3KrKfTPUD6da3UTCUyPWLsNNDFp63ErsFikaZyIRkjkHbz/SrGn6e1wvmSSwxhSytLJIQnHVV4y31p0NidQmj8pVXBB2DcI4+ee5yccdK3tHhtpr5rCycO8IIlm8shQM5KqCMA8YznkVrZGKk7i6TptuYVkRlJzkuFJAXsffniu/8OArbtvyxIwgWM4PrzniqcBf7PgxPtkKoqqgLbQRxWuRHpNuZ2W62NwFyDt9/eoukdEYu2pcubiD7OTKMKU2FGHBzxnNcfqvge21K1TydiuoyATkr7571uXWnzXSJIrqYmG5CWznnpjtiqbQ5mYeYVfjJAxnvjrUyaaKVJ3ujzLVPCeoWqSExb44+S4OOPpXOrqD2L4B2nGQxP6Yr328ghubECJApwFbLZz61xOufDaC/81lt2AjXgqcc561zcsU7GknUjscF/wAJRK7g7gTjtUkHi4W8g3HLemarap8NbyxMjwTsNvSPb1/HNYzeGrqKItO+x+3BY/lVOjGREcRUjudnp/jZ4Z1Mcm1s5BBrqrf4naiZFk85S+MZ9eK8Ymsb2zyxDMq9WVSCPwqza6o1uyhyfx4NclTDHpUMd0Z65f8AjO81BSZJhk4OQKw7zXJZm+aQkMMemK5WLWg4G0846Ul1qhNuOma440+VnoSrxkrmjLfNDkbs85BzioJNeSLJdhgdea5291ZVRstz2wa5XVNa5ILHbXVGnzM4Z4tU1odd4h8QQyriOQA1yV1ruMjzM1zl1qRkbIckVk3WoIr5Z+fSvTp0O58/iMZzM6wa8q8bv1on8SowABxXFPqS9Qc+2ai+2NMCAQK6PZHlvEO51N1rgbO09feqE2oFwefwzWYqMxUsal+z/LnNWoC9pKRJuMjjrig2/Oc0+Jdq+pFWooy/+zS2CxUVOxFSeSKu/Y8jrj8Kctvt96RSpsz2jAwwGMV0Gi3jKqqBzWe1vuBGKS3ZrWYZOFHejoNJxdz0SznVoYwwxjvmpZLgyMwLkRrjIFcxb6iwiAPQ981dt7ss2Rgljjk1zSiehTrK1jZW5IGBjy+7HrVWW6CttHOarvIEYksdwONuODUckiDBUbmrKx0uV0Okm65HFVJZhg4GKS4nJUjbj8az5pjuA65raMdDjnKxZnmO3IPA6r61Tkl3qRUbyMQQRgUzzNtdEYnHKSCRyoNQbtx5p8zjaTUa+taLY5yORvmGO1QNnd6VaKjdnNQSMNx4quhLEj5zUv8ADtqFDtqYEFaogP4cVGV285p5OKDhuKBm54LXdr1mCM4YnHrgE17CM/j/APXryX4fxeZ4it/RS/8A6A1euVDENbpSM3YUrdKjbrSEKtDfdNKOlI33TQBHTKc3Sm0AO/hptKTSUgBulNxkGnN0pM4XNPoA0pgZzTacXyOlNoAVaCMUq0hNDASk2/KaWlxlaOgEB64paGXDZzRQAU1vumnUjfdoAY3SgihulBNACfw01vumn/w01vmBo6gRN92mU9+gplWNBSyfdpCaGbcOlHUze4wnApu/dninsuQeaZsxnmgnoPU8VA33jUyjC1Gw5pouOxyS9aev3hTP4qev3hUjQ/8AipF60vcUKvNNDFpF+8KdjJxQEwc5pjAfepy9aYetSLQg6j4/vCpcZbFRR/eFTD7wpMTFCYOc0v8AFS0n8VIBy9aG60L1oagBKVetJSr1oAdTWp1J1xVIfQcvpTl60gGKVetMY/saF60DvQvWpJHAZNL5e05zSA4NO8zccYqQCnAYptOBqSkIPvU6k/ipaYCg4qG4XejkcnHSpgMml8v0apYRdpHL4/el85AGCvofWiRhtI25qa8jEd1Io+UNVaPbuX5s5NYyTPRhJND42MPy4ypqXduGcVGzfMVYYI6d6crjhT06ZrNo6Yuy1J0kwVRyNv0q7Z3HySKrEEdBjrWXcEtGSmCVbDD05qzbyG4+cYQY69c1LQ+bXQ0+mwFSR3PUn0/WrC3TQgLMm89yxwF9O1UlYSDas21gMq23g88jrViG5aGRmTcGYYYkbs/hxQkdF76m1DLFJHh4kSJhzNuBC8cDGOeeKvWl4HRUkVZCo2wsrBFj55JGORiuYKM0qyMP32flYHGPXjp0q1AftUx52spwzKdrKP656VrHYzludlp0ktxaqYm8uDztssy/dYg52jnJGR1rasWjiuDkHDy5kCMcgDpkZ55rCscSkL5kcLRJujVlyo46YzwffvWzBMdSvImiTySUw7Hg/UVMnbRGsIHf2dxapsmBKTE7RHsIyPXOeKn3NPayBv3ab8Fup/Oqxlgg8mOFfOjRFLyH1z69qWa+SOPYCuGOcdRXI27nfGKsX5VS4jWN2SJLdflZTjP1FZd1choWdVWbPykBsEe/Q5prXCv5iSFTtIO4cZ5HGKqS/u5jKyqR/CAcAUrs1SEs5JmKqQUTOSxOcVLeOVkZhdSAtgeoHPp3qv8AaHEigsQjHHAzxVCS8eMeaEaWM7sbuCce1CTbHzJLUtX13BpkLTXDlz2+Xr74rzfxF8SW0+6khsNPhZpVyk7EEr6np6VD4u1q/mvmkedbOMxkRK3zEe/5V5ndWPnQvd3N87xMQqrH1PIyRzXdCGmp42Jq+9oXdW8Y6teSAkNcqT8zgiMH2xiqk3iYlQkkO1zgZOCAc+tNtY9JjnRJ2neEZOHOB0q3qU2lSW+IVjtRjjJ3nPY1ry9LHm87vuFjq/2gOvyxMpwecn60Xt1OrbNx45GO9YkmpQBiZgrHGN6cE4PXFPtfEUe5lGZc8BmGMVk6MdzWOJmtLkt1M6ruyxY1y2r35C5J5b+Gu0keO/tMqVyB2rktY0lpgMAFs0404piqVHKJyt5fzMrbThayppXZ8k5rbvdJuIQzFS0Y64FZj2rZ5FdmnQ8qV1uVgzNx0q/ats+U8g1HHZnqT+S5qxBay/eCEqDTMol6DC4PNX4z5i1lrMsagHOSdoB4PvWhbSfLjFJo6YtFyGPcwGa0oIxiqMK/Lu9McfpWjA4RsEZrKR0x3LAjymKQRc1LG4YYxUirzWZ1LYrhQp+7moZkV8gjAq+0Y9aie33KcHJ9KCZalS1maM+W7cn7tbFggmZdz7VBySOayLqAlcgYdejUul6htJVztwccnrSlqtDKL5ZanWO0LKTjAByc96zJHKOSoz7k4ojuHnwDtVD2B61DMckqSQD3rn5Wmei5LlIbh3JJLDFVJHJYHOMUrnOeCMHrmq9xIsYyX59K6YrQ4KkhHkKnJOaj84+lRySA4wc0zzB0xg1skcdydpN3ApRhl25xULN8hPemK34UwuSlym7PaombdQzbiCeMU3PzYpksf/DTkyoznNMY4qRhtXA5zTIE35bGKC23mmj7woL9sUwO0+HcO7WA4/gUt+YIr1ADIrzz4ZwFp7qQ9kABx79K9DBwKze4DW6VHUjdKj70gHUjfdNLSP8AdNICJulNpzUlMBKKKKQA3SkxlaVulFMBhTAzmm1I33TUdADl6UhGKUUhNACU4dKbTj0oAjcd6Z61I33TUfY0dACkbpS0jdKAGN0oIpaRulCAP4aaxwKcelMb7tAEcnam09+lM9atDEbpTac3Smin1IHN0pjcA07dTW+6aQrMN2VqNutSfw1G3Wmikcl/FT1+8Kb/ABUoODUgS0q9aTrzSr1oGH8VOpP4qWqQDW609fSm/wAQpaBkkf3hU2cHNRRj5qlxmkJjlbcQMUuMUiJhhzTmpAC9aVqRetK3SgBAMmnbMd6av3hUlADaT0paXbTQCg0q9aTbtpV+9TGOpR1pdtJ/FSEOpE+/S0if6ykA+lHUUUDqKkpC9xS0UUAKDg05W5AxTQMmnBfekLqYuvw4cSjo3B9qyI9rRrkZP1rp9RtPtFm6jqBkcVxkczeYVAwVYg80mdEZ20NIbtxYnj0pwcqQRwRyKjhyyEsw+lJu3L2z6A5rGSO1SuOVvMY7R87EknPDD0qaGYQkK6nYDwF5qpH8rZzmpWkbyyMkKeDjrUFrY0bPUVkkeIxqFznbu5H0OOaufajD0bah4yOSKxtphIQoFHVGzk+/NTmQOVjIJB7r1osUpWNR9QCxvEdwZgMHHJ75z2qO11UxzsjDJOAW6E4NZ00hTc3m71/h45HsRU1sSzsJE5K5BrRKxPM7nW6beGWcDJcytgEc49Biu20KeS3cIxVbkISFc5CgHnH4V51oDLDdxO2SqnIxxn0wa7zTSk0YaUHLNtc/xNyCOe3IqZK50wqWOvl1ZY7FIYIiFY7nbdnc3ZcY4575q1cXQj2xl4yBFk8YIf8Au/8A164+6mm0xRPdRyRwlTKG6ZwcAfnjmorzV5LixjTKw3BmR2Zj/CxABz25NZ8tzoVZWOkkmZWGeVwNw3YxzxzUslxGu5ZAzKoyOeK5SLWI1h8uadJ2MjI3XbkdBmsyPxdDaXEhG8XbHaiqcAcdc9KXsyfb+Z181/IlrKFICxKHD85bnpjBINYOqXF3Yx2t/qLvBbLETHaOQsj7jwxHYc5qpN8SbuC0+x2lzBDMxzPeCEGXk8KpzgHJxmvK/EfiC7ury++0Xks7xnDs5yxXOQM/WtY0zlrYqysWPG3iiPVbyRguAq7Dk5JrmbOOZ7FWaZI1U/IgbLHJ5NYq6hFNNKk2/LjjHzHr0rW0+zZowskeGB4bOSK6rWPKdRzdy61nHcSBHR5gnJdW6+nGPWp5PB6XcZusPuztPX5vTA7VesoYrdgYpmBA+8q8n8Kna/kgRIh9oY78mVnwo+oxSvYau1qYP/CFzLuZImcLznOCKkvNMg0mG3aRSBJwVbGfyrVvL57OVlkeSZGGQUPFcxdXkmrXZBhyAeSxIIqGOx0+n+S1sTEixj3FZ1zMPN8tgoOeuMVJaQt9l3hikSkfdGSeeeKoX7rPfGSNxtA+6w5NT1NW9CjdK+90SRXB68dOayNa0dLdVeMqWbBIrekwuWWNct61WbTbnUF3xtFu7JIwUn6etbRaOaUbnKFdoKYwT3ziokkkt3wjlJTyhbkflWzdWRtZtt3C8WP7wwD+NUrsJcj7uwL93HOfxrVHLaxY1dob6G01G1gEYKeTcKGyPMHVs44+lVo38sggZFMs5Hgs5bRZMxOdxU9d3rVjT7GS5MiqCSgDEYyeT6U2OO5ft5g0YGMEn1q8r5kPsKxplazl8tzgipYbr5ic5z2rBxZvGRuQyhSO9XEkDcdKw47rCjP86sx3QPQZFTys6FUNPfg0GbYM4qnDdeZwo+pzUqsCQDz7ZqLM1UkJOHY5B4rGuM28m4dc556VuswYY6Vl6lD1po56nka2l6j9ohHmbQF7KOTU8soIJH3PpXL6XeG3uBv+6P8ACt5rgzRjbyG9qmUWb06l42ZFM+7odoqndAMvzLg9jnNTyYwQapzdSSenQntWkNiKhESO3UUm7PsaRrg/dwPrTCwyARz61sjkJ923jrTWb8KarbmHNJIwwcUCCNjzmnR85bPSoVk2gjuacrFVxTEWFO8EkYpw6EGmB8jgYxR5lAhc4alTmRT79KaT0NS26/OD+lAHp/w1g2aXPIerPiuyFYHgu2NrocC92+c9vwrfFZPcBrelMWnt60xaAFJwKYXyKc33TUdIBtHY0FaSmAUUUUgA0UmcmlpgI33TUdSN900wdaEA6mkYp1NJpAJTm6Ui9aVulMBjfdNM/hp7fdNM/hoASkbpS0h+6aAG0UUUIBG6UxulPc4Umo926gBr9KZ/Cae/Sm/w1aH0GkZFJt+WlJwKQt8p4ph0EprfdNKDQw+U0C6CD7tMbrUiruFMZfmNAHJdxTlXdSMtOXg4qRdR46YpV60gpV60DF7ilpO4paaAB94UoGTikXrSj71UMmjXGTUi9aijbnGKlqBD160ZpqtuIGKfjigBF606mr1p1ADV+8Kkpi/ep9ACfxU5etJ3FKvWgBW6UL94UbqF+8KAJKTuKWk7igBaSP8A1lBNEf3xQBI1A6ihqap+YVJSJKQGloC/NSAUHBp6tuIGKYBzinqu0g5pgP2+p4rjtWs/smqSyAbUkHC12O6snxBaG4tgwGXTkcdfWkOO5z8L8HA/A07cAWJAAPt0qtCdu4g5ANPmfcmAO4/nUWO+LuicAGMtnkfw4pfO2Rk4qPevJxtBHPOcU7IAwR16Vk0aIcrmSMAHLDnB71LCrPhslNvUryRUIULyowwqaQyIqlePWmkO5WaQpNKFPDEbmPU8/pWnYx/MGTdljypbPaspl8xlbnIP51oxMVh2nhiRyfTNWKO1zsLGFTHEiYDoclmIArftrlrmSONyVj3ZAUZDccc9q4bTJ4trMpym/G7ByeecDNdPHcFbpZIN2wDhN2McYNJoq5ua1MbzS44ZGDsimPk9s5yK5z/hIJY2cON2NoMzcYC8gY78itN282GJeqI+455I9s964XxdcTSedbwusaNJ9/OP0qoq4pz5UW9Q8SRtAkLXChY8yCEEZdiepOOKwbjWnvFeNJyiKQ0km3HfhQaw7i4TSbooXjmYLjpkn/CmRzXM4VRhYt28AfTOD61qonF7RvY0ptWWNFG87IzuHykknHAz9ayZGmvJC7niT95Ix4yByB7cipr6d7i1he4dgroSu0ADg9DWPdSNbyRFHZmkUqFzwOOT78VaVjGUuYZpO5r4yBPNVnwFXkj0HvzXXRreW9wIZFNmcZZ2GWx2+lZ3gCxleRZVXCxyffZMA8devFa+sG4u9WnvHuVmKnaB0HtUSauXBNImsLNtSnkCyyJsJyxbgccmm3V0tvcCES71zgPIcL75HardmXt7ARvA/wA5zK3C/Tn61VaE2oZ4oleQ/f8AM5Ws7myH3EMMWzZc+cZOpjBwKryaGschlQ8Yz6k8U5dSZlWN4sFQSVTGDxxxipYIZDje7YIznoR+FTctLQpXLsrxwwsIFjXcwLdM1THNtkp+9LYyOR9c9q3/ALHHcyOsaKZGXYWPJPNZ1xolxBHIkZGxvlK5xgg5zRcmWhRdVkiUIQQOrEVDcWkSwKVwx77jk59c9qLy3uY7TG3DR9Np61lQrdbo1fO4n5lI4FNPUzkaujzRX1nqKX0a3QhChefmGWA49OtcvcRm0LopDKG79QK6nR5YbDVrtrhP9Glh2Nt4+YDg/niuavlLCR8A7jgZ6nniulSRySuZUMZku+pIHp3rrtB1S10PUrnVJtrbbfyo4S2MsRjd0984rmYLfy1AJOe5Xg0fZhcZDgkDoDzTuQWGm+3FpHOXkYktSupGMDGO9RC1dVUqNq9B3xUzbmx3I7Y60gu0BYqOuQakjumhZTngVBIxZeQyn0IqHzAuSccdqAUmbFveJu3cj1ANXzcrgEEmuZjmKONo+Y9K1LaR0yr4yRkVnKLOhTNVZtxGO9JdLuX3qrA+PcmrrfMvI4qLWZd7o566zDIQOuetbOnXRlhxuxiszVo/L3EHJ47e9N02Yr0yfatJaomLszZlcE4xk1WmXchx1p7ZVQWDD8KglnwpwOaiOxpKVyvkKxB601j81EufvAfNUO75t1aowuTbivPpTHcgg+ozTdzMDwMY65pjvuIGO2KYidPm5p9MThaeMEZzQImXkUbaRDxTgaAH+X8vWrOnwma4jQD5mYAfnUGNyhemSBn8a6HwXYi+8QWakfIu5j36A4/WkB6xZwi3tYIgMNGm1v8AGp26UbfmJ7t1obpWYwJptLQ1AhrfdNR1I33TUdIApGXbSilb7ppgR0N0oooARaWjGKVetADW+6aYtOc9qRaABulNpzdKbQAq0rdKF6UN0oAY33aa3SnN0prdKAG0H7poob7ho6AMoopexoAZJ901EtTOMqah6UdAB+lN/hpWNI3SriPoMb7tNbpT26Um2mJ6CUN9yl20jcrSFcSPtSN9405V4qNn+bpTQzlV+YgU4R7SOaRRhhUnpUiADFIPvU6m/wAVAxw+8KKB94Uv8VMfQRetOC7mFIBTl+8KoOg9Eww5qUDNMXrUi/eFSxAq/NnNSCmj71KG5pAAGKWiigBB94U+mj7wp1AB3FFHcUVSGhxHU0L96huFNIrfMKGIlpv8VG6hetSAlOj++KQ9aFbac0AT1EvWlEm44xQo+YVI0OBp69abtpy9aQCj7wp9MzgilD5PSmNDqZMu5Se3TFSL1oIHfmkBxep2LWl8eyEbgv8AMVCpOeV/Wui8QWrXFvuQfOhyOP0rlmkMbfNyAcMPSk9zrpyViZWIyWHH1pVcMCS2SOgqBmULyDg980qMEU5HJ6c1BtzItRuWGBxVnzD5JU81Rim8tgMZzVjeHY0DvdaCKueh5zU97OWj2quGXB3Z681GqhZimcgEc+vNS3CCNS+4dcYNBnqkO0+e4jdS0i7A2QoHTPH4102n3zrHK7DIDAbgcEc+lcvbzEMDhWxzgce9aljJGVDSGRA5ydnJU44qiYyZ1NzqEShxCFUsgZwWOR6YGOa8y8TRTeS1y7EoWyFU5J59O1dnJezOhkaRcEBULYy3PesjULWW8kdYggZx8zdR78ULQipeSscn4Z0WfVLnz/JEvUKWOB0Peuih8H3MrsC/TgKortvB/hM2MIG5SrDJUjGPxrvLPwvHYDzZPKTdg9dxpSqpHRSwvMtTw638G3MbJZTKz+WMAdepqz/wrqe6KyKjYSQLjbggZ5xX0CuiaVxPwzycNz/WtGMaZa4URq7LjDYyRWbrdjsjgoxPOND+Gt9/Y08NjYYGAcs359q6Sz+Bkf8AoayGGOUx73cPg59MV2x8SQ20IitiwDcM23AFVn8QuN4VVZscOw5FYczOtUYR0OX1D4IQWWDCxneXgs7bsfTmuevvgzJ5TOGkadm2lcYWu4m1y7Xa28kqQRg471LH4subeY5PmqTnaRUOUuhpGjTlqzyG6+HtxpZYtD0OAV61lXljJCwja3YrjBG3k85617cPEkUly3nwiU5J+7jHHSqF3cabeTZkj8oE5J25x3qedrcf1eHQ8c/s4/alMCGJ8g7W6Hnnmr03hs3l4QIzyc9fau51C40lZGMYDOOgxisq88UfMoSJFK8AqMGj2j6EPDx6mBJ4NMMfmuoEa9VPJ9qyLzSLZWbcqlj6DFbWqa1JIpxI2T+Vc/NI8jbiTWsZSe5zzhTjoZ1zocDE4j5rHvPDazOdy8Dpx0ro2Z8HGSe3FMkdxGSTgit4t2OKVOL1OQm8MrGpI4x7VBcaL5Me5eoHTHWullus5BPFU5pgeT0FaczRyunE5v7HJtwRhRVO4t3jywJGPSumMiFTmqtxHG6kHnPatoyuc8oaHKbnaUcsfqeKqS7lY10NxDGM4AFZd1CNxFWjmasUBOVcYXofWtmznaXDvyccVlta81fs28pAOtBSLvmFWB71ZjuGbGTx6VQMntU8MmMDFJmqZDqDE81Dp5PmL269PpU12vmKTnGKhs/llHel0FdXNQ7mIy7Y96rTNgkZp7TErjFUrglqmKLk0Pkk3KcCoAwbII4pxbCmolBcEDrVoxJAwRgBkAinqpZgR0pg6kMOF75qbG3BVsimMf1GKOelIjHd0p38VADlJWpk5qGpo6AJ0PQYzz+XvXoXw108+ZNeFfkVPLU4688muAt4TJIiL95jtHHrxXt+j2K6TpNvahcMqgtxjmpkBd3UE0zdS1ADlpHOFzS/dWmM+VxigBpfI6U2ikbpQAqtSs3pSUUAMopxWkoAKQnbRSN900gGMd1LTRTm6UwEJpKKUdaEA6mk0rdKbSARulNbpTjwpphNMBpo3fLjFDdKbQAUuaaaWgBG+6ahapSflNROeaAEpG6UA5obpVoBp+6aKD900h6UEy3Bm9qaz8HihulMbpQSSKagb7xqeOoWHzU0WjmV+8KkqNfvCpKkApO4paCMUDAfeFL/ABUg+8KVqroNADT1+9Ua9akX71MCRakX7wpi09fvCpYh/wDFSAUvpS0gE7iloooAF606kX71OXrQAncUq9aTHSlXrVIaFbpTY/vCpNue9Ise1s5pgxVoXrSjvSL1qBMVqbTqRV3HFACx/eFSD7wpoj2nOacvWpAdSr1pKVetADgM8UBMHOaVfvCnHigaBetK3Sm04GkMayhuMVyGvacbW8LqMRNywArsWqpqFoL22dONxHBx70hp2OCkkXIUtgelOjBZSd2SvUYxiotStWguCCNrKeRTGl80Bm/1g644zSNlJFsnJBHarNucyZz1FUYW3rgnBPepoD8+M0mdEWi/ChaRTnnNPmlww7kHOMdeKhDbmGDj3pWQP/e3Ag5UZNASHyXC+WNrL0yQRhs56AVNHqpjQjdhfpzVCTbIzOo3eWSd7DaRx0xUTyNLjyyGRhnkYP5U0jmuzSGo7shQdg6Z5Ip9rrnkyEvtAPHHBFY4ldSIzyG69qlg+Gt74njmu9PupC0A3PDEC7kd8DIzVcugKo4s73TPFShFIkxtGCuc1sL4pkmXh/kxzk14bDNq2hzOs8MmzODHIm2TA74rqNL1S7vbMTRRSNH1OBkj1JrmnTdz0qWJR6jFrcvlKBIeOetaemawxmBkcnd79K81s9bVYlJO/ceNpyD+NadprWGDFSmDx3qFBnX7dSPYI7yAwjYSxPJ5qeOYTLuG0Kw59vSvMo/EUu1drbU7kHJrQj8UeSrFZG5x8mM55pcjKVRHdeYijcWHXnHNZN5fbJnbPyjHPSub/wCEqkZ38ttx4+XbjHPrmpLy/NwwdmHzDld1LlZXtUatveKzsxYsW9+laf2VZoGcDqPvMc4/CuMXUVhztYBs8EmtSHXNqqrNuBHIDVEolqqihrCm3mYAKfccVhfaAZipAye1aHiC9UKsq9W6AmuVkvhFMCRzg8g89KtRRlUqPoac67oycgZqk0qW67n6Cs+61YeUowx56dKyLzV5ApUkBT1HWrUTz5VNdToZNTiZSAPx6VkX2ogBh2PXBrDk1hvJ+ZgAeqiqkuoblJDZNbRizCVS5pyTKWzu61Qur5UyN2azrnVWKkYH1zWXLcGY9cVqodzlczSk1Aq+VODVd9Sk7txWZJceWeTx61n3OollZVXJ+tWlYzlM1p9SOT8/FQrcGRx82RWRDDNdEEnYv51rWtr5ajLc+tUYastAjb0pYz0PakIwtLGOAKZaJVJY4xUy5WlhUYHFOkbaCMUFEEjnGKjhb5iTRI/tSJ3NAFgTZ7VBJJk4xS5NMIyc1KGxqtuyMU9VK5INMC7cnOaVW71QiWP7xLfMG6jpTh8pOOnpUaPuYDFSgZOKoQ9Bkg0/+KmqNtO96TAUDJqxEoZgCcZ71AvWrMKhnHOBmkM6X4f6Fc+JfElpZWq5uCskwXGeEVmP6LXV6X8R7a61C5sb4i1u45jGyMfT8K6/9j3RY9Q+Jl1eyoXjs7BmbjoWyu3P0avM/wBrDwH/AMIj8S5Ly1Hl2t4xkRlG0A9cUtw2Vz0hJg2GXBTGQwOc1IrV4f4A+JsunzLa6k5eH7oYt0r2q3uYrqFJYWEkbjKsKiWgr3Jy+R0ptN3e1G6pGIaKVm9qSmAUUUUgCjHymiimAykb7pqSmSD5TQBH60E0fw0lABSrSUv8NHQAJppOBS0jdKAEZvlIplObpTaAEP3TTG6VIfumo26UAGeaG6ULQ3SgBjcCom55qVvumom6VfQAWhulKKRulMfUT+E03+Gn/wANMP3akzluNP3TTaefummGgQ9emaj21IPu0yqRcTll+8KkXrUa/eFSL1qQQUv3uKRutKn3qBi7MHOaDTmpF61QCbdtOX71DUi/eoH1Jlp6/eFNj55py/epCJKKB1oHWkAuKSnU09aAFX7wp38VNX7wp/cUAJ1FJTgKQdapASL0paRaWjqNhTV606jbtFJiChP9YKKVfvCkBJSL94UtIv3hUAONC9aVqbTAeDg07du7UirupwTBzmgBKVetBpQMUDQtIF+bGM05etG0jkdaQzmvE2jmZGnQYkHJ755rj0UiY/3VOB716lMvm8HntjFcN4k0ptNnEq/6lzkYHGaHqNGd91h6U+M/NjPWoDIsnl7T1zk+nFMWRlkUYyPWpsa82prQMOBU+0noTn2ODWfHMARxUwmEi8HBpG3NdFiRJGiKMoZfdsH86bDbp5gLriQjaGU5x+FS28kbBN5yO+R0rahUtbl4kTPb1PNUnoRGLMldLK87vmHJYDla6T4dznTfEUMrvcbVJL+VJtLjB46cVFBYtIvEewnlmzVixUWt2rBgpHp16VLnY0jS5tzsPi18P4pmOq2yEpcbWZW+ZlBGQvvz3riPAFw2j6o1hcRpDYzODM7Lk4U7gMZ7kYr23wzdf8JJYi1nIcAbsnk4A6Vw/ivwktnrDTRI2FdTzwOopc1zR03F3RW8V+E9LXSUvJUW31XUJ2lt4oDiOGEdDjuTXEt4P1YW011ErTW0XV8gDkgDHOTya9H0/Qbm6vLdJGaRScCRudik5YgemM8U+40VrqSEW8bCILvUjIKrk5JGcdATRqjaNPnPK7WW+twwZXBX1WnQ6ncGTnKqOrYxivWn0mxt9PaafEkjHFuVGRJ6lv7vH1rDfQeJP3SlGP8AdqeZGn1eWyOBGuMk4bf8jcNuOKZceJXjYsQigdG7/nXYap4Jj1AIGULt/uLisa++Dsk8bEu5Q8gA5x3pc0epp9UqnPQ+LkFwC53AHkb8Vvab4ujvGlA2CPABVTkj6VyN78GZmy0crgZydrZwOx61hXXww1qxZ3s3mUDuHNFovqc8oVqb2PTfEmtRvYxqilX/ALxNcPda1iTJkI2n6D865b7L4w877JvZwvA3IT+ualXwfrt3zdM3PVVXA/nVKKMZTnLZGndeKIvMJL5PGF3Vm3OuJdHiTHt1qeH4fTrl3ibcv8RNSHwa6tggj8K0jyox9nUerRkzagJn4YgelQNeHkKCTW63hUqPu5PbjFJ/YezooJFaXRDhLsYDiVmzgn1FHltt3Z/Cugj01o8lxhD/ABelJJY+U5BXK46+tVdGcoNbnLXFs7LwSe3Skt7HMmMbvwrdksyrEDoe2K09L0tY8yPyT2xigz5blC305YYwMZJ74xUUyBMgVt3yiHAC5rIlXzHoFy2K3l7h1qaOHpzTvK96cp20CsS/6sA9ajdwRmlkfcpAqszHmgBJKF+7UbN3p7NtwAM5pgBNN8ylLZpu3NAri7tw6UUCnKuWAzQF0LHw1Sq2D0pnl7e9KvWmiSZXycVJ0WoY/vVL26UmNEiLmrEMZYhQeScCoIcsp46VftYWZ028sxwq/wC0eAPzpFH2F+xjoaWvhPxHrLR4N3draoxHZVycGuU/bT8PxX/h2C7Kfvrckqa96+DfhdvBfwz0LTJFCTfZ/tM4x1kY9/wNeG/tdawjaC9uGHCnv7iqQPY+HIpCqqCMEHGevbNelfDjx++kzfY71y1uxwu5sba80iXoSc7jn6YFTbSzbh97sfSny3Oa9mfVsMyzRJIpzGwyCKkryn4Z+PG2rp1/JluiMxwDXqu4duaylGxupcwtKRikpzdKkoZuo3Um2kpAOzzS0i0tMApHXcpoJwKQNmgCNuOKbT39aZSAKUmkopgFI3Q0tB+6aAGN0php7dKY3Q0AG75cYpjdKWg0AIOlDdKWkbpQA1hkVE3pUrfKtRYy2asaCg0pFGKYhp4U0wmntypphWpIdriN9ymVI33TUdAh4+7TKePu01utUVHY5VPvVIvWmL/rBUn8VSMGpV+Ug0HpTlXdQMGHGaRetObgYpq9apAK3SkX7wp1Io+YUxk0f3aePvCmLxkVIBnmoExy9aG60L1pWoAUGkakXrTqAEX7wqSo1+8KlHWgBKT+KloqkPoA6in00feFOpMYq0NSp1oakSNpU+8KSnR/eFAD6RfvClbvSL94VIEgppGKcvWmNJu7U0BLH0FPqONuBT91KwWFopN1LQAq9adTV606kNCLlTwcVS1LTY9QtmhZflPTPNXgMmnFADyaYdTyq+s5tLmlgk+Rc/L3J5qNG2qOMg9W9K77xLoSalal1H75BkcfnXnvzRsyPlecAHrSepehZWToo61dtd0kmN4Vh0461k5IwQcc1ehkDHJ49eaRrFmpbybLgY289iuRXQ6beGbjATHpXMwSYZR2Oa0ba4KtvRtrLWMrnVTaOut5mYHD7W7ACoZIX3Nli2R6iqNnfFmXPTv27VoJtkYVnc6UuqOl8G+JBpN1HI3zR4Ksu7BHHB6V6He20fiPT/tAcnaMhVXJP6ivGLdY7e5JwQp4PNek+D/EHl2sVssgBz96o5rM6FFSRfs7ZljjVQUdcEN1PXpVvVLiT+zpzBb7by7eOEkdkQHOBjvXV2ehqltHLDOCWJdv3e4jjp1qGbkSXb23lyQoxRW6McHn2ro+JXIj7rszyq1sZdR1GVJMq6nYUUYGAeuK7fTvh/f6orrZW7XAhjMkhUcKoHU1HpGipb+bdTgSzyuz7Pu5UIWP8sV6tBeXdxotrpNhDHaXU9urXckHyMqMRtjJ7nHes+VvRHqwlGMbs8Xjt4764+ywLvcrkN05HJH5CmJayW/JimCgkNGvLHg8ewr6ns/g3oknhyC2vLNTLHHvheH924Y+v96vJdY+Gk/hNp2N/E12zGTYuVkQDkYOSD/hUyi47nXSxEJvlPLtUvrTUPD1vE2hRJcrKdt/C2HHqjJj9c1iLYqRtQM4PXK9K7WPT7jUbzVLuOASG2QNM6r8uT1OOgNZd4y2wdx1wCCFxnjOKxcrHoRoxqdDO03wnHPbTXAt1K52livIrIvtBiikZjHjHYLXtPhrwpcSeE7eZYS0k2Zdu/j8a4zXtNd7ggp5TA8jOah1HFh9Tp2ukebPpUTYUI2W7Fce9c7q+li3kIMZQjrkdK9JutKabJLEA9AOoI5rmtWtBPu80lpFwAexrSE3I8/EUYxWxwc1mGBA/PFRnTIGhbja1dBcW6xk7RkDrWNcIVckHj0rqjex8/Vaj0MC4tVVyD930qrMo8vB5I6VraonK4P1rLmUZrZM8qpLmKS2vnSY6frWhtCxgKMYpsMYVs026lEOWI49M1oYq9rmdqcw3ccms4jc2aWaQySljwM03fjnFNEMcRiom+6aeZPlzio5mC8daBEfmEGmM+7OOv1pJOaYvB55FMQ4MdpJH4Zo3cc0wAKScH6ZpcfNTJHbvl6UueKSjNBDDd81KpywqNqdEw3jPApoRMBg9acvWmFxuwKevrTKHrU6/SoVq3FHnvSZSJrNR06ZOBXpXwL8Fnxx8StH04x74Ij9rnOOAqZOD+KgV55awbgf4eM7j245P9a+w/2Q/Ab2HhjUPFFxFsfUpFgts8EQryTnuCRU2Kse9a1fJBDcMoEcf3VGeigcKK+Ev2qPEYurgwK2dxx973r7B+I2tR6bpMm5sHJwOmPxr86PjFr51rxJKobKox75BqxS0RwiLtYewxUooRf3eKdt+WqOQdBdSQyoytgqeCODmvb/AId+No9atktblv8ASl4Vs/e49K8N+6Qe4q1p2qT6beJPA21wcipkrjTsfUavlsfkfWnt0rm/BPiqLxFpinIE8Y/eLnJrpGYbffuDWUkzoi7jaRumaWkYfKakobvo8ym0UgHF8jpQvSminUwEb7tMxTyaa3SgBtFFFACE0bvlxihuhptAA3Smn7ppWPy03d8uKAG0UUUAFN60rdKRaAEk+7UfY1JJ92o/4atD6C57UtNWnMdq5o6mciM02lJpKRAjfdNM/hp7fdNN/hoKHL92o2b5jUi/dqJvvGqRaOZX7wp/8Qpi/eFSVIBTlPQUi9aVfvUDHtUY61JTdvzUwChflYGl201qY+g/duI4qwvpVdV71Ohyc0hDl606mjrTqQDR1p1J/FS0AC/eqRetMH3hTqADNApO4papDQK3zAU+o1+VxUp5GaGAqdaV+lInWnmpEyNV3HFPWPa2c01OJBU1JgNbpTV+8KkpgXDUgCTtTKfJ2plUh9CVDjAp9Rq25hUlNjHLS0i05etQSxKcDSGhetADgcGnhsnGKZQDg0gHMvWuP8VaCzA39uoJP31AxXYrJ8wxwaZNEJUZT/EMEVQzyWH983PyjOM1ahG4EZxirfiDSX0m6yvMLHK8YxVFG+6xOB7c1Mi4mrCwXaSN2KthQse7IXPc1nW7B2Azj8K17N1bBKhgvVWHWoZvFvoLDM0bL+h6itmzuu+dwXqay7hWkZSCoH91VxRHI0PzIcA9VrnaO2nLQ6BpVmjIX7x6DNWNK1Y2dygztYHjmsW3nRiC3yn+9mppY4nXeMrIORznNQ43N+Zp3R734L8cIsAt5SNz4CsX6V1WrW6zW6yJJ5hDL8qt15GeK+atE117eYMThkOQSc/pXrXhPxvBeSIJ2DlecbtvXjGalScdGdVozWm5vLGFlhkYEJbMcE8B+c4PpxxXa6Lqn9kapb3MqqxuGEzhZMhmPyqCccAZri7yNRHLMjZgkfKKG3Y9aq218ws3MTFlEi5yORggj+VbRqJG0qd1qfWV54kMli05aLzLeHzNiLuCgjGCc+9fPnxV8YRahqJ8iST7QVEUg3gBhjJOMcVi6544u5tDnUXLxzyfIyxHaWHbPX615xcX1xfaoqzSswCr+8ZeenNOVRSFQhyO53mj602geHry3tZ1Cak4EysuSQBkYOfUVjXF5BqDGBuA2AAF9q5nULsDUGgiZljROCG6HGSa1PhzENU8WWCM4VFkDtJI2QAAT0/CuOR7dGs4vU+m9Ht7PT/CCtCk3+j2S70dcYJIGc9q+ePEWrMt9OG43Elec969T1Lx497fa2IJd8U0IiBU7U+UgdK8L8RzCNlA5cZ3DNPl5i5VpRTKt1q7eSwDcjmuavNQEr78gVHeXbcn1yOtYF1dGNgCa1hGx49evJmlcXCbCBx61i3cqZNU7jU9uRj9ay5tQMkjdh9a60eBVqNslvplkO2s1lJJOeBS72mYt0Apk0wijbJ/GqOTzCS4EUZPese+uXmfG6m3l6C21TnNVPMO7NaIhyuhzngH0pplxzikL+1RO+FpmRI0nyk/pUDSZOKTdmkqhC5NC9aMU7G2mSNPyqaasnPSnSfdzUNBDJjINtR+ZUWcHFLupokfu5pjOegFIzUqt2NMCWHdkVaVsDGKij+7U8ce5gc0DJI4/M74rQt1PCjkngf0FVY0LfdGTnHXFascXkqckZxxjk9On1qTWJv+CfCs/jXxVpeiWas0t5MqNtXOE/jbHsARX6IaNpdp4T0G10q1Gy0sY/JjA4GRjLf/AFq8c/ZX+E58I6OvirU7cJquoRf6KjLzBB/Uk16V448QLoujyOW24QsxJ9wc00XseG/tJfEJdN0+aBZQGxkLnGeRXw5NcNeXE00pJd2JGa9E+N3jh/FXieWFJC8MZzkHrzXnMa//AFqownJMeq06iimYBTfLp1OWmBr+F/EM3hvUknicqjN+8GeK+hdL1aHW9NjvYWDblww9K+YjgckZFd78MfFjaVeixuJM2srYAJ+5x+vNRJGkXY9q307d8uMUzjPHI7GlrFm977BTadR1pAItK3Sl200mgBKZuzTm+7TaaAKKKKRQH7pplSt901Ew4pskRvu1HUjfdNR0gENLRRQAjdKFoJ7UE4FACSfdqNulOZt3amE1a2AFp0n3aatKzblNBMiJulFFBOBSJEb7tNbpS7t3akbpQHUfH2qJhlutSZ2qTURbJqkWjmV+8KlqJfvCpV61IIF604feFN/ip69aBjqb/FTqTuKAEakpWoXrVIaHIeQKlX5Tiol+/Uo+8KAHr1pQaFoApMQtFKKSkAq9adSL94UtACdxS0UVSAO4p6yfw4pq9aUffFMbHp1p9NX71KDUCDoc0qybmxiim/dbNICWkpqybmxinikAUyn03bTGgUbWBp+7mkAzSr96q3AetLSJ1p22oYmL96kHWgCloAWkpaYaQD4z84p+c/Wo0+8KkXrQBR1PTY9SgeKZd64O1fSvNLq3l0udoW3AKeNw6160Iyx+Xluo5ra+NXwHvvCnhPQ/EjMXh1FcoAmCDjOOvNJmkddDxexdpMZGa3LV38os4VyvTbxXP2rGN9pGCo5Vjghu4xWzp8gVN4+YDgjP4UjaJfEgTk5YNwMUjQmJivzMoGc7cVYt40kTlcDquD0qeKBmkZgx+YdKlpdTaN+hQh3SNg8L7nrWjExWPEijPY7qhmtRE288Bep6VEu9stuDBenPNQ1rodKfcdNGQSyybfwzUa+IJ9Fu43QsUGAePenrNmMFgE9yajnbziMKkgHvUcvcrmtqj0rQfiQrxJCHUHqFLZPTmustdQiuoE8ttgkJJA78V83zWc8N001qChwSQWrV0v4kX2mrGl3ExKHAZW7Yx6VDpv7J1QxetpnuWqX3k25QAMAuM9DnPXNZliqO5keRshcY61yen+P7TWI1jMyl2/hJ56Vdj1qNSeWC+oNZuLW53KrCWqNVIy32mZ4zs5BY8VqeCL6HTdbyEUhYnJy3B+Rsdq5E+JMQzKGLKcfKx4602x8Z/wBm3EksSr5zIVHHTjk0rGiqpdT0az1l1hZRICGRsLGvvmuK1i4l853lIy4z1yfyqgvjX9yuPMViCCdwweKx9Q17zMZ+QYwdxyevWrSInWVtwvrhYRjOa5jWNSXOxRknvnpS6trDsSqncvr0rnJpG3FmbPPTNbRT3PLq1USXEzuSQahU7Msx47iql1qUNvyXGaxL3XWckIMg991dFrnkTkrm9dakkcZC8H6+9ZMt1JOep2nk1l+c03LHBqxGxXHpVpMxlLsWOOuOaTdTfM56Up6GqsRHzHE4U1CzblIpzJgHmk2+1NAyPbRinmm0xCqe9LupucKabI3l4NBEhZD8pqEvg9Kc0gIxUJbmmiRzdaTNBxtJzz6U5V70wEAqVY845pm2rMMecDNAD44+nNWY42YgD86jjjO4DrWna24XBIqS4xuPtbUx4Gd564xiva/2cfhA3xC8Qf2vqMJXw/YOGJYf6+QdFHoAcHvmuN+F3wx1L4o+Ik0+zRo7KE5urs/cjTHOD3PbFfd/h/QdP8J6BZ6TpUSpaWq7I1XjcQOXJ9TUm/Ka00626uygIFXCqOiqBwAOwr5T/ah+LAsrN7C2mzPINm0HGORmvbfid46g8L6JPO8qpKE4G/v0r86fHXiy58X+Irm6lfK+Y20ZzVx2M5yRz7F5pC7tukY/M3epFWiNdop9Wcgm2jApaKYCbc0vSnCloAjbpUkUm2Xep2N1DdcelMPNAG2kB7t8O/FP9t6SsM7j7TCu1u5b3rr+qkjt1zXzv4U16TQdUjuIydrNhhnrxX0Da3yahZxXUTApIvYcVhKLN6exODSrTF60/dUmordKYVp5NNoERbu2KKXbSUwClX1pu6nZ4pDDdTW6UtFAhjrhDULdKnk+6aiK0AJSN0p200jD5aAGrQ33TSihiNp9aAI6ZTj0ptWAv8NLjcp/OkJpzfKtBEtyKmt9004+tNb7tAho6Um6lbpTaQEn8BqGpT901E3WqRUdjm0+9Ui9aYv+sFSfxVIw7inL96kpV+8KBjqKG60DrQAjUi9acfSmjrVIBy/eFSrywqJetSR/eFMZKvelooqWIVetDUlO+9SAQHBp27d2plOX71ADl60lKOtJTQCr1py9aTbSqeaYx1KvWkoNJiH0jUgfPanUgGr94VKvWo14apF61LAKF604LzRjbQA0jFKv3hQ1C/eFUh9B/epKYKduokgFopu6nVIhpOaSlNJQAq/eFSggHJ6VEv3hUm4Dr0Jx/SgDp/hz4ek8TeMtKsVUHzLhVYEZ+XPJxX3j8cfhXF40+CN5pMduBcafH9os9vWPy8Fh+StXzX+xz4QXXPHVzqjrmOwAO7qM4xX3zbQW01s8E5yk0bRMvs3BrojTvAhT5ZKx+KOuaO7t9qVVWUgrIoHO4HnmqGnuCNo+VSeSe9ez/GrwWPAvxS8S6Ft2Rx3hki442sM9K8l1fTW069G1SY35C4wB+NcV7Ox6fLdcyNOwYYAJXrjg5rZtUUqSORkgnp+Nc9Y3BKh8KirxuHPWtq3mSOZdpyu3BOcZ96GXBl/7Okp2lQfwzVKbSCpLDaB9Ofyq5DdjlijYXjCnk1bjje4xIq5TuG61FzazOYexZgY8bvY8CmfYfJU5XBx0ArsG0WOSMsHY7umEGD685qtLppRCvlFx7cmpbQ3Fo4q5jUYHOG6r0z+NUpLffGAQpUdc8EfjXaz6G1xtIgAVeSzNj8MYrGvtMmkumNvassW3LGQ4AOP1qoszlHqcbLaRW8kjQv5cqjKsp596yjr2rQnCTt5ZODnmuru9DuYoRK1uQ5zj5cA/jWCumz+YRtCn0etVFS3OOc5J6FeLxlqG3g+YqthucfjVqPxsg3GVMsPfOaLjw7K8IaK2Yblw2zmucutLurZ/Lljwmcll5PtkdqrkiR7apE3rjx1FCUHlZAYHvg81V1D4gG+neWO2SH+HaGyR+lc8bF7iZNoYbTnkZz+FIdPaSaRyjKc5AUU+WJDrVJGjN4svAuPLyD3PGKoXOtXdxkD5d3pS/ZXZcbXGPUU5bTDKzdB2xVJR6GfvtalVVeZSZDuqeOEY+7VvywBUscO4cDmq0RMU+pTEO3tUqgDr0q0LXP19KT7OwOCOKC+UgjzuHHHrUtOaIqCQM/hSbTtyRQIaRkUbeCc0obOaRiQhqgEdf1qAnFSNIWxxULP83SgQhl6jFMeTzMDp701mANM3UiGxSpbv0peaaimnM2FPFUiRNuWHNSgYpkY5BPFTxr8wz0oARVyeeKtRRnjHNEdvuxxWjEqRgfLk/nUmkUmJDAEAJPTnpXY/Dv4f6r8SPEEGlaZExLENLKy4WKPuxP0FT/DP4W6v8TNYFnYJst0YfabuQfu4V9c9z2r7d8AeBNH+HOgxaTpEChRxPcsf3lw+Mk5x0z2pGqRL4D8BaT8O/DsWjaVFm3jbdLMes0uPmY+g9smr+ua1FpdlPLuVNq9cYAXPSrF5fC1tzuIXAOAowPrXy5+0Z8ZBYQtplhcZkkG04bHekXeyPMP2g/i7L4n1eXTrWb/R4zhmBznmvEoIwuTnknJpWZ7qaSSQ7pGbLMepqVV2jFaxVjhk7sWiiiqIClUUDmnhaAEopdtJQA3bTZG+Q1IelRSfcNAD4W6V6t8LfFiJaNp95OF2n5NxryiP7tSbjGu5SwcdGU4qWrjTsfTyssihkO9D/EOaduz93kd68H8MfEbUdEZI5ZTNbA4I/CvYND8T2XiC3WW3lBfHzJnmsHFo6IyTNmhulJuCsQRg0bvSgYlNf7pp1I33aChi0tLtpKQgpe1JQzbR0oARvumo6cXyOlJ/DQAlI3SlooAik+UA0zdkdKkm+7Ue2rQxG6U2lLcUZpgJUknCmmKMmnSfdNLqZyImbHambt3alb7ppopCBulJ/DRupGbavSgCT7ymoW+9UiyVG3WqRSOdX7wp/cUxfvCpKkYo60q/epF60vQ5oGOakXrThyuaQdaABqZ/FT2pKpDFXk1IvykGo1+9TwaBEgfJ6U8VGn3qkXrSYCUq9aGoXrSADSr94UNQv3hQA5qF606mjrQANQpw1DUL1qgH7qWmr1p69aBiL1qQDJpoGKcv3hUsQuzBzSr1p1J/FUgLTvvU2lXrQAlIv3hTmFIq/MOaY0SL1pSKFXmlqlqAyn01h3o3VLQAy9+9Apc5pgbbkscADNIQ4fKwyOKjuryK1hkeVlXaMgE8n0rl9e8aRWO5IX3P9cYrgL/xJd6tMwaRgp44PFaRi7kOSP1F/Yj0NdP+HLaowPn3spY8fw19C6hfCHYDKsRfgbuMHsa8r/ZBt1T4M+HyACxgz+OK7b4naRPcaTLNbnZMill9OK7YabmNrvQ+T/24vA8tj4h0rxOiDN/+7lb1Kr97NfNTKNStTBLgMwwrYya+qvHfjyD4pfCPUdE1baNY0qQtEx5JAYcD04FfKNqBGoDAgjJ68jsBXk4hJSuj6DDLSzOYubebRbhraQc5+RjwH/wq7bSHygSMN6hv6VuavYf2vapG5CzL918ZP0rkz52n3ggmUrIpwcnj6+9Y05XWpNSn7OVzp7O4URhuSf7vStS1kWNgoJYtx8xyB+Fc7BdRCFts+ZFOAmz8+c1dsbzayjI3NyGY4A9qclqbQkjqrbEMwAIJHIHIA9f0q9uhmYosgwehORmsK11SK4cJM/lHIBZTkgVavNWWK6MSsZoQPlYgACszrVjf0/T4WYOm3cvOFGT+dVNQ8Ni4k8x0YZJOWOSBjgZ7VnQ65LbDaxARufl6/nWlD4jTAZ/MbcMjd90e2aLtGijCS1M268Mie3VGkkUL26j2zWXD4TDTFpIRLt+62MfpXWtrCTbiEYZGBkDFMuLpdsZG0hfvYPWj2jRk8PCTuZlj4TtplcTBo1bA4IAHNQ6p8N9PbdKgiSRcY2dTnr39KvtqEapIFGHHQ49xVePUZDIQoALDuc0nUl0NfYU+qOQuPBtnFK+AXZT6jH5Vkah4bt4pDhVGPQ4NdxcTeYZCQqMfTr1rn9QLSysNq/XGTWkZto5alGEXojkZvDcZDYJ9emayJtHHmABeD3xXYTuRuzj0J/SqU0Py7UYP/tYx3rSMmcsqcWcz/Y67TluR220gsAvC9exxW7LCIiwPJ6hsVTldVY461V2cjgomXJa+Vg45qCQdeauXUhZuuBVSTvWsTOSsRN8vaoHYjP8AKnSTY4xUEso6DvWiMWREYOc/hSNJ8ppzMCCM1HJhc0ySPzsNjFRM/fvTt205xUDSbpAMYpoh6hzuzmnbhTd3zAU7B9MmmSxcinL8vPX2qMYzz970qVELMKASYcseBitC3tWVQ0gAUVFGu3AwAfUmrUa7pBHhpJW+VEUEkk9sVJtGPcfk7SR8q9QW4Huc16h8IPgnqnxQvFuCklnoScy3kiEb+PuouRnJ468Dmu0+Df7NEmrrb6z4tUQwEKYNNDHe+DnLf3RX1ZZ2Eel2cUFrDHbW8X+rhjUBE47e9K5oosoeF/C+m+CtBt9K0y1W2tYRwo+8zdCXP8X0rXmuEhiwWZyQSdx/lxxVeacdWbpzXmfxS+Jln4X02Z/PxJt4JbGOakqxhfHD4uQeFdLmjhuMTFcBQ3I5FfD2sazd+JNSlvLmYyFmJUEdK0vG3jS68X61NPLIxi3HapOaxY1Cr0+mOMVqkck5ChQBilooqjEKULmlC04CmAKu2loooAKUCkBp26gBrelMZd3FBfL4xTl5NACRptptxxHj1qeq9wdzBaAGwZVhgjPuM1qaVqVxpFwkttIYiDk4PXis+FNozUobnpStcL2PbvB/j611yARzSCK4GBgnOa65iByDkHkHsa+ZkkeORZIyUdTlSpr0nwf8TG+S01M5/hWTPT8Mc1nKPY2jLTU9O3Uu7dUUEq3UQlhYSRn7rKetS8r14rOzNOa4tJQKWkMZSN901LtqKTgkUAR0pNH8NJQAjdKWiigBkn3aY3SpH+7UdWtgGUbRTsc4oIpgJnaCaa75U8U4/dNMpESGMPlNMbpTnftimE0CEpG+6ad/DTW+6aQAv3aaSfSlH3aKaKic6v3hUq9ajT71SL1pDQfxU7GaTuKcv3qBijgYpO4NLRmgApopWpF61QCr96n96b91hTxzzQMVfvCpV61Ev3hUo60CHUgGKXd81KakBKReGpaUfeFADqTvS0CgApAMUo60rVSGIvWnr1pq9acvWkA6lX7wpKVT81DESUUm6lqACiiigB3WheGFIvWlXORgUBYkXrSA5OKTJ9KY0yRglmAIp7D23JTwM5zTJPk5rF1LxXa6en+sGfXd0ri9W+IEkzskJPpw1aWuTzJHeXuvW2n5zIoP1ri/EnjxpN6W7YbGBg1x15qlxeOxkc81TZieSMmmokSn2C6me5bc5yc80+JlQqMYqNeBk1E0m7OOMCtVuYH7Ifse6gl18E9AaM8hNhGc9q9g8UWputNaPPVT0FfNH7AuqNdfBexDHPlSbQK+rrqMXFqGA+6Olb9DSG5+avx0hvPA/jy8XmO2uF5YDAJ78V5iix3EQmTDK/cdq+uP2vvAf9taDJcRxf6TCu/zAvUZ6V8T/D+6mns7m1uGw8EhGCc5Ga8yvFnr0KmtkdGoA++cgd8YxVHXNDTVogeBMvKSemDyPfjitCRfMVgRipFbaoXGQOxrzE3FnsqKnG0jzdmms7gxyhoyX4JFakdxuLKV+6Mhs9a6XWtGi1eDLDEyjKFRx+VcLfR3WmzFJk24OA2eorpT5jzZ03SfkdJHdKY8FVyfvMDyanjugi7isjKeMk8f/WrlY7tixEhXaOeeQfwq3DqkeCOCx4OMgflTcWVGpodH9sfA8ogDPKtznn1q0moNCADMw2nOVIHbpiuTXUwzcED68ipnvItqqpXPdgCM/rU8pr7Q6g6kG53+YfQnk/jT1vynAfk8hSa5NL8R8ggkdg1N/tJ9xAGSehzS5e5Xtux1UmsMrMNyq7cA4yKhXWDCzA9R/FmuVkuHZmB3BhyDjOaY90ZCSdynGMEUcqJdZs6v+1EuGyXEfHXrVBr7bn5sP3HXFYIuSinJyPY0n2rKSE5ZmxznGOapRIlULEl0N7kjzM9WPy4qp5xXdkkheoHU1FcXT8AtlfYYxURZ9zheSRwc1pFHPzMJbw7Ch3e5K1nyXKhmbk47VJceZtUl/mP3hnpVFkLdX4b2rRI5pNtjppRJ2xVWaU/dAyabNIseeckdqpyXBY5BxWiRk5dxWPzFiP1qu3Gec03zG3YLcGo2YmTrxVoxuSM+1TTNwY+gpm/cpDfLUM0xVSq8mmQyZmC98VXdgsgOc09VaVcP8i9260jMkZGwbiOhpiF2/wAZbAFJ5j5woJ/SgfvGBKn6VbjhdgFwQT/DtpGkY3Io4S2Gbg1bgT5gyqxHZiMVe0nQbnWLqOzsbZ7y7c4CwgsB+OK+hvh3+ylcXEkN94plaKL7wsIe4xwC2ePypFqLPFvBXw/1rx9qP2XSLXzwpxJOc+UnHUn/ADzX1p8JP2fdG8Axx3VwqaprH3mnlTKoSOQFya9K8N+FdO8PWCWmnWMdhbAY2wgKW92PettVMMeEY+49aRtFWGRwkSM3O5gAWbBOPSpZJMfebC1XmmaNslgK4rxj44t9AtZZGnXKjOd2MUFXS3E8feO7Tw3YzHzVEm0kMxxivhn4pfES58Z6tIiSH7KrYPzfe5rT+LnxSufF2pSwwTMIASG2tnPNeZiMcexzVJM5KlTohYotqtyOfapBxShcLnNFanKFKtJUirQAAUtFFABSfepOtOFABSbqWmkYoATb8wNSLSKKcBQA5etV2XdNipnbapNMioAeFwuKQdaevWjae3NAAtLz3I9uKUKfSikB0nhnx1d+H5FRy01rnlN2MfpXr+ieJLPxBbq8Eg3Acrnmvn1cjlSAfcVc03VrnR7hZraRkIOSB+RqWhp2PorlTjtTlrkfCfjq31xFhmcR3OAACc5/TiutzjjHOMmspaHQpJjqjZd1OZuOlNDVKGRsNvFNqRueaYVoGJSFuM0McCmb9y0bgKW+XpTKWkq0QwxQ3Sik6mmOIuMio2+VakzhSaifmp6iluRMuaTbT26U1aBDSaa33TSu23tTfM3DGKBCr0pG60/opqMtzVIuOxgL98U/+Ko923mpevNSMWlX7wpF605eGoGKwpi9akamfxVQC00dadRt+agA61IvHFNC8inL1oAVeGqRetNX7wpw60DHUv3qSnAYpMQ2lX71G35qXbtakAtC9aDQvWgB3eiiimhoRfvU/vSKPmFOpgFKDSUu2kgYbvmxU20VEOKeJPak0A/FFM8wUya8jhXLMBSJ2JT3OM1FNexWoLO4GBzmuW1rxpFa70jfLdua4PVvFl1fzFQ+E74NVGLsS52PQNX8cWtmzBHDMOB81cTq3jm4u2dY3IB9DXMMWkYs53Me5PSoWYx5AGa0UTKUrk9xez3DZkcyUsC5waZChlxnirSKFGKu1iRrLzQFGck1IV4zUEzYzQIhnkwcDvxSbdqNnnIpgUyNU5A2nPQKaa3A/Tb/AIJ53G74SxjPSavtSH95blcdAK+M/wDgn7Z+R8H4ZSDl5MgV9lafN8oJHUdK3LR578VvDMWveHb2Bost5LAHGc1+T+pxS+Dfi5d6dODFBOzKVbjHXBr9oNStVuY2UoCGBFfm7+398H20XUrLxjpcBQ27AzFV9wDWFWN0dNGdpHm8kXzMy/dXHPc0ir61n6Bq0etaPa3kTb1dM5z37itHd1NeHONmfU05JxGGPHOePSqepaNb6sv71cnGAfSrv3iV6D1pyu0f3etY80k9DVxjNWZ51q3hqbTWdokaZF5V+nfGMViNI0efNXYfQ17MvluFDpkL0zWTqXg6y1NXYgJI2MNjgV1U6itqedUwltYs8sF15fKgMfc4p0d/jIb5iei44rd1f4f3dnMfswFzERk4+U+tc1NYzxSbDE6Pz1X+tdMbS2OGXNF2ZcW+HTZ+VSR3AkbeQ3GazxayqoY7lz6jFSw2smdu7huCxbgVXIZ8xb+3TMBGHx/tY5qNpmwymQsx6CmpbncSJFOGwcGle1Xr5mD/AHj2ocLC5ySC6Xb13Y6ipy0kqnbtC1SigWM5VlJ9QeTTtzBgACG67s8flS5bFXJmiZVAYfeOck4xVa4uBk/Nt44xRcNJMzbm+U9qybtnyVVsp3b0osyZSsh8tyqszGQs5qncXe2I7eo71XlcLkEHP96qsjOZAuCc1pE53JhJcfeB6nvUH2gHPYUkwLsyxncR14INOi06WVXUcYxksOBzWiRm5EDTDdnkiphbmRSznataNro8ildkRlHeTGFH1qaSxRQTMdxHRRSbsLlctjJCPLhI/u+lJ5Pknc3LD+H1rTWzLqyIG2kcKoz79adZ6VJeTCKCKS5lJwEhQuaBqD6mQYpZmxu2qe2KljtQvXBNew+D/wBnTxf4kKO1mun27f8ALWZsED1IxXufgv8AZJ8PaPIj6w7axcLyVztjzjpjvT1NFA+SPDvg/V/FF0tvpWnzXkjHAMSkj1POMCve/A37Id3dyR3Hie++x+Zgi1g+dz7bs4FfUmieEbDw7CINNsobG3AwY4VAB9MnrW5DZqjMVXardVHQ0WZqopHHeD/hrofgq3SHSrGOBFAzIwBkJ9d1dV9nVckL87cH3q/tVVIxULP2C7qmzKK/llWAJqK4m8gZpbqbagkztx2rgPGnjaPTYXRZBvI65xiizFdLcPGnjaHSbdyZFVsdz0r47+LfxTuNcvZLW2kzGxwzA9Oat/Fr4qS6ldSW9tMWycFg3vXjxZndmZsljyTVpM5alTWyGqp5ycljkn1p9CrTgKs5R2eMUlFOVaYCqvenUUm6gBaaTmlJoAoAUDFFFFABS0AZp+2gBoBzTtppwwDnFKWG08YoAryt8xQc0Rkg4xTbdS8zsT+FWQuDnFADV607BI4OKcPpS7TQAnOOabtp+00u2gBtHPalIoFADrdpbebzYpCjgghh2r0/wf8AEcXG211KQLJ90P615e3SlwfM3Z57Y7VLjcadj6PWQSRhkIZCMhgaVvlwK8d8K+PLrRGENwWntmODlsY9O1eq6brVprFuJLaVX4y3PSspRsbRehbLcUlDDFJmpLEkGVNQ1MxytRMvFUhhSUtIaDOQUn3VzS0jfdNCLjsJu3KRime1KtIfWkTIY3HFC0N81DdKBEUi5poWpG+6abQJhntioqkI4zTcVSLic/jNTL6VEDUitQyhR1p4+8KZnmnr1qQFam05qbVAFKPvUlO70MBy9aP4qRT8wp1IYoODTlbLdKaBk09U+aqAetOpFpaliBetONNBpd3PShDEpf4qXFFAgoopaQADShstjFJigHBpj6DytKDTfM9af8q8lqGFxCcCo5pFQcmqOpa9BYI2WHHfNcLrfjR7h2jhbGenNVuRzJHXat4og0+N8MC2B0b3rgdY8YTX0jJGxAPvWJczTXUm6SQtn1qBY9mTnNUomUpX2CRnkZmYlmPc1GudpHHNS0Mv5VRncipRCWwcU9YSzDnFXY4wEx1pgQxIAMYp235qf5Z3daXbjvQAyT5VNZ0+W5Bx7VbuJwqMAOaz924/WgCa2HBqUpuyOOaZAuFzVzTbYahqVrbEEiaZE9+SKa3A/Wr9i/Q1034L6Iu3BZfMzj2r6KgYxhQOa88+Bvh0eGvhfoFlgfu7ZMnGCSRXoca7sVuBoRt5oB6V5h8dPh/Z+OPBOoWU0KyFo2AVhnJr0uNvLjqG/sU1C1aJ+mCCPWpkro0py5ZXPxZ0WGf4e+LNV8MXq/LDMzQgnGQT0xXeKvnKNrAFhkV3/wC3t8Bbzwrrdt430KIvbKf9LRFyQM7c5rxbwX4mt9d02B8tyBnnnHqa8jEQa1PfwtVP3TqOUbaR+NOSQHORVjy1C7VORjqarSKYe2c158Wj2LC7jmpluNo9/eq55jJzg1GMnvT0FdpmoLgbR8oBx96oprGyviv2qBZUAOdpCE8cc4qn52MA9PWmtedt20UryvoOXJPVoqXXgTRb7JSaa0kB+VGG8H8ciseb4c3CSMIsOinILcA10q3hYDcyHB4bODSyam7NgSKPTBz+ldMa0onFUw0JHHt4Bu+SlqFIOc7uDx61Vk8I3FrMI3i8wsM4z0ru59Rby8GVumDjgVXOsRqNrReYQMbmbjrnpit1XvuccsKlsefroNwt0V+yvGF/iVcinNpEigl1dR67a7ptVt2Y7VVD/s1WfU41Y/LwfxFV7Yz+r2OFXTC0n74ukfOWCZPTjjNVLvRV25iSQqTz8vNdjNfxzMQQpORjt3qGWeOWTiJsY4XORT9sZSw+pxp8MvMrKFZG4wWTg/jnio28JMzKryRqO5PIrrJMybdoyQfQ1UulSJT5+2Mf3pCAKaq83Qj6uYi+H7K1VvPklnZuijCp+XU1aRltYgtvFHB1DOEyxH17VpaHomp+LL0WejWM19MTj9ypKDjOScYFezeGf2PfEuppFLrt+mmRPz9ntRvkI9N2QF/KtlGcjK0Inz0yLLMIwzyyMeFiJYn8AK73wf8As/8Ai7xeqXUOnmztGP8Ar7njA9cd6+yfhz+zn4c8Dxh7bTfNuWGTPc4kfpyQccV6fD4dhgCqIvu9C3JH9K3jT01I9onqfJPhj9j3S45FfVtQm1KReXjjUxp06dTmvZPCnwo0TwvEkNhp0Nvt6sEBY/jXqbWvlnaDg88AcGolt+pxhq05B37HPLo6RqQy/LxxjpUy25wADx7LWlNC5OMcUxbRi2MVPLYqL7lBrfapNIVAUgjA9a1DZlV5PH0pj2CyKRu/T8aTiyuZGLuJ3ZXAHeqlxKYlDADkHvir98VgIBIA5GBya858X+JhawyKkvlqpwWJxj6ipsw5kU/GHjSPT42iWT94R1z0r5R+LnxQczPawy7p34+Vvu881c+LPxaVZXtbKXzbgkqSpyB3zmvDLqR7ydppWLyscsxpHNUqdiJnaeR3c7nY5JoAxS7MLnNJTOUctOxQq+tOpgJT1ptOoAG6U2nGgDFAABRRRQAUtFSKtAAoxSgZNOCZOM04R4Oc0AN8uork+XDnuatqvOapagfmRPfrQBLbxgKDmrCqKZbodgFTrF70AM8vvSkYGcVMEx3pCtAFc96OanKjaTTWXtjrQBDtpdtO2/NiloAjIpVp22kIoARs44ODVvS9WutHuBNbSMvqoOc8VUpGzt4OKLXHc9Z8M/EK11REiuWaK4PGW6GuvjfzF3IQy4yGHNfOy</t>
-  </si>
-  <si>
     <t>qyn7xxnPoa6vw/46vtHxHMxng6FehFZuPY1jKy1PX92Vwcg0xulZ2jeJbTXrdXt5lZgPmRjhhWk2OAOvcHtUj5kxtL9KNtLSYhhOBTC+R0qST7pqLBplxA/KtNLdae33TUVIHuFFFLSJI2baMYpnWnyLwTTBVIQ70qM0/dhQcVCW5NBcTCqVaZtyakFMoF61Iv3hTF+8KevDVLAVhTKkamGmgEpV60oGKQ0wHdKevNIFyM09VxxmkMReGqVetMC/MKevWgAanfeIpu6no2CDQxC+XS+X3pfM9qXzKkBu00qrzRu5py9aAE24pMU76Cm7vWgAY4GaQqfwqCa/hgUl2AArmNY8YJFvEZ5HAw1NK5PMkdLcanFZqzSMPl7E1yGueNGyyQ9PY1y+pa1cX0h+chc9M5rNZdzbiSTWijoZSld6Fi81Oe6kJaTOT0qqMZJK/Me9P8AlC9OaT8KszEqOT5VNSUqx7xzxQBFGpbFSCPLYqRUCVNGAxBoAjWHmpVTb3p5+lCjcQM4oAj25PNQ3D7VI6mpp22ZxzWdK5LUAVpmJeos7eamk+9mmIu6QUAXLePKgE4DHrXf/AbwjJ4y+K/h6wQZVrpXcdeAa4q2UCMsTjapP6V9HfsC+FzrXxuS+27oLODzGPoSDVJAfqtplmljpMESptCYjCg8AAYzWjBFuwc1AzKsaqg4OSRnPfNXYY9sYOa2AcF+XFTxx9M8j0NQnpT45OgAoF1OK+KngWz8beF77T5oVeOWNlMbDg5r8ePiZ4I1D9n/AOJl1p04ddNuHJgOCBj+6BX7eTxrcRlSud39K+Z/2tP2dLD4teELrNuq6lEhaC4VPmDAjArCpDmR1U6jjJWPhPRNVhvrVZVOXIB69K1Wf7RlQNpHTJ614lpt1qXw18QzaBrCsksJKMsh5wDwc16xp+pRahAskTZyOgNeJVouDPqMPWVSNnuWpJPLymTu9KIzmnMCyHI49agkJVd2OnauW9zraHMw3EnkVEXB6KM+/IqvJchgRzupv2gL7VojO6RNImckoM+1VpoxkDBXPdeDTluDnhvzFMku23Zyp9q0RLkiGYF+FLZ9zxUBjcHLNU7XLN0UVBJI27J4X0pmMlcj3Dng57HqaZ5Z7qf+BUlxOkDDEmSe5GMUmn6dqGv6klnpttcalescJbWylm9TkdAMc8mtIrmMXJR3I2aOPOSobr8x4qOKV7y7itLSG5vrubhLaziLyE9wVBwOOeTX0p8MP2Hdc8S3EWoeMbr+wrJ/mFlB880gx0zkbfyNfWPgL4GeEfhrZiLQNIjt3Jy9w6h5n9y5rsp0HLVnBWxCi9D4v+HP7IPjTxoq3WtOvhjT8BhGf3lxID0wuRivefD/AOxP4C0aKJriyn1W8HLTXkpZc+u2vo2OzdT3z2Z+SPpUrWoRSxau6NGMNjz5VpTPNvD/AMJNI8KR+Xp1otqrdVt1CqfqOSa6WHw/HBGwVWQHGehFdAy4cMO1NkBbJ7VqZO/UwZLNYXXj8arzQhckH8MVtXCBuStUp4QueOKBmDMgWTcUyRVb7PuY9s1ryRh5DxTfJFIqMkkZi2oZQwFOe1Ve2M960o7fy1APrx70txbhlyPTpQXzIwZFXLoeQOnvVK+u47OMFVyzcDPbtV3VrhLWJCBh/WvMvGXi42qEJIPlBLOTgLgc1JRT+IHieOxtXd3jXZyR0xjnOa+M/iz8eHvrm4sNH2yq3+uuiCO+MAU/47fHWbxFJPoWlTf6MvMt2vWQ56e3NeEICepJOME+vuazZjKfREjuWkO4s3fcTnJzyaKQL93nkdT61Iq80jnE25GKBHUhGKFoATy6PLp9I3SgBNuKKd1BOKMdqAG5wKbupXwvGaYzYoAcDTqao71KqkrmgByx+9SKmGBpY0I5qU/SgBoGTTvLoVTuFShcUAN8v3rNuG33SjHQ1qGsy4Ux3SnrnNAGhFjaBUwFQwNuXgc1PtPpQAlG3dRTgKAG+1Jtp5FG2gCMx5BqNl21YPIqJ175oAj7UlObpSCgAC96aVxUlFAEa0vPY4NPZabtoAms7ubT5Fkt5DG2eor03wn44h1XbaXbBLpRhXzw1eVv93kU6GYxsCvyvnIYHBqWrjPoE5HaiuB8H+PBIostQky68LKT1rvEkVwCpypGQ3rWb03LWo5vumoyKkb7ppvrUXuaLRakTfdNMqWQfKajP3aYmNozgdKKRvumgBrNlcYpjdKd2NNqkLcRvuVFUzfdOKjoLRiUqv8AMOKQUY2tmmUSipB94VGvK09TzSYDqbTu4oVaAEXrQy0oX5qdtpgIh7U9etMUfMKl4zUsBV+8KNtKp+YU5qYDNuaevpSL1pdtADqQ80q9cUEYqWIF5binVBNcpaqWLVz2qeKo7YMFO73zTSbE5JHQ3F3HboSzAYrnNU8WR2obawLdua5PUvEE15IwVmC+mayJMzNljk1aiZuRp6l4iuL52AYhD15rIILsS5LE0+OPZSkYq0rGbdxgT0FJtqSj73FMQwLQVpcbaeqlqAIgtSKAOKcY9pzSYxQAjDinxA0m72qeH6UAJiopG2A1YkkCrnrVGVtzdMCgCORixqswy1WqryL82aAIJFxzT7SPfIGzRINy4qxZw7SOaAFkYhSoOAeM190/8Ex/DoZ/EesNEcYEKsfrXwvcD7wr9Rf+Cfvhs6J8F4rkxhHu5d5OOSK0iB9VWC5kJJyD2rT3/KABVDT1+YVeK4rQBxGVJpqcsKevzcU3hZBzQBKAM88iq99p8d1CUYbh6HnNSmYKuTUUt4uAAMkEHGcd80FX6n5/ftxfsoy+IoJvFvhy2/4mNvulljUcyAdRXxJ4G8ayWUxt7lZFZSVeNuNp9K/cHxF/xMLW5iaCORZAflI7Y5GfpX5U/tjfs+TeDfEj+I/D9jJFbXDb54I1yo5rnq0+ZHVRqSi+ZGfY6tFdwgq24Ng1ZMwjYHhhXj3gvxgeIpTjAxtz+GPavSra9S4VQGwTyOeK8GpT5GfTUcQqsfM1pI45lK8IT0aqs2nyKp4yO1J5g4ByR6jpTxc7f4iaUdjdpMoyW7r1iwPY1DJbttyAUPr1rQa6fqCKgmvHDbNoYGrRjKJnNDNyRKgHqxqL+yr67aNY540ZzgK5O/2wo5JrvPh18KfEHxa1b7D4f0+STb/r70DEMA6klu/0r7w+C/7KnhH4Y+VePbx6z4g8oedqF0m4o3fYDwtdtOi5atHnVsRGGh8mfBv9inxT8QGj1DxLcnQtDblV24uZ1xxhc/KK+3/hh8EPCXwn0tLTw/pEVswGJLqQB5pT0yzda9H8kAE/xEAErgBh2BFNaM7cbsV6MKUYHjVK8pvQpNaqo4NJ5aqMVM3pUbfLW/oc2vUrt6Zpki9VxU+zLA5qKQ0i0yCSPCkg1Cy7hjFWSMjFRyYXtQO6KEsWQQBVS5UYJPX0rUfkHHBqrdQgxnPXjmgZiGL5jTkjDZqxLGI2xSKu1aVgINpbOR34PpUOoMIosA8nHNaKqGjKKoLHkc4965zXr1YYwQdzklAnQZ9SaBnH+MtajsrcbTmXJBJOAoA5Oa+CPj98cjq1xcaBok0iKsjLc3Kt1PUqPb3zXoH7Vnx6NncTeFdBvC04OLyeI8JzyoPfpjNfIzZZixJyTyWOSfx9ayk7sqUyJYfQtjvk5J96d5e3PFSqvFOK/L0qTnIB8vJ6VMyhc5GPT3oKjZjFKuXjGTyO9ADGGBQq0q/NyR0qVB04oAj2Gl8vvVhVBPSiRO3b1oAgI+XFRtxUrfL71C1AEDEmQU/bkCkZdvNPjyxHFAD4xVlFpIYelWVj5AoARVpyxluByaeI/enKpQ7geRQBFtx25p3PpUkalpME9e9TC3y2C1AFQ/Ss/URzG3Qmtl4QpPOazNShMgBzjb+tABZtwOau7jtrLtSVrSh+agCRV+XNKBmnhsDFIW44oAQ9KBSqC1OC5YDNADNopjJkHmpMUjUAVmXHGaNtPb7xpMZ4JoAZTlpfLK9eKKAGk0qik205etADHX5TUfl7uKsbacyjFAERBXGPvDuOK7jwb43NuqWd4+9BwHzjAxXEsu4daGU54OAeuBzSaTC7R70s6zRh4yHjYfKwPBpN3XivK/C/i6bRZBHcMZLQnBBPK+h/OvTba8hvrYS27iVGGQR1rHl5TVO5Nu3Z4prUYO3pSUhjcdaa33TUjNhTxUY+bjFAxi0wnbxUn3TimMM81RUQ+8KjqXotR496YzE/ipTRS0DJI6cv3hTY6ePlwaAH0UitubGKdQA1qUGik/ioAX7pzSq27tSUn3TQBIG2t0p+7PaovMXbnPNMa6SPOSB75pBsWM+nWjeB14rKn1qCEH5uR74rA1HxKOQnJ+tFmZykrnWzalHBnkfXNY+oeJY4UbDDP+9XFXWsTzSY3EA+9VHdpDlmzVctyOY1NU8QTXTHaxC/XNY8jM7FmYtR0oq0rEN3EzxijbS7dtFMQyilYUu2gCOnKuSOadtz3pwTBzmgBvl/MDmn9KUUhNABTGpxNNbpQAxumalWQLGeOaizntRtP/1qAGy5bJpFG5aeB3NKTwRQBCRUMid81K7bcio2bK4xQBCy1ct12KCTxVZeWFaUO2PbuXcMHjOO1AFKSE3VxFDGNxd1XHTvX7J/s56CPD/wn8L2aqFP2YO3bPFfj3ocQuPEmnxgbRJcxjPXHzCv2p+GdusPh3S4wMLFZRqPyHNaxA72yG3FW2kFUIZPlPHSnmRm4wa0An+0HdgL+tMkkZ+1TW9u0n3fmI+8vQilaEKxGQSOcdD6n2pDSb2KqZyM9KXy/myOlZt74v0LTv8Aj61fT7YdCZrqNcH35rFuPjF4IsWPneKdHQDrm9Q/yJqeZGipSavY6a6gLLuHUdsetedfEjwRa+KdJubaa2V96bdrDPWtdvjr8PmXavjDRS56KLpc/rSL4+8M622bXxHpUgPTZeRk/gM5o5k9Ai3F2Z+aXxj/AGP77QtTnvPD0Lwvy4hZeH9RnPFePeH9eu9Dvm0/VoGguo+GhmGGHav2L1DRNL16zcStFdccsjAj2IIr5y8dfsp+Hfidqc1jqluLS/jDNZ6jF8u5iDhXPcVjUoqSOynV5dmfGtrqUV5kiQRgddzY/Id6ttiNQ7EohHBbFdT4b/Y7+Ln/AAmmq6DLo8VvZ6fJkapczYhZCcAg45r6l+F37GFhpOj6jb+Jmt9anvFQfaY1KtAQwPynPfGK876rK53rHRsfHGm2FxrVwttp8Ml9cSDAit1LN0/ya+jfg3+xXrniq4ttQ8XSf2PpYGTax8zyjtg5+Xn2PFfXXw/+BvhTwFaLFpOj28JYAPNJGGk45yG4xXoUNulkhVCfLx91ucfQ11Rwqi7s5KuNk9Ec34Q8BaN4D0mHTNDsY9PtUHLRjDvx1c966BjtA5OB0A4H41MZAykYqBq7Yqx50pOTuxhakZuwpGphNUZkci87s1ExJXip2+7iq7krwDzQBGGZW5Tj1zTWXPepdx2kE0ygBnl1BOvymrNQv96gCqMltuKiuuhFWcDeKguBnNBcTNuI+Q2aYOOScCpZ5Pn2YqpcXCRxtvIA6A0iyG6uFgIdnIU8ZHXPQfrXzH+1t8eE+GHh/wDsexIPiO+BARXyIEPVjxzkZFeifHT4zWPwo8GT6ndsouXBSzgD5aWTIA7dBnOa/L3xZ4w1Lxvr91q+r3EtxfXbFnaQ5CLnhAP60pPoS3YyLi4nvnleaRpGaQyMzcksepzTPLwOtKqkMB29akaPjrWJDIxT6VY6csdAhpxg8U0Dy3G44Wp1jzSSRh+D0xQAwRleo4qWNRuAxilhUyW5cc7e1PEeaAAx+lPmG1SCOQOtTRrtXkVFdNu3MOKAM+brULNjPFSzNioGbHOKAEb7pqzBEW7VHCpZhV+HCsOKAFjG2pV5YCnLHls1NGgDA0wGLGad5dWGUDA9aa0e1c5oswItnoalZ9zoQOlNUbjipFj8v5utFmBEzHd0qpcReZmtEASNjpUEkfzEAZ60AYanbIVx3q9byDiqd7C0M2ccMetSQNSA0d1PjXdg1DGpxVmPpQA7aKTbhs5p1FAEXTNRPJ2xUrt1qux68UAN3bqfHGDzmo161PGDgUAKybuCfocVCyFThhj0q6FG3mkVRIwVhn09qAKe0/hQBirElu27g1Xb5G2kHd9KAHCg9KN1LQACk20tOWgBjA+34jNbHh7xFPocvDFoO6E4xWUaNtFkxpnsWlatBq9sssTDcPvKDV3txyK8c0nVJ9KuFeBivqM8HivR/D/ii21mELvCTjqrHrWLiaJ6G033TTfu0u7cCMHPf0FI3SgY1mzzTD7U5vu0i0FoUj5agbrU7HAqLFBMjFFLt5xQOtOH3hTNBy8EU+mL2p1AAvytUnWmL1p69aAEo9MUpps0ghXcWwaQbDmwnLGqF3q0VqrHdyPesnVtcCblVufTNcpeXzXTHLEU0jKUjo77xN1CnJ9jWNca/O2cN+tZOM9eac2MYA59atRM3Ilmv5ZidxqvuLt70lKv3hVWsIXbzkmlp1IRQIaRQBingYpGFACU3bUgGKMfMKAIwtG3nFTFQabsoAaEwc5pSKWigBtFBFITgUANb5aYXyOlOZsgjFMx7UAC8tT9tCpg5zTt1ADd3BGKbSmkoAhmFQ7easyL8pNQCgBsK75AM45q/N+7UVXtYczA5xVm8YKuc8CgC34Rh87xZpCgctdRj/x4V+1XgFTHodsCPuW8aD34FfjR8MbRr/4ieH4IgJC91H7Y5r9qfCls0ek2sRXDhACe3ArWOwG3CpZfSs3xZ460D4f6LLqWu6nBp1sibg87Bc9uKxPil8TtJ+E/hO51nU51iEa/KrdS2QAMfU1+THx/+M2u/HTxIL3Ur+WLTFkZbey3Hywo6Z9acpWRrGnzbn2R8Q/+Cj1k0kmneBdFl1iReDeXSbISc9cYJNeA+Kf2iPib8QYpBrOr6jDbN0tdMX7MmM8DOTmvF/DfiQ6OoiK25ESgJgYP1962tU8YXGoQpEl4Vlk4yp2qg7kjvxXHKUuh72Fo0Yx5pPUyfEdvBdTE3CXrTE5zLdNKw985/pXIXlihYhIX/wB5gc/zrsJ7XR7D7t9LdXTcvKYyAf1rKvDDISBPJGD/AHl4qE2b1qcJK6ORuNJHLLFk9uSf0zXV/CHwHrvj3xla6TotwtjOHG66uJDHHGMZJ/IYrGPnXcjpb4lIyPm4FX9B13VPCuoLdRK0LJxviJB+ue9bRlbc8adLsfrj8JfhmfB/huzt9T11dWuowBJNBGQvTOPvHNekR3mkQs37vODkAjJx6CvgD4FftfQoi2Ot32woMAynHavbNR/ae8L2ccczXu5f70R3V0qSZy8skfRV94ssbeS1wjJFu255LJnjOK6i1jSSEOsilM/KFIOR618gyftceHIcKLG6u0YHDLHk1b8J/tqadp+v2tpPpF5HoUrBJbhzloPRsY55qjKS1PsDztqgY4FMebK4xVfT9Rs9Ys4L2wuUu7K4QSQzxnIdTz+BHpUpFAIaXqNnpzCmPkAkDJoBiM3YVGTRuDKSO3Wm7qCQqJ1/izT99MZuMYoAYvzU1lxxmnL8tB+agBNvvVeTG7OasMu5SKrOuGzuoAh/iqG4PWpSwLbelQXK991BcTLmmVZCWBHUDHOSeBXFeNvFtn4b0WfUL+eO2s7RWM8pbKjA5Xtz2+tbviHUt1qwtwRKz7U5xnnkk9hX55fte/HZ/GniCfwnot3nQ7Jx9paM8XEqkEg+wYUir2PL/jp8Yr74yeMJNQd2TSrf93p1uTjamfv+5rzpFJwmfl9+Tnuc1LjdkqvfJB5/AelOiw6ggc9/as2QyPjbt/8AHqXZkYqUJukFSrGPWpsySDyiCKdt21MzDjioyMmgBNuQaUR4XPXmnbalCjy85pAV932e4GB+7bgrU6xmNj3DdPemNGCpB5NT2rGYbGHzR9OetAEuzEfuaq3CbFPPOK0DGTtOPrVHUF20AZM3LVGF5qRss2cYpyLhhQBJbw/MDV6OPoaS3h+UNV6OPHamAyNc8Yp/l7ec0/gU7b8wyNw/KrQCFGypwMUNHuXGaewLEYBAHbNOVD3pgQpDg5zmpHjzHjNKrBeW49qrXeqxW+QGDN25oAm8kR5+btwSMVTmvIrXI37mNY91q81x8qsduarw2rzNuIZm7VDAuXt0t1hVHIpluG44qzbaflh8vzVof2f5ZXLDJ9qVmBFEpOBirAQrgVJsVVAx0pXIbGBRZgMK0j/dp5HymonfquKAIJD1qFm3VNN92oV69M0gHxLlqtKny1HCuR0xU/tTAFajbuajbS0gF2ijjoV4o6Y70d/SmBHJArdPlpn2QnhWye3FTGloswK7WcygnbkD0PNRMxQ4YY9u9Xsk8DIP1p+TtwVBHuKLMCiq5zg9BSK/zEVaaNWZm6EjGajNq2SwwR+VFmBGTtGaIZngkDxnYwORtOKSTDAgZyOuRTamxSO/0HxoJgLe9bYwGA/rXUiQMqsPmVum05rxrcW4PPv0NdDoHiyXTWWKb95AeDz7cdqhplXPRWPYUn3RVbT9Sg1GESQuGBGSM9KsSZBwR+NKzNI7Cbt2eKjLc09uFqItzQKRlU5BupO9PT5TSKugApaWl20DuhAaXdtak5qOeZYVJc7cCmF0PnuFhjJJFcprWufeCnJ6dah1nWmaRlRs/jXPSZkYs3JqlHuYylqLJIZWZm5JqFQAenNPxRtxV6dCBretJTqTaaBDGFLH94UoGacikN0oAUdaNtO296VetADB1pdtO20lADaVfvUEZoX7woAWinGm0AIwptPprcc0AJTWWnDpmigCNY+RzTtopSu2gmgCJhtOacBkUpxjk4FKqnaSOlADDTSKl2buaPLoAgcZU1CF2kHrU8nANRbvmGelAFmGP5c1HdMduQMkCrceFj4OTVWbLZwcGmB7P+yH4Fk8XfGLT5SrCGzImJxnOAcD2r9Zpr6DQNHNxOwhijBJyeg6k18I/wDBN/wS00eu6/LuwD5cZxnHNfQP7TnjZtB8F6gBIUAhYZ3YznAArWK0Kiup8XftdfHaX4o+Ln0mxuXfSrOYqfm4kx04r511aRkZTtJEf3V3cVrLG15dGVuWkYuTjJPNP8TaaYY0YrlXHXGMGspHTFmFuWVi20dOoq7b7fkJOwjgtnr6Vm22Nu1TuKnmtO1jEjKpHy5yfw5rE6VeSsa82bixt2SRl2NhycEY+lU5JF1C6ZhEXt1HJL7QePpVyyjWdpYjxC/K+/rV5dEj1Bjb7jFBHydo60jahGcna5mW40u+XartbOD90dD/AMCqSbSJAhMEwkT0zk06+8NtdN5Vlt8qP7zYrFmuLnSJmjVjIi9WU4Iqd9ju9ooaTiNvLdYZM3EG4j+78p/Km2uq3djk290SnUJJyPpjNTjWjq+ETanYMy5J9aguNFP+sUA47np+NWro4KlpP3DtfDHxd061jEWtW1zheskTjH124r0rR/G/hLVI0lsdYt4pP+eNwxDn2x0NfO01rG52PGoPqoxWdeaeEJ2kMp/h2VrznHKm10P0j+A/x4k+GOYZpWvPDExzPEjiQRHoHTuOccV9r+Hdf03xdosGraLdxahYXABSSNhkHuGHUV+B2l+J9W8P82N7PAACNocleRjkenNfTX7PP7fWufCeWy03W9NtdQ8O5CXLW4McyL/fHB5B5xVqRjy3P1kIB9qg8zIJx0rK8A+PvDvxS8J2fiPwvfx6lpV0vEkZHmIcch0z8lbLRhWYfMM8jcMZHqMZq07kSVmVSu0nbwD1FNK1Z8n3qNo8DNUQQEU0ipSKRl24oER4+WmleKkI4oZcKaAIm5Q1Vm7nNWZG4IxVObmNuaAKZk3Sdao6jeLbqxflQMnnFOurgRyfJ85HvivLvjt8VLH4YeB73WbmSMzBcW8BfDPJuAGBjnGc0FrQ8U/a6/aBbwLo58O6Nc7fEd/GWZozkW8Z6n6kZFfAUmPMDEsS453HJyTlj7kmtjxV4s1Lxh4gv9a1KV5ry8cySFuQFJ4UelZMUY2gsec5zUEtjVXbyhJPHGKmIAbzFXA7rTkc+YMjMfQmpkhMeSx+90FAiFo/mGB1pcbWxU6JtB70SL8qsBmgCDy896TyT2qZcEjHI75FSKu456VL1AgSJlYEjineTub71T4+bbmlACnk1NmBEtvSCM29x5u7A7jFW1Tv1FJJH5gxRZgSRyLcRmRDhW4HfNUNQXpTrVvss7RY+RjgZP3akvIdzEE4IHpkCkBjtH1FEcPIqRvv4zmrUdvuj3ZpgWbNf3Y4qwflUgCmQrtXFPI3DFWgI2VvSrC85GOneo1hCsD7Uk13Hbx8np1OaYEuefT8apXmqJbqfm6elZN5qzTMViyeetJb6XPd4acEJ+eaAG3eqvO37sEe+agt7GW6bL5JPTNbsGlxQqMLk1cW3VcFPlxQBlW+jKv3uW+laUNrDGApXDfTNWCp9eTTdgHLE/UUAMVfmOFwPXFP8kHOB83Yk0pGWBDNtHb1pWwqnI3CgCFlAjBJ5PamgVIWPlhe1MoAY0n8OKjb71PZNuWpjN3qWBDJ83FNWLHNS7d1LtqbMCWEdABk1N5e6NiDwOtQxg8YODUy5jzzlT17Zq0A3aOeeaRl205sN0GKQnd2qWA3d8wp2KQrzml7VSATbRtpwbPal20wEVcU446UjHauaVTnFIBvHQ0m0L83f604/eoYfKaAI5f3i4IGe1VpIygz1q35fGc01lzzUsCr0Uk0qsRyMD9amaHd0OKjaPb3qQJ7PUJrGQPC7IQc8Hg12Wi+NYrgJFdgxt03H6Vwu3PBpdvv9KRSlY9dSdJVDo29D6U3d7V5zpeuXWmsNjF07qTXTReMrVo1Lkhu4qGi73LvenL1pKcOOazAVetLmm7vQZNR3Ewt0LHiqQBPcCFCSa5LWNWMrMoPHpmnaxq3mSFVOR6ZrDk+dix6mrSE5diOTLtuPWkxUm3j1plWZjTSdacaFXLdaAG0qruNSGOhY9p60AIFApCtPpKAG0mOaWigBG6U2nkdqTFADaPelIxSUAHmUm7NBFNoAXdSbt3GKXbu4pVTBHNABjijGOadjFI3tQAjGmEUtFADcButSKu1cZpAnPWn/dWgCMr8wOaGGFNS7eM5qKRuCKAIXXcDUSpuf1qVqLZC8mcdKALbqIYl45xWVNJyx7Y9a075tsY46Cslf3khB/iOMe/SmtwP1T/Yj0mLwn8BrG7Zdkt45kLY9ulfN/7ZXxNu9e8XNoVrLi1hAM+1s7ufT616j8HPitL4V/Z3gtrtBELSJhE7NgscccY4r411zWJ/EmvXmoXMhlnuJGcsfTP3a3b0sarYoaPahposj+IV0PjTSX/4RM3Kx/6mTJI9CQKg8P2JuruGNBuZmxX0Zb/Be98R/DDW1ityZvspdBsyTghjj8BUcvMi47nxDYkLczKOefz4resoztCAfO5wPb1rN+wSWurzwyIY5FH7xD1UjjFdDpcJiXzn5ZhhK5pLlZ3UPeZLGoikjVG5j/hx0yPWt2xkWSERAbZpDjGewHJzUSWCLaRhx/pExAx3p2mr5EwaUHy9hBI6owPT8uah7HXGLpVF2ZrR2DW8IS1GHkzlj39aqX2g2s1m0RjVppflBUYJOf0HvWlY3DMJZSMhv4cdF/vCrdtN/ohcIBNM21XYADHTPtnpntWGqZ9F7GnUjZni8GhjSdaubOZ2hdSduTlVOOee/HerazTWrFZFdoyeJAMg11fijT47O7g1BFWSIllYEbiyqDn9RjNaP9jxaxGTA6pFt3ZbhUGQOnc84x2re+lzwqeFcZuCOFZYpvmDBuP4ahuLVZFVkAOeoPBFbepeEWhuHGnbpGXkrjlvXArmrx73zntjA0LscYI5yD/9amtTGrCVPSSK1xHDCxEuVwOmOtZkcMt1dBbddoPAbPHTvXTaboKM5ku5GlkYcIautoKw58pNynnaDg072ONUXLU639nf9oLxj+zT4ge90qX7Xpdyw+26XNkwyp3A/unvX67fBX43eGPj/wCC4fEvha4/dEAXenlsyWj9CpHBIz3r8XUXy18tweRjDL09ea7n4N/EDXfg34wj8ReF9SmsZ4yPOtxzBcJ0KuucdD17HmtYySFLDH7RN246+lNZdwxXnvwP+Pnh/wCO3h1L3S5Eg1WFQ17pJcGaA93AwCy++BXorMNxXerHOQVOQR9fX2rZO+xwShyuxXaM445NQwzC5ZwgI8vqTVyTO3g1A6GTcMhN3dVqiCPgHBPNK4BQ801mViBg5HGaTHFAFWbG7GaoX7GP5A3Ld6u3Hy5fPSsPVrnz+IslhwAOpPYUFo5bxBrEVi0rGZY4YkaWWVmwFVQWY/XaGr8zP2kvjRP8XvHEklrM3/COWbtHYqR97sZPxHGK97/bY+Oi2Xl+BtCuwZmG7VJIeGXkHy934Yr4taPKhQTheFXoAuc49z70N6WJkQtGrMBubjpzUqwnYVHNSRw8Z24981KsfvUEjI4wY+uQOvFTZDfKSSV6HFOSLbwDgHmn7TuOec+1AEe3FEcZVcDr2NSUo+V8EdBQBDk9NuB3qQLtUtn8KesY5oKHp0FADfLz82aBGO54p+Nq0FMrnNACDOdo6GpFhkkYqvBxkEnA4FNClWIH50/5sZzn8KAKciLcKUCkvjO4dOvSp7XE0BibAlHX1ant90Y+U5yPSoJImg/eocuDkdvY1L1ApPbfvh8uCTitCOHbHtHOak86K4ZSDtbptpJphGTngL3oWgCD5ccUya8SFckgY96zr7VFXKxsCfc4rNVbjUMnDeV3PUVVwLt9rQOVjG49sGoYdPvNTOWPlx9881oWOixWm1iu9z/E3Qf41pqSowh2+woAo2ukw2i8De394ir23cozTlX/AOvSnjnr7UANUfMKdgHvijdk9Me9Jy2eMUAHX2pcKoyeRjOMU70xwaViSOcHtigBjYA4GBjNMK7uKcwJYEHAAxihjtUmgCBvSmn5VPelbLe1IflznmgBG5jNVz6VKWzTdnvQA2nBM96QjFSxruXrzQAKNvvUvVaTbt96bnmgBVG7NDqVYDr70evFNVcZ7mgBwPIp1IBS0AFOHFIB+NLz6YoEDLuGDSbQykAYIp6ihRgZ65oGRr8xwRSscds0/btGaTGWoAYF3cUnlnaTipeh460ikqCTyKQEJ4pjR7u9TN87ccUg4apYFfaV60fhVhlDKaZ5fXmpAjFO/CgqValoGehrTh1oXrSqRuGaxRoNb5MknFczrWokMyjkdMZrU1a+ECMBz+PvXH3EjSyEk8GmkK6IWBZtx5ptOptamY2kNOIoAxQA1V3MOaeI9rZzQnDipCKAGkU2pAtIRigBhWk21JTSKAGlabT6QigBpGabTqQigBtNp9JQAgGTQ0dKvDCn0ARhMHOaXFLRQA0mkpxGabQAhFNpxOKXbu5oActKy0qpgdc07bQAm3CZzVeSrL5VMVUkbmgBjNx0qxZJtViag9BWhax8Mvt1oApao1V9JhSXVLUSHEfmqW/Agmn6lzJweBUVmpNzHj1pgtz2jxx8S5tZsbfRrGTZptuoBCn7/FcbbRdDjvVWGMbQSOM5ArTgA2AVdzc9Z+APg8+KPFUUflEoG64z2NfpN4L8G22jaXHGIlUCMBww4YYwR+I4r5J/Yv8AD6Msl46gux4yvTivuS1jOEHXIChMdSeBXQvdjqZSep+VH7cnwpsfhh8eok0plS21q1+3G3Uf6rvtzk5ryLSYEupCxcLFHygI9BXqv7eXi5vFX7TGrhbgNa6SselRsvc43M3t0xivN7OFVeCxhx8wBZgM9s9a4Km57GDV3Zl+xt2uXkuH+UIp2LjPOODQYWVLknhji4jTH3+zD24yav7Q00dpEQNoy7np09KszYR45QmTbH5sc/IeGH5E1hdHt1qV6fMt0QQxi8Y+W37pVUsdvGzH3evrxVmO3Nw5ijRU7qeoQd6q2cxhWeyQAKk2F9WVvmWtK526dYJCCd8mTJ2IHbBqZHdg2qkFIz9Wtv7QVooYl2Khij5+6AM59zkZrD0TUsWctjIVVo5Gk9Sc4z+g6V2HlppGki6cfv5FzEp/hHdsd+MiuIvF/s/WrK/miD2srbsKMbuDxmnGSasYYuLozjUj8zpLeQ6GisIgLqRN7MTkwgjgdOSR24xWS2hWusCW51GUxIylkK8M3sKteXLq14xyxjcmSRgcdB+nHGKralciaZY7YHYo2xqRyOev9KWsTqk6dWN7aHEX1kukTB1Ek1s/I5wR7Zq7p9+xXdCRKO6n7wrU1a4MdqdPCLuBy0h556la5S3s5BfOIZDFIvIx0bjn6cVcdUfPVpKlOy2Ol/tCKRSska4IwQ/Bqsq28MbPbmVXBz5jthB+HesC41x5SEuYg7LwF6Z/Gta3t5pVSSYBo9pYeSOnHAxnmrRzzq+00ia3gT4ieI/BPxK0bUPC95Nbal5mWmhz+/UKdysvdMZOK/WH9nz9o7Tfjbo8MV1HFp3ilY2kn09WH70rwWjGB/DuYivyB8P+IJtK8df2ksph+zW7IpkjBT50ZDxnrhuvY1v/APCaan4fvrbVdGvZNLvbOUTWt1bSnzE9enVT3HcZFaRlY5uWHK+Z6n7dyOrKFyC2MkA9Pb61FuK8ivlr9lD9uLQ/jekXhnxXdQaT47jUfMcLBfYGdyN0DYH3a+p5FKHBG0dMtxk9cY7mt4yueZJcrISGaMg4we+KrsG8wRj88+2atN8qmoZGVckjop6dc4qyo7GfesVjk4z+PWvGv2iPi9afBHwDd615kS6rMfIsLVnw7yHGWxjooJPvivWdWuodJgea5ZUtIUd55i+NiiNmbj1wK/J39pj4zz/Gz4m3urK5OjWrm106FjwEUEeZ9TSKPL9b1S813WLrUtQmae+vJWuZnJ++xzz7cHpVTyzuBBp7N8xZhkkBSaeqluR09akzYK3ykE8Yp6/e6HoCMjGaFUdDkjgce/Q1YvFdZEglaNniXhozkH/CgRGrDG40r53cDikGCoBHFDEjp9MUAOXLYAFDSD5jjnpil27W4PShV6g9+9ACo248jAp27Jx+tJxtPPtQW25GOQOtACopkAz8uaXbyV9s/kKRfnUfw4p6x/KcnqpH5jFADvLDb8YyCP5ZoVfmC5p7shIKIU+UDrnOBTDnOQOaAAqM4zUcjblIxihwxyTxT+x4+6OTQBi3ym1YzJ1HOKq6pdyrLEnysZUDYRs4/Ste6UMrNgdMYIyDWFpsO3UHUAA56Hvx09qhgWtN0UNJvn59FI4Na8cIVQv3QP4VHH41KkeMEDGRyvrT1DKDxgGmgEXIxnkU5U3N1xTwvvSMoXGTkH8KoBoyWxgY+tOZc0iqBzk4qXyyRkdKAI1jDECpAi8encUu1e4yKAxAK/wnrQSRsDuwpyP7uOtLtDd8D3pWj3HlSB9aGUZGfw9aAQ0xt5IcDIPXnmmHB6nAp23dzyMe9N3KHC8k0FDH9hx61FImQTmp5flBIPHpUeN3AoAg2YGaRulTOvbNM8ugBipk4qVY9pBzSqmMc088d6QDW+6aiJqaTCjg5qLoc0wEzT0XdQF3ewp6sE5+97dKQDfal207O7tinKtMQ1etLz607aKUL2oAbSjnHpRtwadx0zzQAhGRSKu3mnU4jIxSGQkbjSMeoqUJ6mmtHnvTEyMUjL3p7JgdaQg7akBpNH3Rml280u3NJjIzhucU3y/ephHR5dKwHe1BdXCwxk9TU0jCNTmub1q+O4qD+tYrU0Zn6tdmeQ9vxrOqRm3HNMrRKxmMpGFOYUg60wEAoC5bFOC5bFP8vac5oAaI9uOacBSiigBppKfTaAGGinU2gBp4pKdTaAGkUlPppGKAGkUlOpCKAEX71OpF+8KeRQA2mkYp1FADaTGaUiigBjDtT41460u2nxpyBmgByrt5JpThuAalVRwDzQyqM4XBoAryngiqjdatS96qOcZNAAi/OK041G1vpWfApkINaLYWDOe1AGLfcy/jipNNh/0xCTnbn8eKguctNVnTuLo5FA0dPDiRV4xWlar93jdzjHTNULNTsGOtdD4c07+0NYsrYAsXlUFcZ704rW5snofoB+yP4bNn4PhnZNu/mvpi41BNJsbnUHwI7O3e5bPT92pb8Pu1598GfDaaB4PsYejCMcYxnip/2gtZPhn4D+PdQV9kkWjzKpzjDSL5YA/F66qmxnHWR+O3jLVW8Wa5rmuXDmS6ur6W555yWkJ/QCug8N7LfRkuUPmSS/L8wwc9ufrWPpGnpdKyS5EaJ8wXqWKg5/Or/gWJRcXEU0j4t2zFGy/r1rz5anuYePLNM6mztXsbdpZVJlf7zEcA9h71cEaqiK2T5gzJ2DL3H5Ugj81vMZ2MScqpbgH1x34qWMGRGkkG6MN8o6bu2M9q5up9TGKlHl7mMrNp+oWjzJudd8Ui568Eoc/QYxW3pNsNSvnubnP2aIb3bH5L9c4FY+rQy3sckozuzk5GAHXkHPfgYqzDrrS6TZ29vw0h/egfxP3P09qqWq0OTC2o1XTexfeKTxLrTLGcRhdvzfdVcdKwPGMkM4EFupeO0Vgm1cgnBya6fUpx4e0YWqbftM43THoVXrWI9r/ZWltdS8SzoRCDyCDwWI+hrKG56WMhz03DqZOna5DH4dW3hJNyP9c2MH7xGP8Ax2oJJjZQG4fH2iTiPjAA9MdvWsrT7pbHWmSfHlsGZVxjByxH15NOvJXvrt2dtkZHzd8enFbtX2PDpVvc5X0KssyzM0zguF5XJwSx6msKa4b7QJh8p5HX2rQ1C4Ekiop+VeBisu8KlQucEc1UVY8rETvsMk8tlIZRuP8AF+FVbPVLrS5GCynYRj5hxSs2Y/MPPaoGj89SDyT09qs41LrEpR6tHazXEk2B5h56nPPGBWZqHiGa6k/dMY4/T1p2qaTMshc8oO+K1NE8N22YpZyZc4YKRgfSrRz2nN2MvQ4dRW8trixMsLRyq8U6Eq0bg8EEcjmv09/ZT/ben1KGy8J/FW+jXUgBDZa8zD99x8scwx14xvr4T+3S3MUMMdlb2UUYyjQrtPHQ5qrJoC6nOZr2fexbOUyCD6jnrVR3NZ0VBH7nTI/lqvy/OgkEisCjKeQUbo1U5GMbAtnC8nHJ/AV8HfsqftRal8O9NtfC/iaS71vw7G22G6lYtNZj1Axlx2xkYFfYvxG+Kvh/wD8MdQ8dPqEVxpVvbmS1kVgDPcceXEBzzkjPoK6OhzWsfLf7fXx0k8P6bH8PNJuBFqOoL9r1WSF/mijyNkeexPevgL+FAR8yjav0rd8Z+LtQ8ceItT17Vp2ur/Urg3EsjDnLZIX2CjjFYQjLEFjnHSovczkNMZZgMcfWpVUquOgqWNUAGcj3p/G3gZHfJxSJI9o28NinLECW4AAHDAYJ/wAacYwwyBT4/m2rnAHU+tMBix42/Wn+WmzeGy27GzH65oK7gRnBpu0Bi464wP8AGgBoxvOT17elSgg7htyB3zTBhmGRzQrFXbA4btQArqqED+939O9M4ZmIzngYxTweN+eRTlbnBwc+1ADUXap5qTOEpu07gO1Kx+UDFAAM0H5SB3NKxyQRxikbGQT0FABgtwTkelObPlkj+LjFD/uyCPmB/ClHzKBQBUkX5RkZDHpWNfQizuxcRqQR2/SugkUlRgZINV7m1E+QQcgdMZFAEumzfa4Qc81bWNjnPSuatZn0+4ZSTtJ+mK6KGbzI1YHIxzQAjjac56VHzJ7VP/rG5HFMAAyMYPY0ALHF071N91T1A+lMBK4AOD607c453Db34oJAjgntTc7GBzj3xmnFfM6daUlFU85YdBigREH3NkDJpf8AW44wT2pyqeScEHqvT9aHTaoB6fXmgCNlHBBIU9OKjZmU4yMfTmp26Ng5OORioQS0oyKCkK67kNV1Yqw4qw2c1E2XycAY96AGn5jRt704CloGM698U3B57gU8fN04pcBUIzk0ARc4I9aAmaWnqu7gUAIgI6GnsDtB456jFIylT071J99icYz2HNIBq9MYprdcVIU2Y5bPuMUvl/MMGmA3bjFKvWnMvHUcetC8HPJ/lQA3vyKON3AxUnuBz6Ui43ZPHtSENPy496dSbffNO+71pgI3pTNp6dTT+GOQaT+Lg80hhtHc801h8pp/bkc0hoAi24FKKexGMYpNtIApNtOC5OKNtAHT6nceWp/nmuSuJjLM2elamsXBkZlBxWS1ZR2GyOkanmm4zxVCGgZoVMt1p2NtKv3hQAeXtOc06nUn8VADcYoPNPIptADKQinsKbQAygjNOYU2gBtJTiKSgBlFOIzTaAGkYpKfTcUACrkg0uecU+NflprD56AEIptPpCKADbTSu3mnbqM54oAFXd3qVY+hpI4/mxUy/KQtACUO3ynilYYprcoaAK78gmq0ijNWnGFNVmG5sUAT2ce5sVPeZWMio7ZfLXdnNO1B9qcigDEYkyGrumqXuM9ulUmXljWppA7470FI6S0UpgDqOa9g/Z58Lt4k+JlhFt3JEwkPy57GvJrLDgNt6ivrT9hjQxfeJNT1Fl4jUKvGea0iV0PvLRbUWlnGgXsqgdMV4V+3drX9n/sz67GshR7u5trU9t2Zkf8Akte7mTyIFfdnaC+OnbpXyN/wUg11ofAPgvQRIAt7qc08o9ViQgZ/Fq0qNcoUU5TSPhfRoivyLzI7bz2yOMD9KmvLb+zvE8DCQpBL99gOBx+tT6FEFD3B7nag/rmr/iDTxcaWsqqFkiO4sx4bnpXnXVz6uVNqkmkdBa2v2q6MKHZF97nptAyTn8OlRXIa/uEtbTKjOFGOo/vVFpd8n9gwQq2+WXmUL2XrjNa6Kuh6X9rdGF7OcRnGCI/XH0rFrU96g1OmiprTRR2sOkxkARMGlYdSSeTXNeHpE0jWLr7SPMjjBkt1A75wR+RzXS6XAsET6ndEYzmONhkv+P61xOtZiuBeKSGXLMQ3UE8DHbrTW1jhxsXSlGstzordX1q/mvLkkwqMmRh78L/Ss3VLp9WvdoOyEfKFzkBR2/Spb6+EGnwWsBbLAOx3cNkdMVm6hOum2uwNmVhyR25/X0pcrTN3WThfuc14tmjbUYpI1KRxAKWU9TUd1dg2cYiO8yHLNjn6VLqXlrp85l+/JgqMdORWHpt1vhk3EAIeldCPmak3Co/MlkYRrnq3rVCYH5mJyasMpbce1RMu5SKo5pu5TjzIuwDvU8dueArfMTgcUyGMrIcGtbTbXdtH8Td/SmY043YyW3X7K4aPfxtOOu4nGPeultdNgtdLto5LYLOByN3T36VveFvDKtpM+r3UOba3OIN3AeQ/KT78HNZ91GZGGR+8YnJz1FWXUjyu6MubdIMY2qOOma67wV4Iu9cmUrASoPGF61e8BeAbnxZqCwpGWi3Dc2M19w/CH4JxabZxbrZdwHUr3xxWsY9znlJvc8z+GX7P95fG3PkBAxxlxx9D7V4T+1F46j1LxXJ4R0W4ZtA8PzbXVSRFJdYIZwuccAkYr7p/aY+I1p+z/wDBu6ubIpH4k1cNY6ZETg/MNskvvtUvgV+Vm5y0jTSNNPI295GOSzk/M31JrSduhzt9yDsud27qxJ4J9cdqXYW4FSbdwpQnaskQJ0XAYA9PWlVecnk4608W69cEH1zT1Xa2OvFUIbGmIzzksaVl2r170/btZR6U1vmUg/Lz1696AGNxMMdKPUetOO0HPJHrg0rfKwI5FAEbfL70sYJkORwtOzlgSKk3gBuMZ5z+NADVUZOemcUMA6nA2kdKYSWU4H8Wc08MA6kk478ZoAN20ZI6U4REpknGOg9aHYN8uGGTxkcUGQK3lnn0agBCp7cmmt905FNkugkpSNWkYdeMYqePFxBuAwe/tQAzy/l68UvbFOUbgQTgikIwaAHR+WGHmqWTuF60k6fMfLV1DdM8ihCQwIqV5DGpVQSG65NAGJqVgZo2IG1uv61FpV+YyYpBjHTmtdwzZ9fSsTUrN0k3p8uDmgDeSQNgg05huIPSsrTbxXABPNaindQSSeWDgk8DtTsbSRnikUHbgZJ9qXIDHdnnjGKAFZmjJB6dh61EzN8y5+X0xzUj52rn5gO/f8qVDlmYYx79qBDBllOBx9aThmAYFV/vUFi2GAxz1zThzweRQA1iGYkcCmHC8mpZNnUcH0qJnwM9P1oKQx13At/DUaxhc9akyG5AJPrTdxZTxQA2jbnjpQxC5Y5oDD1IHrigYzBDbc9e9O2Z43fpSPjdgHg9WpwXoA3P0oAQRncP51LHDhh82PwoGR1PFKwVlwpoACh3ZLbx6Uc9hz6ZxT1XjHekTG47geOw70ARnO/nOfTOaemcHinDG4E8L3p8kfzHHKjnIoAjIOOg/nSZ+v4Gl42nrxSUAHXkUcYORz2pSOw4pSu7HHNACKtKfel5XHHFHXml5gCqBTSvzdafQy8ZoAbSbcg804Up6UARbKKew+U01aQC47038KfRQBDcyGSU1EaX7zH3oqAGUbcU7vmigBu3dxTlj2nOaI/vin0ANpdtLRQAykYU9hTaAG01hT2FJQAykYU4ikoAZSEU4ikoAbSEZpxFJQAynKm6gjNOjoAANopuOakZaYOtADSKSpNtN20AIVpoXmpAMmneXzmgBY+CKX+IU5FyKd5fvQAVDI3XipjUD/eoAZIMKar7fmBqaVs0yHMkgAFAFyCPaoFVdSbNaEbggKeDWZqTdR6UAZr963NJTEfTrWG3UcV0elruCjGM0FI6GxwsfToM/XjpX3h+wZov2bwfeXci/NPJkcdBXwhZxlmVAeWOBX6a/sp+HzoXwysAy7XkGTxWsRM9r8sOhDHIxg18Df8ABRrW1vviF4M0VDhodNe5PPCmWQHp9Fr79SMzfuwOW+UfjX5mftt+IE1z9p3WooSpt9Lsbez6Z5Xg0qmx1Ya3OrnlulwJ520f6mMbcgcE4ro7eCOSFjLGHj2lRGeQxIODntgnNYulxiK3VOdzvz2/T9a22Tc0NvG7O28KrAYzk15z3Pu6MFKHL3MDwrDFFq0kFzIsUaxtMV6EhckL+JGM1trJL4q1Y7dyomMrnhUxkj8hWD40ihsL6J7eRQ0amB5ByWYfNj24H41tNqVtpehQCCZZLy9HmSMnBHHAA+venJX1Rhg5ujN0ZlbWr5L+5W1tctFGdkajjn1z2rB8TBQwtI1UlUKOD6kf5Na8atpNmbmVVFxMv7v69SfbisKP5o5bqT5lUEgMOSx4J/Wpjua4tOpFp7mfYzYWRpG3vEAqqDycDGar3MhuZDM2dqnk461SmujHesNoUSL/AA9uetMupmRPKUlgvJ561uzwadV2cSO8m+1TEOQU7DHSsDckOpSxIcxt+FasrBYyo+8aybyNY2SUcEnn3po4sRK+pak4baDxURX5qf8Aew3XipEiJaqTMFqVY49kxJPCjceO1d74I8K3HiXW7PT4Vx5vzMwGdkYBLMfwB4rkY7UyXKgDdnauPxGTX0L8JNCbR/B+s662BdXTizhYj7qgjJB+mRVxSepdP3b3KPjO4tppI9K01Nml2J2RqD/rWxzIfT6VzemaHLqmpCKOMuzHAA7V09/YlpljRMqvHHOa9t+CPwrW4miup4CXY5G5fateVXOecne52PwL+F6WNjETBsc4JbHJr6v8PaLHp9q5kdIY1iZpHzny1CksfwAJrD8G+GU0+IExBI1GWI7Ack+/FeR/tzfHAfCf4Wp4Y0q5EPiXxJ0aL71va5BLn/fUFccYzWmi2ObmufFf7X3xs/4XZ8YLy5spm/4R3Rz9g02LOVG0EO4+teJso5bvTxtWNUAOFGBk5yc5JPqabJ90k1BDGKu4077rUvCAEHNI33zg0CHF88dKkyFyQck0kcY6k0MUJwAR70AI75IOOlNZtzA8rj0PNO4ZtoPWkMfGAaAHJI6x7GZnV+o449KbtwCM8GkZi2WAwB2pVXPJoAQLzTsDuMj0pVAzSseKAEX5eMcGmLjdtPGf4vSl8wHnkAUKowZD0XqKABmKj7xc547VWlSS6u1ijB3Eg5B6YOc/kKt7EYjBwTUDQkF2BYH1Xg4//VQAt1cRWriOA5cNlrhj1yMY249/WoIZpYZGRjuZfmPYY7HNOa1SG3YK4+zNgK7LlnJIGOvHXrSQR7isUgfCuFDqODzyPcY5oA0I2WRFfIGVzTCd3JGOcYqC3by5ioQ75MuwPG1QeKsOyybpEOVAoAVG2tyKnVwFOVzVXBccdatooEWCcE0AQyx7cMDVS6TKknkVfkwelVpArfezjvgc0Ac7MptJd6jCZ5rZ066SZAuefWobmASLyMK3QVmxSNZ3AH8OfpigR1QXbjDH69KBluckEdMnNVbW8WaPCjJ+tW2cKVHQmgQm7kdj2NNVRJkL979DTiu7lRuP90UKFwcBg2fTFAhp+X930K/rSN8v3gcd6kxlifWmtlWBLfpmgY3b7YX1qJs7sY+X1qxuDsDgmkxu57enrQCIl7DeMemKGHyGjarNu6EdqbJJwRigYLHgZ3Y/DNMeNuSWGV6kD8qlWQ7cDCn1PSmq/YKeOjdfrmgCPyQ235cNnnnp/jT9oMjsBjjincEnggAZA96btPLEBQ3egYu35sdRThhW+7SrHuwB+dKqjOP1oAYylugJ9hT+CAMhfY8k04xgZOePyNIM5wMY+mT+dACbC3AAJ9DxQcqwQnp39aVdrZB5PoOP1pAhyqjr/P8AGgBNvBGetNX0qTaRweKRsbgw7dvWgBgyWwBT/u+xpduRk0ZOMdqQCAnPqKXIA6UbaXb05zQAwAs44pWbPy4p5A69aVfmxQAzbhaBTpB8x5/SkzQAxueKXZhaXpzRu3cYoAatJT6TZSAqY5oIp+2m1ADRRS45pTQAi/eFPNMT7wqSgBo60MKWloAZTSKeRSUAMppFPIxSUANppFOPFFADKaRTyMUlADKQinEUlADakVcDNNC7mFSgYFADG6UbacRQBk0AR0VK0dN8ugBoTBzT1G5gKXHGKFG1gaAH7dtFPX5qDGaAGVC681ZC45qB3DZ4xQMqSLk4qS3TrzyKa33qlhH60CJlUFff1rL1D/WAZrVkXy1HNY11+8m64xQBCq7pFGa6fS4wq9egz0rnIF3SjnGK6bTd3AHUnH4UFI7r4ceH5/Efi3TrKJNxaRTjr71+rPgPR/7G0WztQNojiUBQO+K+IP2J/h4uu+JrrWriMtFbcISvHQiv0EsbcRqMcA4wPStoqyEy7ZwqtzAXb5A6lj6DPJr8cfitr0viX4y+K9X6/adZnAYnICJlRz35r9dPHniJPCvgXxNq7D/kH6XdXA5xllhYgZ7c8Zr8cULXVs0kpzKySXLNj7xZhIP8Kio1sd2Gg5e8uh1Wnq0hMo+YrwARit6F/stobxThpBthXGMr0LZ/TFZPh9TqEMCRkeZ984/u7SWPvgVoTyjUr5baAbIV/dwLnJC/xNj8M158tz7rBy5oKRj3WkpcaTqF3cliu3bErYPmPn17H3rn/DUf2m7mhldQlqgbJXoNxX19Rium8T3X2po7C1f91GfLGO7/AN72rjvEkMeg6sfIL4KbXw3y5yWIJ78nNXHaxw4z93P2iNXUrptUu2VTlenXjj/9VZ+pXAkzEgwMYCjt71agxZ6dvZsSyrvVvRfX+lZe5UjM5Xcx425x+OaVncqVTmgpdzI1WNI2XZ1I5Ppg1RaYspl74xtq1NE03msTgdc1lrJ+7KHrnrWp85UfJU0E3ZyTyaqX0Zlt+DgrzVljzimOu5GX1FMxn72w2yYSQjI46VoWsW7npWbpCnDxtw2eK6Oxt+AuM80FUlzCWdm7XkagYZjwv619RXmkr4e8C+GtMBLGUG6c4xjI6Y/rXg/g3Q5de8WWttChkZpVUBRnvzX0p8RB/wATiOzhUGOxt0tzju3GfpW0FoEtLmD4D8M/214jVQpdEbnIyDxX3B8OfBqWNjEfKAG0dB0GOTXiHwE8E8GeRMbiCTtr600axjgs1HKjZjge1bHFMddPZ+H9Nur+/lW2sLSBrq5kJ4SJBuY/UgHjvX46fHn4t3/xs+KGr+KryRmgmLQWEa8KlqrYj/E4zX29/wAFFPjhJ4U8G23w80qcRal4iC3Go7Ww8VspBCfRitfnJuVZPLXKIMYXORwOBSZzEYPrwKkaPAAP4Cl/hAK4LU7PIJ5x0pARrGvQ8k05owcsByaNm5s5qRT0NACbSnBprdM4z2xjFDsS4JPA7U84GM9KAI2QK2QPehfvjJwKfu/dnAJLcD25qNwFyM5x+tACZBbYoBJ/CnEgDHU96RVDDIGDU3l7ThemMkevFAEW3hufu0K205p23cwPQvxt64ppj6gnBoARicFMAhqFX5CnY1JtyhPeiP744oAYFGOmCOlI4PBHH65qWX5nGBjFNXl8UAVX37mK7c4xhugHfj6d6ikhCwqTI37wbI0U52j3qzMN2faox+7YsQNuCGXHUY5APb0zQA3cZFkXdmViFSXPG0Dp9O9Im9EHyBMfII93Le+cUrqt1FvjARNu1mZseWvYf7Rz34zTmceWjTMEmVcx8YJB4zj156UAWYcbdwPTtVhTvOStZsbeXwzFFjG5mYcHPb86vw3SshTADAZ6+/0oAUkOSAMVFHIYZN4GSOOenSpG/duQevWq/nfNt28HvmgBsqjaT09azbm3Ei5xgt2rTf7pqvMvDEceg9KAMqzmNrNsOcfXFdCj+dGpBrAu4i2SPlI71Z0m8ODET82aBG2Mrj09QcUv3mBOeOhzxSMCNmTuBpVxuGRuX0zj9aBDgcEBhg9qGXvmkLfeBOMYwuKXjjBJ/CgBNxUc9PQCmZO04qTcV5FRkZbOOaBDTiMZIyahbDHBIA9TU7LuwM4qLaPMA+8fcUFB5ZXpgj+8elEY/h5ye4+7Tnw2FIz/ALPY05VKPtU5HXHagY1VIcBTz64yKHj8xjubAP5VJtPmdDjtz19aTdtftn0IyKACPMfqV7kDinBdxz2pP4t3IPXjp+VPUAKsmOaAG45wTStGAuc5Hp0pv3jS98E8euM0AAACnC59s80522rgdD2pVXaDk429e/0pjY2nv6H0oAVmbAUYIPY03arL6GnLtfkngelOCttJGNo7d6AGFdq0iin8beetNpADUu3FKoNLxj3oAbSlaUUc0AMwQmM9KQLk4qRsKOmaBQAxl7ZpNmFqQ880jfdoAjAp1Lt24o20gKlIwpetA61ADBRT9u2kIoAaDg5p2/ccYpFXc2KcI9rZzQAUUrCkFABTTxTiMUlADabTqKAGU2n0lADaaRinUUAMprLTyMUlADo484OaeUwM5p0aY5zTmXcKAIQMml2bWzTgmD1p1ADKQrTm4pKAG0q80uzctOiX5hQMeqmpBS5+U03kHpSZSGScVUk+XJ61auvlAAPWqLnmmJjDyaswptA5qCNd8iitBYxtHtQSRXX3fwrEbLXHX1rbvGwpFYW7Mx46UAS2q5kH1rpdJiaa4SJRyzAA+ua5yz+ZjXqvwa8MnxV400+18stH5is2B7E00rsD9Ff2UPAq+EfhrZF48T3P7xm29eK95hI4GMKDkn09TXPeEdPTS9FtbSP5UiiVQuPat5fmyh4DjYT6ZGM10AeL/tmeJP8AhGP2dvFbFxDcah5OnRDPJaR1Lj3+TNfmzocY+wnKjdO6phudqAD/AAzX1/8A8FJfFDTWfgXw5FJn7VPNqcyA47eWoIr5V0W3XzhJKuIIOCAev+elclV6n0uW0rxdxunSPpq7c7JButyFGCOcg57ZAxWyZP7H02S7OBJM3lQbhzsxy39KzryGa4lkuCQqXW7LY4VlUlD+YAplxqUusfZo2C5VQhXqFwPm4/WuZ66nsYWfs5Om/kVYmayt5LpgpkkJEeTn8fyrmdUtTqFpO7MUVRuyxyGPf/Ct7XrgNdLbW+MKAuAO/c1k6ofLjWADcF+8M4Dc/pSQsT78WmZGk3kuqstvIeYY+ec4HYUX90ryeTGuMcdc1Svlm0nUvNG35xjKjGOOlSr8qmZl+Yjg561qzx6dR25GQXk2yNI1O31HXNZUsfkspzyOcetXmw7M7Dp0FU58uSxb7vSmjjre8MxnmnKnemx/MpGKswx5YAnjNUjGGpUsF238ob5i3Ttiupt4diJxknAx071z0fy6wp25DcfpXeeG9Fn1vVre1giab5gMKM5PYUWuzal7qbPoP9n3wVbeG/DN94tvYsyoSLYMOrEYBz+NbujaLPrurrJPl5JpDM7dc57V0urW48O+D/D3h0R7J1j+0Tr6ZOAuPxzXc/DDwgJ5FlZfmJ+9j24FdMVockqlz1f4a+HE0rT4yE5CZwB144FeieIPEVl4J8N6jr2oyLFYaVbNdzM7YB2qW2Z9SRtqlpNvDpNmjMRHtHHf9Pevjf8A4KFfGaaKx074c2FyySXK/b9YijbomR5cZP1w1Uc1+58hfFj4j6h8XvH2seLtRkZp75z9nVjkQ2+7KRg+vGc1yO0ZLEcmnoGI28ZPLYGAcDAGOwxTN3Q9/SpIYjZ3Fjz6U5BuUk8UnmVLCo5yaBCMqr0bNMZtijHODT0O7cNv0OaUoNoOMc0AMaPdzn3xS+hPGBTmyxJHA9aJM+SQBlu350ACkkAZ4Hf8Kj8obSpOSf4sU5csm3ofWl2feBPTvigCNTtO3GaeztwQmMcdaXYFIIbJ+lKGLAH1oATaRLnHQflSbct6n1pWB+Ylslu2KfGg25J5oARFwo77qThUB5yTjAp/PA9O9N4bC45HfNADD989cdsijyzuzT9vy43NleTnvTXyyAg7SaAI2K52nqaasXnNtAGc/wD16cExznJp8cRjbLAlT15xQBBJH8p2LvfO7aRwT247880ySNJIw4y7sQZOPmDZ5Cj071eky/tjoRxioJVZPmVtrKS3Tk5BoAr7WOxZnB8t/wB1IpBA46MP0qW1RpZnFwskkoOYo1ICjj178c0xozJGkgQHePudBx1J9elFufnWSVSG6IqMQV49aAJZN6kKTzn5iRg+wqJThScc0+QNIdxJOOmeTTto4PpQBC0h2nim54zj8KkONrHHSoWU4Jzii4EcsYySV4xWWNtreKy5OT0q7dXQRTlu3Sqel27310HI+VT9R0NT1EdNH86oelSiHPJOF9c01I8DJHzdjUjBWZTjn0zwaoQ3Hzbh8o6ZoWMcnBJ9c0/btGBzn+Ghl2gDsaBEZw3AI3ehNR9HU4wD6jk8VMzFSQVVh34xTd3Lbj16lufwHpQMjZN3J59qYQOgHPp3/OrDKWQlTx602OEbhk8+uKBibMLjqMfd/wDr0ir5abWOe/vUzEbV456UjoCvJoGQq5UDJzn73bPpS7Sfm6D0pfK680bgEagAwW4HWlb7vlgZI6ehpVTdz1X8qf5f7oA8qOvvQBCGw5U9e1SYKSAg889qT+AKOnf3qRs7QQORgUANVeMA4xyD6Uxvmyp59+lSuu35erDGBTThRycZ9qAExtTI7UORkHofWnEErjt60m3lQeaAEZQcDr6n0pFTLYzS88rnin/dWgBrLtHByab9etL1pW6UgEpccUAY5707JoAbt3YpCMVIOKb3NADccUh+6adQRkYoAaDuYUU5V2802kBT6NS980tJUAFNp1BFACL94U8imJ94VJQAykxzT2FIKAEptPpKAGU2n0lADabTqKAGU2n0lADaRV+YUuMVJHHnBzQBIF+WinUhWgBtI30p1MdsdqAGF8ttxTtuOaQR/MDUu35etACZBQ8U9Y+jZzTdvy1KmcUFIKXj0oIpu7HFSVdEE3zcZqnIBuxVuQ1Tkb5+lUQx1un7wH0rQb92ABzmqtuu3Ddatqucc0CKOoSbYjxWOrY3nFamqSfKwxWX92MmgC3YL81fXv7EfhI3viB9QmThOilc9j3r5G0y38xkUcksBj8a/S39jHwb/Zvhr7XJHgyAY4rSG9wPqSzhCxrxyRn6VYKlVZweVUkDHUgZA/PimwnoasRYaeBW6NKg/wDHgK0Y+x+eH7fepxX37QFhYiUOukaFGjqO0juGrxa0X7PYwRA4d/mdjzx6VJ8e9W1TxH+0R4tvL63khee+eERtksqIcL2GQcZzU+iQx3NzJPN81vbody5GRgHA9snArgrau59llfwk2sYtdNisQcOBvk4zg9QPy5rk7W6Gl30rtgNKuwLu5WTHPH+7k11i/wCmX0lxNwi/PIvpx8q5/SuT161e6lmmUKjSZdm7q2MLz9OKzi1axvjotfvokUbcy3LsNwO0A9TWWX86ZpJD8q9BU/nGTT4AOJMbGHU5+tQX4W3jjiJ+YDLf4U0jNVeemjI1OFtQMmzlwCVz0GKzbe8aS1WJs+apxite5/cW5I4d+hzisGTNjdRt1Vzzx7etaI8ateMrk9021dueWqqThCDyTUzHzXLYyMZ3VDt3NnsDQYSd1cLcbZtpq/HH6VSTMk4GME+9bNralV57ZNV0IorWxV+yuL6zYDqT7Z4NfYv7OfhWy8K+FrrxZqVuLgxHMSFcEtkAY/E18vaDoc+ta9Y20SF9vzMqjn2FfbetWP8AwiPw+8N6AQEu5T58y9MLjgEd+a6Kcbjm+R2Kei21/wCMNfe/u1Z3k5HHCqTwtfTXgXw61nYqojGdvfjmvPfhD4T3Qx3DqwZuTnoeK+gbK3jgjESgEYHIH9K2lbocL11MHxV4gsPh34V1XxTq00a2ejxmYq3RnA+VPxbC1+PHjrx1qHxK8Zav4o1WRnv9Ule6OTnbGXwifgK+z/8Ago98YDE2j/DWwuFC4GoawsZ75HlxEezBGzXwuvKyBuCTnOOvPp2FZGciJZCpyBzimr8yHIwQaeY+OtLtAQkHn0oJI1B3CpRheT09Kav3ql4xnGaAGD53wG2j6Z7UiqSME5C/rUhxtJAxRHtXeN2QO+KAG9P8KemWPTinBDjO3/69JuxzjA9KAGEfPTtuS3Gd1OCb2B/QDNJuIYABvqRQAjKu3JO0jilWPb7haPK3E5OSaftbnjANADNm5hzxT/LyoIYZPalHBz1pIgzyoi7Qc9cY7UANIGwjPNJgJjvUrKEyCctnHFQ9F9dx4oAYo2vuJyPSmt244FP7Um7YCcZNADRgqDk81Ksm5eRSDPy5II78UgXEgGeDQA7J6DpTXj355xTqKAIGX5QuDge9G1cghcD61YVQxxjmgwlmxxz3oAi4VS2OBSNGGQkEj8KlkiaPhl4PTmmbieD09KWwEDttUEDisnUr4RZVR831qzqN8IY2QdR2z71z0khkYseSal6gGWuJMnmuq0a18i2yPTuKyNFsfOkEjfdXqCK6WOMxx+g9AapaCYqAk8sd3ZcdadgNxnj3p3JjKsCQecjgj8aaWLIOhHrjkUyQLFZCoPyjqMdaVYsqcj8Sen4U1c+ZuB+nFP8AqaBibW5IHXuaRgrNwP3nbPAp6u2WXGR29DTN25ucMvUjFAxBHu5DA56DOPrSqhYdh2FDkHO7AB67R+VKqpsLA5J7UDG8LgHrTuW4A5pduVznj0xzTlUKM5H9aAI+WypGGpqxsvGPxxmpPLPdsr6Y5pyqwIGcr6YoAi2/MARz61Lt+TbTtoZvejA6E0AQbdvWpFG5cEZXr1wal/hIGM+9QrgMC350ADfPuPRf7tJjcwGcL3FO2lQ2OQe9N27s84oAG+QZzkelGd5B6Yo2/KRmhSF4NAC+X3zQwzwDzTm+ZTg8UirjnNADSoA5PPpQBTmUbcnrSUgGnlhTgKMc0UAFNbmpNvFN2Y70AIBRtpxFLjAoAY33abUm3NHl+9AFDHNDDvThSVmA2ilxzS7dxoAav3hUhFAjwc5paAGUhFOIpKAG7qSlIooASm0+koAZTafSUANptOooAZ1qaHjiowvNTIu3FACkUlPpCtADSKjYd6ex2ij7woARfm9qesfGM0D7tSKKAGqvapUxwuKdsyhNNX5SDQA1vlph5NPcE80ygCtL1xVSTlxVq46nmoI13uBQBYhXCdeasentUSxcjmp2GxCaAMbUm3BuKz5DtQDGcnFXr6T58Y6mqbrllFAHXfDzR21nxFaWygt+8UYx1r9b/gv4dGh+EbKBUCbIwCR349K/OP8AZe8JHVPF1tKyZAcN09jX6neG7VbTTIkA28AY9OK1jsM1EG0ikub2Gzs7m5uH8m3gieWSTrsRQSW+oAzT+nOfavLP2nvEEnhb4B+NdQhl8mX7F9nV/eWRI+PX5XY1T2HHc+Afjf8AFpPjl8QtT8QfZLbT9JjU2tqYMCTCMAJHbA3Fsegrj7fX7dl8tbVYEC7ZbpWJ83j5flx647muF0+F9fvT9mQQ20YjDR7sg4Xnj3PPtXplrpNnFpLSqgt5I+BGv3jzyc9vyrjlY+mwLnJe6H9tafLovkQXf2m7klD3IVcCNRwoznnnFUL+3jk0UuZlWZ5MGMHJwDkfyrgvGGpBWZoW8qQcF4xjPPf1rD0PWL3zDFlpzIcZdiMfpWSj1Oirj037OSO2jU288ckh2xyNjYR91scHPv0xTLhTcagVdctnJ5yCMZqni5Zdt5JGkL/KFDcgjkH8xTI9Ua33Rv8A67JXd+FaWOGnUUZWew2+UXNwUC/ItZGrL5gWJBwAa07edQju5G7rjPWs/az+ZIelCJrWkrooQ3A+y7CMOOozTkOVIxyaqH5bhmIwGq5D/DjkUzzlK+hYgXaVcDJHStmGTZFuJ+nv6CqEMeIiwGT6Vs+F7H+1tUtLbGQrhm46+1O10bL3GfS37KHwxhuZpvEGpqBHCDMxkXAwATjOa9FuLmb4geOZ7ohjAzhIR12xr0/lVpbc+E/gzp1gimK61WfaQp2kIMNn3GFrvfg74PVYUumUZP7tTt6j1rsp6LU5py5meteAdEFhYISPurwMY5xXQ+MPFtl8PPCus+KNScJY6TD57bjgNIB8iZ92wuauadaiCJVP3QAeByfQV8W/8FGvjSjQ6Z8MdMucSH/T9ZVT2J/dxH6Nhs05M5z4z8deNr/4ieM9U8U6i5ku9TuHuCXbdtBJ2r06AVhzSM7GQ8nsBxQyjcGA7Acew6Yp5XjFZkMYGyuajJJNS+WfwoZMA80CGJxzjNPbJBNPjjAG49qc3XNAEYyy7cU/aq7iF69RmnKmeelOC4YDrQAqfdOWx6cdKSeLZGTjLHpShC+D0p25gw3c8Y69OKAINx2naM/jineW64JBwepLZqSOLgKP/wBdSFQqtk80AQYK8jrS5fv0pzdDimFZTwBk+goAA3BJ4xTY18zLfdCnrTi+XAKNgdaFICMoHDUADKEUknknIzULA5UdR60rksozyen0qQN+7wVwfWgCIDLAE4z3oYfNjrS7QzNgkFfajGGANACKpCkdc07yjwc9KVWw444pwJBJBxikA6RVRRg5J9qiqVslDk5P0puz5c0wI6eoDRnIIPbmjaOMnHOMmnlT0yoIOAM0ARyN8uWJPpVK+ukto2O75sVbkkMedwwBznNcrq169zLgDA745qGBVurhrqUkjA+uadawmWQDHXvUQU8YrodEsW+VmTjrzQkBoWFslva7Dzuq2qAKdxOR19qZwp243fyqVWYKe5PB561oSw3hlGAeeM03btwB60CXaoB4A9KVl3Kc8BeTg+/FIBVz8wyMjtjrSYXGG57YHFIuV3EvsU9Se1LjDDHzHuaBgufmUnKr3xTj904GF79zSK3lsVI2r/AOuKUfMcg/N+lAxvllhxyKXymjyThSPTkU7AHXrTtp4Ck+oH4UARNDkBiTuHXbxigZ6dR6kc1Lx5hUBuFyOPz5pylVhcbMydmz70ANVe9CMr5ByPbFN984PrTlbcR2P0oAXj7oyR9OaGyqnjijDf3v0pPOKn5s4oAFyy+/pTJECtzyfSn7NwBIwD2zzTuVGO1AEJJC9OPSkBIOMdalzuVsLzQVBXPRh2oAjA2gmjYfvA9Panjr0z7UhVuvQUANWP5hknNKWpy9aRl4zSATrxSrwc9aBH8uc4pNvvQArY9KQClpV60AJSt900oFGN3FADCeM0dcCntH8vWk8vdjnFACNwKTdSEY4pKAKnShhS0VmAwUoO1qdtxRt3cUAAbJxilIpRHg5zRQA2mkU8ikoAZRt207HNFADabTqKAGU2n0lADdu7ijy6VeGFPIoAj2e9SpTKkXg0ABFJT6aVoAaw4oVcnFLT1XAzQAMmRinKuOM0itz0p3figB38JFNpS3tR94UANprJup5FNZtqnvQBQuflY0yD5pAcU64bex7ZNS2cf7snNAFmOPjrRN8sbc0ofauKiuM+Vn+9QBiX2GkpsEP2m7SPryKS6z5o+tavhOxN1qw5yFPp7Uxo+uP2StESHVkkHBQd19q+/9HmMluo9q+Jv2aYVt5mfp2r7O0OX/AEZSDkYHFaxTSLkmbkZHmxluVDAn86+UP+Cifiv+zfg7ofhlWYXGuXwklKnBWOEMRx3DECvqwHchwPmYbQB6kYH6mvzm/bx8bf8ACSfHYaTbzCSx0SySz45HmnBZvb0qZMqkryPn7RtNR2hltMQspye+cDua6fxFMLSxieOYGWQZdBn5fx71V0PT/scqyZ2Qt94A5z71m+MrxLdnijnaWJuVfbjdz0x2rkep9ZStQotnB61J9omIb7uecc5rR8N6O7NG8ax7lOW3n5FH19fw61mLJ9ougu0ZJ9cg16J4X8PNcQLJcSRwxDlVB2L+Jwc0bbnixjKvU91Etj4Qm1RnudizRq25SBge4xms7xBotvJK4I8lx1JruG0qaNGmimXYg4aE8CuS1yS3uhl8+aOCS2TUc+uh7U8JGnT97c4C</t>
   </si>
   <si>
     <t>6sZoWYjkZ4OetVxcPGCrHg9q27qM7t27K+lZd5GkeWfAHXNang1IuHUzr35ocxj5hzVvTMyW4JrKhklZmIUslWdJuDHKI3PU9+KpHMpLmOnt1CxkscAAn9K9e/Zx8BSeKPEUUmzKyMB93OK8lkia4it4UH7yZ9oGe3c19u/s4+GY/CngPU9aZBE0duwjdh/ERgH8zWkUdNSxv+PryPUvGlrotqRNb6dEluNvQSdGx+Ga+iPh5oC2Omwrt/1aYA9TjrXh/wAEvh9Nq98dWuw0hJ87cy5JcnBOc+hr6n0vT0sbWMHoDngc9OBW5xSepV8V+LrDwB4V1jxNqTLBY6RAbiR2PBdVyi/i2Fr8Z/HXjK7+InjHWPE2pSGS/wBWma6kLckKxyiZ9hX2j/wUX+MQjtdN+GWnTZkk/wCJhrIR8cZBjiI9cgHNfCSLuLdBltx7cgYH044qWYthySAOnpSqe33TQ2d20Fc+oNSADjikIjyd2OtPEZxkhvxFIVIcYqVM45Zj7E0AN2nGQefSjaQMmn7TnIpNpbqc0AIGDxkDg1Msa/L82B346U3YqqQBnPWkRNy4J60ASSNt4HReS1MVWcK2eD1oXMnmJ2/+vQxMasccelAD1Uocg5I7AUhkBAG05J6kdKTd82ASDtzRGAq4JZjnrmgBucNTlYg/eKf7QoULu64FIzAsFB696AI9vmE8n3Jpu0RgsW4FLK7hhjoOox1pFwQQwyD2pAIOGTI4pzkhhgVHtbkdQenapJMqowMn60wEfcmSQCGFR4z3xUzKxAJxilWI7gxGVHagBirtXI5pOxFOXOG9M9KMAUAIuegFPGChBOCOMU1W79KVsOwI6igBrKMZ64PSkyU5ODzkcYp/8W3HWqOqXotYiuPmI45pXAo65qXGxOp64Nc9yfc5p0ztJIWYljUlvbmZhzip3At6bZtcSLlcD1rqY7fyYyrHCoMtjr9arabZi0iXIw59ulXjs6gH0x29x+VUgGmNuV6Mv3l/mM9+SKciLtDZ57n0pV6AkbmHQ57nqf5UbQGCjt1HrTExuMoD68bvSkCgL8ucg5GTTyQigE8DtR5a46YU9STQA1Vjkzn5vQY605cEt12+ufvUqoVJCrhfTGdv40qxgSYHQ9B6UDEz8p3cigKu0k9KP4QOjfmKcvyNzw3r1BpAK0ZAwCMDrSfnjGPQ9Kc21lA5G3pxSbD+FMAUDALElVGMZyaTDbTtPyn+HvTkBUEDrSNx9aAGgAdf5U9m3FQP5daHULtbqT7dKT5mUEY5NADsfMV7j2pHwnP8VG5txycr6YwaN25SMYFADFO98kZPb2p28Z2mhY8DdmkVdzZx07UAIoIbA6HvQw5p3Ktu4x6UY3HNADQp7HFLzzls0rfdNNwQCetABGvmNjpTnXBxnNMTOcetSbe9ADSvFNK1Iw3A9qa0ZAz1pANJpVFAFLQAUo9KMfLRn3oAVuhpjZ2nFP3cYxSYwKAGsvy+9M59Kkx39KdtFIDOxzS07g0lQAlIDtanUbd3FAAGycYpSM0qx4Oc0UAMpCKeRTaAGigjFOx3oyKAGU2n0nWgBtNp5GKSgBq/ep1IvDCnkUARq249Kev3qai7WqYJzmgBCKbUm2msKAE255ozxinLRt3fWgBq/eFPHWlWPBp22gYlJ92looENJzx0pkq7VJzmpNtRSj5GoAz5m+bpVy2BVPrVZ4/mrQhX92BigBANzUy6XZCpzmp2gwpO7n0qG8/1I9hQBzsv7yU9sV2nw5s91wZW7k8Y9q5Dy98zY9a9S8B2IFqO3vimty43bPp34ByCPdxt6V9ceGbrzI4wfSvj/wCEB8ldoPUivq3wXIzCEA5JIAFdK2NpbHbatrlt4W0G/wBZvG2W+m28l3L6ARqXxn1+WvyB13WpPF3i/Wtbvm/5Ct094ryH/lmxyvPriv0H/be8eHwz8GY9CspSt54kuTAvOCYUId2+nylcV+fVrZyJCVTEpQAbmGQvYfL9DXNI1oXWyLC6pb2OmyQmNti/cdzgrz2GPm9O1cLq2oSX8zbdwUHlsV3GpaPbC1SRJ5LmXbh1kIPl+4FczNAJZMFQ204AxtNYHp1IVJR94zdD0wSSgIDvY9WXNep6bYQwWqiW52uBwNmP61z2h6LHHh5SwVeoHNddDDYSlVWeSJ8YG4cdPWs5M9PA4bkXMQ6haz2lr5sbbou5U5GM1xOstEzHacZ9Oa63VvM0mJhIMoRkNndmvNdY1RbmQR2kZDE8knrURRWPrKK5epUv7pbfKhg+e2cGs1bWa4bdPlUPRTzWmuihWSeb52/LFTTsSvK/d6V0nzlnN3lsZckCKCFAVTxiorvSlaFnjOcAk8c1dZRu5XirMkBjtWKkBG4I79aYpJWLvwls5dc8UWVpO25d4UcfrX6K+OtL/wCEV+GfhvQ7MYF9KI5GXjOMMOPwr4f/AGbfDp1bx9pcYH3pRlh25r9CfiXawah4i8DaNG2XWbzXXHIUAiuiCdjl5mepfDPw6ND8N2kYiCFYufVuOlbPjLxlY/D/AMKav4l1OVYbHSYTMxbgGQDMad+r7Bn3rbsreO3tUXOFXBGPQHGMV8S/8FHPjANmm/DLT58Ow+36vtbtkeXER6g4bNXsYO/U+LfG3jLUfiH4t1jxLqUhmvNUna5kZjkqpPyrn2FYO3apOcn0qzGoRSOAPb0A4FJs39BxUCKvuVFS9M47VN5O4bfxpI1VWBcHOc7fXB9aAE3KqMT1XsKarDqcr6CpRCvmFgvVt3X2pWUN94/QYoAjVlZgC2MnrUhQqx9M4HvTVhXcOOBzUm5lLc55yKAGSFSQEJwepxSR5XAHNO3NtKgfeowdvT8c0AIFICEEdeTSDf5vqMH+VO29AARt9+tKxwM96AEZ921zhSw2lcdPfNMLBvlB5NO/i2lelNYqjA9B60ANZSq5zmhV745p78kow2k9O+aZu2tjr70AO298ZNNdWVhhM54607zD2o84iMnPPX9aAEyg4684OO1MXaCRhjSr3xwWOc07n5l46daAEXaAQVLZ98Ug+8CucDqKftwu7PPcUcbc/dFAEfJyBzmkxzgHJ9Key857UZ2fd+Ud6AG/oaTcy8nkU7cnXOTQzDYWxxS0AjuZlhUvu5FchfXT3UzFjkCr+sX3nMUX5fxrLWHnk8n2qdwGxru7V0OjWJVgzAeuCMjpVXS9OMjDIz3xiuhhTylOOfU1SAl2YwyEjP47qPmYHPQe1N3fMCjbQvTjOKeH8yQkDk96YBwcAdfpSu21gcc+tLu5APX6UMM4xzQA3I3ZPBH40pkVmAI+bsCMilVD3H605QFB3YPvjFACbnz1PP3sDFJJtbOD06e9P3E9OlNbaScDbnp7UAIq7mz2/u1Jxtw3PsaVUwRj060ehH3uxIzSAaHbafulf7ueaVm6jGMU5gJMDADf3qXaBnI+poAb0z6io92W6U/h2Jz+lKqhWoAarEAUcYHHI75qRgOaYyllOKAFzUbMqqQDTlU7gWAIpTGrdqYDVJ8s4XimjjI9ak2bVI3YFIIjQA1YwTwKU8HFLnawoxuOaAEoPSnHpSD1oAFXvSt0pM806gBuRkgct2oViynIxStnn/CmnJbOcCgAZu2KFXvSlAvOaM0gE60u0Y6UvFLQA3ZjminnBFN6cUAG2m5p27mm49qVwKPeg0UVACUbtpzRRQAu7LdKWiigBtJRRQAg60NRRQAlJ3oooAWmUUUAL/FQWxRRQAqcnNTbvl6UUUANLcU3dRRQAo7U9V2t1oopMuIrdqTNFFMli9aa3FFFAhpY4pkzfI1FFAFRT81acfyxiiigBu4+Ziq942VNFFAGZbqDcD617B4QQR2qYHYUUUdTelue6fC+QxzKB619UeDJmWONgcEYIoorp6Gk9j5U/bi8XXOofFiy0iRP9E0mzSCBd38TkFn6dT0xXiFqq2d0u1dyuMsCevFFFcVTc9jAxTM7WoI4Zy8QZFfou7OPxqnDaK0v70LIM+mD+dFFYxPUqpXR1Wlw2ttujkgaUEdn2/0qz4i0ePSdMOoxMWAH+pbpzx1/+tRRQdEm40XY8wvdQn1e8SCSWRY+eNxIqV9KhtbcNFkMP4jzRRVx2Pml70nzFWVeMk81SlbtRRVDmRKAzDimTLvZVycZ9aKKcdzlkfSf7GOkwTeLrWV1y0YZh+tfYOnMNW/aGjWddy2OngRj3J5NFFdsNjmke+T3raXp8l4F8w2tvLcBDxuKDeB+Yr8ZfiB4y1H4geOtb8QarJ5t7qN1LK5PO0BsBQfQUUUpbmMjntw3Yxn8aWP/AFmOgJI/nRRUEksbb88etM3fJjGT2NFFACMx7cUsah2APNFFACyHy92Ogpm4s1FFAErH5fSo9zNxn9KKKAFWT923HWo2kbbwcUUUAEkrAEk5/CmeZuUgjNFFABvMkh3HJA4paKKAANwDTd24A9KKKQC7sLTufmNFFMCNnO5jTlfdhSOKKKAAsW47U7y+KKKQEMUY+YHmqOrXjRwkKMduvvRRUyA5oHczMeTVi1j3yLzjmiimtgOmhH2WFSmN3rirUn7td/U0UUxMXzCsZcDA/u0kWZG5OAaKKYIeWKuE7GlYlehwaKKOoxNv7tZTyx/SpdvHrRRQAik7TSbc/NRRSQD9xDAUZ24oooAft3Ju6U1VCr/9eiimADCZIHNN8zkcUUUkA7d8tRs2TjFFFABjbRuoopgL1pzNuZe1FFAEbHDCpCPk3ZoooATNIc0UUAFLk0UUkArdKb1ooo6AKW6UUUUAAp1FFHUBRTf4qKKmQDTShuOlFFSB/9k=</t>
   </si>
   <si>
-    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/4SjoRXhpZgAATU0AKgAAAAgABgALAAIAAAAmAAAIYgESAAMAAAABAAEAAAExAAIAAAAmAAAIiAEyAAIAAAAUAAAIrodpAAQAAAABAAAIwuocAAcAAAgMAAAAVgAAEUYc6gAAAAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFdpbmRvd3MgUGhvdG8gRWRpdG9yIDEwLjAuMTAwMTEuMTYzODQAV2luZG93cyBQaG90byBFZGl0b3IgMTAuMC4xMDAxMS4xNjM4NAAyMDIyOjA2OjI0IDA2OjU5OjM5AAAGkAMAAgAAABQAABEckAQAAgAAABQAABEwkpEAAgAAAAM4NAAAkpIAAgAAAAM4NAAAoAEAAwAAAAEAAQAA6hwABwAACAwAAAkQAAAAABzqAAAACAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAMjAyMjowNjoyNCAwNjoyNjozMwAyMDIyOjA2OjI0IDA2OjI2OjMzAAAAAAYBAwADAAAAAQAGAAABGgAFAAAAAQAAEZQBGwAFAAAAAQAAEZwBKAADAAAAAQACAAACAQAEAAAAAQAAEaQCAgAEAAAAAQAAFzwAAAAAAAAAYAAAAAEAAABgAAAAAf/Y/9sAQwAIBgYHBgUIBwcHCQkICgwUDQwLCwwZEhMPFB0aHx4dGhwcICQuJyAiLCMcHCg3KSwwMTQ0NB8nOT04MjwuMzQy/9sAQwEJCQkMCwwYDQ0YMiEcITIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIy/8AAEQgBAADfAwEhAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A85pKQwpaAHUtIY4U6gBadSGFLzTGLRg0ALiigBaKBMOaSgQlJzTGJikpCEpKBBRTArUtABThSGKKcKAHCnCkMWlpjDFOAoAa80Uf33UfjUTajbr/ABE/QUCuINStyerD6ipUu7dzgSLn3osK5P1GRRQUFJigTExSEUIEJSYoENpKAEopiK1LQMWlpAPFOAoGh1FAxaUCgCGa8ih4zub0FUJr6WXgHYvoKaJbKhJJ5zSUyRMkUmaAJobya3PyNx/dPStW21KObCyDY/14NJoaZexxmikWFIRQSNIpCKYxCKbSEJRTEVaWgY6lApAOFP7UDFFKKBjuAMk4ArKur5pGKREqvr60ITZUxTghqiRdp600rjrSGIVxTCKBCYpKYi9aX72+Fb5o/wCVbkbrLGHQ5U0mUmLiikNiEU0igBtNNAhKSgRVpaYx1OFIEOFOxQUOAp4GKAMzULrc3kIflH3veqiRk0ybXZL5ZHQUoQ/jSuVYCh6d6ZtPWgVhrrxUZGKYmJimkGgQ0HFXbG9NtIFYnyiefamI3xhgCDkHpRipNBKQigTGkUygQhpKAKtLTAcKUUhoeKcKBj1FJM/lws3oKBGEoLsSepq/BF8vSlJlU1dlkQZGKU2xxwKz5jfkEW0PeoZrQg/KPpVKREqbsRG2OOahkgI7VaZm4kJSk2HFMmxEVwaaaCTa0a53o0DHleV+lauKTKQ0ikNADSKYRQJjaSgCrS0wHU4CkMcKcBQMeKqak2IAucbjQJlSCLODitKNPSokbU0Xo4MgE1P9kbGf51kdSE+z47U14x6UA0VZYx6YqqyDHSrTMZRRXdBjpUBT2q0zCSIJ0wtVu1WZsn05/L1CI5xk4NdQaTGhDTcUDGkU0igQw02gRVpwpjHAU4VIDqeKYxwqhqHMkS/jQA6FcVfgUFhnpWUjohsbNpGGP3c/WrjxFeCo6dRSNUVJcA9KqznC5x1pWHcpyHNVpOlNGcis1RtVoxkQSjIxVRlxVmTGRHZco3owNdeBkU2CAim0hjTTDQIaabigRUFOFAx1LSAcKeKYxwqhf/6+EUASp16Vei42ms3udC2N3TnXHzH8cVsP5bR9j7UWLT0Ma5AJqjc9FA6ZqRlSQ4GKpydaETIhaoSa0RhIhkPFQMKpEMrn/WjHrXYp/q1+goZKAimmgobTSKBDTTO9AioKcKBjqWkMcop9MBwqjfA/aYeOKAJVHIrRiQkDis1ub9DYsl28ADGa02b92CR2602XEy5gWYn2qhM3r2qWUiq/SqcnWhEyKjNzUZ61ojnbGHmoXGBTJZXQbp1Hqwrs8YXFDJQlMIpFDaQ0xDCKb3oBlIU4UgHUtMZIOBS0gIrhmAUDgE4JrPWaWS98iQg+Xzmi5VtLmrbIGk57V0um2kMqN8wyBzmsm9TqglbU1U03yxnI+mahnI2kE5A9KOYrlsZ8u0ZHcjiqUsJJAPGRQFirJHWfPGR0pozmVDG/XFMII7VaOdoZUM/3M1RLGadEZtQiUDgNk/hXXdqGJDSKb2pDGEUlMQwim96AZSFOFIB1OApjH0tIB6QC4bYXVF6s7fwqOSfyrHbyoNSZIC0qEk+Zt+9UXfPaxtZez5r9TUh80DiJ/wDvmrjXRtoN6O6yY5GNtCWo3NWsUV8S3cb483cvoa0rXX47r5ZPkb60pR7FU6utmaEe128zqO1MuJVE2MEDGKzudJUeeAcvj86zri/t1PVaau9jKTilqVn1C3I4IOarGZZDkVrFPqc85J7EZIFV7mQBMDkntVmTFs5ns3YRqGmYcsei1t6TdTXBlWR94X+LHegLWNIjimUgGkU3FADSKZjmmLoUhThSAWpBTGKOtOpAMmB8s47EZ9xVqG/aG+jKRqYkwxjHyhvbIqk7ILXdi9r3iWC905bSy0tbO5MgLTJIx+Udhk1lXtnMmkQXovbgjdtnA5KcelRKdmi407pnNxPc3MhXO7AJJYVNao8zttXay+neqbRCi9zctdTe2spHZgzJjCHvVCXXJbks5GwegqXTRosRJKxny35J5yc+9JGrXJXbG5ycDAzVKyM23J6kbqgPDE4pBIQeD+dAhWmfv3rV0tbRbG7e5iDSBMxuT37Cs6qfL7prRcef3inFtTcD99uTW9o0BhsASPmc5NaGZfNNpANPSmGgBppn8VMCiKdSEOFSUxiilFIBxGVxiqtq2bpkbqKRcS0IBNdMP7ozxVue6EdoYiWLkYI2kZH1HWpauap8pz0izFisEJXd6CrNrbyWI3SEnA3MOwppEa3uTeFbBdQu7y/nTdDGpEYI4z61jatH5N5IEGBnIFO/vWE4/urma2Sw4rrLC4RdI8k/upAdySJgkN0574xmlO9tBUt2ZcMCxOWkAYdhUL24ZyygDPYU0wcbIR4c7E71Jt2rtB4quhHUjji3X+0HJJHFdiqBI1QdAMUmAh6U00ANNMNADSKb3piM8U4UDHrT6AFp4pADHCk1UhjkaVZYceYpzg9/apbsaQV9EaUM/wBnmkkljaMuB94cCrltcW10x8x1UD1IosaKS2ZdI0yBCxniXHcsM1h308ert/Z2nZYyNmWXsq/X1pLuErP3V1OhgtYNL0ryIflAG3NcXrUQl+ZBll/Woi3zXNasUoWRRtIYbmPtuHUVeFmQOtatnJFaAtkzHFSmz2jmlcuxQ25kdgcgfKDTD1qjIm0eMvqZeQY+b5fw6V1BoAa3WmnpQA00w0ANNM70wM8U8UAPWnUAOFPHWkAj/cP0qOyOJBUT2NqW53mlCK9tViliRuOQRmorjwrpbTMWtlxgngGkm7G8oqT1K8uh6FCMC2j3Ad+apQRxQuVt4wB6gYqJSfU0hCK2RJdhmhOT1rl7yF1diexqYPUK0dDJa2TzS6sUb2NWo0u8fJPke4zW9+5xqGuhMEvh/wAtgPolMeCR/wDWzSP7ZwKV0Pka3I2AVcDgCoMZqkZs0tIh33DS/wAKfzrapksa3Wm0ANpp6UAN7UzvTEjPFOFAyQU6gBwpw60gEf7p+lV4TtINRI1p7nTaPftbkEE++DV281eQjCsc+tZo69LXMxzM6CSQt87YBauh03SEkZDLNEqtwMN1qZ9i6T0bJtc0uG1jBRgR6g1xd4qlmqYqzLqO8bmPPAuwkkCqlndeVc7G5Uniui10cLdpI6DepjzVKY9T2qI7mk9jPlbNRCtkcjOns0WOyiCqBlQTgdzUtAhppKAG02kAw03vTEZ46UopjJR0paQDhTh602AuMiqn3WI96iRpT3LdvOUxg9DzWpbbbiRcnIzzUI6L3N54ovs4iKgqO1YOpbLE7o7mQZ6IBnFL4mW/dV0UJNbuJY9kjszDpk1z17q1w8uOeKIU7Mzq4hyjoQLNJP8AfYn2qwIMYI61raxgtdy/FcMY9pPIHSq8s5z1qUtS5S90rsc0g7CtDFnWxjbCi+igUHrSENNJQA002gBhpvemLqZ4p1AyUUtIBRTqAHCqlypSXPZqTKjuMRyDwa0NNnxLuLHPpU2Nky1da60MmzG5h61iS3U2oXTSPnYvQDtTStqTObegpT5gUVQQecDmqc8Qc4YEEn0pp6kNaFJflJ65HAqdLkghWqmiIysSNJtYOOh4NMlbnNSim9CPdk1YtkMtxGnqwqiTrKaakBppKYCGmHpQAw0n8VMCgOlKKAJBSikA6lpgOFNmj82Mjv2qQRmBiHweo61MkvlsGGaRpfQs2ssHnl57ZnL9CRwa3bS+sI4yEiiQ9/lzSdzWm42GzS2sof8Adx5AyMDGaxbq7h77QPQCpSdy5yjYx7i6hycKKpFlkbcFIHatUckndkpJ2801mzTEOWtXTEMcc16yForcDeR/Dk4zQBvRypLGrowZWGQRS0gGmkoAaaaelADKb3piKIpaBkopaQDhS96YDh1p1ICjfW5A85B/vD+tQW7gsNw4pMqJv6f5L4gbABbdG2ehrXj8Ord3XkKqBiOM9zUXudMYrqULjwmPtfkK0scmdp2SZrGvfD0VuSN7sQe7UlLU2nh48vMjIls40baBVeTZuwvAHStUzgktSItmkzTIZInJ4rrDGulfD+5kkGJb9wqA/wB0UwOb0bUzZyCGU/uXP/fJ9a6vIIyOQaTEgPNNpFDTTT0oAaab3pi6lEUtAyQdKWgBwp1DAXvThSAXrwehqndabPp7wSSIVhuF3xH1GcUhrceodBkZx7dq07XxFNbbVmLfL92RetQ12OmMrbkkPiGGK68/7Rlhk8nvWHqWrI8jFJAcn1oSdy6lVctkY8l00uQM/WoWzWqRxNjCeKaMk0yTo/DWhSareAt8ttHzK56AelR+L9YTUtRW2tuLO1HlxgdDjvQhvRHO4rpdCvvNi+zyH50+77ih7Erc2D0pKksaetMNADTTe9MRTFLQMeKdSAUU4CmA6lpAVbrUIbUgZ3Of4Qa9D8dWkCeH9Fh24aOFdjAdQQM/jnmnb3WOHxWOBjlML+XL+HuKtEWcwIYEe4rK50JLZlSXTNOZMZO7sc4rKmsLdG+Q4A96akyZU4oqyKidKrs3HFaIwZGMk10vh3wrdau6yuDDag8yMPvey/40CSua/ijXLfSLL+wtJAQ4xK69vx9a4ECmhSeotORmjYMjFWz1FMk39O1oMBFdHDdpO341tDBGRz71LRaY00wjmkhjWpo+9TEVBS0DHCn0ALS0AVbnUoLYYzuf0FZE+qXNwSAdi+i0JEtlI5L4zzX0X4g0WTU/h9abVzdWsEcij1woyKq2gRdmeTvHHcRDI4PQjqKpS2FyhzE4dfTODXOnbRnbKN1dFdobofeRqgmWYDhDWlkYNspi0uZpNqocnoAOa27DwLrN8QWh8iM/xS8fpVIztc7LSfAOn6diW7JuZRzhhhR+FU/FnitNNhNjYEeeRjI6IKLFPRHmTM0js7sWZjkk9TRVGIoGaXbk/SgB2K0tP1SS1xHJl4vTuKTQI34riK4j3xMGH8qdSLGGm96AKgpcUDHgU+gCGe6htx87c+g61k3OpSzZVPkX260JEtlHbk5NOYBFqiSxolkdR1yytME+fcJH+BYZr6zjRREE2jbjGPaqQHi/jjw6/hrVDdRIf7Mu3yCBxE57H2PauaLHqvI9q5akbSO6lLmiLbW17qNytvZwSzSt0VBmu60j4YSMFm1i4xnnyIj/ADb/AAq4QuRVmkdZZ+F9K0sf6LZxq394jJ/OpWtlLHjit7HPc888d+LE0oNp9mQ10w5I/gFeSyPJNI0krFnY5JPepYpMTGKFBJoJJQlCdT9aAH7aaRzQA+GaS3ffGxBFdDZX6XaYOFkHVfWkxosGmd6RRWFOoGV5L+GIkZ3EelUptRlkBCfID6dadiWymcscnk+9JtpkgetNbp60AdR8OIFm8d6UrDIV2f8AJGIr3DWvG+jaDK1vcTtJcquTDCMsPr2FO9kVGLk7I5C8+Jmha/8A8Si70i5aG5IjJkZABnv14otPhvZNqHlprI+yNykfBce2e9S0po0UnTZ6DpGhadoNt5NjAFz9+Q8s/wBTV1jVpWVjJtt3ZC9cd408Uw+G9Mdlw15LlYY/f1PsKAR4HcSzXdzJcTuXlkbczHuaYE5qRCSjBAqSKLigCXaBmoODL8nINAExGBTVGeTQAbPSlXcjBlJBHQigDYtNRWUCOY7X9exq7xUlIrcAc1n3d2WzHGcL3NNA2UMZpduKZIUlACYpGHFAHW+A7mHS9Q1DV5SN1laN5Snu7EKP61h363cl2t3cM7vc5cu38RzzQ9i4bim0Z4i6YLAfdNJBqepadIk0NxIrAhl3c/lUpm84PlR7L4D+Iya8E07VlWDUOiP0WX/A16Ay4rRO5zyTRl6zqMGlafLd3DBY4lyTXzp4g1m48Q6xLezk7ScRp2VewoEZ2ynBBSENaPcwJ7daXfk4QZP6UIA8nccyNn27VJsCjgCmBG1KowKQC4pcUANK96swXssPyt8y+hpMCW8mwvlqeT1rPxmkgYuKQimA3FGKABVyaCMuBQBYsd7O6KTh2GVHf0r0Tx9bxWGneHdMWJVdIi7tjnOAP50+hpT+JHKogVwPWqdwVQPG2COoFZHovSJlNdNCcqW+XkY6ivXfAHxMkvQmma8uxz8tvdE/eHo/off8/WtInnz1Mn4peJjf6iNHtJM29ucykHhn9PwrzwLVGTHAU4UARzJlfpT1C7RtxigB+KQigCPFGMmgB2KXFABtpu2kArkuxY96TFIBCKaRQA3HNGKAHAYFNHUn0FAG34Msvt3iOwgK7g9wu4ewOT+grsfiNJ9q8XGLPEFui/Q8n/Ch7G1BXnY5O4lHkhh1HNYt5N5jhs1CR11paD9MsDd3DZBKqu416Db6NbeFvC8ut6hGrXs3yWkTdmPfHt1rRHFJ6HnjFnkZ3JLMcknvRimZhikJI7UAPGD+NRf6p/8AZP6UAT9aQigQwj0pQKBi4oxQAuKTFIBmKXFIBCKaRQABeKNtADiMLmojxGx9aAPSvg9pIn1G41GRcrbptT/ebr+n86zvEd39q8U6pdfwmcxj/gPy/wBKJbHRhvjv2OXuZcOw7HkVmsCxIqUXVd3Y9I8B+HTdGKSRSFkYOwI/hHT86zviH4hGt6+YLdv9BsQYYQOjH+JvxP6AVa2Oeb1OSxRimQG2kK54oAQAqabJ0O7pQAsGTH7Z4PtUpFAhu3FLigYuKMUAGOKMUgI8UuKQCEU0igB2OKAtACSfdqOUYiA9aAPdfh1apo3gT7ZKMbleeT6Af4CvJLm+BXLo2Z3LAZyRk55olsdFB8tzNuj2OQ3XmpdHsjqGoQwD/lo2CfQd6lBJ6nr2q3qeFPBLyRYW7ux5MHqq46/gP5145gk5rRmDHBaXbQIQ0mOaADFVZCZ5vLX7o6mkBbUBVAA4FLimAuKXFADcUYoAXFJikAzFBFIBCKbigB2KdigBjjOB70eV5k8Ufq1AHr2oai1l8M1tkOJLkLbrz2PLfoCPxrzSO3aS782QDZEMClI6qMW/QpXx86ViBhex9a6/4Y6St5q07OMqgVR7bjz+maIkVHdtkXxA1r+2PETwwH/RLP8AcxAdOOp/OuVCmrMBcUGgBuKMUAQXEhUbF+81Pt4fLTn7x6mkBNjmlxTAXFJigAxRjigAxRikB//Z/+Ex6Gh0dHA6Ly9ucy5hZG9iZS5jb20veGFwLzEuMC8APD94cGFja2V0IGJlZ2luPSfvu78nIGlkPSdXNU0wTXBDZWhpSHpyZVN6TlRjemtjOWQnPz4NCjx4OnhtcG1ldGEgeG1sbnM6eD0iYWRvYmU6bnM6bWV0YS8iPjxyZGY6UkRGIHhtbG5zOnJkZj0iaHR0cDovL3d3dy53My5vcmcvMTk5OS8wMi8yMi1yZGYtc3ludGF4LW5zIyI+PHJkZjpEZXNjcmlwdGlvbiByZGY6YWJvdXQ9InV1aWQ6ZmFmNWJkZDUtYmEzZC0xMWRhLWFkMzEtZDMzZDc1MTgyZjFiIiB4bWxuczp4bXA9Imh0dHA6Ly9ucy5hZG9iZS5jb20veGFwLzEuMC8iPjx4bXA6Q3JlYXRvclRvb2w+V2luZG93cyBQaG90byBFZGl0b3IgMTAuMC4xMDAxMS4xNjM4NDwveG1wOkNyZWF0b3JUb29sPjx4bXA6Q3JlYXRlRGF0ZT4yMDIyLTA2LTI0VDA2OjI2OjMzLjgzOTwveG1wOkNyZWF0ZURhdGU+PC9yZGY6RGVzY3JpcHRpb24+PC9yZGY6UkRGPjwveDp4bXBtZXRhPg0KICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgPD94cGFja2V0IGVuZD0ndyc/Pv/bAEMAAwICAwICAwMDAwQDAwQFCAUFBAQFCgcHBggMCgwMCwoLCw0OEhANDhEOCwsQFhARExQVFRUMDxcYFhQYEhQVFP/bAEMBAwQEBQQFCQUFCRQNCw0UFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFP/AABEIBDUDqwMBIgACEQEDEQH/xAAfAAABBQEBAQEBAQAAAAAAAAAAAQIDBAUGBwgJCgv/xAC1EAACAQMDAgQDBQUEBAAAAX0BAgMABBEFEiExQQYTUWEHInEUMoGRoQgjQrHBFVLR8CQzYnKCCQoWFxgZGiUmJygpKjQ1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4eLj5OXm5+jp6vHy8/T19vf4+fr/xAAfAQADAQEBAQEBAQEBAAAAAAAAAQIDBAUGBwgJCgv/xAC1EQACAQIEBAMEBwUEBAABAncAAQIDEQQFITEGEkFRB2FxEyIygQgUQpGhscEJIzNS8BVictEKFiQ04SXxFxgZGiYnKCkqNTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqCg4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2dri4+Tl5ufo6ery8/T19vf4+fr/2gAMAwEAAhEDEQA/APkNfvU8mm7dp60VBoLRSUGgBDikoo6nFACdTilC4PWgLg5zSk0wAmjpSUUAAGTTtu09aarfMKdSAKTIprNQF5pAO4o6UlAGTSGKv3hUq9aYqYI5qT7tACAd6XPNNzTgvTmgAVeetOxSFaKAHZo3Cm0AZoAcOadwKaq4NOFAC0UUi/M2KAHDrT1XBHNIqbcc0+kOwvSm0m6nDB70gsKKQDJp23bQq4I5pFChdpzml3UjU0CgY/HvQq8jmkAyacEwc5oCw7b70oXBzmgdaKBjs0vC96jpR1oGSbuaT8aaBQDk0AOx70CjbRigB2AxpNvvTaXdVALt96No9abmigeguB60o4Oc02l20CHbqN3vTdtAFAD/AMaMe9JRtNAai496Me9JtNG00BqLj3ox70baTaaB6i496AOetKF96XZ70BqGPejHvQBS7R60BqH40fjRt460KuaA1D8aXNHl0eXTEFLx60nl0u0+tABx60cetG2jbQABQe9O49aRVpdpUdaREkHHrRx60m6k3UEjvxpMijdSbaBDqDikxQelACHFN2j1pdu7vil2e9Bomuo0qAM5oyKcy5B5pnl+9Md0Ln3pcg0m3C9c02qAcxpuaMZpCvpQJi5pDyKQikoJsOA2jOaA1IBkUm33pCFZcg81GVwM5qRvrTSvXmkIaGo+79KXZQy7c80gCk9xSfSlBpgH3himsu3PNOIpOoxQAyinMu3vTaACiiiglhxScUGk28UAOyKQ02nCmMTbSU40m2mAlKDSUUAKR3o+8MUA0vuKAG7dozmil+8KTbt5zTAKTAoPSjdTAzqKSipAKbRSE0ABNIv3hQBk07bt70wFJpKKKBgOaVlpFb5hTqQhu3bzmhmozRjJpCEC80tFAGTSKADJp23BznijbtOc</t>
-  </si>
-  <si>
     <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAQDAwQDAwQEBAQFBQQFBwsHBwYGBw4KCggLEA4RERAOEA8SFBoWEhMYEw8QFh8XGBsbHR0dERYgIh8cIhocHRz/2wBDAQUFBQcGBw0HBw0cEhASHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBwcHBz/wAARCAC+AM0DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwC6i1Oi01Fqwi18Hc+zALUyLSqtSKtIAVakCUqrUwWi4EOyk21ZCUmylcCvtpNtWNlcT4y+J/h/wUTDdztPf/8APrb4Zxx/F2X8aqEJTfLFXYpTjFXk7HW7KaVr541X9onWJ2ZdM0m0tk7Gdmlb9MCsq1+N/jIT5aWzlU87Ht8Aflg13Ry2u1d2RyvH0U7H0yy1Gy141oPx7Zpki13SxHGxx9otCSF9yh5x9D+Fev6dqdnrNlHeWFxHcWsoysiHI+nsfaueth6lH40b0q9Or8LFZagdaustRMlYmtiiyVC6VedarutMRRdKpypWk6VWkSqTAypUqlLHWrKmKoyrWsWS0ZckeaqyR1pSJVOYYrRMhozpVxVKQ81fmrNmOGrREM9vQVYQVGi1YRa846CRRUgWkUVMq5pXAaoxU6imhalUUAIBS4p4FVtRvY9M0+6vJjiK2iaVz7KMn+VCA8k+MXxUk8Mg6Hozj+1pUzLOOfsynpj/AGj+gr5+0/SZtXuZJpZHkkY7nkkbLMT1JPer8klxr2q3moXTb7m8laV/bJzj8OldNptktrHgDHevpKNKOHp8sd+p4spSrz5pbFCx8LQrww3fWty38H20i/6vOe/Wr9iAzAV6DoGlpOFyO1DlLubxhBdDzv8A4V0J48wsw4J59ah0K71X4Yax9oKvPpFwQLuFckf76/7Q/UcV9D2mgwiHgcY9K43xboMYSVGjDRsDkEcVM23HlnqmNU4N3hozropY7mGOaJg8UihlZeQwPQ0jCuN+G2qBrG50SR8zaa2Iwephblfy5H4Cu1cV4NWDhJxPRhLmjcrMKgcVZYVA4qUUVnWqsgq44qtIKaEZ8y1RlWtKUVRlFaRYMz5hWdNWnMKzp+9bIzZmzVmTjLVpzVnTferVGbPdlFTpUK1MgrzTpJhUqVGoqRaBEyinqKYtSrQMUCuH+LtzJbeAdUWP78+yH8GcA/pmu6FfLvxD+JOoeIPEGoaak3laLbymJIgB+8KnG48dc8/hXThKLqVE101MMRNRg79TF0uAW8G5uWPtV4y4Kr3NQRfMY17VDf3MlhJvjhaUnAAWvdvqcEV7p1OmquVLED3NepeE0DbMkVxPgi+1DUtL1JLjSVNtYIHkdlAyCccZPzH2XJ9qs6Lq4stXjjgci3dhhc5H4VnNuO5tTUZ6I96htSsAAGeK4zxVF+7bcK2dZ8WJoOlQ5bdM68AVxsGt3niaGdmmtFVBxGTy345qXUT0GqTTuzj9GjbTvGVhdRkhJg1tKP7wIyP/AB4CvVmFeU6LO9x4qtbSRCrrLu/IE/0r1dq8vGfEvQ6qKsmQMKgerD1A1ciNis4qvItW3qvJVIRRlWqMy1pSiqMwq0IzJhWbOta0wrNnHWtoszkZM4xWbL96tO471mSj5q1Rmz3ZKmSoEqdTXnHUTLUq1EtSLQImU1KvSoVFSrQMkWviHx5b3Fr4x1CFVZYY7ybcoOPm3sc4+mK+3RXyh8bNBvNJ8ZS3000ckN5IZUCMchcjgjHBGR3r08rl+8ce6OHH6U+Yr6dIs1tGc/MBXT6TaLdsFKg5PcZrgdLuGhOwnpXfeG79YpFLdjmu+rFozws00d5YeGNQ0+LzreMxq45YZziuPkizrStG+7EmSfU5rqfHXjbVYfCqQ2IEMLsEkkx8wXgHH+NYPhz+xy1q41KGRwRvTeC2e+awlpG52U1eVrHZa3a/2lqSWsuWjKqvykA49ASDj61x2r+DF0uyuLfT57xZpJRIjSStiI98ICByBjnOO2DmvUNas9LN/DcaXqCSYhEjK55UgdK6TR5tH8R2LyTQiO7iXDow6H1qaU5apMVeEfdckeMeB7KU+K4mnYvJBbu7MRyTwv8AWvVWrlNNhjg8cXiRgfJAwOP95a6tjXnYp3maxViB6iapmqJqwKIHqu4qy1QPTQmVJBVOYVekqnNVIRmTVmXFas/NZk4reJMjJnXrWXMPmrZuBxWTMPmrVMyZ7ctTpVdalSvPOksipFNQrT1NAFkGob7UYNNt2nuGIRRk7Rk0GTaOOTV+10NNUs7iG4U/vlwT9e1dmFwjqu8tjnr11TWm557YfFO21bU5rGw025dYR89w5ART2GOpzXnXxYjl1Q2dwyFmiZuccjPJOP8AgNeu6F4Cg0eG8hity0sdw28bhk9x+mK5/wAb6B59o0PluiNuAYEgqQT3H1r1aWHhRlzQR5tas6keVs+braJrW8MTMSGyV4wcetdhodwE5b+HrWb4ghuI4G86Hy7lGICt8vpyP0/I1mWd/JEskKo5nOFAIx6cfqK7JR50c1GryPU9Dm8SW92y2bKGbp85Cr+tdB4b+Hei6veR3N5JaqkY3bY59rZ9c1xFp50sFvPc2qPLGuGBQc+446816p4E13wHdWk9v4ht7OG7YYEjqsTenfBz/kVySgouyPUp1PaRvNjNR8Hw6Bqy6hDbrNAgyB5wc8eozgjpVbxF4i+yK19YTArcL8+zvWr4pi8E2thCvh/Y9xLgyf6Q7kAe5Y4/DFeQ3+oRx2jwqditMxClucfWlGnzPQqpWVNK7PSPhhcy6rf6pfTZZtqrvPckkn+Qr0hhXM/D/Qv7B8PRq+4T3R8+QN/CSBgfQCulY142KadV8uxvQcnBOW7ImFRMKlY1CxrnNiJqgcVOxqu5qkBXkqlLVyQ1TlNUiShMKzpxWlKM1QnFaxFJGVcDismcfPWxcDismb71bRMmezqalWoFNSrXAdBOKv2tujfNI3vgDOPrS6fYBtskzADqq+vvXS2emo2xfKG08k4JP+e9erhMDf36i+RwYjFW92JXs7eFhj5FHbK4/OtywEUcpQbSwGAy5PPTIqSOOGIlXCLETwSR+YFXYobaFwyyxoM5IAbP16V66hbY8yU09zJTSE/tyYIAouYN/l4wAUO0/mHX/vmuY8c+FLlbdGj/ANWW+bIzjIH/ANevR7uKzli817gKEBJcblZfcEdPzqqsN7dRyW8rJPYkBo5XULI+B6Dgjnrhe3BzkNoyc3uj4y+JmgNEyXDRsPL2klWwDj6fTrXJeFo7a71G6uL3dOyg+Sro3y8nPQ9c+vSvqP4h+Bp7mFnkXdsB2KBggc9j069/fsa+c7bTY9J1L7NdKYI3nXBxgEd1LYz+fvQnZWJkk9TVu7hIb3zzGJcZdiDtXBICog74z+v0rqdLtfDOtmFLvTUaQDc2dw+bI/LrWHrdoIoreBYxDO8h+6vzSDAGOnTK5/AfQ8mbqYXUsbealxMxdQp7AjPp/EP89KORS1HTxEoLl6HceLxo1npbJ4fwhVgruXzgnnAB68Aj8KseAPAEPjHU9Nkm2i2toTJNEuNzcj5T+JPrwaxLDQb66MarEZDLAB8mT8ucnn6HFfQ3wg8M3HhuGa7v1WHdF+68wBGWMckn0GaFFRWgpVXVmr9DSl8LkoBHleMLngfSsG+0u5sT+8Tj1HIr01JdO1q0S9sLiO4ifgyRSB1z9c1C8VvcRtFNEG45z/OuKtgaVXVaM9CljKkdHqeTtULV2+raBbrlPK2MeUdTgGuOvLV7WTY/fkHsRXkYjCTo6vVHpUcRGrtuU3qB6ncVA4rBG5WeqsgzVt1qB14qkJlCVaoTitKYVnzitIksybnvWPOPmrauR1rIm+9W8TJnsCmtmwt1SPzG2s+3cMruA/DI9Kx4QGfB6Yya3rcyLaqg2KfLPJ54yT0+h9a1y/Dp/vJfIxxdVpciOl065RJ1VI49o54RAMYJ7Dpx71tpHHqDY+8Qvz7iDkD+WK5TTI3V/nkBULw6nPOD9R+grd0h7dJZ90j79nG44H3h+Ga9yB5nKtzeNhbrHyXfYc8xqAOmR97p7+1PS1tWizslDL8p/eA/jwp96SB5DMrZDI/X1H+QabbmUbx5YGRkAsOCDnI69s1pa6IcX3JLa1j+ZT93odzHP8qTRphYTtpRUqi/PayE5JUdY89ivPP90jrg01jMJeiJuAPGSMj/ACKiurVpyq+cC/3o328o4zhv8fZj2NQ0ZOPcsa5pwu7dugHU49fWvK9Z+HNvqnmJJbqu/wBuc17Bpk/2u2Es2PMBKSpnhHHUD27g9wR61alsoVO+T7p6d2b6Co5Xe6BSVuVnjem/CLTtStoTfo32iD5QynH0Pvwa5zxX+z9a2Fr/AGno91BFexEiKC9bCS5H3Q3Y8d8j1x1r6LtI1uJVMcYXqMev49/r6V5h470u/Os+bf3qyWsUuPLc7FAIyBjPTn8+tfS4SnTx8feSv17nwOaV6+SyvTu4p6K+lvP0PnD9n7xjrlt8aoPDniu1+yswmszbTR4KMw3Kc98jgEcEHivrgwg20UVwqyC3Jtpkdchh93kdwcV4L8QZbPwv4k+HWspEJNbgvfLTzUAZrc9i3QgE/KRx8zYr2nwx4rsvFt3qUlvG6RXRd1jl4dSkjRtkDod0ZOPeuTH4P2VGy+yz1clzX6xiedq3Olp5/wBI17LRdN0b7QNPs7e0Wch3EKBFcjvgcZx3oksiSGjOe/FblvGksMLEryOf5VGsZj3IigjnDYzXiWR9bzdjDbThew+XtJPbP8J9K5jXdDMlncxtGFlhUyxnof8AaFd0VkSbDvt3cdc/jUGoWsatDPITw218DAIPB6/54qalNTi4vqVTquMk0eEMKhYVoalB9mvrmEdI5GUfgaoMK+Was7H0Sd1cruKruKsuKruKaBlOUVnzitKUcVRmXitIsTMa5GAaxp/v1uXY4NYVwfnroiYyPYYIZH8w/dib5NxOB+vX6e1aVjDGFUXFwWYqdu1cgjsNx989qp6bZwurzSSkuTjgDj2J/P1rpltrOFBC6b1wAVlYNgkey+vvXq4eCjBLseZWm5SbNPSIYLPy5PIk3R8kmQBWA5/u+2OtX7SaxaJ1W3dyik83G4enGV96q6YsVrIPs6xpGUYYLO38PoTjuOhrp9NcGLDRxEkA8Q/7Q+prtiY/Ijs7uDzVjFrOVwcAYIzx6AVqJ5JkQsTbxsdoV8knrnH+B680zcwZM+X3/wCei/yNW5YoZrZ90cY5BDb3buex4rSItOxRuvJR40YzrKOzBUBHTg896juL2KFFEkMyYPysZdwOfwHp+vvV65trUQOfLd0PzFHkGFzzwBz39ah/dmLy1WJcgjbt3jpkct9Ov6U7ENJmf/asOmaglyqsLW+ZIpCxBWN+iP09cISQf4c8Ka6GKKSdiJGOOzsPve2P0x26dhWNJbQ31hLb3NtG8TKyOpQKCpGCDt/H86m0O/mmgms7yQvfWJCF+nmR4+Rx9RwccblYCs5KzMZK2qN4OsHyopGeuD8x+p/XFL4i0W38T+H7uMlRI8eC2OcrkioFY3IO3APRjjv/AJ/rU2mzvGbi3UjdICEGf4scV04LESo1U0zzM1wcMVhpRkr6f8OeI/CvT7Xxp4i1C01XR4L+x0eBGgvJgW8mYu2YwDx0yT17VDrAk+Hfx3hsocR6LrNo1xbIFACyGRmlGfdmLV6r8F7S0tvCCSRReXcX001zPnAJZ5GA/IKB+Fch+0xohXw9oXiyBSJ/D18jysOvkOdj/lkGvfxtT21ScejPj8ow8cLQoz3cbP8Ar7z0G3ljZpFYEYbcMHsfwrmvH3i+bwbYwXUNktzHcSiNg8+zaxGR256H8qs6DeC802xukP3kCn8hWJ8YdF/tzwJcqw3NbSRzDAyeGwf/AB1jXyq+KzP0iKTszA0n4wafq2oW2latayaNq0smyKGV9yyjOOGAxnPbrXo9whe1PBO5ep9a8ITQ7WW7+0XbJ5UhRtrjDZ5BcEr8pB4/GvTPhl4rHizwtdm4njlvdNnezmZDu3lQCH9sqwP1zVVIKL0N3C0FU6M4bxJbtDq1wzYxKxcY9CaxGrqfGNq8N8rEfKRjNcs9fLYqHJWkkezh5c1NMgeq71Yc1WkbFYo1K0nFUZjxVmV81RmatIoTM665zWFcJl63bg1kzLl63iZM9c0v50G1Wbdx045B79MV0TGaSdtqsu1gMEcdfXt+ArF0+W4toY381MJzsRN5x69QM9O9a0Wp3MRypim2fMd/yP6ehFe3TVkeXN3eh02mJcbXZpIeVzjcSeq+/v6V0NksxjbcsbYA7E9/pXO6ZrkckbRvppRmXAbz1YfeU5wB7V1Wmz27xOu5CxKnaq5x7da6Y+RnrbYsfvmePAjHBGdx/wAP609rmaOEsY84KgHjnIbvxTh5SSIpkVW7K27P8jVqeFfJj3SQ8kHazhecH1AqkiU/Iqyvvh2rGdwjUEZ4HHrnFYl/LP8Au2wEx9Tn5T/nuK6AKXk3IEaMx5LrICuAxHXPH+etZWrmCCHMkjNtUg+UmQvy5ySSOPccc1TFzLZCabIbiSVRIGJjzwCcHcBn16GmSr9huI9QbpAdk7DjMRPUj/ZOG9hu9aw/DmqWbyXh+0bsgIoZ1UD5l/2DXWBrVmbzGXaycjzA4PrxgVLV1cia8jXtxtYqu1Y2A56BfSs3Ub1rO9R4dygna79GP09P/wBXbIFTQ5pmWTSGyz2QAhyPvQnOxjz7FSSeSvYNxqX8K/ZTIDumUYLH+Y/x9z0yazfkYLfU6DQ7NbbS0jhiWMlnbaBgcsTj9aZ4n0WHxH4Y1TR7yMNDeW7wuPZlxmszwHrAvIZYHbLBiVz1wDj/AArrJ3T7pIBPAzXs0KzqRUj5rE4WNGUodD56+CuqXVz4bfSrkGS501jbSYTnfGxU5x67c/jXperQw6hoN9bSJjzImQgk9xXjFpcN4O+NutaczCK31LFyiH+8Rhv1X9a9xibDMjAEOuQeK4MbS9nWaXXX7z2MpruthYye60+7Q8mvdGt7+K3ghae5uTCqDy0yG9S3pnHfgE9ah+E3w2n+HMOv3V1MGuNYm85bdXOyEAYCn/aySSR6j0r1lLezsYf3UEUeQAxVclj7+v41n3srXMsKoOckDP51zTm2rHrN8zucP46AFku6NDLuzlc/KK83c1654t08R6XdSuMyMcD39q8hvFa3neNgQV7HqPavDzKm1NTPUwNROLiiCRqqytxUrMTVSY15yO8gkOapTVZdqrSc1oiWUJgTWfInzVqSjis2Y/NWqM2e4aJZKRDuHmMmXPBC4x0x1Oce1dEvkwSB3tYpPmJIaINznqMn61g6JfyWpWFol8sp1PGTtP6fWurXS7oNDKZU2sN4+TtXvw2PImtdTZNlZ6pbE287RqQN8cYCjqeoB/nSw+Fx9lmEF9dwMWUbkbb2Pp1osoXghdldPmABGD6mt20Mn2Zx8u7cvR8dj7VstTPZaHKvo2vaaxksb9JVC5IdCrEfXB5pIPFW2ZbO8WK0vBnDXAJLHpkHGOufSuu/f7s4Q/L0yRWJ4n0RNatFjkh/eplo2GBgj8fpQk1sNS7iXcxGpachuQ8jRuEZZFUqPl5xnkcirF9bIlo0nEjANjy22pyp46En8uM15FB4lnfxxpOlyuzzabbyNcZHQuyhc/QIT+Ir0++vvO0ycx5bGfmzwOMf196dxST7nK6HLatMV+zwhmc5G7HO4D+hr0OzS2PzLbxg7eoY/wCFeO+GLuVdTuF2MQZeMDOM5Pr/AEr1XT5XDAeSwbYMdPU+9EXoTKI3V1XT5Ytai3E2zEXCCQENA+Nx6DO3Af14IHWtTVp9luZIyHYg/THemRkvJKrRsVMa5HBzkD/aNUtK+W1vtJ2bZLQgRL1JiYfIfoOU/wCAE1MjC3Uo+C5hZX7ktnLlw3sc5A/UV6Zd2huoJNrENjKt7145a3LaZqW1WzOxwH6hDkDaPXPA/IDrkep6PqklzDGmxinlbjIx/L6/XvXdl9Rxbijx85oxlFTls9D5l+PUstpqngrxmnyvHfNpN8w4wxPyE/UA/lXu+lOL3SbG6UcFRkjvn/8AVXjPxiWDUvCXjTQ5f+Wri8tmHVJlIYEfiP1Nd78Gdbm8ReANNu/OlbdGpKkk4bHI/Ou7OsO4SjO2j2/M8bhDMY16MqV7yi9fVO1/nudPe+YEkXkKDnjk1lgttDLj5OTnkCuguTiR1kjy7jPIx29KxJoXeJjKwEeDwenTsK+fZ9spaFa7SCRS/wA8rsML5aED8/8A69eUeM4fL1QME2bkAIxjBFetwQxi22xALt9BxiuJ8ZaMZoZpI1ZnP7xT157iuXF03UpNI68NNQqJs80c4FVJTxVhzVWU14CPaKrmoXNTPVaRq1RDK07VmyH5quzNVCT71aIhnvGnx+U5LGOR/LD7EwxxjPUnB98V0lrqWoRrGUtFuk5VQk2Mfht4/WsrQ7LzWLGQv5SZLqdqg4C5BPXqeMV1lrNY2zRrbwK8zDnY75PvgcV9BE8ab17li11qR4WWfRbyMbQchiwzkew9a2rW481WC2kqrxne23j/ACarBy1vta33MwC7U3Mcdeu7HpUtsPKVT9liAPTe7Z/IE+3etUyNLbf195YW7hSXy9+1nHG1TICc9BtyfzApmpXUkUbSQw+Z5aFjltoP44759KhkEs52xtFFtOMeSW5x6kmqc8EkTsf3MzIpAL5GT2+XjincmyPCPBFhe3ut6rrF1YmG71C8eaSIfvFjOduzcOu3bj8DxXr+r3CWOilppkg6jDhjz6YHI/GvNbeD7HcvNdXECzSMzyKofAYnJA4x1JxRrOsSX4isba4df4W2oGGOfRv5iouW9dDa8H2BnuWulnjELyY3NuTdjOPvY/vfpXptpGM83ERHGfnU8AexrjNC0aG2s7dXkMsgQbmkVgTk56KDxjHeuostMtpYx8oXdz8vmHqf92qirESd+puRQ/vTtkiPyhCAw7Y9/euD+IOp3XhLUtN8QJIDp7brHUUU5/dPgrJjvsYdP7rOO9dTBZQpLIxUH1Hz5Bz1+79f84qj4l8P2mr6PdQP5gVgOgYdvcD+lEjLTuQPp8M1mtxlJGKhgAdy4OcEnv16d85P3iK6Dw3rUk8M0bEmTG2Td1b0b+leW/D/AFqTQ55PDWoSvIkJP2GWVdoZf+eZ9SOenUfSuyaKXT7+G6wRGzcJ+hBP+f6UUqnJJTXQjEUFWpypy6o8W+M+qXHha5upLxTJbzE8jrg1sfsqeIobrw5qFlbzK8MVw5TOMgFgcY/4FXW/GDwfb+O7KOBZYfMZd2zeN1edfBHwvN8OfG+qeHLy3eJriBblPMA+cEgZH5V9Zms5YjBKppZa+Z+c8NU6GAzGphop8zb9Pv7pn0ywQszNjzAM+v4enaub1efY7RnlZSOp7k1vXPy+S6bRkkfyNcT4tmKW7P5skWHwZVYKUB75PAr49n6dTSNa0K9BlRjHygkfnzUGqWongKtMw2/3nwPyFebwTw3MhkhvdV1KNGwZRK3k57jcTtP4V09hGjLGW08qzjq7DJ/PH8qkvltrc858Taf9gvpGSSOSKRiRsP3fY1zrtmvVtb8MWl5bMzR+XMvCyCQHHtjArym+gezuJIZPvIcfX3rxMXh/Zz5lsz2MNWU42e6K8jVRmap5XqnI1YI1ZBK1UpH5qxK1UZW5rREM+idJaS58yKNgEPyvIx7g5/PpXXaZGkWY4YxtJAyW6/jgZrldFj81BbqBkHv0zgGuq0BIWndXklLKxO0KMcZ75r3obHkVJJOx0ggk2p5kwC4yFQY6nv8AlVgFI1XnGBjhT659amZAmwiPK4XrIc9PpTru+SNc+S3yrnAkx0H0rUyu30K8MzEDG8g5P3cY/OsbxZeC002/eSYw4RgGU/MOuMYrRbUXhjEwjAjHy5zubP0wOK4r4tLcWXgXVbppEJEBlXavUKQxB/AU9bCUknqeLSXkiBtmJWb5QVfkfn/StXTmt7V42kDtJgMQynLEnv7dPyryLTPFz3kwIVh84B7f1r0LRtRb7Uu8HKJGFxzgbVAqHGxoppnr1tqhhkZd5DJ3chRwMd8eldvpd3viTdIrgDoJFPYn19q8x0/UT5qochnxjaMDrn+tep6YM2vmLwy9DQnqTO1iaN4jDGMoWxzhhz70kcqPZSrndu6fNu/kavwlnjh6YZcj/vo4/SljQIiBhncR79cUzI8fvNHh1SWZVDpMnlujoGDK2eGB7Ee9dtoWonVNMkt9VAj1G2wkqIeX67ZBjopAP5MOSKw8osk1yuQrRgfdBPDgfTvUutmSxs31iLasthC0r4JzJCvLp9cDI9CAc1MfIqWx02n6vpdgZZNXt4fLiIRGZQQnJ4/+v357V5J8Q/Etvo/xh8Jw2MciWVzC4g8oEECQEsq4/hBhBA7F2r1LQ4bTxHcG1nh/0Z4d4T044+p7Z9MAV8nftEXS+F/jD4RsbRpnW0uImBkbOA5I2j2wT+de/hpRngpczd1p8j43G0q1LN4ckVySs79b67907fefZ32jfp9u032hVJ4aQHOfxrznx9qtvB5FvIdrzMzIhwRlcZyT/Ouy0aU3/hyzZsKCA7Y69D0r5D+MvxButS+I9zaxBobXSsW6IP4iOSfxJ/ICvBSbPsIaHtem6rHNCp+0FYwPkjiHf0A/Cta2lDSeZJJ5WeSd5Zz9T0/SvNvAVxt0+O4ly7FQ3PbvXots6NLG3l5eTGFJ+UVmdTSWpq3ElpJDyjFWGCxDV5R4wsTbXvmK25Dx9K9s03S11AsshROOQi8D/P0rgfiPoIsIBJvV16qcYP41hiYc9JmmHqKNRI8mkaqz81ZmA3VVkevHR6jZXkFUZR81W5ZKoSv81WiWf//Z</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEASABIAAD/2wBDAAUEBAQEAwUEBAQGBQUGCA0ICAcHCBALDAkNExAUExIQEhIUFx0ZFBYcFhISGiMaHB4fISEhFBkkJyQgJh0gISD/2wBDAQUGBggHCA8ICA8gFRIVICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICD/wAARCADIAIUDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD52SDgcVYWH2qwkdTrFWRqV1hqdIasLFUyx47UDKwiqQR1YCU4JSAriOuf1PWZYbkQWYXO7buYdT/hnH51f1rVltYmtLdv9JcYyD9zPGfr1/I1w094rJI8acbgB7jkDP8AP6mmiWzqTdaxCvnAwXCFRIVUEYX6kD26ZrR0/Ure/RVKtDMePLcEZI9PWq2meXfERpqkgkVVfZJJtIIHQZIH8R7dCee9ZdxYCzvGIldhk+WY2AYsB06kHHFcqrq/K9zslh3yqUdjrTHTGjqpoupw6haqnmq1wgw4BrVK103ucxQaLiomirQMdRslMRmNHUTRVpNHzULR5oEZphGelFXTHRQBcSOp1WlVKlC0DALT8UqinbaQDAKp6letZW2Y4zJM3CKBnNX22qpZm2j1rR0LQJrrFzcfvjK+5Om0J/Dj+dZVaipxuzejRdWXKjkLHwfe6q4uLxDC5+dgDnLep9MDAx65q9eeCrGOAxRqwYAKvoB3/M8175ofhVWtRvUfTFUdY8KJ5m7H3fSvLliKz95bHuQwdCK5Xqz5l1rQ7zTk8y3y6nhgDjA+ncVaurOFbBZkt4tkpDrIVOVz1VuSeuevp16Y9G8VaT5cLbFz+FcHpLwtcT6VePtWQFkDgFT6rz649RVxxEpr3uhz1MJCnL3epjaPMtnfxTsUjQthypGGDdz34Nd6OQCOQa4/VLGyhcOkW0SHDRrIQAB2GTmursiHsIZFbIZchT1UZ4FdtKqpaHm1qLhqTUxhUlIRXScxXZaiZRVphxURWgCsY6KsbfaimBZC04JTwtPC0gGhaeFpyrT9tAFeaJZIWjY4DcZr1LTfsejwWsH2eWebywoSNcn6ntXn9jB52oW8ZH3pF/nXpmqaTqU1jHJp2PN3AnJ2jGfXB/lXl42XvRie3lsfdnM3LbxBpnmpZ3MsunXDdIrlDHu+h6GtF4vN3rI/ygZrxvXdX8RDxkLK404yQROqK5ffv5wGGQCexru/GWrTaH4bglDkTyryAea4q0uSVkepRXPG7/I5XxXJZ+a8bTQof9pwMV5BrlrEXM1tIjEHhkIODXYatZ6TJ4dm8QXyG4kYqrFd7AO3ReBgH2JBPpjBPA7bSaQ+Sht5h2HGPqP8a2p0pK0mcletF+4iK41i3uWWO5DeakarG0h2qGHX145P4/lU/hKS8OozW7SK8IjJJ6ZJIIwK2dH8L6frGn6xJeREz21uZIsZ4IBOab4c0WOztYr1phcSuvySDpt6EdTnHI/CvQpwsrxPIq1Lu0zb2U0rU+KYa6ziICKjIqZhTNvNADAtFSYooAsgU8LQq1IFoAFFPC05Vp4WkBp+HbfzvENlGe8mfy5r6JtbGwh0M3N5MsSIOtfPXh9Zf7ftWhGWVt30Feh6zc6lqelCwjd4oW/1jp1A9vevCx8nGvH0PpMrhzUJa21NrS77Rda1G7WztRKIG8vziyrl+uBnrxzXDfEy0up9RtLP7Oz7CdwjO7j14ro9HsPCtpbRafAbFvsr+YWdfOYSDq2717ZzXnvjm3STWWvLbWLyMg42pcYQgegHOPYk15/sZykp3PWc1GLijds/Df8Aa3haG3hk3WO7O1CCFcdeOxrnNc8E6VpGnSTRxk3H94nmrXgbWo9HS/gmvjN9sk8wluzdPw7VV8WeIlcPCHzuyKtSqKaimYTjB03JoxLJm0LwZqmryRllu2FqoHoeP0zWfpFpNa6XHDOxZwzHk5ABY4A9sV2cenx6l4Bjt5FRkgInKOQN3Dfr3/CsAivo6cbWPla0r3RWK1GwqyVqJlroOYrMtMxU7CoyKQDKKWimMuqtSqtIoqVRSEKoqQLQq8VIq0AOt7iWznS4icqUIJAJG4Zzg47V6doOpRX1vHyGSYYYeh6GvMdorV0G+ksdQMag+U/zKAAApA5/OvKzCi5qM10PayuvGm5QfU9ct7y08ImXyIUtLaYZMkUahSe+8EYNeRfEDxXo+sS/2fZWNvOEB/0iONUbn3UCvUI/FWm/2U32jBfb0PIryXxbqWltO0kYhjAyTt61wQqydons1ElFy0MPw9Z6dp8L3VzvwpDYdyc45A/OsW8lGpas8vSPdwKyrnWjcMY42xEv61BDqcMB3SSYH5muuNNuXMzyZ148vKj0O31vS4byystUt3uLRI2mdUkMZ4wF5HX+LjvSOFZ2KjCk8Adq4jQr2y1LXriXUcCUBY4ISfuYIwfr/jXdLEsUYRRhRXrQi1ueCq0at2ujK7LxUDirbCq7irGViKjIqZqjNMCLFFOooAvqKmUVGoqUdKQEijimS3McKSNy3ljLbe31PQVB9oiuA6rceTCmWeUHnaOoUdz2pzWoKxS3VpkNzaadnGf+mkh/xreFO+rPAx2bKhJ06a17/ou/nqklq+l4vt9w0oggtfMuGG4Qq2So9WPRf1pseo3Wmy/2pfXC+VbsCyRrhD/sgnkk/wAqkhZriSS2S+8+QnzLhbaMLH6Km70z/Ws3XkkvJdP0e1Hm3MzrII16xx5ADMOxZyG+i0qqhGDbOPB4nF4nEQhzWu1svn2Wnby1u9j0PUdFN9F51mXi387QMj8q4jU/h7qVxG0il3I5w2QP517HparbW0QkB+RQCT3xWD4y8SLbwx2dgpa6uPlT2zxn8+lfIYadWpU9nTVz9dxiw9Knz13ZP+tDwe68G65GxQmNcc7VPQe56CqCRWmn6WlyrLeXshKoeqqfb6etej+L5Tp2hxaVDIXu7r/Wv1Lf3j/Qe1R6d4Yj0fQ7e08qM6ve5bcygmBT94+2B+tfWU8O4K0ndn5Dic4jioqolanKVoq+soxveUn0XXTbzOR0jwzPb2y3FwsrX94QIo422sFPUknpXQQzXmk3RsZLlL5B/ArF3j9h8uP1/Kuks7S1+z/bLgsdMscJCrcm4cfxH19h/wDXpqW80qvr2ozNa2yqRHEhxkH+f9a6PZo4lj6tOUqsn5esn8MEtbu1rrp1fajDeWt0P3EyOe6hgSKJKzbWC6v7u4uLO3eOEfcld8ncOxJBzn07VYhuvtBZCo3IdpKurAn8DWDg0fS0MwhOTpVLKStfVde/ZjmqFqlc1CxqD1BpbmioWbmikBsrTzJtUxRwGWeUiOJSOCx/wHNNUZNSw75rVb1pWha4zDapGuXYEjkenA5Pua2pRu7nh5xinRpKnHeWn9W19fK463s1jMlpZTIojw17fsAQmOdi54qtdfYLppry6urt7eWQIsaI2+fHRc+nsO/WpZ2l82PTYrGT7NE37qzH3p2H8ch7Lmse+1TWL7XYtC0a4W61hj5ZW34hsh357sP0repONOLlLZHzOGw1bEVlCm7yl5q/q9H2XaMbJRbkdFodump6t/ZqxJp9naATTRpjEX90yt3Ynon513mkeH/DulpHPo8azTNNiR3yZ5zg9z+fYYq/4X8G2ug+Fjo8cz+fOC1xdg/vHkPVs+o7Vo2Oh2ekXMmt6o1vBHaqyRFWPAbG5mJ7kgYHb3zXxmLxv1qWje9ku5+xZTlEcrp62u1eUut/nf73dvqzO8V6oul6J9nS0T7defuoEZssueN2B6Z4561594j8vTRpgt4xPqMedsj5YkY5J9eTxW/cJdax44bU7+MwW43C1WTjIUdh9CWzVG3jhvfE8+qXX/HtarmIH/lpt4G3155+pFfUYDC/V6PK/ie5+bZ9mkcwx8akbujSg3/icvdUfn1XqmZV7orprOlXV232zU3UZgPCAjkHjoAfzxV50i/tXUtQmcy20EYilJ/5aPjGxfRf61Zha6Y6hqjR51F/3UUXeBcZyfTjufT3pG09ZtH06KJv+JYm2a6uuili2D7k9ePcV3+Z87GnKThRqPZcra6X99qNvlCFtW7vXlVq/wBnS08Gm41CMSPcYFvC33Yx2wPpk5796g1OxkuPCcV5rF4yNvV1VVAAU8ABRgZxzW/rFt/a/iiz02Bd1jb4DMo+Xkbjz06YFYvjKX7brVvosbiONGAbPADH/Af1pu1n9xdH2k6tH7MpOVWT/khsortdWv1fW5nXDxajYwafpW+1syhMkhwG2A4wv1J6/WvLbhWvtXurNCsAsi3kvEuCCGxknqeldZp1xcS67eH5o4fLMMRIwvysMKPfAJ/OuY05M+JdVjP3sv8A+h1zTdzuoU/qkq0IPRJSXe7erb6voS2HiC4utRhuJFc2MhMMm45ZGAyG/X9K6GRsMfmBHqDkGvPI1b/hF7uID5lmGR/3zXaW/wAtmkf/ADzCj8CMj+v5VgfTYWfLJ0uiul8rf5k7NzRUBbmikemdJJtaJkZiEYHeV6he+PfFTrcXCyFbaPF8UCDaMrZR9kHq5/nTopIbdd7qzyPhdifebuEHucZJ7Ae9c14o8TDw7pH2Wwwmo3OVi2HdsPR5S3dskqMcDBrrprljdnxWPqSxeKdOnC9tFfZ97+S697drp5niPxZfaYH8NaLKhvZWIuZ4uWTP/LMN3PUk+pOK9Y+DPhfStO0E6jDcx3eoz/64g/NEf7p7/wCNeC6Rpv2GP7TcfNcyc5PVa3rPUrvT5xdWd3NbTdnhcofzFebjaUsTDkUrH2uUxp5fJ1OVOT3ezb/rbyPr5UEcYLcE9K4PxNfyav4otPD0Lf6LAwmuMfxEc4P0H6n2rhPCHibx1rV9HG+sSGzQEu0sSMSPY4zn3rrPD+uf2Dfa0tvHHe72817m6QMsTAHaRjliCT3A/KuPAZU6NT21SztsXnPEdKop4Kk3F8t5O17Xdlt+W70sjd1xbKLS7m1vbcmaeJNxDbTBEHV8Nwc7wOVGDgjJG4Z5qG72QXXia8X9448m0jP8I/z/ACNRXk02oeF5b+6naISTB2d/me4OfmP5kkD1BJPOaffxRrZaTfXv7qyiI/0QcsVxlfqSBz6Zr6JdZfM/PK0MO3HDxVoqTp2W9ormcV3lN7tbLR2b1ZcQy6b4XVXydR1Z8v8A3tp7fqB/wI1e8QxtaaRpPhm2IMj7S4Hc9P1Yk/hS6jcxpr+na1qoKW/k7obZBucMOQPryDn2xUqRzP45fUtVKW9vFGJIzIwC9MAZPcck+4pvsZ0qii4V59Oep/imvdjFd+RWWmgniuZrWPSNF09isisrLjg5Hyr+ua4D4kw29pfhbd3eaYsZHY5GTgnA7f8A166+S5XUPH090f8AVWQJUHj7vA/8eOa4rxcf7Se1vYf30PIeROQrMchT74IqZaxbN8BKVDF4bD3+y5Tfdzu0n92xR8ebo9FslQlSsgwRweFNc/qkbaf4ds9UtgEuZGR5JMZMhKknPrk11fxAVTp9uifMUkywHVRjAJ9KwdfT/igbTcOkcR/Ss5rVmOXy/wBkw1/tTafnc5eeOOx04ScuNRG/HZHxlR9MnFdXGoNidw2yfZ4nIzkgqcEfkwrltUXf4OsJe6MOfzFb+m3KyTyRkjMtusik9ByAf0wfwrA9+hNp8z7u/wAmv0/IYW5oqN8q5U9QcUVmfSHUoywxtNdSGI7Gkmk6GGIDc2PRiMfQFR3ry6G4k8ReI7jWLlNkKkLDF2jUcKo+g/Wuj8a6hJb+GvLhJAvpGt1/65JISfqSQufYVl6Tbrb6ZFGBhiNx+tdVR9D5zKKF3LES3ei+W/46fLzLTnceelbWh+H59TR7xoXkt4jghV4Jxk5PYD/PeqVlp7312kMeTkjcQPfoK9XubYWVjY+FdOwssoDTEfr/AFP0FKnDm1Z15jjnh5U6ULc0nd32UY6yk/T9R8SNo+lQ6Xp+19SvgOU6Rqehz6Dt+Jp95ZLG9p4Y087pCRJcyep9/wCf5U+7TzNUs9A0smMQbWllX72R3z7D9TRJdbfGaWumN5ZQt58g5Lnq2SfyHoa6n2+R8ZSqSv7e/vOMqrv90JS7K3wRV+9yO6dNS8RWuiW/NpZ8Mvb5euf5fifWtC7jOs+K4NOX57eyHmTehPXH8h+dU7NY9P8AFsdjpkAYtGfPd2LHJ5yT7cfXNVZNXj0m81TRbE+deXKsPtMh53/xE47cnHv9aPXv/SItJtToactK8b7rndpVJdnbVLr8mSPfLrHjfKnfDa/cHbg4B/E81PMv9s+LhBIc2tkP3h7cckfnx+FZHheE6LLqKzbrvUjGsiIiEgnsMdeMg/Q+1c3rXi9/DekTWsXOo3Ev73J5HoD+ZP41LlaPvfM35Je2lLCL4YRp0v8At5Xc/kuvVmv428YHT9Su4dMjhNxOiwO7AkljwAOe2R+XtWloNvHb+CbuTGVHmNk+yj/CvMtJ0+41K5uNYvmMiWqq2W/jmc/0G4/lXpt0zWXw0dZG2MYypXocs/Q/nShJybkzTH4SjQwlHCUtZupThJ9W0v0v8jn/AArEs6anJN+9D7Fbf827rnPrXL2DHUfElzBcEy2scbqkTcqq5AAA+ldZ4Z223hm7ujx87vn2Cj/69cv4ThZ7u+uDzhAufqc/0rN7JG1Sf73HVu3LFeT20MO5U3epS+H1by7ODdswMnI5GT9TUdjc51a3iUHbbIbaZu2SpH5ZFTab+/8AFmoTdv3h/wDHgKyUPza43+0T+rVzs9ZKzcOyX3y0b9TpJJPMYS/89FDn6kZNFVll8yCFunyLjHuAf5k0VDPoqUuaCkZvjB2ktfD0Z+5sdv8AgRKk/wBKsxzYGFGSBgD0pvxAaOOa2t0Tb9muJMYHAVlQgfoap6RG95q1nbLz5sir6962n8R5uWythIzeid38m2z1vSLC30Ox0nVLssTIC7QquWZzymPwx+XvW/Yytba3qd7eANftuW3gU7mYBc5HtgAZ+tZN+wuvF2lacvMVqnmkdh6f+gj86k0O8jufEmsaxKfktwUU+gHf8l/Wu1aWSPhsRVniKE69bVyg2/SVT3ILyf2urRqaTN/ZegXeu3DBru5BZc9TzgfmTn6YqPw3Gtnpt5r15ks2duepA/xb+VUPCkqXn9panffOhUoQ3IA6sPp0puhXTazDeW90x+wxRiOOJeAuTkH3Ix1PrST+EvGR0xcaj05oObX8vSnH02voamkXiafo+o+Jb0gzSbipPoOT+Z/lXK+Brd9U1HUPEOoMRBGCNx/76b+QpunvdeK528Oxt5Gl28ZDSryz4PB9OTzj9aTUvEWm6J4YufDenMouVVt0pOFdgwyAPfpmoutG9l+Z0VqVSpLEUVpOpKF7fYpdPwW2+peh8RwWZ1PUWZRcztsUZ+4OpH5bfyrxVtU+1+J31C4jFwZrjcI3GQeuB+op41O4mtp4AzSXDBmZR2zwf0pfCFgb7xnpETD5RMJnHsDn+lc7k52R78MNSoSrYhrpb/t2K0Xpoe0eCbOWHWLuK4CkpEjvEBhUkwO3TI5FO0lP7Q8TalHcDzLYs8piblS28YOOlXfB7hta1+Vuf3+M/wDAmqr4QbzNQ1CXvsH6kn+ldSXwr1PmsRUkljanWMKa+bV9DDv55pPHU+nQylLafEMka8Ars5+nes3xFc/8I/qtrDpUaRRmPLx44kycc988dauQMsvxHmbrtllP5Aisnxa3neMLaL/rmv5t/wDXrF7N+Z6VOnH61RoSXuqkm13drXfdlG/hg8LzwzLvna4LLKW644PH41hywNY298LllWS8RnjUH0yeffmtnx0264sox0wx/PFUtfXGtaYvow/mKwkdWFlKdOnObu5ptv8Awu6JtNZfKjWQf8sI+D68g/yoqGxUyXV6p5KSYGew6/1NFJWNpYlwfLck+IMGZrxzyY50bI9Nij+tUvBObdp9YaQSmzVfLjPZywxn/gIatjWoI7/wTa3StmW4tXndicljGVGPbCj9KxdJjax8HpI3DXlyWHuqKAP1dq2fxXN8LJSwscPfry/do/k+Vnpq362Ot/2xfMI/7Ri2wJ1KgBSM+meKoafPJpfhHVo7r93dyDeY2+9sYBQcfXNU9ZSS817Q7VPuq36Ar/QUy6kW4+Iqx/eSJdpHUHCZ/ma0bPn6UIyppv8Al5n6U5e6vmvx1NvT777J8ObqQHa8ocn8SF/lS+G7v7P4RvroH5iZHz9F4rmZ7h7nxnc6fLITZ3BAlj3YB2oD+HIFQ32umz1Ofw/YBVs7hRGAB/qyw5Iqea3y0NJ4Z1oSp9ajVV9uXTT1X9djZ8Pa3/Zek37xf612VAB14BP9a8+0qK81XVrm5eQhsFie/JrSuLweH72OCIfaElXc/mHnOccelQXcg8OxRPZS+ZLISJC44YD27Vk3dJPoeoo3qVatNe9VtZ+itr2MyxhC6/dIzcLv69+a0PCrm28R6ldQfJLbwNJGfRtwGfyJqlqPlRaeLyAlbmdxI7A8jdk7R7Vf8NTo8l4nBkeyd3bHJYFT/IUo7nVUfNByto7J/r8j1G9mk00aYlk5gOoKjXJXrIRjv75OfWrfiidvD7ebpQW3kvs+YQOm3+6Og+8azNaYm38N3HYxj/2Q1o+PY9yWB/3/AP2Wut7P5HzWFiqlfCQqaqftOZfzcr0v3tZWv2M3VLeHSLaDxFBHuuTGqupPyuzDlj71hmxfU7ODxNcS7Z4ZDJIqj5WRG6D3wK6nxYo/4Q2DH/TL+VY9kf8Ai302P+ec39aiS1sTQrT+qRxF/fc+S/8Ad109DldUaXxGjXtpDsFodvlk5Zgec/8A1qqa1PDdatZS2riWOGRVdl5AJbjmtLwuf9Avh/tD+RrC0k/8SrUz3ChgfQgEg1zyPcilTnOMdqVkv+3t7lywONT1Jf8AbU/pRWRDfPYWUFwiCR7gHeWJ52sef1oqAqYKrUlzRWm33afodjr+h6t4U0K9s7q2drG3SVba4B3I/m4UrkenJrM0W2hu/De26y32WPfGd33flDY/EmvW/CHhbXvEVg0Pii2fSdLmQ2q/aMPJIW4+Rc8dfvEce9Znj7wVovhzRY9P0KO8QSMEnuHfe0h3DGQOB+ArzcLj+eSpVPi8j67MckcKbqYV2i3d9Gle7t97Zyd3qlvpo07XdSuEaVomUQRcYznbj2wTk/SufOuTWutS6vBp806XCny/lKgE445HOBxXWan4R0u10fRo4IxNPPjfITuYkAAjP1b9K1/FdhDHqOl2KQhIumFHqQP6V7jjL7j4TD1aEp04WuqnOu1oxb0S9dPzPM7218SW9x/bklsIzcN8qHqMj/CoL3SNat4odeuAAz7WCAeo4/SvU/GzIJrK3+6u1jjGOpAqLxo1rFp9nAANgY/oMD+dJ0kr67F4XHSqrCvlSdXmXpGPQ8nvtN1i5sk1i4j2xqBweuN3/wBeoZtN1bUdOOoOuIY9x59uteo+IpLODwbaRqBhhGDjv8uf6Vl3V1bQfD3EcYBKD9X/APr1Dgk9zeljpypwnGO9TlXkjz5dP1K+0qS4XCwQHv7D/A1o+C7WWbVmzhI5ENtuPq+Fz+G7Na9pcp/whl190bhJwPpiqHh+9jtdPaTGHFwHBH+ztb+lSkk0dVStUlTqwitpWR6jYWsesX50m4Zli0diqFesi9FB+m3rU8cj+MoooZmFu9mT5rKM7wemB26Gs7Q70QeO9TjzlLiJZFbHXp/iad4KuFj1rUrVjgjt9GI/rXUtbI+Zm5U6dWtT+KnGEoeTn8f3tu9/LsLqd8dYs5vDkEW27hk2Rlj8rqhxknscCspp4dJ0648PXco+0GFmRh91ywPyj3/nU9q3l/ESVemZZR+YJrH8aDyvFNtL/so35MahvS53RoQdaGDjpCUfaf8Ab3+Wm3n6FTQI5LGKaC9QwSXPzRI/BYDrx+Irn9K/5BmqD/Y/o1dF45QobKZcqVZsEHp0rJ1xhbx6f9lAijlUowUYBDAVzyXQ7qE3Wj7XrV/Dl/zOfuj/AMSnT/8Atp/6FRVi6tGlf7HDgJanALHqGAP880Vme3SrU4x1e9397ufU13a+Kb/xxbSrMsWj2rrKCH37mU5wB6E46+lamu2Md/YPb3Cbh976miivi4abH6o0pRtLU8quYofDb3/kyGaGWN2jSTkwMVO4D2PFTaBew6xoE+o3X7+6tUaOJmOSgC5H45PWiivtMuqyqUlzO+5+LcTYanhqlWdHRtw+V9Gl2T6ojsJLTxEhudYkDNafu1ydobPOW96o2scfiora6i2xrP5mZBgvnHB9OlFFd61tc8TE/uHipU9PZ25P7t97dr3d/l2RWu7H+1Y20m7gNpbwTfLdFTtKrkAHtn3zWVf2Nmbebw/uEcKFRFcls5GQ3I79+lFFRLY3wT9rV9m9ElzJLpK61/4G3kQx+HYXsrjTLUTzxlcRypA5bJ65GAMfjVVfCOl2sb21xrMkDY+aMwMXVu+R0/DNFFS0rXsehQjOWIdDnaVr30vfTumvwNLR4/7Iv1vLO4vtReNPJRHiGHTP6YHTrV7Sb+103X7rVNdtZdMhuQ+xnHcsDjA5/GiimnZXIxWFhzypXfvrlb62306b+RG0M7eLrfV7NxLp9w5dJsgqBtOdxH3T9ayfGkwuL6CeJhJGq+WZIzuUNnOMjvzRRTl8Jz4KXPjKbf2U4r0Ta1JPG21tFtnP3hIv6qa5nWJPM0XS5M8goP0/+tRRWFT4jbLV/s9L/E/yM64uPKvbhv70mPyUUUUVifQUqUZQTaP/2Q==</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCADIAOwDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD53trFFwdoq8sIxwKVV9qsRx+tbnhDI46lWOpFWnBaCrDelPEhFL5eaUQk0D5R8c3rU6tmoo7c8etWorfGOaB2Q+P5hUlPWLb3pwSgaRHtpNuKm2A05Yam5qolTy80oizV3yR6UeSKk0RSFqGzmlNuBx2q9s2imMvqKRZR8kUn2fLdK0VjB7UeSPSgZQ+zUjQgVoNF7VEYaZSM9ocfSo/LrSNvTGh9qksoeXTDHWh5J9OKaYj0xRYCgY+KiaGtHyfao2hoAzpIaiaEVoSRZ7VC8PHvVAZ7R1XaEE9K0Wh9qrmP0FADEarCtmqMZOKsx5p3PMLS1IneoFzxU8YNFxkirUsaE0kaZq1HH0poBI4yKmVcU5Y6cENFxocoz2/Sn4xSxpUvlFqk1SIQgPapUjPpU8dvgdKmEJxwKDQrCM07y6tw2M9xIIoIZLiY9I4lLMfwrI1ybU9NysVgN4OG8wk4/Af41jUrQp/G7HVRw9Wu7U43LRjzTo7ct2zXCSeONbsZv9J0+B0z0UMv9a6LRPHVjfqFuYpLCXv5gyn/AH0P64pQqwqfC7jqYerR+OLRui3x2oMWO1XI1WRQykMrchl5BpzQj0rYwM9o/bik8n2q8YRSeUPSlcuJQaHmo2hrQaHnpUbQ+1FxlEx0wxgVcaEelRvFxxRcCo0Y64qBhVplPIqFozmi4Fdkz2qGSMVcaPbUMi1QFJ1B7VB5PtV1o6j20AYkaH0xVlITn/61PjjFWI46djzBkcZ71Yjj9qVV6VYiQUhhDDVyNAMVGnFSq3tQBIEFOCgUId1Soo70GqQgU+lWI/pSL0qRBSuaJFhMMOlX9G0ttX1BLVG2L1kkx9xf8aoRtxwuTXrvw78IwwQxyzKpkbDyMOmcCvNx2JlQhaHxM+gyfLljq37z4I7/AOR0UF1aeFfC7afoWnpbzzr++vGG6Z+P72OK8b13SZmZiytnPevp+bR7CbTQq7EbGBXk3jLRWj8zZ1AORjHSvjsbGrUanUlex+rZdHD4eLp0YWPnnX9LKqxK8Z5rU+G/ibwzo8NxbazpdvqCSYB85eQOhweop3iLKpMHHOOc14/rV01vcGRGIIOPlNdWXVnRldHkZ3ho4mm09D23XIdN0+6W58L3X2yxdWlkscfPEo5P8+vfvUlrdJfWsc8J3RyDI4x+B968m8O6vPNG5hdklAxlOuDwR9Oa9F8F209pZyRT8q7eYhxxnuP5frX2kKiqq6R+XVMNLDyabujY2n0pdhq0VB7UbB6VZkUyuab5Y9KtMo60xlFAFSSLOT0qu644q8wqJ4w3bFAFBo6jaHFXzDjmoWTtQUUXQelQSRAc1oNDmq8kdAWRSZR6VUar0iYqq0Yz6UwsjNjq0q9KrwjBq2tUedyj0UZxU8a1HGvep14oDlJo0FTLCp6VArEYq1GehpFKI6OPFSrH+FOXBxUirRc0SGqnFTxx7qdHFx0qxHHUlElnbj7VCT93ev8AMV7X4V1JFWKJjsBGPUjFeMMzwoXjTfInzKvqRyBUGi/HifUdYvL/AMOaYsVlayJbxSaijTyySGNGcNEhQR7S+0gu3zA+leJj8NVrVIyhst9T7XIsZSw9KcJX5m9NLn1RZ+PvCkcbWtvqkFzeL8rxch17HgjNc94r1iymCIjoUkZlLdc/KcfhnFfIfxE8SfEG48YXUV75Gl3O5VjeCz2pPuIAKHJLDHfP5VmeK/ib4y8EWsml6nY3Go6gtot1bSWbrHH5bMVLSBgWDgqfkGcg5zxXh4jD4mT5Icv3n1eFxmGinUqc3/gJ6b46bSbRp3uLyOJRlcnp0rw3xRf6DFIzWkdxfxvgmdQVQZHP5VY0Pwhf/EZrC8vdbZbu8hS5eCPascAZd3LOCHOMZUKPTPc5PxG0zVLbU9SsbHXbybRIAq2m/wApWfgBi42AA5z0B/rWuHwbo61Jq/r/AMA5MZjnWXuU3y9NNfz0PSvhD4XtpLm3uSDPZTOCDtyccZBHt/Wvc/F3h210/wAOxyRiNGinUKqAD7ynrj2/zzXyv8CfEXjLUtak8M2d863cLo63UqxrFjBYqFEZ5KtFz2Ibrnj03xZqV78OvG0EXinxGkp1GEvLbKzusTAqqE/IB2c5AGORg9a+wo8sKV7nwWIcqk7WZ0vlmgrVjZhiD24oZAe1UefYpstJt9qstHk1G0fpQVZFRoxk1Gy1bK+1RvH3oCyKjfWoXWrbR9ajZBjpQBUK1WmU1dkX0qvIuQaAKEi+1VmWr7LVVo+aAMSOrka1ViWrkXWmeeTRip4489aZH2q1H2oGPjtcipo4COtOj6VYjG7FIoSOHpxVhI/anRpVhEGKChix/nVhUxTkTNWFioLIV1DVtIvtOuNJlWORbyITq0W/fCTtZfbqDn2rqNL8K6fpvizW7W8jS0tdZlS+t5mAWPz9ojmhJPAJ2I4z13Nj7prGt5GtZ45kPzowYenFeh2viSKNWkmgS5guWLPBKoKkHnBHcV8hnHPh6say1jLRn6Tw3UhiaDw9rShdp+TNux+HOiJbpqWrTJJFAP3bTPhQB6e1QeJvhjpyR3XiSGFAt7CtjEZMARxpvfIUjO5i7HP90L71Q+H/AMJdF1LxDeeJrjTrezQMY7GK3hWMR4+9IFA6knGfQe9ReOPhlr+n6VLBYeK72+uNUvy0TahHvSJmDYUbcYHAFeLiKNWvSfs9W11duvzPqadWGHqrndknsl5fI+TvDc1t4T8UXOj6hcC0tUnaK1upvlRkz8q56ZH3cegFa/ir+yfthja6sZUYZMiXCsff5VyT+AJPpXDar8Mdc8MeItRtNev5pv3587y8mMuCeQG6Z9q2jDZWOnv9nVAnUbRXTUpvmi+a762PNp1G4Si4pLpfdHcfs6w2un/Ea1uZ7cwvcTMItwHC/dUH/aChfxrB/am02/8AFHxq8RaNbFb3z7a3ECbOYDtXAz6Zbdn3NXvhx4wgvvF3ha0jQMbdi8zY/iB+X9K9Y8V+GbNfiHqWuqga6uVQLJsKnZ5aKByOfunBB7kdRX1tOHtKCgn1Piq9RUKzqeRk6Ppn9laVZ2QYyC3hSLc3U7VAz+lXfLFTbaNtekj5zd3KzR7aZ5dW/LprLimBSeH2qFo8dauMKjZaAKTR1XkXrWjIvFVZFFAyi65qvIuKusvWoJBigChItVG4atCTis6RvmNAzHjFXIaqR1ct+woPPsWolNWFWmR9qsRLQMmhjJxVyOLb9ahh4q3HQOxIimp446ZHVhGoKQ5I6sKKiFPU0ix9dF4dnhnU2sxw2Mr+dYCLup0scq7Zbdts8Z3L7+orysyw7xWHcY7rVH0OSY2OBxcZz+F6P5nrU2u6zpWlWw0PTn1e4XhbdZEjUe7FiOB7c1T1Kz+J3iLSrSS4uNN0USZOyWWQmNiCBjy4yuQcc7u/WqPg/wAQTT2u0BhJj+E8g1lfEjXviPd2/wBm0JlFqhy0i2qtJ+bAjFfMUJRS5ZrU/TKqes4P8r/keCfGzw34q8Jsd+rWOrTySMZFUuvoc5bJ9fy968zuFmsfDNsZnXz5pOVRsgcc44rrvHNv4gurh5dcvJGYHAj2hcn8AK4W+hur7y4iuAiEIpPQdz/n0r0KSUlaKXyPnsZLlm27/M6D4SyLp3iCLUJF3Jbxs2OvPYV9T60vnafoMxkWSWbT0eRk6A73+X8MY/CvF/gj8MZPFEkcMrtbaekim7uFHzHGD5a+5yD7cV9WfEDQNENv4b0qy22V6Ld4raEH5fKQA/N/wJsZ/wBontX02GoTjScnsfD4/Ewc1BbnkwjxS7asXFu9lcSQzRtHNGSrIw5BqJjn6VscREy1Gy5qZhmmsO1AFZo/WoZPSrUnCmqzGi4yCTpVd1zVlqjbBplFORcVVk65q/IAQapzd6AM64YYP0rLlf8AeGtG7O0GseaTEhqQKseDVqPAbis6OSrUcnenc4eU0oX7VajkrOjfkVcjJouVYvRv0q5G3SqEKn0q3GCuKVxl6JqnVhxUESGpljLUXGkWoytSqgPfFV41K9qsRqTSNCZRipl5qNYz/kVasbK4vrmO3toZLidzhY41LMfoBTA6jwn4evpvD+ta3YNufT5IBLb44ZH3gt7EFV/OuY8VfGzVdK0+W0AhshnBa4lRA3bjJr6S+CPhCDwHoviK/wDF95Z2Gl3NqqXKXUqrFGpJ++5+UHkjr+NeKeOvhXpPjvVJZfDV1beJfDQlKpqtq32iKHjLK5UHlR1IBzxjJOK8rF5fzSVaMG+9j7LKMyfsnQqTtbZvY+U/GfiG7ubzzL29td0pGxftCszZP8Kg5P0Ard8J/CXU9ZmiuruRbO0lGXkZf3jL/dVT0+px9K+0PA37Lvgfwvp8V3pFhb3l3Kqu+pyRDzHz/dBGUH+z19ckVv33wxtoYyzRbvRQF6Zr6DDZXRppNrXsfNY7Na9aTUHp3PIPDMNroOmIkCC3trcE7iOnOSxPcnk5rzeXxtqXiTxtLq8ayGBV8mzjfIIjH8XT+I8/lXtnjLw2i6e9jDEqGYYbAx8ueR+P+NYXh7wHHY4ZIVMh4LMBx7CunEK1oRPJoUue85lTT7WTXYXGsyrFKsZMd2RymBwr88r+o9e1ZureGdS0aMSXNqywnpMnzJ/30OAfY816BqOhop0jT1Ch7q6zJtHPlxr5jfgSEU/79d3a6WyL5Y+ZGGCp6H1yK4uQ6FGUdj5u20le+678LtF1mNmFsdPuD0mtRgE+69MfTFeY+JfhfrHh+N7hI/t1mvJmgByo9WXqPwyPes3BlKSehxUimq8ikVcdfUVA69eKzNSmymomUjpVplqJgFycUAVJO9UrjParrgsx54qpc/KpoAybzoaxZjmQ1rXjdeaxpG+c80rlFDmrsPKiqyLk9Kv28dM4iaMHjir8C5xUMMY4q7DHigCzAM9quxxjiq8Cirka0DJUqxGPaoo4zmrsUfSgtaDkjytTqoXtVnSdNn1a/gsrWMyTzOFVR/npX0D4T+Cmj6HHFPqS/wBqXowSsn+qU+gXv+NXGLkFzxvwb4F1TxldrHaQmK1z+8u5BiNB/U+wr6H8I+BdM8E2Oy1i8y5cYkunALv/AID2Fb8cKwwBIo1jjUYVEAAH0Apy5ZsHmuiMVEWr3PP/AIzLp+p+GLbStQPm2Larp9xfW/XzIvO2qjD+6XK59ga9q8D+C9G8OaT9l0nR9O0qyP7x4bS2SJScckhQOfevMtE+G8vxMt/GdxcSmK2uryKxtWx/BblWZh/203D/AICa9L8RvqWj+Cbq7t7iBkaEsdsbfKoH97d7HnH4VtibRhGMXr1PUy6TqRlTeibVvy/Q8o+I3xvtPAvijT4bO0W60+e4+yCyt0HnXEhPCwrwN2epPGOuM5HfeJZ7Sw0yXULxvItYVDyM4zj2AHU+w79K+dvgL4fj8X+KtV+J/iT5oNNDxaXbS8rbLjlv97B5PqT7V9A6DoKzeE5tZ1dTJdanN9rjhlPEYIxGoHbCAE+59q9CNNUaac3scmYVadWvyUI2SVv+CzgbO1/4SK2F/LZvZi6y6W8w+dI8/JuHYkYJHbOO1U9asZtBSF7LSZtWnnkCKkRRFU/3pHYgKvHXk+gJ4rvpLXzFOwAMfu+gqtrGsab4T0G+1bV5FtbKziMs0j/dwB29fTHqa82cuZuREVyxsjj9F8H6tda9DrGtT26zQwPDBZWSsY4Q5QsWkblz+7Xnaox2ruLfTRFHnua534Y3ur61oP8AamsRC0N9K1xbWRGGtrdv9WjerY5PoSR2rsypb7vQVncoz7izUqMdvaltlWNdwIxVtoywx0rN1LUI9OjY8syqSAoouS43OX8Y+DfC2sRu9/awWM5H/HzCRE/1IHB/EGvC/FHgZ9JEtxp97Dq2nr1lhPzxj/bXt9Rx9Kv+NNY1HV9QuJJpmUEkBMkADNYfhuGWLUoC0xKmYB8dCpPIPsawlK/QVuXqc6yVDIvFbGuaf/ZOrXlpjCwysq/7ueP0xWTKR9KgspyfLms27fFaE7daybxutIaMy8YcmseT75rSuiTkVmSMA5qCh8aCrEa7TTY146VLtqzhLUDDj2q9HIMdeazIzt9qtRN05oKsaUL89avQv2rLhPTmr0LdOaCkrGpCatRybaz4ZOOtWQw9aBntfwA0FLi4utXlQMVb7PESOnG5j/6CPxNe3yMGbPNeY/A3/R/BtkSuPNmmYe/IH9K9IVvMkx+NdkfhQJFr+EAVFd3SWNncXMh2pCjOx9gCal27AhPrnmsfxl82gyW3RryWK0H/AG0cJ/WtIx5pJCk+VNnqHgu2Hh/wFpquoWVLQTyjGP3jDe/5sxrK+KUx0v4GeISnDx6XIq/Urj+Zrd8QMVhtrOMbRIwLAf3Rjj88flXGftGXTWPwL8RBTtaSKOH/AL6kUVD9+rFeZ6mFp+zpKT6v8jwT4Ixyat4P0LwyPuX1281ztHHko2Tn64C/8Cr6R8YXvmXENjH/AKuFQDjpk14h+y/YpHeXtwwG2xgSHI7HG5v1b9K9Xkma6uZJXJ3SMWOa9XMHyzVNdPzZ41D95KVV9WLaw9z+deJeOLz/AIW98WrXwjbYfw54bdL3V2H3Z7nrDAexC/eI9cDtXe/GH4hL8NfBM95BELrWLp1s9NtOpnuZOEXHoOWPsDWX8H/h+3w/8IxW905udYvHa81C7YczTudzsT9Tj8K8jU7DuodsaBEVQBgAbR0q0v3WJI6elVowcjtinTTBYyKQDZpgqqoPLVxfi3WTHFOsIyx43fjW5JeeZLN84RY1+8exJx/jXM6tPA0ZWBGuHxgtjC/n/wDWp2A8j8VWbLMCWyw5ds9TVLw1JC98Y2U9eCenFdV4qsfMUTSsxGMbM8Dj0A/nXmdnqTWPiBVYkKzYIrmloweqNr4lWn2XxI75+WeGOQf98hf5qa4yX616J8UoxcWuh368mSAxN+GD/wCzGvN5j70hLYrXDbQayLw9a0rljzWRdN96pZZmXTcGstzls9Kv3jday5GIbrUlXNNalXk0wU9as4kSbRU0faoFzViLtUFlmImrsDE1Vj+arcK4pgXIWPFTeYarxHkVbjUNg9qos+lfhOQvgvQGHTLZ/F2Fei2n764I98V5h8Lbpf8AhCdIBP3GZf8Ax816npUe2MydCSTmu1bIhFuT7wGeKydSj/tDxd4O08glZdREz/SON5AT+Kj860/M8yTAGar+HWN18XdGgYbhbadcXOfQlo0H/oRral8V+1yanw2PRr5lutYJckCMKox9M/1rzz9qi7jh+DtymcrJdW4PuA4b/wBlrv7WQT3lxL13StjPoDXi37aWqf2f8KrKMH/Xakg/ARuT/KssLaWJh6nvVouNGy6L9DP/AGb7drf4c3l+/EmpXjlW7lF+XP5g16VGNp4P51z/AMOdF/4R/wCH/h7T2Xa8NnGZOP42G5j/AN9EmvP/ANqL4k6l4F8AnS/DeZPF+vE2OlxoRvVmGGkGe6g8Z4yy+9b4qp7StKTPEpQ5IJI4eb4h6F4+/aCk1DVdRhg8NeFg9npzTNiOe9LbZZB67SNg9wcV7X/wn/hqUjGu2Cj/AGp1X+dfJnwp/Zt8c6PpcM+qaKRcYxFHJdRFYFwfmOHOWOTz7n1NdnqHwB8W6pkO1nAo5PmXBAA/4CprPlSNT6Wtde06+C/ZdQtbnI48mdW/kadeXSpETuyADnH0r461L9mvXrq7eJvEWn2G3rLbrJMw599nP41q+Bn1D4TajdaI/iO+8RNdK4kN2dkVuqIzZjTLEMWIBJbGO1ZuyA9v8N+JB4gtNanVtyJfm2XPT5FBP/odaLRll46LxXm3wEuF1DwFJOx3tNqt1L14yGCf+yV6Dd3DHMKEjPJNJaq4GD4ihNxYy7Odvf8ACvnjxBcG31jcDt2vnr719L3Vqo0+VD8w6cn1/wD1180+OLX7Pqjrjbk5H51y1tho9M1Rv7b+F1tN1ltnD/gCVP6H9K8ymfrXofw7kGqeDLuxzk4dQD/tZH8zXmszdazvpcUexWuG61j3T5zWhcv94Vi3jdalsso3TcnNZkjDceauXMmQazJJMMai47HRqtS7aYtSeZ2rZnGkIqkGrKDNQphscVOnWpKLMKVehXjFVIGHFX4WFUgJ44ulW40wtV1YdalWTkUwPbvhROT4PGeRDcOPp0P9a9xt3WKCJFYZYZr57+Fdw6eEr8g/8vJxn/dFe76LcCazt5jzuiXH/fIrsj8KGaMYy6jvVrwDbq3jLX9Sdeba2htkb/vqRx+iVWhByWzxUfw01yO7/wCEwjH347xVYn/ajRR/6C1bQvaTXYTXNOEe7O40yTyI1GMZ5J9a8Q/a9tn16L4e6EmXk1HXFTH+yF5/DBr37T7aOeMAuv3cYzXk3xN07+1vjZ4MhZd9vo+nXd+R/wBNGZIk/Hlj+FY4WXLVU+1/yPosQ4uMjory6ttJ0+S5mkWG2t4yzOxwFRRkk/QCvjzwh4guvjn+0QfE0qsNG0kNHYxyA4VcEL+JyWP1A7V6D+2B8S/7B8LQ+FLB8alrA/fbT80dsD83/fZ+X6bqpfs1eFU8P6LHK0f76XDuxHc81nfmlY8M9+WRljICjgA9T/hWTqGqSRJIsceCB/nvWizMisVx+YrDvmLbtxGD1wea2A888SatqMdxcSJCucEbt3/668b1zU5tNuri/nl/0lo3RAMKE3Dk8AZPNe2eLbtI2cGNnGemK8M8fvBdYSJCSUJIIxg4Armm9BnY/swao114P1O3cndY6lOn13HzM/8Aj9es2ebq+ZyflXoO2a+cv2YNSmtb7xvZsSf9IhkVD2Zl25/Jf0r6T0qMxR88E9a0jrFCHXkO63kz0wa+cfidamLWMgY5I4HvX05cRxnTJH+bCg9OK+evitCft6OEwm7P51lWXujRX+C988WrXNnuP76Nio9GABH8q4y4yjMCMEEg1s+BZ/7H8ZWe75R5lZviqMWevalCOkdxIo+gY4rlj8ILcxbqSsi8kz1q9cSDnNZN1J1qTS2pRuDwT7VnnrVq4fKn6VQZuetBR1Yang5qFTmpkX0rY4idBjmpN1RrmnqKQE0MhVuauRy+9UVU+lTxAjFBVjQjmK471NHLVSMHip14pjPYvhyxj8I7F6zSSOT+Q/pXu3gudJ/DOnu3LiPYR7gkf0rwr4S7bzw9KM5NuzA+2ea9X8A3DzW81tG/zwOflP8AdJz/ADrvj8KJO1mn8ixmkzgKpP6VU+D2l/Y/CtzqMvztrWoSXQyOkYUIo/NWP/AqpeKrmWPw9cJCCZ5MoijqSTgV3FvpsWg2OlaUjfJZ26Q5H8RC4J/E1re1OXmaYeHPiYeRpW+myGYvbXLL6oec1wXxF8R6f4FuvEnizWZQltY2kMGSBuOxS+F9SzShceoFegafINyqQT81fDv7bfjy68Z+NrXwJpTl7eO5BuAp/wBZN7+yqfzJ9K4oy5T3cZJqHK+p5f4d1DV/jL44vvF+sj5by4xBCeVjjX7ka+yj8zk96+v/AAXbvZ2EUatGgUADC8dBXivhjwzB4Xk0TSbdFYQRBmPPJwMk17do9yI0G9cKB6j/AD2rSC6niM6S5+VH3S547GuR1qJZFO+dgc9c1rXupDaMEbW4OSB2NcNq90LlijSHB3DhsnoapiOe8aKtpAQl0cnk8f8A168V8RySRqCZd/q2a9L8XXQFq+A2dvGR+leX64zNGiFTkr19ck1yzehSHfs76oLP4z6zo8hydRs4rqP3aNipH5P+lfXsa7FCqOScV8H/AA21BtF/aQ8Jzu2I5i9sc8Z3o4A/7621982C+WokkKgKc+uTXRS+BCe5NrSfZ9JMeDnYOK8N+J1jnThLs5GD1r23VpDLZtJJuJcnABxivMfiZZiPw88hXPHf68UTV0xHj1xiC+0u8BwGUHIpvxKXyvE9w44WeOOYfioz+oNPdftPhyzl/ihlZCB+lU/iFcC4u9NkB+Y2KBvqGYfyxXnp2Gtzkrh+vPFZlzJ1qzcSHOO1ZlzJyalmpUuG5yaos4zU9wxbvVFmwaQzs48+lWI80UVscj2JqkjNFFBBbhwRVhFFFFAXLEa/hUoQ0UUFJnpnwzuJNE8N6rerG8z3DrFHGozkqMk/rXVfCHX9WXxpJDeWM0NvdQyL5jDChh8w/kR+NFFelT+ED1u9ug2ueHrc8h72Et6Y3j+ma7u8uBNqkrEE7TRRVv8Ahs68v1xa+f5FuHVILPT7ieQ4+zxvK30Az/SvhD4eaFL4y+J2oeJb9d5V2ZSwzl25Y0UVwr40enmC5ZpI7e3mM3je42jIjjKrxx0r0SzY7MZGdo6UUVqmeOxLqOeZTs5Uetcvqunm3BMjqrtvCr/wFutFFNsR514ms4Y7ctLdBgRkLngda8q1e9STLxfNtwMdulFFcs9i0eUa1r0uj/ETRdQT/WWdzDKoHqGziv0s0x1vLWCRTmNlDgn3H/16KK6aWxLLGoYliHOEXFcZ8RrUXXhmdVHzdBntiiirlsxHhujr52k39rnDKwmX8Dg1ieN12xWEncoy/lt/xNFFeYV1OKuJOKzbl+DRRUmhnSSCqTMNx4zRRQB//9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCADIAMgDASIAAhEBAxEB/8QAHgAAAQMFAQEAAAAAAAAAAAAAAwABAgQGBwgJBQr/xABBEAABAgQEBAQFAQUFCAMAAAABAgMABAURBhIhMQdBUWEIEyJxCRQygZGhI0JSscEVFmJy8RckM1OCkuHwQ3Oi/8QAGgEAAgMBAQAAAAAAAAAAAAAAAAIBAwQFBv/EACoRAAICAQQBAwIHAQAAAAAAAAABAgMRBBIhMUEFMlEiYRMUM3GBkbGh/9oADAMBAAIRAxEAPwDpUE2PeCJTbvCSm2+8GSmKjoNkQmCBO2mvSHSOQ/MTCbDpDCNjBHXXtEtB3h9T2EIDWwFzEiZFYn2hAAQQNE7/AIETCUp2EHQmQQQojQW94kGTzIHtBbE8rDvEgi43MGURkD5I5kw/kp7wXIIWQQZIyB8lJ6iF5PRR+8GyCEUQZDJTltQ6GIkW3FoqSg33/MMQbaiDKJyU2XpDHuLwdTQVtoYGpCk7i46xOBkwZSFRBQtvt1gtukLffeIGTKdSf9YgpPaKhSLHT8QMi94XBYmUyk232gZFvaKkp07QJSbe0QOmBIhRIi0KIHKtKdYIBf8AqYQHL9YIBlH8hDmdsQASLW+0OBfUwgOZgiG82p0HSJK2yKEFfYQYJCRYCHAvttBEptBn4EIBF94llOw0iVrd41V8YPj9wp4XgaJKSyMTY2cbzppiHsjMpcXSX1i5BO4QPURqcosYlLIuTaSZmGJKXU9MPNsMp+px1YSke5OkY9q3iK4a0aaMtNY5oKJjNk8pE8hZzdPSSAexMcKeOHi/4mcdKyKniHE88lhCiWJKSeMtJsdQ00ne38SiT3jCrmIqgpQPzkwctwCXDcDpvDrauxcs+mvD2N6NihDhpc/Lz/l2zhlYUUX62isqNfkaTLOzE7MsSrDQzOOvOBCEDqSdB94+cThX4ksf8HK9K1XDldel3pZedLThKmldQpPMEaEH+cXHxl8YnErjtPZ8Q159mTzXbp0k4WZVoHcZB9R/xKJMPiHaIyzuhOeKfhjI1FEicYU6Zm3NEsynmTCr3tr5aVW162i+sM4zpWL5UzNKn5eeZSRn8hYKkdlJ3SfcCPm1pWLqlRliYp8+topN1rlnVNLPclJBPLc8hG73gj8dc/R8cSFExvVVPSbqwzKT1QcUtDBJsGluqJWhKtgSSkG2YEHQ+hrjsE3nk7FjYG8Ij7+0QlXkTLKFpJIUAobHQ+0FKOkVNDZBFAPvESCN4Me8MR9+8JjA2SmW0DqnQwMjkd4qijpA1oCx0MT2MmU+2h2hlJ1vziZBBsd4jsbcoB0wJAsT/wCiBqT+IqFJ1uIGoRDRYmUqk8oUFWm4hQpZkqkpsIcb3MLc25RNKc5tyG8OjO2OhGY3O3IGDAZvaEBygiRygyVtiAtpD3AHQdYW+20a8+OPj+3wF4GVqelHlCvT6PkZANfUhawbuX5FKQojvbpDxjl4ENZfHf8AEknsD1CoYF4VzbTNTl1eRO4hQEulDmoU0wDdOYHQrN7G4HWOUuJMRVTGOIp2pVadmKrU5p1TsxNPuFx15ZOpUo6kk84hPTUxW6i64o3sFOG675R1J5k31PO8VdMYYZknluIK8oOWwPrUdtBroP5xL56FPEqMq824EvqHmpSB5aTfIOlht7RRZCg8j7ReeF+H+JMevrlaTILmFJNsjKcqAe520jMWHPBNiuflW3aiPlHVjN5abKyjlfuekUSthD3M1Vaa679OLZrSAb6C8GbZVdJvlSTuRtG3VJ8C88EOrnJl1TadBlTYmPXR4bKLRJF+Xmmg7mOU5wPSbaGMstbTHybo+lap9rBqRLFckgLSWnkbL1Gx5HqD3jzpgfLukoJF9ATobdDGUOLnC9GE1oekv+BqFA8uv9Ixc2lyZIbvmUk2AUfq7X6xshONkVKPRy7K5VScJdo69fCl8YkzxDpC+EeLZxUxXqPKl6jTj6iXJqVT9bCid1tXBB5oP+COjG8fNNwH4nT/AAU4w4XxhT5gy8xSZ5t9V9Atq9nW1dlIKknsTH0pU+cZqcjLzcuoOS77aXW1DmlQBSfwRDsrDFIPeIEEaiC2ht/eI6JBe34iKk84IpNtRETr/UQNDAFJziAkbg6GKpSeYgTiMwuNxEZyOmA7RBSbHsYIddYYi4gLEynUIUTV35bwoXBYmG2EHQnInvzgbacyteUHSLmGZnZJIsIl2/MLaJITzgSK2SCbRx4+MNjurTvGWi4WebdbpEjTkvy6TdKFrcUQpfc+kD7e8diRHLL40fDlj+0OHOMm3iH5kv0l6XzKssIAdQu2wtdQ6nMOkWReMis5wYAwq/imsuSrKrtIBK9NFhKVG33KQPvGU+FnBmdxviinUvJ5P9oulgKG7SQseYT0NyPxGV/BLwYTiOSnK3MN3Sy6MoVoFEHbuLXEbpcM+CEhQcSOVSWk0JGZbrarb+Ycyxa3psofpHN1GpcMwguTt6LRKxKyx8HtcPfD9hzANAlabSZFEu22kJU5lAWs8yT3i9nsIsNSigltAzrNyANbaD+UXhJUtzKjPf08yL8okKQ682EmxQok3tbXpGCNTay/J3Fds4T4MT4jkJdhgthACgDpGBcb0xDzr2QWz7J7DX/32jZvHGFXEsKdKSCQfUdI17xPLKk3HA4tITfQ72jlamuyL4R2Kba3Ds1h4s4acnWXXPK85lKSogC/pAP55/p0jTaooUxOvhACbKO3KOjeKZZp+nTXllLocFiE6666fiNOMZ8NH5CqzDyGy2ypagHFD0q7f6x2fTLt0HXLtHk/WKcWKyPTMSzMx8wAXNHRobJ+od+8d7PhpcaZjjL4V8PrqU8mdreH1rok2rZdmgPJKupLSm9edr73jgzVZMM2W2CWs2W53v8A+iOw/wAGaiqlOCGLagoBPzNZDakpdvZSGk/UjdKrKBvzCh0juHnDoTe8IiGhwbwq5AYj8xBQsbiCGGteJJBH9DA1Cyu0FtY2POIKF/eFfAyKZacquxiGxtyg605kEc4AdREliBrFjf7GFE1DMIUQWZDtjKi/3gyBYd4gBsIKP/MHkpY9tbQTbb7RBAglv0iStiAjTT4qfCh3H/hvNfkpYzE/hOcTUrJ1Py6hkesOdgUn2SY3Li3eIdMbreAsR052Wbm25unTDCmHhdDgU2pJSexvE528slJyaSOb3hIWcNeG/DUzISap+qVILmClof8AEdU4sankABGVpmqcd5aZW9SaRh1FPSEhpMw+fOsNypAFhfsTaPN8JvD+bwTwhk6FUAoT9FnJuTSSeSXl5SPdKgb94NjPidxMm2a6nBGHWEN0+XKpaZnGS+5UXUuJC2GUAhKDkKyFuaEgDmSOWpNzcYLLZ6ZUtQW7P0+EZXwlj3EUy1Kt4glmJScSbupY1QrTlHvVzG3yrTRQotIH79usazcDsYcWqtPTDHEjD7FND7rqmFhKWnmkC3l50JUUkquQctrW21jMvEGosy+FA06Al8ptcRmnfOGVLtHVp08LFFpPksHHmC8UcYHky8liifpcqn/lqIbPTQbxiXGvh2qXD5orm8eVaquK9SkvtgIT2A1NvvGR8PYZdx1W6S9OT65mk0cKLtCdCxLTS1Xs46UKSpQANkp1AOpBNo15xj4UMQYIq9RnqLjesVEOWRKSqXFoQwkWCc40SuwABJFzqTckwRslOn8R2JZ+xTbp3HUKCryl98FPRZKcla15Sp0T0s45bNbLb3tt94uPiNghip8P6lUJSWQt5iWUp9IT+7bX2N7axcPDDhfO0+l1WqV2Y82adQENtq2SQNVDuYybwuwyzXqfUJJ4FUtNyjjS02303/EZqLd13Rl1lOync+jkziWgOM06amE2UhC0lRItY3yke+0dz/hx8PV8P/CnhREwywzO1NK6i75TPlrIWfR5l9SsJAFzytytGkPFXgFSeFTUtiOoSTDtFkJRydTJvm5qk+48USzJH/LQE51dr+423+Hbi+t1zCVVYrE6udK3C+EqSlKGlXAIQlIASmxAsNBYR3PzK3qtLs49fp87dLPVRfEMf9eDcSG5xIi0RMXnKH3ENDp6QiIckGsRE6wQi4gfI/mIJQNWhinWnKsjlFS51gDw2PTSIRYgQ5iFDnRV4UBYiqSPVBOR/EDRuYJyEC7KWERtDiGTt9olEiiO0QcbS82tChdCgUkdQYmo6ww2iGKYIn8Ot4axTVZJkZWlKQ8nTcFNif0ikboLEpmWnM2Vkk+WrLf8RePFOV+UxPSp0XAmGVsKsNLpIIv9lH8Rbr1QYZSpbhBSkE3jm2Vrcz1mlslbBS8s8F2gy7EwFoaAdUb5jqfuYxbxwLkjTQoetLR1B5xeNf4t0rC7kpNVVubcmJteSVlJWWW8rITvlQCe5PKMIeITjxIzlRFIksPVaqTTibql6fKKUW08yoqsB7ExnnVGcMLs7tSshPM+j3PD1Uf7zMTrso+lc5KOFDqEmykHcXHQ8jGYJ1piZCm6iyMoTzFxeNO+FtSxTROO9Fn6JR5yRoS2ymfdmW8iHG1J0SRzUFWPbWNu8b1Rv5cupV5YWnNYHS/OKoVKEcNllqlKzn+zE+P6syyFsSqUJQrQJHKMh8GUS7eH2HUkLUslCr25DaMF4lmW5mdfR5hDmlu/aMw8OiWKDIKaOUZ/UojcbbQmmX1tnE9Wk3BQ+DX3x8idnsQcO2lzTqmENu2pyNQUXSVzGUDlcoKjoLjvG2vw/cKrpXCRdUcbt83MOIZcIIzoCySoA8tvxFl8RpOlVLi5QqfLtygxRVMKzUow5OWU2qUU8pDqUJO6wXNhrY6bEHb3BOHJXCGE6TRZKXTKy0lLNspaQLBNhr+t46NdblZufgxW61Q9PWmgsOWM/sm3/uD3NxDQ43ho6J5oaJGIw/IRKAaBnRcEMQc3gGBqGloC5q3FQefvAFfQR2hV2OgB2hQx1TCiWWIrG/qMT6RBGhMT5D3gRUwg/pEhvEU/SPaJCGEGV9UIbQ5GsMNoV9kFh8ZpFb2F2ZxsHPJzCV3HJKgUn9SIwyZhyfYy6hCtDGzVTpzNXp0zJTCczD7ZbWBvYjl3jW0yZw/WZ+hVE5ZllRCTycSdUrHYjX/SMGpTi93g9F6Zfti4eVyiUqwhASMmdabEkchAsU1WQbpL8xNuSzcuALOqUkAna1+ftGNeJfB6cxS2hTOLK/LNJcLi5CWqBZYXpaxskkfmMWVLgbRX5ES1SaxPV1gkqZXVnijMdBZSEjS2941VbJwy5JfZnqdNp43rfZYslbjTi9SsOKD6alIr+XSSUtzKCcupFtd9Iuyk45l+J+C6bVaS785LPM+ZnbSQknbn3BjXeY8NUkZ1kJocnKMtOFSmvlswO2q3FkqVttoI2RwZUpTDFF/sspQlCGMqCRa/K1uXYRytS44cU8j2VWVWZUk0vgwxNOKexT8uskC7ij1ASND+Y2C4f1BuUwVLeYQXFq9ItqRGr9WxK2MVVpQdQhEuS0txX8alXyjvpeMr4AxKa7/Z0i0v9mmw0PLvGGiTgzh6/Fi/k3f4SyDU7Tvm5iUl3Vy6kiWfU0CtslPqyqIuL+m9oyPzMc+/E18QiU8ONKwrh7AypCu4lRUErqknONKUyZMJOdIcSoFDhVlCVa2sbgxuxwp4mUTjFw/omMMPTAmKVVZdLzd/qbVsttY5LQoFJHUR6aMXGKTPITeWy7hvDHeHG8NDCDHeJcojzhzsIlAMYG5/SCH+kDXvAMMrnAVfSYKrcwFf0E9oVdjopz9MKEfphRJYirT9X2gg2MCB2MFH/iDyVMIg7Q4iCDyiYOsSKOraGEPvDbRDFHEWDxU4ZpxvKszsi4mUr8lcyr6vocG5ac/wnryJv1i/ofcd4VxUlhjwnKuSlF8mqlMrrU/OzVOnW1yNUkleVNSbws40r25g8jsRYx6brUoWRlKSU/vE69rR7Xid4frqJo2I6PKqarTTplnpxk2u0UkpSu2/qFgeV7cxGtFYxHi6gE+ZMtjkPmWSLH/MnQ/gRibdTwz1Wm1kZwW7hl54/m5amodmXXG22xdRUo2HsI1N4icdyxXHJKiLSt5oEvPH6WRsLnr2Gpj1OIcjirHi1tz9bAYXf9lIk5j2HSPP4e+DPGuP3ES2HqO4xT83rnJlRaZB/iW6fqPZNzFbrjdL5LdT6jLZtjwvkw5NYgLSEPTLxP7RS0Nq+pbij6nV9zpYcgBGQn8b1fhlw0mcTT7b9KlXh5Mo456HppwjRLYPXc9BcmNy8IeBnhpwAoMzjLiHWm61MUqWVOTc9No8uRkm0i5LbepJvoCbqUSANTaOXXiu8Rk14ieIzs+xLrpeE6cVS9EpJsPIYvq4sDTzV2BV00SNEx1a9PTUlOfMvHwjyluruseyCxHy/JiSv4kn8UVyaqtRfVMTkwrMpaje3QDsI3G+Hj45T4b8SO4ZxdNOucPKw95jygCs0yYIA+YSkalBAAWka2AUNQQdJwnWHKsg032EBQfUVR6zI1+ly1Rps2zPSM02l5mZl1hbbiFAFKkkbggg/eKyPm84A+JXHnhxxczW8HVt6USVf71Tn1KckpxPNLzN7H/MLKG4Ijs/4XviD8NvEXSpSTmajLYSxmQEPUKpTCUhxfWXdVYOpPIaLHNPOIwBtHvEjDJ36QiYESht7wMm6oITYe0C6xJKIqNhAXNG4Ks8oA8fpEKh0DVtaFCP1CFAWoM0cyPbSDJNxFM2rKu3IwdJsYH8lTC31BggN/5iBDp+Ikg30iUIwl4RHOGvGP8AjRx7wL4fsLKr2OcQS1GlDmDDKjnmJpYF8jLQ9TitthYX1IiSGZAvGJuOHiq4YeHeSU7jbFUpT54oztUlg+fPPdMrCbqsf4lWT3jlp4k/iu8ROJ81OUrh35nD3DCiUImWiF1WYT/Ep3VLN/4W9R/GY0oXMTdeqz01OTD0/PzKyt6YmXFOOuqO6lLUSVHuTEJEHbzwreNh3xicVsYUinYXFGwHRqUlxKp9XmTk2869lQV5TkbTkQ56BmN7HNyjI2NMAuS1U/s9MiagxNqPyqwjMV8yhfRSep0I16xzm8GHHGV8MXhs4k40kmm5rEmIcQSmGqE26jM2Xm5cuuPOC4u22Hys7XshNxmvG5XgG8T9X4rf3jwTjusmr48pTzs386tDbImZYry5UtISAnJdF7XBz35GIspVqx8Gim50vJnDAvAOg4fCZuoyErNzqtQz5aS03+nrPc6dBzjKCGUMtpQhIQlIypSkWA7AcoLbSNYfiE+Is+H3gDUF02a+XxViIqpNJKFWW0VJ/bPj/wCtsmx/iUiCuuFa2wRFls7Humznx8T3xdP8XuIcxw8wxUXBgjD75anSy4PLqc8hRClm31NtH0pGxUFK/htoqd4r6mbrFydtSdT9zFBzh3yUDWAgZ9TnZI/WCKNh7RFtN03O51iAFaJJWptQIOo1EI6Q2kAGyPAv4gHGLgX8tKU3FD1XojNgKRXQZyWCR+6nMQ42P8ix7R0u8OnxS+GnFtMnS8YW4fYidIbCp13PTX17eiY0yXP7roT7mOH9om28tk+k77g6g+8AH1GNTLU0w28y4h1pxIcQ42oKSpJFwQRoQRzhzpHATww+PfiR4aJ6UkpKeViDBqV/tsNVJwqZSm+vy6zdTCumX033SY7VcAPEdgnxJ4JaxFg6qImMoSJ2muqCZuQdI/4byNxzsoelVtDEPoZGTFaq9oAs3WTyGkFWcqSecAOgiCxDdTChE5R7QoCwceoQdCs6b84p9tesTQrIq/LnEiNFUk3HeJX5/mBA21G0EB+8QuBGYm8VXiEkvDRwUreNZhhE7PtZZSmSDiikTU45cNIJH7osVKtrlQqOA3FririvjLjKcxTjOszFbrU0o3deV6GkXNm2kbNtjklNh7nWOhHxk+ISpnFPDnAjTtmZSUma9MtA/UtavIZJ9gl7/ujmVUrofycwNYfHBWBl0eYo32t/pFawsyUoo7PvXSnqlPM/faIyyEok1uK0694pVOKN1KuogbfbaDoDOuDmnsZYDwVhKVJDEq7Ozy20mwMw+/kUpR5WZl2fwesZx4aeIOh8OuL2DMU4YZ+dmqFMIk8XTq2fS/IkhpyYbUVaWSr1C26AYxK5QJvhlwsemJV1qZfq9G+Yp1U85LTbjeZCJlLIXZS1pU5b0j6bqFxAfBlwqPGbjFhbCSEvolJuYLtSdABHy7X7RY9vSN+ZEb3txGC78so55b6O/wCl5LzSFtKDiFgFKkm4UDsQY4X/ABGeP3+2/wARNUZkJjz8OYYzUanBJuhxSFf7w6P87gIv/ChMdUfGbxoZ8OHhmr9VkHflKouXTRaIgK9QmHE5EKHP0IC1/wDRHAl13MoqJKu53Pe8YXwX8+SmnwSArpFBY37iK95XmDJa/vHnhC3Scx0BtYQoEF2XdI111PKDJTZN94fKE6C0SPQQADy3PaGKYOEjppCDe5P4gABluYgqDKOWAq1N+UAAibGMmeH3jpiLw/8AEmmYuw5NKZnJVYS6zmIbmmSRnYdH7yFDTsbEaiMb+X5l7bxJLCkqSbG28AH0yYDxvTuJWCqFimkLz0yrybU6xrchK03ynuk3Se4Me7uewjQr4SPGdWLOENYwBPTBXUcNPCblUrNyZN9StB2S4lX/AHiN9FHKIh9l8eURWbm35hRBR+xO8KFLkgiTmESGhsYEDbUfcQS+YfyMSI0EbXlOU7coMDlF+UUw6GCNqJIQdibAwdlbRxF+Jlij+9XjRxbLNuBxukSMhSkkG+UhtLih29Tqo1AqS/Nn3SNs1h7CM0eJbEhxb4quLNUzlxDmIptCFH+FpxTaR9ggCMIOHM6TzvFr9qKQjjxUhDeyU8u8Gk0srmmBMBRl1OJDgQbKKL6gHqReKYfUYrKWEqqUolYunzUkjr2hVywNruM81/b3CWjl9hLweYZW3lAyy6EJypbbvfIALDTcXvcx7/wxagmheKvC7bi2w7PSs3LBpoghKVMKIuRzukab8zFJTaWnFPB6WlQQpyXbOUdO3beMd+HPG/8AsB49UPGk62VSdHemHX0A28xIlnvQO6jlH3jq6qG1xklxgyUyymvOTO3xcOOZxrxmpfD2nzGelYRY8ybShXpXPvpBVfqUNZE9itcaGE3ST0j1MV4sqWN8UVbEVYmDNVarTTs9OPK/fdcUVK+1zYdgI8gnbp+sck1jJtnGtopC4UPOJ5E5h/WKhxYbBKtLbxRpJdXmV9h2gAMkc76wRAtvEE73gue6rwATG9/1gKyRz/WCKcygADfnAFm5gAGo3vEdokd+kQWYAIBZQsKG8e/JhEzJJcCQSnRUW8YrqVMqaUpAVoobQAdAPhAuPu+InFSm1kMf3ZcDiB9JHzDOX8G8ddVKuewjkP8ACFrTNN4+Yikl5Q5U6C4y0f8AE26h2w/6Uq/EddVKtES4NFfKIqMKILVaFFZoJpOsESq2o+4inQvrBEq1iUxWioFlAfzibZ/atg/xD+cASq2w9xFs8VcbscOeGGLMVTLiW2aLSpqfKldW2lKSPurKPvDFbPnnxnOmocRscT5VnL9WnnSq++Z5w3//AFFjHVZ949KRfcekp191RW86oqWo7lSiCT+bx5hPr06xY+kZR0nXtHpUHKqsy99SD6Rbn/43jzEb25x6+FWXZnEcu2whbj5IDaG9VKUToB3gj7kQ+jdTg1JOzOHZalMNKmp99XlpYbGYpJ2AH8XW+g99sZ+LqiUTALFFw00+3P4qfcXP1Rxk3bk0C6GmAf3lE5lKPLKAIyfwzxhL8L6EqlU95tyvvt5ahVUm6ZRFrqYYPI2+tW+lh2074iYwdx1jOqVpaleXMPEMhX7rSdED8C/uTHT1NznUkuF/pkqhtsZb+a6T0hioAXJiN/tFO+4XFZE/cxyjYRccMw5/gB0HWCIRfSGbRawA5QQ+kac4AH2uIcWtvb7wFJv7QVSglHeACOcFzsBfSIE5jEGzcLPcCJXsNOUADW1gbh1gh0AtAlG8AEDcxKXXkdvtEDEb6wAbWeAfGIwV4jcBz63A2zMVZmQcJNvS+lbO/usR3TUbb6W3j5wOHGIn8NzUpVWFFLlMnJWfQRyLbyVb/aPo0lKg3VJNidZN2JltL6COaVpCh+hERLpGirygqlc4UQJvrCis1JEgq/vBUrv2hQoCGESqNM/ixcS1YK8LDtEl3S3N4qqbFNIQbEsIu+79vQhJ/wA0KFDIps4icZJRwilLF93Iolb221hQosZkE2f2n3i5uH9URSKvOzLaVfPFjy5d0f8Awkn1L98twOhVflChQ0PciH0XxWsWKoeB5xhlWSaqB+VS4FeoNkesD3FwTubxibNprtChRbfJuST8CQWAb7vlpsB6zoITLYQm51J1hQozlgUm2/8AKAOLzHnChQAO0bHaGmHAEwoUAAWDdBHUwRRhQoAHV6UwEmFCgAgYQFzChQAXJhtQNPqLR2clzp7LTH0CeGTEhxd4duG1WUrOuYoEmFn/ABIbDav1QYUKIl0X0+5mSibwoUKKjcj/2Q==</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAgMDAwMDBAcFBAQEBAkGBwUHCgkLCwoJCgoMDREODAwQDAoKDhQPEBESExMTCw4UFhQSFhESExL/2wBDAQMDAwQEBAgFBQgSDAoMEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhL/wAARCADIAM4DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD5EValCjFNUc/Wpa9A88jIxTCKlcd6ZQAyl206igApQtPVcU9VzQBHgCnc1KEpfLLMFVSzMcKoGST6AUDSuQZqJmC/eIH1rqYfBs8cIl1RvILciFfvY/2j2+lVZvD0ceSqL8vfHJ/HrXJVxtKno3qd9HLq1RXSsjA+0xR4DSoPxoE0cx/duj4/utmr9zocfJ2cisG/0fym3ICjD7rL1FZ08fCTsOrl1SmrmhTay7e+ubdgtwDcR92/jX/GtKORZ1DxMGVu9d/S5599bD1pTzT1XHNIwwfrQDIqRqc1JQIZTKkpjdaAGt0qJqmqNh2oAiNMbipGpuKANRetTfw1ElTUAR7aj6VKeppjetADacgptSL0FADwoqRVqNfu1IpoAl2gc9q6fw5ZCzIupFBn/hP936e/vWJpVn9pmBYcKRiuxtLfhUQH8q8PNMbKP7qHzPpMly+M/wB7UXoPkaS6cmQljVeaxbaTiup03w7JOqttJz+Vac/haSOMlkPTivG9jUfvM+mU6a0PMbq35I29qwtRs8g5BxXoupaL5IJK4rktTt9mQRjFXTumcuIprlPPrxPJkJWqLah9hk82IZUn97H/AHh6j3rW1yMbia5S5kPzZNe/g8Q7crPkcdhlzc0dztIZFmiSSIhkdQVI7inMvFcz4R1Qs01jMeU/eRZ9CeR+f866bzK9M87oMNMp9NNAhrUxqkPSm0AR0xqeaa3SgCJhTKlao2oA1168Cn0iiloAYetI3IpSOaMUARgc1KtN285p69KAFpyLuPvTansU8y6iT1apm+WLZcI80ku51Oh2YhhDcbj7da7Dw7Y/aLhNwJXPPsKxdItvMYDgDbXeeE9MM0gMY5Jr46EnUrc0j9ChBU6KjE9M8L6HbpbqZVH3cdvwqbX9NhW3JVBkjpj9eat6bZ3EdqoKYH0qnqkU3lsWBIyMg9q9aU0o2OCFOTlc881qxRoWOzGBznvmvJvE0YikcL+Fey63ayCNjg9x615N4stGQs2MVwyZ1zXunluucBg1cjdDJJrs9eX7/B6VxV9JlvlrpoyZ4WKSuU7W5On6vbzg4AbDf7p6/pXoPPrmvM7wkkV6NpMwutNtZM/M8S5+uOa9yhLmgeBVXLMnBpGp7DbTDWxkJTTTqRqAGN602nmo6AI2qNqkPem0AbIFDU6mtQBGaTNLR+dAAKfSAU4CgBCDVy303UPsjXthbtKkTgFuwycc1Wr0bwrCkXg+7aHYJLi3cyL/AM9QrN15wCMKR9PevPzLF/VqKla93Y9bJ8B9cryhe1k3p5GZoettHF/piLFJHHvn+cYjGTwc9DwePyzXd+GfHJ06H7Va26PCo+9JMqB/oDz+leY67o323w5d3COVLbFmA7pu6/hn9aw/CvhGW+8UXFjrWqXdrALSQW0iHKibH7veGyNmcZwCa48PRwsoqb/r0O6riMwhUlTvorWta79b/ofQUn7VFvZSGC401diDBKT5/wDZagt/2gLDWCV2mBXb5d/Q+gz/AI4r59PguaG4vZNRvo7G4Ev+i2mRKHXnI3L34GCevPStyHQU8N6DLe+JJo4N0yRqdu75SeuO5xnjvVV8NTqS5Iu3mugUsdiqMPay18nbX7tn2Pdr34gad/ZAMpDOTwByTXl+u+ONMu5XVzDGcnO6Vcj8M14/rniTVY3umaKW3tiymEk4LwlgDlc8HGOK6bwh4ZvvFkl3/Z8QSOztnl86XdHFKwXITeMZZjwMsq+9Z0MspuN51OZeWgVs9xEpOMaXI10ev+RW8STw3in7G8RB6/vFH9a861HdZzFJAyE8gN3rR1qz1VI7ud1FuY5dscDO29xz1yT04rK0e8kurO+GoIXjjiHlrIucSE4GPTv+VdtPB01pGR5GIzGvbnlG/lazMu6nVSPMcZP513XhKUvocJ5xuYL9NxrgLljKpF0R+7XA2ALj6461seF9YvG1SytN0hh24IkbOVCnGPyrohOMEl3M3TlNt9j0DdRSbaQmuk5h1NoooASmU9ulMoAjplPpMUAbNNan4qN6AG8HtTqQYpaACn0i05aAEr1H4TGDWtJ1LS7yUxS2qvNatgfMXADLk9B8gx7t715eRW94I1STSdcWSMkLLG8cg9QRn+YB/CuHMqKrYWcX2PUybFPD46nNd7fedX4Zs7fUoZ9OuCfKu0MR9s8Z/DrVq/8ABeqaDd2ra9pN5Iu0AXtjHJKsoH8XyZIJ9D61y2i3rWlwJCSNr5zXtOn/ABtvrPQZLfTsNdGMpCdvO7GBgetfPUsQ6cnTauj6qeFjWgqkXZo5bR9e+H2m6iEuGeTWjwIprSaScEeikbs1cs/hvcfEW9k1G+srkWtnITp9nIm0s3eZ17Hsq9uSeTxt+HvBMem6PNf6hNHL4jupPtNxdTjdufGRHnqFGSPzNczefFrxvDNcS3GmWNlYWKHElhdKzEf3io6DGO/ceta4ipWlTcYR073FhcPh6dSM68r66K2nk2eV/GLws+nzSi2TfcxttMXqO4+tM+HumwXHh1hp+sxW12MrcWFxN5bDHcA4rnPH/wARdXvtThu7fSr+dJiZPOmjaNX64IJHP4Vy2lwXeseJIL3VLONYYwcq5DZzTwVSpRo8lRaM48zpUa2L9rReu22h6neeC7eRml1K/TZ3jR15/HivPvGbWdoPsul+X5cXzSMhBy38IyOOAT/317V6FrFhomoaT5sWlWMVzCuJNkIX8eK8W8R3SLM8UYCgZGBWmGr3k4q5yY7C8sVKVvkc5fbmhnZPvbc/rW/4R33WuW0ud3lW7ZbHbGB/OsSNRMrK2cOOcda7bwPpLW9vJdTgAyfJHxj5RXqqHNVj5Hke0UacvM6YmkpWFRs1egcDH0VHRuNACs1NpaKAI6BzSt1oWgDYxxUbVIc1GaAEAxS0Uq0AOozRRQAbqcjFeQSDScU9V3CgDqNMhFxGR3PNbdmDoKy36q0n2WMyKuMk49PeuX0XUPs8iKcYxiu/0ny9Th8vdgMMetfK8lsS4y7n3VKfNhYzj2H6f8Uo75jBfzx2w37XVTukTHr6Gurv9O+Hl/4ck0+1126mu7jbLNIvBgwRgcDAGRWDe+H9Ph8t7yys7gJgN51urgjPcEfWvdPhXr2keFvBd7D4fm0vTxMoD2i2sbpKm4kqOMjkk81spuMpK10WqDqU4uUrM+M/G82lTMdJW7uLq2s2IjuDgEjtjjoPfpXnOr6/a6PKrWN1JNtyCsgGSPqP8K+9fiH8XNE1rQJodS0bw/byfZ5LffDYqrbCMED0PA5FfCnxd1nRdc8RXEy2Nm74CItvGYUwBgfIDjtUUmqktnY5sdRlQhdyV/I1/DGunxDpclzGCPLVo2/2htJH6ivM9SU3F5duOkf8ya9H0CSDRfAGUVInlRmbA4Uf54rz6cC30t5JBh7x9/PXb2rtVGMJ3R5M6sp00mylpVmby8hgVzGZm2hgM7c98V6nawraWcUIJbykC7sdcd68/wDBdsbnWo2x8sClyf0H869GZMDrXq0l7tzxqj1sQMetR/nTpKb+VamQfnSqufWgLT6AG7fc0386kprLn60ARsDSqp96X8qVRQBp0yn00/SgBKUGkp1ABuozRxS0AKDT1aoxUisqKSxAA7mgBzyMqgpwy8ium8M+JPs0iFmPX5ua4q41y0j+VZPMb0Tmu/8AC3wo8QeJ/hjfePtItGfSdP1X+z7nbyytsRg5Hpl1X6kVx5hlNaUPrCjax6OU51ShU+r817nq2j3drrMSCQj5hwaxvGfgx/s7vYsY8jmSGQox/EEGvPtK1690Q7J1lAT2PFW9X+I1xNblFc4x3J5rweWpCWq1Pr/b0KlO1zznxRpN950kRv8AUGXPRrpmH6muGm8PJDKNw3MzdeprsvEniHzFJkJLH+FK4S+1i6mcmNGiHQHvXdRp1Jang4qpRTsmaur3gmhg0mB/3EeGuWHTaP4fzrk9c1H7XcbYvuJwqj07U95p2QxQI5aRvmPUse1eu/Dv4Rx+G9BuvGnj6ICPT4GntbOTpuAyrN6nOABXbSouctTy8RiYU4HlfhXxGnh/VJrXUovLWRgkjt96Nh2I9M16RJMGUMpBU8gjvXhd9eSahqFxdXBzLcytLIfVmOT+prb0jxnf6XbpApSaBOiyDkD0Br1fY6Wiedz66nqJkzSq2a5fTfGtpeYF0r2znueV/Oumt2WZA8bK6noynINZyhKO6KUk9iYdKXFKqE07YakY3bSU/aaRloAjZc0qg0tKtAF1TTqYpFO3UALSUhaoLq+t7Vc3EqRj3NNJydkJtJXZYpryLGpaRgqjqTxXPXnjCCPK2cbTN2J4FYN9qV1qsn+kOQg6IvAFelh8rrVdZKyOGtmFKC01Zv6h4viiJTT189xxuP3R/jWHNfX2ryATTNt/urwoqusKxjFadqqeTmIgg96+iwuXUaOyu+54WKzCpNa7C2cKQsEUc1+r/wDwTr8O2erfsw31jq9tFc2Wq61eJPDIuVkQpGhBH/Aa/Ka3XbOuexr9Zv8AgmvfJdfs8ywofmtNeuo2+pWN/wCTCuXiNf7Bp3Rvw1K+Za/yv9D5/wD2j/2bdW+GGr3Euk+ZPolw5NjdSRiRQDz5bnsw6e+MivkzxHb+ILCdwbGznUf3QV/qa/czxN4d0/xdod5pOvQJcWV5GUkRu2ehB7EHkHsRX55fGP8AZt8SeHPGK6Roml3GswalIRpl5BDkSr6ORwjDPOcDv06fnU6taErrVH6dTw2GrxtLSS/E+GrjUNXkTaNCgLfWuo8E/A34j/EeNbjRfC0Vvp7n/j+mjZY/wYn5vwzX6U/s7/sQ6N4Vji1v4qR6frmscPFpyES21sf9vPEjD0+6P9rg19Hav4dsfJ2RwRIqLhUVQAB7CuyOInpc82eApXfKz8v/AAD+yO3hqaO88SYvr1OfuYRD7D+tea/tja5/Yun2HhTT5FV7n9/dRp/DGp+UH6t/6DX6heJNItLK1uriRURIY2Ys3AUAZJJr8ZfihrknjzxzrGrTzNPHc3DrbM3aEMQmPw5/Gvdymh9Zm3bRHzeZ8uFceZ3bPIha/NV+Kx/dN0zir02mPbXGxwcE8H1qzII7SItM6xrj7zV7dPBxje5xTxTlbl1H6fapNDHIFXawBxWval9ObfaOYz12/wAJ+orP8PhnsuVYIJG8slSNy5yD+ta7IPzr0oUadWkuZXueVXrzp1nyu1jU0/xVBuEWoAW8p6MT8rfQ9voa3I5o5uY2VgfSuFuLNZFG4Zx7U23VrVs28ksJ/wBhsV4tfJLyvTdkenQzf3Vzq7PQGQUxo65q18QXUPF0VuUHfG1v8DW5Y6pBqCAwt8w6q3DD8K8jEYGtQ+Nadz06GLo1vhepMyY9qTbT2NNzXIdI9ZKVphGpZiAFGTUG6sfxFeEW4hjON33vpW+GoOtVUF1MMRW9jTczN1Lxbcz3E0NkRHGnG4dfzrF/eTSbpnZ2PdjmnWsI8st1MjFqvQ244J/Kvr8PhadONoqx83XxMm9XcgitzwelWNu0YxVgx+gqGRTkV2KNjh9o5CLC0rfKM1dtLIW7M2SS3WpbeMRpWgtvbrprzSyv9paYLDEoBBUAl2Y5yOSgHHOT6VtGCWrOWpWk/dWxRg5uRX6Tfsra3rHhX9lyy0r4P+VqfjHxFe3V3M8UYmTS8tsBkz8ofZEpCt/ezgjr+bdup+0Z7AV+tX/BOLSl0/8AZ1gfYFe81GSZjj72Ujwa8HiSfLhI9rnu8Mw5sa+j5T48/aO0D4m+B/HWmaV8U9f1PVE121W8trq41RyvXbMiuTsjZeTtACj5eOQKyLf4x+MPhdo8aaZ4o1+wit/9XYz6tMsQPls5UwBiwYl0w67VOAPavsv/AIKJ+GrfUvh74U1NU/4mOna+IImEfmEQTwyCXKDkruSI8AkYGOa/M/4hX7614zn0i3V7a2tJJIp40QxBv3nzKN2XcEKuNx4yPWvn8PKM8PzNa7H1GIjKnX5U9N/6/r9TsNP+OnxM8XeJReeGdY1o69PKqyX3257SW5RQVQMVbnDBycntjOCBX6Pfsw3/AMdrzRY0+O1po95p5tEe3vzOsd+WxyHSNTG69OSVb1LV86/sMfs8xa5fnxL4kskNtassdvGw4L43En1PTJ96/RUlLG1kkYBY4k4HYAVwYqsvgSO/BU3L943Y+UP29Pinb/D34I32maS+zW/FU39mqv3XhhZS0z4/3Bs+sgPavyhCDceMgV9mf8FKvHX9tfEzQPDaMG/sHSzdXQ/uXF0wcqR7RJB/30a+NSNvToa+0yLD+xwcX1lr/l+B8Nn+KdbHSSekdF+v4kGoQme3Ii2B/wCEsM4rMsNDgV/NvWa5uR3lHC/7o6CtqVSuAylTwear3GxYyzkAKMljxivUnThJ80lseZSrzjHki9yTywq44GKa1R6XLJcW4klXAYkp67e2au+XuxgZraLUo3RlNOEmmV/L3dCRUbR8dM1bEZX60jrhc0OIlMo+Vntim4kiZTCSHHKkdqssM8DqaqajdLZwtGh+cj5mrCaXK77G9NyckluW4PGC2EnlaxIrLxtdBkj610sNxHcwpLbuHjkGVYdCK8X1K482bk5rs/h9qjS2M9oxz9nYMn+63UfmP1r4zGwp+0bgrH2GFc+RKTudgz1i6ovmTN7Litas2YCW4kI6dK6sjhzYhvsjhzqpy0YruzGso/8AR4h321oxR9B3qpp4/dqPTitaOMH0r6ylHQ+axFS0mQNHioGXcyj3FXZvlqvGu6Re/wA1W9zKEtLllVCqBTuaeVPpSbStanNzX1Eh/wCWh9FNfsv+xLpg0v8AZz8LDbt+0QCU/wDfKr/7LX40r8sUx9VxX7J+Fteb4Tfsi6RqNvhbyz8OxfZBtzm4mAEQxg/xuvavluKNaVOC6s+s4SX7+rN9EfP37cHxKsPG3xG0rwzo5jvIvCSTLeFSG8y5nCBoV+VvnCABeM7i393n4u8SaS9n400fVmCNbbo4WJX5YlYoBESEUGUbySK9Gu9Qe8uLi9u7iQCWQTSOrAzGPzhiWMPLnzgSQOPu5J6k1xfj24/s3S7SGNbN5rq7tYpFjZGQZMZEsWHO6Q+UwdscZPrxxU6EaeH5X0PSq15VMTfufqT+ymtknwv0hNPVVYLKZvXzNwGT+tes69IrRwWzsqJM+ZWLYAReWz+ANeBfsaTySeFXRslBlx6cn/8AXW9+1p4+/wCEB+CPjnWIZPLuTp39lWJBwfPuj5ZK+6qzN/wE186qLqYhU1u3b7z6GOIVLBe1eyV/uPye+PHj5vih8XPFnibczw6tqksltntbqdkI/CNUH4VwW0HrUs33zUVfqUIKEVFbLQ/J5VJVJOT3eo5rg+T5cyiQL/q2PVPx9PasW8U6heRWKk+WR5lwR/cB4X8T+ma0Z5liieSUhUjUsx9hUGhW7/Z3vLhcTXjbznqq/wAK/gKyq+9JQXXf0Oik/ZxdTtt6/wDA3NNUCgBR0p3lnvTY33MKsMuV9K6Ujgk2nqV9hqOZsfePI9astgKfase+ujnZGcuzYX3JqajUUbUYuciZWwry/wAK8L9a5rVLhpGJ4OfWug1ZltLWOGPnaOfrXIak5ZCF6mvOxdTljY9fL6fNLmMS6IkmbkH6V0fw/uPs+pXCsQA0Hf2Yf4mubWAjLdq0dDuDDdOU4PlkfqK+UqJu7Z9QmloeqSybVY98VRtPmBPXJqe8fbCRnBPFQ2YxXuZBS/dyn3Z85n1TmqKHZFfT4P3kinqkjfzz/I1opH19qrxjydS/2Z1z/wACHX9P5VPIzBSqj534HtX0FPRWPBqtylfuVJmM0m2ME4qeO3MYDMOlS24SH5I/mPVm96lc/ITVpESqNe6gamSdOBTyvpTWB+lUZIWOMvEB3d1X8yK/VD9rO/Gg/s1+DtFG3bffZEljyN7JFbFvlBB6OIyTjhQ1flzpcPnahp8K8mW+hQD6uBX6V/t7asmi6b8NtN2RFil0ymRsLlVgQIw3r8rK0gOc8AjvXy+fv/aaC9WfW8OK2HxEvRHyfGkq3OVMq3BuD5TJvVfOmTgj/VjbNt4PRVGfSuA8YTjVvF3hSyj3vE9w90reYxEYUZaFVMjYRZHcAnk/jXaRrbtCfLQzxLG6EYQySQg7uSsbYdf4jn5UAFcbaBtW+OSpIjF7KxRGlwQJy75SQAquAUwAMdBXJiPdp/1/X9dbtrspPmn6X/r+vwSSf6l/sq6UNJ+HyTSLtzCp/Qn+tfOX/BTbxwbPwv4L8IQyjfqVzNrN6ncBR5cOfY75f++K+vvhToo0v4f2NooK+cqx++0AA/oDX5jft+eOF8ZftI+IIYZBJa+HYodJtyDwPKXdIPwleUfhXDkNH22Yc3SN3+h38Q1vYZWqa3lZfqz5sc5YmoW/2amdahkYRgtIcKoyx9BX3rPz+Blalm+vLbTkziY+bP8A9c17fieK3ZlCQ4HAArF8Kxm8e61OYHddPtjz2jXgf41vXCkxkCsMN70XU7/l0/zN8U+WcaS+zv69f8vkULWTfJitCToBWLbM0d4R2FbUg3bSM9K2pPQwxEbSRR1G6FpCSxAJrF0Ob7dezXT/AOqtQSPdj0/SsfxZrUlxqhtLf7sfBNa0MR0nR4bf/ltN88vrz2/KvP8ArPtazUdo/mevHCeyw6v8U/yGaldPdSHaeM1kXEP3h3rT8s7d3NZ1+fLVz3rKvdq7OvDq1oow7hgpKrT9Pfy5Cw/u4prQt5LyMOvSq6ybehwa+cqp82p7cVpoerX7Fiq9u9Pt1wevSqt1KUusdVIH4VZRtyfKcV9LlMOXDRPlc1lKWIlclf5Zo29G/pRcXRVcRgBj3rOuLqaGZFkXKFgM1aVfMfpXpp30R57pWs2W7OMRQjOSxqZv9W3pio1bavTIp/DIe2RWiOWWruLmmv8AN0zTt4Cio2csaBJHU/DOx/tL4keDLMjd9q8QWUZHqDMua+2/+Ch+pPP8VNA0+EPIth4fEhVd3HmTSbh8qkjiKN+COEI718efAGEXXx3+HMTDg+IrVv8Avlwf6V9RftxXMeo/tDX9tNLGPs2l2kI8x1Cxbk3KfmcAZZiG4ztz618tnFpY6mu0WfYZFeOAqPvJfqeCpqU0OoJ537wvNEQ02djl14J3yfclHLDHAwD6VnfAHT18RftBXEMQkdJb+0hAkxnYMkjgkAYHA7DFbkFqsnlra2zTF1U+TEu1n+YCWHKR/KTwwAPCAdzW1+x3Yvq/7Rk801x9u26gZDNsK7tkA5wQDjoPwrgxbkqX9f1/XXU78Moyq27/AOf9f8DQ/VeC4t/CvhMXd8wS10jTpLqdj/CqISx/IGvwx8YeILrxZ4n1bWdTbdd6vfTXc5/25HLt+rGv17/bE8WHwT+zP41uYm2z31hHpcQzgn7Qyxvj/gDufwr8b7j7xPP5V18LUbUqlXu7fd/w5xcX1716dFdFf7/+GIWzWF4ouHa2isLc/vtQfZx1C/xH8q22rn9Ib+1/El3etzBZDyIfTP8AEa+hxUm4qmt5afLr+B8/g48rdV7R1+fT8TobO3Wzto4IlCrGgUfhU7uFX5sVCzbW74+lQXkh8k84rpvyxsjls5yu+pXnjxJvjPPetGObzLbevULz7VgteeX3JqT+2IrWCUSEIWHy7v8AOawVWMbtnVPDzmkkrnH6bCb7xhJvGUjYu/0H/wBeusmQzTGST6D2rmfC8yf8JBqEjNwU+90rTv8AWkjbbHyRXl4GUY0ZSb3bPaxkKk60YRWyRcmYZxngVj6pIDGdpBPSnwtcXmWVWxSPpc1w+0A4FbVXKcbJE0Yxpy957GLds7W+Bwq/rVPyzGoMgwT61v6s0Gl24STa0nZfeuc8yS6kLyHGeleDjIxhOzd2ezhpc8LpWR6iGS6Zye5OKswjy1x1xRRX1OHio04pdj46vKUpNvqJcyRqmZSFHvQrHgrmiiuhPUz5fdTLasduDUo5XrRRWiORjN3yLRRRSEenfsyQm7/aL+HyD/lnqgl/75Umvcv21L6d/wBpzxPDGX2RW1llULcg2cLMCVAxkfNy2f3eB1oor5LN3/tyf90+2yNf8J8vOR5fK6yG4N5IzoMs7K6ecyNtKSoHkYh2/i77a9K/YbsTJ8ctWkZbIOLiRM2YHlNnYvGOO1FFcuYfwPv/AE/zN8BriL+n5v8AyPcv+Cn/AIq+w/Dfwp4fjcq2r63LdsoPVLeLbg+26dT+FfmrI25jRRXu8PxSy+Fut/zPnuI5OWZ1L9LfkjH8Ral/Zek3E4bDldkf+8eBUXhOzNjo8KsMPIN756kmiiuqMubGSv8AZWnzMbcuBi19qWvyWhoT3Ea5+Y8f3aoXOoBlKpGTn1NFFdE5smjTi9WY91NIEJ3bFH93j9awpuWLYNFFeVit7Ht4TYz9Lll/tCVLf78vFdxpXhNYysl8wZm/hoorPJKcalNuWtmZ55XnSlFQ0ujoPssVvHiNQFx6Vy/iLxFFpqNHbYM7dB6UUV35pWlRw7lDRnn5RRjXrWqanMxaXJdxm81N2UNzk+lU5rpN22zUqg/iPU0UV83i0qSio9d31PpcPJ1OZvo7H//Z</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCADIANUDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD4aW3HTFWI7fC8ip1AarCxigCtHbhjU/2cVZjjFTJD60AVo7XaM09bXc2cVeEeelTxwgUwKItuOlSx2o4rQW33dqmjtRQO5QW1AqxHa+lXltuBUyw0hlJbapVt8VfSDNP8nj2oGtSitrTvsorQXT7mZCYk2j+8/wDhXL63HqtszGO9ZMdgi4/lXkSzXCxnyKV35HtRyfFyh7RxsvM2Ps/vQ1uBXnk3jTXdIlDSPFeJnBjkQKcexGK7Hwv4vsfFEZSImC7QZe2k+8Pceor0adaFVXizy6lGdJ2ki60Ge1Ma3A7Vq+RUbQ1sYmU1v+FMa3rV8n2qNoRQBlG3PNV3t+tbDQ1DLCfSgDINt7U0wbe1ank1HJEB0oAymhzziq80PatSROelV5YwaAMh4vm9KKtsg3UUwMuGTt6VdhYkVSt460beKhEk8I3Grka54qKGH86uRpQIdGlWoou5ojiw1Wo4eaACOPdVpIM4oRORWhHAWxSArJbipltvarawe1TrBQBSFvW/pnhh5mjLru7kH19Kh0+3VryEN93cM5r0bSVtVv7S3LA3MuBHHgknPTpXz2bV5qKw9P7W/ofWZDhac5SxNXaO3qVbX4Z39/YtLFESo6nPH0rjPFPwyu4FkYg/KM8CvoPTLi68lrazvIGeM/PBghh1zwcVmeLvC+p6lbNKJYIYWTJLNgkf5zXzipQgttT7aU3UXkfDXizQ5LKeQMuSOtcY3nWN5Dd2rtDcwtlWWva/ihZf2XdOJWjKE43Dj+fX8K8ouI0bcw6Zr2cNKUEmfH46nGUmkev+F9WTxHodveqoV2G2RB/C44I/r9CK0WgPpXEfB+7DXGqWSn92uyZR78hv5LXpTW4r6iEuaKZ8jUjyyaMdo8VBJHt7cVryW+M8VTli5PFWQZ7LUbKKutGKgkXH0oHcpulV5Fq7JVWQZzQBRkXkmq0ncVdmXap7mqDLQMhcDNFOaPdRQBnww4HvV+GPHanRwc5xzVmOGqsQOiXAzVqGMHr3piQnFW7ePbjPSpAmjiq1HD+VJGh7VbjXNADYovmFatvHxyKhhiAYVqwQjaKAGRw7sVMtru7VZjgqxHDjtQA7QdGXVtYtrR7qOwidgJLqVWZYlyAWIUFu/YHrXpGo6x4T8P6d4nn8PWj+INUsbNXEMysHkY/KBF8m5iCBnaPlBBOOtcj4TsBJrFtNIAYo5Apz6kHH8jXtjeA4ZLaTUVggTT9uZbibPlj1HHU+xFfIZliOTFqLjeyPuspwTrYPnhUcW35Hz98I9N8R6h4oj1ed/sVkALi6UTsyHuVAbLZABzn096z/AIseKvEXiDxz/Ymi3sh03z2i/c8SqqglmC45A/qOtfXvg/w5aSGCS3tzHbLF5jt5ITzFBz09OB2H05r5V+Iuh6gfHM2pxXEtvp1veuyytxHCJCNx9skA14lPGUZ1bNafqfSVMHWhRtF9r+hxHxc8OWnw+0XRbbU4bvWbvVrWW7iaW5jmKxocFggIZeQfvKp4PHFeH3dmtjoK6pHJDLazt8lvDcpLMvBJO1WJAHH3sHnvg4+kfih8P9RhuF/te4aSJ0+R3HmrsI/hJHT8a8N8S2NjoVm1tZoAvdsYJPrXs4bE05vlSd/U+dxmEq0/elJW9P6uR/A3VIm8VXqs/ko9tsXzjsLuXXAAPU4B/I17w1vuWvmHwnp76t4v0iyhXZLJcxymXoSquCwH0AJr6v8As21RX1NF+7a2x8ZXjyyTb3MaS161mzw4Yiulmg+U8ZrJuLX5jmug5jDmjxVSZflrWuIcfSqE0Z5zQBnMveq8gx0q/MoqnJ19KBlOUAqaqNED9avSDdmq7L2NBRVaI9qKmZeaKAGpHU8a80JGasxp0qiCSOOrkMO4e1RRJ0rQt48DHWpAdDbjp2q1HD6Cnwx8j0q9DCPSgBIIOlatvDSW1tzWhHb4oAjjhzjNWo4fyqaOGrCwmgDU8MxSSW+pQx8usQukXOPmjPJHvtZ69S8G+Il17R4V1Jm/suycSywgE+dID8seO+SOlea+E9R/sHXra6O0RZMUu4ZHluCrcd+CT+Fd34i8Fzana2cKIy6Z5oluZbZ2ACsuAVIIIznGevJ6V85meFVSaq9LWZ9lkmO9lSlQ63ujp/EQ8TztcXWkaq2m2sxJNheTr5Cgr/AAC6884zjrxXyh8RNF8WXN3eRav4rWTTv9YLLS41KOP94jcT78CvcfEl14S8EwrbX+ga1qSZUwzWM0r4APfMgI/X1r5v8AiY+n+KdTZdK0K90u2z8slzNKrY+vmEk/gK8OlQoaVI2+7+tT6qvOsoODfyv/AFodzr/xQs7j4f2ULSG6hgT7Osj/ADFSoGQTXzHrWp/8JFqxitFPzuEUY7k9a9isdB+y+GTYTw3CxHayXLncG4O4sDznGACc9e+a5XWLez0dbkRRrE8wXFxIcbSPmOO/TPPoTXtYbCxpPmXU+XxuOnXXLLSxofCPwOZPEVtqm0+TYWxQy4+Vpm4IH0UnP4V7S1tjrXkHwR+Kum6jNdeHWkCzpK0ltK3H2hcDdj3Bzx6Y9DXtSMHXNfQwjyqx8hUnzyuZs1uNvSsy8tuCRXRyRBhWdc2+e2a0MjlbqE81mTxdfWumurf5jxzWPcQdaAMGePbVKVOp71rzx9aoSx4z6UDM1l61Ay5ark0fNVyo3UDIWTBopzfeNFAyyseamjh+YcVYih9qnjhwaZARwjNXIYabHD83NXoU9qQElvHxWjbwnNRQw4xWlbx7SKALEMPFWooz1pbdc9RWH408eaZ4HtUe8LS3Mv8AqrWLG9+evPQe59KaTeiA6mGPvVpYz6V4g/7Ql08zG10aFLf+Bp5yWPuQBWLrvx48R6lbmC0+z6cGODLbod/4FicfhzWyozfQnmR7/q2uaZoMIk1K/t7NT082QAt9B1P4V6l+zr8dtI8aapceCXhlnt1tWmi1MoU2KHUFCG525dcHHqK+DQ3nSedNJJdXcgDNPO25ske/evf/ANlvxVoXw/8AEPiTWPEV5HY6dZ6OWmuJRu4MqDAA5JJVQAOSSK76OBhWl7Oo9GCqyp+/HRo+kfiR42g8E3qWA063u4pT5cV5dIoDHBPU8c44P+17GvMLvUtL8WSJPcx2hs03yyXMKjyo1DHBZsccDp9fpXFfEv4sXXji9jh8K6Lf6LbLH9pR9aDJ50bEgMsODtB25GG9iO1eA6143On3jaZ4l1ie3eRnzcW6CRQGGPmjAGMDuATyeK8+pw0qUnKPw9z2f7erThySlueifGH4uabbIYdLMaW1uoRI5CDhevzDPX5j78HHt8z+LPH154liFupZYOGZsnMhxzkfjj8K1/GPhSKTWHe0vp9VsVVBFcynh8jOQMDA5x+FQ6L4VW4uEDpkA88dqI4P2crM8uWIdRWOZ0LTb/7ZDc2zvBLG4aORCQysDwQR0NexeDPjN4r0u8kkv7k6xbRt5c0NwioBjurKBg/XP0rJW6s9KufsFlafbtQXG5Y+I4vd37fhk1ZXQZprdo0UK0jmSWQKQpY9ce1dcaMbGGp794F+KmhePg0VjP5N+oy9nNgSe5H94e4/HFdPMuCa+RIdFOh6gtzbzG3niO9ZlyCp9jjOatah8TvENngW+uXzEd3mJH5HisJUGtbj5u59P3Uec1i3Vt1NcZ8H/inN4ygm03VWT+1IF3pIoC+dH0JwONwOM49frXf3K8NXM9NCjnbiELk1lzrya3LyPg1h3XekMzZ87qrPxVmb1qnI3BoGRM3zUUxn5ooC508MeOMVZjh+aiGPvVmGPmqELHB0q1DDTo48mrUcR7VIE9vD0PWtKGPFV7ePp7VfhUlhxQBPGFjUsTtVRkk9q+Z/GeqHxj4z1S8bcbeHEMIPYEfpxj/vo17F8TvFD6bappFqwS4ul3TSE/ciJIwPdsEfTNeVWmmrBNIxGTNK0hb8gP0Fd2Hh9pkSuzETTVt7c5HQcBhg1BHpiJMCxJYHgZxXaXWkpcQMykdO/Wsi90gRSeYSDk5/Wu/lIuSWWnbpI2GGbI5bpXofwc+Cd58YfigYnSZ9D0dbWe5hH+qnk3Myo46EYJrk9Mty6pgY7biOK+nf2ZdXfwJ8PfiT4mkhdYvt0VtbuRgSutuuAvPJBfH416OBhz1lZXMqrtHU5z9qTxVpnhe+lbTIMLo9o1iyrJlfNYqwAB6AAHv/ABV8a+B/DNx4/wBen1fVHLWkb7yp6yN1x9K9Z/aMuJ4fDUJlYyXN1M0szt1MjnJOPX+VQeAfD7eH/B1mGX9/dDz5M9sj5R+A/rXqZnJQfK3e34s5aClN6aD59OgkdV8lSnpjinrptvA22OPaxGQxXgD61s29qVwBxIevFZviFDeOmkWoImnG65mXgpFnGAf7zYIHoNx7Cvm27K6PR8jBh26hd/alBa1hJWDaP9cw4Lk/3euPXr6VNO0zJJLK4giXAJ9Bnp9a27+O10LSZJpcRxwx5O1eEUdAB+lc3LFeay0aMrQWsbbpTjO5+6gd9o4z6g1F7aDlexyWtP8AbJH8tpTj5QoQmuZv9PuYWPJHfaykV6TqRgtFaNVJ/iO4da4nVbpzI4OD9KwlbdkvsUvB+tSeHfF2mX6sVEM678d0Jw4/ImvrmZsKfWvi2Vv9I3g5IOa+zoZPtFvHIOjqGH4jNcFTcqOxnXXzZBrAvlxmuivl2g+tc7qH3TWRZkTH5jVGRuT2qxO3WqUr4zzQBDIw3UVC8g3c0UAekwx+tWUj+YccUsUfTtVpY+BgUwFjj7CrkS9KjjjxVmNehpAXoYeBUzOlpC88hIjjUuxAJ4AyeBRbfdrl/ixrDab4XNrBuE9+/kAq2Cq9WOO4wMH/AHqqK5mkB5NrGtDWtYvNUlcf6Q5MYc4AQcKvPtj8a0tLjSawhJ5PP3hyOT/n8KymsI5LKTcWj+XnHzD8QeDUvh+48rQ4xGyyeXIy/Kxx16c9Pp2r2Y+6rIytqdNawq0ZC/jz0p82irJbjIy3fIz71BpcqX0KTQjG/h1x0IrprNf3JBXJ7nHTmtLeQ7rRtmDa6e6bVVSACMn0r2Pw3qi3fwc8P6Mr5M2qXt5OqnskxjTP1K/+O156qBWyxBGc4WtH4OyNL4XaRzk/brpFX+6vnycfmSfxr2spf+0X7I5sRH3LeZxHxp0k+JvHfhzRMboFLXVyB/zzXGc/Xp+IroJrfbLH8oA6fLUur2yyeOtW1KQfNGI7SM46Ko3N+ZZf++auf8fBG4DaP4q5MdUdSvKz2NKMVGGq3KV4qWNt5m3zJGO2NAcFmPQD/PHXtXPWEaQ3z2yOss8jeddzjHJ9B6AYAA9BWd4p8STWutkoPMhjQxW5DD75JDufcY2j/gXrW94fs1ttLM+0tLNy0jfeNeXe7tY6LdbnE/FTWktdQ0bTViNw9xOJ3tl/5abOUQ+xbGfxrQt9BufLN1rdyJpsAi2jJS3i9gB976msPTLW58WfEbU9WiiV49NK28M0wJijOPmOP4m6YGR15PSup1mS7jgKJIsso+9I8Yz+AGOKhPVsS1OW8R6hb2cIEXkqCOFUAfjj/PWvONTuFZuCOc/Wuy8QvP5btJJLNjkkhVGa881K6R5D8232JqKjIKp+Zm5r7L0FSuh6eGGG+zRg59dor43s4jdXMUSctIyqPxOK+1VjEMYQcKowK4JsuJmX38Wa5nUWxmuov+9cpq2BmsijCumxk1nTTdas3cnX0rLnkzmgBrSc80VTeb5qKAPcY1q7GuAKrQrzV1O1MCWOPNTLF7URrirKrtpASwrgV474w1hvEXiq4Bk821s3MUDKAAOm76/MOvtXo/jDXP7B8N3U6HFxIPJh9d7cA/gMn8K8es4kt4AuSHxk5Oa7sND7ZErPQnuEaOEZ+bP90dfwrFt9QhhsZiisqpMdwIxzx0ro7PT7nXNUtdN0+Mz3dzIsMSKerHj8PUmvoOx/Y30r7M7Xeq3l6dqtKihY0LgcgYGcfj+Nc2PzTDYDlVd6votz1cvyvE5hzSoLRdWfOHhO+/fMMlopBu/HvXfWcgYkbuOP170fGD4cp4AsEvdD02WJLVttxErtIGj7sNxJyOv0rB8N6tDfw+ZFKJFbG3B/H+ddGAx9DMKftaL07Pcyx2ArZdU9lWWvdbHWRbD8rfLxktUvwfkQeF40U5P267Lf9/3qjvyoYHdlc1n/AAnvvsXhnUmLDMV9dge37wkfzr6fLZ8lVt9n+h5FdcyTNS7mSS6mIYYaRmJ9ckmsvxBqn9j6XdXMY3yop8tR1ZycKv4kgfjVCa+BR2Uj5j+Ve0fBn4KWnjHSoNc163+12bSbre2dyqZU/fYDryOAeO/pXzePxsMLCVer/TPXwWDqYyoqVJ/8BHjXgf4P+IviVfxQaVbiWK0RUe6lJCAjrlsYyfTnrXumk/sqeJHtfst3r2jacZBt3zXK/uwcDJ6dOuBXvK2GhaHpMNhYiSVYV+S3toxFAn1wuCfzq9I+pWvh9JLu/wBF0GIuMSeVvZRnrliP/Qa/Oa/EmKqTvSXLG9tv1Z97h+HcLTjap70vn+SPlHX/ANnG5+EumtZaddN4vsYUN1fa1ptu5tUlYsWDPyARj14GM15XrluNrBV9+DX3V8f/ABtHb/s1+JdObx3b399fRm3httPhWATBmAKAn1GSWxxzXwRfakbW3VJpoGjVQoa3Jdhx6HrX2mU4ypjKT9otuv8Aw10fG5nhIYSolB6dtf1s/wADg/FR8tCgb5erV5pfMJJCMd+9dp4m1NJHkKsRkniRcGuGuPnY816VSWuh4fS7Nv4e6eb7xtodui7t15EzD/ZVgzfoDX2FMMdq+bv2fdBfUPGEmpFD5Gnwn5v+mjjaB/3zv/Kvoy5kPl5FcUty0Z2oN1rkNYk5NdLqE2Aa43WLjrUDMK8l61lXEvWrNxJuzWZOxGaAIpJDuNFQPJg0UAfRsS1YUdKjjXAxU8fWmBciGeDVnZxVVGxVhpGWB2QZbaSo96QHmHxO12BtXtrCSdY0t13lSwBZ2HbPoP8A0KuNn1a3jOfmUY43Y/xqKO1hmuZDiS81W8PmzTNJhxnuzEcAdl6e1dDY+CNIktTA9jFOScNJMN5J74J/pivZhBxiomV235Hrf7JOhRaxqeo+IWVmEbfYodynhiAztyPQqBj1NfXl9byy28aIu5jwFjPJHvXy/wDs16/4U+E1zqFhqP8AxLobyRZIZGbEKtt2kH0JwOT1+tfSWteNNE+z297balDHDMAkc+4BWJHAz2NfiXENWtHNJxrJ9LaaNW6H7NkHsVl9ONJrS9/W/UxLj4G3fxMumhMh07T0bbLcyDd9VQdz+g/Svl/4ifAzwt4J8ZXNp4Q1/UL+3jkJuftEcfkiYcERFccZz2xnpxzX3L4k+JKeH/grqV3ZoY7uDTwkc8bjiSQBdwI9GbNfDMurSLHuSPfgkla/WMqy2ll2Fi0vekk2/U/N82zGtj8S1J+7FtJehix+EtRVci4V1wegxXJSw/8ACufDOoRareQxNeXzyW6x7mZ9xU7QoXJPB6e1enafrEV4xtwSGYbkAPVeB+lcpZWqat8WJZ7xA62OnRi1V+QpeR97D3wgGa9tVJQbceqt954nKmkjmtD0LVdaaB2sri2tHcBpJkMRCk8na2DwPavrjQ/iNofhvSU0+089LG3RREqxsNxA6c9B0FeW3jpHBH9eoPsap3d0nl4LZxn1rysZl1PHcqqt+6erg8xqYC7pWvLur7Hs0n7SHh3TYUbVbW6ZFUH7LZx4OdwA+YkFjz3I69OKST9tTTPDKztp3hGKIwxtLBNOiGQLjDdAxOMgnb2Poa8EuFt7ryS3zqMoeO3X+lec3fnBrtY7pory1ZIIFdcqHjLAEn0eNkBFeXDh/B05Kpr9/wDTPQqZ9i6sXT018v8Ag2N/xf4tm1vXNQ1C/mVptQuJLuU52kPIxfGP7vPGOOleWeLNcSKRljLY6Yq5q+vR6xpztcBop4fkaM9UI4I+lec6pfu5KSSbgvRvWvctGnBRitFsfOznKpJtsoalqDzSNuPXpWaf7xNPuGEhyOlGm28+q6tZ2VpD9qlklUCENt389M9vr2rllIg+ovhH4XPhPwbbrOire3Z+0zlc5+YfKpyB0XAI9c11dxcgKaYs223QHghQDkk/qetULy6XnnNc5RS1K6HzcVx+rTbmNbWp3gwcVzN/LuzQBj3Um01nTSZzVi6csTVGQ4oAgkbLUVG7fNRQB9PqKmQVEoqdB7UATLxWd4t1O40nwrq13arungtZJE+oUnP4Vog0k0cd1DJDKoeORSjKehBGCKa3A+bvDUkmn2P2i8k33dwPMkdugHp+VdhpetB4wVcopG4evtmuB8QXC6XJcaSzfNHcmAseu1Wwf5CpYfGkOm27FVjnMYyeelexGSMvh2PWjqBe1cXkkc0BXLCQAgL7/wCFPt57RNPktLPUrrTreZVBhUiWPrkEI+Qv4Yrxa+8TalrN5Z6Z5a29xdOssiA52RZBUH3PXHoBXpf9qaZ4Wsw99cJLclRwT046YrGrSpYr3asVJeZ00a9TD+9Tbi/JntfhXWtRt/g7q+if2hNfWVtdQJvuNobEjl1HAHAMbfmK4q8heNlcBsZ5/wA/hWR4B8e3OtWupWcUBh0ydop2dx8zOgcLj0GJG/Sulj8/ULuCztbdrm4mk2JGgG5jzXXKa5EtklYyfxc29znL1L6xkSe3G0I29PbrkfSqC609xereBWguVDRuq9WU849yDyPqR3qbVvFIs2ltlSW48mQRbo4t2TkhuByMEY5AB4xnPORqi/a4/OibBYb1dcd+Qay5lLZgvQ7H+3ruSEp52MAMGxwy+tPg1yW9hKPIA6jHoD7157ovi7zd9leTLBcIcxyNgK5/oSKttrnzZRmWdDk8jg/1FPmV73Hra1tjtVkYxsMg45BXqK4/WGW18SK7EC21KPY5x92ZAcfmuR/wCprXxpHvw7BHzgqcVmeKidR0uVoDh0bzEYdQ45B/MfkTU3Vhu7ZwXjZhpesSHd8si7XwcZ/+vXC6tcLNMAhzgYyDWt4x1YatqEk2BlguRno20Z/XNcvJKIVznLdhXFUlrYgjuJjCuB1P6Cu7+BuhPf8Ai5dQbYYLBdzBupZgwXH6n8K85Z2LfOc5716v8Bbt47rV7fHyMkb7vQgsAP1P5VzMZ71LcgL1rLvLkAZzUM11hTzmsq9uuDzipGRX1wDmufu5i2at3lwT3rLmYsaAKcw4JNUJmzxV26faKzJWpdQIJO3OKKZK3zUUAfVMZGKnrNhnwfarkcu4UwJ91DN6Go/MpN3vQM8v+InwTXxdqj6np2ofYLuTmSKSPfG7Yxng5U+vWvP/APhS/i/RWV/7Ms9YiiYusdvc7NzdiQwGfpX0lGwzVyLBq1OSDlR8cQaP420nWry+fw/qT30+5Qy2juAT6EA8D2pF8MeMLu6Sa58OatKQcndaScn8RX2eIUPapfsqkcCj2kkLlPjvT/ijJoN5JZmK5sZVby5Y1A3BlJBBBB5znitZv2hrjT5EktJpGnjbckzoVdSO4KFSD7iuW1/QIr3xhrjMN+b6c/8AkRquWvgO28kyNCoY9K64+0khcxIvx61eORnEdygbzDut76ZPvkeYRknBYgFj1JAOc1Yk+PCTW/ljTZIMKFXy5AQMDGOg4qG68HzQafLHDJthkXDLjkrwcfTNcdqHhcwnhcVP7yOoF68+IbX0zs0JVWOeabD8QLiPaEZiB03H+tc/Jo7r2IqubF14qHOYjq5fiBJIwYxfMPQ1bh+Kd5HbvCAxDDHPNcM1sy9qXy9vWp9rPuFkXrjUpLiZ5G6scnFV2Yu2T61HmnKazKJDF5i4r1T4J3Uy2upW7RKI0dHEwXBJIPyk98AD6ZNeWZNetfB+4UaHfJ/ELjJ/FRj+RqWC3PQ7i6IXrisW4uiWIzU15dcHJxWNcXHzE5zUFkk02e9VJJuTTWmznmqztuNBAy4k3ZrPmbGauy/dqhcNxSAqs3OaKbJiigD6Whmq9DNWHDJ6Gr0M1WBrrJu6U7dVGOb0NTiSgpFhW7Vbt2I71mrJ81W42C1AzVRs1U8Ua9H4b8L6lqTtt+zwMye74wo+pYgfjTo5McivOPj9NP8A8InYRRuVhkvFEqj+LCsRn8R+lVFXaQjwrS7gLM0jkmQklmPUk9a6/TZzLAGkG5ieNvNcPDumkZo/lVmbG3pwSK7DRVZMNIuSGzn8fSvYhZIxV79yzrUjwrIpTgYzj/PvXK3xMytnp9a1NN1j+1v7QkkdmUXcsQA6YAGKr3iQ/wB4n2AqX73UpbbHOT24bJ25WsyWzZmJ2YGa6O4hVjtQkDntWdIhX7uSfpWLQ/kYVxZld2RVSS328Vvy2cknRcsRnrxVaTSpfvuML/n8P1rBxHqYXkEnFN8kr7CtmS0SPjdn6VC1mG5K0uUm5m7xjmu8+FOoeTdahbFsB0WQD6Ej/wBmrjJIQucLjFS6NqR0nWrS6BwgbY/+6eDWckNHst5cbs81lTTe9OnuAy9c1nzSck5rE0LKzdqRpNtU45hmnM+6gkfJJmqkvWpC1QSNmgRDJ97riio5OWzRQB9AQze9W4Zs0UVYFuOfpzVyObd1oooGiZW5q1G3yiiioKLUTHrXl/7QGtLZ6HploF3ySztMB3+RCP5uKKK0p/EiZbHjfhe0c6bahx0Xc+T+Na+oap/ZsMLrMWd2YmELwkaozMxOOpO3HPb3oor0btRSRFupz3w9uhdaTdJuJlWbzG+rD/61ddDo0kkO5k2nHOWB+veiiqppOMWS27M5++sRZXWD0/E1mXFxtJYZz3OcUUVEi+pnremG6Qg7S+U68nI/xxVhoZZwCwYgdzRRWfcEr2HxaazMFC7iaLiz8qMl3VAOetFFVYUtL2Me4urMHarmZvRBmsm4YPvAQqP9rrRRXPLYDu/DWqf2jo8LE5kjHlv9R/8AWxVyVic0UVzM0Ig1P8zPeiikIGbjGajZqKKYFdm+bk0UUUhH/9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCADIAKYDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD8rKKT/PSj/PSgBaKT/PSj/PSgBaKT/PSj/PSgBaKT/PSlx/nFABRUkNrcXDbbeB5SeyIW/lV1fDfiBhkaJe/+A7f4Um0h2bM6irF1puoWP/H5Yzwf9dImX+Yqt/npTELRSf56Uf56UALRSf56Uf56UALRSf56Uf56UALRSf56Uf56UALRSf56UUAL+dH50n+elH+elAC/nR+dJ/npR/npQAv50fnSf56VueEfCepeMNWj0zT4yQeZHxwi/wCNDdgSuUNL0jUNauls9NtZJpW7L2HqT2Feo+H/AIR2NmqTa1ILu4I3eWMiND6erV6T4c+HFr4Xs1tbeFVyMySdWY+5rQkscZCrXl4rGuOkD3cBlqn71Q5u30q30+ER2tvFGF6KigAfgKesWSOCa2m09+cConsWj+ZkNeZ9Ynuz3PqVO2iKjRrcQtDcRpIjcFXXII9wa4DxZ8LtJvN1zoeLO5OT5Q/1Tn0x/D+HFekMmxQPSqF4uSa3o4+cdzhxGVU56rc+btQ0+70u6ks76B4pYzhlb/PNV/zr27xZ4ZtfEFifOAW4jB8uQLyP/rV4vfWU+n3UlncqFkjbBr2qFeNeN47nzuJw0sPLlZD+dH50n+elH+elbHML+dH50n+elH+elAC/nR+dJ/npR/npQAv50Un+elFAC0UY+lGPpQAUUY+lGPpQAV7/APBXRV0zRVvCuJr394zd8dv0/nXgdvC01xHCoyZHCjj1OK+pfDMENjawwRgBY1VVA7DFceMqckUkelltFVal5dDrkk3RiPBJPWpbTSWupDtjJAzkmoLP5iAwJNdT4eRPNCspO7rz/n0rykuZ6n1FOKgtDM/4R3HzCPOP1rP1LS/JX5o+fpXpTWAMfm7SB2Pv0xj9a57XLFeQq889MHpRUhFHTBSaPNrmz3Z4qg2kzXH3Iya6a6t9spXbj0rZ0W1t5B8y9ByfT/PNc6iiajsjzC802SKNg0f6V5N8UNDMCwaqseCG8qT3ByRX1XrHhdJDujh3ZXPTFeOfHDw/9n8Ky3Cw7TGyscdByK7MHLkqI8XMYqpSfkfOtFGPpRj6V7p8wFFGPpRj6UAFFGPpRj6UAFFGPpRQAfnR+dHHtRx7UAH50fnRx7UcUAanheFbjxFp0bZI+0IfyOf6V9D2N0ysqDrXinhPwzq1vqGl63Jbq1q1wqsVbLR5HG4dv/r16reXEsccgt22uTtDeledjLTkkj2suTpRbaO3sdesbW4SO6ukUn/a9K7nw7rOgT3CrDqUJbj7p/pXifhO18ITXrSeIJrq5ABRmjCYBPUFndVB/Hird5c/D1LrGgXOo2nknasnnpIgPPB8tmA/OuX2air6nr08RU8vvPrPTLG21C1RoZFkUcbgfbp7daq6xpOnrFJNNKFK5yWYDA6Y/n+deRfDnx5qFjAbOSRpBuJVt3Wrvj7xdeXmmy5kaLaMmvKxE5Opyn0FCUVR52Qa9qHhu1uma41KFVBOOaoQ+NPCtrj7PqMTnrw39K8z03RY/GGpJbnVLmIMCEVInmdwM8hEUsR79K0v+EA8O2+oLb3d9dQbGBaWaCaHHqTuXC/jXZTowhZyk/uPFrYmtUu4xVvU958Fa3pXiaB2jkRiF+X6GvOPj9pcX/CFauFUfu4XYDA7c11HhLwu/hOVFsbxLiEqJFZFGGRhnOc4P178Vz/xiuFvPButKzZJtpT9flNdFNKMk0edXm5wal2Piij86kmt57fH2iB49wyN6kZHqM1Hx7V7h8yH50fnRx7Uce1AB+dH50ce1HHtQAfnRRx7UUAH50fnRn6UZ+lAB+dTWkazXMULHAeRVz9SBUOfpSxvsYMDyDmga31Psm88FaPpPwyv9cSJI2int4YSgA3yMys4PrgMB9QK4jT9JXVYSvTPtV/xL4ua48GWFn57CO4lEnlnOPmCSAjtk5Of90VZ+H/lTXEUcmCC3SvnKanSUnLuz7etOjia0I019lXLngyy8N+E9J8SaL4h8DnWRrdqILXU45Nt3pbA7g8G5Sg+bBIG0nGCaw9J0y6vLHxBpQ0C/wDEWpeIb9L281nUIUjmVlLEshG4oxLsWIkIboVIr6e8P+C7e8tFkt4Yt3y8la6L/hG9J0NWa8hjWTnJOBjj/PNNYupCLUtjV5RQnNSSSZ8+fDvw2+l6xZ6fPA0ZVRuDc4P5AV1nj/T01Sw1C1toVCiRhx6DtxWja+SPEr3SLlFdiOO3arumvb3l9JDLgxySHNeBPGyqVlLzPpf7OhSwrp+R5z8Idc8F/DnxHDrnj7wjf65YxqdtnBP9nhJ9XAGZTjjEjbPan+EdD+FfiD4peM/EFno+rDS9eV7nSrZnWwn0u5JLARyws6iMMT8oQgqANteiXvhrSbyOe3SOMyRMQcYP581yDaKNDunFvCFZuu0Y/lXryzSpH3TwHkdOpFSlrYk0fS7jwvusXvluXPzyFF2pvIG7CjgZOeBxnJAHSs4eH/8AhKtetPD91I8UF5MUk2nkqOSB+AP5V02j6RNJCbyZc56Zryj4/XE+naPbzafctb3EN15wKvgnCkEf+PV1UJSrR5up4+IhDD1OR6o84/ai0FPDPjK90G3lY2VjND9hjY58uJ4mOB6AhFP1JrxD869U+OGqT38PhtdRnM2qJp6R38jMSWZVGxTnuqPtPuD6V5Xn6V7GE5vYx5tzwcwcXiJcisg/Oj86M/SjP0roOIPzo/OjP0oz9KAD86KM/SigAopP89aP89aAFopP89aP89aAPYrXxjputeArKwEyi/04QwyRHqQvAcZzkEYzXV+E9Qa1lgmRuOCa8E8PMP7WgjYMVlzGQh5OQQMfjXqmi6kLe3jw2RtHNeXjqNqfunu5Zi/3yc+iX4H1vofxYs9B8O/bLiRDIinbk8g1y8uveKPFEUvjDxBcXBtI28y30+MEt5eD+9YDr0GAPXJrx/TvEVndNG2pMv2S1bznVv4yOi/icVpL8UPE3iLEmgWczxN8qtFGT9On4fSvMWFqTp2kfTf2lSjU0PTPDfxW8Lx3k263eVTEdolQo3seRzV7QfiV8Mbe2udL8Xaktk+oHMMyud8ajPIA7fWvM7qfxb9mhh8ReDS9jMxZpWsXQgbjtIkXHOMZNcfcSabY6otwvhpsMw3GRXZivodxz0NY/wBlQjK6lf7iqme1ZRs42+89o/4Six8L+NoofDviaLXtE1K2WVply3lNkja2e+ADXVNfWurXYZGR9393Ga8q07xJ4T1DSntZofsbIMBFjEZBxn/P0qPQNY1C11obJ/Oh6xsD94Hjn9acsFJteQoZpGMHG59C3lrBY6akce3AXqo/z6V81+OJm8QfEzS9DW1W8I8xhC0u0bypI9M4C5xXq9x4qubq1ELTBUSP5j7V8v8AxM1i4jvNU1CGYpK8e+CRDtKbpQowRznYG/Nq9TC0b+6fNY/ELmUt9TjPireWc/iqWy0+9+1xWCiB7gMWEs2S0rAnqN7EZ9AK42jdn/8AXSf56160I8kVFHh1J+0m5PqLRSf560f561RAtFJ/nrR/nrQAtFJ/nrRQAtFFFABRRRQBLa3ElrcxXURw8UiyL9QcivRbW+tblmazYrDcfvod3UDOGXr2PFea1s6FqywKLG5bam4tDJ/zzY9fwOB+QrOpD2kbGlKp7OXMet6bpf8AaVstr5ix+f8AIWbtXbeGfDosb+HSLfxBNYoqD7y+Yu7+8BkYB/pxjpXlWjeIpN9lHIwUxyEyDI7dM+3/ANavTtWt9UvdIs9U0SYLdQED2ZWHGevQ1w1IuMeWR7uGrRlPnjrY9jk8HfF7T9PjutPvLDUbaZPleOTyWI9T0/nXOWfhz4pXmsR20lvEJi2f394WAXvkgnArh4fjZ8UNFs10u+0qOaOH92jpvTP45I/QVHp/xn8WTXiLb2qW8jkb95ZiCT6n29q5pUJN30t8j0p43D8loXT+Z1PxWs9d0nfBJ4Y8PKxwrXUbMzH1KqoUH6t698VheD7ForGNrrA8tSAW5DEZNT654juryCSa83ySMpZmZugwScd/09K5L/hN4dM0+O18wiQDf6989MZJOMe2T9a2jTfLyo8ipWip8zOm8SeJG0zRruG1kxcXG4LvzwoHPPvwPxryf42fDnx14D0jwrf+KNNNvaeKNKXW7Ft24vbPI6R7j/wEtj0kX1Fe2fspfBXVv2nPjLZeHZ1n/sK2xd6rIp2qLYMCwP8AvEqvrzXuv/BVaPRbr4l+DPhXo1rb29r4e8JOkcMKgCASybYkwOgAgBAruoU+U8vE1XUlc/MOipLq1uLO4ktbmMpLGxVlPY1HW5zhRRRQAUUUUAFFFFABRz/kVb0vTZdUvFtY22g/M7noqjqa7zTtJsdOTbZ26Z/56yLuc/j2/CtIU+YmUlE8/gsb66/497OeX/cjJ/lV6Hwvrs3WxMQ/6bME/QnNehESScPNIf8AeYmlWz4LEVoqBn7U4618FvndfXoA/uwrkn8TgD9a17bw7o8IwtgHP96Zyx/IYH6VuLbquW9KkjXcwUdCcCtI0oolzkzoZfghq978E7n44aPMZbbTvEH9h3dqsf8Aqg1uskc24DAAbKnPqtHhbxfcWejxRyxlzAv8XPAHp685xX3t/wAE6vBWg/FD4F/En4X+JrdZrDUtQVCvdHNumHHoQVB/CvkD4sfCPVPg/wCK9T8K+KNOaxuLCf5VKHY4BGHXBHysCSMcYJxzWOKoQbXMduEqVIXlT3MG4+K0d02ywso90pIRduScckEDvwO3cVUml1DWdJn1dltrbYQW804IyueD14bjA7g+hrhdImvIb77attbSJaycQhigYdMDHAzj6816Hoqx2WkOmoW223lcmLzMDarn5TjOdvHQeh9TXH7CCOmWMrVFaTOY1rVbuGxt45piftMSyqd33QN3bsSffvTPhl8OvGHxU8X2fhXw7pFzqGoajII7e3h+85Pdj0VF6sxwAO9ezfDj9mj4mfGDUImTTZNG0CWQOb7UYsFl5GY4iAzkqRjoOB81fpd+zP8As6/D/wCBumt/wjemFtTuYwt5qt1hri4Gc4zjCLnnauB0zk80NdInO/5panQ/sv8A7PvhH9lP4UuL24tn1WW3F5rmpcbNyrkxoTyI0GQPU5Y9cD8nfjV8Tm+Nnxu8ZfFDdIbTVL4xadv/AILOICOED0yq7vqxr7x/4KRftCSeFfhU/wAOfDOoGLUfEsv2GRo2G4QYzL+G3g/7wr8xNLZbGxEIyCq8YrqhT5Iq/UxbuzO8QaDpPilrhWhjS9gGVlB2lvY+v415tfeF7yHzDagyGInzIj99ce3f8K9Ce5lgZnWQ/OeapTySXF3HcbgrkEbgOTjH+NaezTMpSaPLzkcHqPaivV9Q8F6T4lh3xyi11E9JAvyyH/aA/mOa851rw/qnh+6a01K1eMj7rdVceoPespQcS1JMzqKKKgoKKKKAOx8LWXk6QbnbiS9mEYP+wp/xz+VdbGgVNuMelZ2n2q262Nn2hjz+OOf1zW197p1r0KcdEYT1ZFBCpbcwzipZNig7WPI5zT2XbnFVc9fm4rR6EEW/buA6GrOmxb5DMRlUqq/zV0nhfQ7zXdU0/QNPhklutQnSBFjUsRuYDOB6ZqYLmYj9Lf8Aglz4D1bw/wDDvV/FuoeYkfiLUzJbxsuP3cSBNw+rbh/wGvUv23Ph78B/iF4ZSHx18QvDPhPxRaRldOutQvoojIDz5Uik7ihPQjkE59QdvQ7HxB8P/h/onw4+HdkovrPT4rd7t1xHAdvzPgcFic49K/Nb9rf4P6x8N/jY0er61c6g3inTl1idppWcmUyPHIDk8glM/wDAuOKyx65V7TpsfScNZX/a2NjhVLlk9rGl4D/4J4fG7xp46l0f7DDpGjRqsza5JMJLSSB+VaEoczFhyAMY/iK19wfC/wDYM+EfwphgvLi1m8Sa1HsZ77UgCgdRgFIR8i4zxnJHrX5vfD/4z/Eb9nzxJD4o+G/iq7guUQJLp9xI0tncxg58uSInBX0Iww7EV+tn7OPx6uvj38OrHxZ4h8GzeGdRuF+aFpRLBNj+OJ+CAf7rAEdMnrXJheWV+VHdxNkWKyKsqdaSfobFn4R0+wIYQKAvtVHxN4mXSLR7ezKq205YnAUeprrtYWTLRxryelfK37c3jwfCr4M3kMMhGteLi+kWe1sGKNlzPKP91DtH+1Itd0KcW+aR8s2fnZ+0N8VLn4w/FS+17zGbStOkez0tc5DQqxzL16u2W+m0dq4OSZBEFVjtx0z2psdr5UajbkBePanCFpG2swBHy8mpl7zuSjMWPzGDMpI7Ut1bLFJCxVhztz7H/wDUoq07W9rIzXMygk/Kg5LY9AOTTJhfaoRFDbm3hyrGSblsBgeFHTOO5z7UWEySGSSPbtcjHStM3lnfWx0/WbWO5hYYO5c/5+tU3T5c56dAVPHSomk2+g7AdKGhHPeIvhfHIrX3habeD8xtZDz/AMBbv9D+dee3FtPaTPb3ULRSxnayMuCD9K9otbt4JN0MjKR2HepdX07QfFkKx6taBbnbhbiMbXHH6/jxWMqSexalbc8N/wA9KK6rXvh3r2jzf6HbyahbOfklgUk/RgOQf0orDlaKujr4tq3W7H8OR+NX4tv3jWdCd049doFaMe5OO9elE57iuQqHuaq7QpJ657VbuHXy/unNU23bcMcClKwhbePzrhIlwOea+7v+CZvwfsfGXi3XviNq1uJIdB8m1sdy5HmsSzEe4AX86+GbFCkL3LZyeEPvX7F/8E6fh5ceCf2e9Kvr63EVz4gkfUmyOSjnEef+AgVSfLFyKgrn0zDaxRqf3ScD0r82f+CntxZ23xX8OzQqBLD4ZBY9CN1zNj+Rr9M5xsU+pr8dP+CgXjqTxt+0D4xjhud1l4at7XRrfj7rRKWkB/7ayyj8K83FT5qZ+g+HL5M8VW1+WE3/AOSs4f8AZX+D2o/Gz4pW1qQzWVjKs907DOEB5/Gv2W8KeFdN8OaTb6fboBFBGI0XHQCviP8A4JVaTpP/AAg+ua5tje/vLhF3DqsYUMB/49X34qbvaumjFU6SXzPD4mx08fmNScnonZFJtPjVvMt2AA/gfp+HpX5H/t5fGD/hbnxwu9P02cv4f8HK2k2iA5WSUMftEo7HdINoPdY0Nfpb+098WrH4GfBvWfGU8g/tG5T+ztIizzJeSqwTA9FAZz7Ia/E66uJLu4kmmyzzOzMxOSSeTnPWtU+bU+ebRS8pfvLyp6K1J9nHLNwW6j1NWkVWXzGGwdB71Vt7yG4kkWOVm8pjG3bmqS7iuVmto4ZHmtoUyxy/GSSPfrS+YRn5QOemTkVOd3J+YsB+B/8ArVlQrNfX/wBpX5baDciLnHmPwC30GOPx7Yp2tsK9y821k3KFBxz71C1uuCvyjA3deuf/ANX6VbEbbCy59DhfcelNbYctt2ZA6gDpxSaAoLGVB+YYFLtZPT3x3q7HCrKrFiQf06/h2NMdYUYsy8Mdo+X3wP5ip5bCtcbDql1Cu1ZmXGR1/pRUMdok0rhQ5C9ccc/jRSsHKjIs2WSYN6KK1E/vHmsjSjuY/StePPG31rWBmFwW+RcZ3A5qk2ZbhIlGcnFXbp187jgKgqtpa+ffbhyFqXuB2HgnwjeeNvGnh3wLp8e6XVbyG3O3qAzYJ/AZP4V++nhPw7a+FfDel+HtPhWODT7WK3jVR0CKAP5V+Q3/AATz8FHxd+0lYarNCWt9AhkuiccB9pRf/Qifwr9meqp9KjEScYqJtCJzXj7xdpfw/wDBet+NtemSKx0PT57+Zm/uxoWx7k4wB6mvwJ8aeINT17TNW8Sa1cGbU/EF/Jd3Mh6vLIxdj+LMa/Q3/gq58d7rTNJ0P9n/AMP3QSTWlXVddKN832ZH/cQnHQM6s59o17Gvz8XR/wC1rbTYeDDFIZJPwNeViZaWP2DwxymriPrNSmvflDlX/bzSf4M+3/8AglTfy2+oeIfC+0+VDb28vtv5U/8AoP6V+lKxInzbRkV+ev8AwS38Ozf2l448QNG3kWzQWit2MjAuw+vzfrX2l8bPiXZ/CX4X+IvHl5Io/smxeWFW/wCWk5wsSf8AAnZR+NddJudOK8j4bjCjHDZ3iKMNou33JXPzl/4KTfGR/Hnxft/h7pOpeZpHgyIwzRq3yNqEmDKfcouxPYhx3NfHrYcldpIHt2+taOvaxfa7ql7rGpXJnvdSuJLm5lfrJI7FmY57kk1nRqx7/IBllzz+dd8Y2Vj5h6kk5VcL68AZrHvLF2mFxbN5UoPLLyGHvzWlIjcybwQOh/8Ar1DPI0UZn2lnYYQKeWJ6Ae9NoRSuDLcSJptu2f4piD9xc9iOhOMfmauxW8cMQjjhUKiYUL0Udhz2wP0p1rZNbwszSb5WP71myoLYwcE9hx+QqRTlVLjLjnH5nj171MV1Ab+7EY+X0z8wP696bLGrMYpEYEsFPyg47H+lTsqrHvxlclcjoOg6D2NVJpAW8zzM4/uj8P6VYDHYCEEMoH3s47HHb8/zqlNJ8xVVXJAQbe5zgdPfFTTT7dzNtx1B3c/55rOsWa4uDcSbQkPzAZ4Zj057f/XFRJgacNv9mjEI858dTGnfvyRRVWZmkxJGJASTll7/AJUVncDnPDs/nK6jqOtdFD8qkq1cx4d2pJIq/wB0E100S/KG64NaQd0ZEV2VVmJ67ak0RPLjluvRTVW6OWk7ZOKvW/7vSH2/Lvwv5mhfEPc/RP8A4JS+ElaLxH4xkjOZpVt0Yjsoyef+BCv0gubu3sLGW9u5ligt42lkkY4CKoJJJ7AAV8m/8E4fCK6D+z/pOqNHtfVN923vuY4/QCus/bw+KkPwz/Zh8YXEc5S+163/AOEfsVVtrGS6yjkH1WLzW/4DWGKfNL0OqhCU5Kmup+Svx3+KV18cPjh4q+JlxI7W+o37pYKx/wBXZx/u4FHp8iqT7k1T0NpGs1Vjx1xXIabDsUdAfp0rrNNfybct2VST+AzXkVtWf0v4ZUY4VTqdLWP1L/4Jx6Guk/AWTUli2y65rV3eM2OqoRCnPfiLP414/wD8FOvjI0t5o/wP0e6+SEJq2tlH53kMLeE/QFpCD/ejNfT/AMC/7N+CH7LOg634pItrbRfDq6nfY6/6rzCo9WJOAO5NfkP8VPiHrHxM8fa94/1o/wCm67eSXMkZbPlKcBIwf7qIFUeyivXowtp2P54zvGPH5lXxT+3OT+9nKyfO7Mc5JJ3dKYpVeN2cHjnqabnzl/dn5jwy5pN27K9AMj6f/WrpPJFLZYu2fT6VFZItxcm8dMJExWJRyM4wz5/MD2B9agupDNKlksgR5eWbusY4P59B789quLHHGnlwoiBBj5f7o4HHsMUAT+WPLCiRdjD5u4z37+oFRx7VVm8w7cH8fp+dQbnUnOBjJBXjIyMj9KYWO08Nhxg/NweMfnnFFwLMsvlqGVkI+bkH8P8ACqt1cDzC0jEAt8rKOM5B/rUU10zAS7mGSAWXr2PP61Rm1BY/n+TIVuSOvTGfyrOTAztc1DyUcnI3Drzz0q9psKwWdtBd74vOIkkbbwCccda5uJW1jXIrPkxqxZsH+Ef/AF8Ct/UJJJJCf3qquF+gGO1QmB0Fto0duuN0jofusikZorBtdZvIE8lZG9uecDiipsO5ynhyQm+dS3LJXYRviPGaKK1pfCYlW6O4sp9anlk26OnXc0mAM9eD/wDWoop3KR+637JOkNo/wI8Kaa0eww6dCpA9dozXxL/wVi+Ijal468J/CWzmJg0azbW71N3BnnJjiz7qkbn6S0UVyYmTUme1k0FPFR5j4ZtuFz6V1XhpZLy+sLOG3NxJd3lvbJEP+WjSSqoX8c4ooriSvJeqP3nIa08Lk+JnT3VOb/8AJWfev/BRz40x+G/h/wCHfgDo91tv7q3t9Q1pYmwI7dBiGE4/vOpfHpEv94V+dG9dxx8y54J7gf8A66KK9inpE/m9tsbt/wCWikqxHOO1DTxwxPJcNhYxlto/z60UVdxXILRTHG00yuJ5vnYhvu/3V/Dp+verDrkuw5JH3lXnHc8+2KKKLhcasjLE7vt5PylflJ7/ANDVVpljib5uQcYHfA/LtmiiokwuUpXXyxmUqTxn356/mKyNUul8o/MAdpP1+v40UVmwuVPCcWRe6kylsssKFSB0yT9e1aa7Wk2mNsFv4uQf88UUUo/CFy99jhLDy0LZX+Hj096KKKAuf//Z</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCADIAMcDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD4CW3PpT/IPpV5Yx6U9YfwoAzxb5pfs9aPkilFuD2oAz1tvWpY7bGOKvrb+gqeO29qAKcdr7VPHbduavR23tViO2HPFAFBbbtUy22McValaK1X5zz/AHVGT+VZtx4igt2x9nmI9cAf1qHUinZs1VOcldLQuC2p621Q2PiLTrtghkMLnoJht/XpW2tuDjuKpNPYzaa3Mz7KPT9KPsvtWutuKDbimIyPsvsaQ21a/wBnpPsw9KAMc2tRNaj0/Stprf2qNrUelAGI1r7Uz7NWw1v6VE1uPSgDK+zmk+y+w/KtTyB6UnkAdqAM37OaTyK0jCKYYBQBnm39s0VeaPFFIDMSP86kEfrVhYR6c09YT6UwK6w+9SLCO1WUh9anjh9BQBWjty1Wo7cVYjt/arSQUAV47f0FaWl6O2o3AiDCNAMvJjoP6mmrHXqHwz8DHWmRcHa3JPrXj5hi3h4KMPiZ9Fk2XLHVXKp8MTgZ/DcUcbCNMn+93NcnrWg7AxK4/CvtIfBuwhsWkkwHA6e1eBfE7w5DYXUiQKNi5HSvmYOrB3kz7utRoyhaK2PnLUrPyWIxkVa8P+KZ9ClWKfdPZd1zynuv+FWPEMJWZwwrnPIeaURqDuNfUYeo7Jn59jKSjJpHtNpJDeW8c8DrJFINysvepfJHpXL/AA9t73To5LS5RvIf54mPY9x/I/hXZ+WPSvTi7q54zVmVPJHpTfJFXfL9KTyqYii0GajaGr7R1Ey0wsZzwjniq7w4zkVoyRnrUDJmi5JR8sUjRirLR+lRstMZWZR0qMqKsMtRsmKQiFlopzUUwIFi9TUqx9sVIiVYjj4wKAIEhq1HD7VIkVTpHSAbHHtqdY6ckZqdYzSHYWztfOuI1PTOT+HNfTHwX0K6+zRSRRhd4yCxGa+dtLjka6HlYMu1toPrtOK7jXPFGgeEvhj51jd69f6tZ3C29xqFpKyWyXB6RAkgM+MnaOcZPQGvmMypupiIpPW2yPusjrrD4WTaVr7t27H1dqFhPHaMJLtYweMMa+YvjCthYtMJb6FHOfvMMmuq8K+IL1fhzcXeszXU9+wPlLK6lowCQQ3vkV5j8GtJg8d+PrqS/srO+utzus+sOwtreNQDubHTJOAcNz/CQSR4VGpKtUlF9D6vE/uaUZL7X9dDwHxJc27agUim83POdvFN8L2K3WtQjgjcM1sfFTULzV/EF/JP4fj07bdSRRG2YdFbAbGBwR0xVHw7bS2OsWLSHHmEK30r6uhZJJ/nf8j87xScpSa1Xo1+Z9FyeFI4fAuo3SWvm/ZlglEgXmMuQN2fTG4Vw4jrrPiJ8cNO+Gul3Phu4sprh9S0qJBPEF2xgShjuyRzgdq5WxuIr61huYWDwzIsiMDnKkAj+dey7bI8Gz3G+XxnFR7TV3ZTTHSEUmWoJFq9JHVZ1NAFORarutXJFqvIhoEVmXNRMtWCtRsKBFZlpjLU7LUbLjNUgK0i0Urr1opiHQr61bjX2qtAvbNXo1+UUmA9UqdIwKWOOrEcdSUMWPvVhExTkjqdIulAzS8Jx58QWXAI39+nSvqXw94RsNE8Jtd3fkWekXDiMwqi7rqRjwozwMk8k9K+XfD8iWmsWcj8IJBkiveNa8a2t5rXhqe6Zn0TSYiy2qjP2m5b5UXb37n6gV8ZnEaksVFQf2f1P0jhyVOOCnz/AM36I0PHNn4es/h/eXUGrWEce8qsEEok2jOPvLwcd8elfOvhHxH4YsdastNOqR6ha6jMbdL6xYh7Wdj8ozj5l7Ee/WvaW8E6FqfhrVW1nRdF0/TZd729nHM4MRbPUK2MEn7q8V842d/Z+AfEUMt3p9pc2UEvyy2uC0K57Z5HHevLwuX+zUr3bfy/r5Hu4zHOTg9El13t8u3qdT8SvAreEdRkS8zP/EkjfxD1ry/S4W1bxTaRQpuYSZwK9b+Mfjuy8SW8LwzpOqxgJIpzlMcfjXmvw4vLez1C71GRlzChC5/Wvey+jK/v9D5TOKtO1qezJP2ltFm1PXPDVraR+ZPcW0qF9pwQAm3n6hvzrqtJ01NL0u0s0GUt4liH0AArcFuNe0ax1ycW7HY8MKeWd65cHduz1+XHI79qrGOvqPM+Kl2IPLHpTHUelWNtNZRTM7FGRarOtXpFFV3joEUpFqs61dkWq0i9aAKbrUTLVlulV29aBETVG/SpWpjLhaYFcrRUmzNFUKwQJ3q9CtV4kxV2FOBUhYnjjzViOOmwpVqOP1pFBHHVhYz6UqRn0qaNemaAGtCWjIH3uo+vatjQtXtPG0/hzSpLySxm+3ETiM4ddqNkZ7HPAPvVBVrm9e8N3NrqCa9oxK6jAwkaBTgTY9PRsfnXHiMOq1pLdXPVwOMeFvF/C7X+R9B6tY/C/QbB4vEFncQXqDa26WdhKByCDkg8+lfOPjq40DxnrXkaL4cWzsVYqbg+Yvy565Y5J/xr1G3/AGqNH07w59l1XRZLi7ZfLcuBuT1yDz1rynxj8bLHVLdv7OsUhjZThVUDt614lOniI2XLqfdYrMsLWpuPNFR/wq/3nE/ELWrXTbxrazG2DYCoGfl7EVyPh3VrhpHBZhC3XnHXtVTUVudYumupgVU9PpXvn7Pf7NN/47mttV1e1lttBQh0hwVe69/ZPfqa9+EOSPmfnVetzyb6dD0Hw7oc9r+z5/wl90/kaTZ3cayySIfuOSocY/hDMgPu3tWZGUuIlljcSRuAyspyCD0Ir2r9orVJvC3wE13RvKit9PezNutuiAA5GFH0BwfwFfGfw0+JkWh6XZ6bqbE2+dkcvUxjP8q6Em0cinzPU9jaPiq7LViG5huk3wSxzJ/ejYMP0psi+1K5oVHXNVXWrr1Wkj70ybFORBiq8icVbkTFV5GoEU5FGDmqrYzVqQg5qq4w1AELU1qc1JQA3bRStmigCSJauw9qrxLVyOPgUAWolFXI19qrQLV2LrQA+NanVaRVpLzULTSrczXc6QRjux6/Qd/woKLaR8UtxeW1jGWnlWPjOO/5VxWoeOpryN106JoIOn2mQZY/7q/4/lWat3JqTRRvuUAbpNxyWI9a3jTb3E5H1x4q/Zdh+NnwZ8IfELRtEW+nbThaX9vbrsuD5DNEsq4xvyqAEcngYzzj421j4Q3GneJPsOn6VcXcjSCKGHaWZmJwFCgZJJ7da/Qm8+O2ufs2/sO+BrvRLKO41/VYd0E0q747OCaV3Fwy9+JY1APG5xnIBB+O9e/aw+I82h3k1/ru+aT/AFl4LCCGeY4ICeaiKxHPTOMGuWdOSk3B6HVGtHktOOq6nvX7P3/BP+4t44PEfxGtkN2xD2ug8FIB2abHDP8A7PQd8ngfV0fgm10O12QwLGiDhVGOK+V/2G/Gn7QHjy+Gt6hqkGseC7tiTZ6w3O0Hbutyq7owNpAB+Xg/Lk5r7a8aalYaFoGp397KtvFYWr3VwCRuVEBJOPwx9SK1SOST5nc/N/8Ab88eRx31r4Ls33TlVur8qeEB5jj+p+8f+A+tfFNvpcss21hwOlet/GDXLrxr4z1jX7zDXWoXDTFc/cBPyqPYAAD2FclB4bn1W1QpJLHESGZYcAyDnIDdq6OXoRYr+DIpoL6aCGeSK5HzgxOQcd8ke9enWXibWrIKs5jvEHH7wYb8x/hUPhvSdNs9PVbCCONFO1gv3t3fd3z9a1JINy9P0rT2aa1KWhZtfF1ncHE6vav/ALXK/mP8KvpdwXSkwypIP9ls1x97ZjccD9Kyb5jar8j+UQNxfP3R61nKkug+ZnezN8xqnK/vXneh/EGOC/C31/ss87F87kk+ua715N3IORXO1YOa5HI9VmbmnSNzVd5OakBzNRmojJSeYaAJGNFQs59aKANSNeOtW4enSq8eOKtx9KALcCirkcfeqcf3auwye1A0YXizxFPpMcdtZBftcvO5uQi+uPWuYt9Jl1Gf7VqEz3Mn96Q5x7Advwrc1m38/wAQOzDOEAFWVh+QKOntXbTikkyXqZckaq22IbVQYX6+tanhPwzdeINWttOsoZJrm9fyVWMZOO5/lVc2/OT1Y/yr6U/YH8NnWPj7JO8XmWmlaZIW3DIEjMoH9fyq56RuCPoj4qfAeTxl8N9R02WRYtC0jwYNPs4wcHz4oCVYjoAHVDyew9K/LDxh/wATLxNoegyRNbp5kayK2Oc4GeDX7f8AxyZdP+DPjaUDy9uh3rDHH/LB6/GHxFZbvjpoqjgfaIc8dgQT+lcdtGyrto/XT9mHwvaeEfhTpUEVusEUNrEgwuPmES7/APx/d+Oa8Z/bg8brp3g5NOhbF3rU3lDBwRbx4aT828se4zX1Hd26aH4X0/TbYbWaNUAA6nHJ/OvzY/aq8dR+NvipqaW8u/T9IX+zbcg8HyyfMb8ZC5Htirpq8iEfMHimP/SlCkksahs45LGGNIFZriZtkaj+Jj0/AfyzWnfQi8vjIxwF9a2fBelnULltVkTESZitVPT0aT8eg9s+tdXUOpr6PocekWEcY+baCXc9XY8lvxNMuLgSMUQbT71q6pJ5ceMgKBzXPNcqbr5GwMiqKG3UYyzO2Auc1wPja+VYfsazLBJMQ8jNzt9B/n1Ndzq2oK1wkBZQpUyvxn5VGSD9cAfjXjOuabealfTXcsgl3tklaznKyJZJBpDX0r2ZCHT7hRF5ow3lv/DJn2PX2r1+3t5bO1ignGJo0VHGf4gMGvELWW40ORZYZd2PvRsOGHoRXr+i+LLbxVpsNzF8lzGixXER6hgMA/QgD8jXLK1hLctSdDVOSTB5qaaTriqUj/NWRZJ5g+lHmCqu80hloAneXB4oqr5lFAHUpwKtQtx71Sjq3DQCNCGrkIqjb1cjP5UyzBuJBPq0zqSVXKn6jAq1FhR17VTs2Bvb2PjcruOD6tmtSCEGFj69K9COyMyG1gDS7iPlX5iT6Dk/pX3L/wAE2vBzx+G/E3imaMhtRuVgjYj+BBnj8WP5V8TS25TS7wqPnYCJfqxx/jX6p/sx+EV8DfA7w5ZquySWATMMc7n+Y/zqKz0SQHD/ALc/xQj8E/B240qJx/aPiK5XSoF7+SSDO2PTZ8v/AAMV+c+m+GX8QftJ+BrAISdQ1G3hPHZmCn9K9y/bU8fH4gftFWuh28nmab4bX7MAvKmb70rfXcdv/ABT/wBl3wjF4m/au8I30iho9Mt7q9YY7pEVQ/g0i/lXPtEu2h9r/Hvx8vw98Ja7rauq3NpbC1sVJ63Ug2offaMvj0U1+VWtTvIZWJ3PIxyW5J9TX1L+2N8TJPE3jaLw5bzH7BpG6W4CniS5cDOfXYuF9iXr5W1mRba3mupCdigkY5z7D1renGyuK2hzMlg+r6pDpUBwZPnuJF4McY6/ieg+vtXp2k6LdXUa2mkWE1y0SBRFbxlti8AZx0HIFafwl+DF/dR2mpazPBpFhqMglvtQllUm3iCuwRVySW2xuAvUnnGCM+ieP/HHgXwQsiapqOs+C9Ps0ht9MFjZETXCgOxa5cJh2csWB6gYHrjvp0lyOpUdo9/0NIw0ufOvjSS+0uWFLqLZDMzIkq8ruU4ZSezD0rFSYRQvKWHy+hruvHXi/QvGnw+1ZoL+71GLVHii0u9YrAEukyZJpwAAFwAOffGcc+AXPiC90+xlsr4eXdRfK6hge3UEdQa5anJGVou6M5LlOmttaWabW7tmJSGFLdee7tnj8ENctNN57ZW4y3VQxqrod8J9Au1Y/PNclj7hVGP5ms6S3ZlOxtvpzXO3oZhqGpeRJsu4FkX+9G2G/OtrwRqWjJrUQtb6S0uJf3bw3QwkgPYN0yDgjNcrNHdBiCglH+0M1oaFotpqF5FFqVk6RSHaJI3IKk96gD12XK7geCvBFU5G5qDTIbu002GC+YvdRgozn+PBIDfiAD+NOlasShjyYPWo2kqN2qBpKQyxuoqo0maKAO+jWrcfQcVVjNW4sEYoLSLVuauRNmqsKirceAKTGcn4Zc3V5cMfvzb3/wDHh/8AXrr4bM/Lkcd64nw/cJDr8IQ5jyyA565B/rXpEKjcoODzyDXpx2RCFis1EmlxEZE18iHP0Y1+qureJrf4c/CG712QL5Ok6W1wkbdCyp8i/i20fjX5b6pF9lt9OuwcfZ9Qidv905X+ZFfY37YXxA/sv9nPSdLik/ea3NEHX+9BEBIw/wC+zFWNb4gtqfDGg3dxrXi7U9Xu5GnuZpWeSR+SzE5Y/iSa+jP2TdYg8J+PPFfjG6YC28P+H55Cp/jeRlCL9SyAfiK+e/BsIj0+WYqAzsTXY6P4nbSfCPifT4OJNUlt7eZv+mcX73H/AH00f5Gsrczsa9DmfEmuXGua9eXdxMZrq6laWaRurSMSWP5k/nXA+Jdbe+16DT7FfOWz2ySgdGl/gX8Ov5Vf8ZeJovCej3eoy/NIo2xJ/ec9B+dYXw+0+S3s47m6+e9uG8+Vs8ljyfy4H4V1PexG+h2N/a+dokUF8PNkGZH3DI8wjkj3GcZ9BXnviq6vpTBNJq13eC23eRFeTtMkWeoVXJA/L0r0HXprcaWUA+diWLN1ryLxJGDGxByPalLaxLZha14q1O7t4LaW4HkW6eXFHEixgDGOQoGT7nk+tcZrmsTX11PPK4aWTG4qoUcAAAAcAAADA44q/qnyZ5/Wuaum659a5G2Rdvc6vwW32iLEjfKuePUmtmG12sWfjbwAa5bwbcBLnaTxurr7of6Q652g1cdhDY7iK3dgq7zUTa0kOoW0k4/dRyBmC9cVPDbr0H1JNczqySTXjog4zim9EB7PeXFtfaba3lndx3UZXy2KHlSPu7h64/lWTJLt5zXm/h+a70S/SRHYxN8sseeHX0rvbiTaxB7VhLe5SB5d1QPNzUUk3NV3mqRljzT60VT86igD1OM5q3DVKJqtRGg0L8LUapI0Wl3bocOIm2/XFMjJ+tZPjTVJLHR/KiBM1wfLGPTv/n3oWskI5OPUI7DULQJy0cysxz1wRXr0kgWRQHx+NeLwaatrbtPcHMmM/NXqei3Salp1ndIdwljDceuOf1zXpR0IiztLqNtU8M3MK/feH5R23AZH6in/ABI+NLfF3QvC1iG3DSNLjgmU9ROSS/5qsdRaJMzRtE3PcV5F4XsJND8deLtNlyUWUXEPujg4/lj8Kzq9GaPoemaDGYNChXcCX5/Wm7PJafDHDyeY2TxnAH8gKWFxDb2kSjO0DOK84+N3j0+F9D/s2ybGq6gNqheSkfQt9ew/+tUw0Tkxy0Rw/ijWj8RviHDp1qS+lac+WK/ddx1b8+Pzr1LS4AkwRBwq9q4r4S+Czomj/ariP/SJ8Mc9vavRrJUtlldh29KuN92Qu5k+J59tuUYnHJA6V5T4iuEhjyzEFlLAfUgD+v5V1/jzxJBZqRvGf1rxrW9ca+mJLHHp/n8aiciZFTVLwzyYB4rHuFyM1M827nNQyKzLyOK5yC34el8vUEHrXoMiiQJJ/eUV5hayfZ7mOTP3W5r0/TVkvrSPyl3E1cewF3TNPe4R5G4Ra47VdQEGoSeVgnOK7zxJcf2B4ZVBxNL8v+NcDo+kNeMZ5ASuc/Wql2Qxsd1cON7cCu1tdUGpWcMpGyVVCSD3Hf8AEYrNs9De7m3yJsgTk9qbp95HJeXcK8DqmPbg1nKOmojRkkqsze9DvUMjVkWP3+9FQE0UCPX4atR1ThbFWo2pM1Lsdcj458RR21zDaraSTyxfP5gICqSOnXmuoaUpC7DAKqTz0rznRbG61IyXl5NJNczEkspIRM9gOhrSmrsmWxi3+sPqIBnnWCE8hSCM16x8MZvtPhO1G5T5bOgZTkY3E/1rz3WdIktFH+mSIrAnbKFKn8MV1Xwe1dJdJ1C2Mg3Qz5+UAABgO31U12LciO56xpcqwXCyZyMYPpiuU8XWP9n/ABCsL4f6vULF7dm9WjYMv/jrN+VdBburKADkdjVTxrZvrWh2ksAze2N0kqDodp+Vx9CrH8qcleJuU9Y8SWnhvRbnU719sEKfi3oB7k8V4j4L0W++J3i6fxHqqs0Jf90h+6AOij2ArT8STXHxa8WR6LYSFfD2mN+/uB92R+hP8wPxNdfqvjLRvh7paadp6LNKi42pWfrsiHZ7nYf6LpVqXnkWKOMfxV5h4w+MtlZb4bEfaJcY+U/LXF6tqniHx5dMrNJFbk/cXIGKdZfD0QsFdcnuzUOTexHMzk9T1XUfEFy80pwOvtVe30G6uhuYhV9a7nVLGx0WLYWDv1KjmsGW4ur5sQxeVF2xWVu5BmrocFqu+aXOKzb5jMxESbY+gGOTWvd2v2dd1xNj2J5rHuL4FiIhgdqlgUZrcwr8x+b0r0PwLdXEenxPj7u5RnvjH+IrgmikYq0nTrzXpfg+3CeFYpT97zHf/wBlx+lEXZhEk1y5XVI41u0Zdh3AVc0m400RiKMc44AFWrM2c7YuApHvU1xqnhrRSB5sXnf3F5b8hXQMzfEGrrbWLRxDaW4ridOee2ulmXnB5HtWz4h1qzubrebe6IblV8oqP1rCk1y0jYB7GYJnvwaylqxHRyNyfSomaqtrqVpfRj7NK7bRysgww/x+tSs3HWsChxcHvRUO6ikB7IjZqzH9apRtVqN8Cg1INfult9LkVzjzj5I/Hr+maxLXWbXT4WJ3BQNsaoPmc4+6vufTvV/xfCs+hyOQcxOsg56c4J/Imun+COj6LqEcviJ4Fa4Vhb2pLB2XCjzGzjhi2VGOgHHUk4V8VHB0XUaO3BYOWOrqjF2OT8VeGdR1iMR2lhMk0XIM6+UHBz03Y/X1q/8ABv4QeK2m1QjS1eOYx7THcxMQV3ZBAb3FfR+k69o2j6S7a14Uj8sZMt9dEMrckjCngADH5VBD8Vfh3pszXdk0enXX9+zlCZPvzivnf7axVTWEV+J9r/q3g6TXtKkvwPLJYbnQ9Rl027UwXUP+shf7w9D7g+tcN8UfGEltZroVjcra317GTJM+793F3xgHDHoO3uK9S8YfETwd4tvvMvdUmeS3JEU2EEir6EqBkH3rmvDfh/wv4q8TXGo6Trsdvqltp7c6lFBNBtJx0kUjfluDhsEZ7V7FHNlKCVeLjL70eJislnGT+qzUo9NbP7jgPD9j9h8NQWumt5No6Al41O6QnqSe9VofCtpHM0s6mZ85+fmu50uPTofDdr/ZgX7II1ETdSVx1Pv/AI1j3catnBznsK+gS0PlWrGW15DYx7IYlRQMcVzmp6tcS5VGEe70rpLuNMYYc5rnryKGRiABmkyTDuPstvl5f3zZ53H3/wDrVk6n4ifaUtkWPt8ta99owu5Fw6omOrGqy+HbGBt09ypOex6VlqI5mPRpdQcPNKzFuxqydItdOj8yRtx7Ctq81SxsUK2672Axurj9U1CS7kIJwuelQ7CI7q6E0xIGF6Aeleh+B5RN4c8s9FkZf5H+teaxxjGTmu98B3A/syeHusu4/iB/hWchR3KB8K6prHiT+z3uWgtCpdZ+du3I/XkcV3ul+E7Twhp008Jt5ZlGWuHUs3HtVSGxmvrxX3tFaxLudgcc9hSaprF5NF9i0/TbiZB1mK4B/Ouin8N2WY114u0ua6aa+8p3C4G2Ft/t14Fc3qniGzvwBHAE/DFX9UsmUYvLZYpPwrnrqzEedihh6iok2SWtF8trmWRF24XH1ya12es3R4/LhZ8Y3cflV1nrEY/JoqLeaKQj2aI5arSUUUG4X0P2mxnhz9+NlH4iqfwa8S/2fos1qq4vLC4dngfdlgST3APXcOnaiivNzCClh3fpY9fKakqeLjy9Uz33/hei3MP2hdBOyMcxyfMv5EVxHij4/eBr7el/4U0WaU8Hz7VB698UUV4NHD05T2PssVjK1OndO5503xa+HEYuMeBtBcnO1lgGR+lctpPxh8H6frEX/FG2JsmlzMkdskjFO6qXBxk0UV7dPAUW3e/3s+Xq5viYqNuX/wABR2GjeI7fxFBqNzY6b/Y2mmbNpZ5/1ce0ce3OcD0rIvL5kkPoDiiivoYx5IqK6Hz1STnJyfUybrU92SxOO1c++p+YzH5doPc0UUmYsyNS1cTTBI2UgDGdwx2rPkbcOXXPX7woorIRTm25GCD9DVDyBMzMcYz60UUhMayheBXQeB5pF1xbRQStyNvtkcg/z/Oiii1xLc9ptY4tNsREQHcDJCjOTWJrmo3PlMI5Bap+tFFdXSxoeY61cr5rF7hpm9zWB5j3MgRGOGOKKK5GSdAGEKKijAAxUfmc0UVkAvmehooopgf/2Q==</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAQDAwMDAgQDAwMEBAQFBgoGBgUFBgwICQcKDgwPDg4MDQ0PERYTDxAVEQ0NExoTFRcYGRkZDxIbHRsYHRYYGRj/2wBDAQQEBAYFBgsGBgsYEA0QGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBgYGBj/wAARCADIAK8DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDxVBU6CmIKsIvFdh4w9Fqyie1Rxr7VaRKBMciVMq0IntUyr7VZIKtTItCpUqIAKCRAo60kjpGpZ3VFHdjgVj+JfElj4c00zXDr5jcJGWAJ968V1XxfqGs3jMZpNwJ+UthFGeO+AKiU1E2pUXUPeft1iGx9shzjP3x09atIySRh42V1PRlOQa8Bjv7e0tsPA8zNhjjOCMZ/n1r1HwDqIvrF1V2KFQwUnIU9CB/ntUxqKTsXVwzhHmOu200r7VOVNMIrU5iuy+1RlaskVGy0AVylROlWitMZaBmfJHVV0xWlIlU5E9qgpFFlqIrVplqBh81BQIOasRrmokFWo1oAlRatItRRr7VZjFUiCRBUqgjtSItShaZIoqpquq2mi6RNqF7IEijH4sewHuau4rzTx1c/2j4yt9LLkwWcayMg6GRs8n6KB/30aipLli2a0aftJqJjad4fv/G+ufb9dnk2ytuWEMcBc8D2xXvfgj4XeF7JUZdMiL8ZZlzXA+FVSKWKRVBKHJ+le/8AhB4DaxuepNfJ5jipydrn3mU4WnHVo6TSfh9oEijOmwc/7A5rP8SfBvSbq1mutGhj0zUCvyzwRjDEdA6/xD9fQivVdCt4WhWQoAB61uGG2kgJx1rmoudP34vU78RGnVThON0fEzLe2epXGk6vaG01C2OJIjkh17Ohx8yn1/A80N0r6B+K3ga31bR/7Ws4wt9ZAujKOXT+JD6jv9RXz+wzX1eAxf1mnzPdbnwOa4H6pW5Y/C9URGmkVIaaRXaeZciI9RTWX2qUim7aBlWRapyL7VoSL7VVkXFJlIoSLUBFXJVqsympLQxB6VbjU1XjHNW4xQJk6CrKCooxVhBVkMlQVIBTFGKlFAhMV5b4ug+yeP5pc/NcpG49gF2/0r0PX72XTfDN/fwrukgt3kUe4UkV4jb319f6rbyahdNLceVuwz7sDrj2xmuTFVElydz0svoOV6vRHfabrcOlIrMcs3AA716H4b+IHiSxja8t/BOp3tqOTJChP6DNeZaNow1y4AQjzVwEHqfavUvAHgrxhpXiSOfVtU1Oe0TcWhSSNYGB6ZRgSMccV8/VjTv7x9Vh/ay+C9j6B+GnxS0fxjoqC32Qz7wjxFvmQg8gjqOlX9a+Id5pF4mlaRob6xeM5Vo45QnljPGSePzNeA+GktdC/a3slsiRaahABIvCqzqMAgDA/THHHFej+L/hbqHiLxBHqNvfahabZtzPZTeW4IIPcHqB0xXNzJTUeh3+zk4O71PQ7PVdUvrG5i1qxW0Zoy6oG3YXByG7ZGPWvmKcf6TIBgfMenTrX0r4a8KzaStxJdXF5NbyjCwXcplCAjBALc4PuTXhPjq2a0+IGpQvt371ZtqhRuZFY8AYHJNerk00pzguuv8AX3nz3EVFunCpfbT7/wDhjmiMU0insR0ppr3z5MaabinUhoGQyCqsg5q09V370FIqSD1qFhViQZqu1QWiOMZ5q3EKqxA1bjBxTiJlmMVOgqKP7tToKoglUU8U0U4DtQJlXVohc6HewFd3mQOmPXKkV4DocNxHql1PcWx+ZQoZvvLjOQB1/H2r6K2+tcPrHgW0s7W81KxnkXBMogxkZPBGfTBPGK48VTlK0kenl+IjTUoSe5m+DdQSx8QIJeVDA/8A16+rdC8R6BJ4fa81SaMQwJubd7DPNfJWgWwutYhDIysFJb8MV6Fp9+mn+C9S1a/t7q4tLfZGsMSFi7PnrjsMfzrwMTR556H1mBxSpQfMacWvWev/ABy0fxdZtELadgsMKnmJQTjPuetfYC3tvYNFcsnmwy7C+3naCPvY9M4Br4R8K+EtC1vxlba1oOneIbRjIGjFlGXGe28Y6ZA7HvX1hp3jQeEvC2NY0bVGlCp5zvCzMF3YJIPRRkn0FRUw6TXKzsp1Z8jlKDtueo6jc29wIYLfHzsoyPQmvln4nRSQ/FrW0lGGMwfHoGRWA/Iivd/FGujwz4Ru9dtUjkeIBoUkztYsQFHH1zj2r5r1vWdQ8Q69c6zqkwkurltzsFwOmAAPQAAfhXpZTSnzSqPbY+c4hxFNxjRjvv8AmZ2M0wjBp5pjHNe4fLDSKaacaaaARC1QSVYcVA4zQUVX6VWcZq1J0qualloZFVuPpVSKrcfSiImWkFTpUKVOgqiSQU6kFLQSPU0l3JFFp0zSoHQqVKH+LPGKIo5ZWKxRO5AyQoJwPWnahoOrSRI01tJFCRlQRy2e9ZVaiijSnByZ53a2jW1xazorN5iK6lX9RyvPccj/APXXU+HNZvFjg04nFuLgM5cEZAzjORkn5v0pH8OXlnHJa3Ab7K7GSKZfvQOe30JqtaS3Hh6++16tZTeSeDd26blx6uO39a8CrLWzPqMLU5lpue1eFvh7Yab4mm1S0lWNJFLtFHuCq3PzKQeCfxr2W1tLWx0nzzH5iuAjSMS7NkY6HNeI+DvGloFRLSTz45Bw0eWIAwQoVuQR0HXqfavZoNRnn0eO2ihmihJBL3GMkfT/AD9awk6aWstPxPSjVqtWjHX52PJPiT4lee3t/C8LZjtm82Zgc7mxhF/BTk+7e1edGvQviH4Tlh0fSvH1pHjT9dTzWTnMUpz+jgbh757Yrz3BNfR4Xl9lFw2PjMdz+3l7Te42mMOaeRimtmug5BtNPSnU00ARPUD96neoH70FFVqrtVpqqt1qWUhsXaraVTi6VcjPFCBlpOlWFqCOr1pHZtNH9v1CGwt2cRmeb7oYgkD68U20tWJJvRBGCzBVBLHgAd67fw/8NtY1Zlmvx9htzzh/9Y3sB2/Gu88GeCNEhtVvtLMWptjP2qKRZcDPoOn5V6RaWSeSpRVAOOnBrlqYjpE6qeGvrIwvDfgfSNMsDaW1qq7lIYsu5pOxyxqtfeD4tR+H+m3DoPOltopNwHRtgzXd2+6Jinp2/wDrVkatb6raRpp+kapuWbKwWU8KyJEB1II2sFGe7HsPQVxyberO+MElY4DS/Bn2hj9qtFa2b5GDgYOOvPt1zXX6d4B0axZGayWa3I4YruBHoa6VbH7LI9tcBSeDuUYHArT0m4+yXBguY8279cjpmsZ0+Y2hocpqHwU0eGSPxL4Cihs5lG6bTchYZfdP7je33fp1rKOj6zrWqWvh6WKbT5NQ/dvcyAosMWPnKMeGcjIULnk56AmqPx5+IfiPwVptroHh/TnWLUd3m3UuVjkTkeTG/QOeTzjjGM5OPGLXxNZeMtIu5XuJ57q3QmW0vGLPEwB2sM9MHoR0rycUqaqJ29T7jI8prYzD87qqK1t1Z9galZaJLcS+Djp1u1jYWduqWjqGTyiHVBg+nlkfhXjPiz4C2F3dSXPhW+WxlOT9iuMtHn/Zbqo/A/hVn4MeKPEGrapNp/ixp/7ds9NisLn7Qf3kggkdkkbPOSJmU9yYye9emahdXx8QxWUenyfZjamcXwPy71YAxMO3BDA55wR2r28NiOaPPDY+FxmGSm4TPkPxF4R8Q+FbryNb0ya3UnCzY3Rv9GHH4dawjzxX3MiWup2bRXUKzRsMOjgMD+B4Nc3ffC3wTcCZn8M2P7wc+VF5ZP8Au7cbT7iu6OJXVHmzwbT91nxyRimtmu4+JvgR/AviiOCCZ7jTLxPPs536le6Nj+JePwIPeuHPFdMWmro45RcXZkL1C/SpnqBzTArsarN1qw1V260pFIjhNXI+lUITV2I/LSQ2XA6xxs7dFBJ+grB0rxFFa3F5pfjKxkudF1FgxePh7dhnZIh9s4x3Fa104XS7hj0ETfyqv4L17w18vhrx3aeZpsp2wXynD25PYnutYYi5rQ3Oq8JXXif4Y6lH4j8LXx8ReGmOZZbPLFE7iWL70bAfxYx719X+D/FGheNfD8Ws6HcJKrj5lB+YH3HYjFfPUfwhTwpd2+ueFvG11psE+Ps96B5sGCeAxBGPx4rtNI07WfDeqR6nqdjb6PeykH+3NJUvYXp4/wCPiIAbGP8AfAHXnOK896HpQPeILWN5FPUHq3PNT3+lmO4juLNlW4i5UHGHHdc/5wce+cKy8QiGK0uL+NYkuGVJCjB0Rz0ZWHVHxwfXg4PFdZflW05bpcnZ+opqzRoYrSxX8S3kAKtGSjoRgqw4IPuKseR5sY4BK4OD2/xrK1NrixYeIdNikuIcBb+1Qbi6DjzEHd1HYcsOOSFFbemz215bxXNjPHNazIHjkQ5DKeQQR160hlLxJoNh40+GOqeGtUgFy4gYxAjByORgnuD3r4a8L2LWvxQWK4Lssqy2rSrld6gsoLc85wDmv0A2m2uhNEvO7p6j/Jr428R+HW8OfGubSx8yR3bNEx7xsd6Z/wCAstedmEbWl8j7TgxuWInTvpa/4pfqfROuPE/xS+HXiyOPyzq2ny2k+AMtuhWVMnuQQ35mvQGiJ3FvpzXzbpXxGY6hofhTWZMXGka3BNp9w/8AHBKShiJ/2d5x7ZHYV9NgDbyCd3PFdeFqKabX9aHhZ1l1TA1vZVF3t5q+hjaNH9n1p7Zx8qnK9uD0rclT74+7g8jBx9ap/ZhHqUUyLknqfQVclkkTUwNvyOvX1NdS0PGPF/2htH834W2V8qhmsb8jJHKxuCMD2zsH5V8vtX3Vrkem6wt9od7bpd27p5LQONweVwCBjsVChs9sg18V+K9PttI8b6vpVmX+z2t5LBHv67VcgZ/KuzDTuuXsebjKdpc3cwmqCSpnPpVeQ11HIQOeKrMankPvVVzUSLRDC3Sr0RrMhbpV6JuKQ2O1WQpoN0R/d/qK5GRRJGC0e5X9egNdVqgEmiXC9iB0+oqPwbplpr9xceG55UiurpC1jMxwPOXkIT/tDj8qxrGtI7L4Zax8Q/DOktc6BFD4m8PP8txpEz7njHfCnoee3X0r3bwP4q0/VFkTwjPIjKP9M8K6rlJE9fKLdvbp9K8L+GOqWHhvxk2n6xdXWiX6sYZd33d3+0DxX0jLoOl62Le91PSYbxkAMOraY2JEP975eR+GRXBLU76bJ7mwtJtAvF0KOZtNlDJfaS4xNZsc5kiB6EHB29OAR7b3wp8UXeuaBceG9bkjfVbACN3TlLiMj5JV7kMPxHIIByKreSkKRzTam7TRDbFqCriZR6SDo61x0iSeD/jJpvieGVI7fUf9FuIIeYn+8wkiz0XJbch5ViuODxldxZ07o9Ctr+bQ/EkmnXDsY5GIGeB/npWgkCeGrptQtX26LcSb7mMdLR2OTKB2Uk/OOgJ3cfNnP+IFmIZrXVoMDeRlhz/ntW7oU0V3o6xSt50bKUZWXII6EEfjWi7Em88aHG7BY9+vFeLfGnwsg1HTvFkMfzp/o1xx1zyjfoR/3yK9I0K5Ol6tL4TuXZ1jjNxpssmSZLbIBjJPVoyVX3UpyTmrPizSk1vwhfaa6qWnhIQns45U/gwFZ16ftKbierkuOeBxlOt0vZ+j3/zPjrxHaRzR3Gqg4msNl2rDqfKcSY/8dr7at332qSqV2sob3ORkGviLXZXXw5riMdjCynBB7fu2619o6FL53hbTZD95rWJvveqCuPLXpI+q48j+8oy8n+hpptOONpqtfMFurWTPY/5/nTmlWGQLIGGRnIIx9Krapdw2tr9rlcJCkbkt6cf/AK69N7H5+VNLt0tJ3v7rJuJmZkUj5ju6n6nAHsAo7HPzf+0T4efT/H0Guw2DxwX0C+dMi/IZgWGCezbQv1x9a+lYLqGURXrpkHHkxjk49cetYvjzw4njD4e6tpssameaA/ZwCMJIvzJz/vAZq6E+VmOIp88LHw05qu5qxcRywTPDNG0ckbFXRhgqRwQRVRzXpnkEEh5qq55qeRvWqrHmoZaKsLVeiasyFquRN70DLk6mWyljHVlIH1rlQ7xsJYXZGBDK6nBVhyCDXURvXM3a+Tqdxbk4XdvXA9e1ZVS6Z7R4N8ReDPibHb6D8QY1s/EEQEdvqsZ2faAOgb1P1r1bRfhlr3he4V/C/jS/t06rHOBNA49xxjrXy54P/sm41yKx1eHCFvklTIYHtzX2H4Fa5g0eGG11Ga6t4xt8u4PzD8e9cM1qd1OR1+h6prGVsvEUUazdFmt8tG/uQeRWl4h8Haf4g8Mz2wREk4nikjAUCVeVb2PYkdQSDTrKJZWV2Rcj0/wrdtvkbypF2xtxg4qOW50RZzWp3Eep/BuG+X948cSvn3Apnhe5jPhq3uGbO4DLHIGcDioEkax8B6l4fjiZ/LaWCIk9AGKrn61S02aK30e209ZMMiAFd3UjFTzFWNrxa0raTDqmmor6ppb/AGy1UHmTavzxZ9HQsvsSD2Fb9hq1nrWg2er2UvnWt1Ek8Min7ysMj6df51yM909vZ+aXy6H17Dt+VR+CGFhJfaAFP2cH7fZLnhY5WbzEB/2ZVc+wkUU+bUdj58+LenHStf8AF9vGMI8E0qAdNrxlgB7fNj8K+ttKTyPDdjETysEa9P8AZAr52/aC0p5dZhltxj+0LZIGI7lZdpA/7+IK+i4GCW8CEkDaD+nrXLhYckprzPquIsX9Zw2Dm9+X8Vo/yCedpJnG1uGAz04rnvHAu7zwY1rYkoz3MCyljyIi434/Dj8a37hv+WhB2nrj0xXH+PfEVvovgW61WSd4lRo13BQxz5qADGRnrXXLZnya3LUGoahealHbExxSbeUi6Qp0Bb3OOldhaRxi3FtgFI15B5//AF15j4P8RWE8e+3kU+chlLufnduxJNdhpmtWFzZPHFdpNJuO9I23MD7+lTTkDPG/2g/h5YDTW8a6BabJo5MaksQ+V1PAkx6g4BPfOexr5rkNfoHc/YtR0yaxmtBJbXCGOSKQZV1IwQRz1zXxT8UPBT+BPHk2lRyebZyr9otJOf8AVkkbSfVSCPyPevSw9W65WeZiaXK+ZbHDyH3qs7VNIearMea2OdFCFvlFXEas2FuMVcR8UkMvI9ZOtwjctwqZzwT/ALQ6VdWTHemXhEunyq3ZSw+o5pTV0VB2ZhpMWVJ0J3A54POa+pvgZ41N9pf2DU1y0X3ZT+WM18orlWJU/Ia9W+CuuyWnihrNZmXd8wXswHUVwzOyOh9uWbeZh7aXKHHB71uwNHgIxUHHr3rjtHHm6WLq05k7gdD+FadlrdtZyMuoWzWpzhZcZyfQe9ZHTE8o+K+u+J9L+LAsLaXytLu7WOZHwMq+WRuOv8OfyrS05GGnJm7aaTALSFQuT7DtXR/EnSNL1HwXdavrCxw6tFbPJYSLGSyeWC4ViB0bkHtz7Vw3h7XZr/w3BdS2PlZUZJ/mK8zFSqQnvoe/gKdGrS21Rv373FzpZt4nCvxh2ycH86u6ReXVvJpdwYke4shJEzhj+9jcDcvt8yo2eehHesT+1IW6NtPoDV+z1KLaNq9PfvXLHEVL25jpng6P8o660m4+I3xNs/CfiTZpsKR/2npl1Z/MX8mWIyQyhuucIQVI4B4r2a50O/t4QYVW4C8bUIVsfjx+teZ+Cry31T9oLTIIZFeTT9Gup5sdULyQooP1+b8q92r18HHmi29zycdN3jT6RWi7Xdzh3so54wTclRypUDBBBP8A9ftXMeKfhj4d8W6P/ZetSalJamVZ/LjuPLyynKnKgHg4OM4yK7rXYktNQimBCpdtsI6fvAM8e5UH/vmqiSMvyMfoPUdj/n0rdpbM4E7ao4/RvhX4K0L57HTppGySPtFzJIOTn7pbA/KtYeGdKimcpbGJDyRDI8Yz6kKcE++K1DMvl4/iHp/n/P41VubwNbOBlT0qeVLoDberI0tLeOPyo920cDMhYj8Tz+tcd8S/AWneNvBtxp0yK2owRtLYXJHzI4Gduf7pxgg/XqBjpJr1owJgcgfe/wAf8/0oe586IT27q3oQffpVRdndETipKzPz3lJBIIwRUDGut+JmixeHviprWl26hYFuDLEo6KjgOFH0DY/CuQJr007q55LVnYyYX461ZV6zoX96tK/FIbRa8z3pfO4qoZMd6aJRmgEjKspxJvikJMqNtceh64/Ij9a1dE1aXQ/E1rqCEgRSBseo7j8q5PTPMh1C4ErDzLh2LMTwpBwD+JOK0XuDJGwkG2SM4YdMH/64riZ28up+ifhHXdPufCttrdvdxfZZYgxOQQDjpU1trLal4kt9U1BGSyjkAijxwq/3z6k/pXxT8MfEviu13QaRqZa2V/ntJuV+o9K+m/DHia61LTVt9RgjglX+6c/kOv8AkVg9DZHrmoSafqmqfaZJ1kgijKLEDnIb7xbHr0x6VfsIdN1jS/sN7ZQzW6rtXK/cA4AB659815tFLL5gPlzNGD/q04Lexrp4rvWZLfbcPHYWigYij+8R6E0tH0NYya1Rh+JPhrHpm6/0i882DzEVoJ2+dN7hRg9+WHv9ap6v8LvFslntsL7SY2ORvaeQBffATNdtBdwz+Sz/APHpEwZd3Jmk7H/dB5+uPSpG1+Bw0cRMjkgFuufXArm+pUW72O1ZjXStc+ao38U/BzWbzUfFVpqVlcXUg36/Zubq2kUfcQlQHQD0K9+vp6v4S/aIubm3DG+sdYt1xulgcOV/3tvI/GvQ7qG11K1kt9SgS4ikXDRSDII+hr5++I/7OOjais2teBg+jaimWCwMYxnBztI5U/Sj2LhrTZg6ntHee56148+JMeteDNM8RaZBLEuiavbXl0ytuRoW3Qvg/SXnNd69wrQqwfA9Qa/OPU/HXjrwR4fvfCfieK62XZ+zT3yXUiSEKwJWTBIcYweRnDA19v8AgvxD9v8AhT4evriQGWTTrdpSWBO4xjPPfmtacpNvmJnFJHZmbHzBx9M/596zLq7C+YoOOMjnpXP3vi2wifYk0e8nGN4w3QGsS78VBpCUuIxjjCt2B55rUxudNPqP2cEygyQkHd/sjsawj4ng0TVIUMwbT7pthBPMbHvj0zmubvfG9np0LPeXcKQ85aZgox2rzDxd498K6pGUttQMkqkODaAttYc8HoOfU1Si29DOU7I5741yiX416s4YEEQ8j/rkleeM2K0te1i417xBcardE+ZLtHPXCqFH6AVlE16UVZJHmSd22YMLVZDcVRharIYYoKJGaoGlIpXaqsjc0DRn7FuNYz0Uybjn0X/6+6q9rqtvqkr7gFuI/lYdnHY1PeXKWlndzAfdQoOe54/xribVpEuPOjJVgc8f56VwydjvjG57d8MCB4oVScK/DAE4NfWWhpa2McZaAZIzu4yM18NeFdfuLHVIb20lSOdD88THGfpmve4fjlcwQRtaaMkrhAN7sGXOPT/69YSZoos+n7DUYnG2wjMjKPT7v+H1rI1/xHpmnMY9S1FZmUAtaxHIPsx7D+deFWXxF8b+Kx9mk17T9FtSOfs+A3pgAdD+NdZoOjeEbWZZ7zWjqMvUtM+ct64pDudvB4jvNabCsbeEnBYDACnsorrtLnt7ZGEFtI20czS9z61zdnrOkW8aizSBRggcjnt/n6VZfWEmXyptTjijPVUAyfp/n+dO4HWrezzuWH8RPQ/yqxNcvHanzG6dh1rk7XWtOEYWLUhEQMbu5P4ipP7QtJlxHfmTOfvckk+p/KgZ8vfH/T4bnx/JoW+Lz7yKC5tk5JaTzGjfA/2kwf8AtmK9i0zxXpUHg7T7WGOP7PFGltG8jYQkKBjJwOMHjPY/SvE/2j9Ovte+MEbabCxFrpsUckik8Sbmfj8GFef6PZ6pY3Hl6nJK7GLq7E5bPJ5qVQdR25rDlWUI3tc+htX8ceHYLL7Y9zZtKclLGy+dlxxgsBgZ5Jy3fFea6t481q+dktHWxtz0WPl8e7H/AArmDTSa9Gnh4wVtzzKmIlN32I7yJNQm82+aW5fsZZGbH0BPFKAFUKowBwBQzVGTW6ilsYuTe7FY80wmgmmk0xHNxNipw1FFSajWfvVaV/eiigDA12ZxZxwJjMhLt/SsiCNo4cELyR1FFFefLc9COiI5cq3Yf0pYLm8tjm3upoc/882K5/KiipNEacHifXbb54753x2YBs/1rdtPiRqtswE8AkUHrG5X8cHP86KKmxa1Oo074tWhkxqD38IP8S8ge/ynmu/0bxZ4V1La0XxBtbd3wNl2Xj/A7x6UUUrCcUX9N8brY3l5GtxDqVtC+37TBco4VSQA/BI28gk4xg9iK9AsvHEcl5FBBaTGR4/MWFWyCpyAenPIIJ5HTpRRXJNPm0bNoWa2O8XwTbNHJd6nGJLu5Adyw/ixgr/n0ryb4q+E7fTtJOpwoEZZAMAYLDOCaKK9Clo0cFbZnj+8etNZ/SiivSPOIy1NJoooAaWxUbPRRSGj/9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAUEBAQEAwUEBAQGBQUGCA0ICAcHCBALDAkNExAUExIQEhIUFx0ZFBYcFhISGiMaHB4fISEhFBkkJyQgJh0gISD/2wBDAQUGBggHCA8ICA8gFRIVICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICD/wAARCADIAIwDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDyiBOKuIlNijwBVyOOtDlYxY6lEZNTKntU6xj0oEQLF7VMsftU6x1MsfFAFXyT6U5Ifaryxe1P8qi4FQQ+1Hk+1W/LOaClAFIxe1NMdXShpjR+1MCkY/aozHV3yzTWTigRQZMVCy1edeahZKBWKTJxUJXmrrrxUBUZoBDY15q3GlSpDz0qdIag0GItTqlPWL2qzHD7UARxx+1WVj9qnjg4qdYxQIrCPjpRjFS3U8FnaSXFw4SONSxJrzPXte1rWf3OlpLZ2h6MOHkHr7CplJR3NIU5T2R6C1zbK5jaaMMBkqWGRSiSNhlWBHqDXh82jXKhm8uV26sduST/ADrPWa8tH3QTzK6n5drsMcfWpVRPY1dCS3PoA00ivM/Dfj26WYWuqoZoj0lU5Zfw7ivT4WjnhWWJw6MMgjvV3uZOHKRbeKiZaulKiZaq5nYoulQOtXZFqu61Qiky1Cw5q24wDVVvvUAaccdW0iojXmrka1BRGkNWkip8aVZSOgCJUx2p+2pvLp6x8UhnKLZ/8JF4tks7oE6dp+0tHniWQjPPsBXVahoMEkO6G2RNq4GB0FZ2jRCz1Odn48+dnbPUnOB+gFejslt/ZbyM6IqrkljwBXzdeq6tWUb7H22Dw0adGErbniGoaesMpDLiuT1HSYZXMUkJeZvuOhwRXtV54O8Qam4m0/RLiWFuVkkKxKwPpvIz+FYUfgLVl1J3vLe3WNB977XEMHGeMtycVVB1YSSadiMXGhNNqSufOM0clnqL2s2YZ4SRhx2969P8A6tMQdNnZpEkJMbE5KHGSD7Ecj6Gq3jrwDrclzcXscmnXEMK7zK15DG4H0LjP4Vzfg2+vdHja+mspfs+xmgeRSE3KCSm7HpnHpz6V7kWfNyV7xPb9tROtV9G1qz1ywW7s2OOjIeqH0/+vV1xWxwtWKTrVaRavuKqy00SZ8g61WPWrklVWHJp3Cx0Ea81bjSq0Zq3GcVIywi81YUVApJqdaLlWJVWq2oNdx2x+xczkgRp5ed3rls4Xj1HNW1ahxvXHQg5B9DWVRSlFqLszSnaMk5K5xoZrW6vtY1rRWlhtmRJbgXAXYzAlQoGN3Cnp34rSu9Wv9R0CWzihlYxXBhDNwHJ5VSOvbvxkitZNNaaW4unhZdoBLFwEIA7+tZWs3vhRNN0+Gy1KeWW5LOwt42dixySTj/9QFfL4qcZySpp3TPtsDSnCn78tGl+RY+3+JI/B8yx6n5c8bosViEY+Yn8TbscY7Lx/Q8NqNneSas0rL5USl0hjVdvHmuQSPoRXpPhbVLjVpLqDVY5beOPC290qCNm453Ajn69OelYeux2sGtxN5hkUOAST/kVrLEymowasKODUZSqXN3xd4TOvfCq4uChl1C1tUnRCcBihBP/AI7n9K8CWaL/AIRe71S4LAPA8Do7ZPmAjbj2+bH04719M6tqMdx4Qv7JZhClzps0QY/w5jbn8K+WvFbQ2fhDT7SGAw3Ex/eqTjCpjBx6sxOf9wV7ElzyhY8NP2cZ3Or+E8J+zX1wp+SRUDLu+6wz29Dwa9NYcVxHwz0e4s9C/tC4yv2obo0I5C+p+td1IOK7o7Hi1LOWhTk6GqUnU1cm71RkPWquZlWTpVRvvGrErdaps3zUBY6KLNWo81DGuKtxikaE0ZNWFJIqNE4qdRSAcuamUZpoFTqvFAypcPexkpCpMUmOR6jtWPD4iuLZZY7XwzczFCVMu0YB789q6ljN9laGN8AsH2noSM/0JqrZ2ejzGZr64kiDks0SyFQG79K+dxFONGq5SWj2/U+7yfF0qlLlqq7irW29GcNZa7rWoa7Ci2KWcTZ3Eybiw+mP1p3iVo4ZIz5oZyQTj1q5ruqaHofm/YmUuemDk1wV5d3F7ILu6JUMfkTviuZJTaaVkbVqiTduvQ67+37HU9UtNJ1G7jt9MiUC5Z22iVe6Z9CODWf4j8H2nifxzbXMMMo8PtYw4ZlCM5VQuPY5U5NYVhJZ2t/HK1stzPuBjjfkE9ifavf72KO/0SyvbZBJJBBuuBEuRGOOTjoSSfrmvZw2suZvb9bf5Hy+O0W25ykFrFa2sdvCmyKJQiqOwHApsg4p1rqWnaiHNhew3Gw4YRuCVPv6UTDGa9K54rVtyhMOtZ8ver0rcms+dqBWKM55OKpseanmbrVFm+Y80Admi9KuRLVGJulXI2oGXU6VOq5qqrcc8U+1aS8vo47a4VIo2zM7KSOP4QfWpk2ldK5St1L0cbtJsVGLegFNmuFtm2yQzFvRYmNM17WtWa9tIdI1oW4XJnxGhBHGOMcd6kHjm+0aLyZmtrxjyd67X/T17DFefVx9OEvZp+96XO2lhKlT3oq6Mm68TGEFbfTpZpQwXZnHXp68+1V9Z03Ub6I3E1usLhRlY3II7DLevIrXt/GS6/FIreGJUmicN5gCsoZSCcE4J6dhXaEWssLLJEJre4j2Oo6lTg5B7EYBH0rgxuIkrQvdM9nL6EVGVRK0k7Hzje2a2k5MljcPNnjerMfwqS28Oatfg3uoEaVZLz5lzwx/3U6/nivaLnwvDDcYttVuZIDyuF2so9CCDz9CRViPw/oFugmaKa6uR0aTLHP1Y/L+A/KuT28UvM9b2PNqk7Hj1p4amuZzFpMDxQjBku7j77+/sP8AIBr0vSre803Rl02G4lMO4SSs3WRwDg/QZPH4/Tdg0/ewWG32rnPlxjgf59TWdr8HiZUNroulkysDulZ0yn0BPX3P/wCrKE61Z2prQVWnh6f8Vq/Y5rVodItdSS92RQ6gDl3iADMMfxdunrzWFN4s04XsNslyJlbAaTaVC578Z9ulbumfDPWZhJdatdQxSMdxV5d2c9yRnP8Ah9a0tP8AAfheO7klvtXhFyOqrtRgOxyT6+1fR4XDzhdykfMY+vGq0oK9v67mJdRFIRMskcsZGQ0bhv5VjzOGXKnI9RW34o8NaHp9hc6hYa9u8pARCGDhicDGQeM/jXEW0+l3losbRCKTOWdThs+o7dv17jBHVGT5uWSsed7KXLzrYtzd6oO3zGtKaLzLW5liX5Ldx3z8h6fkePxHWsd3+Y1RLi4ncRtVuN6px9quRLuqhFlphDazXBTf5aEhT0LdFz7ZIrJu7/xNqdpDpGhxwRLJxIsUYGB13Fyfl+tdhoaaAdM1WfXEWWC12FlLEBMg/Mcen+Nbvh/w34fuBJdaJcFRLgq0Unmx5H1zz+Nc8lPnUr2itz0KU8OsPOEoXqPZ9jzu38D6zp+nSR32owuxIfKF+/ck8nnoMZOScVwt3cTWWpNbvayI8b/vA3OBnnp/PNe9ar4f1yaTnVbZ4lyViwUz/M5Pckk+lM/4RfULeM/ZdFhneUKZJ0Kgvjp74Hp7VzxhGpUfuWXfuyvrtehRUFLbsv1OHs7i7s/s2pmRIYYmDKr/ACKV9OcY4rcg8d6WdTFpaQvcljl44Bnyz/s8YOT2BqTxNHDHpFxp95pMqiZCgEkRPzEYB47j+f51zHg3whLDONQ0y5maWLO93YCPpyvQ5J/ED3rycR9XwVGSry03XS3zOnCVq1WtGpBevmeh32taXYvs1CcWjGPziJvlwnck9OMc+lYP/CfaG2oiws7e4u5s8tt8uMD1LHnH4GvM/GF43ijxHZpqGoRmKFZEuzF8qLGrjKA8/eYepJA47Cui0m4082bXCWssbH5QZE2hgM7SO3THHbOPelgMNCUIyxK1trrpfp6ndjswrQvTpafnY7DUPHd1hrTR7KGFsY3v8+DnGTjGa5I+LfGXmkzXyI7nHlwRD+Zzn/PvjC1fVNQhklt7K2EHnHPmxnk+uMdOtWNL1S4ZwbmFXmJwPK5zn+vX1zkdfm3e9NQhFKm0o9f+AeHRpVa0m5JtmxrN3rV7pLDVtRnQNwqpJtyx6DjHPI6jpjuygc9ahtMtTDHIfLPO3OefX61dbSdY8R6zG2pT4sIsFRC2MDrhck889TnOc5Ocm34mbSNL0eeNbYCRIyqs7sWJxjJOc9Tzj1U9qt024xdGWm514etRpqca8Lt6HFeM4biOw0+6hkEkN2WZW7rgkHP4qf8Avk9e2HFa219apGmpCO5LDcu4AsfQH3pfEGv/APCQ3dlpWmy/ZdMsYVt47mTO6bA5b2ycnPcnPYY0bfwZoqWDyXcmPLBLO74Jxnv68dO2Kr3pNM5VOEISS1uadjZ33h/Q5/PuPtlpqbCOKUeoIbn0PBrOZ/mNb/hzR4ZvDmp29lcSTWiRm6iR+fLdTg4z6qWrmGb5jzSi+bU5p6WR6VGnNWJriGytJLmdtsca7mNVo5R61na5aSanFb2YZhBv8yYKfvKOg/P+VVKSguaWxEYuTsi9outWzaTeWWobS+pTFijNjKBe/HAxx+eOa35vE1hpOnrDazFZgAqxw5jCj0OPujP8I+Y96wv+EbN0yTW5+yQRRpjYrMzsGPI7E9B0P4YycnWNJvcKbGIDMuxs/wDLPIJ6468HNeXTxkajVOO/XyPZq0qPtJVZ3tpZd9DqrXV9Ul3alea7cgEFUhDZBPTcc56f3fb8K1U8daxZWX7zUVcEZwY1XH4gCuW0HSriCxWOYrKBnaRwFBPT/OP0qgND1nWtZlaRYY4baTG5QSp54IXOST/nocddXCzqRjabVvxPMVXmqSfLo+nY6fT/AIga6UK3Vta3LngMI2Q/jz+nHHXAqzb69q19cnS9K0Owk1K8QnZHI0aKn/PSQ91GRx1bPHHJwNbUabYu9rZQKVBOwtkYz29ecA5OGbuQK1NF0PUtBjeefV3XUdRKpI8ZCZbnCKcZ4OfxySCdwXSWHjNWl7z+Wh2qtyfCuVfPUuaL8I5/tLNeS6e0jEuccAsT2AXAA7AcDt6nqLj4bR7o2kvoocdQik7u/Tj/ACaig0zXbbS2kGvXklxjIMsxy3sORiucmjvrwC2vtWnVp9yoDcFWJA/h5zn8CfY9KxxFRUmqE43T2ZEYupeqnZo17r4breSLGmreWo4UG3J/H73+fzB0LD4aabpsRa6vmkdh/DF8zfiSQPy+ued3OWsmp6fKILXULrA9bhunPJy3se/Y88F1drTX2rQJY6jeTNCzD5fNKnI+uOeDxgdMYGMR81aOGhKNFvfobxrYidPyR2tnpGi28TRb51kQk7iwOcknrjrz36kDJOTXkHj6zg1Txfp2j2w+0wBzPcxuMqqJ3btjOFGcHsciodchu9G0KXUdLupraKE7XSN2AxnG7rnrxk8jOD2qr4C0/UbnwrrHjnUkNxczqbW1kcD5I920t+JJ5/2a653j+7jp0RKpwcFU5rvqiN/Bui6bpskqSS3UrnMcjtjysYAVQOnX6jI9DnBurHTmtpIpAQGztxnK8YyPy/IY6qK3bK7vWtxDNb77OV2be4GV3yH7o/i4J49yP4qwvEuq21rYtI1tLMZMkMuCEY46tnP+OM9RluavCM3GKn76/EiLcU3y+6zZ+HqyWV9LbyzebHKGRo154YMMj1z/AJ7446X5JnQn7pxVvwPrRPiCynjbOZlSRGGDgn/P5fWmeIY0tvEd/DGMIJm2/TNd6lJ6S3OSrCMWpQ2Z3CuAhZmCqOST0ArS8I6ppviK7lhZcw28mVRzjem3Ocd87WPoOM1RghjmUwyMoMx8pd2Mc8Z5/wA81btdDsNKmxpwzAsaRlj1dsgE++Rnp/hWFerC0lKN+Wx04PDSq1Ix5uXmud7rOn3l5OP7MEIKweXIFYKV5OMk84Pzc4GcHgDFc2vhPXL4+SktoqpwqrI3Q4/2fX+lY48SR+HzdNaQJLLdrEGLudoPzNnA653f55xv+H/GN604jZbQS4y5CNg9jj5s4z+fQVnSdGteKVnIdfDVaE7Sd0ib/hG/EGl2BjFuLjacqscik+vdh7fkfapoE12wsg0OjXDzMucFWbbkYIzzn09+gwOt/UfFlxHPA0NjE4cHzMEr078Z98n2Ptm9p/iy4nn8ptI8mIcu4lOU9Bgryx9P/wBdbyqclqN9TejQlyuu17pxj2M+oataprYnsAr/AGtzJuRpBGRhVYoMDJUZHAHT3y7mxutX8S7V1JmhhYbLndtCAHAKpgY6cAY6dsca8Nv4j8aXbeJbdESwlUxWSCcZ8sNgsScfeIz24x6Ctzw/4d1dPPSe3ZWVzjEyHeMdRjt2/wAM8cVTEzw8H7KN7HdWw1OpGM6s0m7aLoXr6eT7ALZb8vNtx5/y5Y/3sDj3x9PWvHtSg8Qw6/8Avrx3ntm/dy7xgAjqB7j0r2v+ybmO7HmW8qq3G7qB064/+t07YBHEeJLX7dqlwiRyjyyIwZoygPH8O4dMk9MfQdK6PrjnSVRR18+hy4bBQq1vZzlZb+pmaXf3aRqbkP5wHzOyMATg85APcD8s/wAKYwvEGsasbhbj7VDFNaENFb8oDxg5DL83HBHTHFdlpHh23022NxdyLNOw3bVyQnGex5P+Rz8y85r11ax6gGWNWuZMR71LKQDnH8WBx0OB0GOBiufD4WMKjqtammOq0nFU6N9N/M4/xR42+36YmkWMbx3V6RF5B+8Hb5cfr1PUcHOAa+iLfRbXw98ObPS5dohghVZC4GMKMtnP+6fy7YynynoOnCP44aTHdAvE1yJEO0evHHb/ABr6L+KOq3g8MQWsO6K1kZll29W+U4Bx2zj24HoAPSjZ2c3qeUoTs3FOxzuvaWzQ29hYJwiKi44AAX8ePmHrnPfI8zlNe8Oi106SO4n812X5iOg457+vr/48eB1FmuqpEzXJDwZHljPzgBVz7YwTjPc9gTnkPHmuaxZaa8cNmiwu2xrhXJKErg4GBj0B9sH0HLhsLCEU5Pml3NcRVk7xtZGH4YsrO11y1t9g3+YuZDwcjk//AKqz9cmeTXr1m5PnPz6/MaueF9SXUdatZGTDoCG+u3k1Q1yVW1u5ZcFS5I/E1tGV5NPocktIrsddZ/2teXS3pj8qFGxGskm1gBuG/HA2hhjnPPGOw9OtfCz32mT2Tam1resgke3dN8keVIDMigsBz/GFzjtWHJrWjeGlnluZf+J48qx2thaqJZrbgBZHzlY3HCrvPyYLbWOAL8N9t0/7OALeKQ+ZJFGxYM55LOx5dv8Aabn0wMAcE60Yq8vu/Vn0H1ec6n7tbdf0j3t36vY818S6B4osNS+zmAakpfKzWgZgTjCgqRwcfX/HW07w34ohC3k1kbWdcZhMiCRSeDlc5HXocHH5V6togt7XSZr+FVE5YRRtjlCQSWHuAOPcirtnbrgStHkDkKK5JYjpFWOiWFdR3qSvY8yuPCHiu6cXDzJFAg+7uy5PsAMdhj+nQV7izvrO2fynleIZiZdg5OMEAYHJHbHPGR0z65JNI8KXdq25Ym+eNv4vY+hrA8QWuk6xaJdW9p5siNiSI/K6nuM/yNawxrU25q9wq4K9NQg9ji/h58SdPsPC1hoL2au1tGYyTKRnk85AP+fyrvNM8d6dc6m6yWzrFERteOTO/PT0PcfmMZJFefWng7wTHYvb2eo38Zjz/o8kQdgeuMkZrN0zQdei12eO202YaacbLibCEnvld3Tk9vboa1o4q9Vr7Pmc+Lws3CMnHXyPaL/xzoc0fl4nBPQpg/yPPXt6jHVQeSn8Z6ct7JEt41uyhWLNG20g9OeQe/5elYd1o2ryOJBFFu/iBlPPHvnnk+vU5zlt9Sbwnqms3MFpJdQWSMSDNKzMoYn6HGfX6ZJxXZUxFNQ/dtXPOjhavN76djpLvxHYXkbtA9ncyYOBuXB6dfyH5D6jyXWLqMeIJY1tQ0jqqkCTHzn8ffFekaB8IrLS9Ze08d3bSxvxEbOQoq+jEkcj+VdHc+E/Bnw91GCxutNhm+1MWtb2WIO8hznBbGAfy7Vn+8pwc5a/5GlJUq81STs3t6nimm6f/wAI94tTWPETRwXEMamG3hfzpAdwPODtHA6Fh1rvNZ8WP4k0iNodKlS1STdulGd2ByMAn/INWvFGqWsmpjTb7TUXT7ld32lhk7hwM8fT9D2pdJvbTRjFp8rRWoziHDcMcllyTwCTuHJ53e1Qq1Gu4xT1a0fQ6YPEYGTU1dR3Xr19DGfxPJHOk0bRkAgOpbiUlQMdOPr79+c5viLV7PU7KSMRlI5AQ8ZOCoIHpnt9encAber8SzaK1pIVs4H3JgSMoBIx5iZPU8bl/Cvn/wAU3TLqkv8AZ7lbf7oUtwc4JAHYZrop0vZNRvoYYvF08THn5WpfgdZaxWkPiINZDyohC3AP3cDGe/t3/TFcss7SqJHPzNzUun6ndDRJb25CiZk8hCvVie5/T9feqO8KAuelarSTPLnK8Y33R6Jd2+n2DXN1YTMv2d4vMj+75hYrtkYcZO09++a0oNakdQWkwBXDap4qfVL28kutPPnXcHkTSeYBuOeGwF6969M8B+C9M1/w7b6hfa4JJ2Db7OAhWXacfN356/jXz6w8op85+g47GUq0oOi18OqSejuPtfiBb6VEtndxvJHJIpVoxuI7dPQ5/QV6Tp2swXo22bE3IO5EPQj0IqhpugaFDA/9k6XGjwHDzj5sEcnLn+XNYeteJtI0yWLzNSjidAT5pIDBu3PesnHXQ44t68x0v9q3F+88+moIrmL5Li3f+RH8jWS00xifVtJkD3MWVmt34JA6qw9feuTPiq0a0bxFaX+dRkdVj2L8sq553H0xml1bUtMghk8TPqCRTNiJrWJgDN6557c0cjL54rW5sfb4ftcGuR7I7eeVYHhLfPuPt7V2k0kTRjyumK8D1jx/4c0rXLG50qD7Qix4meRRu3HuB2x/WtW1+LmlT/K1wIiezcU3Rq2TUXYx+sUXJrmR6pJdLGcd6ga/hxhlrzs/EDSpDuW9iP8AwIUh8aaXJ1uU/BqShNdDT2lP+ZHpuoNH448Ly6E1wU1ewUy2pzzMg6oc9f8A9RqHwzq9l478F3PgfWJA2r6au62eXl128An3B4PtXmI8Tx2+o2uqadeKs1s4dTnr6j6GofFfirZ40tPF3hCPypVVXuSQQplx8y4z0I4PrXrYfEpR5ah5FbLqlarfCq9/w8y/qV5c6zoV7oupKINQsmMUiH5irDoSenNeaap4juNY0a3sJgXubRyHcnJcAYB+vX8qv6rquo+I9ZvNe1aUxeZt+0vCpEca8AZA61zHiI27Xkd3ooYWyYVRnl/9o/X0rDDQpwqtRXu3uvJ9T180w1SeFjOo/wB5Fe8k9XG+j+X+ZNp9/emSTzpJhsTaqyMcc5yAOnTdTG0iWd/tVxMPK6jk5amSXVtaWaXbLm5f+E/MVPcCoGv9Q1Fcy4ghPYfeavTceaXMfE81o8o9pBNcbY+LeD5Vx0ZvX8KUvzUZKogVRhRUe+tFpoYt3NqGeGR/9JjDjP3uhFdLY66bOzFrFI6RKDhonMb8/wC0Oa4pWYVPDM27aelKdKLR2UcTOMlqd9o95JD4Y1O3j1XULeC4kDOVnP3iP/rVwV54at5JfM+1PKTzudsmum064U6PcWjdWZXH4Z/xqFIk84Ejp2rlinCTsd0pqrFKWpzi6GqWW5UzsYbhuIJ98VYudCtWsw4kxc5/1Z6YrdAEcrttyT09BVdyrKTjMjd/Sr5mLkilaxzU+gRrcRRrIpVxnI/lV+Hw3AvLKDVvC5CkAlTnNXheow2jgihuXQhQpp3aMdtGgBIEY/KozpUKt92tWSZQeagNzH5gBI5p2kF4FK302ee9jtrVWDMcDFaV1o+p2niJNJ0+f7a0iqZFycA+h+la9vdx2MI+zFWmk43DqK2rea00DTnu1YS6jOvXqV/GlyJ6yLp4mpSkvY6O+5h6T4rm0S+vfDGs2cP9k3JCXIVclTjGSe6+3asTUNKj8M6lKvmefYXAL2jk5wp7fWqGoSFnld23zSsWYnrzUTNq2qadbafBZPdC1csszHCpkfdyajlTjZbHTiKs6eIVapO838X+X3GfHY3Mwe7aQRgN8g9BmrMbWIVoxcYnbO1VHykjtjtVifTZrKxY6vqcUGc4hhOWPt/nNLpuuabZTW0Fr4ehmhAO+WcZdz1zntW0ed9fuPOqVMPFOMIXb6t/ojOZqbupjTLMTNHE0UbElVY5wPTPem7q2seaXgx9aesm0g0UVswRqW95heDir0F3ubk80UVztJnVGTWxK0/X3qtLIoHydaKKzSR087sUoZA2Szc1JGV87rRRWhnLVIkn24yKy5JAJeaKKtGHUlF0wKkHpTLrWnz80v5miimknoLmcXdCvd6AuiPczXUtxqjnEcEY+Vfcms+3fxPNb/Z7US29ueeB5effPU0UVnWfJHRDi3UleTKsunw2c+/VLwPIeSiEkn8etdHaa5dQvbw6RYwx2uw5Ei8seeeD9PWiisZO8FNnXhKMalV03sZt/qeq6uIvtkdvFHEPlWNefz5rMooqqM27o2zPCU8PycnXuf/Z</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAQCAwMDAgQDAwMEBAQEBQkGBQUFBQsICAYJDQsNDQ0LDAwOEBQRDg8TDwwMEhgSExUWFxcXDhEZGxkWGhQWFxb/2wBDAQQEBAUFBQoGBgoWDwwPFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhYWFhb/wAARCADIANMDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDxm2iIFXIUNJCtWEUYroPHsIqYNSLwaUDmnqvqKA5R0ZPepFNR80u40XDkJ1IxQWxUAc9AaehJobGoEuN1GylWnUrj5SNkFRlRUzAmmMMUrlxiRFajZDU+DShM0jWKKcinpimmM+lX/LH+RTWiHpQWigYzQYvWrvl+1NaOgZQaIjpTGTFX3TFQSIKCilIuT0qNkqy60wrjtQOxVaP0pNlWSmaGT2oLKjRmomU1eZfao5EFAGfsNFWinNFAGtDU61DCKmWrPOJFHHWlpqU7FK47BQFpyr7U+NCTUlWGqlTRxHrmlVKmReKACOMY/wAawvFXinTdFl+zM3nXZGRAh5A9WPapPHWrXGmaYkNhG0l9eOIrdVXdgk4zj8eKyPCvwo8S6tfPd3suFkGWklBb5vbPWsK+Ko4dXqysduEy+vin+7jc5HXvGWuXKvIbl7WMN8kduNuV9Sx5rCXxtr8c++HU7qP5ukx8wfjnP6V7ifglZJbyC5upJZGHMmMDHsB0Fc3rXwgsbZWCSsfdupFeZ/buFlK0We7/AKuYqEbtI57wl8TkYrBrtssfOGuIASo9CV/w/KvR7KeC6tUuLaVJYpBlHRsgj615L4o+GupWOmyanYl57e2bE6j+Bcdf0NO+EPiiaw1lNGnO6xuZPLjZhgxyHp+B4FerRrQqR5os8PEYeVGbjJHrpFCqT2p6qSaljjwK0MSBkOOlMZKtsnFMdKYFKVKhkSrrpUUiUroCg8ftUZiq4yUxkqSir5dNZD6VZZcdqYwzTuCKzLUMgxVmQVBIvNNM0K7LzRT8UUXA0o6kVaZEKnRKtnngq04CnqlPEfpUlDY1Y81Yij9aIkxU0YwKAEVB6U7b9actPUUFJFf4aaH/AG38Y7m6vot1vo9qnkI33S7g4bH4t/3yK980/SN0IWNAAB0Arzn4KxqfEWpnb83lW2Tjtmbivd9HhRbPeI+3pXwmdS9tjnTb0R+j5DFUcvjNLVnEX2huFwErhfH2nm3jZyMYr2nUkV1byw3HUYrzD4j2jyq2VPcnNeVyRhNNM92NSU4tM8S1KJpXljkJ8qRGVgD1zXi+pWf2HxBJEuV8uTcrAd+xFe9atbOJZI4lLPyFAHJ+leZ/EexgjtYpvKMcrlhnPTHr+FfX5TJu/Y+MzqmtH1PUdBk+2aNaXZHM8CSH6lQaubaz/h3Itz4H0uUbf+PVFODnkDB/lWyYhXvJ9j5VpplUrUbirbxVFJFTuBUkWoWFW3SoJUxSHYqyL6VGymrTLUMmOlAFZhUbCp2GKjYZ6UFJFeQVCwqzIPaoHFBRDtop+PaigC3EatRmqkNWYx61Zw2LCVIoNRpipkFAJDlBFSKKaAfSnrQUoi4qSMECmotTqopFpGx4Vj8TR3EMvhx9Og89iJ5bxmUHZjauRkDO813fh/4ieLNOvpLDXtG0z7LEuWu7K9WUjngMoOR+NZHwt0q28Q+GdU0W6j3r5kcigHB/A/8AAR+dbNz8L4ZvEU2sT6fZwtcKqzlkLAIpJ2xoSVjySSduBkk4r4rMKsI4iqp6S6aX/G5+i5TRc8LRlH4ba6/pbub3j7x5beGdCW/S2WW4uUBt0c8Ox6DIrxXxd4l+IGt2t1c6nc+HPDtrHgSG4u/mjycDIHQ9sHHNek/HGyt5tF0e1aKNIoZQSdvyoF5HHpkCrMPhGDxT4Ai05LWxfTpJVneP7MGVpR/Hk55//VXn4LFU9edfhc9XFYKcopwdvnY+ffAOqT2fjFIdX1uHWLMyhPMt1XcpJ65HUYzWv+0bpNnqGi6XrsFsyW0iSxXLIuN+xSykAdyOPwrufEHw10rw9qh1GKJRO2ekYVQT1Prn61t+LNLs5PgvLFNbCeS1t57qNP8AaCNjj6V9DluLVbnVNaJfieBmeD9goc7vd/geCfBSYtcXEUUxe2nt0lRcnajKQp2jt1/lXoRWuV+DehfYdF+3bg0dwuE9QxO5+O3JXHtXYsgr1cBf2Or6nz2ccv1qyVmkr+pVkyB0qJqtSJ3xUMiHrXYebZFWQAVXm9quSJVaVKLhYqsOKhkWrUi96hYUwKzVGxqaQVC61IyFiKhkNSuKrSE54qh2GlhRUfPrRQM0Ihg1ZjqKIGpkFWcVrliP6VNGKjiFWIh7UDSHKhNSLE3pT4gKnjXPBqblEKRmp44+BUsaD0qVY/ekUjtPgjq1vpN1eefxu2FT9M126+IL/W5bzUYlMmm2R8tIozgzSDljnpwB/OvKfCNxFaawnnn9zMPLc46Z6H867fUNLnvvD0dhpOtXmmJbFmMVpsVWck5Y5Uk5BP518dmlGCx8vatqMlfTy0P0DIa7ll8Y00nKLs79tznf2kfiFpAOl6Ha6Lf3E90AZUjTDKMAnOcAfnVr4E+Jta0XTb22v4DbWjTl7a1J3NEhA4OOnOam8SeHLFtBeaXX7437xHdELZX3E8Y3E7cYA7eleb6f4a8Uy6g/2jxPfQ22eIomRc8YyzBRn+nPrWcsPhoRvz2b/roel7XFPTlTS6X/AM0db8VvGzXkiJbqzBn5IXjFbOk30GoeE7CS4IKzxvC6FsZB6/oa5fx9JYf2hFptvJuTTrJfPmc5Z3xksT3JPeqnwZvTrPjXT7NzjTrJ2uLlmPyhOMA/XAH41rk7jSlKKWjOHOU6sIt6NEWl6fBpthHZ2qsscY43Ek1Ow9ayPDGvw6j4g1zQZJEe60XUJrXevAnjRyqyAdjgDI9a25Er690/Z2jayPgXUdRuTd2VpFzUTLVlhUTKaQFWRc1A61bkWoZExQBTkTnioJUq5NxVWZqAKky8VXkq1Kfaq8hFAFSToarSZ3VZmI5qqx+agoiPWigkUUD0NaEVZhHtUMYqzCK1OImiUZqzCvNQQircNIokjX0qxElMiXirENSVYfGmKlWPPaqWq6vpulQ+bqF3HCMZUE/M30HU1xXiD4ohWaPR7QY6eZMMn8FH+NdmHwNfEfBHTv0Oeti6ND43r2WrPRhCBzW34O8daVaapHpdzf27zN8uFcMcD19xXztqHiPxDreY7m/m8onlEOxfpgda9G/ZD8Pwax8dNEtpoFmht/OuZkZdwKpG2NwPbcV6+tdGP4Yp1MJKdeeq1Vu5WU8RVqWNjChDR/Fft/mfQmraz4f/ALLaP7RBuZSQ6gV4r4+8ZLb74tLj81gfv4wv5969o+OHwnisUTVfDsR8uViGtFbLA4JPljOSMA8DJ/CuB0L4NeIPEKi6j0yOzhY48+73Jn/dXqfrjHvX54sA41eWd2/wP1VYynOh7SEkk++54lNqmsatP9gjVmkvHzMyjlvb2Fen/wBnJ4A+Ft9qtyoSRbcyyMww0j9FX2GSAB717J4E+C+g+FVOo3Cm+vFH33XCg/7K9vxzXiv7c2sBVsPClu4V5ALy7QdhkiNT/wCPEj2Wvfy3Lfa1o00vU+fx+NVOjKpe9tvU+X9D1zVdP1iTUbad1upJzM8obksSSfrnNew+E/i1Y3MKRa1bSQyKAHniXcpPuvb8K8tt9PjEo+UYz1pbGPajso+9I5z7biB+gr76OX06qVOa0X4H5xVq1KTdSD1f4n0XperaXqkYewvoJwwyArjd+XWrDrivnXzdrAfMpXuDiuk8N+Mda01VjS+a4hH/ACyuPnH4HqPzrmrcOTtejO/k/wDMVPO0tK0Leh7BIAKrzHArm9H8e6ZeKEvA1rJ3OCyZ+o6fjW79oiniWWGRZI2HDKwIP414OIwdfDu1WNj16GKo11enK5DOSarTHFTzOKp3DiuY6CGZqqzPUkz4FVJJPelcaQkhzUEhxSvIKhkk9KQxtFRluaKdx2Ogj61ZjqunDVYjOK0uctizHVmGqkZyasQ0hpFqNqZqt/FpulT38x+S3jLkevtT4QS1c58ZpfJ8CTJn/XyKn9f6Vph6ftKsYvqx1Pdg2eYahe3ms30mpXsjNJMdwBPCr2A9gKW3t8KSafp8WY1X2FW/KA2rjjNfd0o6JI+flTSbk+otgr58tW4znivrb9inwfY+F/BN98TNadYVuYJFikY8RW0Z+dj7syH8FHrXy/4W0uW/1K2tIVzLdTLFGPdjgfzr9CtH8AaZF4J0Xwow/wCJXpmwzWwHy3O3JAb23kMR3xXjcQ4pwpxoR3erPa4fwlNSdeeivb/P+vM4rwXeW/ju7tfHRsZPtkyOljHcu+bWLcQAqE7VYgAlgMn1r0bR9e07+0ItBv7+3OphP9UrZJA7Env/ADrO8RBrG51C60ryvMgZIQnknbGfLB4wR2x2rz34B6G/inxpqPiDU1Mlvo128UTE5866BO5z/ujgDsST6V8hL3Uu7P0KcKFbDyqzfLGK0XW72Xoex65FDHYySSFVRFLMWPAAHOa/Oj4ua1J4q+IOqa7JlhdXTGHPGIh8sY/BQor7Q/a58R32hfB28a1lWJtQk+xb93zYcHKqPUqG59B718OzxqZG3hvYr2/CvqOHMPaM6zW+i/U+Hzio2o0r+Zzt9byibasghiYcyYywPp6D680sNikMYRV+VR0PWruqRNPcJZqTtb55eOiA8fmRj6BqkZHLbADmvqacY3bSPm6zb0MqSxMnQU02Togz8oz1rorW0ROWPNUvEG1I22n/AGR/WtpSUYtnMqKlLU4/XLuUSLBESEU81v8Aw/1y80PUrdpC5s7hf30YPA5PzY9uK5rW41C7l4zWtpMkyaRbXLp50KYSRT6E4rw1H20pxqbM6qy9ioyhoe0TSZ6Hiq0zVFpMy3Gj2syHKtCuM/QUTNivjKkOSco9mfSU5c0FLuV7gnmqknWp5m96qytioLI5Pu1Ax5p8h96gkPvQMQsaKhLjNFA7HXqM81Iue9NHNPUVocpPDVuFaqwVct6TLSLNup/OuO+PTlfDtlB3kuCfyU/4128GK8+/aAkbzNJQZxucn/x2u7LY82KgY4p2oyOUsU+VcjrVzYBMqj0qHTwWZeMAGr0Cbrwcd6+2pRPFqO57X+xX4Th1r4kXF/dRLLDo9iZkDDI852CofwG8/UCvsnzHNv5szbUjX5scZrwr9gHw/wCT4F1rXnGG1O9W3j4/ghX/AOKkb8q9e+JV59m8OzWsL/vJBsGPf/62a+Izet7TGTt00+4+vyug3Sp0l1/Uh0O4iuPC+oavJgxzTSygkfwqNqn8lFUf2e9OOm/CLT5WB87U/Mv5Sw/imcv/ACYVD4jd9J+BepKh/eCxeOPH95xtH6sK6yH7LoPgqMzyCK10uyG92GAqInJ/IV5cleSR7OKly0pRWzl+CX/BPl/9vDxKLzxNpvhS3kJj0yA3NyAes0mMA/RAD/wM1893EiwWzyyOqpGpZ2PYDmum+IWuXHifxpqev3JbzL+6aQAnOxc4VfwUAfhXH60v268h0pV+Q4muiOnlg8L/AMCI/IGv0TBYf6thoU0tf1Pg8VW9rWlPoQ6THJJA13Mm2W6O/aeqL/Cv4D9SamugLOMyOfmbgVfASON5W6LXO6hePf6gsS5Khq75S5IKK3OHl5pNm5alY9GadyP74zWLrwZmEYOdo+b61e1aTY1jYD/ltOuQe4X5j/KoNaITcc7jntUz1i0G0kcX4gi42Dir/wAP7yM3DaddH93LGUYH3PX8OtVNZzJKCRxWNHObbUDIhIKngivE9p7KtzdDoq0/a0rdT33SYkt9LjhQ5VAQPzouDWb4I1KPU/DUNwv+sA2y/wC9V64+9XzOZR5cXUt1d/v1PVwTvh4eSt9xWmPNV5SKlmOaqznHeuFHWQzHFVpnp8rdeapzNii40NZju4oqAnmii4z0MZzUiUxRUsdbHOkTRVYjOBUC9anjHFSUi3bsT3rz748NuvtLB5wrnH4iu/txXmfx8mP9vWEYPMcGfzb/AOtXpZT/AL3E5sd/AZR0/AKj2rQsVAmMnYAnms7T/vVtaLYyX11FYwgma9mS3jA/vOwUfqa+0jLlg5PoeRGPNNLufev7Muhr4Z+BPh+3P+snslvJc9nm/eEfhuA/CrHikveX0MYIOTvI+vA/ka6K5t007w7bafb/ACxwRpCuOyqAB+grESIS63I4Pyo4jT/gIx/PJ/GvzeUnOo5M/QMvioXl2M34sOU8F2GnAgG+1ezgwB1HnK7f+OoaxP2zvFH/AAj/AMHf7Iik2Xevy/ZwAeREMNIfpgKv/A61/ikRN4s8F6ZnPm6s05X12Qv/AFavn/8AbU8THXfi8+mQS7rbQYVtVAPHmn5pD9ckKf8AcrvyjD+3xqvtHX7jnzir7PCQ87/i7foeM30sdrbSXMp+SNdzYHJ9h6k/1qppdu8atNOv7+5O+XH8Poo9gMD8M1FJINS8TLpwP7jTwJrk+sh+4h+gy3/fNazGFPneVQB1r7+n7zufDVNNDF8aXYtNJ8sfef3rC8LoHZZj696T4gXRnkxHJtQHrt5xWRpOpSJeQWEBYxPudi+CcgdBgVy1Kq+sK+w+V+zNiS8Nz8QLO33ZEUcjAf8AASP61qahEnO/5m7Adq4rRLmX/hZ0JDdY5AfpsP8AUCuxmlRuc9uSavDTdRT9f8iayUeX0OZ1xf3nIAAJPArmbgZk3Dua6jxL8iucVzUi/uckcjmvKxcbTaOqlrE7X4N6kyXD22/KyY3J/IivQpmzXhXhfUm0vxElypOxX+Ye1e3tIHQOpBVhkH2NeHmfLKEJ9dU/lsdeBUoynHpuv1IZmNUblzVq5bg4qhct/OvHPSRXlfg81UmfNSzNVOZhQMaXOaKh30UAepLU0YqGM1NDWtzEmQdKnQdhUUYzUygg0gRYt/U15P8AHhy3jCNf7sCY/M161COBXjvxycDx4Vz92GPP5Zr1cn/3r5HHmH8Em00ZZfc16P8As/2kVx8avCsE65X+1I5sHuYwXH6qK830Xc90BjpnNeo/s22k2oftCeFbOL+CaSZz6KkbMf5Y/EV9Njp8mCqS8jmwMFPEwT2PunVpl+yO5IGxc4/pWbotudkZAOVGSfepdTtGWBftD/66QDAPsT/Sq2nw31lcM0TLNCT3PIr8/gup91QilSdmcp4xvoh8a7a+uiRZeEfD9zqV16bn4QfUhH/Kvi/xxr8hXVfEupMJJpHkuZj/AH5GYnH4s2Pxr6R+Pmuta+G/Hd+G2yatqltoluw6+XDGJJPwyZB+NfInxEL32qaX4dQgi4l+03AB6Rp0B+rf+g19RkVN08PUrLeTsvyPB4gqJ1qdHpGK/wA2X/A1l5Hh1Lm7Y/a78m4uTklmZj6fkKtXkRVCdu0di7c4+nNWI2EO2NRhQMAVn61cLtYeZ1GRX1kKfs4KK6HylSV5XOQ8XSRrJtyWPtwKx9DkA1DzQoUKhHHXn3qXxJKrXDbSfxrPsmMaly2OK8apP9/c6l8FixoLbviCjAYIjkx+VdvFEMgNz7V534bnVPG1qzHIcsh/FSB+uK9Ks4w8xPqa6stknGfqYYqOsfQ53xjGVhIAPzGuWYHaciu28eIBbgqOB0riJWwce3euLHK1VnRh/gM+bKzbj3FezeCb37f4TsbjOWEQRvqvH9K8fZVlJTv1FeifCGVh4dntmJzDPkZ9CB/UGvAxsP3LZ24eX7xI6eZu9UbpsZNWrh8VnXD9q8Y9IrTP3qncN71LcNzVSZsmlcBuaKi30Ucw7M9ahNWIzzVSM81YjNbXMi7G2KmhOaqoasQtigC5CwFeG/GG7S58fXpDcRusY/AAV7VNMsFvJcSHakSF2J9AM1846te/b9WuLxzzPKz/AJnNe1ksP3kpnnZlL3FE77QTm4cgfdX+tfQX7A+ki9+K2tayybjpuliGPj7rSuDn8o2H4mvnzw2rCGWUk4IBFfUv/BOmN4rfxRqDxMy3FzDDv/3FY4/8fr1s6qcuBa7tBlMHLEX7I+gPFUuy8sbfzO0jnJ9MAfzNS6XztOSuRnr1FZni4ibxE/lniOFFOD0Jyf6irH2xbTw/dXLjb9ltXcse21Sc/pXxq2PuIQ/cx8z5V/aO1Vf7L0Swkl2rKb3WbhieD59w+wn6JH+Rr568AzPrXiDUfEs+7bK3lWob+CNeB/jXT/tNeJrqS1SxBK3ElpbaVGvdRFEiy/mwb/vqsnwlbx6X4dt4No+VRnjrX22V03GNKn0irv1Z8XnFVTxNWfdtfJGzcSxBcvtJrE1eVXjJGB16VakuFfHybec81k6tcL8wQV703aJ4N9Tjtcwtw5561ntJ+7wBVrWXle554XriqEjZ7181Wl77PShHQpm4+y6hBdf88ZVfj2NesWdyFhWRCDlQQQetePaoRtIrufAuoNdeGLcNndEfJPvg8fpiryutbESpvrqLFw/cqXY3vFSh9JVj/EM1wV6AGb2r0HxQQdNReu2PP6V55qJxIw5rXMviTJw3w2KqttnVunNei/DJfLtbps8OIz/6FXm8hxXffDG5DabLHnnj9P8A9deNW97DVF5fqdEdK9N+dvwOmuZOtZ9xKN1TXTn1rPnYk5r5u57KI7hs1VmapJH9aqyNQVsJmiod5opXIPXIX9atROKoRtVqFq3My7G3vVmHlhVOOrdueaAMj4rXMtt8P9ReH77xiMH/AHiB/WvBUt7qABnRW9h1r3b4tNjwNcHnaHQsQOgzXhrX100pFrayy4P3i20V9FlVo0XLzPLxy5qij5HougyEaUcggbV6fSvsD/gnO0J+EOqXQHzSaxKrH/dVB/Svjy1l8jQmmf5G8ofKD3I//XX1X/wT0gun+AexMZ1DVrifJ7LkL/NDV5/U/dU4/M7ckpOUpvoeta9erJ4huyjL+9uNi477QF/pUnj29isfh/rF3eJut4rGQzqvVkK4IH1yaxrwxG6CZzsuW+bvjca439sfxXJ4a/Zr1lonxc6rLFY2xz/Ezbjj6KrV4FOKlKMT7fEWo0FNdEfEuv303i34pSTu/mQWbsN3ZnJy7fic/gBXQXl2BMIYzwoA6dKwPANgbS2cgZZhlmx3rTjjBmfk596++wMHGnzS3lqfmOKnzT9Bbu6DcMzE9DgVnXI3RtgMfetX7LEuWY85rM1m4WNWWMV2Tdo6nFyts5HWm/0r7xPWsyQgA1c1Rm88k9SelUZgdpycYr5mvL32erTWhnaiQVIrqPhjIV03yxzuuCR+QrlLz52wPWu2+D8sC3UtpKF3MoaPPqM5/n+lYYCVsWpGmIjzUeU6zxA2LPGP4cV53rR23Neha8wk3IgzgdK8+8RKyXmGGDXrZl8CZx4b4mU5T8ua6T4Z3GzUWizw6H/GuXY9K1vBcjJrtuV7vg/SvClrGS8n+R2dU/NHoNw464qlcP6VNcPmqczV84ewQzPVaRqkkPFVpDk0iRM0VFmigD12M1ahNFFdBJbjbNWrc80UUCZz/wAZLyO18CTBxuM0qIoHrnP9K8Zu5PKgjMFvJNK/RT0WiivosrbWHdn1PLxiTqq66HVeIPtMHhWOZ0ZVkGwNt+VmCjIB9RvT/voetfbP/BO9Vi/Z/wBOlbBCyTL/AORnzRRXJnU3Kqk+i/U9TJ1+5fmbIuVN4pY43NkH0ya8m/4KEGaX4a+GbQFfLfVS7k9CRGcfoWoormwSviII+vzjTAysfOGmXMcMDxwYwMDOfvGmbws7Fj1oor7qm24o/Lqq95kF3dFFJV6ybq4kkJGKKKmrJtGMfiOd1BSbzaxrPvyB8q0UV4GI3Z6dPZGfcjFafgud01qEqceWS+fYDNFFcuHb+sR9TWr/AAmzr9PfUtRvHaFPlXkk1z/jQNFqXlP99fvD0oor3cy/3ZPrc8zBr96ZCnNdB8O41k1iSQ/8sYywHueP60UV85WbVN+h6sFea9TrZmqpMaKK8A9EqTN71Wlc0UUARbqKKKAP/9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAgMDAwMDBAcFBAQEBAkGBwUHCgkLCwoJCgoMDREODAwQDAoKDhQPEBESExMTCw4UFhQSFhESExL/2wBDAQMDAwQEBAgFBQgSDAoMEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhISEhL/wAARCADIALcDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD82EhqdIalSP2qwkVSCIUiqeOOpVhqZIqAI44amWPNSrDUyQ0hpEKw1KsPtVlYfaqt1qlvaEr80jg4KqO/1pOVilG+xIsNQ3VxHbSGNQXlwDt6Z/HpUatc38qKvmwLKuI9mPvdec9elOs/D/7x7jVJSI45hF5nUKTkjPp0NZSqrobRoy6gs08ao13ZyRq4zuHIqxBvmXc0RjUkgZ9ql1qabT5FNjOJfLG0ZbKyqRkEZ6cZPP8A+pkmpakbgya0I4klXcqpg4B74B45qVVZTorYk+z+1J5PtVObVhZyKztvikHy5YZB/pWlazQ30XmW7bl7+oPvWsZqRjKPKVzD7GmmCtDyaQw/SrJM4w03yfatAxe1N8ugmxnmH2pphrQMNNMNAWM9oaiaH2rSMPtTGhoAymhoq80VFArGYkftViNPanJHU6x0wGLHU0cdPSOp446TZVhscVWEi9aVI8VV1aQlY7O3I866O3k4wvc1DdtSkrsa1217IYLAEp0kn5wv+76mp/7DbUJBDpqkCEZ3bOmO/HWt7wj4DvfEOt22iaQzARrvuJOcRr659fSvqHw78CNO07S1to1XcR87kcs3fJ9a8PHZjCjK0nqfWZRkNXFU3JKy7/5Hy7qVhcWV1a+baRPGigP5XRweh4+6wJNZl1bvBJdxWoadZiCVcYLD6dCeT+favpzxB8G7m0nDRRoYt3yOy8c8Y9vzq7pvwLh1FIpLmFEdBhmXgN/WuZZtTSuz0ZcNVm2j5AttDuLuaIrG7rDyqPnGcd6sa19rcot5CoYNjco27cf5/Svr27+CsOkr+5iR9n4/561x/ir4b29wkwaJEdlO2QKMD1465pxzam5eRnU4ZrQp+Z8sapp7wrtYxP5nOF5H/wBaqui376fdAKxVM/vEY8Ef56V3Pjvw7eeG75IbpmntO2E4P5Ec1xl1pc0JWfyh5Mg3Ic546dq9qlUUopo+SxOHlTm4yWqO1j2yxq8fKsMg+1L5dYvhO8M2+2Yk+Wuee1dFtFdUZXRxtFXyqb5XtVvYPSjy6q4ikYvammKrjR00x+1MCi0ZHbNRsntV5oqieKgTM946KsyRUUCM1I6nWP8AGnJHUyx0mMYqVMq0oWpVXGKQ7BGlZqaa2oeKUXcVjhVS7DGR3rZjWtLwBpY1HxglqMebc3KIfUgn0+lYYifLC51YSn7Soon0v+z58Nzp+iy6pcLi41WQPu24YRj7o9s9fxr6O8M+FEYphcEAfN3/AA9KxfCelx2dpFDCoWOJQqqBwAOBXpvhuIRqOOe1fm1WrLEYhyl1P2zC01g8GqcOiJE8D2ksQNxFuxzTbvwvbRwkQwoCBgcc/nXVKx8sA9TwKp3gPPX8q9F0oKnojihiajlqzyDxRoflpJ8oAPGMV5VrmkDzCoA6EYPpX0B4kjEkbBhyRXlGu2H74n34rym+WWh7MWp09T5p+L3hkTaNdfLzCQ6nb93+vrXgGtWbW8flMzu8Y+WTsR+fpz/+qvsXx3p5lsb1VXOYSDzjivk3xY6NNPuVy4QhX9Oc9u3+NfW5LWcqfK+h+a8T4aNOtzLqYWkDydQtHbJMjFGK9s9M+vf9K7Ex1yGhgz3zxkrkSBl/MH+WfzrtjHX0VLqfGTK3l0myp2TFJtNakEG2k21PtppWgViBkqJo6tbaYy00xFB46KtNHRTAyVWpVShFzUyrUgkNValVKcqVIq+1IoI15FbPwyb7H8XvD0bDMd5exdu+e35VmItdH8P44x8RPCksg5h1aEg+xP8A+quXFx5qMvRnbl8uXEwfmvzP0N8P2LNs2jjHNd3pNv5WBwa8Si+IWpteT23h3T55ord9skgUESkjgA9R9cVQH7SV94TuntvF/hrU7NBnbIITt/M8V+d0aElK9j9hniE1a+59QJNHHGu7bnvUV1IkqEoBj2rzjwL8RrD4gWT3Ghy+cI1zIvdCc8H8qyfGXxu0fwTZzDVJWEsOR5S/eJ7cV2PE83upGP1VRXNc7DxJbptLLzXluvx/veRwua4eP9oPxB411IReEvCuqXdtn53it3PHrkgAUur/ABDudNm2eINOvbdJcZ3wbTH6g81yVMNLmvY1hjYKNk9jD8aSmLT711GSY2xx1/CvjzxG63GpTCNTtkcp9CSSD/MV9kakkPia3eK1lAWWMlG9PYj8a+T/ABZosuk+ILuNl+Tbv3DruGT/ACGK9/J/cTT6nyPEn7y0l0OW0i3Gn6lC0yHkhRxnd16/gBXXMtc/aEtq0VzdK7woAZBHgEBsHA/EEV2esW9tHfFtOWVbWeOOaFZGDMqugYAkAAkZxn2r6SlUXNy9T4yphpql7RrS9jK20m2rBUU3y66kzkINtMZKs+XSGOmIqlT6UzbVorUbLQMqstFTFaKYjHVanVKSNanRaQIRU9qlVaVVzUqrUDQipWx4VuDp/ifRrvAZbbUIHYY7BxmsxVrR0i3e41Kzii+/LcIq/UsMVnVV4NG+HfLVi13PsfxV8KdUude0+WHW7/TNDJDXCaexillyRxvByBxj8RXP6p+zI974jvL2PxjrsuhbXNvBPJcearnJUMzjBxwM56DPfj6Q8LLBrWk2f2o53Qrg+hI5ro5PDFvJGDdM0iJyF3k/z4FfDYTGzjSceVP5H6tXwNKc4yldW7O34Hjn7PPwtufhh/aDatqIvm1SBZNgwQm0MM5B5Jz+g9a8h+LnhfUviL8VLGDw7NawfZpjt+0KPLdwM4bPH519YW+y5uLhrNAI7e3ZFC9BXhlvbw2fjSRbggS/aDJtPXrmuX2klU9p6nsvDRlRlF6bf5mbcfBz4g6P4H1K6t/Hcuk66kg+x263SpBImOckbVzkjA46Hk5ryfxVY/Ea1hso9f1m28R3cyETRrtLqB/toNv519y6fYz3diIrcxGORR8rcfnWXcfDjTY3efUDAS33ljTGfYnk4r0PrdP2aSgvW2v3nhTwidaUnOV30vp93/BPlTwz4E1nStETUNTSS3M3IQHoOn8q8T+KlitlrE0V0GzJw+OoXkj6dq+4fHEkE01vYW4UIcKNvpXz/wDHbwDYza/Bel2SNYUjuSMACNcBifXAx361eWVJVJOpLY8/NqMY01RW589+E9Lj1aG6tbdT50cLOvGdxXoPx6fjV7WyPtogTBWziS2DAdfLUKT+YNanwts2tde1LUfJkhtpM/ZWkBwUU7iT7YBrCZSzEtySa9/Ax5qsp9tDwc7fssJSoLrd/dovzZB5dJsqXbRtr1T5Zoh20w1My1GwqkS0QsKjPNStUZpiIWWinNRQBmxrU6LmmKtWEWkwBVqZUpVWpFWpKSEVauWFw1je29zH963lWRfqpB/pUKrUgXipkr6GkG4u6P0R+E2sC50KzbccbFIz6EA16LqeqSPp9ymnxPNOkLNhepwM4HueleF/BXVjeeCdGnTDefaIrEf3kG0/qK7jVvGqWMMtrYuDNEAZ/mx8xGQM+mD+dfmnM4VJU/Nn7VSlGdKFR9Ujk9G/ak8O6Fo80mu6feWEwMkciXEDZ3KSCOOO2fxrw9vjho3i7xdcXtvI9tJaMJIUZSGYZz9CMV65r/hew1qxhguLcbrzc9wrjeuTjaRkdgc8gfSuF0r4T6No2vK1/FFfWqTKYEztCnJPzLnGRj0rtg6PL5oUq9T2umie9+v4n1noGqI2jwzQ8eZCD9OK5zxJ4pNtHKS+QoJ61maX4v08WQtrWZFeJSvldCuO2DXGeKdR+2s6Qsdrcn2FebUqP4TphCFnJHOnxDNeeKI7mYkRJJx9BzWX8Qroajp948iGRGgk+Vlzxg549MUtxGIn81TtWLhTXLeIteL2upLHKRstJGHfJCNx7V7WVu6UT53Nkotz8jzrWL9NF8Ni1V4jd3kYRFjYHy4z94nHTP3ce59K4WnNuY5Y5JpNtfXYagqMOVH59mWPljK3tGrJaJEbLTDU1RMK6EecxjVG1SUx+9UIhaomqRjUTU0SRtRQ1FUIqoKsRrTFX86njXFJjQ9VqVVpIxU6rUlCRr61Lj2pVWpPLqSj6W/Zp8bRN4cGjTkLNp1wSvvG5zn8yfyrr9Q+GOoeJ/F15et4huNG062X93JBErSSM3J+ZsgAfQ18p+E/EVx4V1uG+tGI2/LKo/iQ9R/X8K+xPht4wsPGWlR+TdxGcYEo3cgnvj0NfC51hamFxDrQXuy/M/TOG8fTxWFjRm/ehp8uhhTW8egQzRaX8RdaFyW2M15DBeJn2Uhdp4POa53VfCPiXW2U6b470y7mPQS6YEkUn12SYz717TqfwZ8K6tC1zrN3cQXL8YtwAGHXp3PWpYfhj4b8J2e3RJ5AAoy8uMtgdc1xuu1TU7K/oj6SVT2r9nNafM8T8K+AfFug64P+Eg1C0vLaTazXFuWBUqcgEHOBnPfvW/r2qQW/+jQuN7MVYg+9bvirVrfRbGcxXCNxxlua8EuPEjSXt1dXM65yREu7OPU4rGnGeIlzNbHNUnDCrki9ze8YeLYbNjb2rFnGRx61zXw50u5+InjEaVDKoF4HiZsZCgg8n6V5/wCJtce+uGhtZDvHVlHQ/XpX0V+yP4eTQdOv/FOuZitbSIhJpBjeQDuIPoBkfU+1fT4DC8nKup8Zm+Y8ynLoj5nuLf7Pc3EDEF7aZ4ZMdnRirD6ggioKzJfGVv4h8feKL2HEdrretXV3ajsN8hI/PNaki19RUpuDsz4inPmjcjpjU+mtUFshpjtT271E3eqJIpKhapXaoGbFAmMc0UxmoqhEka1YRc1DGOKtR9qkociHirCLSKualWP2oGhyrT1SnLH3pl3eW+nwmW+mSGMfxM2KkokEdd58M/DPibULfXta8DzSLceGbVLu4hXJ82Ldhvl6HAy30Brxq9+ICsSmjW5k7edLwPwHU19p/wDBM2zuPEF14+udWdbhTDZw+WyjbhvOJGPTgVs8DKpTfOtB0cU6NRTg9UeYyftPeJrWFYrqzaaVO64CyHkAkHp2rlW+MfirUrkXEslzFhi+xiuCOy9egr2n9oj4D23gnxpe2lvBIlndf6RYup/5Zt/D9VOV/AHvXiy+B3gZjNOREmTuc42/WvlXQw1KTi4WaPvY1cdWpxqRqNxexR1TxfrOtZkvrghieADuxx9MfpWHPLMGCtLLJK/AU/4V618P/gH4l+KEaz+E7J4tJZiP7WvF8uJscExDq/8AvYxx3r6R+Gv7HugeDvLuPETNrd/kM3mriPd6kdT+PHtXZRwc5/BGyPLxeOp03+8nd/efM/wc/Z21Xx5eRX2pxS2mkBgXkZdpkXvtz0B/vflWz+2J8ULL4b+EIPh54LdIbm9gAuhDx9ntumP95+R9Nx7ivqX42fEfSfgj4CutSukiTyV8uzs48KZ5SPkQfl+ABPavyY8ceItS8ceJtQ1rxBMbi/1GZpZnPQE9FA7KBgAdgBX0WBy+NNcz1PlcdjZVpW2XYwY79oNgizlDkMO30r0bwx4wt9UgSC+lSO7UADcceZ9PevOhbHGMVHHD/wATBV/urk/ieP5V31KHtFZnBCTi7o9qNRMa5PR9ems9sd27TQHrnlk9x7V1CzJNGHhZXRuQwPBrza+HnRlZnVCpGS0EZqgkPWpJGqFjWKKImNQvnNStUT0xMiY0UjUVSJLka1ZjXpUMdSS3UNnEZLqRYo16sxxUlllc1I91FZxGS6dI0UcsxwK5DU/iBaWyldNU3Mp4BIworkb7UrvVZhJqErOT92PsPwropYac99DOVZR2O11b4iRx7o9Fi81unmyfd/Ad65a6uLjUJDc6tM0r9gTwv0FQQQiFN8g5qb7ObpwG7fkP/r16lHDRp6panPKpKW4W91hV2oQ7HCg/zr9Fv+CWcqQyeOI5D8zmyP6TZ/nX53Rwh9QijjHyxDH4199fDyO9+BX7O95a+C7bU7vx14w0s6le3GnpltItmiJiZmwQm2M7snnJOOmRpVajSlzGlCnKpUUUfRf7U3xi+D1r5fh3xb4mji8Rwtsj+xWkl19lY9pnQbUAOCQTkDPFecfB/wCA3g74peLHj1jxRpGvWmm7J/7K024Z0ve/7xyoDIOMquc8ZIHB/Pv4fte39xc399PLMMmWWSY72lbPOSeSec+uat2HjDX28c6fP4DvNR0/VIbiNrN7KRkn83ICjIPUtgY6c185VoUqlaNSUdUftMOFfq+RKpSxLi57Jpb9Wne6R+33/COW2m20drp9vHDFCgSNI0CqigYAAHAGKyNetrfQdJu9Q1SaKzs7KF57i4mbakUaglmY9gACa4H4T/E74i6FZabpvxy8M3WqCWNVXxNosKsucf8ALzbqcqf9uMFT/dXrXzL/AMFAv2pIfE12/wAOPh7eeZpNoyvr13ESPtMwORbj/ZQ4LerYHG059XD0JVJ26H45iIOlKzafmj5q/aY+MU/xu8c3FxZtNF4f09mi0m3k4JXvM4/vPjOOwwOxJ8FurVo5jlDx+tdUx3An86xtXhkuBtjmkg5G7y8ZK/UjivZlTjGNo9DjMWZkhXdIyRjHVjiqWnL9pme4H3S+FPqo/wDr5q//AGJZJJlBJOx6tM5c5+hrQa1EMPQbjWcacm7sVxIVzFupqyz2rF7KZ4T3A5U/UVcs4x5YDYpZbU8lRW8qSlGzJ6k9p4pdQF1KH/trFyPxHUVrQ3kN5H5ltIsinutcz9nK/epqLJbyeZZu0UncDo31FeZXy2LV4aM2hWktzqmqJjWJD4pVG8vUIJoiDgybflPvWrHcR3Ee+F1dT3U15NSjOn8SOhTjLYGopGaioA0V+UEtwAOa818U65Jq14QrEW6EiNB6eprtPFGqnS9NxDt82c7Fz2Hc151bx+fcZb7oNdmFpX94yrS6DreHyYw7DLt90VoWlt5Y3ycsfWmW0fnSl2HA4WrknoK9SELI5yLa1zOg6AHpWoq+Wm1BiqtiuZSfQVbm+VDW0VpcBdDsZb6+CWyGSedxHEoHLMxwAPxIr9sdK8CxeDP2dr3RdWaE3MfhaZNUuioHmyfZiJHY9SOo56AAdq/MX9iH4bj4ifH3wzb3MfmWWlTHVLvI42wfMmfYymMfjX6g/tReKh4I/Z28fan5scEo0Oe3gaRQwMsy+TGMHg5aQcGuXEuzjE6sLFymkurR+PsV42geA7bywRNctu2sM4B68D1A7167+wb8Mz46+N2mT3cHnWeiq9/MT83zIdsWT/10ZWA/2favH/EGho3hmyubeSYTCJWbc7FWBxyVJwACMZ6niv0v/wCCf/gOy+FP7OLeN/GEUelS67G+p3E1x8pgsY1/dlvRdoeQezivIpQvK5+6ceZlLB4ONGejcFGK8n8T+S39VuejftX/AB4tP2fPhZNcWLRHxLq6taaJA2DiTHzTEf3YwQfclR3r8fb29lvrmW4u5HmmndpJJZGLM7E5LE9yTzmvUP2lPjpf/Hn4naj4guWli0uMm30ezc/8e9qpO3I7O3Lt7tjoBXkM0m2vpcPQ9lTt16n4HKV2K0u7d6Cs+6ukjV5J2ASPl29u1SySfuyBxnqfSs61g/tWZZWH+iRHMIP/AC0b++fb0/OnKPvXW4rkmnwzXkxubhPJVgBHF3AHdvc5/CtG5hBUA1cgh2KKSRdzdq2jGysKxStlCnGatsgK89qrqoWYj3q02NtUgKrR1UuVEeWY4q/IwjUliBWa8izR+e/3OsYPf3qJiKcgZlLTEqp6L3P1qnFdfY2P2VzH9DUeqakqKTnpXOS3c1w5MeQK4K1SK03Gl1PQ9L1YXi7JCDIB19aK4G0vrizmBbdzRXDLD0Zu97FKrOOm51Pja8+0ap5MeSLdAv4nk1jQp5ahQOWp95dfbr+ac8ebIW/DtRb/ALy4HotdNCHLBIU3eVzRjURRhajLFjx0p7/N9KjB3NtWukResVxHn1NSXHOB6mktV2x06NfMmUehrVL3bCP0I/4JZeDVWTxp4pukAWCODToJD2BzJKP0hrlv+ChX7SLeOvGEHww8MzAaRo9ysurzIcma6xhI8dxHuyR/e6/cr034C+Jbf9nv9hWfxddKgutUe71GONuPOlaT7PbofUMyRk/7O49q/OjSbufXvEF3qeszNcXN3K89zLI3MhY5kZj2zuz6kjA715mJleq2fa8I5YsRXjUltdJev/AR674e8MzeMtQ0PQbYA3Ot6jBZR/xDzJZFjcZ7sN2fQV9bf8FDvjZB4V8O6Z8IfBLrbRm2ik1ZYTgQ2yYEFv8A8C2hyPRU7Ma8U/ZhutO0H4jL4s8U7f7L8B6Xda1eqygF2ij8uEKOilpZoto6k4rwD4g+OdS+IvjPWPEniGXzdQ1m7e5m7quTwi5/hVcKB6AU8ro83vvofTeL2NjUzSjh4/Ygvvbf6JHPyyHkGqcjFmwODU0hwue5rN1C6a1jUQjdcztshU+vqfYdTXszdlc/JURzA6ldGzTPkx4N03r6Rj+Z9vrW3DCsahduABwBVLTrNbG3VFJY9XY9XY8kn8a0V9u9KEbavcokHyr3pjD607OKYz9ea0JbKv3piemKsEjaN1V+rcd6h1K7W1t2LHp0A70m1FXYrkF5J9smNupPlqN0p9uw/H/GsvUZLiTIjO1BwFxV9f8AR4SH/wBZJ80n17D8Kyry8252muao9NQMmTSbi4fMsgC96iuGgsflDBmHpRdX01wdkZKgmki0MTLl2LE81wNa2ih37lVtTRmyw4opLrSxboTycHFFYt1FuK8S6vABq5ZLtb8KqKpXb3U1ct/lya64LUCzI3YVLbx7RnrVVTlqt/djA9a2SJLcLfuRzUtr/rgW6Dmq8JxCv0qxD3HQtx+da9LlLc+tf2zvG39h/Br4O/DTS5Aog8N2Wp6ii/3/ACQkYOP9t5yR/umvmfwhFtlSSMFiGyijkkqM4A6bthIyeBj1rV+OXjY+Pvihq2pQyb7S18uwseflENvGIlIPYEoG9t59aq+G4xFC02VVFxgtwqkfPHu9iNy7Qecc14lV3vI/aeD8MqcqUOyu/wAzptd8XSaT4Zu/D+mudurSQSXUiZw8ERZo0LdXyxViT3iSuIVs8mlurxtQupJ3LEO3y57L/CPwGBUW78zXt4Wl7OjGJ+bcU5qs0zivio/DJ2X+FaL8EJcyKql5GCpGCWbpgDrWbpqtfTNqEykeYNtuh/gj9fqev5VFqW7VJ/sMbYhjIa5b17hP6n8PWtVFMaquF2jgVd+aXkjwSxH26VKhxVdZCueKcbgf3TWwiznioZn2rTTMD3xVeSdZGcKc7ePxoE2OWQIrO2MCsWO4/tLUHkbmC1P4F+w/Dr+VM8San9jtEij5ll4VR3J6VNp1mLOxji6sBukb1Y9a55y5p8q6CI7yQtuxkCsi4jyMse9a91nbgVmTocVhUQ0UCoVc+pq1Y3HzYzUEkTGkhVo5Aelc6upAzWSNWb5gGB7GiiHcy0V1xWhztGOjssIVugb5T6e1WY2xEfU0UVzxNiW39atZ3YooraIFmJv3aj2qPVZmg0ud1OGC8H0ooqqj/dsuHxIdaxsoRFP7wAKuP73QH81U/jk100dyYdFVVCZmGxd3/PMndlR3wdylj1zgcUUV51OKlUimfqcsRUw+W4ipTdmo2+9pfk9Cqvyiquo3v2K1eVV3Pwsa/wB5jwB+dFFexUdoNo/LCDTYRawlZN8jsd7ybD87Hqa0VuBtwwkz/wBcz/hRRSi7LQANxFt+Ziv+8pH9Kja6gLcSx/8AfQooodRiY1rhH+66n8ahgkH7w5GC+f0A/pRRQpXaEcqtwdY8WZ5MVqcj0z2rrJG2x/KBzRRXPhneDl1bHIzJ2dm64FUpcjqaKKcwRXeomY0UVzsGXbW4KiiiitVJ2Mmf/9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCADIAOMDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDwAUopMU5RSAUU8DNNC1Iq0AJtp6rTlWplSgZEqVIqVKqVIqUAQqlPCVMEp6pQBEEpwSplSlYBRliAPU0ARBKcEqRQCAQQQe+acuD0IP40ARbKUJU4Wl20AQbKTZVnZRtoAreXTSlW9lN2UAVClNKVcKUwpTApslMZKulKjZKAKeymlKtlKjZaAKxWmkVOwxUbCgCPFFLRQBV205RSqKeFpCEValVaVFqZVoGNRKnVKEWplWgBFSpFSnheKeq0AMVKkjiZ2CquSe1PC1v6dZfZ7cSuoLsMgHt6VMpcqOnC4d4ifKtupzmrJJZwgIhMmMk46Vytza314N7+YwzwuCf0r0TTrC61u+dbcgW0TlWmI6nvj3/lXcaZ4Ut4Ivkj3NjljyTXFXxsaOm7O+nlzrO60ieOeG9Hm2zpf20wjZcqSSoBq/dWunCPy2dYX6B1O3Br1G+8O4BKgj6VxWvaAg3bkGfUVhRzBSl7xtWy3lh7px81xc6VInnEzWzHAY9fzratZY7mFZIWDIaybfdaySabcjfbyj93u5w3p+P88VR024bStQaGQ/uC2G9vevTjNSV0ePKk1odVso2VOACoI5B5BpNtWYkGyk2VY2UhWmBXK03bVhlphWgCArUbLVhhTSKAKrLUTrVthUTLQBUZaiZatstROtAFXbRUu2igCooqRVoUVMopACrUqrSqtSqtAAq1Mq0KvFTKtACKtSquaFWpUHNAFvSLP7XeKn8I+ZvpW7rhkj091i5nbEUX++x2j+f6U3w3DthmlHViqA/qa1rKFLrX4FlIEUCtMSTxkAAf+hN+VcuInypy7H0GXw5aPnI6jwloENlptvbxAbY1Az6+prs7WwhCgcVz9jrOn2Kq0/nGAceYsZ2n6Gti38QaZeE/YZlcAcjoR+FeSqbtzzR1Sqa8kCPV7JI14XrXnXiC3Qs4I5r0PV9UgS13SNwBXk2veJftNy0Om2jzODtyRwT6Vl7Pnl7hqqnJD3zjPElhlvNj4dDuBrldYUPIkyjCyDn613+qLepBnULIIpH3om3FfqK4m8i3QzKh3CNt647jr/n6V6mFbS5WebiYxbbRreFrv7RZmBzl4eBnuvatvy64nR7n7JqlvJnCSfI34/8A1677bmvQizx6seWRW201lqyVpjLVGRVZaYy1aZaiZcUgKzCoyKnYVGwoAhYUxlqYimkUAV2WonWrLCoXGaAK+KKl20UAUlWpUWlValVaABRUqrmhFqZFoAVFqZRSKtTKtAAoqRF5oVamjXNAHS6X+7tbZO2Wkb8B/wDXq9p8ULandNOT5EaRkjsfvHn2/wAKztMIfZnqq7fzfb/7LXUeB4Y7mfUvPVXVpFiIIyOF/wDr152Pny02z6rCxXKl2X6GfffE3TxZTQ29tLNFCSGkERZeOvPAFWNEkj1GH7ZZI0U6bWkhZNjbWxjg84IPXkV1TfD/AEeSF4PI2WkkvnmBDhC+MbtvQHHHFX10XT9JhxbRhGYgEnknHv8AlXLWlRVK6uZUXW9rraxyPxOU2mkwmAtmQcjNYNnPFpOjyz2duZbmKIPI/AIB6kk849lBOOtdX8SbWcaVDOyEopBx6io9DtEv9HaCeJcgYMbjkCubD1YR/iI6K0Kkl+7Z47N4pubsxm8tyguFLIA4Y4Bx0HI/GqOo2hhlEgTCzICR/P8AnXquo+FrG23OkCI3X5UArhvEARXiix1LIPbI/wDrCu2liKcppU1Y5ZUKkY3qu559eIYo8fxI5Fei6VP9r0+3mH8aAn6964LWFOyQn1BP1711XgWbzdH2HrG5X+v9a9SJ4+IjY3GWmMtWStMZas5Coy1Ewq2y1C68UAVHWomFWXWoXFAFdhTCKmYVERQBG1RsKmIqNqAIcUU/FFAFdVqZVpFFTIKAFVKlRaFFTItAAq1Kq05VqRVoARVqZAV5pY1pZHKBgMfcLHPoBSZtQhz1EjV0lsRRYBO7GfoNx/rXQ+ALtWu9TiDfOs3mY9jkD/0E1zVm5ht4CepAPT0QVkeCNXa28ZQKWwl7Z4we7qzH+RNedj4OdGVuh9LSmoOKfU+kYr1ILFpX+YqvA9a5vU/+EjNrDLpLWYkmYmUXCFti9tvIqtDeSzwxKBuQHLD1ApL7x3p1repZyM8lzgbkiQuV9jivKouVVJJam7ovmcY63OY8ZQeLpITAsMcqhBh/M+Qfh1/Cub8O3PiKz1q3n1K7EoQkP8uMj04HSu18Z+Mo2t4009ZVc/f3Qupx7givNZfFqQzgXEcpBP3xGQBXW8LUgrKKNKmHqQiqtVNI9Q16+iltxJGR8wya8a8VXgF5EVOT5ox79a7iKf7bYXM+dsSxbxkYryjXZt+o2QJzvnBqcFScampw42suRco3WhlZiOmOP8/StP4czfvLiEn7yBwPp/8ArrP1kAWisP4owPxAOf5VH4KnMGr2ZPSQmM/iK9qJ4+JV20emFaYwqemsua0PPKrioJF4q2yVEy0AUmFQyCrbjrVdxQBWcVGRU7ComFAELCo2FSsKYaAIsUU7FFADVFSqKRVqVBQA9VqZFpiip0FAD1FTKtMQVYRaAFRapXsny3hHGyLYPbJrVhXLD61nX1uY2u94+UrupM9HL4+82WzMEtMNj5Y1PT1WuHEjw3WlXkOfMgR2Q47rhsfQ9Pxro9RnYwuQeJIuR+dcXqkslvosUkROVdoz7ZH/ANaueS5lY78Q+WF+3+Z7/wCC9ettTtIbi2cFJQCB3B7g11F5DBHD5trBDHNnduCYyfXI5zXy98P9WvdJlzEW8h3GVPTvyPyr37QPF1rNahbpgrY5DV5FWnLDSajsdWHr/WIqb0ZV8Uavq11bmL7H8wG3zUnPI+hFcXZaOyM0t2nzMehOf1rvNR8SaTFIFYh93IArjvEviiCRXSzVQPX0q416s9DepVahyuWnYy9d1j7NYTWsZwZCFOOyj/P6V5zHcC/8SWuOY45UQfnyak17UXlLhGJLdWzVPwnA8uv2ZUEhZBmvRo0+VczPArVXUqKC7m1r5AjiQekhP4D/AOvWZokvl3Vge6yqau65LuuHA6Rwu3/fWKwbSQpcQN6Nx+FdEdia7/eHu2OKawptjIJ7OCQch0Vh+VSkVocDISKgdatMKikFAilItV5BVx1qvIKAKjioWFWWFQOKAIGqIip2FRMKAIqKfiigB6rUqrQoqZFoAEWplFIq1Mi0APRamVaaoqtrVwbWwYqcOx2gigZca6gt+ZZkUA9zT7m4t9S026a1YMyplq4BSSzE8/NWpoF4LS/Xf/qpf3bg+hpyjodWDr+znZ7Mku5MW7I2QQgUD8f/AK9c9qibtLvoRzh0nXj2AI/UV1nii2KNDNEMq2VYDsRz/SqGlWovJPu4kUFWycZBGRXK3Znt1abnHlO5+HXhS01mWKyS3H2SaxDrIPvI2VIYfiCD/vVPr/h+O2kmtN2Z4Tt3rxn3x/Suj+DNtNaPp93LMj+Xbx2roOMpIWwfwIK/UV1Hijw5PqMN9eyQlbi1fyxKBy/swHYjHPUHNeVXk4u5UHHTtZL57Hzxe6XdLI22ZsVnto91O2zcxHc16h9kiuBlA27OGUjlT6Gm3GnrbQM23BxThiegpYNPU8dn0GZrpLeJWkkkYKigcknoK7LTfCMmisjg7/JJMs6/cLAdFPfB4r0r4e+Bxqi3esXBdIrfKxlePmxyc/iAPr7VD8Xp49K8nRdPjLPFbrHsjGSzdT+Jbj8K2lUqylFJaHPQp0o1H3R4HrDgLfyf33WFPoOf6VhxgtMoXkrWprUbeXGu4GRJCHXPIc9eP89Kl0uy2gEjmvViro8itU992PQPCmsWa6PZ291cLHcRoFYMCBx79K6ddrruQhlPQg5FeZRwALVm3nntWzbyvGf9k8H8K05TnZ6Ay1C4rm7bxLcRYF1Gsy+o+Vv8K1rHWbO/bZDJiXr5bcH/AOvSsBNItV5BVt8GoJBSApuKruKtuKgkFAFVhULVPJULUAMxRS0UAWVWpoxQFqRBQA5VqZVpEFTKKAFUVzPiC7aa6MQ/1cRwPc962tZu2s7PMf8ArHO1T6e9cgzF2LMctnJJqorqDYkY6/Wn45pIeUB9zUmM1QImudWuVhKOiyxkAH1GO9MsdRgXUbRJd6Q3DrG7DqgyOfqKQJuXBqrPagv+PGKylTTO6GOqxVm7n0VBam4aOwsWlhuIV8y1fI5UNwJFU9GPIBHr6mvT7W5hkvYzdKVj1KAJIvQbwOVPow5rybwhqFpqXhvT7n7ZDBdxyx+Z5odsyqR12g7cgAbj/iT3FytvZeHopIrmBjlikMbh03ZyN7j5g55+boK450XFXjq1/VjpVSM3aWzOTvPDrW+u6hbrKh1K2dSsQU7ruNjwwHdgCM4qHVNHu5VIktJ4lQfMXjIAr1LwXFb6nGmrXEJiuzCIAXILYzkj6Z9/y5qh8VrFdS0RdI053+3SurkR8lU6ZPvkjHuK55ZfTtzR0NaePqRl7KWpynhm81KK40nw7p8fkWxc3N1LInDJy2cntwOe9cP4zt3vdfstStCim8iHz7wBG+0fOxJztG7k88jHevR4RL4d8LXNxZ2j3F7FaiK3yN4CH5fLC552kfMT7njOK8Y+JOoyQumiz3IudcnHnalPHlRCpyVhA7Eg5YfQdhVUYy5lB6v8EvIwqTjdzei/NnnN9YwS6rO1rzaRsY4mzneB/Hk9c9auwQhF4FWBEAMAYA6U8rhRXrJWR5knd3IMU1hipmFQzHtTJKV5KIoWY9etYH2iZJlmjYo6tuUjtWpqDrLKEBz3IFZlwBuxjHOKliPV9NuReafb3A/5aIGP171K9YfgecyaIIz/AMsXK/gef61uSVIyvJVZxVmSq70AVpBioGqxIciq7dKAGUUmaKANNRUiCkQVKooAelTIKjUUl1cJa27SyEDA4HqfSgZgeKbxXuo7dekY5PuaxJDhSaSdmmZ3fO5jnPvUe7KEN94CtFoiS3bjEKZ9BUijmkjGI8elSRDJpjHRjml2bpBTwMCkjHz0ho19C1S90PUIr7TJvKuIz1xkEehFep6T8XtNH73WNCntrvGGutNkBZvqGwe3qa8e7UVLSZSk1se+w/Em2uohcac95NbBgHknZRIpJx9wc7RxyR3rM8H+I73UvHFzdStvh8zDM+Cu4lFjACk9i3PoCe2K5H4TzwWd9PPcRW7KZoEZpUyUTcSSpzxgha7vS9PX/hKZbt9O2afJciVB5RBdgjZIH904P071xV3yJno0U3C/c6m70y8mtGOk3UkhlDl4kIXc6sQzpnIDAbfUHnNeD+JvCrPaXOuWEUzyRti+JUcv/fwCSM89fQ9cV7rpmrh799KmuRHG8T3NjcQjGBGcEHk8EY6DFZMM2kwafFfW88jrJC6atCwJ+YY3EA9w2SPf6mow1W8IuO23zFOF21M+dLdxIBipWWun+IXhSfwzrLSom+wmCyLLGCY8N90g46H+ea5aaYKvBr0Iu6ucE4crsRyECqkrZcD6/wAqJZ8tgAmqcjEzkcg+WTz9RVGZXmmSNiFRAc9QKzJn3zelXfs+CzO2apbd0xI6VLEdL4Lv1tb97WQ4S4A25/vD/Gu3Y15VJuhCSpw6MGB9xXptrcLdWkM6fdkQMPxFSxiyVVkqxIarOaAK8nSq0hqeQ1Wc0ANzRTM0UAbyDipVpi1KooActct4tecXaKpwgTKjtXVqK5XxNdCe9SJANsIIZvc047g9jnGvZYziWFivqtPWeKdcxuAw6g8Gpd0bcBgarT2EchyMZ9qsRtR42A+1SxYz1FQQ/wCpUe2K7HUbzRj4QtLO1tojqSyK7ThMMBt5Unvz/T0qZT5WlbcuMbps5ljxSxjvSBNzc07702B0Qfqf8/rVCJmOBSD5uBQw3V6T8G9N0m4vrqbVFjleNkWNXx8qnOWweM9B7VFSfJG7KjHmdin4DULoV8ZDsUSeYGOcEhcKOncnFdr4Amn1H4fxXmoTSlo5xbMEJZ0VsgEjPqyfhXWTaRYCRHgW0eyaSNXMKhYRuccAgYJyW9zuFZXw/spo9SvtPltTDaW9zPHI5OFbJ3ITwOm1e5+8K460XNuNtz0oVFGmrPYi0LSL1tbuyoeeGDTktSwX7pJfhQVIOCByMcjvV26sbyPwmNBvIIftMKeZJdBwflbd1HUnOc4/niu+kmFlvmiWQQR5IjVD+8Yk59+p7DrXnuqXaQQRahb6bcQjUZJIDBcMweU5AAHPGTyMdeeOTWWHw8qKte6vsS6ntXdoy7PVftXw2tdF11bfypZns2lncgQxDcQSfUbSF/4DXz3JZ3EV4YbnIUcq/Zl7GvatO1SHQPFB07XV+1goLW7tG2Mo3fMjc4UkAAE59O9R/HW60fVtF09vDqpNc2Cs0nkptEUG0ZBGB0447YNd0Za2OepT0ujxa5lgtVJ4+prGt7r7RezPkYCbR+dZ+tXBlIwenNVdNlKFsZyxrS5yG9Mu5CM1FHCoxSbv3e5qas6jk0ALfD9w1dP4Ju/O0gwsfmhYr+B5H9a5S4mV0K5rQ8IXH2fVGi3fJMmPxHI/rSYjtpDVeQ09zVeRqQyKQ1VkNSytVV2oAM0VHuooA6lalSo1FPWgDnvEHiJrOV7e0TdIOC/ofauTe9eZz9oDLuOST3rV1KIx6hOrcneaqPHv4Zc/hVpElCS1H3o2I981Az3MPVty1prCy8AfL6VXmjBYgnGKLAbcGDEmfQVaUccE/nVOzbMMf0q8pplD0XkZZsU9VCk4zyc81HuxUiHNAyRRXcfCCwN34uW4Fqbs2MElysIXO9gMKP8Avpgfwrh91e0/s8R2iNq09xcW0czeXEiSSBWZeWOB3GdtTJ2Rcd9S9p+mXcFxLc3dpexRSS+ciSy7IVfghQOCWBHTuQO1T3Ut7pPxSvJJJ7u20i4kW4VsbonyqxtjOcnLgn/dr11Jo7yzlAKyKzbchgwPA/CvKvEGoG38Uado8zLLpksjs0cnYhTlQc5AI49PwzXE52qRi9tfvO2CdRSmyW38Wxa9f3EOmQ3P2iG4e2jnWQBWYsyqAgypP8W4nqCeOK5+xk13XvEUGnzQlfs06RNGJCUQJ0OSTyCpJIxkkV03gFbK/wBclm06NUstNWQosSgLlidpA9WJdvoF9aPD4jv9T1OOOZ7NYJTPJdn93MVIwFxkYJKsc4PcYrovtoJWV9dUcB8XtNhXxdLdXscVxYK/mOfO2PGDgEHHJXILDGepp2lzJqWnnStOs7a3s73dGqxLvL8EffIycZLE9ABj2rGuNWm1/UPE14bxvszEQxxFSRMmeVyfl4HPqcZr07wb4dg0TTI7uaX7TqDQ7DMeipx8q+g/zwOBndmitBX6nx3rNlJZald2c2fMt5Whb6qSP6VW0kESMPQ113xWRYPHusBMbXkEn4soJ/UmuOsZdt23PBFbxd9Ty5KzaNW8nBARe1U9rucnpWjFbI/zZqVrcKOBVWEZDxMFqNGkikDKSGU5BHatWYfwj8arvEC1AHY6TffbtPjlb74+V/qKmkesPw2+1bmMdmDY+o/+tWpI9SMbI9VnalkeoGagB2aKi3UUAdsvSsPxJrh00LDbJ5lywyB/dFbucDJ4rhNWnS51WeaHLKSFB+gppAzJkn1OWRpXClmOTmmrqc0XE8RHuK0Akp5LMPbNMkjb+Ihh6MKskqXF9PcRf6Iy+57isOae6SQh3bOa22giEgZT5Tfoam0bT01fVVtXbCYLOw64HpUsZPoMsn9nxGUNk5IJ7jPWtZZK1fFGnR2um2klqgWOD90QOy9v1/nXNJPx1ppjNISZFPV8jg81RjfNWUNAzR0u3kvr+2tlIBmkEeeuMnrivb/DvguSOS3sNKlnnspgs80gjXcG6bWcdBx0z3rwm1na3mSWFirowZSOxHSvp/4Ca49/4Yv5rwoZjeMW2jBOVU9zWVS9/I3pS5btLU5O20fWNJuL4eY1vHa3vW0xvdJHwVXOAexwT61malJb6348s7bSb2W9hkjmiUzqUZJTC/ynOPUc/wCFdH4k8V3FlrcrXFoALxEngixk8NxlgSCcZJ+gpvwz8GNeXd14g1ZmiW5kMkEeed211LH2+c4z6ZrClF8zlNbbHZWm1BJPff8AMwvh/PfQw6to8lm0t+JmBeGVcqCgVQcdtqke2eetdXrdlYHw/r2p6ihnWOMhHGNryKMuw/vYfI5z0qXRfA0Vvr8JLWssKRoB5IMbzMUJYvkHGeuP/rYofEzSbxJGdDFFZpbrZ2kEUzEDcCp3Ljn7w+uBzxVymopszUuZqK6njFqWPh02NgZ5GnkaSYMyiE4Gc5PORkZ9x717vp955nhaxkwSWhTOPpXP6b4BsZ9BuBHfTLPcLtkupoxIq/NgHAIIBKgd+nPetzwnGV8L2SN+82KqKcdccZrFNy16FyabPmH4xokPji9VAQdkZbPXJUH+RFcHasRcg+vFdV8QdSGs+NNZvc5SS5YIQc/Ip2r+gFc7CsJvIo5ZDFGzDe4GSorrirKx5s3eTZoQ3UkbcqcVoQ3iSDBPNRSW4iuJITztOAfUdj+VNks88rwasktsqtyKqzLsqAm4g6ZYU4XwbiVaALWj3HlahtY4Eq7fx7VuSPXJTEB0lhJ3Kc10Ql8yNWHRhkVLGOd6hLUjtUTNQBJuoqLdRQI7LXXdNHu2jzu2HpXH26BEAooq4gyyq5oaIkc9KKKoDF1a1PlMo+qn0NZmhX1zY6rby2wLSBgu0fxA9RRRUSA9vkgS7s5IJ1yki7SPSvKbxHsr2e2k+9G5U+/vRRSQ2TW8u6riPxRRTBE6vXq3wM8SrperPa3R22ksiu7EZC4Rsk+3GfwooqZpNam1Jvmt3Ok8a6NGPEltFp95D5GGltf3hcbXAwv0DE4GcdKs69pdp4Y8TeGrrS5JTFOv2K4ii3ZkGAAwHdgTk9+PY0UVhf3rHZO/LGTNKb4g6Hp+tNFG95JNGTbtth3bWwqAEDkn5TjHqfw47x98TtPvbiOHTre5uzCweQcxYOQMEkZH5UUUpUU1qxc9pbGro/xA0po0tNStrizimiJdhKJEAJJ+bHPUt9KTxLrn/CN/Bpr6LabiSMRW7Zz8z5AYfQZb8KKKiklc0xceRaHygX5yaqzEFyc0UV1nkG/bSM2mWcx5ILRN9B0/nV+G5Q/eIooqkMl3QyfxA/jVee1jcHGPwoopgZc0Jizg1paZc+ZbbT95OPwooqWBYZqYTRRSAbmiiigD/9k=</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRT/2wBDAQMEBAUEBQkFBQkUDQsNFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBT/wAARCADIANADASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwDFDVKlQK1SpXqnmE9L+VNXpS0AFFFFAD6KSloAXbQFpaetACBTT9gXrSjb1PFcreeME1C7a10x8xqcNdDBBPonr9fy9axq1oUY802bUqM60uSCuzqNyoNzMqIO7HFRx3sEzYjuInPorg1hafodrPIstwDcv/emYuf1reXw5pky4e3Q/hXjSzZX0ie/HJZtXlPX0JSrEZHNJ5RPtVCbwfHZ/vdMuJLJuu2I/Kfqp4P5VJY6xJDOlrqYSKZiFjmThJD2B9D/AD/Su3D4+lXfLszgxOW1sOubdeRa8kimsu0VemULxiqkvtXpHkldqbTyKaRQAlFFFABRRRQAop1JxQTQBlpJn2qwrVWVKnWgCyjU+oV709TQA+iiigB2PelpvNOoAOfWnrmmrRJMsELyOQqICxY9gKCbnlXxi8dT291F4csJCjSAPeSKcEKeiZ9xyfbHqareE38to07cCvOhqLeIvEl5qM2S11O0gz2GeB+AwPwr1nw1pDeZFtH+TXy2Oq+0lY+xy2jyQv1PU/Duji4jjC/MSO4rtYvCRKKAu5vZazvBNjIkYbbjavpXqmmwCSPc5X5QOK44U4yR60qkos801Lw69rGTtZePwrz3xJDHdW0sUiAjoQa9Z+IXiy3tVNrAwllzjCnNeY3unXN3aSSyRMgwTmuWpG0vcOiEuaPvmP4R16a6aXSr1y93brvjkbrLF0BPqRwD9R710LrXnqXB0/xBpV3wNs32eT0Kv8v8yD+FeizEHgV9fgazrUU5brQ+EzDDrD13GOz1KrUw1I/fioyK9A80bRRRQAUUUUAFFFFAFFVxTxShadigBV60/FMVsVJQAo9+aUGm0UAPpd1MzSeZj3oAmzXNfEzUjpfgHW5wcMbcxAj/AGyE/wDZq3/MGMmvJvj94ytbLSLbw+Q7XWoMsinOFCowPPrnHT2qJvli2EItzSPJdK1BdPaKRlLbegHc19AeENS8SXXh2G+0rTLGaI5OH3PIccHoeOQfyr5/l0a+fTUuLGD7RKD930/CvQfhZeeJPt0Ftca1bWVnKu2fclyJITn+BYnTcceuOvSvmKkI1Huj7ChOdJNWZ9O+AfilbX9sLHU7aLTtQ4UopIzj2NdZqmjrHH9qj1N0gdc8NwK+XdUs9bt9SsZbnUBeyRvzcYPzKe2WUHP1HccmvfvEWoT3Xwv0aOM4uZVYM46jBxXBP3G4s9ilecVK1joPDuhQXV4PITTBxhZNSmZnkbPYAcf5/DI+Kiz6O81lJHAmF3K9vJuUj6EZr591fTfHWh659stb9SI3DW8c80sCMuR991I28e56UXniLx3rutous2X2kMRi5s7pJYkJHQsCNwHT8Ccmt6kOWnpY5YVHKr717DNavvMt7gAnI+YY9q9Xs5PtVlBPjiWNXA+ozXjPi5G02Zo3xuIOSDkV6x4ZvBdeHdOIYF1t41cdwwUcH3/xr0sqduZHiZwtYy7F6Re1QNUkrGoWzX0B84I1JRRQAUUUUAIRmnotItSocdqAKNFFFAD1XuadQOKKACiiigBrEio2NPZvypjUAQSSYrxr9oLQWvIdF1dRn7LO0MnHQOOD+Yx+NezSLweM1yPxKsRfeCdZiKlmW3aVQBzuT5h+oqKkeaLRdOXLJNHCfDm9j3xK6qUx/F0r6H0Tw/pS6U1+8EELAZIVQASBz9a+NfB/ip7do1UkYPNfRPhXxpJeaSN7KIVxnd1Jr46pSftG2feYetF0klubbE+KtSkkt7ZmsreXyTKcAA5HQV7fJ4OuZPAtrcpEdkeQnofavjO88ceLPB+sXf8Awj97Z39peO05tZkJ25POGFd1Y/tFfED+xVsBZQaXcbd6NeTb064O1F5PXvisZYapvFXTOqOMprSbs0fRPhnxZ4cvpx4c8RWosdRjUeVJMBskHYg+lT/EjwfbeHdH8yzWDyZufMjOS/1rxaCbT/iJ4PWbWddA8VKxdNQtYTEsBHRNpPK5znJ59q56P4r6vZ2Mmi6zKZLmzwN6kskikHa6k9j+nINayU/Z2aMYyh7RNMw/GcBvb61hyFlmmWJWxnq2K9B8K+Fo/B1jcWKTvcO9zJNLLKxZmcnBOT9BXkdvrb+IPG2kQITkXIkOOo2/Nn9K9qWUcDNetldFxj7RnzucV05eyj6k7NTKbuozXvnzkRKKKKCgooooAVakqNaeKAKW6lzTKWgCRWOfWn1FmjNAEtDHAqLd70buMZoAViD2xTGbHekZqjkb5etACPJVS4jS4jeNxuVgQR6ilmkK96z9Q1CKxt5bm4lWGGJS7yOcBQO5NAkj5Z1jTm8D+ML3T5lOyGU7Sf44zyp/LFekafHPqnh+SKzu0gGfMG/JBGOhwQa8v+J3jr/hYHiqaezgVLOziKxyYxJIoYfMfxPA7CtPwB4hkkj+xebh/wCEE8GvFxFNX5ke/hamnLI+iPhB4N1bXLiMy6v4Z0hgrCK4e0efPygBSxBK5Bx0x6nmvoH/AIVvrWnq1xeeJPBEMrAwi80/TfPuJUxu4jVBgEnt3NfGHhnVvE/hXVkm0Sb5w+9beQErn29K9ttvi98WdStXjuNMtbGKZAkt1sPK/pXGkle56/Ne2/4f5G1q3hi71TULy0bxFDLpiqxzDpEVvKWGeSSWwMY7Z+leQeONQtrGxjikIe7TKFmGDjJx+pNd9Nrj6Vo9zcXtyWdgS7nALH0A7CvnPxVr0/iDVP3IaWWZ9kcajOcn9axhFzdkrIqtUjTV73Z6F8HdMOp6/dasyfurVfLVj3kYc4+i/wAxXtEYNcx8M7awi8I2cOnkOsWY5j384HEm733Z/TtXZrB8vSvp6NNUqaij4vEVXWqOTIQtOxTym2krUxTGUU7FNoLCiiigBVp6mm05aAMwPTt3vUPmD/Jo3igCcNQZKg8z/OaY8lAE5k96b51U57pIY3d2CIoyzMQAB615z4o+PHh7QWeK1dtWuV4223+rB93PH5ZpNpbjs3seoNNVO91CGxhaW4mjgiUfM8jhVH4mvm/Wvj94m1TetkLfS4jwPLTe4H+83H5AVwupalf69N52oX1xeSdd00hbH0z0rN1F0NFTfU+hfEnxz8NaOzxwTyapOOAlouVz/vnA/LNeN/EX4jat462W5j+w6evP2WNy24+rHAz9MYrlY7NmcGNlDphvmGR+VW7iSbycMiK5+8y5P5VDk2axgo6l74S+HrbxB4ybR7tvKS+haAS90LDg/gQKy9f0TUvh14uvNI1KM2uo2ExRjj5W7hh7EEEexrW8AyPY+LbO5U4ddxz9Of6V9w/Ff9nW0/aM+Ftl4k0mS3s/GGm24VWmYRx3sQGREzE4Df3WP0PByOqNH2tBtLVMzdX2dVJvRnyDpvxKjjhiE5Dtx8y/LtP1rpLP43zQrFbi4cIem9v4cn1OPWvI9U8B6po9/PZXME1pdW7mOW3mQq8bA8hgeQau6L4ButWuB5twygnnbHk14sqdLdntQqV7WR23if4kSeIFjto5DNuPyrHyW9gK9h/Zx+GMem6fr/xM8R22NM8L27XaK44e7C7oo/8AgJwx/Ck+BfwHstcvIIohDYWzSrDPrGpTJHHGxGdibiN0hA4T8TxX0H+3DdaV8JfgboHw70BEtotRnCuI8ZdV+eRye5JwD/v124Skm/aW91ficWLqOC9m3eT/AAPhH4c/FPUPh7rE25Deabcyb7i3J53f31PZv0P6j6T8L/FPw34uCLY6iiXD9La4HlyZ9ADwT9Ca+T9Ws45SGTCunfsRVWyVhGwYbRncpyM5xWqk1occqalqfcTmmNXy94H+NWt+GGjt7yVtU09eDFO3zqP9luv4HI+leu6f8ePCl4F865nsGPa4hJH5rmtFJHO6ckeh03bVTSdasNcthcafeQ3sP9+BwwHscdKu1RN7DdtKtLRQWFOWmjrTxigDn91LuqHcPWl3E0APaSq9xcLHGzu21FGWY9h6052K/SuX+IWpJpvgvW5pJBEotJVDMcfMVIA/EkUDPmzxx8Q9S8Y6xdSSXcy6czkQ2quRGEB4yvQnuSe9c7tG1WXlScfQ1UW8tdxG7H1rQtVVmChv3cnBPp6GuPc7bJLQ0Y7Mrbq56GmKoXtxWvp9v9q0h1I/eRtg+3Y1mNw0id04NUTfUfFHtkRuzAr/AF/xqdot0ZHXmnRQn+z/ADAOUIb6c8/pmr8cG4AAcEbqdhNlbw2wtdctGbp5m3/voFf619PeM/hR401/RtBvcyXHhjTbRGWx3na77d0rkD+IElfonua+bdDhh/t22FwP3BlXeR1AyK/Zb4Z+DbGHw7qmg3CLP9g1K5Xc38SSOZl/8dlWvawFaNGLk9bM8/FRcmrH50S+G47m3On+IrG4t0VMW+o3UZL2Z425kxhoDz8rN8vBXuDR8KfDefUPH2leG7gNbfa7oRSSqeiDLMynoflBIPQ8V9+r8LLZor/Ro7ttK8Q6Gnn6betylxa8hN4P3gBiNh22A9+auh/BKPxB4s0XxtqMNvpckUKSy28ceZFcDpGwIVcknJC5PrSx+Ho4qarRtF9fP+v+HNsHi54aEqcte3kzxL4//s23Pjb4fWsXh7TvsqaflLaJgyqoAIJRfqRljyzEk96+RvG2q60fD/gnQdcvZL2fRNNmRfNfc0Qe4k2pk+iomPQYFfsleTQ2Ni81xGqQQwNcNDjiONFyq4/M/jX4qeMNYn8S+KNX1S5VEknuGVViOURE+RFU4GQFUc9+tFasp0VHltbT5GNGL57tnJ3FxjzQYw7FuGYngenWqse4KHIA+lSXYZrjaP4jipZEVVCqQQBivIPRvsVGXqRRyYsHnmp4YN27PSmsoUAVIyzo99eaXcJPZXU1pKvSSFyjfmK9P0P48a1p9rEb9INQhVuZHBWVl74I4+hxXllqpNvIP4mIRfXJOM/rn8K1rrSUulVPMCIowBnGKpXMpJSep9a6XqVvrWm21/Zv5ttcRrLG/qCM1awfSvLv2f8AVC3hu70Z5PNOny5jbcD+7fJA/Bg35ivU62Wxy/C7BjFL6YpKcG9RTKOVyKN2Kj3Uu6gBJGPJrx79oqSf/hF7BFz9ma8HnAH72EYqPpn+Qr12Rh3NeJftIag0el6RaDiOSZ5WbPOVUAD/AMfP5VE/hZcPiR4eqvIMKkf+61WIbSSNgYV8mTP+qY5jf2B7H61FApWNZCSFbpt6mtzSzJIpH2USL6PL1/DbXMkdjNTwvqMcl06kbRKvzI3BVhww/kfxqrqFmU1q4ReE2byar3zf2dqFpcCJ4izbGWTrtPuOGHv19a2r6MSK0/8AF5ZT+tadDLrch0kLe6TOqnIYFauaWxuLOKXj5lBIrM8HybtKcE960vDrBrWWIf8ALOVh+Zz/AFFNAxP9Tfxt6MDX7LfAnVP7Y8O6TfF951TQtN1CRs5JlMAjf8QYhX413y7Zgw9a/V/9jrVl1T4LfDu63craXthKf9qO4JjH/fOTXVSe6OatsmejfF7TXutLs5LY+TfmdbSOYddkpCMpPpyD/wABFdF4WS3vnm3XKzJZsFMajgHnAP0wenpVPx8RNqXhiALvV78s6jvsikcfqorZh0ez0OzmuoYBC9y3mzAMSGbnnGcDr27k11OS9movfp95yWfPdbdTzP8AaT8bnwb8FfHetCTbOlk1vDjqXkIUAfnX5Bn9xaKCecV+gX/BQjxkbX4S6DoCOVm1vVzK6g9Y4Eyfw3Olfn7qeFhPauarokjrpbXMMyHfJL/dGF+p6f4/hVi3hMyhR1UYpiw7/LiA6/M349P8+9aGmj/SCWGM9K5DouPS18m0PqTWXaKt5dOWcJCG2gseregroNSU/ZzjA5z+lcz5flahChOFt4/MY/7THr+QoHE028u1uwjMAkI81z6HkL/M1Qa4uPEcxWKR7WxzjcvDyfj2FYl9fNeTGHJzcP5svrt/gX8ufxrpNPkW2hAlCwoBwGIB/Kle+g7WOi+G7ReEPHGkXFvd3EEckywT+ZJuR0fghh9SD7Yr6vr4xvLuKVR5MgbHIIzX114Z1P8Atvw7pl/nJubaOVvqVBP65rSPY5qvRmpRSDNKTWhC2OOzRuwKh3UbqBhJ0r5k+OXiL+3vGBsk+a304GFVPQyZ+c/mAP8AgNfS0jcV8i+Mr4ap4t1W6UgLJdSFdnAI3EA/lWVR6WNqS965nW4l3KTGrYGBmuq0ZkZQNhR+4wTXO2Sjjdkj9a7fT9Nhhto5bcs0xAO12wP5VlE3kyLxFp/2zSZF2ZYDcnqGHQ/59azhdGbS4W/56Kp/p/Krur6xLbQ+XeWs1sD92VcOp/EVkWMinTvkO5VZsEdMZqna5CvYg8KzbbCQZ7n+dbnh9guoXcXZgrjH4g/yFcv4fk2RyRnghiP1rf0tvL1K2l6LNujP5Z/9lNJFyNXVk+XIGK/R39gXWDefA23RpMHS/EbKRn+CSBAPw3Sn8q/OjVF+U4/Wvtz/AIJ16wr+AfiDZSNtSzmsb4Z7YaQsfw8pa6aXxHLU+A+3PEentea/4emU8288rMvsYXXP61d8XXhtbMR5ydlIsgk1eHPO1JCPX7y/41jfEK8wyBSRlVX6c/8A1q6Y+9KKOV6Js/PT9vTxM2q/FrQNDVsxaPpKyMvpLO5Y/wDjqx18vakPMkRM4Dd69N+PHij/AITL41eM9XRg0LX7W0JHTy4QIhj2+TNeZX4A85ye23/H/PvXNUleTOumrRSK1mBN5zD7xB2+3HH9Kt3ULW6pIvGKy9GusTOZGwqkY/Ot6S6S4h2oQ7EcBAWP6VijTqI0i3lqijq+Bn0Ncjq90PtF9t5Mkvl8d1VR0/DP51uSRz/YcJHIJAx54UZH1rhtWklt70QygpIzM5XPqMVMiorUsWazTTMbdSZGPzyqcfgD2H0/Suht7BrCJXMRmdv+eEYb83bJqjo8j4RYvlVRwqjP51sC/KE7LWaSTttDH8fT9aSKb1K8l3cXmY10/n+85K8fUV9OfBC8a7+G2mB1KPC0sRU9sSNj9CK+XpVklz9o0jJI/wBfOC5+pA6fhXvv7NcxXwlqNsZXbyrwssROVRWRcbfYkGtI/EY1fhPX6axopjGtjnjscR5gHWjzBtz2qsZKQyUiin4l1UaVoWoXmebeB5B9QpI/WvkWMl5gSeSc19G/F++Nr4D1EA4MuyMfi4z+ma+cbcfvB39q56m9jppbNm5psck2Vij3nucgAfUmu30W0eKEJLJGzZ4EZJI/GuR0mEyOoaRUA6KSf5Cu00+FIYwMLvHQ5K/jyBREcma3h3wnd+MPHGgaPbWD6sl5eRrLZqwG+MMGfkkY+UNzmu6/bG+Gui+BvEWi6j4b0dtAt7uNoNR01YSkcMyAYdccAMp6DHK575PEeG/HF/8AD3xno+v2kZM9pOG8tf41PykD1yCRketfXfxC8PW/xy08/aY5oY9Y09hDJMCDBcouVTBGRlScZ6FAPSvLxVV0a8ZPa3/DntYOjGvh5RXxXPzf00bby4Xt5jfzrfkby7dHBwIZFf8ADOD+hNU7jR7jQtb1Cxuk8u6t55I5EPZgxFXNhuLWWLuykfpXoxd1dHlSTTszemlEke7HDDIr6e/YC1w2+ofETSg3F14enm/GMgD/ANGmvk62uvO06NyeSgzn6f8A1699/YU1XyPi9d2mfl1DTLu1/wDIRk/9p11UX76OWovcZ+p+k3RupVuE+ctBvTHQhth/rXkv7QHj6+8K+DNa1SaFbaays7iWOE/3guY+e/Oc4/Cu7+FFy114Y0GdmIZtKt2P18uPP6186f8ABQLxUuleA7i0EmJ9SmitU7nbu3t+G1GH416EbQm79Lnn2crHwD5rtGWclnIyzE5JJ5J/Os+4hadXjCmRV4YLj7xwe9TLMu39SPX2pbbcjJKOdw+f615m56Rl2omsZh5cUUT54bJz+eDSXV5JGPnkBdRwQvI/HINa16kNxGSWAcc5Uc1y2oXQZ2XvUPQpakdxrl1DuaNsN6tz/OuVmvJb6/eWZjJIPl3Gte5b9yc1j6Zjzmf/AGs/rxWbNkdXo8MdtHmcBpG/hx0rpLWaGRceSnPA+UVzFmxbnn8q2baQ9Aeg9KtGckbHlJIpULGc/wAJWuz+Bln9j8eTCDbAjWknmoGbD/MuPlzjOcc46Zrhbb52HtXW/DPUBp/xA0ty2FmZ4G99ykD/AMe21otzGWzPo9qhkYipGPFVpnrc50zz9pTmkaTjrVdpKPMFQWcF8bpiPBoXOA1zGP0Y/wBK8HtRvkBBOCdo29ST0A969y+NfzeDs+lyh/Q14laslq0E+QfJjaTHoxOB/LNctT4jqp/CdPpMbRyKgYgZw6QHaQc45brk1v32mx3EMQjDSYH3ndmOe/JNcp4dkNrb3Luf3iptGf7x5P5E4/CujstcMcSIwGeme9UrWFK9zS8K3V94X1vTtUi2zNp91Hdxw3ALpuRgw755xzz0r6C1P9tjxFrUNwdX8M6bLPMsXlS2MjwMrRk4kO7fk/dHb7vOa+f4b5JYyW6t0WrDQpIFY4rKpQp1fjVzaliatD4HYofFHWLbxl40n16wsJLH7Woa5hdw37zuQe4rmFmMasGGD054rr308NuYDNVn0vbwVyAO/rWkaaglGOxMqjnJyluzjdNvCdPlQ/wSMv6k/wAiK+hP2DMzfHjTIwcnybr9baUf1ryRtMSRsPErL0PFSabJc+EdRtNT0e4n03UVk/cSWsjI646tkHNaQ92SfYyl70Wj9jvhEzx+CdD3DaV06OP8sD/2WviH/gop4n+2eO9E0ZZMpbQPcSID0LEKp/R6+cLfxd4ihnuZB4i1JZ7kBrqf7XINy/3Tz09qyLi3fUJbiacZBPRuSf8A69dlSspc1upzwpcrV3sZS3C+YAWGByx7Y7VO2pwRr8sgxjHymom0cRyENGGX3FffX7I3wE+G/wAWvgTHJrfhDTLjVY5rnT59Q8gLO/O9W3DB3BZFAbr8orljFyNpS5dT887q+Dk7ZcD2NZNxMWyS2fevqnVf2ZNAsrOe1W2O4ElWEjFwenBzn8Dx/KvPbT9nLTL0yr/ad/BJE5jdXZDtYH/dry3jKdrs9dYGrdRR4PeTEQse2Kp6YxUDFe+a1+y0xspJLTWpDheFljDZP4YrwVYGsZnhbh42KN9QcVdOvCt8DM62HqULc6N+1k+Uc5Oa27IgDofriuatpvLj3FljHqxrU0/VIZJMC5U7eo7D8a6kcUjqLf5WBHJ96msNQ/s3XNOvB8ohuopT+DA1HbMskPmKysuMhlIIrM1STbGxB5ByOa06GZ9jPJiqFxJzinx3AktYpAeHQN+YqncP1NdJyxOA3ZpS1R04moKOM+K0JuvBV9gZMZST8mH9DXgWnYmuoonOE35f/dHNfTWvWA1TSbuzbpPE0Y9sjr+dfL0kb2d9JFIpSRSyMp6g9CK5amkrnVS2sdDaXWbPPQyu0hH1PFXIptuPzrDhmIUL6DFWBebeKm5pY6K3virBq0IdaI/irkFvPQ1NHdFetXzE8p3VrrkZG1up7+1W/wC14JG5+71rhI7puxqxHMzsAOtPmI5TtJNQtkjLNgKAWNU7WYXVw8zjBUbFXqF7n9ePwrmoZWvLwxBj5UfLe59PwrQgmlmwuPIgB6KOT9TTTHymrPMJXKRDdGpy7f327L9K1Iv3kaAg4HJY96yo54VRl3iNUXIwuefSnPrSW8aqXLbyQcqAFxjHOee/ancOV2ua8jK7EMvAPWv0G/YBkEPwh1QA4jGtzED/ALYQV+edrMk6q6kPnJ4r7F/Zt+Kmk/Cb9nPW9U1fUbawEmq3CWiTzCMzzGCLagyfXr6DrgVvT1ZjPsRzeI4tYupk2j52OGAHGff0rkltYl8bX8MWCksSswA4EiBc9u4cE/UV4zY/tH2lraO2l6fJdzsdqtKAq5rm7P4neJ08QX2ttJCmo3SGKIAb0gj4yqg8biQuWwelfLQwtWXNpufX1MbRg4WezPovX9Z0vwxZvPqt7FYxnOzzD8zEf3V6n8K+ONV8PW+peJNSvIWb7HNcySRKVwdpYkZ/Ot+4vLnXLx7nULmW6uyfmeVtx69B6D26U5FFqRuwYicBvQ+lenhsIqGrd2eTjMc8VZJWSMiTwjaTW4LQnenKsrEE+2aaNPGnzwPDGzErkLn5zjrtPcj0NdMs/lcqOf8AP/1qoatCbywdYh5bxnzYiOqkentXdbseXdlH7CskYvtLlCTtyQOEl9Q6+vbPUVlX9x5iZ2tFkco3VT3FSQ33lw/bUOyKRvLu4wfuP2cf19R7iqN4H865keTf/tZzn0P5VPQpI+wtFmMmhacx/it4z/46KJ2JY+lQ6Cpj8P6ajfeW1iB/74FE8nNdfQ5Dh05wal6iiiouK5BMteJ/FvwTNDetrVjEZIn5uI0GSjf3seh7+9FFZz1jqaU5NSPM0virdcVMt5uOSaKK47s7iVbwDknirS3oXB3Kfxoop3EXItQHt+dW4dRVfm4z9aKKrmYEVvqv2JkChXeR8c56nvxn+VWm8QMzXCLb/wCqO1sSEhvnA+X5eeOecdD9KKKXM7mkYq13/Whdu7uW25jj3jaWbzM8jpgc/me2RTpMt5ZdQ6yDcI8/NEeOD39eo9xRRWpzmjY3Edm2EmHlt1Unoas3UKane7pZvPRECwwSMSgJAJIHQE8ZI9PaiiquT5kC6fZXURMcQRlBWSNQM8HkFehx/X3FRW/nRghG+1wq+3yZGxIh7YJ68dM+/I6UUUyS35dtdMJUkNpOOBLjHPo4/oauR3C7fJvI1VyMB1O6OQf0+hooouA1ZBbsEZt8J4SRjyvs3qPQ1Y3DduDYb0FFFFwMTUbVdPu5LqFFkgmXbPAeh96xltpLprazUZkuJViRf95sAfrRRUsq+h9hsRHEqAYVRgVQl+ZuaKK6+hx3P//Z</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/4QCORXhpZgAATU0AKgAAAAgAAgESAAMAAAABAAEAAIdpAAQAAAABAAAAJgAAAAAABJADAAIAAAAUAAAAXJAEAAIAAAAUAAAAcJKRAAIAAAADODQAAJKSAAIAAAADODQAAAAAAAAyMDIyOjA2OjI0IDA2OjI2OjMzADIwMjI6MDY6MjQgMDY6MjY6MzMAAAD/4QGgaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLwA8P3hwYWNrZXQgYmVnaW49J++7vycgaWQ9J1c1TTBNcENlaGlIenJlU3pOVGN6a2M5ZCc/Pg0KPHg6eG1wbWV0YSB4bWxuczp4PSJhZG9iZTpuczptZXRhLyI+PHJkZjpSREYgeG1sbnM6cmRmPSJodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjIj48cmRmOkRlc2NyaXB0aW9uIHJkZjphYm91dD0idXVpZDpmYWY1YmRkNS1iYTNkLTExZGEtYWQzMS1kMzNkNzUxODJmMWIiIHhtbG5zOnhtcD0iaHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wLyI+PHhtcDpDcmVhdGVEYXRlPjIwMjItMDYtMjRUMDY6MjY6MzMuODQwPC94bXA6Q3JlYXRlRGF0ZT48L3JkZjpEZXNjcmlwdGlvbj48L3JkZjpSREY+PC94OnhtcG1ldGE+DQo8P3hwYWNrZXQgZW5kPSd3Jz8+/9sAQwADAgIDAgIDAwMDBAMDBAUIBQUEBAUKBwcGCAwKDAwLCgsLDQ4SEA0OEQ4LCxAWEBETFBUVFQwPFxgWFBgSFBUU/9sAQwEDBAQFBAUJBQUJFA0LDRQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQU/8AAEQgAyACuAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A+QC3akpB1pag1HBSx5qZRwKYgxU0a5qQHKp/pU6L2H0pqrmpkXb9ak0SFVOlSj2pvGKcq7uopFpCjNSKppk00NnGZJpFjQfxMeKwL7x1bW+VtomnPTeflX8O9NeQnJLc6ZYSwzS+WV7Vwc3j7UG4jWKIey5/r/Smw/EDUUb5/Kk9imPw61VmR7RHfhO2DTth6VyNh8RomcJeW5jHQvGcj8R/9euqsb+21KLzbWdJU77TyPYj1+tJ3L5lLQkKe9NZPTip6Nu6lcl+7qimymmMv4Grbx1Cy1W4t9UVmH51GRVllzxUJQ9KCGiP9KQilxg+9BpoDGWnL1pKkjFNldCRV7VPGO1QrViMVJSXVki8dOtSLTVXdVmOLPJ6UtTRCRxlq53XfFyafI1tZqs044Z8/Kvt7n8an8Wa8dNhFpbHFxKMlgcFV6ZHuecVx9rp7TfNjI/OmrdTNybdojLq7uL+bzZ5Glcnqeg9gPSo/IJ+tai6eynGwjsfWnNZuq5IwMdO/wDnNPmXQXs3uzHe39sdhmoXt8deta0luVchgBt46/pVe4hPHOfxppkuPkZZU+lTWV5Pp9wJreRopF53Kcfgfb609l9sVHJEetVcjl6o9D8M+OI9Q2W2oBYLhjhZFGFb0B9DXWtHXhSuQ23FejeBfFRvgNOvH/fqP3Tt1cAdD7gVLXVFxl0Z1u31qKSOrRXt3qMr2qPQ0trdFN0PXFQsufrV6SOqsi7TTI33KzD86bU7DIqIjFBJiKNxqZVpiDpUq02X2RIgJIGKsIvc0yNcVKvpUXNESxruqyOBUcS7abqEpt9PuJRwUjZvyBo3H5nnuoSHVdYuJ85Bfap5+6OB+eK6fS9LCwIhHXtWRoNiGjRiNx6+3riu70ez+0SouOO5rCrLojswtJP3mV49DR/mKjPr1oXw2rSbiST1+UYHWvSdK8OpNGpfaq/3cc/y6U+60WKEFlVRxjjJrjvI9j2VOR5ZqXhEzqpQY/z1rGuvDfl/K27I6flXqt9brGoJbj8vwrm9SRS3Azz1NaxqyWjOarhYbo81utBkjYkLkdaoNpxyfl5rub5QGx0rHuIB8xFdUajZ5VSio6I426tmhbJHeoFmezmjnjYpJG25WHsa6DVrfdFkda5+4jwpB4rdM45KzPbtF1BNY0m2vUGBKmSPRhwR+BBq2y4rmfhfcfaPDPl94ZmX88H+tdUy5qbGsdVqV2XIqvIn51cK4qGRaNSGuiKDLtqJqtyJnpUBFBJhxqcVMq1GoqeMdKT3KXckXtU0X3vWogKnhTJzikWidVPSq2ucaLe+nkt/I1cWqmtDztIvY0IL+U3y59j1qkPoYWiqBawEdSuSa7fQ/wB00bY69q5LR4j9jtht52r+td/o+lyTLG2wlV64z+f51yS96R6lG8YaHrPhG3tp7MI2MMMbSwyeeR06fj3FU/FGmw25Kxtk4yvOemRjP5VP4XheGFF2LnbgjGOAP6/1qt4iPnSFAVG3AOPrzUuKR2xbaTOG1hAtrGmASXyW/Pj+VczqO1V/2sY610usMVyCOF6f4/Tmua1EbVJbr1rIqWxz1w2WPpWVcMMnmrepSFDkdf061lSsXPfNdcEePVlq0VL8gr681h3keFcnp9PwrdmXfwetYuqL5aFT1PFdETil3O7+D+W0vUAfuCZSPxUZ/pXeyJ8v6Vxnwft9ug3cp6tckfki8/mTXbsu0VDdmKJRcdajdaszR9wOKh2/nVX6op90U5F/Oq7p81XpV56VWZeaZm1bU55FqwoqJKmX7tQUhyqSRVyNdq4qCFckcVa74oK8hV6VxHi+2mjUiJ3E7zEeajYAj2lmBPqBjjvmu5VcmmawI9d0SfTb+5ntNMtXV/Is0QPPI3HmFyOuCEx0+UVElJtcpvBwSamVdBjjV4ixGxFzj8K9h8I+KtD0vT3/ALUiMCfKVlUA5XkEk/XHWuVm8I/D7Qvh5Jra+LpJ9Ygt0ZdEkEgneRmC+WGMSqSM8spIwD+PDeNNSv7Lw3p1zc6ddQaddwyT28hvoh8qkBsZXlssPlBzyazlSXNqztp4hwh7sT6Nh8aeGL6EppN0sh6Y3AEenHr07d6xNV1JWkDImXLYUYxg/WvkO28QFf38Ms8IDbQ8qjG7HTIPUD2r2HwD4+vLi4jstQVpH25V8joFJJ6+gPT0rGdKa+HU6KOMpz0mrHoGpaSq+XvzlgXwcepxjjtXN6hpLTK+EJX+9n/PesrxF8VtJmnC2NwbgxLhmwyj3B49TXD6n8VLiZTFFPFGOmMnPt2/rWcYVG9joq4jDxW5t6h4feWQ5cDHbNYd9p5tCQWya52XxFrM6vKlx8n+yVH9apx+ILrzMzuZG6H5gf612RjNbni1KtOXwo3W5asDxBIFdB1LfLj8alm8QK3EanPoa0tS8LyQeHtM117+Gea/Z4Y7dFYG3K4LE56kBl6DHzDrWjmoNX6mKpuony9Dv/A1xYaLpFhpb3cf2+RfMaLdkhmOQD6HBHU11bL8pryXwTo/n+K7CBC3kQqbmRgeWYHAyfqRXsDKMcUS3MttCkyBlINVmXDe9XWX8+lQSp3qYvox+RTkGaruuTVyTFQN1rUTWhzEdTDtUSdM1Mq8ipCJahX5c1Mo70xRgVIKBoljXdj9ayvEMv2Py3xiN2UO3YYYEfqK2Y/X8KydYiW5uooZBmNhgj68Gs5SsbU1zSsaF3pC6ld2UJHzMN2evAGc49M1peL5rO58HxaPdQeeFcSiKNDhGxguuV+UkDna3OeRmtXw34R8S/Z7e/srX+2IrWJokkidVmCEAjcGIyQPQnIFWdP8UW0Nw8WvaPqolVtoVbCZu3AJC9foe4rKykrnp6xunpc8Ut/Dl/qSx21tYm30+3bzWaRcj3J9zWzb6Zc+JviB4Y8NWBks5W2m9kt/laOEEk4PY7SF59e9eva342tI7VRpHhLWLuUnKrNZtbRFs5ALPjv7Ve+GvhOPwsL/AF/VfLm8RakzT3DR52xZHyxIf7qgnmk6ns1ruKOFdWSS26nzt8XvDtr4T8UXlvpsTRWm4lVJJ6E559elcPpUK3Gt26zRGSLeNy5AyM88/SvZfixbrrkkgjwLhWMiM3qR0J9x/SuM0F9KvUEV0Vs71PlZJcKenrWlOfNDXc48RR9nWajsb/jzT9Pv3sl0mC1s7QHzZLeNAGRyiKQXBO5fkDDB4LNxXJ6podrJLH9jVlVVw+5iSW9fauzGg20gBSdSMfeDA/1qW503StJtwZr2FCf4S4yfQAZ6/hUxbiOUVNt2OAl0gtJbxnCuASzdeBjH55/Srd+0sliYvOwtvE3l7uQuTkke55rSkhDSSzqGEbHbHuBB2joce5J6+1Zd9BJcWssUZCNIACT6ZGR+Wa6L3tc5ErbHovwh0zytHlvH+d5CI1Y+gGTg+hJ/Su5cbQayvBECW/hSwRFwNrf+hEE/pWvN/wDXqWQys61BItWmHAqBhSYFKRetVyBVplJzUDLhjWqKOUj6VYi+9UMY4q1AoP5UugkWKmiqGpoutIfQsJwprL1P/j+iPTC5/WtRB19zWfq67ZIpOvasp7G1F++j2r4K+Jo7G4SCZ2ETDJ5JGccY/SvTPEPjDSNHmluEPzNtKgKM8FjyM98joO1fLnhvWmsZPUdcdutd7psLeKtQhVpRsJw3Pt0/IH864lfY+jUo2Te50OseNLjxNIkKwpESfMDFRnB6H6nI/StVfB+pLoT3bWzmHb1bHX39utJc6XceHdQOoaHJDFcKig29yoaJ8Y5zjg/Uf1rKuP2m9YXS7jQ9RFpMF4Eke18EdgQOo56Vy1ISbvE9CjVhBJTer7nlPjTw+u+R1Qq5Gfx715rqFqtp89xbLLHnlsc+9dJ44+LcIvDGsJL5w3UD8BXJXWvXPiJPLVVjib+Ff612UYzUVzHh4ypSlUahqdToXhPR9ZtkmihiCNz90emcH8asXHh2z0tv3EMUZxn5UAP51ieELltAkeJwSkn3ee9ausa0MuDyT1q/eUrGd6bp81tTD1SRQpA+lM0bTX1jUILSIqkkjY3PnAAGT09ADVW7m8w5BHWuh+HaeZ4ogI/gR2/8dI/rXYlZHkyetz1G3tUsbWG3iGI4kCr+Ax+dNkqeTpn3qBulSZETdKhYfLU7DNQN0oArSLtyfxqq3XpVub7wHaoG+9zVruJaPU5KMcVatx8xqFRnFT24xmn0K6FhV+YVLGvSmKPmFSqv+FIepKvSoNUt2n099v30O5fw6j8s1Oi1YQcdOvFQwTs7nJW92Vkyp56V23gLxE9nPLIZcSYJVSeOh5/GuF8QWb6VfCRR/o8nKn0Pcf4U+ymuHcG0wXxg1ly9D0Y1no0dj4k+MWoala3Ftp9uXd/kWQKWOScHA9M1y8mh3sdmFurWbzD0klR8Z6ZHseetd14cm8QeH7eER2ltcRBVljaCMK0itkk8g8ggg/N1rU1b4n3kIQ3thfrHnD7Y3kU8dyAfepcuVWijoUPa2lOR4nr+gyXjbpbR89pFj4HHc471zNs0tgMlGRs/NuUAYGAD9TzXoniP4gG6mfyLa5uIwx2sY3C47EcVwmp6tqWoS7Y7fZv4+cDHuTW1NtqzOCvBRleLLcGrrqELITtfpnPQ9jTbnUDc26Ox+ccN+HBNZNvG0O4sQD1JAwCaa0pK7e2c/nV8qvdHP7R2s2XEn3MPTpXoXwpsy+o3l2eRHEE/Fjn+Sn8684t+eK9ViuD8M/DPg+/vtpsvES3EjcYeExyBFc+qke3aqeuhnfqd1IO1QnpTllWZBIjB0YZVlOQQRkEH0xTXHyk1mBHUMlS1A3WgCtN3qAj14qd85NQ/xGr2FexzUa5A+lTQ8NUcK9PpUsf380FIsqPmz+NSp96mYNSJwaARIi/Lx9alhPamRr3P0qVVO4kUu6DyI9QsItTs3t5hw3Ru4PYj3FcjpcVxpd/JbuSssfI64YdiPY10+ra7ZaHb+fdzBB0Cjlm9gK9p/aN8AaZo3hP4XXmnxrFqb6DG03GPO3fvQ2ccndJIOeny1Mo+7c1pfGkjgPBPjy002N7LVYv9ClBVZDkmEngnH90/pXpeu+LNB1HS9MgstNhEuzE13HIMSZICnHTAAGeO1eIWLadqUbC6/cyLwcDB9CCKrX3ge1kYtaa/JaREEhY8jk9CVzz+NcjS2Peo1p09UrnX/FvxBo0OozpZ26i2yPL5+bhR2rwvV9aikkkMOCzcEjnHrz61b17wncRTES6xJdqP75IHT0z0rm7i1issqrZ7e1dFKKS3POxmInWneSsQSTF/aq7S8kCmXFxlsDiuo+Hfw51r4ja0ljpFm07ZBkmbIiiXP3nbHA6+/pXSeU7yeho/DDwLf/ELxRZaRZL88zZkmIO2GMctI3sB7+gq5+0Z40svFXjiLTNGOdB8P266XYkHIcIAGfPuR+lelfEnxFpP7Pvg+bwX4YuBc+LNSixqeqLw0MZHKr/dzk4Ge5NfM6p+VVHuTJ8q5T1D4R+NHVhoV6+VPNq7HkdymfT0/GvVTnGc18vwyPbXEc0LmOSNt6svUEHII9wa9c8F/FJNSVLPWClvcnhZxgI/sfQ/pUyj1RMJLZnoFVzVnb8uRyOtV5PuntWPkbFdu9Qk1M/yqarMxqyepgx/dqVetMhUnrU6IA3NBaJlXgVIBVa51C209C086RD/AGiM/gK5LWPHzNmPTo8dvOkHP1A/xqkmQ5JbnXajrNposJlupljHZc8n6CuB1v4lX14xi0yP7NGeBIwBc/4Vzt1JNfzGW4laWQ9Wc5P0+n0pqqsanaOatRW7MpTb2Kd9czXEwM8zzzNyzyNk1+p3xp+E93r37K3gjVEheXWfCmk2s00SqS8lv9nVZ1AxnKjD8f8APOvzP+HfhlvF3xE8PaQRn+0NRt7Q/SSVVP5Amv3ft0iSzSEoDHs2lMZGCMYx6YrblUotBCbhJSR+QOpaHa6wonSVoJWXKzxHIIxwSO/51ztz4W1SHOL+CdPXcVP4g/419F/tMfAPUPg94su9U0HT5rnwHfFrhfJUt/ZUhOWjYD/lkSSVbHy8g8AVz3wt/Zz8ZfGC8iNjZy6Zoxw0mrX0RWEKQDlO8hI/u+2SBXkezqRnyWPo3Uo1KftG7M+etU0fURFtBiL45+cH+tafgz9m7x58RZBLp2mSm1bn7XOpigAz1DsPmwf7oNfp98Nf2U/AvwvjgnSy/tzWU5bUtRUOwb1jTG2PB9BnHc13+pabGYSFQDjPSvRhRaV5Hi1KsZP3T88/A/7CFrp8kdz4q1STUHXlrOxBSL6Fz8xH0Aq38avivoXwH8P/APCNeEbO2ttVkXCwwqNsIIwZH9W47nnHNe0ftbfHKz+C/hGOy0945fE+pKwtYMgmJehlYf3R29T+NfmfqN1d61qNxf308l3eXLmSWaU5ZmJySf8A61XKKRm6nKrRKl3eXOqXs95eTPcXM7mSWWQkszE5JJpoyanuIDCo9T0qxZ2R27iOetBzPUq+SeF6FjU32crVm4hMDRP1GcH8f/r4qwsW5cjkUAdF4R+INzoKJa3oa5shwvOXj+h7j2PSvTbHVLXWLdZ7SZZYzx8vUexHY/WvCvKLZ2jIq/omr3ehXguLV8Ho0Z+649D/AI1DjfVFqTWh7VL0xVV+GPPeqmi+IrbxBa+ZEdkqj54WPzL/APWq1IvrWfXU1WruZC4jUsSABySeK5LXvFckjmGyby0HDSjqfp7Va8UamW/0SJsAf6wj+Vc0sG7k1pFdWRKb2KkjSzuWldnJ7sSTTfLA61cePbULLzVmRAy+lM2HFWGT0FLJCY4c+tAHon7Lukx3vx18IyzyrBaafdtqlzM2AEhtkaZiT6YT9RXafGb9qbx18UPF1+jaldaZ4cn5sdLt5niijhBIUuFI3ucElmz1OMCvGfDN5c6dq7C1laF5bV4HKcEo4w659CpI/E19J/tGeBtJ8FzfCzQbfTY7bVo/DgutQuADulaWQlVb3Vkl/wC+qJfCdmFi5VEl1PN/hf8AHnxh8B9Qv7jTli1AakiiSPU1aVPlOQUbdwee/XIr7a/Zi/bq0H4q30HhLxQV0DxRI22zeRQlveEniNW3HEnYbj83GOeD8OXlpGunvkZNu2drc5GOePcZ/KvPtYvLfTb5ntY0RCdxCqOueq89T7cfSsoVGerisFGC57n7lTRtnmvN/jT8TtK+EngnU/EGrSYit4j5cIIDTSHhY192JH618xfseftyXfiL7F4M+IccwfCwaf4gmO5pWAxsuB9RxIf+BdN1eNftqfHE/Fv4kS6Npdx5nhnQpGhhZGylzODh5vcAgqvsCf4q61K6ueC48r1PCfH/AIz1f4oeL9Q8Sa1MZry7fIXJ2xIPuxqP7qisOOyJ/pxWgse0AdBUiIO4qbEGTcWXn3EWFO0dfwPNWvMSPMcSea442rjA+pqW+iLKrAsI8/vNvHy/5/rVq3t0jUIgATGRjpQlYDONjNc83DhU/wCecY4/E9adNGI49qjHatRo9qniqkkIZjmnYCtBCFjHrUnkq3JUflUyx7m9qkWOlYCtC01jOk9tI0Uq8gg/p9PrXXab45jmi230bRSr/GgyG/DtXONDmo/s5NTKKGm1sJJulkLNyWPP40NHgVOYwfrSsvapEUmXcKhEWWNW5I8U6OEeXkjnrQBUWA7qLiMtsX1OKuxw9CR71G67rrJ6KM0AdR8D/CsnjT4u6FpMURl+1X0MbKBn92HBcn2Cgn8K+i/2uNQ/tb4+eIgvz/2RbWtrHyAOIhKVB9MyMPzqD/gmz4HGtfEzXfE00eYdJtfLiYjgSykjI9wgf/vquD+K/iP+3PHXizVhKssl5q103yurYj81hHgg4wFC9D6dqVT4bHsZal7VyfRHnXirWgp3xH5JF246e4/r/nFcr4V8PP4p8QWVlzseYK7Dnao5J/Bc/lT9akbzmi7E7l/E9vof519MfsXfBoeKNck1S9TZaklFkfAURqAZXz9Cq/8AA29KzhHVI2xVZ1JtvZGvrXhTTf2cvgnJ4hmgi/4TXxarWmjoR81jbEDzJlHZgrABhzudT2r5RWHbk4r1v9pb4rn4u/FK/vrWXOhWA/s/SYxwot4yQHA9XJZ/+BAdq8wWPdzXV6HiSd22yr5femyK6rleKvLCPwpki7jiggghYSggjHHNV7d/sc/kt/q2+4fT2q61sN+Rx7VnH/TNQFvHykZ3SN9DkAe9AGkV+WoGjDNjnPSr2wdMe1J5I9OaBIqrH8oFO8urXk7QM0eWM0DK3l8dKTyzVoR/jR5dAFYR8ikaOiisgI2XPUU8RnaO1FFAEirtXpiq3lnE7gdBj8hRRQB9qfsgeJovhZ+zf461vhL0I1xGeMtMyiOBfoXZfzNfLVvo6XmpiW6j2WOnQ7F8xsAseTk57nNFFRV2R7uBhFtnG6hbu+oeZEp8sNlY2JyfYV9y/EC/i/Z3/ZgtNFsZQniPxRD/AGcm3AaG3QE3T/Vndl/7aD+7RRWlPY8+u3dnxasJHUVKE2jpRRWhxDG+b296bs9qKKAKGqXht41ii5nk4XH86n0vT1sbYKeZG+Zm96KKALqx1Js7UUUAJt9P0o8sUUUAHl85oMYPU0UUMD//2Q==</t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCADIAOgDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD9U6KKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAoorxD9qb9qLwx+zX4QW+uII9U8SairDS9J83bvC/emlPVYl/NiQo7kJuw0r6I9L8d/EjwH8MdHOveP8AxXpuhWPKrJeTBDIwGSqL952x/CoJr5r8Qf8ABTr9m7R7ySz02LxRrOzOJrTT0SNsHHHmyI3X1UV+ZPxP+JXxb+PHjG68UeMXu9Xupm2xtgiC1jPPlwpnaqAdh7EnJJrS8N/CSeYiS4lhhMiDzF+9g5PPGMHHH4muKtjY092d9DL6tf4Ufpt4Q/4KRfs1eJrxLDU9S1vw3JI/lq+q2H7snsd0LSYHucAZ619K6D4h0HxVpNvrvhrWLPVNOul3w3VpMssUg9mUkGvxtT4J2F4sKG7MaRMGXZGOO5Gep/HOK9e+A+qfEz4C+I5NW8Ga1HqGkTzbrzRZnZI7lO/qBJ6PxjA6jIrKlmVKcuVs3rZNiKUeZI/UWiuf8C+NdF+IHhu18SaJI3lTriSGQYkt5QBujcdmGfoeCOCK6CvTTueS1bRhRRRQIKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKAGyOscbSSMFVQWZj0AHevxB/aC+KmpfGr45eJfGl1dPdafPdNaaZGRkQ2UTEQovOBkAMSByzMee/wCxnxr1qTw58HfHOvRMVksPDuo3EZU4O9bdyuPxxX4leF9JjneW9kK/u8AAflj3xiuLG1PZwO/AUfbVLHa6GrT6fHbhBF5SDCrxiuo8PWrbwsgYj9a5GCW+tVQWtoZ8n1wB9T/Su00XTfieI4r7S7bRZ4MAmNom+U+mc818tKXNrc+5prkto36I9A0a3WRlhjzgDJytbH7m3wULK2eMjFO8G6lb38ph1LSUsLmBV810l3RucDOO4Gc9ag8Xa7a+H4Ivs2jz6zdOu4xQSKu0Z4ySf84rCNT3rI65U/c5nsfQP7MPjqaw8WR+HZ5f9H1eNozk8CRFLI314K++4elfWVfmt8JfiNdaX8SvDNxrnhi80VBqETeY8yyxld43AlcEfKT1GK/SgdK+syyq6lLll0PhM5oRpV1OO0haKKK9E8cKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKAPkP9tz48eKvDZuvgz4b0nTjbeINFaPUr67V3dVuRMipEqsAGCxO25tw5HHr+eegWLWWlNbv5ZcS7S6DAYDnP45r77/b4+HVx/afhz4rWdu88UMbaXfRD7u4LI8DH675V7dR618UWWm6edDgudPXCGVyUPUNxuB98183jp1vbSjN+70Pscrp4f6vCpTXvdSndafrF5Cllo7okkYLAlMjd2+v/ANar/wAP9J1HQZ7+TxdrmrasZbV47eG3meF4LnaAJP8AVPuAbJ2k9MDI610fgm4tftyKpAY8FiOnOMV3XxI1n/hGfCvkaCF/tS9iYtNjc8EZ7r6EnpXjxrOnK0Vue+8PGtHmk3p2dvyPHrXWvGY8X2ltOjGCTCyM8ZAbHfHXp65+tXfF/gnxtHr3naXr17aW0zLKrQs33c5IJAJC/Tp1rX8PeJPhhp9vb3F1rbtqEbbTGEeRsnGScDoOpNes6l4++GtwtjpNlq2y5cDZLGrFi/GOMfKOvXiojVdOd1H8DeVGNWnyuX4nDaLo/jLTb43R1Rr/AEb7NbrEtzcfaJ451VfMk8wIgKswYhQvyggZbrX6q6PeLqGk2V+hytzbxzD6MoP9a/P6a60vUNBW4tWjDt8knyjlgdp9xX3T8NWlk+HfhdplIc6PZ7geoPkpX0GS1HUlO/kfJ8SUVSjTs+++vY6SiiivfPlAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKKKACiiigAooooAwfHPg3SfH/hPUvCOuRB7TUYTExxyjdVce6nB/Cvy++JnhD/AIRDVNY8NNIjyaXfSwtIhOHIYgsMjPJU19//ALR37Qmj/A3wuZoTbXfiG8Q/YbKRvlAHWWQAg7B0HIyenQkfDXx70zx5Douh/FHxZaWpXx5YJq0kllGVghuZBvaHBLYYAg9ecnHQ483Mqd6anY9jJ6vLVdPueQ2bSWOoW9x57RIswVtpxkdcVc8T+KF/sY6nq2oLCl3IV82VshAMhIwfZf1ye9c1FrUd/p8sL8SwsH+oHWtbTlstVs0s549yKxZSP4Sf8mvmlFKV2fZ80nHliM8J+GvCOt3gul1ayf7pbFxCrE+wOTk5Bx9PQV2Enhbw3pt5NqGi+IkBtVaWY+fFIFXklm24IAzVrwFpB0u4a4tY45dn3VLYU/hgiuy1CW9vISt7p8UETfMwV8h/c4UZ/GtfbJkxwsYx1vf+uo74eW954s1bSPD+mTIy61eQR+ZGdyqWYKXB7gjB/A+tfprZ2sNjaw2VsgSG3jWKNR2VRgD8hXx5+xz8Mbe88QXHjKSDbY6O223BHDXDKRx7KpJ+pWvsmveyqh7Km5/zHyWe4r21aNL+VBRRRXqHhhRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFQX19Z6ZZz6jqV3Da2ttG0008zhEjRRlmZjwAAMkmgCevDf2nv2pvBv7PfheX/AE6w1DxZdKE0/RzMC4JB/fSqOVjXrzjd0Hcj5e/aa/4KPalctfeDP2f9lrArNDN4jnH72QdCbaMjCD0kbLegU4Nfnv4j1jWteu7rV9Y1C5v9TnkM8lxcStJJK56lnbkk+p9a6IUG9ZGbqJbHovxQ+N/in4ia5eeIvE2ry3t9etukkboPRVA4VQMAAcACvtX9g/4veB/2hPhRffsv/FmGG9v9HhZ9MWZsNdWAOQYm6iWBjjjnYV64avzJW6W8UMjZ3DIzWx4R8T+IvAfiTTvGHhXVZ9M1jSbhbmzuoDh43H6EHkEHggkHINVUpRnHlYqc5RlzI+3/AI8fsL/EL4W3V14g8Exz+KvC+WkLQJ/ptomc4ljX74GfvoMcEkLXh+nabeWiloNzgHO0/eU/Tt/Kv1A/ZM/aY0T9pT4dx6xthsvE+lBLfXdORuI5SOJowefKkwSvoQyknbk2PjF+yr8N/iss+qwWa6D4hkBYalZR7fNb/ptGMB/97hv9rtXzuKyrrS+4+kwWdShaNbXz/wAz89vBOvWtvmTUJlgboV6DPfHt0r0XwnYat8TNctvC/hOze/u5n+cxodkK55eRuiqO5P8AOuE+J3wH8bfDPxvZeFfElhczT6lN5enTW8bTx3xzgCIgZZuR8n3hkZHIr6S8RfC3x58B/wBknXfFGi6xd+H/ABfbXtpq80ljNh4bdZBGIZCPlcBJXdlOVzxzjNedhME69b2clZLc9nG5nHD4f2kWm3tqfVXwx8Aaf8NfB9l4XsXErRZkuZtuPOmb7zY7DoB7AV1dfm78Kf8AgpT8Q9ImXR/il4dsPECRYR7q2/0S6+pCgxt9Aq/Wvrr4a/tefA/4mNFa2PildI1CXGLPVgLdiT2VyTGx9g2favq/YOnHlS0R8PKr7STlJ6s9oopFZXUOjBlYZBHIIpakAooooAKKKKACiiigAooooAKKKKACiiigAooooAKKK434yfEez+EXwt8T/Eq+hE6aBp8l0kJbAmm+7FHntukZFz70bgYfx2/aI+Gv7Pnhlte8caxGLqVT9h0uGRTdXjf7CE8KD1c/KPrgH8rv2hv2zfiJ+0JeyWN7qB0fw0jZg0SykYRHB4aZuDM3Tk8Dsq14P8RviZ4w+LPjLUvHHjXVpb/VdSlMkruTtQfwxovRUUcKo4AFYlkNzENya66cFH1M27nQmZX+Vlz6cVBNCzHd61HC21QGFX49pwkncZU+tbpmbic9c6P5bNNDOIRyxVlyoJ5JHQjJ96bZQXUi+ZcoIwGO3BJ3Ds3QY+lb99p4vLd7cuybhwy9VPUEfQ1R028a4kk0u+RY7+2GWUdJUPSRPY/oeKppCuz0H4A/GnxZ8A/iJp/jzwzMX8hvJvbNnIjvbViPMhf64BBwdrBT2r9m9D+KEfxU+DbfEb4N3lhdXWoadJNpy38bvHDdBTmGdIzvBVgVYLzxxkEZ/DBrX+Ja+mv2If2nbj4D+OR4d8R3jnwX4hmWPUEYkiym4VLpR2xwHx1XnkqornrUr6rcuE9dTmfiZ8SfjLdePZvEXxK129i17S7pEZZbh4mxIWx5EDEL5agFTsULg853ZP0l8CPFni7xt8J/ib4D17xhLrWg32gzW5s745m0lpopI/tULEk/ZkfZ5idI8B1AywP1D+018L/hn8RvhZrGt+JtAs782dhJeW+oQqpmjUIWEkbgHPHIzkHvkV+bv7NXxI1r4SeNLKa+1S4ubbT7x7XUNKjmjmsLuymHl3J3h9jNtWMqRuUkAk4UZ6YL69RlCMbSW3/AM5fuZpt6HhEd9JcWtvfSKyTRE28yMMMrqcEEdcirsWtTwsjLI2D0Oetdf+0B8PJPhn8Wda0jQ/Kl0vUGTWNJZhuhuIC3H1Dx7HyP+egNee3E/mO0iW6QBvn8lGLKnHIBPJ71nSnzxUrFyXLdHtnw1/ac+M3wzxa+EfHmoW1mw2razFbiBf8AdjlDKv4AV+kH7In7TkP7Q/hG8h1u3t7Lxb4fZYtUtoeI5kb7lxEDyFbBBGTtYY7ivyDs5AY1k9K9V/Zp+L1x8Gfjb4e8aLM66dNN/Zurxg8SWcv3iR3Kn5h/tAUq1NSjfqKEmj9paKjgnhuoY7i3kWSKVQ6OpyGUjIIPcEVJXnnQFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFfN//BQ5Zm/ZJ8aeSGKh9PMm3+59tgz/AEr6QryX9rLwvJ4w/Zu+Iehw8yHQ57xBj7xt8Tgfj5WPxpx3Ez8FbuKRZS0Lgj+dWtNufmCzfK3T61W1C3dZW2NwD0FLZs3CyKGH6iu1GR1MS7l3GrUa74zGzcHoR1U+tZVlMy4VmLp29R/jWgnLblY/1qgJbPUE+0NYXeFmX/x70Iqv4i0Nr6OK+sZhDfWjb4JcfmrDup6EVS8SWk01qt9akrc2nzrjqy9xWv4b1SPWdPWQ/wCs24YVcXf3WS1bVEOhapHrMLpJF9nvbf5Lq3bqjeo9VPY1oSQeWdy5BFUr7RJGul1HT5BBfQghHP3XXujgdVP6dRV7SdQh1OORXiMU8LbJ4W+9G39QeoPcVdujJP0O/YV+O1t8UPAeofs1+PNSkF9BYyx6FctJh5bXaQ0APdogcqOcpkYwnPzLa+E9S0PxLc2K6Wtjd3ccmm/ZrqJDGRuaN3SSbhfnQjcMYIb5hivKvDOva14K8Rad4q8O3slnqWmXCXVrPH1R1YEH3HqDwRkHivdPEnjPQ/iZ4nv/ABnoKtFNrBW8u9N2E/ZZ2jWS42MT90zeey4/hI7kiu7KoxjWlC3xfoY4p3gpX2OD+LmrX3iLwT4avNSaOa48Hzmyhl8xTINMncII5AOfkmMYUsOVk44FeSXsAim3DPJr2fxva2d7p2u2NmJjDd29xBaPOyKRGEdo/MVRy4cRMMHqhHPGPHvNW+0y1vl5E8KP+YrHF0PYVZJbPUqnPniu4yFvLs3j/unH4UQzDziWJ+TbIPqCDSZ/0eT3WqEjNKZIo5NrSxlFI9SOK5Waq5+x37CPj3UvHn7POkyatcNPPod1No6yscl4ogjR5+iSKv0UV9C1+Rv7Avx78TeDfjr4e+Hlvrznwp4jWSz1DTpXzFFcMALadQeEkZsKSPvLwc4GP1yrz6seWRvB3QUUUVmUFFFFABRRRQAUUUUAFFFFABRRRQAVX1CxtdUsbnTb2MSW93C8EyHoyMpVh+IJqxRQB/Pl8bvh5e/DL4leJPB8khdtF1O4smfGN4jkKq+PRgAfxriLSYbx5i1+g/8AwVQ+Fuh6P468PeOtJs/s154ptJ1vGUARzXFt5a7j6M0cig+uwHrmvz58vbIVKlWB6HtXZCV1cyejNiFu+0keoq/HNbsoV2KkdzwR+NZdmzbgN3Na1uFbhwPyrQQs32hI88TR/qKwNHvBo2sPHGxEMrZUeme1b72ksf7yzk2H+6fumud8RRyBVu2tzFLH97jhvoaAPR4/LuYhNHjkc1l6ppdwtwmsaVhb2BdpUnCzx942/oex/Gq/gzWFvLVY2YEjg107Rr1raL5kZvQo2OoQ6rZpcQAgHKsrDDRsOCrDsQeK6nwRry6LdzWc9vDJBfhImkYEtAQwIZOQAeqnOeGP1rhNSU6DqDa1D/x53GFvkHRewm/DgN/s8/w1usy+WrKRitKVR0pqS3RMo8ysz2nVRdvZmSRo4l1C18sbTDEkttD1BA+7IWhXGfmYj+Itz8/6Au/Qza/xWlxPb/gkrL/SvbPD+pab4g0e2ursyF43CX0MKxpmGMLlkZif3hAY/d6kdckV4no80jXmupK4Zhq10Sc9Sz7v/Zq9HMXGcY1I9Tnw+jcSWW2U/KwO2oP3cJG1QPpVycbl9RWXdPtyvavJeh2J3LPgO4uPDepJqtjeJBfRXQuFl3fMCrZTkdCOv41+1H7O/wC0X4V/aA8Oy3ekxy2esaZHCNTspMYV3U/PGQTujJVgCcEY5A4z+HljdTfaiLlVWAscYzlua+h/2XPjlqHwX+JFh4otZPO02b/Q9UtV6y2jEbsA/wASkBl91x0JrGpT9pHzHF8rP2YoqhoWtaZ4i0m01zRryK7sb6FLi3mjbKyRsAVYfUGr9cBuFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAfKf/AAUh+F83j79n2fxJYj/TPBl0uqHauWNsw8uYD6Blc+0Zr8dtSj3SedkF+7D+L3r+hrxv4bh8ZeDNe8I3DBY9b02509mIyFE0TJn8N2a/n88deGdQ8K61qGl3MOyXTbqWzuowchJEYq2COoyp/Kuii9LESMezk5DZrZtyOG71zlrIu7jvW1aSblB7it0QaytkUyaGO4jaGVAyOMEGli+6KlVc9KYHGWc3/CLeJhpokbyLhRJHu7c4I/DFek29+skYy2c965Dxh4XbWreK6syUv7TLwt/e9UP1x+dL4c1WS5s18zKOvysp4KsOoI9auGhL1OvuAlxCyMA6uCp9MGsfQblrGaXw7eMSbdd9qzfxwdAPqn3T7bfWpUvjGuWbiqWtf6XAt/Y4+2WbebD23f3kPswyPxB7VbJPTPAGrpGuoaLNaJJFNsu/O8vdJCY9y4U54VvMGc9dq+lcJCt5F4n8VR6hGsU76xJOyqqqP3iI4wq/KAQwOBjGccUvhPxBDHq2matHte3aRCyvnDI3DBgD6E5FYekXCDXfFHlSFh/a0mcrjB2rkY9jkfhXROpzYeMez/QzStUfob+pahHp9qZm5x0H1IFc9capHIu9e/NL4qutun7WbJGPw5rlVu2VTlv4eK5mzQv6fqUDXs+27zJ5jDyi3ArqNLv5I3VlGSPevKbW6guLuVZoSreY2HX611+k3UlqV/0nKjsxrJMs/Vj/AIJ5/tE2Wr6OvwV8S3iQX9mHm0VpW/18RJaSEE9WUksB3Ut/dr7jr8C/CPi46TqFrqVhqU9lfWcyT29zCSrRSKQVZWHIIIBr9lP2W/jlZ/Hb4W2XiCa4hOuafiy1iGPAxOBxIB2WRfmHYHcv8Nc1aFveRpF9D2CiiisCwooooAKKKKACiiigAooooAKKKKACvyG/4KBfBuP4V/HS71W2w+iePhLq8AIwIblnxcRZ9PMIbPYSIO1frzXx7/wVA8C3niP9nyDxfpmnx3U/hLVYrq4yoL/Y5gYZAp6j52hP/Ac9q0pytIUtj8hdRsX02+aPaQAeM/196tWM+COetXr7dqlipuFKTxIvzN1wfu7j+BUn1A9aw4JGikMbcMp6Hsa6k7GR1NvMpUZrQh2lfm4Fc/azg4PY1pLL50LQ7ypYcH0NUM37zTNS0po01CxuLVpVDoJo2Tcp6EZHIrjtTWO21BdQi+WO7YrIBxiRe/4j+Rr6H8BfHb4feJtDg+HXx1tUjaL5bW/fKqSBgOjj7rEdRUGrfs8+C/GVjP8A8K58bQSwCTzY90izbGDEdAQfUdT3ryY51TpSdLFRcJL7j2XkdWtBVsJJTT+8+fortfJ+92pVvwqn94FGK9Gn/Zm8fRpNFperaPfmIkYWR0JPPGSu3P415Z4t8MeLfB92dL8VaJc6dKzYTzF+WQequPlYfQ16NHG4fEaU5ps8zEYHE4bWrBpEOk3Bs7y501jhJM3Nv9CfnA+jc/8AAqseGbr7Tfa5cNGqNJqBZsZ+Ztq5Y5PUmsrVp0t7a3vEbElq4Y+6Hhh+XP4Cq+n61HZ2+oTR43yXBI+vloP510baHKaniG/W4t58MODx+Fcq+pRrEcnOKpTaxJJI1uu593y7V5JotfCnizUl2w6TMobjdKRGP/HiDUyfYErlax1VoI2VrdXLtu3ZIP0ro9L1RZFU+STIT90Hp9TUWn+BbiHEOoQ3aTf7AUqPxGa6Kx8K2mmp8tvOZB9/c3J+nQVnFSW5o7PY29DuJm2lti56fL/jXrHwP/aG8bfs7fECx8Z2NnJPpQkVNUhs5TsurTPzpJGemBkqw3bSAa800ezheMNbsfl+8G4I+oNbqQjo3ateW6JvY/dP4d/EDwr8U/Bek+PvBOqR6ho2s263FtMh7Hgqw7MpBVh2IIro6/Nf/gmP8SL7w38Qdb+D81039ieIraTVrG1ZvlttQix5vljsssWWYesQx1NfpRXBOHJKxtF3QUUUVAwooooAKKKKACiiigAooooAK84/aO8J3njn4E+OfC2nxtJdXui3HkRqu4ySIvmKgHcsUA/GvR6KadgP517q9+w6oNNuN7TDcuWHEkZ4KsegJOSO3P0rK1CHbIdnzFV3Ke5Tsfw6ex49DXq/7V3hW10H44eNPD+k2whgi16+hIA+7Gsz7R7ZUjFeYyQ+dbrHJNsnT7r984+975HDDuOfWuxO5iZ8WqLbr+8bAroPDeleIvERNxYadJ9lT71xJ8sX5nqfpmu4+A/wLh+K1j4s8UN9lnm8IwwTNpMkwVpBIzBpsH76IFzjPOcc9D3F/wCJhaWc/g3wtocWrX9oNt5fbgun6eR0TK8yOP7i9OMkV42Pzd4ap7GlG8lvfZHvZbk31un7arK0fLcf4V/ZluPENqjeJtYT7NIoZooYw3ykZ+83+Fep+E/gX8OPhtGY9HjCtJ8xaR2ck+yk4H0AArltE8EeJvEmixXnir4ta3BZpGrPBpzJpluFx3ZB5hHTq9dz4R8K/DPRbUf2f4iS4kY7Wml1JrqUn/edmYdRxnvXzONx9bEfxJ3Xa2h9dl+XUMLZ04WfdvU6nSJ9FeSO1s3iUqBx5WKu+IvC+keKNPfTtX0eyvrdzykkYZT+DZxjnmqsGm6DYsv2F/NLODx82f6111jJ5luF2KAoHzY6c1xKpyrmiel7NSbjJHzr4i/ZY+HmpK/l+G7qDevSG7fHvwSRWT4B/Zp+HGk3U+o+JvAdrqa2F4bTybi8uPs8j7EcM6LIGyUZT97BO70r6lmaNmEdqodwvHygYrmF0m/uP+Eht33iQatb3EfcKv2JQ/GccnZjj+E816OGzLESjKPO9Fff0PIxmVYWMqclTWsrPTumdxffsc/AD43fBl9a+EPgLSfBfi+xVowtiWWJrpFBMEoYkFHBUq/3huUknDKfzy1vw/eaHqV1o2r2ctrfWMz29xBKu14pEJDKQehBFfot+yd4/wD+Eb+KE3g3U70R23iS3a3hRm63kG5047bozKp9SEHpXEf8FIvgvaabq+nfGDQbFYv7TIs9W8tcK8oH7uU4/iIG0nvhfevrcrxn1mknLf8AU+LzbBfU8RKnHbdeh8D3FmhbKsQ3rihYc4Eq5FXJYGzkUqx7lr1jy72K8cEcLiRVwDwfxqdpG24bjHemruU+W+M/zqw1v5gIUZbAoSJbueyfsa3mrRftJ+AptGQNcrqZimX/AKd3hkSY/hGzn8K/Y6vy/wD+Cdfwh8Wat8Y7X4mNps0Og+HYblWvJIyI5ppYXiWJCfvMPMLHHQDnGRn9QK4sQ/eNafwhRRRXOaBRRRQAUUUUAFFFFABRRRQAUUUUAfi9+3Vqng+8/aJ8aat4YvEubR7mMTSLjYblIUSYKe4Eitz3Ofavj/U724v75buOR40gbdHg9D60UV2R+FGT3PWfgD8N7r42eMJtP0+4uYZNO0241C9tbSYxzXKRgARx45IcsoIHYH2NezaFrGjeArFfDsXhd9S1AfuUtLZlitLf08yTn64UM3r60UV8nnsnOvyPax9nw7FQoOpHds2dV8M6hNplr4q8Ya5brZ2s2/7PMywafbYPAWM8M3ozbm9COlI/7bnwX8P+G5fCMNjq2qzyahBLHPZaeNihY5ElVA5QtuJi6cfIKKK58swlPFwlKpfQ6s5x1TA1IRpJe9qe0+HvGml6/p0d9a+G9VsI5E3Kt/bpGzgj0Rjj8a17a+WOEKyeUhHAfrk0UV4SjY+l5nK1zL+IPxf8H/B3RYdS8SXDTX10P9FsYcNPKPXB6L6sePqeK5v9mT4veEf2mvixrPwr1vxNqugX+p6dPqWlJYSIiiSPy0liy8eZHMSI/GMCF8dTRRX1mVZdQeF9tJXbPiM8zTErFexjKyjqrehwP7QXgr4qfBfx0LrwTr8FzJo19HcWl9OjJcRvG4Zdw5UnIHIOD+lfof8AEuOx+Mn7KN/rXj/SZfDct94a/tieC8TD6dcpD5oJB5wHX2JU8gE4oorswMI0pOMFY8rH1p1+WVR3Z+R7Wu5sKufWhNPZ/wCHPbgUUV9IeGdb8Pfgn4/+Kmr/ANjeCPC1/qkikeZLFHiKDP8AflbCIP8AeIr7m+Bn/BO7wz4Zkg174v3kOt3iBWTSrVmFqh/6aycNL9BtXjncKKK5MRVlF8qNqcU9T7E03S9N0Wwg0rR9Pt7GytUEcNvbxLHHGo6KqqAAPpVqiiuM1CiiigAooooA/9k=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3780,13 +3783,6 @@
     </font>
     <font>
       <sz val="5"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4221,10 +4217,10 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9520,8 +9516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L36" zoomScale="63" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="L120" zoomScale="63" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="183.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -9561,19 +9557,19 @@
         <v>710</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1172</v>
+        <v>1162</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1173</v>
+        <v>1163</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1174</v>
+        <v>1164</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1175</v>
+        <v>1165</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>1176</v>
+        <v>1166</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
@@ -9605,7 +9601,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1173</v>
+        <v>1163</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>4</v>
@@ -10153,7 +10149,7 @@
         <v>100</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>1072</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10194,7 +10190,7 @@
         <v>106</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10235,7 +10231,7 @@
         <v>113</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>1074</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10276,7 +10272,7 @@
         <v>119</v>
       </c>
       <c r="M18" s="15" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10317,7 +10313,7 @@
         <v>125</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>1076</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10358,7 +10354,7 @@
         <v>132</v>
       </c>
       <c r="M20" s="15" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10399,7 +10395,7 @@
         <v>136</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>1078</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10440,7 +10436,7 @@
         <v>142</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10481,7 +10477,7 @@
         <v>149</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10522,7 +10518,7 @@
         <v>155</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10563,7 +10559,7 @@
         <v>160</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10604,7 +10600,7 @@
         <v>167</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10645,7 +10641,7 @@
         <v>173</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10686,7 +10682,7 @@
         <v>180</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10727,7 +10723,7 @@
         <v>187</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10768,7 +10764,7 @@
         <v>194</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10809,7 +10805,7 @@
         <v>200</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10850,7 +10846,7 @@
         <v>207</v>
       </c>
       <c r="M32" s="15" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10891,7 +10887,7 @@
         <v>214</v>
       </c>
       <c r="M33" s="15" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10932,7 +10928,7 @@
         <v>221</v>
       </c>
       <c r="M34" s="15" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10973,7 +10969,7 @@
         <v>228</v>
       </c>
       <c r="M35" s="15" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="299" customHeight="1" x14ac:dyDescent="0.35">
@@ -11013,8 +11009,8 @@
       <c r="L36" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="M36" s="22" t="s">
-        <v>1188</v>
+      <c r="M36" s="21" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11055,7 +11051,7 @@
         <v>239</v>
       </c>
       <c r="M37" s="15" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11096,7 +11092,7 @@
         <v>246</v>
       </c>
       <c r="M38" s="15" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11137,7 +11133,7 @@
         <v>253</v>
       </c>
       <c r="M39" s="15" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11178,7 +11174,7 @@
         <v>259</v>
       </c>
       <c r="M40" s="15" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11219,7 +11215,7 @@
         <v>265</v>
       </c>
       <c r="M41" s="15" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11260,7 +11256,7 @@
         <v>272</v>
       </c>
       <c r="M42" s="15" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11301,7 +11297,7 @@
         <v>279</v>
       </c>
       <c r="M43" s="15" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11342,7 +11338,7 @@
         <v>286</v>
       </c>
       <c r="M44" s="15" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11383,7 +11379,7 @@
         <v>293</v>
       </c>
       <c r="M45" s="15" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11424,7 +11420,7 @@
         <v>299</v>
       </c>
       <c r="M46" s="15" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11465,7 +11461,7 @@
         <v>306</v>
       </c>
       <c r="M47" s="15" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11506,7 +11502,7 @@
         <v>313</v>
       </c>
       <c r="M48" s="15" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11547,7 +11543,7 @@
         <v>320</v>
       </c>
       <c r="M49" s="15" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11588,7 +11584,7 @@
         <v>325</v>
       </c>
       <c r="M50" s="15" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11629,7 +11625,7 @@
         <v>332</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11670,7 +11666,7 @@
         <v>338</v>
       </c>
       <c r="M52" s="15" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11711,7 +11707,7 @@
         <v>344</v>
       </c>
       <c r="M53" s="15" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11752,7 +11748,7 @@
         <v>349</v>
       </c>
       <c r="M54" s="15" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11793,7 +11789,7 @@
         <v>357</v>
       </c>
       <c r="M55" s="15" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11834,7 +11830,7 @@
         <v>364</v>
       </c>
       <c r="M56" s="15" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11875,7 +11871,7 @@
         <v>369</v>
       </c>
       <c r="M57" s="15" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11916,7 +11912,7 @@
         <v>376</v>
       </c>
       <c r="M58" s="15" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11957,7 +11953,7 @@
         <v>383</v>
       </c>
       <c r="M59" s="15" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11998,7 +11994,7 @@
         <v>390</v>
       </c>
       <c r="M60" s="15" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12039,7 +12035,7 @@
         <v>397</v>
       </c>
       <c r="M61" s="15" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12080,7 +12076,7 @@
         <v>404</v>
       </c>
       <c r="M62" s="15" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12121,7 +12117,7 @@
         <v>408</v>
       </c>
       <c r="M63" s="15" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12162,7 +12158,7 @@
         <v>413</v>
       </c>
       <c r="M64" s="15" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12203,7 +12199,7 @@
         <v>420</v>
       </c>
       <c r="M65" s="15" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12244,7 +12240,7 @@
         <v>426</v>
       </c>
       <c r="M66" s="15" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12285,7 +12281,7 @@
         <v>431</v>
       </c>
       <c r="M67" s="15" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12326,7 +12322,7 @@
         <v>437</v>
       </c>
       <c r="M68" s="15" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12367,7 +12363,7 @@
         <v>442</v>
       </c>
       <c r="M69" s="15" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12408,7 +12404,7 @@
         <v>449</v>
       </c>
       <c r="M70" s="15" t="s">
-        <v>1126</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12449,7 +12445,7 @@
         <v>455</v>
       </c>
       <c r="M71" s="15" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12490,7 +12486,7 @@
         <v>461</v>
       </c>
       <c r="M72" s="15" t="s">
-        <v>1128</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12531,7 +12527,7 @@
         <v>468</v>
       </c>
       <c r="M73" s="15" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12572,7 +12568,7 @@
         <v>475</v>
       </c>
       <c r="M74" s="15" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12613,7 +12609,7 @@
         <v>482</v>
       </c>
       <c r="M75" s="15" t="s">
-        <v>1131</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12654,7 +12650,7 @@
         <v>489</v>
       </c>
       <c r="M76" s="15" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12695,7 +12691,7 @@
         <v>495</v>
       </c>
       <c r="M77" s="15" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12736,7 +12732,7 @@
         <v>501</v>
       </c>
       <c r="M78" s="15" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12777,7 +12773,7 @@
         <v>506</v>
       </c>
       <c r="M79" s="15" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12818,7 +12814,7 @@
         <v>513</v>
       </c>
       <c r="M80" s="15" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12859,7 +12855,7 @@
         <v>520</v>
       </c>
       <c r="M81" s="15" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12900,7 +12896,7 @@
         <v>524</v>
       </c>
       <c r="M82" s="15" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12941,7 +12937,7 @@
         <v>530</v>
       </c>
       <c r="M83" s="15" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12982,7 +12978,7 @@
         <v>537</v>
       </c>
       <c r="M84" s="15" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13023,7 +13019,7 @@
         <v>542</v>
       </c>
       <c r="M85" s="15" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13064,7 +13060,7 @@
         <v>549</v>
       </c>
       <c r="M86" s="15" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13105,7 +13101,7 @@
         <v>555</v>
       </c>
       <c r="M87" s="15" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13146,7 +13142,7 @@
         <v>560</v>
       </c>
       <c r="M88" s="15" t="s">
-        <v>1144</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13187,7 +13183,7 @@
         <v>565</v>
       </c>
       <c r="M89" s="15" t="s">
-        <v>1145</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13228,7 +13224,7 @@
         <v>572</v>
       </c>
       <c r="M90" s="15" t="s">
-        <v>1146</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13269,7 +13265,7 @@
         <v>578</v>
       </c>
       <c r="M91" s="15" t="s">
-        <v>1147</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13310,7 +13306,7 @@
         <v>585</v>
       </c>
       <c r="M92" s="15" t="s">
-        <v>1148</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13351,7 +13347,7 @@
         <v>591</v>
       </c>
       <c r="M93" s="15" t="s">
-        <v>1149</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13392,7 +13388,7 @@
         <v>597</v>
       </c>
       <c r="M94" s="15" t="s">
-        <v>1150</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13433,7 +13429,7 @@
         <v>603</v>
       </c>
       <c r="M95" s="15" t="s">
-        <v>1151</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13474,7 +13470,7 @@
         <v>610</v>
       </c>
       <c r="M96" s="15" t="s">
-        <v>1152</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13515,7 +13511,7 @@
         <v>617</v>
       </c>
       <c r="M97" s="15" t="s">
-        <v>1153</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13556,7 +13552,7 @@
         <v>623</v>
       </c>
       <c r="M98" s="15" t="s">
-        <v>1154</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13597,7 +13593,7 @@
         <v>628</v>
       </c>
       <c r="M99" s="15" t="s">
-        <v>1155</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13638,7 +13634,7 @@
         <v>633</v>
       </c>
       <c r="M100" s="15" t="s">
-        <v>1156</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13679,7 +13675,7 @@
         <v>639</v>
       </c>
       <c r="M101" s="15" t="s">
-        <v>1157</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13720,7 +13716,7 @@
         <v>644</v>
       </c>
       <c r="M102" s="15" t="s">
-        <v>1158</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13761,7 +13757,7 @@
         <v>651</v>
       </c>
       <c r="M103" s="15" t="s">
-        <v>1159</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13784,25 +13780,25 @@
         <v>796</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>1177</v>
+        <v>1167</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>1178</v>
+        <v>1168</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>1179</v>
+        <v>1169</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>1180</v>
+        <v>1170</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>1181</v>
+        <v>1171</v>
       </c>
       <c r="L104" s="3" t="s">
         <v>653</v>
       </c>
       <c r="M104" s="15" t="s">
-        <v>1160</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13843,7 +13839,7 @@
         <v>660</v>
       </c>
       <c r="M105" s="15" t="s">
-        <v>1161</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13884,7 +13880,7 @@
         <v>667</v>
       </c>
       <c r="M106" s="15" t="s">
-        <v>1162</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13925,7 +13921,7 @@
         <v>673</v>
       </c>
       <c r="M107" s="15" t="s">
-        <v>1163</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13966,7 +13962,7 @@
         <v>679</v>
       </c>
       <c r="M108" s="15" t="s">
-        <v>1164</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14007,7 +14003,7 @@
         <v>684</v>
       </c>
       <c r="M109" s="15" t="s">
-        <v>1165</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14048,7 +14044,7 @@
         <v>691</v>
       </c>
       <c r="M110" s="15" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14089,7 +14085,7 @@
         <v>698</v>
       </c>
       <c r="M111" s="15" t="s">
-        <v>1167</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -14169,7 +14165,7 @@
         <v>1008</v>
       </c>
       <c r="M113" s="15" t="s">
-        <v>1168</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
@@ -14210,7 +14206,7 @@
         <v>1015</v>
       </c>
       <c r="M114" s="15" t="s">
-        <v>1169</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14251,7 +14247,7 @@
         <v>1034</v>
       </c>
       <c r="M115" s="15" t="s">
-        <v>1170</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="116" spans="1:13" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.35">
@@ -14293,10 +14289,10 @@
         <v>1047</v>
       </c>
       <c r="M116" s="18" t="s">
-        <v>1171</v>
+        <v>1161</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" ht="203.5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>1048</v>
       </c>
@@ -14333,11 +14329,11 @@
       <c r="L117" s="19" t="s">
         <v>1056</v>
       </c>
-      <c r="M117" s="21" t="s">
-        <v>1187</v>
+      <c r="M117" s="22" t="s">
+        <v>1188</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" s="9" customFormat="1" ht="209.5" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>711</v>
       </c>
@@ -14362,11 +14358,11 @@
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
       <c r="L118" s="7"/>
-      <c r="M118" s="18" t="s">
-        <v>1182</v>
+      <c r="M118" s="22" t="s">
+        <v>1184</v>
       </c>
     </row>
-    <row r="119" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" s="9" customFormat="1" ht="235.5" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>712</v>
       </c>
@@ -14391,8 +14387,8 @@
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
       <c r="L119" s="7"/>
-      <c r="M119" s="18" t="s">
-        <v>1183</v>
+      <c r="M119" s="22" t="s">
+        <v>1189</v>
       </c>
     </row>
     <row r="120" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
@@ -14421,10 +14417,10 @@
       <c r="K120" s="7"/>
       <c r="L120" s="7"/>
       <c r="M120" s="18" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
     </row>
-    <row r="121" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>714</v>
       </c>
@@ -14449,8 +14445,8 @@
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
       <c r="L121" s="7"/>
-      <c r="M121" s="18" t="s">
-        <v>1185</v>
+      <c r="M121" s="22" t="s">
+        <v>1172</v>
       </c>
     </row>
     <row r="122" spans="1:13" s="9" customFormat="1" ht="338" x14ac:dyDescent="0.3">
@@ -14479,10 +14475,10 @@
       <c r="K122" s="7"/>
       <c r="L122" s="7"/>
       <c r="M122" s="18" t="s">
-        <v>1186</v>
+        <v>1173</v>
       </c>
     </row>
-    <row r="123" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>716</v>
       </c>
@@ -14507,9 +14503,11 @@
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
       <c r="L123" s="7"/>
-      <c r="M123" s="18"/>
+      <c r="M123" s="18" t="s">
+        <v>1185</v>
+      </c>
     </row>
-    <row r="124" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>717</v>
       </c>
@@ -14534,7 +14532,9 @@
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
       <c r="L124" s="7"/>
-      <c r="M124" s="18"/>
+      <c r="M124" s="18" t="s">
+        <v>1183</v>
+      </c>
     </row>
     <row r="125" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">

</xml_diff>

<commit_message>
procurement director details updated, MC images updated
</commit_message>
<xml_diff>
--- a/static/2025_LC_DELEGATE_PROFILE.xlsx
+++ b/static/2025_LC_DELEGATE_PROFILE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Getting to Know the Delegates" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1190">
   <si>
     <t>Username</t>
   </si>
@@ -2697,9 +2697,6 @@
   </si>
   <si>
     <t>IBIYEMI, AFOLABI GABRIEL</t>
-  </si>
-  <si>
-    <t>HEAD - CATEGORY DIRECT SERVICES</t>
   </si>
   <si>
     <t>AKINTOLU, KAYODE IBRAHIM</t>
@@ -9519,8 +9516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="63" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="63" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="183.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -9560,25 +9557,25 @@
         <v>710</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1163</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>1164</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1165</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1166</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9604,7 +9601,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>4</v>
@@ -9619,7 +9616,7 @@
         <v>7</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9660,7 +9657,7 @@
         <v>14</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9701,7 +9698,7 @@
         <v>21</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9742,7 +9739,7 @@
         <v>31</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9783,7 +9780,7 @@
         <v>38</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9824,7 +9821,7 @@
         <v>45</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9865,7 +9862,7 @@
         <v>52</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9906,7 +9903,7 @@
         <v>59</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9947,7 +9944,7 @@
         <v>66</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -9988,7 +9985,7 @@
         <v>72</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
@@ -10029,7 +10026,7 @@
         <v>79</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="255" x14ac:dyDescent="0.3">
@@ -10070,7 +10067,7 @@
         <v>86</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10111,7 +10108,7 @@
         <v>93</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10152,7 +10149,7 @@
         <v>100</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10187,13 +10184,13 @@
         <v>105</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>106</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10234,7 +10231,7 @@
         <v>113</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10275,7 +10272,7 @@
         <v>119</v>
       </c>
       <c r="M18" s="15" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10316,7 +10313,7 @@
         <v>125</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10357,7 +10354,7 @@
         <v>132</v>
       </c>
       <c r="M20" s="15" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10398,7 +10395,7 @@
         <v>136</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10439,7 +10436,7 @@
         <v>142</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10480,7 +10477,7 @@
         <v>149</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10521,7 +10518,7 @@
         <v>155</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10562,7 +10559,7 @@
         <v>160</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10603,7 +10600,7 @@
         <v>167</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10644,7 +10641,7 @@
         <v>173</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10685,7 +10682,7 @@
         <v>180</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10726,7 +10723,7 @@
         <v>187</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10767,7 +10764,7 @@
         <v>194</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10808,7 +10805,7 @@
         <v>200</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10849,7 +10846,7 @@
         <v>207</v>
       </c>
       <c r="M32" s="15" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10890,7 +10887,7 @@
         <v>214</v>
       </c>
       <c r="M33" s="15" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10931,7 +10928,7 @@
         <v>221</v>
       </c>
       <c r="M34" s="15" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -10972,7 +10969,7 @@
         <v>228</v>
       </c>
       <c r="M35" s="15" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="299" customHeight="1" x14ac:dyDescent="0.35">
@@ -11013,7 +11010,7 @@
         <v>234</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11054,7 +11051,7 @@
         <v>239</v>
       </c>
       <c r="M37" s="15" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11095,7 +11092,7 @@
         <v>246</v>
       </c>
       <c r="M38" s="15" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11136,7 +11133,7 @@
         <v>253</v>
       </c>
       <c r="M39" s="15" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11177,7 +11174,7 @@
         <v>259</v>
       </c>
       <c r="M40" s="15" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11218,7 +11215,7 @@
         <v>265</v>
       </c>
       <c r="M41" s="15" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11259,7 +11256,7 @@
         <v>272</v>
       </c>
       <c r="M42" s="15" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11300,7 +11297,7 @@
         <v>279</v>
       </c>
       <c r="M43" s="15" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11341,7 +11338,7 @@
         <v>286</v>
       </c>
       <c r="M44" s="15" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11382,7 +11379,7 @@
         <v>293</v>
       </c>
       <c r="M45" s="15" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11423,7 +11420,7 @@
         <v>299</v>
       </c>
       <c r="M46" s="15" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11464,7 +11461,7 @@
         <v>306</v>
       </c>
       <c r="M47" s="15" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11505,7 +11502,7 @@
         <v>313</v>
       </c>
       <c r="M48" s="15" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11546,7 +11543,7 @@
         <v>320</v>
       </c>
       <c r="M49" s="15" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11587,7 +11584,7 @@
         <v>325</v>
       </c>
       <c r="M50" s="15" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11628,7 +11625,7 @@
         <v>332</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11669,7 +11666,7 @@
         <v>338</v>
       </c>
       <c r="M52" s="15" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11710,7 +11707,7 @@
         <v>344</v>
       </c>
       <c r="M53" s="15" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11751,7 +11748,7 @@
         <v>349</v>
       </c>
       <c r="M54" s="15" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11792,7 +11789,7 @@
         <v>357</v>
       </c>
       <c r="M55" s="15" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11833,7 +11830,7 @@
         <v>364</v>
       </c>
       <c r="M56" s="15" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11874,7 +11871,7 @@
         <v>369</v>
       </c>
       <c r="M57" s="15" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11915,7 +11912,7 @@
         <v>376</v>
       </c>
       <c r="M58" s="15" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11956,7 +11953,7 @@
         <v>383</v>
       </c>
       <c r="M59" s="15" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11997,7 +11994,7 @@
         <v>390</v>
       </c>
       <c r="M60" s="15" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12038,7 +12035,7 @@
         <v>397</v>
       </c>
       <c r="M61" s="15" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12079,7 +12076,7 @@
         <v>404</v>
       </c>
       <c r="M62" s="15" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12120,7 +12117,7 @@
         <v>408</v>
       </c>
       <c r="M63" s="15" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12161,7 +12158,7 @@
         <v>413</v>
       </c>
       <c r="M64" s="15" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12202,7 +12199,7 @@
         <v>420</v>
       </c>
       <c r="M65" s="15" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12243,7 +12240,7 @@
         <v>426</v>
       </c>
       <c r="M66" s="15" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12284,7 +12281,7 @@
         <v>431</v>
       </c>
       <c r="M67" s="15" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12295,7 +12292,7 @@
         <v>888</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>889</v>
+        <v>989</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>756</v>
@@ -12325,7 +12322,7 @@
         <v>437</v>
       </c>
       <c r="M68" s="15" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12333,10 +12330,10 @@
         <v>438</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>890</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>891</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>761</v>
@@ -12366,7 +12363,7 @@
         <v>442</v>
       </c>
       <c r="M69" s="15" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12374,10 +12371,10 @@
         <v>443</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>892</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>893</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>769</v>
@@ -12407,7 +12404,7 @@
         <v>449</v>
       </c>
       <c r="M70" s="15" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12415,10 +12412,10 @@
         <v>450</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>894</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>895</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>761</v>
@@ -12448,7 +12445,7 @@
         <v>455</v>
       </c>
       <c r="M71" s="15" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12456,10 +12453,10 @@
         <v>456</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>896</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>897</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>848</v>
@@ -12489,7 +12486,7 @@
         <v>461</v>
       </c>
       <c r="M72" s="15" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12497,10 +12494,10 @@
         <v>462</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>898</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>899</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>786</v>
@@ -12530,7 +12527,7 @@
         <v>468</v>
       </c>
       <c r="M73" s="15" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12538,10 +12535,10 @@
         <v>469</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>900</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>901</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>774</v>
@@ -12571,7 +12568,7 @@
         <v>475</v>
       </c>
       <c r="M74" s="15" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12579,10 +12576,10 @@
         <v>476</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>902</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>903</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>745</v>
@@ -12591,7 +12588,7 @@
         <v>739</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>477</v>
@@ -12612,7 +12609,7 @@
         <v>482</v>
       </c>
       <c r="M75" s="15" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12620,10 +12617,10 @@
         <v>483</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>905</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>906</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>769</v>
@@ -12653,7 +12650,7 @@
         <v>489</v>
       </c>
       <c r="M76" s="15" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12661,10 +12658,10 @@
         <v>490</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>907</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>908</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>774</v>
@@ -12694,7 +12691,7 @@
         <v>495</v>
       </c>
       <c r="M77" s="15" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12702,13 +12699,13 @@
         <v>496</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>910</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>911</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>739</v>
@@ -12735,7 +12732,7 @@
         <v>501</v>
       </c>
       <c r="M78" s="15" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12743,10 +12740,10 @@
         <v>502</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>912</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>913</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>745</v>
@@ -12755,7 +12752,7 @@
         <v>739</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>26</v>
@@ -12776,7 +12773,7 @@
         <v>506</v>
       </c>
       <c r="M79" s="15" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12784,10 +12781,10 @@
         <v>507</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>915</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>916</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>774</v>
@@ -12817,7 +12814,7 @@
         <v>513</v>
       </c>
       <c r="M80" s="15" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12825,10 +12822,10 @@
         <v>514</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>917</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>918</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>774</v>
@@ -12858,7 +12855,7 @@
         <v>520</v>
       </c>
       <c r="M81" s="15" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12866,10 +12863,10 @@
         <v>521</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>919</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>920</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>756</v>
@@ -12899,7 +12896,7 @@
         <v>524</v>
       </c>
       <c r="M82" s="15" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12907,10 +12904,10 @@
         <v>525</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>921</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>922</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>752</v>
@@ -12940,7 +12937,7 @@
         <v>530</v>
       </c>
       <c r="M83" s="15" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12948,10 +12945,10 @@
         <v>531</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>923</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>924</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>848</v>
@@ -12981,7 +12978,7 @@
         <v>537</v>
       </c>
       <c r="M84" s="15" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -12989,10 +12986,10 @@
         <v>538</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>925</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>926</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>752</v>
@@ -13022,7 +13019,7 @@
         <v>542</v>
       </c>
       <c r="M85" s="15" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13030,10 +13027,10 @@
         <v>543</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>927</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>928</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>769</v>
@@ -13063,7 +13060,7 @@
         <v>549</v>
       </c>
       <c r="M86" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13071,10 +13068,10 @@
         <v>550</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>929</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>930</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>774</v>
@@ -13104,7 +13101,7 @@
         <v>555</v>
       </c>
       <c r="M87" s="15" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13112,10 +13109,10 @@
         <v>705</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>931</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>932</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>619</v>
@@ -13145,7 +13142,7 @@
         <v>560</v>
       </c>
       <c r="M88" s="15" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13153,10 +13150,10 @@
         <v>561</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>933</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>934</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>802</v>
@@ -13165,7 +13162,7 @@
         <v>739</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>40</v>
@@ -13186,7 +13183,7 @@
         <v>565</v>
       </c>
       <c r="M89" s="15" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13194,10 +13191,10 @@
         <v>566</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>936</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>937</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>848</v>
@@ -13227,7 +13224,7 @@
         <v>572</v>
       </c>
       <c r="M90" s="15" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13235,10 +13232,10 @@
         <v>573</v>
       </c>
       <c r="B91" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>938</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>939</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>752</v>
@@ -13268,7 +13265,7 @@
         <v>578</v>
       </c>
       <c r="M91" s="15" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13276,10 +13273,10 @@
         <v>579</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>940</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>941</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>774</v>
@@ -13309,7 +13306,7 @@
         <v>585</v>
       </c>
       <c r="M92" s="15" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13317,10 +13314,10 @@
         <v>586</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>942</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>943</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>774</v>
@@ -13350,7 +13347,7 @@
         <v>591</v>
       </c>
       <c r="M93" s="15" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13358,10 +13355,10 @@
         <v>592</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>944</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>945</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>752</v>
@@ -13391,7 +13388,7 @@
         <v>597</v>
       </c>
       <c r="M94" s="15" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13399,10 +13396,10 @@
         <v>598</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>946</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>947</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>752</v>
@@ -13432,7 +13429,7 @@
         <v>603</v>
       </c>
       <c r="M95" s="15" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13440,10 +13437,10 @@
         <v>604</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>948</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>949</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>769</v>
@@ -13473,7 +13470,7 @@
         <v>610</v>
       </c>
       <c r="M96" s="15" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13481,10 +13478,10 @@
         <v>611</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>950</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>951</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>761</v>
@@ -13493,7 +13490,7 @@
         <v>739</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>612</v>
@@ -13514,7 +13511,7 @@
         <v>617</v>
       </c>
       <c r="M97" s="15" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13522,10 +13519,10 @@
         <v>618</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>953</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>954</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>745</v>
@@ -13534,7 +13531,7 @@
         <v>739</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>477</v>
@@ -13555,7 +13552,7 @@
         <v>623</v>
       </c>
       <c r="M98" s="15" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13563,10 +13560,10 @@
         <v>624</v>
       </c>
       <c r="B99" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>955</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>956</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>774</v>
@@ -13596,7 +13593,7 @@
         <v>628</v>
       </c>
       <c r="M99" s="15" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13604,10 +13601,10 @@
         <v>629</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>957</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>958</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>745</v>
@@ -13637,7 +13634,7 @@
         <v>633</v>
       </c>
       <c r="M100" s="15" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13645,10 +13642,10 @@
         <v>634</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>959</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>960</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>752</v>
@@ -13678,7 +13675,7 @@
         <v>639</v>
       </c>
       <c r="M101" s="15" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13686,10 +13683,10 @@
         <v>640</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>961</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>962</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>774</v>
@@ -13719,7 +13716,7 @@
         <v>644</v>
       </c>
       <c r="M102" s="15" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13727,10 +13724,10 @@
         <v>645</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>963</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>964</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>848</v>
@@ -13760,7 +13757,7 @@
         <v>651</v>
       </c>
       <c r="M103" s="15" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13768,10 +13765,10 @@
         <v>652</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>965</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>966</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>863</v>
@@ -13783,25 +13780,25 @@
         <v>796</v>
       </c>
       <c r="G104" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H104" s="4" t="s">
         <v>1167</v>
       </c>
-      <c r="H104" s="4" t="s">
+      <c r="I104" s="4" t="s">
         <v>1168</v>
       </c>
-      <c r="I104" s="4" t="s">
+      <c r="J104" s="4" t="s">
         <v>1169</v>
       </c>
-      <c r="J104" s="4" t="s">
+      <c r="K104" s="3" t="s">
         <v>1170</v>
-      </c>
-      <c r="K104" s="3" t="s">
-        <v>1171</v>
       </c>
       <c r="L104" s="3" t="s">
         <v>653</v>
       </c>
       <c r="M104" s="15" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13809,10 +13806,10 @@
         <v>654</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>967</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>968</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>738</v>
@@ -13842,7 +13839,7 @@
         <v>660</v>
       </c>
       <c r="M105" s="15" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13850,10 +13847,10 @@
         <v>661</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>969</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>970</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>774</v>
@@ -13883,7 +13880,7 @@
         <v>667</v>
       </c>
       <c r="M106" s="15" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13891,10 +13888,10 @@
         <v>668</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>971</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>972</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>769</v>
@@ -13924,7 +13921,7 @@
         <v>673</v>
       </c>
       <c r="M107" s="15" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13932,10 +13929,10 @@
         <v>674</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>973</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>974</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>745</v>
@@ -13965,7 +13962,7 @@
         <v>679</v>
       </c>
       <c r="M108" s="15" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -13973,10 +13970,10 @@
         <v>680</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>975</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>976</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>742</v>
@@ -14006,7 +14003,7 @@
         <v>684</v>
       </c>
       <c r="M109" s="15" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14014,10 +14011,10 @@
         <v>685</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>977</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>978</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>756</v>
@@ -14047,7 +14044,7 @@
         <v>691</v>
       </c>
       <c r="M110" s="15" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14055,10 +14052,10 @@
         <v>692</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>979</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>980</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>802</v>
@@ -14088,7 +14085,7 @@
         <v>698</v>
       </c>
       <c r="M111" s="15" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -14096,10 +14093,10 @@
         <v>699</v>
       </c>
       <c r="B112" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>981</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>982</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>745</v>
@@ -14135,10 +14132,10 @@
         <v>720</v>
       </c>
       <c r="B113" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>1001</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>1002</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>774</v>
@@ -14150,25 +14147,25 @@
         <v>732</v>
       </c>
       <c r="G113" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H113" s="7" t="s">
         <v>1003</v>
       </c>
-      <c r="H113" s="7" t="s">
+      <c r="I113" s="7" t="s">
         <v>1004</v>
       </c>
-      <c r="I113" s="7" t="s">
+      <c r="J113" s="7" t="s">
         <v>1005</v>
       </c>
-      <c r="J113" s="7" t="s">
+      <c r="K113" s="7" t="s">
         <v>1006</v>
       </c>
-      <c r="K113" s="7" t="s">
+      <c r="L113" s="7" t="s">
         <v>1007</v>
       </c>
-      <c r="L113" s="7" t="s">
-        <v>1008</v>
-      </c>
       <c r="M113" s="15" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
@@ -14176,10 +14173,10 @@
         <v>721</v>
       </c>
       <c r="B114" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C114" s="7" t="s">
         <v>1009</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>1010</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>774</v>
@@ -14191,25 +14188,25 @@
         <v>753</v>
       </c>
       <c r="G114" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H114" s="7" t="s">
         <v>1011</v>
       </c>
-      <c r="H114" s="7" t="s">
+      <c r="I114" s="7" t="s">
         <v>1012</v>
       </c>
-      <c r="I114" s="7" t="s">
+      <c r="J114" s="7" t="s">
         <v>1013</v>
-      </c>
-      <c r="J114" s="7" t="s">
-        <v>1014</v>
       </c>
       <c r="K114" s="7" t="s">
         <v>13</v>
       </c>
       <c r="L114" s="20" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="M114" s="15" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -14217,10 +14214,10 @@
         <v>728</v>
       </c>
       <c r="B115" s="7" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>1028</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>1029</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>774</v>
@@ -14232,25 +14229,25 @@
         <v>753</v>
       </c>
       <c r="G115" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H115" s="7" t="s">
         <v>1030</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>1031</v>
       </c>
       <c r="I115" s="7" t="s">
         <v>219</v>
       </c>
       <c r="J115" s="7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="K115" s="7" t="s">
         <v>1032</v>
       </c>
-      <c r="K115" s="7" t="s">
+      <c r="L115" s="7" t="s">
         <v>1033</v>
       </c>
-      <c r="L115" s="7" t="s">
-        <v>1034</v>
-      </c>
       <c r="M115" s="15" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="116" spans="1:13" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.35">
@@ -14261,7 +14258,7 @@
         <v>735</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D116" s="7" t="str">
         <f>VLOOKUP(A116,'[1]MASTER LIST'!$C:$G,4,FALSE)</f>
@@ -14274,39 +14271,39 @@
         <v>732</v>
       </c>
       <c r="G116" s="12" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H116" s="12" t="s">
         <v>1042</v>
       </c>
-      <c r="H116" s="12" t="s">
+      <c r="I116" s="12" t="s">
         <v>1043</v>
       </c>
-      <c r="I116" s="12" t="s">
+      <c r="J116" s="12" t="s">
         <v>1044</v>
       </c>
-      <c r="J116" s="12" t="s">
+      <c r="K116" s="12" t="s">
         <v>1045</v>
       </c>
-      <c r="K116" s="12" t="s">
+      <c r="L116" s="14" t="s">
         <v>1046</v>
       </c>
-      <c r="L116" s="14" t="s">
-        <v>1047</v>
-      </c>
       <c r="M116" s="18" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="203.5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>1048</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="C117" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>1049</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>1050</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>739</v>
@@ -14315,25 +14312,25 @@
         <v>732</v>
       </c>
       <c r="G117" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H117" t="s">
         <v>1053</v>
-      </c>
-      <c r="H117" t="s">
-        <v>1054</v>
       </c>
       <c r="I117" t="s">
         <v>216</v>
       </c>
       <c r="J117" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="K117" t="s">
         <v>216</v>
       </c>
       <c r="L117" s="19" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="M117" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="118" spans="1:13" s="9" customFormat="1" ht="209.5" x14ac:dyDescent="0.3">
@@ -14341,10 +14338,10 @@
         <v>711</v>
       </c>
       <c r="B118" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>983</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>984</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>774</v>
@@ -14362,7 +14359,7 @@
       <c r="K118" s="7"/>
       <c r="L118" s="7"/>
       <c r="M118" s="22" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="119" spans="1:13" s="9" customFormat="1" ht="235.5" x14ac:dyDescent="0.3">
@@ -14370,10 +14367,10 @@
         <v>712</v>
       </c>
       <c r="B119" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>985</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>986</v>
       </c>
       <c r="D119" s="7" t="s">
         <v>745</v>
@@ -14391,7 +14388,7 @@
       <c r="K119" s="7"/>
       <c r="L119" s="7"/>
       <c r="M119" s="22" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="120" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
@@ -14399,10 +14396,10 @@
         <v>713</v>
       </c>
       <c r="B120" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>987</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>988</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>752</v>
@@ -14420,7 +14417,7 @@
       <c r="K120" s="7"/>
       <c r="L120" s="7"/>
       <c r="M120" s="18" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="121" spans="1:13" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
@@ -14428,10 +14425,10 @@
         <v>714</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>988</v>
+      </c>
+      <c r="C121" s="7" t="s">
         <v>989</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>990</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>756</v>
@@ -14449,7 +14446,7 @@
       <c r="K121" s="7"/>
       <c r="L121" s="7"/>
       <c r="M121" s="22" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="122" spans="1:13" s="9" customFormat="1" ht="338" x14ac:dyDescent="0.3">
@@ -14457,10 +14454,10 @@
         <v>715</v>
       </c>
       <c r="B122" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>991</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>992</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>774</v>
@@ -14478,7 +14475,7 @@
       <c r="K122" s="7"/>
       <c r="L122" s="7"/>
       <c r="M122" s="18" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="123" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
@@ -14486,10 +14483,10 @@
         <v>716</v>
       </c>
       <c r="B123" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>993</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>994</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>863</v>
@@ -14507,7 +14504,7 @@
       <c r="K123" s="7"/>
       <c r="L123" s="7"/>
       <c r="M123" s="18" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="124" spans="1:13" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
@@ -14515,10 +14512,10 @@
         <v>717</v>
       </c>
       <c r="B124" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>995</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>996</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>786</v>
@@ -14536,7 +14533,7 @@
       <c r="K124" s="7"/>
       <c r="L124" s="7"/>
       <c r="M124" s="18" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="125" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14544,10 +14541,10 @@
         <v>718</v>
       </c>
       <c r="B125" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>997</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>998</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>769</v>
@@ -14571,10 +14568,10 @@
         <v>719</v>
       </c>
       <c r="B126" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>999</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>1000</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>774</v>
@@ -14598,10 +14595,10 @@
         <v>722</v>
       </c>
       <c r="B127" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>1016</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>1017</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>745</v>
@@ -14613,7 +14610,7 @@
         <v>732</v>
       </c>
       <c r="G127" s="10" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
@@ -14627,10 +14624,10 @@
         <v>723</v>
       </c>
       <c r="B128" s="7" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C128" s="7" t="s">
         <v>1018</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>1019</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>745</v>
@@ -14654,10 +14651,10 @@
         <v>724</v>
       </c>
       <c r="B129" s="7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>1020</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>1021</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>756</v>
@@ -14681,10 +14678,10 @@
         <v>725</v>
       </c>
       <c r="B130" s="7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C130" s="7" t="s">
         <v>1022</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>1023</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>863</v>
@@ -14708,10 +14705,10 @@
         <v>726</v>
       </c>
       <c r="B131" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>1024</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>1025</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>786</v>
@@ -14735,10 +14732,10 @@
         <v>727</v>
       </c>
       <c r="B132" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C132" s="7" t="s">
         <v>1026</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>1027</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>774</v>
@@ -14762,10 +14759,10 @@
         <v>729</v>
       </c>
       <c r="B133" s="7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>1035</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>1036</v>
       </c>
       <c r="D133" s="7" t="s">
         <v>774</v>
@@ -14789,10 +14786,10 @@
         <v>730</v>
       </c>
       <c r="B134" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>1037</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>1038</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>863</v>
@@ -14815,10 +14812,10 @@
         <v>731</v>
       </c>
       <c r="B135" s="7" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>1039</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>1040</v>
       </c>
       <c r="D135" s="7" t="s">
         <v>738</v>

</xml_diff>